<commit_message>
Daten aktualisiert am 2023-05-23
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>27262</v>
+        <v>27276</v>
       </c>
       <c r="E2" t="n">
-        <v>528165725802</v>
+        <v>528639277835</v>
       </c>
       <c r="F2" t="n">
-        <v>12587577757</v>
+        <v>13874063711</v>
       </c>
       <c r="G2" t="n">
-        <v>1.55224</v>
+        <v>1.74562</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1852.07</v>
+        <v>1852.87</v>
       </c>
       <c r="E3" t="n">
-        <v>222754624912</v>
+        <v>222850581871</v>
       </c>
       <c r="F3" t="n">
-        <v>7366736701</v>
+        <v>7367478450</v>
       </c>
       <c r="G3" t="n">
-        <v>1.97064</v>
+        <v>2.11431</v>
       </c>
     </row>
     <row r="4">
@@ -545,10 +545,10 @@
         <v>83005505366</v>
       </c>
       <c r="F4" t="n">
-        <v>17448676249</v>
+        <v>17897337097</v>
       </c>
       <c r="G4" t="n">
-        <v>0.09531000000000001</v>
+        <v>0.07394000000000001</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>313.84</v>
+        <v>313.93</v>
       </c>
       <c r="E5" t="n">
-        <v>49559679612</v>
+        <v>49568226989</v>
       </c>
       <c r="F5" t="n">
-        <v>461700954</v>
+        <v>476025639</v>
       </c>
       <c r="G5" t="n">
-        <v>1.14176</v>
+        <v>1.26289</v>
       </c>
     </row>
     <row r="6">
@@ -599,10 +599,10 @@
         <v>29256786587</v>
       </c>
       <c r="F6" t="n">
-        <v>3948519113</v>
+        <v>3961433447</v>
       </c>
       <c r="G6" t="n">
-        <v>0.15613</v>
+        <v>0.18388</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.460412</v>
+        <v>0.460605</v>
       </c>
       <c r="E7" t="n">
         <v>23880825093</v>
       </c>
       <c r="F7" t="n">
-        <v>901335573</v>
+        <v>901457129</v>
       </c>
       <c r="G7" t="n">
-        <v>0.8386400000000001</v>
+        <v>0.92757</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.370608</v>
+        <v>0.370853</v>
       </c>
       <c r="E8" t="n">
-        <v>12987019023</v>
+        <v>12994617048</v>
       </c>
       <c r="F8" t="n">
-        <v>157740971</v>
+        <v>157547707</v>
       </c>
       <c r="G8" t="n">
-        <v>0.68207</v>
+        <v>0.74859</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1850.57</v>
+        <v>1851.46</v>
       </c>
       <c r="E9" t="n">
         <v>12286698918</v>
       </c>
       <c r="F9" t="n">
-        <v>7003706</v>
+        <v>7007026</v>
       </c>
       <c r="G9" t="n">
-        <v>1.90664</v>
+        <v>2.07822</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.072925</v>
+        <v>0.072948</v>
       </c>
       <c r="E10" t="n">
-        <v>10165221858</v>
+        <v>10174200775</v>
       </c>
       <c r="F10" t="n">
-        <v>200887247</v>
+        <v>200840393</v>
       </c>
       <c r="G10" t="n">
-        <v>0.19601</v>
+        <v>0.32146</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.88834</v>
+        <v>0.888432</v>
       </c>
       <c r="E11" t="n">
-        <v>8244457962</v>
+        <v>8244403754</v>
       </c>
       <c r="F11" t="n">
-        <v>214696332</v>
+        <v>214674809</v>
       </c>
       <c r="G11" t="n">
-        <v>2.34086</v>
+        <v>2.40271</v>
       </c>
     </row>
     <row r="12">
@@ -761,10 +761,10 @@
         <v>7951418302</v>
       </c>
       <c r="F12" t="n">
-        <v>280252259</v>
+        <v>280395099</v>
       </c>
       <c r="G12" t="n">
-        <v>2.47521</v>
+        <v>2.53619</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.07803599999999999</v>
+        <v>0.078044</v>
       </c>
       <c r="E13" t="n">
         <v>7054934437</v>
       </c>
       <c r="F13" t="n">
-        <v>384276442</v>
+        <v>384180992</v>
       </c>
       <c r="G13" t="n">
-        <v>-1.05976</v>
+        <v>-1.13053</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>91.29000000000001</v>
+        <v>91.36</v>
       </c>
       <c r="E14" t="n">
-        <v>6664804580</v>
+        <v>6667210013</v>
       </c>
       <c r="F14" t="n">
-        <v>382134120</v>
+        <v>380655855</v>
       </c>
       <c r="G14" t="n">
-        <v>0.6087399999999999</v>
+        <v>0.77098</v>
       </c>
     </row>
     <row r="15">
@@ -842,10 +842,10 @@
         <v>6652446439</v>
       </c>
       <c r="F15" t="n">
-        <v>97036472</v>
+        <v>96839308</v>
       </c>
       <c r="G15" t="n">
-        <v>1.57553</v>
+        <v>1.66126</v>
       </c>
     </row>
     <row r="16">
@@ -866,13 +866,13 @@
         <v>1.001</v>
       </c>
       <c r="E16" t="n">
-        <v>5434157786</v>
+        <v>5435876053</v>
       </c>
       <c r="F16" t="n">
-        <v>1246601540</v>
+        <v>1785248241</v>
       </c>
       <c r="G16" t="n">
-        <v>0.20076</v>
+        <v>0.15938</v>
       </c>
     </row>
     <row r="17">
@@ -896,10 +896,10 @@
         <v>5257564228</v>
       </c>
       <c r="F17" t="n">
-        <v>151891016</v>
+        <v>151672461</v>
       </c>
       <c r="G17" t="n">
-        <v>1.02505</v>
+        <v>1.03469</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>14.71</v>
+        <v>14.73</v>
       </c>
       <c r="E18" t="n">
-        <v>4924822966</v>
+        <v>4925729567</v>
       </c>
       <c r="F18" t="n">
-        <v>126647607</v>
+        <v>126639848</v>
       </c>
       <c r="G18" t="n">
-        <v>0.79879</v>
+        <v>0.89701</v>
       </c>
     </row>
     <row r="19">
@@ -947,13 +947,13 @@
         <v>1</v>
       </c>
       <c r="E19" t="n">
-        <v>4648318105</v>
+        <v>4649942367</v>
       </c>
       <c r="F19" t="n">
-        <v>99784737</v>
+        <v>98405498</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.07843</v>
+        <v>0.12258</v>
       </c>
     </row>
     <row r="20">
@@ -971,16 +971,16 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>27312</v>
+        <v>27321</v>
       </c>
       <c r="E20" t="n">
         <v>4260144583</v>
       </c>
       <c r="F20" t="n">
-        <v>67971259</v>
+        <v>68297836</v>
       </c>
       <c r="G20" t="n">
-        <v>1.67084</v>
+        <v>1.70357</v>
       </c>
     </row>
     <row r="21">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>5.1</v>
+        <v>5.11</v>
       </c>
       <c r="E21" t="n">
         <v>3848911442</v>
       </c>
       <c r="F21" t="n">
-        <v>36281421</v>
+        <v>36285067</v>
       </c>
       <c r="G21" t="n">
-        <v>0.81684</v>
+        <v>0.87341</v>
       </c>
     </row>
     <row r="22">
@@ -1028,13 +1028,13 @@
         <v>6.52</v>
       </c>
       <c r="E22" t="n">
-        <v>3369333111</v>
+        <v>3373022006</v>
       </c>
       <c r="F22" t="n">
-        <v>106073849</v>
+        <v>106052224</v>
       </c>
       <c r="G22" t="n">
-        <v>0.18687</v>
+        <v>0.269</v>
       </c>
     </row>
     <row r="23">
@@ -1055,13 +1055,13 @@
         <v>3.53</v>
       </c>
       <c r="E23" t="n">
-        <v>3278763724</v>
+        <v>3284950488</v>
       </c>
       <c r="F23" t="n">
-        <v>249087</v>
+        <v>249464</v>
       </c>
       <c r="G23" t="n">
-        <v>0.38542</v>
+        <v>0.50552</v>
       </c>
     </row>
     <row r="24">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>10.53</v>
+        <v>10.54</v>
       </c>
       <c r="E24" t="n">
-        <v>3080368483</v>
+        <v>3084062596</v>
       </c>
       <c r="F24" t="n">
-        <v>70937323</v>
+        <v>71047397</v>
       </c>
       <c r="G24" t="n">
-        <v>0.63228</v>
+        <v>0.76315</v>
       </c>
     </row>
     <row r="25">
@@ -1112,10 +1112,10 @@
         <v>2831749943</v>
       </c>
       <c r="F25" t="n">
-        <v>10494904</v>
+        <v>10497130</v>
       </c>
       <c r="G25" t="n">
-        <v>5.17962</v>
+        <v>5.24755</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>46.11</v>
+        <v>46.14</v>
       </c>
       <c r="E26" t="n">
         <v>2766185087</v>
       </c>
       <c r="F26" t="n">
-        <v>5837246</v>
+        <v>5840252</v>
       </c>
       <c r="G26" t="n">
-        <v>0.59453</v>
+        <v>0.7467200000000001</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>151.84</v>
+        <v>151.9</v>
       </c>
       <c r="E27" t="n">
-        <v>2754011376</v>
+        <v>2756579606</v>
       </c>
       <c r="F27" t="n">
-        <v>71483513</v>
+        <v>71039057</v>
       </c>
       <c r="G27" t="n">
-        <v>0.00098</v>
+        <v>0.01706</v>
       </c>
     </row>
     <row r="28">
@@ -1187,16 +1187,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>18.38</v>
+        <v>18.39</v>
       </c>
       <c r="E28" t="n">
-        <v>2591455385</v>
+        <v>2595079537</v>
       </c>
       <c r="F28" t="n">
-        <v>64149287</v>
+        <v>64203204</v>
       </c>
       <c r="G28" t="n">
-        <v>1.12841</v>
+        <v>1.25849</v>
       </c>
     </row>
     <row r="29">
@@ -1214,16 +1214,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.088115</v>
+        <v>0.08813500000000001</v>
       </c>
       <c r="E29" t="n">
         <v>2359058686</v>
       </c>
       <c r="F29" t="n">
-        <v>34667800</v>
+        <v>34682590</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.01276</v>
+        <v>-0.02373</v>
       </c>
     </row>
     <row r="30">
@@ -1241,16 +1241,16 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>115.58</v>
+        <v>115.59</v>
       </c>
       <c r="E30" t="n">
-        <v>2244028280</v>
+        <v>2242335298</v>
       </c>
       <c r="F30" t="n">
-        <v>53514958</v>
+        <v>53530295</v>
       </c>
       <c r="G30" t="n">
-        <v>1.18522</v>
+        <v>1.27397</v>
       </c>
     </row>
     <row r="31">
@@ -1268,16 +1268,16 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>5.06</v>
+        <v>5.07</v>
       </c>
       <c r="E31" t="n">
-        <v>2208876466</v>
+        <v>2209821934</v>
       </c>
       <c r="F31" t="n">
-        <v>19992154</v>
+        <v>20013311</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.86359</v>
+        <v>-0.79451</v>
       </c>
     </row>
     <row r="32">
@@ -1301,10 +1301,10 @@
         <v>2041879957</v>
       </c>
       <c r="F32" t="n">
-        <v>225777032</v>
+        <v>225910435</v>
       </c>
       <c r="G32" t="n">
-        <v>0.05541</v>
+        <v>0.14667</v>
       </c>
     </row>
     <row r="33">
@@ -1325,13 +1325,13 @@
         <v>4.5</v>
       </c>
       <c r="E33" t="n">
-        <v>1920625244</v>
+        <v>1918538847</v>
       </c>
       <c r="F33" t="n">
-        <v>85140594</v>
+        <v>85299154</v>
       </c>
       <c r="G33" t="n">
-        <v>1.90899</v>
+        <v>1.98419</v>
       </c>
     </row>
     <row r="34">
@@ -1352,13 +1352,13 @@
         <v>2.06</v>
       </c>
       <c r="E34" t="n">
-        <v>1811158810</v>
+        <v>1812480864</v>
       </c>
       <c r="F34" t="n">
-        <v>38773165</v>
+        <v>38836466</v>
       </c>
       <c r="G34" t="n">
-        <v>1.05418</v>
+        <v>1.34509</v>
       </c>
     </row>
     <row r="35">
@@ -1376,16 +1376,16 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.052818</v>
+        <v>0.052826</v>
       </c>
       <c r="E35" t="n">
-        <v>1663086569</v>
+        <v>1662170418</v>
       </c>
       <c r="F35" t="n">
-        <v>14875102</v>
+        <v>14904065</v>
       </c>
       <c r="G35" t="n">
-        <v>0.82491</v>
+        <v>0.9819</v>
       </c>
     </row>
     <row r="36">
@@ -1406,13 +1406,13 @@
         <v>8.390000000000001</v>
       </c>
       <c r="E36" t="n">
-        <v>1658225385</v>
+        <v>1658363484</v>
       </c>
       <c r="F36" t="n">
-        <v>46506293</v>
+        <v>46827604</v>
       </c>
       <c r="G36" t="n">
-        <v>3.14058</v>
+        <v>3.23461</v>
       </c>
     </row>
     <row r="37">
@@ -1430,16 +1430,16 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.062114</v>
+        <v>0.062121</v>
       </c>
       <c r="E37" t="n">
-        <v>1570315064</v>
+        <v>1569624329</v>
       </c>
       <c r="F37" t="n">
-        <v>5135802</v>
+        <v>5135880</v>
       </c>
       <c r="G37" t="n">
-        <v>0.0459</v>
+        <v>0.05143</v>
       </c>
     </row>
     <row r="38">
@@ -1460,13 +1460,13 @@
         <v>1.17</v>
       </c>
       <c r="E38" t="n">
-        <v>1491467773</v>
+        <v>1491076358</v>
       </c>
       <c r="F38" t="n">
-        <v>161395938</v>
+        <v>151936138</v>
       </c>
       <c r="G38" t="n">
-        <v>4.11139</v>
+        <v>4.18773</v>
       </c>
     </row>
     <row r="39">
@@ -1484,16 +1484,16 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>102.44</v>
+        <v>102.46</v>
       </c>
       <c r="E39" t="n">
         <v>1490434621</v>
       </c>
       <c r="F39" t="n">
-        <v>12441041</v>
+        <v>12444136</v>
       </c>
       <c r="G39" t="n">
-        <v>0.60433</v>
+        <v>0.70685</v>
       </c>
     </row>
     <row r="40">
@@ -1514,13 +1514,13 @@
         <v>1.64</v>
       </c>
       <c r="E40" t="n">
-        <v>1489377749</v>
+        <v>1489716781</v>
       </c>
       <c r="F40" t="n">
-        <v>51323309</v>
+        <v>51352474</v>
       </c>
       <c r="G40" t="n">
-        <v>1.52159</v>
+        <v>1.61429</v>
       </c>
     </row>
     <row r="41">
@@ -1538,16 +1538,16 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.01950807</v>
+        <v>0.01952377</v>
       </c>
       <c r="E41" t="n">
         <v>1419315686</v>
       </c>
       <c r="F41" t="n">
-        <v>33293915</v>
+        <v>33348086</v>
       </c>
       <c r="G41" t="n">
-        <v>0.9257300000000001</v>
+        <v>1.08415</v>
       </c>
     </row>
     <row r="42">
@@ -1568,13 +1568,13 @@
         <v>3.52</v>
       </c>
       <c r="E42" t="n">
-        <v>1295861269</v>
+        <v>1297243483</v>
       </c>
       <c r="F42" t="n">
-        <v>38935664</v>
+        <v>40646797</v>
       </c>
       <c r="G42" t="n">
-        <v>2.65381</v>
+        <v>2.69316</v>
       </c>
     </row>
     <row r="43">
@@ -1592,16 +1592,16 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.164297</v>
+        <v>0.164273</v>
       </c>
       <c r="E43" t="n">
-        <v>1190286859</v>
+        <v>1189504884</v>
       </c>
       <c r="F43" t="n">
-        <v>30080231</v>
+        <v>30106736</v>
       </c>
       <c r="G43" t="n">
-        <v>0.97824</v>
+        <v>1.06676</v>
       </c>
     </row>
     <row r="44">
@@ -1619,16 +1619,16 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.12268</v>
+        <v>0.122792</v>
       </c>
       <c r="E44" t="n">
         <v>1101814530</v>
       </c>
       <c r="F44" t="n">
-        <v>28767692</v>
+        <v>28799680</v>
       </c>
       <c r="G44" t="n">
-        <v>2.28867</v>
+        <v>2.44417</v>
       </c>
     </row>
     <row r="45">
@@ -1646,16 +1646,16 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.366748</v>
+        <v>0.367123</v>
       </c>
       <c r="E45" t="n">
-        <v>1022699496</v>
+        <v>1023332918</v>
       </c>
       <c r="F45" t="n">
-        <v>83985871</v>
+        <v>84048080</v>
       </c>
       <c r="G45" t="n">
-        <v>1.43918</v>
+        <v>1.62506</v>
       </c>
     </row>
     <row r="46">
@@ -1673,16 +1673,16 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.999676</v>
+        <v>1</v>
       </c>
       <c r="E46" t="n">
         <v>1018265241</v>
       </c>
       <c r="F46" t="n">
-        <v>41314279</v>
+        <v>41330700</v>
       </c>
       <c r="G46" t="n">
-        <v>0.06184</v>
+        <v>0.06762</v>
       </c>
     </row>
     <row r="47">
@@ -1700,16 +1700,16 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>2.76</v>
+        <v>2.75</v>
       </c>
       <c r="E47" t="n">
         <v>1006510655</v>
       </c>
       <c r="F47" t="n">
-        <v>154406550</v>
+        <v>154827769</v>
       </c>
       <c r="G47" t="n">
-        <v>14.21923</v>
+        <v>14.03482</v>
       </c>
     </row>
     <row r="48">
@@ -1727,16 +1727,16 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>1.001</v>
       </c>
       <c r="E48" t="n">
-        <v>1004457491</v>
+        <v>1004791651</v>
       </c>
       <c r="F48" t="n">
-        <v>4200031</v>
+        <v>4200723</v>
       </c>
       <c r="G48" t="n">
-        <v>0.36675</v>
+        <v>0.29571</v>
       </c>
     </row>
     <row r="49">
@@ -1757,13 +1757,13 @@
         <v>1.001</v>
       </c>
       <c r="E49" t="n">
-        <v>1000821776</v>
+        <v>1000291325</v>
       </c>
       <c r="F49" t="n">
-        <v>5491891</v>
+        <v>5489960</v>
       </c>
       <c r="G49" t="n">
-        <v>0.12523</v>
+        <v>0.09003</v>
       </c>
     </row>
     <row r="50">
@@ -1781,16 +1781,16 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.51305</v>
+        <v>0.513279</v>
       </c>
       <c r="E50" t="n">
         <v>950967573</v>
       </c>
       <c r="F50" t="n">
-        <v>65460081</v>
+        <v>65460804</v>
       </c>
       <c r="G50" t="n">
-        <v>0.2014</v>
+        <v>0.39961</v>
       </c>
     </row>
     <row r="51">
@@ -1808,16 +1808,16 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.859487</v>
+        <v>0.859612</v>
       </c>
       <c r="E51" t="n">
-        <v>950658816</v>
+        <v>950591945</v>
       </c>
       <c r="F51" t="n">
-        <v>87500709</v>
+        <v>87428329</v>
       </c>
       <c r="G51" t="n">
-        <v>0.99485</v>
+        <v>1.05194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-05-24
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>26346</v>
+        <v>26352</v>
       </c>
       <c r="E2" t="n">
-        <v>510596023192</v>
+        <v>510675236770</v>
       </c>
       <c r="F2" t="n">
-        <v>17396494376</v>
+        <v>9477488509</v>
       </c>
       <c r="G2" t="n">
-        <v>-3.14237</v>
+        <v>-3.12171</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1799.06</v>
+        <v>1800.02</v>
       </c>
       <c r="E3" t="n">
-        <v>216402029053</v>
+        <v>216363342154</v>
       </c>
       <c r="F3" t="n">
-        <v>8046390671</v>
+        <v>8001002124</v>
       </c>
       <c r="G3" t="n">
-        <v>-2.92535</v>
+        <v>-2.88059</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999325</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>83023761196</v>
+        <v>83028796839</v>
       </c>
       <c r="F4" t="n">
-        <v>16894118207</v>
+        <v>23491717970</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.06</v>
+        <v>0.01933</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>305.88</v>
+        <v>306.09</v>
       </c>
       <c r="E5" t="n">
-        <v>48289098108</v>
+        <v>48304263379</v>
       </c>
       <c r="F5" t="n">
-        <v>550907459</v>
+        <v>566911502</v>
       </c>
       <c r="G5" t="n">
-        <v>-2.38539</v>
+        <v>-2.33032</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0.999692</v>
       </c>
       <c r="E6" t="n">
-        <v>29142723430</v>
+        <v>29127165251</v>
       </c>
       <c r="F6" t="n">
-        <v>4579216518</v>
+        <v>3253358607</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.009390000000000001</v>
+        <v>0.0008899999999999999</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.454682</v>
+        <v>0.455152</v>
       </c>
       <c r="E7" t="n">
-        <v>23572225398</v>
+        <v>23601672587</v>
       </c>
       <c r="F7" t="n">
-        <v>1117989578</v>
+        <v>1118517791</v>
       </c>
       <c r="G7" t="n">
-        <v>-2.40233</v>
+        <v>-2.22397</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.364169</v>
+        <v>0.364581</v>
       </c>
       <c r="E8" t="n">
-        <v>12760732161</v>
+        <v>12772728730</v>
       </c>
       <c r="F8" t="n">
-        <v>189303293</v>
+        <v>189263165</v>
       </c>
       <c r="G8" t="n">
-        <v>-1.74875</v>
+        <v>-1.61656</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1798.65</v>
+        <v>1797.72</v>
       </c>
       <c r="E9" t="n">
-        <v>11999249552</v>
+        <v>11992041666</v>
       </c>
       <c r="F9" t="n">
-        <v>11423182</v>
+        <v>11319492</v>
       </c>
       <c r="G9" t="n">
-        <v>-2.80819</v>
+        <v>-2.85186</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.07087300000000001</v>
+        <v>0.070877</v>
       </c>
       <c r="E10" t="n">
-        <v>9886329564</v>
+        <v>9886542067</v>
       </c>
       <c r="F10" t="n">
-        <v>319389630</v>
+        <v>318174237</v>
       </c>
       <c r="G10" t="n">
-        <v>-2.81779</v>
+        <v>-2.80056</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.873851</v>
+        <v>0.874905</v>
       </c>
       <c r="E11" t="n">
-        <v>8111114347</v>
+        <v>8117055439</v>
       </c>
       <c r="F11" t="n">
-        <v>235100801</v>
+        <v>239341729</v>
       </c>
       <c r="G11" t="n">
-        <v>-1.87573</v>
+        <v>-1.77351</v>
       </c>
     </row>
     <row r="12">
@@ -758,13 +758,13 @@
         <v>19.23</v>
       </c>
       <c r="E12" t="n">
-        <v>7613303811</v>
+        <v>7619938877</v>
       </c>
       <c r="F12" t="n">
-        <v>320487470</v>
+        <v>321103279</v>
       </c>
       <c r="G12" t="n">
-        <v>-3.99424</v>
+        <v>-4.11632</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.07692300000000001</v>
+        <v>0.077029</v>
       </c>
       <c r="E13" t="n">
-        <v>6946194792</v>
+        <v>6958382596</v>
       </c>
       <c r="F13" t="n">
-        <v>373204808</v>
+        <v>370834050</v>
       </c>
       <c r="G13" t="n">
-        <v>-2.17421</v>
+        <v>-1.9949</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>5.25</v>
+        <v>5.26</v>
       </c>
       <c r="E14" t="n">
-        <v>6491133106</v>
+        <v>6497062513</v>
       </c>
       <c r="F14" t="n">
-        <v>104784927</v>
+        <v>104965747</v>
       </c>
       <c r="G14" t="n">
-        <v>-2.64857</v>
+        <v>-2.54622</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>85.94</v>
+        <v>86.02</v>
       </c>
       <c r="E15" t="n">
-        <v>6277688333</v>
+        <v>6278838365</v>
       </c>
       <c r="F15" t="n">
-        <v>849349122</v>
+        <v>845772160</v>
       </c>
       <c r="G15" t="n">
-        <v>-5.84816</v>
+        <v>-5.82987</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>0.999597</v>
       </c>
       <c r="E16" t="n">
-        <v>5333721109</v>
+        <v>5333590561</v>
       </c>
       <c r="F16" t="n">
-        <v>1585041716</v>
+        <v>2178215477</v>
       </c>
       <c r="G16" t="n">
-        <v>0.04301</v>
+        <v>-0.02084</v>
       </c>
     </row>
     <row r="17">
@@ -890,16 +890,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>8.53e-06</v>
+        <v>8.549999999999999e-06</v>
       </c>
       <c r="E17" t="n">
-        <v>5031641385</v>
+        <v>5031393684</v>
       </c>
       <c r="F17" t="n">
-        <v>127872333</v>
+        <v>128059992</v>
       </c>
       <c r="G17" t="n">
-        <v>-4.30908</v>
+        <v>-4.18783</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>14.11</v>
+        <v>14.13</v>
       </c>
       <c r="E18" t="n">
-        <v>4719935669</v>
+        <v>4726914375</v>
       </c>
       <c r="F18" t="n">
-        <v>140848734</v>
+        <v>139711690</v>
       </c>
       <c r="G18" t="n">
-        <v>-4.10447</v>
+        <v>-3.91398</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1.001</v>
+        <v>0.999606</v>
       </c>
       <c r="E19" t="n">
-        <v>4633094762</v>
+        <v>4627028447</v>
       </c>
       <c r="F19" t="n">
-        <v>120278269</v>
+        <v>120165964</v>
       </c>
       <c r="G19" t="n">
-        <v>0.04629</v>
+        <v>-0.04279</v>
       </c>
     </row>
     <row r="20">
@@ -971,16 +971,16 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>26395</v>
+        <v>26402</v>
       </c>
       <c r="E20" t="n">
-        <v>4118786462</v>
+        <v>4118586111</v>
       </c>
       <c r="F20" t="n">
-        <v>79416931</v>
+        <v>78160924</v>
       </c>
       <c r="G20" t="n">
-        <v>-3.10592</v>
+        <v>-3.0684</v>
       </c>
     </row>
     <row r="21">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>4.97</v>
+        <v>4.98</v>
       </c>
       <c r="E21" t="n">
-        <v>3751917753</v>
+        <v>3749850755</v>
       </c>
       <c r="F21" t="n">
-        <v>46592794</v>
+        <v>46532617</v>
       </c>
       <c r="G21" t="n">
-        <v>-2.2137</v>
+        <v>-2.02506</v>
       </c>
     </row>
     <row r="22">
@@ -1028,13 +1028,13 @@
         <v>3.54</v>
       </c>
       <c r="E22" t="n">
-        <v>3294603420</v>
+        <v>3294013234</v>
       </c>
       <c r="F22" t="n">
-        <v>223873</v>
+        <v>223644</v>
       </c>
       <c r="G22" t="n">
-        <v>0.85197</v>
+        <v>0.8761100000000001</v>
       </c>
     </row>
     <row r="23">
@@ -1052,16 +1052,16 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>6.33</v>
+        <v>6.34</v>
       </c>
       <c r="E23" t="n">
-        <v>3272163711</v>
+        <v>3274838315</v>
       </c>
       <c r="F23" t="n">
-        <v>154763152</v>
+        <v>155026690</v>
       </c>
       <c r="G23" t="n">
-        <v>-2.8186</v>
+        <v>-2.66607</v>
       </c>
     </row>
     <row r="24">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>10.39</v>
+        <v>10.41</v>
       </c>
       <c r="E24" t="n">
-        <v>3040697324</v>
+        <v>3044569189</v>
       </c>
       <c r="F24" t="n">
-        <v>76988325</v>
+        <v>77186250</v>
       </c>
       <c r="G24" t="n">
-        <v>-1.17715</v>
+        <v>-1.07175</v>
       </c>
     </row>
     <row r="25">
@@ -1106,16 +1106,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>1.96</v>
+        <v>1.97</v>
       </c>
       <c r="E25" t="n">
-        <v>2906027604</v>
+        <v>2896790669</v>
       </c>
       <c r="F25" t="n">
-        <v>12875029</v>
+        <v>12202379</v>
       </c>
       <c r="G25" t="n">
-        <v>-4.80448</v>
+        <v>-3.96794</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>150.32</v>
+        <v>150.26</v>
       </c>
       <c r="E26" t="n">
-        <v>2728736684</v>
+        <v>2727306374</v>
       </c>
       <c r="F26" t="n">
-        <v>66392120</v>
+        <v>64984950</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.70281</v>
+        <v>-0.6789500000000001</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>44.81</v>
+        <v>44.71</v>
       </c>
       <c r="E27" t="n">
-        <v>2687399707</v>
+        <v>2683746185</v>
       </c>
       <c r="F27" t="n">
-        <v>7546292</v>
+        <v>7564958</v>
       </c>
       <c r="G27" t="n">
-        <v>-2.5306</v>
+        <v>-2.76316</v>
       </c>
     </row>
     <row r="28">
@@ -1187,16 +1187,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>17.77</v>
+        <v>17.78</v>
       </c>
       <c r="E28" t="n">
-        <v>2509307594</v>
+        <v>2508960103</v>
       </c>
       <c r="F28" t="n">
-        <v>76300887</v>
+        <v>76149025</v>
       </c>
       <c r="G28" t="n">
-        <v>-3.29843</v>
+        <v>-3.23918</v>
       </c>
     </row>
     <row r="29">
@@ -1214,16 +1214,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.08650099999999999</v>
+        <v>0.086622</v>
       </c>
       <c r="E29" t="n">
-        <v>2317308860</v>
+        <v>2319106249</v>
       </c>
       <c r="F29" t="n">
-        <v>37242949</v>
+        <v>37187637</v>
       </c>
       <c r="G29" t="n">
-        <v>-1.93709</v>
+        <v>-1.74851</v>
       </c>
     </row>
     <row r="30">
@@ -1241,16 +1241,16 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>112.12</v>
+        <v>112.31</v>
       </c>
       <c r="E30" t="n">
-        <v>2174889330</v>
+        <v>2177770417</v>
       </c>
       <c r="F30" t="n">
-        <v>64797620</v>
+        <v>65039739</v>
       </c>
       <c r="G30" t="n">
-        <v>-3.0191</v>
+        <v>-2.81503</v>
       </c>
     </row>
     <row r="31">
@@ -1271,13 +1271,13 @@
         <v>4.81</v>
       </c>
       <c r="E31" t="n">
-        <v>2099061202</v>
+        <v>2099920815</v>
       </c>
       <c r="F31" t="n">
-        <v>27727325</v>
+        <v>27508249</v>
       </c>
       <c r="G31" t="n">
-        <v>-4.46151</v>
+        <v>-4.29772</v>
       </c>
     </row>
     <row r="32">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>1</v>
+        <v>0.999519</v>
       </c>
       <c r="E32" t="n">
-        <v>2039864895</v>
+        <v>2040785907</v>
       </c>
       <c r="F32" t="n">
-        <v>232912861</v>
+        <v>231161664</v>
       </c>
       <c r="G32" t="n">
-        <v>0.00703</v>
+        <v>-0.02085</v>
       </c>
     </row>
     <row r="33">
@@ -1325,13 +1325,13 @@
         <v>4.47</v>
       </c>
       <c r="E33" t="n">
-        <v>1904317882</v>
+        <v>1906259810</v>
       </c>
       <c r="F33" t="n">
-        <v>110655141</v>
+        <v>110355388</v>
       </c>
       <c r="G33" t="n">
-        <v>-1.02814</v>
+        <v>-1.02616</v>
       </c>
     </row>
     <row r="34">
@@ -1352,13 +1352,13 @@
         <v>2.05</v>
       </c>
       <c r="E34" t="n">
-        <v>1797830822</v>
+        <v>1799041584</v>
       </c>
       <c r="F34" t="n">
-        <v>63501893</v>
+        <v>63778715</v>
       </c>
       <c r="G34" t="n">
-        <v>0.0552</v>
+        <v>0.29092</v>
       </c>
     </row>
     <row r="35">
@@ -1376,16 +1376,16 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.050966</v>
+        <v>0.050997</v>
       </c>
       <c r="E35" t="n">
-        <v>1603237213</v>
+        <v>1604273142</v>
       </c>
       <c r="F35" t="n">
-        <v>20064109</v>
+        <v>20052660</v>
       </c>
       <c r="G35" t="n">
-        <v>-2.73854</v>
+        <v>-2.79466</v>
       </c>
     </row>
     <row r="36">
@@ -1403,16 +1403,16 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>8.08</v>
+        <v>8.09</v>
       </c>
       <c r="E36" t="n">
-        <v>1599667974</v>
+        <v>1600806471</v>
       </c>
       <c r="F36" t="n">
-        <v>67325407</v>
+        <v>67392754</v>
       </c>
       <c r="G36" t="n">
-        <v>-4.70491</v>
+        <v>-4.75764</v>
       </c>
     </row>
     <row r="37">
@@ -1430,16 +1430,16 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.059914</v>
+        <v>0.059916</v>
       </c>
       <c r="E37" t="n">
-        <v>1513603346</v>
+        <v>1513456266</v>
       </c>
       <c r="F37" t="n">
-        <v>7725979</v>
+        <v>7728402</v>
       </c>
       <c r="G37" t="n">
-        <v>-3.58514</v>
+        <v>-3.59154</v>
       </c>
     </row>
     <row r="38">
@@ -1457,16 +1457,16 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>100.43</v>
+        <v>100.57</v>
       </c>
       <c r="E38" t="n">
-        <v>1460042003</v>
+        <v>1462866211</v>
       </c>
       <c r="F38" t="n">
-        <v>16002413</v>
+        <v>15991436</v>
       </c>
       <c r="G38" t="n">
-        <v>-2.20419</v>
+        <v>-2.12653</v>
       </c>
     </row>
     <row r="39">
@@ -1484,16 +1484,16 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1.57</v>
+        <v>1.58</v>
       </c>
       <c r="E39" t="n">
-        <v>1431685263</v>
+        <v>1432699621</v>
       </c>
       <c r="F39" t="n">
-        <v>61461472</v>
+        <v>61574852</v>
       </c>
       <c r="G39" t="n">
-        <v>-4.6545</v>
+        <v>-3.9758</v>
       </c>
     </row>
     <row r="40">
@@ -1514,13 +1514,13 @@
         <v>1.11</v>
       </c>
       <c r="E40" t="n">
-        <v>1415232262</v>
+        <v>1415630407</v>
       </c>
       <c r="F40" t="n">
-        <v>191306139</v>
+        <v>191200833</v>
       </c>
       <c r="G40" t="n">
-        <v>-4.79588</v>
+        <v>-4.5947</v>
       </c>
     </row>
     <row r="41">
@@ -1538,16 +1538,16 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.01940721</v>
+        <v>0.01944057</v>
       </c>
       <c r="E41" t="n">
-        <v>1410746766</v>
+        <v>1412961718</v>
       </c>
       <c r="F41" t="n">
-        <v>41027006</v>
+        <v>41235137</v>
       </c>
       <c r="G41" t="n">
-        <v>-0.07725</v>
+        <v>0.13137</v>
       </c>
     </row>
     <row r="42">
@@ -1568,13 +1568,13 @@
         <v>3.33</v>
       </c>
       <c r="E42" t="n">
-        <v>1227559644</v>
+        <v>1228376218</v>
       </c>
       <c r="F42" t="n">
-        <v>68614318</v>
+        <v>73239921</v>
       </c>
       <c r="G42" t="n">
-        <v>-4.80593</v>
+        <v>-4.79747</v>
       </c>
     </row>
     <row r="43">
@@ -1592,16 +1592,16 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.155278</v>
+        <v>0.155338</v>
       </c>
       <c r="E43" t="n">
-        <v>1124710956</v>
+        <v>1124448097</v>
       </c>
       <c r="F43" t="n">
-        <v>48566513</v>
+        <v>48637583</v>
       </c>
       <c r="G43" t="n">
-        <v>-4.94128</v>
+        <v>-4.94942</v>
       </c>
     </row>
     <row r="44">
@@ -1619,16 +1619,16 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.116245</v>
+        <v>0.116614</v>
       </c>
       <c r="E44" t="n">
-        <v>1045249987</v>
+        <v>1047130585</v>
       </c>
       <c r="F44" t="n">
-        <v>38871990</v>
+        <v>38885460</v>
       </c>
       <c r="G44" t="n">
-        <v>-4.96462</v>
+        <v>-4.6736</v>
       </c>
     </row>
     <row r="45">
@@ -1646,16 +1646,16 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.090392</v>
+        <v>0.090447</v>
       </c>
       <c r="E45" t="n">
-        <v>1035804037</v>
+        <v>1035950281</v>
       </c>
       <c r="F45" t="n">
-        <v>42196</v>
+        <v>42037</v>
       </c>
       <c r="G45" t="n">
-        <v>-0.1326</v>
+        <v>-0.07207</v>
       </c>
     </row>
     <row r="46">
@@ -1673,16 +1673,16 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>1.001</v>
+        <v>0.999682</v>
       </c>
       <c r="E46" t="n">
-        <v>1019461270</v>
+        <v>1018676333</v>
       </c>
       <c r="F46" t="n">
-        <v>22115197</v>
+        <v>22087066</v>
       </c>
       <c r="G46" t="n">
-        <v>0.1549</v>
+        <v>0.03234</v>
       </c>
     </row>
     <row r="47">
@@ -1700,16 +1700,16 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.998927</v>
+        <v>0.998424</v>
       </c>
       <c r="E47" t="n">
-        <v>1003070946</v>
+        <v>1002536398</v>
       </c>
       <c r="F47" t="n">
-        <v>10675084</v>
+        <v>10677254</v>
       </c>
       <c r="G47" t="n">
-        <v>-0.12097</v>
+        <v>-0.14811</v>
       </c>
     </row>
     <row r="48">
@@ -1727,16 +1727,16 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.99932</v>
+        <v>0.99992</v>
       </c>
       <c r="E48" t="n">
-        <v>999981890</v>
+        <v>999871469</v>
       </c>
       <c r="F48" t="n">
-        <v>5646326</v>
+        <v>5649721</v>
       </c>
       <c r="G48" t="n">
-        <v>-0.08477999999999999</v>
+        <v>0.02404</v>
       </c>
     </row>
     <row r="49">
@@ -1757,13 +1757,13 @@
         <v>2.66</v>
       </c>
       <c r="E49" t="n">
-        <v>973002247</v>
+        <v>973789506</v>
       </c>
       <c r="F49" t="n">
-        <v>202350662</v>
+        <v>201810285</v>
       </c>
       <c r="G49" t="n">
-        <v>-0.82078</v>
+        <v>-0.68514</v>
       </c>
     </row>
     <row r="50">
@@ -1781,16 +1781,16 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.839062</v>
+        <v>0.840215</v>
       </c>
       <c r="E50" t="n">
-        <v>927967352</v>
+        <v>928634104</v>
       </c>
       <c r="F50" t="n">
-        <v>98125654</v>
+        <v>97822860</v>
       </c>
       <c r="G50" t="n">
-        <v>-2.78818</v>
+        <v>-2.53788</v>
       </c>
     </row>
     <row r="51">
@@ -1808,16 +1808,16 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.331278</v>
+        <v>0.331162</v>
       </c>
       <c r="E51" t="n">
-        <v>925804138</v>
+        <v>924344807</v>
       </c>
       <c r="F51" t="n">
-        <v>271444156</v>
+        <v>273297270</v>
       </c>
       <c r="G51" t="n">
-        <v>-9.085050000000001</v>
+        <v>-9.07572</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-05-25
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>26246</v>
+        <v>26461</v>
       </c>
       <c r="E2" t="n">
-        <v>508651137805</v>
+        <v>512841095632</v>
       </c>
       <c r="F2" t="n">
-        <v>12720808274</v>
+        <v>15295281760</v>
       </c>
       <c r="G2" t="n">
-        <v>-1.76866</v>
+        <v>0.36016</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1786.26</v>
+        <v>1808.22</v>
       </c>
       <c r="E3" t="n">
-        <v>214795011006</v>
+        <v>217310665995</v>
       </c>
       <c r="F3" t="n">
-        <v>7994613865</v>
+        <v>7560810565</v>
       </c>
       <c r="G3" t="n">
-        <v>-1.57191</v>
+        <v>0.39102</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999668</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>83035543148</v>
+        <v>83048716680</v>
       </c>
       <c r="F4" t="n">
-        <v>11364774577</v>
+        <v>16986580668</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.014</v>
+        <v>0.01672</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>305.25</v>
+        <v>304.59</v>
       </c>
       <c r="E5" t="n">
-        <v>48190868223</v>
+        <v>48093350164</v>
       </c>
       <c r="F5" t="n">
-        <v>578175260</v>
+        <v>552148251</v>
       </c>
       <c r="G5" t="n">
-        <v>-1.0407</v>
+        <v>-0.34153</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.999791</v>
+        <v>0.999893</v>
       </c>
       <c r="E6" t="n">
-        <v>29139114605</v>
+        <v>29046812679</v>
       </c>
       <c r="F6" t="n">
-        <v>4422671061</v>
+        <v>4146045655</v>
       </c>
       <c r="G6" t="n">
-        <v>0.01192</v>
+        <v>0.00342</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.449777</v>
+        <v>0.453827</v>
       </c>
       <c r="E7" t="n">
-        <v>23331434768</v>
+        <v>23510158592</v>
       </c>
       <c r="F7" t="n">
-        <v>981032480</v>
+        <v>823922217</v>
       </c>
       <c r="G7" t="n">
-        <v>-1.13473</v>
+        <v>-0.0319</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.358459</v>
+        <v>0.358416</v>
       </c>
       <c r="E8" t="n">
-        <v>12559009537</v>
+        <v>12548450887</v>
       </c>
       <c r="F8" t="n">
-        <v>188107859</v>
+        <v>173579966</v>
       </c>
       <c r="G8" t="n">
-        <v>-2.16766</v>
+        <v>-1.6919</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1786.38</v>
+        <v>1804.89</v>
       </c>
       <c r="E9" t="n">
-        <v>11933799690</v>
+        <v>12079944766</v>
       </c>
       <c r="F9" t="n">
-        <v>6341007</v>
+        <v>7261597</v>
       </c>
       <c r="G9" t="n">
-        <v>-1.55409</v>
+        <v>0.25163</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.07051200000000001</v>
+        <v>0.07091</v>
       </c>
       <c r="E10" t="n">
-        <v>9834328513</v>
+        <v>9884459453</v>
       </c>
       <c r="F10" t="n">
-        <v>319378609</v>
+        <v>277203003</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.98998</v>
+        <v>-0.04145</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.879999</v>
+        <v>0.888668</v>
       </c>
       <c r="E11" t="n">
-        <v>8165875706</v>
+        <v>8241486339</v>
       </c>
       <c r="F11" t="n">
-        <v>273457737</v>
+        <v>293209644</v>
       </c>
       <c r="G11" t="n">
-        <v>1.4245</v>
+        <v>1.73392</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>19.38</v>
+        <v>19.24</v>
       </c>
       <c r="E12" t="n">
-        <v>7679062151</v>
+        <v>7618113002</v>
       </c>
       <c r="F12" t="n">
-        <v>317061278</v>
+        <v>235056524</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.31761</v>
+        <v>-0.08337</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.076931</v>
+        <v>0.076998</v>
       </c>
       <c r="E13" t="n">
-        <v>6949087312</v>
+        <v>6962525507</v>
       </c>
       <c r="F13" t="n">
-        <v>378698318</v>
+        <v>363493525</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.11061</v>
+        <v>-0.27074</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>5.26</v>
+        <v>5.25</v>
       </c>
       <c r="E14" t="n">
-        <v>6497035154</v>
+        <v>6481987436</v>
       </c>
       <c r="F14" t="n">
-        <v>114230940</v>
+        <v>108728990</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.44806</v>
+        <v>-0.2123</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>84.66</v>
+        <v>85.62</v>
       </c>
       <c r="E15" t="n">
-        <v>6180025165</v>
+        <v>6242787836</v>
       </c>
       <c r="F15" t="n">
-        <v>699249828</v>
+        <v>630622046</v>
       </c>
       <c r="G15" t="n">
-        <v>-1.86552</v>
+        <v>-0.24829</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.999369</v>
+        <v>0.999919</v>
       </c>
       <c r="E16" t="n">
-        <v>5328539103</v>
+        <v>5301038364</v>
       </c>
       <c r="F16" t="n">
-        <v>892788552</v>
+        <v>1656697773</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.05377</v>
+        <v>-0.04618</v>
       </c>
     </row>
     <row r="17">
@@ -893,13 +893,13 @@
         <v>8.5e-06</v>
       </c>
       <c r="E17" t="n">
-        <v>5010186027</v>
+        <v>5004629257</v>
       </c>
       <c r="F17" t="n">
-        <v>134264488</v>
+        <v>131936290</v>
       </c>
       <c r="G17" t="n">
-        <v>-1.82902</v>
+        <v>-0.58525</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>14.17</v>
+        <v>14.08</v>
       </c>
       <c r="E18" t="n">
-        <v>4741535725</v>
+        <v>4709807307</v>
       </c>
       <c r="F18" t="n">
-        <v>146564796</v>
+        <v>148626546</v>
       </c>
       <c r="G18" t="n">
-        <v>-1.1871</v>
+        <v>-0.38017</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.9994499999999999</v>
+        <v>1</v>
       </c>
       <c r="E19" t="n">
-        <v>4619488637</v>
+        <v>4621598349</v>
       </c>
       <c r="F19" t="n">
-        <v>115300383</v>
+        <v>93803370</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.07179000000000001</v>
+        <v>-0.01675</v>
       </c>
     </row>
     <row r="20">
@@ -971,16 +971,16 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>26240</v>
+        <v>26525</v>
       </c>
       <c r="E20" t="n">
-        <v>4094655644</v>
+        <v>4130404968</v>
       </c>
       <c r="F20" t="n">
-        <v>100633195</v>
+        <v>81162016</v>
       </c>
       <c r="G20" t="n">
-        <v>-1.96386</v>
+        <v>0.43469</v>
       </c>
     </row>
     <row r="21">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>4.95</v>
+        <v>4.93</v>
       </c>
       <c r="E21" t="n">
-        <v>3729971944</v>
+        <v>3714508265</v>
       </c>
       <c r="F21" t="n">
-        <v>42911387</v>
+        <v>35825947</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.41403</v>
+        <v>-0.81306</v>
       </c>
     </row>
     <row r="22">
@@ -1025,16 +1025,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>3.54</v>
+        <v>3.55</v>
       </c>
       <c r="E22" t="n">
-        <v>3295918708</v>
+        <v>3312230830</v>
       </c>
       <c r="F22" t="n">
-        <v>259380</v>
+        <v>211734</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.2005</v>
+        <v>0.1712</v>
       </c>
     </row>
     <row r="23">
@@ -1052,16 +1052,16 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>6.3</v>
+        <v>6.28</v>
       </c>
       <c r="E23" t="n">
-        <v>3257387402</v>
+        <v>3245978583</v>
       </c>
       <c r="F23" t="n">
-        <v>147734860</v>
+        <v>121588303</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.55915</v>
+        <v>-0.77695</v>
       </c>
     </row>
     <row r="24">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>10.49</v>
+        <v>10.47</v>
       </c>
       <c r="E24" t="n">
-        <v>3068497349</v>
+        <v>3059269614</v>
       </c>
       <c r="F24" t="n">
-        <v>81696415</v>
+        <v>73757240</v>
       </c>
       <c r="G24" t="n">
-        <v>1.12991</v>
+        <v>0.68104</v>
       </c>
     </row>
     <row r="25">
@@ -1106,16 +1106,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>1.96</v>
+        <v>1.92</v>
       </c>
       <c r="E25" t="n">
-        <v>2892942786</v>
+        <v>2834567330</v>
       </c>
       <c r="F25" t="n">
-        <v>9497086</v>
+        <v>9350678</v>
       </c>
       <c r="G25" t="n">
-        <v>-1.36413</v>
+        <v>-2.45678</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>45.77</v>
+        <v>46.21</v>
       </c>
       <c r="E26" t="n">
-        <v>2746484034</v>
+        <v>2772979836</v>
       </c>
       <c r="F26" t="n">
-        <v>17702883</v>
+        <v>16865532</v>
       </c>
       <c r="G26" t="n">
-        <v>0.6091</v>
+        <v>3.28009</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>150.2</v>
+        <v>151.49</v>
       </c>
       <c r="E27" t="n">
-        <v>2725915387</v>
+        <v>2749238679</v>
       </c>
       <c r="F27" t="n">
-        <v>74143150</v>
+        <v>77370081</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.2264</v>
+        <v>0.52234</v>
       </c>
     </row>
     <row r="28">
@@ -1187,16 +1187,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>17.72</v>
+        <v>17.71</v>
       </c>
       <c r="E28" t="n">
-        <v>2500113483</v>
+        <v>2498819995</v>
       </c>
       <c r="F28" t="n">
-        <v>79688238</v>
+        <v>77224810</v>
       </c>
       <c r="G28" t="n">
-        <v>-1.43889</v>
+        <v>-0.57694</v>
       </c>
     </row>
     <row r="29">
@@ -1214,16 +1214,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.086572</v>
+        <v>0.086969</v>
       </c>
       <c r="E29" t="n">
-        <v>2319601754</v>
+        <v>2329514531</v>
       </c>
       <c r="F29" t="n">
-        <v>37458597</v>
+        <v>32556750</v>
       </c>
       <c r="G29" t="n">
-        <v>-1.00989</v>
+        <v>0.54269</v>
       </c>
     </row>
     <row r="30">
@@ -1241,16 +1241,16 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>111.36</v>
+        <v>111.96</v>
       </c>
       <c r="E30" t="n">
-        <v>2160256423</v>
+        <v>2170058440</v>
       </c>
       <c r="F30" t="n">
-        <v>64122310</v>
+        <v>57106195</v>
       </c>
       <c r="G30" t="n">
-        <v>-1.19812</v>
+        <v>-0.20418</v>
       </c>
     </row>
     <row r="31">
@@ -1268,16 +1268,16 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>4.83</v>
+        <v>4.8</v>
       </c>
       <c r="E31" t="n">
-        <v>2108618261</v>
+        <v>2096632017</v>
       </c>
       <c r="F31" t="n">
-        <v>27392235</v>
+        <v>23885608</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.71545</v>
+        <v>-0.5946</v>
       </c>
     </row>
     <row r="32">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.998984</v>
+        <v>0.999465</v>
       </c>
       <c r="E32" t="n">
-        <v>2039372932</v>
+        <v>2039836347</v>
       </c>
       <c r="F32" t="n">
-        <v>229971268</v>
+        <v>201366363</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.05835</v>
+        <v>-0.03849</v>
       </c>
     </row>
     <row r="33">
@@ -1325,13 +1325,13 @@
         <v>4.42</v>
       </c>
       <c r="E33" t="n">
-        <v>1884847002</v>
+        <v>1881920092</v>
       </c>
       <c r="F33" t="n">
-        <v>106364488</v>
+        <v>87034526</v>
       </c>
       <c r="G33" t="n">
-        <v>-0.69317</v>
+        <v>-1.33831</v>
       </c>
     </row>
     <row r="34">
@@ -1352,13 +1352,13 @@
         <v>2.01</v>
       </c>
       <c r="E34" t="n">
-        <v>1767636958</v>
+        <v>1772048288</v>
       </c>
       <c r="F34" t="n">
-        <v>69920817</v>
+        <v>59205327</v>
       </c>
       <c r="G34" t="n">
-        <v>3.50528</v>
+        <v>-1.63658</v>
       </c>
     </row>
     <row r="35">
@@ -1376,16 +1376,16 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.05093</v>
+        <v>0.050879</v>
       </c>
       <c r="E35" t="n">
-        <v>1602164396</v>
+        <v>1599809380</v>
       </c>
       <c r="F35" t="n">
-        <v>18584925</v>
+        <v>16274494</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.47809</v>
+        <v>-0.375</v>
       </c>
     </row>
     <row r="36">
@@ -1403,16 +1403,16 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>7.96</v>
+        <v>8</v>
       </c>
       <c r="E36" t="n">
-        <v>1574192780</v>
+        <v>1585958487</v>
       </c>
       <c r="F36" t="n">
-        <v>57862140</v>
+        <v>40217056</v>
       </c>
       <c r="G36" t="n">
-        <v>-3.45608</v>
+        <v>-1.38525</v>
       </c>
     </row>
     <row r="37">
@@ -1430,16 +1430,16 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.05952</v>
+        <v>0.059887</v>
       </c>
       <c r="E37" t="n">
-        <v>1503300016</v>
+        <v>1512482196</v>
       </c>
       <c r="F37" t="n">
-        <v>6964416</v>
+        <v>5287148</v>
       </c>
       <c r="G37" t="n">
-        <v>-2.37218</v>
+        <v>-0.28133</v>
       </c>
     </row>
     <row r="38">
@@ -1457,16 +1457,16 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>100.52</v>
+        <v>98.53</v>
       </c>
       <c r="E38" t="n">
-        <v>1461997034</v>
+        <v>1435538827</v>
       </c>
       <c r="F38" t="n">
-        <v>18642127</v>
+        <v>17980109</v>
       </c>
       <c r="G38" t="n">
-        <v>-0.34002</v>
+        <v>-1.7878</v>
       </c>
     </row>
     <row r="39">
@@ -1484,16 +1484,16 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1.57</v>
+        <v>1.56</v>
       </c>
       <c r="E39" t="n">
-        <v>1422412621</v>
+        <v>1423951244</v>
       </c>
       <c r="F39" t="n">
-        <v>61892680</v>
+        <v>58596041</v>
       </c>
       <c r="G39" t="n">
-        <v>-2.09682</v>
+        <v>-1.46816</v>
       </c>
     </row>
     <row r="40">
@@ -1511,16 +1511,16 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1.097</v>
+        <v>1.11</v>
       </c>
       <c r="E40" t="n">
-        <v>1398339893</v>
+        <v>1410811743</v>
       </c>
       <c r="F40" t="n">
-        <v>193330839</v>
+        <v>168047151</v>
       </c>
       <c r="G40" t="n">
-        <v>-2.40285</v>
+        <v>-0.66332</v>
       </c>
     </row>
     <row r="41">
@@ -1538,16 +1538,16 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.01920309</v>
+        <v>0.01929719</v>
       </c>
       <c r="E41" t="n">
-        <v>1396343655</v>
+        <v>1402060808</v>
       </c>
       <c r="F41" t="n">
-        <v>41654056</v>
+        <v>38562861</v>
       </c>
       <c r="G41" t="n">
-        <v>-0.61902</v>
+        <v>-0.49899</v>
       </c>
     </row>
     <row r="42">
@@ -1568,13 +1568,13 @@
         <v>3.23</v>
       </c>
       <c r="E42" t="n">
-        <v>1191327672</v>
+        <v>1191675051</v>
       </c>
       <c r="F42" t="n">
-        <v>76499741</v>
+        <v>64886397</v>
       </c>
       <c r="G42" t="n">
-        <v>-7.1245</v>
+        <v>-3.33958</v>
       </c>
     </row>
     <row r="43">
@@ -1592,16 +1592,16 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.152085</v>
+        <v>0.150811</v>
       </c>
       <c r="E43" t="n">
-        <v>1101157862</v>
+        <v>1092287208</v>
       </c>
       <c r="F43" t="n">
-        <v>65376388</v>
+        <v>65603081</v>
       </c>
       <c r="G43" t="n">
-        <v>-4.41471</v>
+        <v>-3.19802</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>GGTKN</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>GGTKN</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.09180000000000001</v>
+        <v>0.116712</v>
       </c>
       <c r="E44" t="n">
-        <v>1051448132</v>
+        <v>1048598196</v>
       </c>
       <c r="F44" t="n">
-        <v>42354</v>
+        <v>31429935</v>
       </c>
       <c r="G44" t="n">
-        <v>1.45596</v>
+        <v>0.18855</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>GGTKN</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>GGTKN</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.11483</v>
+        <v>0.092044</v>
       </c>
       <c r="E45" t="n">
-        <v>1032296257</v>
+        <v>1046827992</v>
       </c>
       <c r="F45" t="n">
-        <v>35898785</v>
+        <v>68601</v>
       </c>
       <c r="G45" t="n">
-        <v>-2.29843</v>
+        <v>1.74621</v>
       </c>
     </row>
     <row r="46">
@@ -1673,16 +1673,16 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.999459</v>
+        <v>1</v>
       </c>
       <c r="E46" t="n">
-        <v>1018501569</v>
+        <v>1018951360</v>
       </c>
       <c r="F46" t="n">
-        <v>33245566</v>
+        <v>28000680</v>
       </c>
       <c r="G46" t="n">
-        <v>0.0535</v>
+        <v>0.08774999999999999</v>
       </c>
     </row>
     <row r="47">
@@ -1700,70 +1700,70 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.999061</v>
+        <v>0.9989980000000001</v>
       </c>
       <c r="E47" t="n">
-        <v>1002452182</v>
+        <v>1003047199</v>
       </c>
       <c r="F47" t="n">
-        <v>14549333</v>
+        <v>15735583</v>
       </c>
       <c r="G47" t="n">
-        <v>-0.02456</v>
+        <v>0.0129</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>EDGT</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>Edgecoin</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>2.73</v>
+        <v>0.999876</v>
       </c>
       <c r="E48" t="n">
-        <v>1001820269</v>
+        <v>999907301</v>
       </c>
       <c r="F48" t="n">
-        <v>203566738</v>
+        <v>5367459</v>
       </c>
       <c r="G48" t="n">
-        <v>8.78487</v>
+        <v>-0.01041</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>EDGT</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Edgecoin</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.999669</v>
+        <v>2.71</v>
       </c>
       <c r="E49" t="n">
-        <v>999668615</v>
+        <v>991826838</v>
       </c>
       <c r="F49" t="n">
-        <v>5660781</v>
+        <v>223721046</v>
       </c>
       <c r="G49" t="n">
-        <v>-0.05019</v>
+        <v>1.8508</v>
       </c>
     </row>
     <row r="50">
@@ -1781,16 +1781,16 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.503916</v>
+        <v>0.509141</v>
       </c>
       <c r="E50" t="n">
-        <v>934053164</v>
+        <v>944138838</v>
       </c>
       <c r="F50" t="n">
-        <v>166029858</v>
+        <v>174435070</v>
       </c>
       <c r="G50" t="n">
-        <v>1.91121</v>
+        <v>1.97515</v>
       </c>
     </row>
     <row r="51">
@@ -1808,16 +1808,16 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.839548</v>
+        <v>0.84457</v>
       </c>
       <c r="E51" t="n">
-        <v>928136713</v>
+        <v>932574554</v>
       </c>
       <c r="F51" t="n">
-        <v>94917017</v>
+        <v>84661316</v>
       </c>
       <c r="G51" t="n">
-        <v>-0.72263</v>
+        <v>0.59019</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-05-28
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>26468</v>
+        <v>27180</v>
       </c>
       <c r="E2" t="n">
-        <v>512903223779</v>
+        <v>526852941206</v>
       </c>
       <c r="F2" t="n">
-        <v>7126326631</v>
+        <v>8667506335</v>
       </c>
       <c r="G2" t="n">
-        <v>0.36415</v>
+        <v>1.8148</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1808.34</v>
+        <v>1844.81</v>
       </c>
       <c r="E3" t="n">
-        <v>217450894711</v>
+        <v>221888062436</v>
       </c>
       <c r="F3" t="n">
-        <v>7524970555</v>
+        <v>5071649253</v>
       </c>
       <c r="G3" t="n">
-        <v>0.41</v>
+        <v>1.01581</v>
       </c>
     </row>
     <row r="4">
@@ -542,13 +542,13 @@
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>83043328337</v>
+        <v>83183082920</v>
       </c>
       <c r="F4" t="n">
-        <v>11334795825</v>
+        <v>10097627538</v>
       </c>
       <c r="G4" t="n">
-        <v>0.06443</v>
+        <v>0.0265</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>304.6</v>
+        <v>307.77</v>
       </c>
       <c r="E5" t="n">
-        <v>48090100899</v>
+        <v>48593813452</v>
       </c>
       <c r="F5" t="n">
-        <v>551217400</v>
+        <v>352236282</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.49312</v>
+        <v>0.87645</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.999892</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>29054489055</v>
+        <v>29065878683</v>
       </c>
       <c r="F6" t="n">
-        <v>3737060407</v>
+        <v>2553878021</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.11316</v>
+        <v>0.05116</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.453731</v>
+        <v>0.473614</v>
       </c>
       <c r="E7" t="n">
-        <v>23537286259</v>
+        <v>24621218448</v>
       </c>
       <c r="F7" t="n">
-        <v>824227008</v>
+        <v>558512875</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.02674</v>
+        <v>0.11697</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.358471</v>
+        <v>0.377697</v>
       </c>
       <c r="E8" t="n">
-        <v>12560534006</v>
+        <v>13211077752</v>
       </c>
       <c r="F8" t="n">
-        <v>173699781</v>
+        <v>187788242</v>
       </c>
       <c r="G8" t="n">
-        <v>-1.70864</v>
+        <v>3.79064</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1806.75</v>
+        <v>1843.19</v>
       </c>
       <c r="E9" t="n">
-        <v>12083645961</v>
+        <v>12548372047</v>
       </c>
       <c r="F9" t="n">
-        <v>7192764</v>
+        <v>10740432</v>
       </c>
       <c r="G9" t="n">
-        <v>0.26433</v>
+        <v>1.00286</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.07094</v>
+        <v>0.072585</v>
       </c>
       <c r="E10" t="n">
-        <v>9892292213</v>
+        <v>10128637043</v>
       </c>
       <c r="F10" t="n">
-        <v>277282380</v>
+        <v>227747667</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.2264</v>
+        <v>1.51491</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.888933</v>
+        <v>0.925192</v>
       </c>
       <c r="E11" t="n">
-        <v>8246329628</v>
+        <v>8582552872</v>
       </c>
       <c r="F11" t="n">
-        <v>293156893</v>
+        <v>190630066</v>
       </c>
       <c r="G11" t="n">
-        <v>1.58333</v>
+        <v>0.71227</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>19.25</v>
+        <v>20.54</v>
       </c>
       <c r="E12" t="n">
-        <v>7623017389</v>
+        <v>8146994638</v>
       </c>
       <c r="F12" t="n">
-        <v>235275661</v>
+        <v>284877172</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.12426</v>
+        <v>5.46737</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.076961</v>
+        <v>0.07727199999999999</v>
       </c>
       <c r="E13" t="n">
-        <v>6951799441</v>
+        <v>6978638437</v>
       </c>
       <c r="F13" t="n">
-        <v>364631544</v>
+        <v>298682212</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.23385</v>
+        <v>1.13409</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>5.24</v>
+        <v>5.38</v>
       </c>
       <c r="E14" t="n">
-        <v>6482169999</v>
+        <v>6652714960</v>
       </c>
       <c r="F14" t="n">
-        <v>108562153</v>
+        <v>97747265</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.40531</v>
+        <v>1.75418</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>85.54000000000001</v>
+        <v>89.39</v>
       </c>
       <c r="E15" t="n">
-        <v>6247949254</v>
+        <v>6527311005</v>
       </c>
       <c r="F15" t="n">
-        <v>632241522</v>
+        <v>490963046</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.44344</v>
+        <v>1.70598</v>
       </c>
     </row>
     <row r="16">
@@ -866,13 +866,13 @@
         <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>5302793567</v>
+        <v>5277206928</v>
       </c>
       <c r="F16" t="n">
-        <v>1509861258</v>
+        <v>622775759</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.06693</v>
+        <v>0.01033</v>
       </c>
     </row>
     <row r="17">
@@ -890,16 +890,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>8.51e-06</v>
+        <v>8.760000000000001e-06</v>
       </c>
       <c r="E17" t="n">
-        <v>5010898637</v>
+        <v>5159141059</v>
       </c>
       <c r="F17" t="n">
-        <v>132071460</v>
+        <v>119342926</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.56887</v>
+        <v>2.01765</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>14.09</v>
+        <v>14.51</v>
       </c>
       <c r="E18" t="n">
-        <v>4711229912</v>
+        <v>4859707120</v>
       </c>
       <c r="F18" t="n">
-        <v>148802188</v>
+        <v>148658812</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.48773</v>
+        <v>1.46754</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.99991</v>
+        <v>1</v>
       </c>
       <c r="E19" t="n">
-        <v>4621833351</v>
+        <v>4624210174</v>
       </c>
       <c r="F19" t="n">
-        <v>94486427</v>
+        <v>71877577</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.07106999999999999</v>
+        <v>0.06035</v>
       </c>
     </row>
     <row r="20">
@@ -971,16 +971,16 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>26537</v>
+        <v>27213</v>
       </c>
       <c r="E20" t="n">
-        <v>4138886776</v>
+        <v>4255248233</v>
       </c>
       <c r="F20" t="n">
-        <v>81966498</v>
+        <v>70526774</v>
       </c>
       <c r="G20" t="n">
-        <v>0.35829</v>
+        <v>1.89795</v>
       </c>
     </row>
     <row r="21">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>4.94</v>
+        <v>5.06</v>
       </c>
       <c r="E21" t="n">
-        <v>3718359137</v>
+        <v>3815039075</v>
       </c>
       <c r="F21" t="n">
-        <v>35995431</v>
+        <v>30997250</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.72487</v>
+        <v>0.9680299999999999</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>3.55</v>
+        <v>6.49</v>
       </c>
       <c r="E22" t="n">
-        <v>3308003035</v>
+        <v>3355324273</v>
       </c>
       <c r="F22" t="n">
-        <v>211594</v>
+        <v>111388150</v>
       </c>
       <c r="G22" t="n">
-        <v>0.23301</v>
+        <v>1.83646</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>6.28</v>
+        <v>3.5</v>
       </c>
       <c r="E23" t="n">
-        <v>3246793498</v>
+        <v>3256793600</v>
       </c>
       <c r="F23" t="n">
-        <v>121205122</v>
+        <v>222266</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.93057</v>
+        <v>-0.14511</v>
       </c>
     </row>
     <row r="24">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>10.47</v>
+        <v>10.61</v>
       </c>
       <c r="E24" t="n">
-        <v>3062642730</v>
+        <v>3103750673</v>
       </c>
       <c r="F24" t="n">
-        <v>73716403</v>
+        <v>64389617</v>
       </c>
       <c r="G24" t="n">
-        <v>0.57355</v>
+        <v>0.81974</v>
       </c>
     </row>
     <row r="25">
@@ -1106,16 +1106,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>1.92</v>
+        <v>1.93</v>
       </c>
       <c r="E25" t="n">
-        <v>2823586431</v>
+        <v>2838382699</v>
       </c>
       <c r="F25" t="n">
-        <v>8108704</v>
+        <v>9825775</v>
       </c>
       <c r="G25" t="n">
-        <v>-2.64663</v>
+        <v>1.17334</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>46.15</v>
+        <v>46.94</v>
       </c>
       <c r="E26" t="n">
-        <v>2772085020</v>
+        <v>2818922203</v>
       </c>
       <c r="F26" t="n">
-        <v>16856007</v>
+        <v>5520461</v>
       </c>
       <c r="G26" t="n">
-        <v>2.98342</v>
+        <v>0.81464</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>151.5</v>
+        <v>153.98</v>
       </c>
       <c r="E27" t="n">
-        <v>2749388901</v>
+        <v>2793570405</v>
       </c>
       <c r="F27" t="n">
-        <v>75473165</v>
+        <v>60314969</v>
       </c>
       <c r="G27" t="n">
-        <v>0.53229</v>
+        <v>1.89621</v>
       </c>
     </row>
     <row r="28">
@@ -1187,16 +1187,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>17.71</v>
+        <v>18.26</v>
       </c>
       <c r="E28" t="n">
-        <v>2499127273</v>
+        <v>2578711360</v>
       </c>
       <c r="F28" t="n">
-        <v>70673575</v>
+        <v>54302180</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.59949</v>
+        <v>1.51748</v>
       </c>
     </row>
     <row r="29">
@@ -1214,16 +1214,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.086981</v>
+        <v>0.08820500000000001</v>
       </c>
       <c r="E29" t="n">
-        <v>2331041613</v>
+        <v>2364172625</v>
       </c>
       <c r="F29" t="n">
-        <v>32596627</v>
+        <v>28628415</v>
       </c>
       <c r="G29" t="n">
-        <v>0.5602200000000001</v>
+        <v>0.34923</v>
       </c>
     </row>
     <row r="30">
@@ -1241,16 +1241,16 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>111.92</v>
+        <v>114.1</v>
       </c>
       <c r="E30" t="n">
-        <v>2172073269</v>
+        <v>2214246094</v>
       </c>
       <c r="F30" t="n">
-        <v>56907987</v>
+        <v>49114846</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.37054</v>
+        <v>1.12935</v>
       </c>
     </row>
     <row r="31">
@@ -1268,16 +1268,16 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>4.8</v>
+        <v>4.9</v>
       </c>
       <c r="E31" t="n">
-        <v>2095066658</v>
+        <v>2139754119</v>
       </c>
       <c r="F31" t="n">
-        <v>23939677</v>
+        <v>25716249</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.67116</v>
+        <v>-0.29036</v>
       </c>
     </row>
     <row r="32">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.999327</v>
+        <v>1</v>
       </c>
       <c r="E32" t="n">
-        <v>2040783273</v>
+        <v>2042403768</v>
       </c>
       <c r="F32" t="n">
-        <v>201451772</v>
+        <v>126444430</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.15587</v>
+        <v>0.00991</v>
       </c>
     </row>
     <row r="33">
@@ -1322,16 +1322,16 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>4.41</v>
+        <v>4.55</v>
       </c>
       <c r="E33" t="n">
-        <v>1882967344</v>
+        <v>1941800345</v>
       </c>
       <c r="F33" t="n">
-        <v>86976904</v>
+        <v>84534240</v>
       </c>
       <c r="G33" t="n">
-        <v>-1.5852</v>
+        <v>2.43392</v>
       </c>
     </row>
     <row r="34">
@@ -1349,16 +1349,16 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>2.01</v>
+        <v>1.99</v>
       </c>
       <c r="E34" t="n">
-        <v>1771653517</v>
+        <v>1753385583</v>
       </c>
       <c r="F34" t="n">
-        <v>58775625</v>
+        <v>25707531</v>
       </c>
       <c r="G34" t="n">
-        <v>-1.83161</v>
+        <v>0.50071</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.050867</v>
+        <v>8.529999999999999</v>
       </c>
       <c r="E35" t="n">
-        <v>1600267163</v>
+        <v>1694769748</v>
       </c>
       <c r="F35" t="n">
-        <v>16283866</v>
+        <v>52444768</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.47853</v>
+        <v>4.94522</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>8</v>
+        <v>0.052486</v>
       </c>
       <c r="E36" t="n">
-        <v>1585039158</v>
+        <v>1650616962</v>
       </c>
       <c r="F36" t="n">
-        <v>40303449</v>
+        <v>14114343</v>
       </c>
       <c r="G36" t="n">
-        <v>-1.48674</v>
+        <v>0.40534</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.059875</v>
+        <v>1.2</v>
       </c>
       <c r="E37" t="n">
-        <v>1512806160</v>
+        <v>1530708979</v>
       </c>
       <c r="F37" t="n">
-        <v>5291641</v>
+        <v>172860255</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.33828</v>
+        <v>3.57423</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>98.54000000000001</v>
+        <v>0.060415</v>
       </c>
       <c r="E38" t="n">
-        <v>1432057912</v>
+        <v>1527615455</v>
       </c>
       <c r="F38" t="n">
-        <v>18021819</v>
+        <v>4052824</v>
       </c>
       <c r="G38" t="n">
-        <v>-2.01079</v>
+        <v>0.35607</v>
       </c>
     </row>
     <row r="39">
@@ -1484,16 +1484,16 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1.56</v>
+        <v>1.65</v>
       </c>
       <c r="E39" t="n">
-        <v>1414516098</v>
+        <v>1497669006</v>
       </c>
       <c r="F39" t="n">
-        <v>58764707</v>
+        <v>49544388</v>
       </c>
       <c r="G39" t="n">
-        <v>-1.67306</v>
+        <v>3.15467</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1.11</v>
+        <v>102.04</v>
       </c>
       <c r="E40" t="n">
-        <v>1410788169</v>
+        <v>1484107837</v>
       </c>
       <c r="F40" t="n">
-        <v>167307036</v>
+        <v>11509495</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.72015</v>
+        <v>1.12492</v>
       </c>
     </row>
     <row r="41">
@@ -1538,16 +1538,16 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.01930521</v>
+        <v>0.02026755</v>
       </c>
       <c r="E41" t="n">
-        <v>1403540620</v>
+        <v>1473567429</v>
       </c>
       <c r="F41" t="n">
-        <v>38554262</v>
+        <v>56168694</v>
       </c>
       <c r="G41" t="n">
-        <v>-0.51497</v>
+        <v>4.76231</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>APE</t>
+          <t>GGTKN</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>ApeCoin</t>
+          <t>GGTKN</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>3.23</v>
+        <v>0.107808</v>
       </c>
       <c r="E42" t="n">
-        <v>1191680697</v>
+        <v>1232509808</v>
       </c>
       <c r="F42" t="n">
-        <v>63347754</v>
+        <v>147538</v>
       </c>
       <c r="G42" t="n">
-        <v>-3.55297</v>
+        <v>-5.96282</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ALGO</t>
+          <t>APE</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Algorand</t>
+          <t>ApeCoin</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.150737</v>
+        <v>3.25</v>
       </c>
       <c r="E43" t="n">
-        <v>1092161362</v>
+        <v>1196806518</v>
       </c>
       <c r="F43" t="n">
-        <v>65689689</v>
+        <v>46191481</v>
       </c>
       <c r="G43" t="n">
-        <v>-3.27491</v>
+        <v>1.23095</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>GGTKN</t>
+          <t>ALGO</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>GGTKN</t>
+          <t>Algorand</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.09175899999999999</v>
+        <v>0.151985</v>
       </c>
       <c r="E44" t="n">
-        <v>1054238259</v>
+        <v>1101296014</v>
       </c>
       <c r="F44" t="n">
-        <v>68561</v>
+        <v>41182698</v>
       </c>
       <c r="G44" t="n">
-        <v>1.4648</v>
+        <v>0.91753</v>
       </c>
     </row>
     <row r="45">
@@ -1646,16 +1646,16 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.116756</v>
+        <v>0.120578</v>
       </c>
       <c r="E45" t="n">
-        <v>1049367196</v>
+        <v>1084465174</v>
       </c>
       <c r="F45" t="n">
-        <v>31441752</v>
+        <v>31214651</v>
       </c>
       <c r="G45" t="n">
-        <v>0.2163</v>
+        <v>0.72404</v>
       </c>
     </row>
     <row r="46">
@@ -1673,16 +1673,16 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.999765</v>
+        <v>0.999923</v>
       </c>
       <c r="E46" t="n">
-        <v>1018788196</v>
+        <v>1019308375</v>
       </c>
       <c r="F46" t="n">
-        <v>27999688</v>
+        <v>25629773</v>
       </c>
       <c r="G46" t="n">
-        <v>-0.05818</v>
+        <v>0.03651</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>FRAX</t>
+          <t>SAND</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Frax</t>
+          <t>The Sandbox</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.9993649999999999</v>
+        <v>0.548387</v>
       </c>
       <c r="E47" t="n">
-        <v>1003111312</v>
+        <v>1011806792</v>
       </c>
       <c r="F47" t="n">
-        <v>15645282</v>
+        <v>153030235</v>
       </c>
       <c r="G47" t="n">
-        <v>-0.09135</v>
+        <v>5.65614</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>EDGT</t>
+          <t>EOS</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Edgecoin</t>
+          <t>EOS</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.999676</v>
+        <v>0.906998</v>
       </c>
       <c r="E48" t="n">
-        <v>999875549</v>
+        <v>1003975901</v>
       </c>
       <c r="F48" t="n">
-        <v>5368823</v>
+        <v>112917761</v>
       </c>
       <c r="G48" t="n">
-        <v>0.00346</v>
+        <v>3.12462</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>FRAX</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>Frax</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>2.71</v>
+        <v>0.999883</v>
       </c>
       <c r="E49" t="n">
-        <v>992159152</v>
+        <v>1003904842</v>
       </c>
       <c r="F49" t="n">
-        <v>222893434</v>
+        <v>7688712</v>
       </c>
       <c r="G49" t="n">
-        <v>1.49577</v>
+        <v>0.12686</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SAND</t>
+          <t>EDGT</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>The Sandbox</t>
+          <t>Edgecoin</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.5086000000000001</v>
+        <v>1</v>
       </c>
       <c r="E50" t="n">
-        <v>942814823</v>
+        <v>1000765774</v>
       </c>
       <c r="F50" t="n">
-        <v>174324609</v>
+        <v>5635090</v>
       </c>
       <c r="G50" t="n">
-        <v>1.82811</v>
+        <v>0.04031</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>EOS</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>EOS</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.843603</v>
+        <v>2.69</v>
       </c>
       <c r="E51" t="n">
-        <v>934024033</v>
+        <v>985768314</v>
       </c>
       <c r="F51" t="n">
-        <v>84618218</v>
+        <v>87786009</v>
       </c>
       <c r="G51" t="n">
-        <v>0.50784</v>
+        <v>-1.23651</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-06-11
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>27107</v>
+        <v>25800</v>
       </c>
       <c r="E2" t="n">
-        <v>525809310417</v>
+        <v>499416847911</v>
       </c>
       <c r="F2" t="n">
-        <v>13192740529</v>
+        <v>13388513728</v>
       </c>
       <c r="G2" t="n">
-        <v>0.96058</v>
+        <v>0.41741</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1887.97</v>
+        <v>1753.6</v>
       </c>
       <c r="E3" t="n">
-        <v>227089162245</v>
+        <v>210295110237</v>
       </c>
       <c r="F3" t="n">
-        <v>6381506812</v>
+        <v>6727715091</v>
       </c>
       <c r="G3" t="n">
-        <v>1.58589</v>
+        <v>0.57262</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999908</v>
+        <v>0.999409</v>
       </c>
       <c r="E4" t="n">
-        <v>83280087724</v>
+        <v>83375403179</v>
       </c>
       <c r="F4" t="n">
-        <v>18538185604</v>
+        <v>14960408295</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.01687</v>
+        <v>-0.16715</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>307.49</v>
+        <v>236.92</v>
       </c>
       <c r="E5" t="n">
-        <v>48552426008</v>
+        <v>36749154092</v>
       </c>
       <c r="F5" t="n">
-        <v>477347221</v>
+        <v>770548238</v>
       </c>
       <c r="G5" t="n">
-        <v>1.09056</v>
+        <v>-0.33121</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.9994769999999999</v>
+        <v>1.001</v>
       </c>
       <c r="E6" t="n">
-        <v>28965337796</v>
+        <v>28372340295</v>
       </c>
       <c r="F6" t="n">
-        <v>3689958603</v>
+        <v>2897778863</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.06967</v>
+        <v>0.05255</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.51608</v>
+        <v>0.509057</v>
       </c>
       <c r="E7" t="n">
-        <v>26832116636</v>
+        <v>26416565691</v>
       </c>
       <c r="F7" t="n">
-        <v>1064585345</v>
+        <v>1085072231</v>
       </c>
       <c r="G7" t="n">
-        <v>1.78094</v>
+        <v>2.51725</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1887.17</v>
+        <v>1750.66</v>
       </c>
       <c r="E8" t="n">
-        <v>13221348374</v>
+        <v>12529452955</v>
       </c>
       <c r="F8" t="n">
-        <v>29005920</v>
+        <v>23360654</v>
       </c>
       <c r="G8" t="n">
-        <v>1.63297</v>
+        <v>0.45745</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.372016</v>
+        <v>0.272429</v>
       </c>
       <c r="E9" t="n">
-        <v>13032872081</v>
+        <v>9407401686</v>
       </c>
       <c r="F9" t="n">
-        <v>232848245</v>
+        <v>786656730</v>
       </c>
       <c r="G9" t="n">
-        <v>1.98724</v>
+        <v>13.35538</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.072118</v>
+        <v>0.062361</v>
       </c>
       <c r="E10" t="n">
-        <v>10074198346</v>
+        <v>8680589754</v>
       </c>
       <c r="F10" t="n">
-        <v>199916416</v>
+        <v>525062297</v>
       </c>
       <c r="G10" t="n">
-        <v>0.60397</v>
+        <v>4.27137</v>
       </c>
     </row>
     <row r="11">
@@ -719,25 +719,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.903816</v>
+        <v>0.069425</v>
       </c>
       <c r="E11" t="n">
-        <v>8386525191</v>
+        <v>6239840447</v>
       </c>
       <c r="F11" t="n">
-        <v>169760753</v>
+        <v>316607938</v>
       </c>
       <c r="G11" t="n">
-        <v>1.44939</v>
+        <v>1.30826</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>21.04</v>
+        <v>15.62</v>
       </c>
       <c r="E12" t="n">
-        <v>8343151393</v>
+        <v>6159449074</v>
       </c>
       <c r="F12" t="n">
-        <v>232465701</v>
+        <v>750045136</v>
       </c>
       <c r="G12" t="n">
-        <v>1.85168</v>
+        <v>6.46173</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>94.61</v>
+        <v>78.56999999999999</v>
       </c>
       <c r="E13" t="n">
-        <v>6921507023</v>
+        <v>5720934564</v>
       </c>
       <c r="F13" t="n">
-        <v>965694742</v>
+        <v>678256531</v>
       </c>
       <c r="G13" t="n">
-        <v>2.2448</v>
+        <v>1.82913</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.076296</v>
+        <v>0.620169</v>
       </c>
       <c r="E14" t="n">
-        <v>6882122031</v>
+        <v>5675193407</v>
       </c>
       <c r="F14" t="n">
-        <v>286483465</v>
+        <v>709691521</v>
       </c>
       <c r="G14" t="n">
-        <v>2.72329</v>
+        <v>7.01136</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>5.27</v>
+        <v>4.49</v>
       </c>
       <c r="E15" t="n">
-        <v>6529850345</v>
+        <v>5554238961</v>
       </c>
       <c r="F15" t="n">
-        <v>117502419</v>
+        <v>161987008</v>
       </c>
       <c r="G15" t="n">
-        <v>0.82156</v>
+        <v>0.76047</v>
       </c>
     </row>
     <row r="16">
@@ -866,13 +866,13 @@
         <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>5170898371</v>
+        <v>4780982453</v>
       </c>
       <c r="F16" t="n">
-        <v>1290390345</v>
+        <v>1037599624</v>
       </c>
       <c r="G16" t="n">
-        <v>0.02462</v>
+        <v>-0.008829999999999999</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>8.51e-06</v>
+        <v>0.999591</v>
       </c>
       <c r="E17" t="n">
-        <v>5019514371</v>
+        <v>4541831427</v>
       </c>
       <c r="F17" t="n">
-        <v>104761249</v>
+        <v>83068865</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.01874</v>
+        <v>-6e-05</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>14.36</v>
+        <v>25780</v>
       </c>
       <c r="E18" t="n">
-        <v>4938374827</v>
+        <v>4031783326</v>
       </c>
       <c r="F18" t="n">
-        <v>129647306</v>
+        <v>89789242</v>
       </c>
       <c r="G18" t="n">
-        <v>2.26664</v>
+        <v>0.29723</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.999277</v>
+        <v>11.69</v>
       </c>
       <c r="E19" t="n">
-        <v>4602455111</v>
+        <v>4016941434</v>
       </c>
       <c r="F19" t="n">
-        <v>125945366</v>
+        <v>230145131</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.07664</v>
+        <v>2.02142</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>27130</v>
+        <v>6.75e-06</v>
       </c>
       <c r="E20" t="n">
-        <v>4242141497</v>
+        <v>3954452367</v>
       </c>
       <c r="F20" t="n">
-        <v>103007900</v>
+        <v>183256117</v>
       </c>
       <c r="G20" t="n">
-        <v>0.92687</v>
+        <v>4.57203</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>5.05</v>
+        <v>3.55</v>
       </c>
       <c r="E21" t="n">
-        <v>3810925906</v>
+        <v>3284236364</v>
       </c>
       <c r="F21" t="n">
-        <v>28879844</v>
+        <v>544951</v>
       </c>
       <c r="G21" t="n">
-        <v>0.70636</v>
+        <v>0.35146</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>3.59</v>
+        <v>4.06</v>
       </c>
       <c r="E22" t="n">
-        <v>3338429033</v>
+        <v>3042886767</v>
       </c>
       <c r="F22" t="n">
-        <v>532100</v>
+        <v>61679498</v>
       </c>
       <c r="G22" t="n">
-        <v>1.36984</v>
+        <v>2.51607</v>
       </c>
     </row>
     <row r="23">
@@ -1052,16 +1052,16 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>6.42</v>
+        <v>5.19</v>
       </c>
       <c r="E23" t="n">
-        <v>3321441769</v>
+        <v>2669744581</v>
       </c>
       <c r="F23" t="n">
-        <v>111087120</v>
+        <v>271578166</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.12382</v>
+        <v>3.40861</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>10.55</v>
+        <v>137.22</v>
       </c>
       <c r="E24" t="n">
-        <v>3086750107</v>
+        <v>2488575691</v>
       </c>
       <c r="F24" t="n">
-        <v>75478013</v>
+        <v>59530785</v>
       </c>
       <c r="G24" t="n">
-        <v>2.20311</v>
+        <v>0.79191</v>
       </c>
     </row>
     <row r="25">
@@ -1106,16 +1106,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>46.06</v>
+        <v>40.86</v>
       </c>
       <c r="E25" t="n">
-        <v>2763871288</v>
+        <v>2441105339</v>
       </c>
       <c r="F25" t="n">
-        <v>4345859</v>
+        <v>9029561</v>
       </c>
       <c r="G25" t="n">
-        <v>0.44842</v>
+        <v>-1.81827</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>145.64</v>
+        <v>8.26</v>
       </c>
       <c r="E26" t="n">
-        <v>2645813927</v>
+        <v>2403508443</v>
       </c>
       <c r="F26" t="n">
-        <v>69620635</v>
+        <v>104690418</v>
       </c>
       <c r="G26" t="n">
-        <v>-1.02828</v>
+        <v>5.95728</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>1.79</v>
+        <v>0.08296099999999999</v>
       </c>
       <c r="E27" t="n">
-        <v>2641252502</v>
+        <v>2227062683</v>
       </c>
       <c r="F27" t="n">
-        <v>8553610</v>
+        <v>59405381</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.36037</v>
+        <v>2.003</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>18.02</v>
+        <v>1.46</v>
       </c>
       <c r="E28" t="n">
-        <v>2546335004</v>
+        <v>2137523261</v>
       </c>
       <c r="F28" t="n">
-        <v>60510541</v>
+        <v>8168681</v>
       </c>
       <c r="G28" t="n">
-        <v>1.23155</v>
+        <v>-0.98084</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.09210699999999999</v>
+        <v>15.17</v>
       </c>
       <c r="E29" t="n">
-        <v>2474383172</v>
+        <v>2137317550</v>
       </c>
       <c r="F29" t="n">
-        <v>44135819</v>
+        <v>104900932</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.16043</v>
+        <v>4.60761</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>TUSD</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>114.57</v>
+        <v>1</v>
       </c>
       <c r="E30" t="n">
-        <v>2223126577</v>
+        <v>2038543739</v>
       </c>
       <c r="F30" t="n">
-        <v>56992042</v>
+        <v>1628220782</v>
       </c>
       <c r="G30" t="n">
-        <v>1.47612</v>
+        <v>0.09704</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>4.98</v>
+        <v>102.81</v>
       </c>
       <c r="E31" t="n">
-        <v>2127600807</v>
+        <v>1981960682</v>
       </c>
       <c r="F31" t="n">
-        <v>157464859</v>
+        <v>75512503</v>
       </c>
       <c r="G31" t="n">
-        <v>6.8555</v>
+        <v>2.11127</v>
       </c>
     </row>
     <row r="32">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>4.83</v>
+        <v>3.75</v>
       </c>
       <c r="E32" t="n">
-        <v>2107101723</v>
+        <v>1622521313</v>
       </c>
       <c r="F32" t="n">
-        <v>23144040</v>
+        <v>32291673</v>
       </c>
       <c r="G32" t="n">
-        <v>4.20412</v>
+        <v>-1.03993</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>1.8</v>
       </c>
       <c r="E33" t="n">
-        <v>2042492775</v>
+        <v>1567446717</v>
       </c>
       <c r="F33" t="n">
-        <v>211509120</v>
+        <v>49908591</v>
       </c>
       <c r="G33" t="n">
-        <v>0.0385</v>
+        <v>-1.8169</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>2.18</v>
+        <v>102.07</v>
       </c>
       <c r="E34" t="n">
-        <v>1903053265</v>
+        <v>1483160800</v>
       </c>
       <c r="F34" t="n">
-        <v>33083594</v>
+        <v>21260584</v>
       </c>
       <c r="G34" t="n">
-        <v>5.80991</v>
+        <v>-0.83519</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>9.01</v>
+        <v>3.44</v>
       </c>
       <c r="E35" t="n">
-        <v>1795323958</v>
+        <v>1464954134</v>
       </c>
       <c r="F35" t="n">
-        <v>102252154</v>
+        <v>177236276</v>
       </c>
       <c r="G35" t="n">
-        <v>7.62496</v>
+        <v>2.38016</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>118.58</v>
+        <v>0.055206</v>
       </c>
       <c r="E36" t="n">
-        <v>1723115257</v>
+        <v>1438248305</v>
       </c>
       <c r="F36" t="n">
-        <v>22257268</v>
+        <v>10516906</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.28806</v>
+        <v>7.40031</v>
       </c>
     </row>
     <row r="37">
@@ -1430,16 +1430,16 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.050862</v>
+        <v>0.04388459</v>
       </c>
       <c r="E37" t="n">
-        <v>1606957209</v>
+        <v>1381268780</v>
       </c>
       <c r="F37" t="n">
-        <v>23652856</v>
+        <v>33749205</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.37445</v>
+        <v>0.28063</v>
       </c>
     </row>
     <row r="38">
@@ -1457,16 +1457,16 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1.2</v>
+        <v>1.008</v>
       </c>
       <c r="E38" t="n">
-        <v>1526348712</v>
+        <v>1276930728</v>
       </c>
       <c r="F38" t="n">
-        <v>145802641</v>
+        <v>311740124</v>
       </c>
       <c r="G38" t="n">
-        <v>4.66287</v>
+        <v>-1.21562</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.059449</v>
+        <v>5.97</v>
       </c>
       <c r="E39" t="n">
-        <v>1502187936</v>
+        <v>1189988763</v>
       </c>
       <c r="F39" t="n">
-        <v>7307760</v>
+        <v>93013984</v>
       </c>
       <c r="G39" t="n">
-        <v>0.12235</v>
+        <v>-0.05791</v>
       </c>
     </row>
     <row r="40">
@@ -1511,16 +1511,16 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.01992204</v>
+        <v>0.0155913</v>
       </c>
       <c r="E40" t="n">
-        <v>1449556066</v>
+        <v>1127965332</v>
       </c>
       <c r="F40" t="n">
-        <v>43346917</v>
+        <v>53737517</v>
       </c>
       <c r="G40" t="n">
-        <v>0.09068</v>
+        <v>4.80832</v>
       </c>
     </row>
     <row r="41">
@@ -1538,16 +1538,16 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1.58</v>
+        <v>1.21</v>
       </c>
       <c r="E41" t="n">
-        <v>1436822942</v>
+        <v>1098208500</v>
       </c>
       <c r="F41" t="n">
-        <v>45777673</v>
+        <v>75773337</v>
       </c>
       <c r="G41" t="n">
-        <v>1.15822</v>
+        <v>-0.62973</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>USDP</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Pax Dollar</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.130307</v>
+        <v>0.999436</v>
       </c>
       <c r="E42" t="n">
-        <v>1172792132</v>
+        <v>1004307950</v>
       </c>
       <c r="F42" t="n">
-        <v>148612997</v>
+        <v>2064877</v>
       </c>
       <c r="G42" t="n">
-        <v>-5.00293</v>
+        <v>-0.11238</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>APE</t>
+          <t>FRAX</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ApeCoin</t>
+          <t>Frax</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>3.11</v>
+        <v>0.999644</v>
       </c>
       <c r="E43" t="n">
-        <v>1147154672</v>
+        <v>1002394014</v>
       </c>
       <c r="F43" t="n">
-        <v>53551284</v>
+        <v>8771050</v>
       </c>
       <c r="G43" t="n">
-        <v>0.11902</v>
+        <v>-0.08223999999999999</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ALGO</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Algorand</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.151539</v>
+        <v>0.101069</v>
       </c>
       <c r="E44" t="n">
-        <v>1098269275</v>
+        <v>905652369</v>
       </c>
       <c r="F44" t="n">
-        <v>31350508</v>
+        <v>59615397</v>
       </c>
       <c r="G44" t="n">
-        <v>3.50574</v>
+        <v>5.33985</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>SAND</t>
+          <t>BSCX</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>The Sandbox</t>
+          <t>BSCEX</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.563395</v>
+        <v>236.13</v>
       </c>
       <c r="E45" t="n">
-        <v>1044949096</v>
+        <v>900932790</v>
       </c>
       <c r="F45" t="n">
-        <v>199315126</v>
+        <v>1232324</v>
       </c>
       <c r="G45" t="n">
-        <v>5.45542</v>
+        <v>-0.9194600000000001</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>USDP</t>
+          <t>RPL</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Pax Dollar</t>
+          <t>Rocket Pool</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.999431</v>
+        <v>44.22</v>
       </c>
       <c r="E46" t="n">
-        <v>1016868472</v>
+        <v>859118106</v>
       </c>
       <c r="F46" t="n">
-        <v>41176405</v>
+        <v>3577300</v>
       </c>
       <c r="G46" t="n">
-        <v>-0.07580000000000001</v>
+        <v>0.50688</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>FRAX</t>
+          <t>APE</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Frax</t>
+          <t>ApeCoin</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.999451</v>
+        <v>2.33</v>
       </c>
       <c r="E47" t="n">
-        <v>1003917644</v>
+        <v>855911646</v>
       </c>
       <c r="F47" t="n">
-        <v>3312312</v>
+        <v>176495193</v>
       </c>
       <c r="G47" t="n">
-        <v>0.05393</v>
+        <v>-0.10397</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>EOS</t>
+          <t>RETH</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>EOS</t>
+          <t>Rocket Pool ETH</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.902846</v>
+        <v>1883.2</v>
       </c>
       <c r="E48" t="n">
-        <v>1000589643</v>
+        <v>827072489</v>
       </c>
       <c r="F48" t="n">
-        <v>86697259</v>
+        <v>1921003</v>
       </c>
       <c r="G48" t="n">
-        <v>2.02346</v>
+        <v>0.53583</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>RPL</t>
+          <t>ALGO</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Rocket Pool</t>
+          <t>Algorand</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>49.26</v>
+        <v>0.108853</v>
       </c>
       <c r="E49" t="n">
-        <v>955800076</v>
+        <v>786778661</v>
       </c>
       <c r="F49" t="n">
-        <v>3675042</v>
+        <v>53314486</v>
       </c>
       <c r="G49" t="n">
-        <v>2.48469</v>
+        <v>1.72047</v>
       </c>
     </row>
     <row r="50">
@@ -1781,16 +1781,16 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>37.2</v>
+        <v>30.3</v>
       </c>
       <c r="E50" t="n">
-        <v>948172203</v>
+        <v>771665546</v>
       </c>
       <c r="F50" t="n">
-        <v>10593056</v>
+        <v>15238647</v>
       </c>
       <c r="G50" t="n">
-        <v>1.06144</v>
+        <v>0.94648</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>EOS</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>EOS</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>2.57</v>
+        <v>0.685325</v>
       </c>
       <c r="E51" t="n">
-        <v>940361339</v>
+        <v>757082007</v>
       </c>
       <c r="F51" t="n">
-        <v>91285990</v>
+        <v>162832180</v>
       </c>
       <c r="G51" t="n">
-        <v>2.69644</v>
+        <v>0.8617899999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-06-18
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>25802</v>
+        <v>26504</v>
       </c>
       <c r="E2" t="n">
-        <v>500595488301</v>
+        <v>514130026129</v>
       </c>
       <c r="F2" t="n">
-        <v>6369370944</v>
+        <v>7719628543</v>
       </c>
       <c r="G2" t="n">
-        <v>0.44327</v>
+        <v>-0.00517</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1751.95</v>
+        <v>1733.98</v>
       </c>
       <c r="E3" t="n">
-        <v>210696959252</v>
+        <v>208408939062</v>
       </c>
       <c r="F3" t="n">
-        <v>6283205999</v>
+        <v>3500759457</v>
       </c>
       <c r="G3" t="n">
-        <v>0.42571</v>
+        <v>-0.20914</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0.999698</v>
       </c>
       <c r="E4" t="n">
-        <v>83408115139</v>
+        <v>83123063318</v>
       </c>
       <c r="F4" t="n">
-        <v>20080085200</v>
+        <v>11356066225</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.00122</v>
+        <v>0.0283</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>236.62</v>
+        <v>246.97</v>
       </c>
       <c r="E5" t="n">
-        <v>36866596856</v>
+        <v>38451250501</v>
       </c>
       <c r="F5" t="n">
-        <v>743668096</v>
+        <v>516731160</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.60977</v>
+        <v>0.64275</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.999848</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>28371716689</v>
+        <v>28343670246</v>
       </c>
       <c r="F6" t="n">
-        <v>2471803424</v>
+        <v>1776435711</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.02477</v>
+        <v>-0.01725</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.511595</v>
+        <v>0.489456</v>
       </c>
       <c r="E7" t="n">
-        <v>26556696804</v>
+        <v>25416120120</v>
       </c>
       <c r="F7" t="n">
-        <v>1060243833</v>
+        <v>576976568</v>
       </c>
       <c r="G7" t="n">
-        <v>3.22591</v>
+        <v>1.84822</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1752.19</v>
+        <v>1734.03</v>
       </c>
       <c r="E8" t="n">
-        <v>12562695228</v>
+        <v>12560665943</v>
       </c>
       <c r="F8" t="n">
-        <v>23226503</v>
+        <v>10084881</v>
       </c>
       <c r="G8" t="n">
-        <v>0.34485</v>
+        <v>-0.17523</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.270096</v>
+        <v>0.266724</v>
       </c>
       <c r="E9" t="n">
-        <v>9444479618</v>
+        <v>9339948530</v>
       </c>
       <c r="F9" t="n">
-        <v>733563422</v>
+        <v>138467355</v>
       </c>
       <c r="G9" t="n">
-        <v>8.14471</v>
+        <v>-0.57603</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.062276</v>
+        <v>0.062283</v>
       </c>
       <c r="E10" t="n">
-        <v>8697784214</v>
+        <v>8705156545</v>
       </c>
       <c r="F10" t="n">
-        <v>491575595</v>
+        <v>187490734</v>
       </c>
       <c r="G10" t="n">
-        <v>4.22588</v>
+        <v>-0.2695</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.069215</v>
+        <v>0.070606</v>
       </c>
       <c r="E11" t="n">
-        <v>6236833750</v>
+        <v>6360975725</v>
       </c>
       <c r="F11" t="n">
-        <v>297841168</v>
+        <v>241906419</v>
       </c>
       <c r="G11" t="n">
-        <v>2.07891</v>
+        <v>-0.8918199999999999</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>15.57</v>
+        <v>15.73</v>
       </c>
       <c r="E12" t="n">
-        <v>6195433378</v>
+        <v>6288152256</v>
       </c>
       <c r="F12" t="n">
-        <v>709387933</v>
+        <v>148119083</v>
       </c>
       <c r="G12" t="n">
-        <v>5.4866</v>
+        <v>-0.44167</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.627524</v>
+        <v>4.61</v>
       </c>
       <c r="E13" t="n">
-        <v>5824127171</v>
+        <v>5727178003</v>
       </c>
       <c r="F13" t="n">
-        <v>679709510</v>
+        <v>90357091</v>
       </c>
       <c r="G13" t="n">
-        <v>7.89528</v>
+        <v>1.30981</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>78.20999999999999</v>
+        <v>0.610446</v>
       </c>
       <c r="E14" t="n">
-        <v>5721375955</v>
+        <v>5667152605</v>
       </c>
       <c r="F14" t="n">
-        <v>657407635</v>
+        <v>234043128</v>
       </c>
       <c r="G14" t="n">
-        <v>1.15937</v>
+        <v>-1.37483</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>4.49</v>
+        <v>77.36</v>
       </c>
       <c r="E15" t="n">
-        <v>5580258420</v>
+        <v>5661924459</v>
       </c>
       <c r="F15" t="n">
-        <v>151747287</v>
+        <v>226898136</v>
       </c>
       <c r="G15" t="n">
-        <v>0.49926</v>
+        <v>0.39579</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Binance USD</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.999738</v>
+        <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>4779419798</v>
+        <v>4416010684</v>
       </c>
       <c r="F16" t="n">
-        <v>1122823868</v>
+        <v>78231889</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.07326000000000001</v>
+        <v>-0.08398</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Binance USD</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.999956</v>
+        <v>0.999952</v>
       </c>
       <c r="E17" t="n">
-        <v>4542725456</v>
+        <v>4293761136</v>
       </c>
       <c r="F17" t="n">
-        <v>102850792</v>
+        <v>1165530473</v>
       </c>
       <c r="G17" t="n">
-        <v>0.03421</v>
+        <v>-0.0453</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>25791</v>
+        <v>7.24e-06</v>
       </c>
       <c r="E18" t="n">
-        <v>4042830718</v>
+        <v>4254974703</v>
       </c>
       <c r="F18" t="n">
-        <v>86871186</v>
+        <v>129185296</v>
       </c>
       <c r="G18" t="n">
-        <v>0.25331</v>
+        <v>4.99518</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>11.7</v>
+        <v>26508</v>
       </c>
       <c r="E19" t="n">
-        <v>4031097052</v>
+        <v>4157107522</v>
       </c>
       <c r="F19" t="n">
-        <v>217402598</v>
+        <v>57980137</v>
       </c>
       <c r="G19" t="n">
-        <v>0.87344</v>
+        <v>-0.05611</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>6.73e-06</v>
+        <v>11.52</v>
       </c>
       <c r="E20" t="n">
-        <v>3966292051</v>
+        <v>3975061234</v>
       </c>
       <c r="F20" t="n">
-        <v>162687111</v>
+        <v>102623100</v>
       </c>
       <c r="G20" t="n">
-        <v>2.52758</v>
+        <v>-2.10462</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>3.55</v>
+        <v>4.54</v>
       </c>
       <c r="E21" t="n">
-        <v>3293095380</v>
+        <v>3418290137</v>
       </c>
       <c r="F21" t="n">
-        <v>638139</v>
+        <v>28890358</v>
       </c>
       <c r="G21" t="n">
-        <v>0.8966499999999999</v>
+        <v>-1.2367</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>4.08</v>
+        <v>3.55</v>
       </c>
       <c r="E22" t="n">
-        <v>3073134648</v>
+        <v>3301646747</v>
       </c>
       <c r="F22" t="n">
-        <v>57263270</v>
+        <v>485957</v>
       </c>
       <c r="G22" t="n">
-        <v>2.11153</v>
+        <v>0.94928</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>TUSD</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>5.19</v>
+        <v>1.002</v>
       </c>
       <c r="E23" t="n">
-        <v>2680024536</v>
+        <v>3116271882</v>
       </c>
       <c r="F23" t="n">
-        <v>247445264</v>
+        <v>112738765</v>
       </c>
       <c r="G23" t="n">
-        <v>2.26608</v>
+        <v>0.02121</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>136.87</v>
+        <v>5.24</v>
       </c>
       <c r="E24" t="n">
-        <v>2486158995</v>
+        <v>2710821626</v>
       </c>
       <c r="F24" t="n">
-        <v>54949285</v>
+        <v>80609426</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.71641</v>
+        <v>-2.04024</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>40.85</v>
+        <v>8.77</v>
       </c>
       <c r="E25" t="n">
-        <v>2455124330</v>
+        <v>2559075861</v>
       </c>
       <c r="F25" t="n">
-        <v>9052172</v>
+        <v>56145492</v>
       </c>
       <c r="G25" t="n">
-        <v>-1.70293</v>
+        <v>-1.26254</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>8.26</v>
+        <v>139.38</v>
       </c>
       <c r="E26" t="n">
-        <v>2416569452</v>
+        <v>2532899268</v>
       </c>
       <c r="F26" t="n">
-        <v>99742775</v>
+        <v>46699578</v>
       </c>
       <c r="G26" t="n">
-        <v>4.18942</v>
+        <v>2.77859</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.082884</v>
+        <v>41.5</v>
       </c>
       <c r="E27" t="n">
-        <v>2226753924</v>
+        <v>2492565490</v>
       </c>
       <c r="F27" t="n">
-        <v>54139534</v>
+        <v>2660769</v>
       </c>
       <c r="G27" t="n">
-        <v>2.23928</v>
+        <v>-0.73752</v>
       </c>
     </row>
     <row r="28">
@@ -1187,16 +1187,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>15.22</v>
+        <v>15.45</v>
       </c>
       <c r="E28" t="n">
-        <v>2155780934</v>
+        <v>2184134520</v>
       </c>
       <c r="F28" t="n">
-        <v>104106505</v>
+        <v>60144446</v>
       </c>
       <c r="G28" t="n">
-        <v>4.2874</v>
+        <v>0.65201</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>1.46</v>
+        <v>0.080692</v>
       </c>
       <c r="E29" t="n">
-        <v>2153693752</v>
+        <v>2171511121</v>
       </c>
       <c r="F29" t="n">
-        <v>7730983</v>
+        <v>32287669</v>
       </c>
       <c r="G29" t="n">
-        <v>-2.13301</v>
+        <v>2.60238</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.998542</v>
+        <v>108.06</v>
       </c>
       <c r="E30" t="n">
-        <v>2038588708</v>
+        <v>2100080215</v>
       </c>
       <c r="F30" t="n">
-        <v>1621114950</v>
+        <v>48058055</v>
       </c>
       <c r="G30" t="n">
-        <v>0.21368</v>
+        <v>1.05591</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>102.71</v>
+        <v>1.41</v>
       </c>
       <c r="E31" t="n">
-        <v>1993609792</v>
+        <v>2081536704</v>
       </c>
       <c r="F31" t="n">
-        <v>73106056</v>
+        <v>3149825</v>
       </c>
       <c r="G31" t="n">
-        <v>1.54678</v>
+        <v>-0.53277</v>
       </c>
     </row>
     <row r="32">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>3.75</v>
+        <v>3.99</v>
       </c>
       <c r="E32" t="n">
-        <v>1631291793</v>
+        <v>1740630565</v>
       </c>
       <c r="F32" t="n">
-        <v>31307051</v>
+        <v>9826592</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.5125999999999999</v>
+        <v>-0.29666</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>1.78</v>
+        <v>3.69</v>
       </c>
       <c r="E33" t="n">
-        <v>1565492493</v>
+        <v>1589042737</v>
       </c>
       <c r="F33" t="n">
-        <v>49254589</v>
+        <v>54585734</v>
       </c>
       <c r="G33" t="n">
-        <v>-3.63985</v>
+        <v>-1.05203</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>101.98</v>
+        <v>1.78</v>
       </c>
       <c r="E34" t="n">
-        <v>1483065603</v>
+        <v>1566185230</v>
       </c>
       <c r="F34" t="n">
-        <v>19896426</v>
+        <v>15396497</v>
       </c>
       <c r="G34" t="n">
-        <v>-2.06121</v>
+        <v>-1.17958</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>3.43</v>
+        <v>101.39</v>
       </c>
       <c r="E35" t="n">
-        <v>1472491766</v>
+        <v>1468856926</v>
       </c>
       <c r="F35" t="n">
-        <v>173858361</v>
+        <v>46266445</v>
       </c>
       <c r="G35" t="n">
-        <v>2.39789</v>
+        <v>-10.24997</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.055226</v>
+        <v>0.04587823</v>
       </c>
       <c r="E36" t="n">
-        <v>1441425857</v>
+        <v>1447494423</v>
       </c>
       <c r="F36" t="n">
-        <v>10155746</v>
+        <v>14169289</v>
       </c>
       <c r="G36" t="n">
-        <v>7.32196</v>
+        <v>0.3569</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.04421969</v>
+        <v>6.98</v>
       </c>
       <c r="E37" t="n">
-        <v>1397971881</v>
+        <v>1438456139</v>
       </c>
       <c r="F37" t="n">
-        <v>32576736</v>
+        <v>134118357</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.49273</v>
+        <v>1.70374</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1.003</v>
+        <v>0.053854</v>
       </c>
       <c r="E38" t="n">
-        <v>1279626021</v>
+        <v>1406369027</v>
       </c>
       <c r="F38" t="n">
-        <v>306994497</v>
+        <v>4073055</v>
       </c>
       <c r="G38" t="n">
-        <v>-1.27178</v>
+        <v>0.9067</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>6</v>
+        <v>1.013</v>
       </c>
       <c r="E39" t="n">
-        <v>1203260361</v>
+        <v>1292434959</v>
       </c>
       <c r="F39" t="n">
-        <v>88383069</v>
+        <v>97846537</v>
       </c>
       <c r="G39" t="n">
-        <v>0.5184299999999999</v>
+        <v>1.34716</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.01571441</v>
+        <v>1.25</v>
       </c>
       <c r="E40" t="n">
-        <v>1142103912</v>
+        <v>1152941419</v>
       </c>
       <c r="F40" t="n">
-        <v>51790710</v>
+        <v>34779761</v>
       </c>
       <c r="G40" t="n">
-        <v>4.69743</v>
+        <v>-0.42269</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1.21</v>
+        <v>0.01510038</v>
       </c>
       <c r="E41" t="n">
-        <v>1104636075</v>
+        <v>1097545815</v>
       </c>
       <c r="F41" t="n">
-        <v>72960357</v>
+        <v>32461668</v>
       </c>
       <c r="G41" t="n">
-        <v>0.47387</v>
+        <v>0.11249</v>
       </c>
     </row>
     <row r="42">
@@ -1565,16 +1565,16 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.998169</v>
+        <v>1.001</v>
       </c>
       <c r="E42" t="n">
-        <v>1004562920</v>
+        <v>1007076455</v>
       </c>
       <c r="F42" t="n">
-        <v>1659208</v>
+        <v>1216097</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.20889</v>
+        <v>0.01424</v>
       </c>
     </row>
     <row r="43">
@@ -1592,16 +1592,16 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.998468</v>
+        <v>0.9991370000000001</v>
       </c>
       <c r="E43" t="n">
-        <v>1002513369</v>
+        <v>1002783822</v>
       </c>
       <c r="F43" t="n">
-        <v>8013847</v>
+        <v>13972447</v>
       </c>
       <c r="G43" t="n">
-        <v>-0.12378</v>
+        <v>-0.10188</v>
       </c>
     </row>
     <row r="44">
@@ -1619,16 +1619,16 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.100782</v>
+        <v>0.101666</v>
       </c>
       <c r="E44" t="n">
-        <v>907155639</v>
+        <v>915694293</v>
       </c>
       <c r="F44" t="n">
-        <v>56806192</v>
+        <v>35304813</v>
       </c>
       <c r="G44" t="n">
-        <v>4.2034</v>
+        <v>1.51025</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>BSCX</t>
+          <t>ALGO</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>BSCEX</t>
+          <t>Algorand</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>237.12</v>
+        <v>0.118602</v>
       </c>
       <c r="E45" t="n">
-        <v>904393606</v>
+        <v>858929426</v>
       </c>
       <c r="F45" t="n">
-        <v>1239178</v>
+        <v>24930131</v>
       </c>
       <c r="G45" t="n">
-        <v>-0.5628</v>
+        <v>-1.56302</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>RPL</t>
+          <t>RETH</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Rocket Pool</t>
+          <t>Rocket Pool ETH</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>44.22</v>
+        <v>1864.18</v>
       </c>
       <c r="E46" t="n">
-        <v>861688515</v>
+        <v>833174097</v>
       </c>
       <c r="F46" t="n">
-        <v>3460330</v>
+        <v>2068802</v>
       </c>
       <c r="G46" t="n">
-        <v>-0.13388</v>
+        <v>-0.15891</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>APE</t>
+          <t>RPL</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>ApeCoin</t>
+          <t>Rocket Pool</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>2.33</v>
+        <v>41.21</v>
       </c>
       <c r="E47" t="n">
-        <v>855871892</v>
+        <v>801936794</v>
       </c>
       <c r="F47" t="n">
-        <v>170097834</v>
+        <v>3947950</v>
       </c>
       <c r="G47" t="n">
-        <v>0.02569</v>
+        <v>-1.19626</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>RETH</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Rocket Pool ETH</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>1882.3</v>
+        <v>0.572309</v>
       </c>
       <c r="E48" t="n">
-        <v>829056230</v>
+        <v>793659211</v>
       </c>
       <c r="F48" t="n">
-        <v>2109249</v>
+        <v>26127467</v>
       </c>
       <c r="G48" t="n">
-        <v>0.30041</v>
+        <v>-3.48531</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ALGO</t>
+          <t>APE</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Algorand</t>
+          <t>ApeCoin</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.110078</v>
+        <v>2.13</v>
       </c>
       <c r="E49" t="n">
-        <v>796730452</v>
+        <v>784794655</v>
       </c>
       <c r="F49" t="n">
-        <v>51655433</v>
+        <v>58858802</v>
       </c>
       <c r="G49" t="n">
-        <v>1.36527</v>
+        <v>0.37583</v>
       </c>
     </row>
     <row r="50">
@@ -1781,16 +1781,16 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>30.2</v>
+        <v>30.59</v>
       </c>
       <c r="E50" t="n">
-        <v>770327338</v>
+        <v>782089156</v>
       </c>
       <c r="F50" t="n">
-        <v>14143998</v>
+        <v>9191552</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.1087</v>
+        <v>-0.27369</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>FTM</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Fantom</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.552745</v>
+        <v>0.273029</v>
       </c>
       <c r="E51" t="n">
-        <v>762591631</v>
+        <v>762847483</v>
       </c>
       <c r="F51" t="n">
-        <v>55596251</v>
+        <v>76183711</v>
       </c>
       <c r="G51" t="n">
-        <v>3.76432</v>
+        <v>-0.90094</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-06-25
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>26504</v>
+        <v>30691</v>
       </c>
       <c r="E2" t="n">
-        <v>514130026129</v>
+        <v>595759907750</v>
       </c>
       <c r="F2" t="n">
-        <v>7719628543</v>
+        <v>12975786163</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.00517</v>
+        <v>-0.03812</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1733.98</v>
+        <v>1916.11</v>
       </c>
       <c r="E3" t="n">
-        <v>208408939062</v>
+        <v>230285731243</v>
       </c>
       <c r="F3" t="n">
-        <v>3500759457</v>
+        <v>7280425873</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.20914</v>
+        <v>1.02868</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999698</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>83123063318</v>
+        <v>83130016547</v>
       </c>
       <c r="F4" t="n">
-        <v>11356066225</v>
+        <v>19416891910</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0283</v>
+        <v>-0.05126</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>246.97</v>
+        <v>239.95</v>
       </c>
       <c r="E5" t="n">
-        <v>38451250501</v>
+        <v>37397549306</v>
       </c>
       <c r="F5" t="n">
-        <v>516731160</v>
+        <v>766763641</v>
       </c>
       <c r="G5" t="n">
-        <v>0.64275</v>
+        <v>-2.16308</v>
       </c>
     </row>
     <row r="6">
@@ -596,13 +596,13 @@
         <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>28343670246</v>
+        <v>28436790925</v>
       </c>
       <c r="F6" t="n">
-        <v>1776435711</v>
+        <v>3155463040</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.01725</v>
+        <v>-0.00446</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.489456</v>
+        <v>0.491939</v>
       </c>
       <c r="E7" t="n">
-        <v>25416120120</v>
+        <v>25713728479</v>
       </c>
       <c r="F7" t="n">
-        <v>576976568</v>
+        <v>542038095</v>
       </c>
       <c r="G7" t="n">
-        <v>1.84822</v>
+        <v>-0.1495</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1734.03</v>
+        <v>1912.08</v>
       </c>
       <c r="E8" t="n">
-        <v>12560665943</v>
+        <v>14141089162</v>
       </c>
       <c r="F8" t="n">
-        <v>10084881</v>
+        <v>2000483</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.17523</v>
+        <v>0.81103</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.266724</v>
+        <v>0.297543</v>
       </c>
       <c r="E9" t="n">
-        <v>9339948530</v>
+        <v>10433002658</v>
       </c>
       <c r="F9" t="n">
-        <v>138467355</v>
+        <v>210087347</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.57603</v>
+        <v>0.56745</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.062283</v>
+        <v>0.06768399999999999</v>
       </c>
       <c r="E10" t="n">
-        <v>8705156545</v>
+        <v>9468276785</v>
       </c>
       <c r="F10" t="n">
-        <v>187490734</v>
+        <v>243364562</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.2695</v>
+        <v>-0.43341</v>
       </c>
     </row>
     <row r="11">
@@ -719,25 +719,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>SOL</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Solana</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.070606</v>
+        <v>17.21</v>
       </c>
       <c r="E11" t="n">
-        <v>6360975725</v>
+        <v>6887534070</v>
       </c>
       <c r="F11" t="n">
-        <v>241906419</v>
+        <v>248616422</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.8918199999999999</v>
+        <v>-0.61104</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +746,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SOL</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Solana</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>15.73</v>
+        <v>0.073522</v>
       </c>
       <c r="E12" t="n">
-        <v>6288152256</v>
+        <v>6603860079</v>
       </c>
       <c r="F12" t="n">
-        <v>148119083</v>
+        <v>246993465</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.44167</v>
+        <v>1.38104</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>4.61</v>
+        <v>88.84</v>
       </c>
       <c r="E13" t="n">
-        <v>5727178003</v>
+        <v>6507691635</v>
       </c>
       <c r="F13" t="n">
-        <v>90357091</v>
+        <v>587917523</v>
       </c>
       <c r="G13" t="n">
-        <v>1.30981</v>
+        <v>-2.40692</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.610446</v>
+        <v>5.19</v>
       </c>
       <c r="E14" t="n">
-        <v>5667152605</v>
+        <v>6456630286</v>
       </c>
       <c r="F14" t="n">
-        <v>234043128</v>
+        <v>127399249</v>
       </c>
       <c r="G14" t="n">
-        <v>-1.37483</v>
+        <v>2.67859</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>77.36</v>
+        <v>0.672648</v>
       </c>
       <c r="E15" t="n">
-        <v>5661924459</v>
+        <v>6251692478</v>
       </c>
       <c r="F15" t="n">
-        <v>226898136</v>
+        <v>228944836</v>
       </c>
       <c r="G15" t="n">
-        <v>0.39579</v>
+        <v>-1.10279</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>30646</v>
       </c>
       <c r="E16" t="n">
-        <v>4416010684</v>
+        <v>4818705018</v>
       </c>
       <c r="F16" t="n">
-        <v>78231889</v>
+        <v>151713562</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.08398</v>
+        <v>-0.27449</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Binance USD</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.999952</v>
+        <v>7.95e-06</v>
       </c>
       <c r="E17" t="n">
-        <v>4293761136</v>
+        <v>4681027830</v>
       </c>
       <c r="F17" t="n">
-        <v>1165530473</v>
+        <v>116390454</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.0453</v>
+        <v>-1.15743</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>7.24e-06</v>
+        <v>13.55</v>
       </c>
       <c r="E18" t="n">
-        <v>4254974703</v>
+        <v>4677112416</v>
       </c>
       <c r="F18" t="n">
-        <v>129185296</v>
+        <v>139895444</v>
       </c>
       <c r="G18" t="n">
-        <v>4.99518</v>
+        <v>2.69807</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>26508</v>
+        <v>1</v>
       </c>
       <c r="E19" t="n">
-        <v>4157107522</v>
+        <v>4450286885</v>
       </c>
       <c r="F19" t="n">
-        <v>57980137</v>
+        <v>87921293</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.05611</v>
+        <v>-0.07027</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Binance USD</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>11.52</v>
+        <v>1</v>
       </c>
       <c r="E20" t="n">
-        <v>3975061234</v>
+        <v>4244868393</v>
       </c>
       <c r="F20" t="n">
-        <v>102623100</v>
+        <v>2106858046</v>
       </c>
       <c r="G20" t="n">
-        <v>-2.10462</v>
+        <v>-0.05094</v>
       </c>
     </row>
     <row r="21">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>4.54</v>
+        <v>5.38</v>
       </c>
       <c r="E21" t="n">
-        <v>3418290137</v>
+        <v>4030766043</v>
       </c>
       <c r="F21" t="n">
-        <v>28890358</v>
+        <v>109292465</v>
       </c>
       <c r="G21" t="n">
-        <v>-1.2367</v>
+        <v>11.56179</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>3.55</v>
+        <v>200.98</v>
       </c>
       <c r="E22" t="n">
-        <v>3301646747</v>
+        <v>3905237719</v>
       </c>
       <c r="F22" t="n">
-        <v>485957</v>
+        <v>1363922665</v>
       </c>
       <c r="G22" t="n">
-        <v>0.94928</v>
+        <v>3.75765</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>1.002</v>
+        <v>3.84</v>
       </c>
       <c r="E23" t="n">
-        <v>3116271882</v>
+        <v>3571855159</v>
       </c>
       <c r="F23" t="n">
-        <v>112738765</v>
+        <v>713801</v>
       </c>
       <c r="G23" t="n">
-        <v>0.02121</v>
+        <v>-1.00332</v>
       </c>
     </row>
     <row r="24">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>5.24</v>
+        <v>6.3</v>
       </c>
       <c r="E24" t="n">
-        <v>2710821626</v>
+        <v>3262044470</v>
       </c>
       <c r="F24" t="n">
-        <v>80609426</v>
+        <v>166878918</v>
       </c>
       <c r="G24" t="n">
-        <v>-2.04024</v>
+        <v>2.4205</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>TUSD</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>8.77</v>
+        <v>0.99897</v>
       </c>
       <c r="E25" t="n">
-        <v>2559075861</v>
+        <v>3135245545</v>
       </c>
       <c r="F25" t="n">
-        <v>56145492</v>
+        <v>189437775</v>
       </c>
       <c r="G25" t="n">
-        <v>-1.26254</v>
+        <v>-0.10681</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>139.38</v>
+        <v>165.52</v>
       </c>
       <c r="E26" t="n">
-        <v>2532899268</v>
+        <v>3011967273</v>
       </c>
       <c r="F26" t="n">
-        <v>46699578</v>
+        <v>95791616</v>
       </c>
       <c r="G26" t="n">
-        <v>2.77859</v>
+        <v>6.16086</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>41.5</v>
+        <v>9.66</v>
       </c>
       <c r="E27" t="n">
-        <v>2492565490</v>
+        <v>2822832048</v>
       </c>
       <c r="F27" t="n">
-        <v>2660769</v>
+        <v>164204223</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.73752</v>
+        <v>2.52374</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>15.45</v>
+        <v>44.96</v>
       </c>
       <c r="E28" t="n">
-        <v>2184134520</v>
+        <v>2705385551</v>
       </c>
       <c r="F28" t="n">
-        <v>60144446</v>
+        <v>4718709</v>
       </c>
       <c r="G28" t="n">
-        <v>0.65201</v>
+        <v>-0.34113</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.080692</v>
+        <v>18.9</v>
       </c>
       <c r="E29" t="n">
-        <v>2171511121</v>
+        <v>2672922535</v>
       </c>
       <c r="F29" t="n">
-        <v>32287669</v>
+        <v>243135797</v>
       </c>
       <c r="G29" t="n">
-        <v>2.60238</v>
+        <v>-1.32338</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>108.06</v>
+        <v>0.091516</v>
       </c>
       <c r="E30" t="n">
-        <v>2100080215</v>
+        <v>2466137755</v>
       </c>
       <c r="F30" t="n">
-        <v>48058055</v>
+        <v>42374487</v>
       </c>
       <c r="G30" t="n">
-        <v>1.05591</v>
+        <v>0.42965</v>
       </c>
     </row>
     <row r="31">
@@ -1268,16 +1268,16 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>1.41</v>
+        <v>1.48</v>
       </c>
       <c r="E31" t="n">
-        <v>2081536704</v>
+        <v>2175995111</v>
       </c>
       <c r="F31" t="n">
-        <v>3149825</v>
+        <v>8993026</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.53277</v>
+        <v>5.49221</v>
       </c>
     </row>
     <row r="32">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>3.99</v>
+        <v>4.36</v>
       </c>
       <c r="E32" t="n">
-        <v>1740630565</v>
+        <v>1910550258</v>
       </c>
       <c r="F32" t="n">
-        <v>9826592</v>
+        <v>14987941</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.29666</v>
+        <v>0.67437</v>
       </c>
     </row>
     <row r="33">
@@ -1322,16 +1322,16 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>3.69</v>
+        <v>4.08</v>
       </c>
       <c r="E33" t="n">
-        <v>1589042737</v>
+        <v>1757764243</v>
       </c>
       <c r="F33" t="n">
-        <v>54585734</v>
+        <v>91776724</v>
       </c>
       <c r="G33" t="n">
-        <v>-1.05203</v>
+        <v>1.22967</v>
       </c>
     </row>
     <row r="34">
@@ -1349,16 +1349,16 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>1.78</v>
+        <v>1.97</v>
       </c>
       <c r="E34" t="n">
-        <v>1566185230</v>
+        <v>1728499971</v>
       </c>
       <c r="F34" t="n">
-        <v>15396497</v>
+        <v>38411138</v>
       </c>
       <c r="G34" t="n">
-        <v>-1.17958</v>
+        <v>3.06545</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>101.39</v>
+        <v>0.053137</v>
       </c>
       <c r="E35" t="n">
-        <v>1468856926</v>
+        <v>1685966481</v>
       </c>
       <c r="F35" t="n">
-        <v>46266445</v>
+        <v>40233097</v>
       </c>
       <c r="G35" t="n">
-        <v>-10.24997</v>
+        <v>1.61432</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.04587823</v>
+        <v>7.65</v>
       </c>
       <c r="E36" t="n">
-        <v>1447494423</v>
+        <v>1589465079</v>
       </c>
       <c r="F36" t="n">
-        <v>14169289</v>
+        <v>88098777</v>
       </c>
       <c r="G36" t="n">
-        <v>0.3569</v>
+        <v>0.17505</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>6.98</v>
+        <v>107.19</v>
       </c>
       <c r="E37" t="n">
-        <v>1438456139</v>
+        <v>1556857575</v>
       </c>
       <c r="F37" t="n">
-        <v>134118357</v>
+        <v>15915919</v>
       </c>
       <c r="G37" t="n">
-        <v>1.70374</v>
+        <v>1.35777</v>
       </c>
     </row>
     <row r="38">
@@ -1457,16 +1457,16 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.053854</v>
+        <v>0.059079</v>
       </c>
       <c r="E38" t="n">
-        <v>1406369027</v>
+        <v>1544761405</v>
       </c>
       <c r="F38" t="n">
-        <v>4073055</v>
+        <v>9708126</v>
       </c>
       <c r="G38" t="n">
-        <v>0.9067</v>
+        <v>0.69263</v>
       </c>
     </row>
     <row r="39">
@@ -1484,16 +1484,16 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1.013</v>
+        <v>1.12</v>
       </c>
       <c r="E39" t="n">
-        <v>1292434959</v>
+        <v>1428066049</v>
       </c>
       <c r="F39" t="n">
-        <v>97846537</v>
+        <v>189993603</v>
       </c>
       <c r="G39" t="n">
-        <v>1.34716</v>
+        <v>0.93971</v>
       </c>
     </row>
     <row r="40">
@@ -1511,16 +1511,16 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1.25</v>
+        <v>1.44</v>
       </c>
       <c r="E40" t="n">
-        <v>1152941419</v>
+        <v>1336181561</v>
       </c>
       <c r="F40" t="n">
-        <v>34779761</v>
+        <v>46751318</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.42269</v>
+        <v>1.02952</v>
       </c>
     </row>
     <row r="41">
@@ -1538,16 +1538,16 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.01510038</v>
+        <v>0.0183611</v>
       </c>
       <c r="E41" t="n">
-        <v>1097545815</v>
+        <v>1335366878</v>
       </c>
       <c r="F41" t="n">
-        <v>32461668</v>
+        <v>51254064</v>
       </c>
       <c r="G41" t="n">
-        <v>0.11249</v>
+        <v>-0.07312</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>USDP</t>
+          <t>AAVE</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Pax Dollar</t>
+          <t>Aave</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1.001</v>
+        <v>76.27</v>
       </c>
       <c r="E42" t="n">
-        <v>1007076455</v>
+        <v>1101005817</v>
       </c>
       <c r="F42" t="n">
-        <v>1216097</v>
+        <v>292426031</v>
       </c>
       <c r="G42" t="n">
-        <v>0.01424</v>
+        <v>32.00964</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>FRAX</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Frax</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.9991370000000001</v>
+        <v>0.114258</v>
       </c>
       <c r="E43" t="n">
-        <v>1002783822</v>
+        <v>1033879778</v>
       </c>
       <c r="F43" t="n">
-        <v>13972447</v>
+        <v>41695558</v>
       </c>
       <c r="G43" t="n">
-        <v>-0.10188</v>
+        <v>2.5478</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.101666</v>
+        <v>0.732878</v>
       </c>
       <c r="E44" t="n">
-        <v>915694293</v>
+        <v>1019377709</v>
       </c>
       <c r="F44" t="n">
-        <v>35304813</v>
+        <v>34354317</v>
       </c>
       <c r="G44" t="n">
-        <v>1.51025</v>
+        <v>-2.65856</v>
       </c>
     </row>
     <row r="45">
@@ -1646,16 +1646,16 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.118602</v>
+        <v>0.138993</v>
       </c>
       <c r="E45" t="n">
-        <v>858929426</v>
+        <v>1007806744</v>
       </c>
       <c r="F45" t="n">
-        <v>24930131</v>
+        <v>31973157</v>
       </c>
       <c r="G45" t="n">
-        <v>-1.56302</v>
+        <v>3.2671</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>RETH</t>
+          <t>FRAX</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Rocket Pool ETH</t>
+          <t>Frax</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>1864.18</v>
+        <v>0.999351</v>
       </c>
       <c r="E46" t="n">
-        <v>833174097</v>
+        <v>1002415962</v>
       </c>
       <c r="F46" t="n">
-        <v>2068802</v>
+        <v>7947944</v>
       </c>
       <c r="G46" t="n">
-        <v>-0.15891</v>
+        <v>-0.11412</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>RPL</t>
+          <t>USDP</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Rocket Pool</t>
+          <t>Pax Dollar</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>41.21</v>
+        <v>0.99935</v>
       </c>
       <c r="E47" t="n">
-        <v>801936794</v>
+        <v>999720595</v>
       </c>
       <c r="F47" t="n">
-        <v>3947950</v>
+        <v>1221012</v>
       </c>
       <c r="G47" t="n">
-        <v>-1.19626</v>
+        <v>-0.04413</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>RETH</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Rocket Pool ETH</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.572309</v>
+        <v>2060.91</v>
       </c>
       <c r="E48" t="n">
-        <v>793659211</v>
+        <v>945129497</v>
       </c>
       <c r="F48" t="n">
-        <v>26127467</v>
+        <v>2297779</v>
       </c>
       <c r="G48" t="n">
-        <v>-3.48531</v>
+        <v>1.10236</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>APE</t>
+          <t>EGLD</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ApeCoin</t>
+          <t>MultiversX</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>2.13</v>
+        <v>35.99</v>
       </c>
       <c r="E49" t="n">
-        <v>784794655</v>
+        <v>918222507</v>
       </c>
       <c r="F49" t="n">
-        <v>58858802</v>
+        <v>27069294</v>
       </c>
       <c r="G49" t="n">
-        <v>0.37583</v>
+        <v>6.69028</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>EGLD</t>
+          <t>FTM</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>MultiversX</t>
+          <t>Fantom</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>30.59</v>
+        <v>0.326793</v>
       </c>
       <c r="E50" t="n">
-        <v>782089156</v>
+        <v>916300078</v>
       </c>
       <c r="F50" t="n">
-        <v>9191552</v>
+        <v>122537258</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.27369</v>
+        <v>2.01302</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>FTM</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Fantom</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.273029</v>
+        <v>1.36</v>
       </c>
       <c r="E51" t="n">
-        <v>762847483</v>
+        <v>879222145</v>
       </c>
       <c r="F51" t="n">
-        <v>76183711</v>
+        <v>103883164</v>
       </c>
       <c r="G51" t="n">
-        <v>-0.90094</v>
+        <v>1.8078</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-07-02
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>30691</v>
+        <v>30557</v>
       </c>
       <c r="E2" t="n">
-        <v>595759907750</v>
+        <v>593304233415</v>
       </c>
       <c r="F2" t="n">
-        <v>12975786163</v>
+        <v>7198239265</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.03812</v>
+        <v>-0.10056</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1916.11</v>
+        <v>1919.94</v>
       </c>
       <c r="E3" t="n">
-        <v>230285731243</v>
+        <v>230729395706</v>
       </c>
       <c r="F3" t="n">
-        <v>7280425873</v>
+        <v>4514773379</v>
       </c>
       <c r="G3" t="n">
-        <v>1.02868</v>
+        <v>-0.32974</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0.999861</v>
       </c>
       <c r="E4" t="n">
-        <v>83130016547</v>
+        <v>83301420286</v>
       </c>
       <c r="F4" t="n">
-        <v>19416891910</v>
+        <v>11563905746</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.05126</v>
+        <v>-0.01214</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>239.95</v>
+        <v>245.63</v>
       </c>
       <c r="E5" t="n">
-        <v>37397549306</v>
+        <v>38277146235</v>
       </c>
       <c r="F5" t="n">
-        <v>766763641</v>
+        <v>788571915</v>
       </c>
       <c r="G5" t="n">
-        <v>-2.16308</v>
+        <v>0.81976</v>
       </c>
     </row>
     <row r="6">
@@ -596,13 +596,13 @@
         <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>28436790925</v>
+        <v>27371288118</v>
       </c>
       <c r="F6" t="n">
-        <v>3155463040</v>
+        <v>2063985824</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.00446</v>
+        <v>-0.06133</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.491939</v>
+        <v>0.478886</v>
       </c>
       <c r="E7" t="n">
-        <v>25713728479</v>
+        <v>25039187413</v>
       </c>
       <c r="F7" t="n">
-        <v>542038095</v>
+        <v>671369535</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.1495</v>
+        <v>1.47385</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1912.08</v>
+        <v>1919.32</v>
       </c>
       <c r="E8" t="n">
-        <v>14141089162</v>
+        <v>14446035044</v>
       </c>
       <c r="F8" t="n">
-        <v>2000483</v>
+        <v>1343687</v>
       </c>
       <c r="G8" t="n">
-        <v>0.81103</v>
+        <v>-0.39787</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.297543</v>
+        <v>0.29049</v>
       </c>
       <c r="E9" t="n">
-        <v>10433002658</v>
+        <v>10178271841</v>
       </c>
       <c r="F9" t="n">
-        <v>210087347</v>
+        <v>167533435</v>
       </c>
       <c r="G9" t="n">
-        <v>0.56745</v>
+        <v>0.66413</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.06768399999999999</v>
+        <v>0.06725100000000001</v>
       </c>
       <c r="E10" t="n">
-        <v>9468276785</v>
+        <v>9429648540</v>
       </c>
       <c r="F10" t="n">
-        <v>243364562</v>
+        <v>335909511</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.43341</v>
+        <v>-1.21056</v>
       </c>
     </row>
     <row r="11">
@@ -719,25 +719,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SOL</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Solana</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>17.21</v>
+        <v>110.92</v>
       </c>
       <c r="E11" t="n">
-        <v>6887534070</v>
+        <v>8137896891</v>
       </c>
       <c r="F11" t="n">
-        <v>248616422</v>
+        <v>1589312202</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.61104</v>
+        <v>3.86075</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +746,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>SOL</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Solana</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.073522</v>
+        <v>19.04</v>
       </c>
       <c r="E12" t="n">
-        <v>6603860079</v>
+        <v>7642140711</v>
       </c>
       <c r="F12" t="n">
-        <v>246993465</v>
+        <v>354930866</v>
       </c>
       <c r="G12" t="n">
-        <v>1.38104</v>
+        <v>3.31162</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>88.84</v>
+        <v>0.075729</v>
       </c>
       <c r="E13" t="n">
-        <v>6507691635</v>
+        <v>6805182509</v>
       </c>
       <c r="F13" t="n">
-        <v>587917523</v>
+        <v>239364760</v>
       </c>
       <c r="G13" t="n">
-        <v>-2.40692</v>
+        <v>-2.49318</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>5.19</v>
+        <v>5.29</v>
       </c>
       <c r="E14" t="n">
-        <v>6456630286</v>
+        <v>6608382738</v>
       </c>
       <c r="F14" t="n">
-        <v>127399249</v>
+        <v>111315656</v>
       </c>
       <c r="G14" t="n">
-        <v>2.67859</v>
+        <v>-0.79614</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.672648</v>
+        <v>0.671883</v>
       </c>
       <c r="E15" t="n">
-        <v>6251692478</v>
+        <v>6256783103</v>
       </c>
       <c r="F15" t="n">
-        <v>228944836</v>
+        <v>164193079</v>
       </c>
       <c r="G15" t="n">
-        <v>-1.10279</v>
+        <v>1.35651</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>30646</v>
+        <v>302.06</v>
       </c>
       <c r="E16" t="n">
-        <v>4818705018</v>
+        <v>5833727668</v>
       </c>
       <c r="F16" t="n">
-        <v>151713562</v>
+        <v>1385395110</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.27449</v>
+        <v>2.57902</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>7.95e-06</v>
+        <v>30579</v>
       </c>
       <c r="E17" t="n">
-        <v>4681027830</v>
+        <v>4796973137</v>
       </c>
       <c r="F17" t="n">
-        <v>116390454</v>
+        <v>49181943</v>
       </c>
       <c r="G17" t="n">
-        <v>-1.15743</v>
+        <v>-0.03221</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>13.55</v>
+        <v>12.99</v>
       </c>
       <c r="E18" t="n">
-        <v>4677112416</v>
+        <v>4488750007</v>
       </c>
       <c r="F18" t="n">
-        <v>139895444</v>
+        <v>104811171</v>
       </c>
       <c r="G18" t="n">
-        <v>2.69807</v>
+        <v>0.04742</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>7.57e-06</v>
       </c>
       <c r="E19" t="n">
-        <v>4450286885</v>
+        <v>4467585055</v>
       </c>
       <c r="F19" t="n">
-        <v>87921293</v>
+        <v>77714208</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.07027</v>
+        <v>-0.53167</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Binance USD</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>0.9994769999999999</v>
       </c>
       <c r="E20" t="n">
-        <v>4244868393</v>
+        <v>4344063201</v>
       </c>
       <c r="F20" t="n">
-        <v>2106858046</v>
+        <v>85636279</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.05094</v>
+        <v>-0.04935</v>
       </c>
     </row>
     <row r="21">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>5.38</v>
+        <v>5.66</v>
       </c>
       <c r="E21" t="n">
-        <v>4030766043</v>
+        <v>4259258962</v>
       </c>
       <c r="F21" t="n">
-        <v>109292465</v>
+        <v>90815224</v>
       </c>
       <c r="G21" t="n">
-        <v>11.56179</v>
+        <v>5.29538</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Binance USD</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>200.98</v>
+        <v>1</v>
       </c>
       <c r="E22" t="n">
-        <v>3905237719</v>
+        <v>4133551057</v>
       </c>
       <c r="F22" t="n">
-        <v>1363922665</v>
+        <v>1358327819</v>
       </c>
       <c r="G22" t="n">
-        <v>3.75765</v>
+        <v>0.01817</v>
       </c>
     </row>
     <row r="23">
@@ -1052,16 +1052,16 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>3.84</v>
+        <v>3.96</v>
       </c>
       <c r="E23" t="n">
-        <v>3571855159</v>
+        <v>3671042216</v>
       </c>
       <c r="F23" t="n">
-        <v>713801</v>
+        <v>1022295</v>
       </c>
       <c r="G23" t="n">
-        <v>-1.00332</v>
+        <v>-2.29074</v>
       </c>
     </row>
     <row r="24">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>6.3</v>
+        <v>6.5</v>
       </c>
       <c r="E24" t="n">
-        <v>3262044470</v>
+        <v>3375016207</v>
       </c>
       <c r="F24" t="n">
-        <v>166878918</v>
+        <v>197370895</v>
       </c>
       <c r="G24" t="n">
-        <v>2.4205</v>
+        <v>3.93766</v>
       </c>
     </row>
     <row r="25">
@@ -1106,16 +1106,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.99897</v>
+        <v>0.999413</v>
       </c>
       <c r="E25" t="n">
-        <v>3135245545</v>
+        <v>3054753793</v>
       </c>
       <c r="F25" t="n">
-        <v>189437775</v>
+        <v>776243138</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.10681</v>
+        <v>-0.21021</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>165.52</v>
+        <v>164.92</v>
       </c>
       <c r="E26" t="n">
-        <v>3011967273</v>
+        <v>2989837150</v>
       </c>
       <c r="F26" t="n">
-        <v>95791616</v>
+        <v>49900901</v>
       </c>
       <c r="G26" t="n">
-        <v>6.16086</v>
+        <v>-2.25734</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>9.66</v>
+        <v>0.107042</v>
       </c>
       <c r="E27" t="n">
-        <v>2822832048</v>
+        <v>2903629265</v>
       </c>
       <c r="F27" t="n">
-        <v>164204223</v>
+        <v>59296217</v>
       </c>
       <c r="G27" t="n">
-        <v>2.52374</v>
+        <v>-0.59162</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>44.96</v>
+        <v>20.32</v>
       </c>
       <c r="E28" t="n">
-        <v>2705385551</v>
+        <v>2878173197</v>
       </c>
       <c r="F28" t="n">
-        <v>4718709</v>
+        <v>307572866</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.34113</v>
+        <v>-5.09377</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>18.9</v>
+        <v>9.48</v>
       </c>
       <c r="E29" t="n">
-        <v>2672922535</v>
+        <v>2778027710</v>
       </c>
       <c r="F29" t="n">
-        <v>243135797</v>
+        <v>78016681</v>
       </c>
       <c r="G29" t="n">
-        <v>-1.32338</v>
+        <v>1.17496</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.091516</v>
+        <v>44.39</v>
       </c>
       <c r="E30" t="n">
-        <v>2466137755</v>
+        <v>2662361327</v>
       </c>
       <c r="F30" t="n">
-        <v>42374487</v>
+        <v>2753550</v>
       </c>
       <c r="G30" t="n">
-        <v>0.42965</v>
+        <v>0.0523</v>
       </c>
     </row>
     <row r="31">
@@ -1268,16 +1268,16 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>1.48</v>
+        <v>1.4</v>
       </c>
       <c r="E31" t="n">
-        <v>2175995111</v>
+        <v>2060300592</v>
       </c>
       <c r="F31" t="n">
-        <v>8993026</v>
+        <v>8861564</v>
       </c>
       <c r="G31" t="n">
-        <v>5.49221</v>
+        <v>2.11258</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>4.36</v>
+        <v>2.11</v>
       </c>
       <c r="E32" t="n">
-        <v>1910550258</v>
+        <v>1859321263</v>
       </c>
       <c r="F32" t="n">
-        <v>14987941</v>
+        <v>33726878</v>
       </c>
       <c r="G32" t="n">
-        <v>0.67437</v>
+        <v>0.13053</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>4.08</v>
+        <v>4.16</v>
       </c>
       <c r="E33" t="n">
-        <v>1757764243</v>
+        <v>1819294894</v>
       </c>
       <c r="F33" t="n">
-        <v>91776724</v>
+        <v>11382004</v>
       </c>
       <c r="G33" t="n">
-        <v>1.22967</v>
+        <v>-0.50182</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>1.97</v>
+        <v>4.06</v>
       </c>
       <c r="E34" t="n">
-        <v>1728499971</v>
+        <v>1756180896</v>
       </c>
       <c r="F34" t="n">
-        <v>38411138</v>
+        <v>114486893</v>
       </c>
       <c r="G34" t="n">
-        <v>3.06545</v>
+        <v>1.41531</v>
       </c>
     </row>
     <row r="35">
@@ -1376,16 +1376,16 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.053137</v>
+        <v>0.050221</v>
       </c>
       <c r="E35" t="n">
-        <v>1685966481</v>
+        <v>1619633027</v>
       </c>
       <c r="F35" t="n">
-        <v>40233097</v>
+        <v>14670162</v>
       </c>
       <c r="G35" t="n">
-        <v>1.61432</v>
+        <v>-0.61434</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>7.65</v>
+        <v>111.03</v>
       </c>
       <c r="E36" t="n">
-        <v>1589465079</v>
+        <v>1618370663</v>
       </c>
       <c r="F36" t="n">
-        <v>88098777</v>
+        <v>13324579</v>
       </c>
       <c r="G36" t="n">
-        <v>0.17505</v>
+        <v>0.34708</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>107.19</v>
+        <v>7.28</v>
       </c>
       <c r="E37" t="n">
-        <v>1556857575</v>
+        <v>1521084062</v>
       </c>
       <c r="F37" t="n">
-        <v>15915919</v>
+        <v>50360207</v>
       </c>
       <c r="G37" t="n">
-        <v>1.35777</v>
+        <v>0.64051</v>
       </c>
     </row>
     <row r="38">
@@ -1457,16 +1457,16 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.059079</v>
+        <v>0.056742</v>
       </c>
       <c r="E38" t="n">
-        <v>1544761405</v>
+        <v>1483568361</v>
       </c>
       <c r="F38" t="n">
-        <v>9708126</v>
+        <v>5532221</v>
       </c>
       <c r="G38" t="n">
-        <v>0.69263</v>
+        <v>-0.17889</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1.12</v>
+        <v>0.02028219</v>
       </c>
       <c r="E39" t="n">
-        <v>1428066049</v>
+        <v>1475395441</v>
       </c>
       <c r="F39" t="n">
-        <v>189993603</v>
+        <v>51341100</v>
       </c>
       <c r="G39" t="n">
-        <v>0.93971</v>
+        <v>-3.59616</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1.44</v>
+        <v>1.14</v>
       </c>
       <c r="E40" t="n">
-        <v>1336181561</v>
+        <v>1453902685</v>
       </c>
       <c r="F40" t="n">
-        <v>46751318</v>
+        <v>130353211</v>
       </c>
       <c r="G40" t="n">
-        <v>1.02952</v>
+        <v>-1.36545</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.0183611</v>
+        <v>1.46</v>
       </c>
       <c r="E41" t="n">
-        <v>1335366878</v>
+        <v>1355731029</v>
       </c>
       <c r="F41" t="n">
-        <v>51254064</v>
+        <v>58594434</v>
       </c>
       <c r="G41" t="n">
-        <v>-0.07312</v>
+        <v>5.41721</v>
       </c>
     </row>
     <row r="42">
@@ -1565,16 +1565,16 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>76.27</v>
+        <v>71.56999999999999</v>
       </c>
       <c r="E42" t="n">
-        <v>1101005817</v>
+        <v>1038801939</v>
       </c>
       <c r="F42" t="n">
-        <v>292426031</v>
+        <v>108421113</v>
       </c>
       <c r="G42" t="n">
-        <v>32.00964</v>
+        <v>5.23283</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>FRAX</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Frax</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.114258</v>
+        <v>0.999134</v>
       </c>
       <c r="E43" t="n">
-        <v>1033879778</v>
+        <v>1002564181</v>
       </c>
       <c r="F43" t="n">
-        <v>41695558</v>
+        <v>3824535</v>
       </c>
       <c r="G43" t="n">
-        <v>2.5478</v>
+        <v>-0.05847</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.732878</v>
+        <v>0.109234</v>
       </c>
       <c r="E44" t="n">
-        <v>1019377709</v>
+        <v>996932030</v>
       </c>
       <c r="F44" t="n">
-        <v>34354317</v>
+        <v>47827544</v>
       </c>
       <c r="G44" t="n">
-        <v>-2.65856</v>
+        <v>3.17619</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ALGO</t>
+          <t>USDP</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Algorand</t>
+          <t>Pax Dollar</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.138993</v>
+        <v>1</v>
       </c>
       <c r="E45" t="n">
-        <v>1007806744</v>
+        <v>987674495</v>
       </c>
       <c r="F45" t="n">
-        <v>31973157</v>
+        <v>102178234</v>
       </c>
       <c r="G45" t="n">
-        <v>3.2671</v>
+        <v>0.05945</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>FRAX</t>
+          <t>RETH</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Frax</t>
+          <t>Rocket Pool ETH</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.999351</v>
+        <v>2065.81</v>
       </c>
       <c r="E46" t="n">
-        <v>1002415962</v>
+        <v>954468568</v>
       </c>
       <c r="F46" t="n">
-        <v>7947944</v>
+        <v>1436531</v>
       </c>
       <c r="G46" t="n">
-        <v>-0.11412</v>
+        <v>-0.34163</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>USDP</t>
+          <t>BSV</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Pax Dollar</t>
+          <t>Bitcoin SV</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.99935</v>
+        <v>49.48</v>
       </c>
       <c r="E47" t="n">
-        <v>999720595</v>
+        <v>954284320</v>
       </c>
       <c r="F47" t="n">
-        <v>1221012</v>
+        <v>94396984</v>
       </c>
       <c r="G47" t="n">
-        <v>-0.04413</v>
+        <v>-1.79127</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>RETH</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Rocket Pool ETH</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>2060.91</v>
+        <v>0.683177</v>
       </c>
       <c r="E48" t="n">
-        <v>945129497</v>
+        <v>951441071</v>
       </c>
       <c r="F48" t="n">
-        <v>2297779</v>
+        <v>18053415</v>
       </c>
       <c r="G48" t="n">
-        <v>1.10236</v>
+        <v>0.61628</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>EGLD</t>
+          <t>ALGO</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>MultiversX</t>
+          <t>Algorand</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>35.99</v>
+        <v>0.123727</v>
       </c>
       <c r="E49" t="n">
-        <v>918222507</v>
+        <v>915147177</v>
       </c>
       <c r="F49" t="n">
-        <v>27069294</v>
+        <v>44120063</v>
       </c>
       <c r="G49" t="n">
-        <v>6.69028</v>
+        <v>1.33658</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>FTM</t>
+          <t>EGLD</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Fantom</t>
+          <t>MultiversX</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.326793</v>
+        <v>35.12</v>
       </c>
       <c r="E50" t="n">
-        <v>916300078</v>
+        <v>901038904</v>
       </c>
       <c r="F50" t="n">
-        <v>122537258</v>
+        <v>8997558</v>
       </c>
       <c r="G50" t="n">
-        <v>2.01302</v>
+        <v>-0.25455</v>
       </c>
     </row>
     <row r="51">
@@ -1808,16 +1808,16 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>1.36</v>
+        <v>1.33</v>
       </c>
       <c r="E51" t="n">
-        <v>879222145</v>
+        <v>859639200</v>
       </c>
       <c r="F51" t="n">
-        <v>103883164</v>
+        <v>70041934</v>
       </c>
       <c r="G51" t="n">
-        <v>1.8078</v>
+        <v>-1.69323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-07-09
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>30557</v>
+        <v>30271</v>
       </c>
       <c r="E2" t="n">
-        <v>593304233415</v>
+        <v>588036487030</v>
       </c>
       <c r="F2" t="n">
-        <v>7198239265</v>
+        <v>2830314328</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.10056</v>
+        <v>0.25133</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1919.94</v>
+        <v>1869.2</v>
       </c>
       <c r="E3" t="n">
-        <v>230729395706</v>
+        <v>224695169815</v>
       </c>
       <c r="F3" t="n">
-        <v>4514773379</v>
+        <v>4691237029</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.32974</v>
+        <v>0.55328</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999861</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>83301420286</v>
+        <v>83382209358</v>
       </c>
       <c r="F4" t="n">
-        <v>11563905746</v>
+        <v>11307100051</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.01214</v>
+        <v>-0.02426</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>245.63</v>
+        <v>234.76</v>
       </c>
       <c r="E5" t="n">
-        <v>38277146235</v>
+        <v>36590426871</v>
       </c>
       <c r="F5" t="n">
-        <v>788571915</v>
+        <v>280690954</v>
       </c>
       <c r="G5" t="n">
-        <v>0.81976</v>
+        <v>-0.5875</v>
       </c>
     </row>
     <row r="6">
@@ -596,13 +596,13 @@
         <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>27371288118</v>
+        <v>27508838298</v>
       </c>
       <c r="F6" t="n">
-        <v>2063985824</v>
+        <v>1791758569</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.06133</v>
+        <v>0.00314</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.478886</v>
+        <v>0.469274</v>
       </c>
       <c r="E7" t="n">
-        <v>25039187413</v>
+        <v>24521869218</v>
       </c>
       <c r="F7" t="n">
-        <v>671369535</v>
+        <v>299284846</v>
       </c>
       <c r="G7" t="n">
-        <v>1.47385</v>
+        <v>0.35015</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1919.32</v>
+        <v>1868.78</v>
       </c>
       <c r="E8" t="n">
-        <v>14446035044</v>
+        <v>14229098867</v>
       </c>
       <c r="F8" t="n">
-        <v>1343687</v>
+        <v>12222143</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.39787</v>
+        <v>0.57869</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.29049</v>
+        <v>0.286559</v>
       </c>
       <c r="E9" t="n">
-        <v>10178271841</v>
+        <v>10042580816</v>
       </c>
       <c r="F9" t="n">
-        <v>167533435</v>
+        <v>157542023</v>
       </c>
       <c r="G9" t="n">
-        <v>0.66413</v>
+        <v>0.17597</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.06725100000000001</v>
+        <v>0.065873</v>
       </c>
       <c r="E10" t="n">
-        <v>9429648540</v>
+        <v>9228668745</v>
       </c>
       <c r="F10" t="n">
-        <v>335909511</v>
+        <v>156099951</v>
       </c>
       <c r="G10" t="n">
-        <v>-1.21056</v>
+        <v>0.78345</v>
       </c>
     </row>
     <row r="11">
@@ -719,25 +719,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>SOL</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Solana</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>110.92</v>
+        <v>21.6</v>
       </c>
       <c r="E11" t="n">
-        <v>8137896891</v>
+        <v>8689837815</v>
       </c>
       <c r="F11" t="n">
-        <v>1589312202</v>
+        <v>436603738</v>
       </c>
       <c r="G11" t="n">
-        <v>3.86075</v>
+        <v>-0.94263</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +746,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SOL</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Solana</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>19.04</v>
+        <v>0.07945000000000001</v>
       </c>
       <c r="E12" t="n">
-        <v>7642140711</v>
+        <v>7138337119</v>
       </c>
       <c r="F12" t="n">
-        <v>354930866</v>
+        <v>278732944</v>
       </c>
       <c r="G12" t="n">
-        <v>3.31162</v>
+        <v>0.28291</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.075729</v>
+        <v>96.31999999999999</v>
       </c>
       <c r="E13" t="n">
-        <v>6805182509</v>
+        <v>7062696026</v>
       </c>
       <c r="F13" t="n">
-        <v>239364760</v>
+        <v>729982986</v>
       </c>
       <c r="G13" t="n">
-        <v>-2.49318</v>
+        <v>-0.7025</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>5.29</v>
+        <v>0.695423</v>
       </c>
       <c r="E14" t="n">
-        <v>6608382738</v>
+        <v>6480679156</v>
       </c>
       <c r="F14" t="n">
-        <v>111315656</v>
+        <v>157131027</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.79614</v>
+        <v>2.11276</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.671883</v>
+        <v>5.1</v>
       </c>
       <c r="E15" t="n">
-        <v>6256783103</v>
+        <v>6386024860</v>
       </c>
       <c r="F15" t="n">
-        <v>164193079</v>
+        <v>68629444</v>
       </c>
       <c r="G15" t="n">
-        <v>1.35651</v>
+        <v>-1.17097</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>302.06</v>
+        <v>268.28</v>
       </c>
       <c r="E16" t="n">
-        <v>5833727668</v>
+        <v>5216489459</v>
       </c>
       <c r="F16" t="n">
-        <v>1385395110</v>
+        <v>370646872</v>
       </c>
       <c r="G16" t="n">
-        <v>2.57902</v>
+        <v>-0.46994</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>30579</v>
+        <v>14.08</v>
       </c>
       <c r="E17" t="n">
-        <v>4796973137</v>
+        <v>4868564536</v>
       </c>
       <c r="F17" t="n">
-        <v>49181943</v>
+        <v>217089971</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.03221</v>
+        <v>4.06899</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>12.99</v>
+        <v>30266</v>
       </c>
       <c r="E18" t="n">
-        <v>4488750007</v>
+        <v>4767058142</v>
       </c>
       <c r="F18" t="n">
-        <v>104811171</v>
+        <v>37987294</v>
       </c>
       <c r="G18" t="n">
-        <v>0.04742</v>
+        <v>0.22669</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>7.57e-06</v>
+        <v>7.75e-06</v>
       </c>
       <c r="E19" t="n">
-        <v>4467585055</v>
+        <v>4581348393</v>
       </c>
       <c r="F19" t="n">
-        <v>77714208</v>
+        <v>136193478</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.53167</v>
+        <v>5.43671</v>
       </c>
     </row>
     <row r="20">
@@ -971,16 +971,16 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.9994769999999999</v>
+        <v>0.999682</v>
       </c>
       <c r="E20" t="n">
-        <v>4344063201</v>
+        <v>4295568989</v>
       </c>
       <c r="F20" t="n">
-        <v>85636279</v>
+        <v>56144781</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.04935</v>
+        <v>0.01237</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Binance USD</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>5.66</v>
+        <v>0.999781</v>
       </c>
       <c r="E21" t="n">
-        <v>4259258962</v>
+        <v>4045267938</v>
       </c>
       <c r="F21" t="n">
-        <v>90815224</v>
+        <v>2184349579</v>
       </c>
       <c r="G21" t="n">
-        <v>5.29538</v>
+        <v>0.0764</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Binance USD</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>5.26</v>
       </c>
       <c r="E22" t="n">
-        <v>4133551057</v>
+        <v>3966710646</v>
       </c>
       <c r="F22" t="n">
-        <v>1358327819</v>
+        <v>68892017</v>
       </c>
       <c r="G22" t="n">
-        <v>0.01817</v>
+        <v>-0.98258</v>
       </c>
     </row>
     <row r="23">
@@ -1052,16 +1052,16 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>3.96</v>
+        <v>3.83</v>
       </c>
       <c r="E23" t="n">
-        <v>3671042216</v>
+        <v>3556172755</v>
       </c>
       <c r="F23" t="n">
-        <v>1022295</v>
+        <v>1548675</v>
       </c>
       <c r="G23" t="n">
-        <v>-2.29074</v>
+        <v>-0.82997</v>
       </c>
     </row>
     <row r="24">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>6.5</v>
+        <v>6.2</v>
       </c>
       <c r="E24" t="n">
-        <v>3375016207</v>
+        <v>3208289369</v>
       </c>
       <c r="F24" t="n">
-        <v>197370895</v>
+        <v>85341069</v>
       </c>
       <c r="G24" t="n">
-        <v>3.93766</v>
+        <v>0.38062</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.999413</v>
+        <v>167.43</v>
       </c>
       <c r="E25" t="n">
-        <v>3054753793</v>
+        <v>3038666908</v>
       </c>
       <c r="F25" t="n">
-        <v>776243138</v>
+        <v>62787149</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.21021</v>
+        <v>0.24568</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>TUSD</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>164.92</v>
+        <v>0.9996969999999999</v>
       </c>
       <c r="E26" t="n">
-        <v>2989837150</v>
+        <v>2944752923</v>
       </c>
       <c r="F26" t="n">
-        <v>49900901</v>
+        <v>939878320</v>
       </c>
       <c r="G26" t="n">
-        <v>-2.25734</v>
+        <v>0.00602</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.107042</v>
+        <v>9.359999999999999</v>
       </c>
       <c r="E27" t="n">
-        <v>2903629265</v>
+        <v>2739496377</v>
       </c>
       <c r="F27" t="n">
-        <v>59296217</v>
+        <v>64654227</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.59162</v>
+        <v>1.49827</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>20.32</v>
+        <v>0.098839</v>
       </c>
       <c r="E28" t="n">
-        <v>2878173197</v>
+        <v>2673991879</v>
       </c>
       <c r="F28" t="n">
-        <v>307572866</v>
+        <v>42479530</v>
       </c>
       <c r="G28" t="n">
-        <v>-5.09377</v>
+        <v>0.39792</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>9.48</v>
+        <v>18.84</v>
       </c>
       <c r="E29" t="n">
-        <v>2778027710</v>
+        <v>2672936077</v>
       </c>
       <c r="F29" t="n">
-        <v>78016681</v>
+        <v>76444042</v>
       </c>
       <c r="G29" t="n">
-        <v>1.17496</v>
+        <v>-0.1113</v>
       </c>
     </row>
     <row r="30">
@@ -1241,16 +1241,16 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>44.39</v>
+        <v>42.88</v>
       </c>
       <c r="E30" t="n">
-        <v>2662361327</v>
+        <v>2572674305</v>
       </c>
       <c r="F30" t="n">
-        <v>2753550</v>
+        <v>1209900</v>
       </c>
       <c r="G30" t="n">
-        <v>0.0523</v>
+        <v>0.62358</v>
       </c>
     </row>
     <row r="31">
@@ -1268,16 +1268,16 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>1.4</v>
+        <v>1.36</v>
       </c>
       <c r="E31" t="n">
-        <v>2060300592</v>
+        <v>2012621476</v>
       </c>
       <c r="F31" t="n">
-        <v>8861564</v>
+        <v>6785348</v>
       </c>
       <c r="G31" t="n">
-        <v>2.11258</v>
+        <v>-1.30378</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>2.11</v>
+        <v>4.33</v>
       </c>
       <c r="E32" t="n">
-        <v>1859321263</v>
+        <v>1880279223</v>
       </c>
       <c r="F32" t="n">
-        <v>33726878</v>
+        <v>64236209</v>
       </c>
       <c r="G32" t="n">
-        <v>0.13053</v>
+        <v>-0.66376</v>
       </c>
     </row>
     <row r="33">
@@ -1322,16 +1322,16 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>4.16</v>
+        <v>4.06</v>
       </c>
       <c r="E33" t="n">
-        <v>1819294894</v>
+        <v>1776295710</v>
       </c>
       <c r="F33" t="n">
-        <v>11382004</v>
+        <v>10474983</v>
       </c>
       <c r="G33" t="n">
-        <v>-0.50182</v>
+        <v>0.28856</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>4.06</v>
+        <v>1.95</v>
       </c>
       <c r="E34" t="n">
-        <v>1756180896</v>
+        <v>1716789854</v>
       </c>
       <c r="F34" t="n">
-        <v>114486893</v>
+        <v>14448684</v>
       </c>
       <c r="G34" t="n">
-        <v>1.41531</v>
+        <v>-0.61533</v>
       </c>
     </row>
     <row r="35">
@@ -1376,16 +1376,16 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.050221</v>
+        <v>0.04710601</v>
       </c>
       <c r="E35" t="n">
-        <v>1619633027</v>
+        <v>1520906159</v>
       </c>
       <c r="F35" t="n">
-        <v>14670162</v>
+        <v>11022242</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.61434</v>
+        <v>0.08827</v>
       </c>
     </row>
     <row r="36">
@@ -1403,16 +1403,16 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>111.03</v>
+        <v>102.49</v>
       </c>
       <c r="E36" t="n">
-        <v>1618370663</v>
+        <v>1491014062</v>
       </c>
       <c r="F36" t="n">
-        <v>13324579</v>
+        <v>10162331</v>
       </c>
       <c r="G36" t="n">
-        <v>0.34708</v>
+        <v>-0.81063</v>
       </c>
     </row>
     <row r="37">
@@ -1430,16 +1430,16 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>7.28</v>
+        <v>7.1</v>
       </c>
       <c r="E37" t="n">
-        <v>1521084062</v>
+        <v>1489407950</v>
       </c>
       <c r="F37" t="n">
-        <v>50360207</v>
+        <v>53610404</v>
       </c>
       <c r="G37" t="n">
-        <v>0.64051</v>
+        <v>-0.92474</v>
       </c>
     </row>
     <row r="38">
@@ -1457,16 +1457,16 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.056742</v>
+        <v>0.056804</v>
       </c>
       <c r="E38" t="n">
-        <v>1483568361</v>
+        <v>1485486803</v>
       </c>
       <c r="F38" t="n">
-        <v>5532221</v>
+        <v>3786181</v>
       </c>
       <c r="G38" t="n">
-        <v>-0.17889</v>
+        <v>0.62022</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.02028219</v>
+        <v>1.13</v>
       </c>
       <c r="E39" t="n">
-        <v>1475395441</v>
+        <v>1445281418</v>
       </c>
       <c r="F39" t="n">
-        <v>51341100</v>
+        <v>103634211</v>
       </c>
       <c r="G39" t="n">
-        <v>-3.59616</v>
+        <v>0.3552</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1.14</v>
+        <v>0.01868981</v>
       </c>
       <c r="E40" t="n">
-        <v>1453902685</v>
+        <v>1359078423</v>
       </c>
       <c r="F40" t="n">
-        <v>130353211</v>
+        <v>31871732</v>
       </c>
       <c r="G40" t="n">
-        <v>-1.36545</v>
+        <v>-0.34258</v>
       </c>
     </row>
     <row r="41">
@@ -1538,16 +1538,16 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1.46</v>
+        <v>1.33</v>
       </c>
       <c r="E41" t="n">
-        <v>1355731029</v>
+        <v>1241815875</v>
       </c>
       <c r="F41" t="n">
-        <v>58594434</v>
+        <v>44290185</v>
       </c>
       <c r="G41" t="n">
-        <v>5.41721</v>
+        <v>-3.09645</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>AAVE</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Aave</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>71.56999999999999</v>
+        <v>0.114577</v>
       </c>
       <c r="E42" t="n">
-        <v>1038801939</v>
+        <v>1043481205</v>
       </c>
       <c r="F42" t="n">
-        <v>108421113</v>
+        <v>18369847</v>
       </c>
       <c r="G42" t="n">
-        <v>5.23283</v>
+        <v>-2.47137</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>FRAX</t>
+          <t>AAVE</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Frax</t>
+          <t>Aave</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.999134</v>
+        <v>71.7</v>
       </c>
       <c r="E43" t="n">
-        <v>1002564181</v>
+        <v>1036823892</v>
       </c>
       <c r="F43" t="n">
-        <v>3824535</v>
+        <v>58130553</v>
       </c>
       <c r="G43" t="n">
-        <v>-0.05847</v>
+        <v>-5.10367</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>FRAX</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Frax</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.109234</v>
+        <v>0.99892</v>
       </c>
       <c r="E44" t="n">
-        <v>996932030</v>
+        <v>1003190654</v>
       </c>
       <c r="F44" t="n">
-        <v>47827544</v>
+        <v>4275913</v>
       </c>
       <c r="G44" t="n">
-        <v>3.17619</v>
+        <v>0.04946</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>USDP</t>
+          <t>RETH</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Pax Dollar</t>
+          <t>Rocket Pool ETH</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>1</v>
+        <v>2012.76</v>
       </c>
       <c r="E45" t="n">
-        <v>987674495</v>
+        <v>940280631</v>
       </c>
       <c r="F45" t="n">
-        <v>102178234</v>
+        <v>698388</v>
       </c>
       <c r="G45" t="n">
-        <v>0.05945</v>
+        <v>0.55771</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>RETH</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Rocket Pool ETH</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>2065.81</v>
+        <v>0.64361</v>
       </c>
       <c r="E46" t="n">
-        <v>954468568</v>
+        <v>895000675</v>
       </c>
       <c r="F46" t="n">
-        <v>1436531</v>
+        <v>8849550</v>
       </c>
       <c r="G46" t="n">
-        <v>-0.34163</v>
+        <v>-0.43981</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>BSV</t>
+          <t>EGLD</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Bitcoin SV</t>
+          <t>MultiversX</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>49.48</v>
+        <v>34.49</v>
       </c>
       <c r="E47" t="n">
-        <v>954284320</v>
+        <v>884951931</v>
       </c>
       <c r="F47" t="n">
-        <v>94396984</v>
+        <v>6261926</v>
       </c>
       <c r="G47" t="n">
-        <v>-1.79127</v>
+        <v>1.2078</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>ALGO</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Algorand</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.683177</v>
+        <v>0.111579</v>
       </c>
       <c r="E48" t="n">
-        <v>951441071</v>
+        <v>845229390</v>
       </c>
       <c r="F48" t="n">
-        <v>18053415</v>
+        <v>22908520</v>
       </c>
       <c r="G48" t="n">
-        <v>0.61628</v>
+        <v>-0.05091</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ALGO</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Algorand</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.123727</v>
+        <v>915.73</v>
       </c>
       <c r="E49" t="n">
-        <v>915147177</v>
+        <v>825393175</v>
       </c>
       <c r="F49" t="n">
-        <v>44120063</v>
+        <v>35168653</v>
       </c>
       <c r="G49" t="n">
-        <v>1.33658</v>
+        <v>-4.52713</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>EGLD</t>
+          <t>EOS</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>MultiversX</t>
+          <t>EOS</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>35.12</v>
+        <v>0.732386</v>
       </c>
       <c r="E50" t="n">
-        <v>901038904</v>
+        <v>814539108</v>
       </c>
       <c r="F50" t="n">
-        <v>8997558</v>
+        <v>93094383</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.25455</v>
+        <v>1.83906</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>BSV</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Bitcoin SV</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>1.33</v>
+        <v>40.74</v>
       </c>
       <c r="E51" t="n">
-        <v>859639200</v>
+        <v>784863474</v>
       </c>
       <c r="F51" t="n">
-        <v>70041934</v>
+        <v>17431619</v>
       </c>
       <c r="G51" t="n">
-        <v>-1.69323</v>
+        <v>-1.87153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-07-16
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>30271</v>
+        <v>30343</v>
       </c>
       <c r="E2" t="n">
-        <v>588036487030</v>
+        <v>589544684001</v>
       </c>
       <c r="F2" t="n">
-        <v>2830314328</v>
+        <v>6019402119</v>
       </c>
       <c r="G2" t="n">
-        <v>0.25133</v>
+        <v>0.00332</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1869.2</v>
+        <v>1935.52</v>
       </c>
       <c r="E3" t="n">
-        <v>224695169815</v>
+        <v>232618512297</v>
       </c>
       <c r="F3" t="n">
-        <v>4691237029</v>
+        <v>4230895730</v>
       </c>
       <c r="G3" t="n">
-        <v>0.55328</v>
+        <v>-0.24192</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>1.001</v>
       </c>
       <c r="E4" t="n">
-        <v>83382209358</v>
+        <v>83669568053</v>
       </c>
       <c r="F4" t="n">
-        <v>11307100051</v>
+        <v>12470789930</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.02426</v>
+        <v>-0.01269</v>
       </c>
     </row>
     <row r="5">
@@ -557,25 +557,25 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BNB</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>BNB</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>234.76</v>
+        <v>0.751406</v>
       </c>
       <c r="E5" t="n">
-        <v>36590426871</v>
+        <v>39485209298</v>
       </c>
       <c r="F5" t="n">
-        <v>280690954</v>
+        <v>3054239962</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.5875</v>
+        <v>3.62814</v>
       </c>
     </row>
     <row r="6">
@@ -584,25 +584,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>USDC</t>
+          <t>BNB</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>USD Coin</t>
+          <t>BNB</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>250.45</v>
       </c>
       <c r="E6" t="n">
-        <v>27508838298</v>
+        <v>39030804145</v>
       </c>
       <c r="F6" t="n">
-        <v>1791758569</v>
+        <v>418541878</v>
       </c>
       <c r="G6" t="n">
-        <v>0.00314</v>
+        <v>-0.24334</v>
       </c>
     </row>
     <row r="7">
@@ -611,25 +611,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>USDC</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>USD Coin</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.469274</v>
+        <v>1.001</v>
       </c>
       <c r="E7" t="n">
-        <v>24521869218</v>
+        <v>27299501274</v>
       </c>
       <c r="F7" t="n">
-        <v>299284846</v>
+        <v>1648574761</v>
       </c>
       <c r="G7" t="n">
-        <v>0.35015</v>
+        <v>0.03536</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1868.78</v>
+        <v>1934.41</v>
       </c>
       <c r="E8" t="n">
-        <v>14229098867</v>
+        <v>14974134987</v>
       </c>
       <c r="F8" t="n">
-        <v>12222143</v>
+        <v>3991830</v>
       </c>
       <c r="G8" t="n">
-        <v>0.57869</v>
+        <v>-0.22958</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.286559</v>
+        <v>0.323311</v>
       </c>
       <c r="E9" t="n">
-        <v>10042580816</v>
+        <v>11344300187</v>
       </c>
       <c r="F9" t="n">
-        <v>157542023</v>
+        <v>233325738</v>
       </c>
       <c r="G9" t="n">
-        <v>0.17597</v>
+        <v>-2.9888</v>
       </c>
     </row>
     <row r="10">
@@ -692,25 +692,25 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>DOGE</t>
+          <t>SOL</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Dogecoin</t>
+          <t>Solana</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.065873</v>
+        <v>28.14</v>
       </c>
       <c r="E10" t="n">
-        <v>9228668745</v>
+        <v>11341103614</v>
       </c>
       <c r="F10" t="n">
-        <v>156099951</v>
+        <v>841124593</v>
       </c>
       <c r="G10" t="n">
-        <v>0.78345</v>
+        <v>-2.53674</v>
       </c>
     </row>
     <row r="11">
@@ -719,25 +719,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SOL</t>
+          <t>DOGE</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Solana</t>
+          <t>Dogecoin</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>21.6</v>
+        <v>0.07169</v>
       </c>
       <c r="E11" t="n">
-        <v>8689837815</v>
+        <v>10037623091</v>
       </c>
       <c r="F11" t="n">
-        <v>436603738</v>
+        <v>683926724</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.94263</v>
+        <v>-3.05223</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +746,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.07945000000000001</v>
+        <v>0.792743</v>
       </c>
       <c r="E12" t="n">
-        <v>7138337119</v>
+        <v>7391342244</v>
       </c>
       <c r="F12" t="n">
-        <v>278732944</v>
+        <v>195075352</v>
       </c>
       <c r="G12" t="n">
-        <v>0.28291</v>
+        <v>-2.69314</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>96.31999999999999</v>
+        <v>0.080164</v>
       </c>
       <c r="E13" t="n">
-        <v>7062696026</v>
+        <v>7195444700</v>
       </c>
       <c r="F13" t="n">
-        <v>729982986</v>
+        <v>199620290</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.7025</v>
+        <v>-1.26956</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.695423</v>
+        <v>94.73999999999999</v>
       </c>
       <c r="E14" t="n">
-        <v>6480679156</v>
+        <v>6949430314</v>
       </c>
       <c r="F14" t="n">
-        <v>157131027</v>
+        <v>532406213</v>
       </c>
       <c r="G14" t="n">
-        <v>2.11276</v>
+        <v>-0.12233</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>5.1</v>
+        <v>5.4</v>
       </c>
       <c r="E15" t="n">
-        <v>6386024860</v>
+        <v>6782096112</v>
       </c>
       <c r="F15" t="n">
-        <v>68629444</v>
+        <v>116415831</v>
       </c>
       <c r="G15" t="n">
-        <v>-1.17097</v>
+        <v>-1.68405</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>268.28</v>
+        <v>14.62</v>
       </c>
       <c r="E16" t="n">
-        <v>5216489459</v>
+        <v>5049286693</v>
       </c>
       <c r="F16" t="n">
-        <v>370646872</v>
+        <v>186434379</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.46994</v>
+        <v>-2.65001</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>14.08</v>
+        <v>254.1</v>
       </c>
       <c r="E17" t="n">
-        <v>4868564536</v>
+        <v>4945184316</v>
       </c>
       <c r="F17" t="n">
-        <v>217089971</v>
+        <v>340341379</v>
       </c>
       <c r="G17" t="n">
-        <v>4.06899</v>
+        <v>0.55036</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>30266</v>
+        <v>30332</v>
       </c>
       <c r="E18" t="n">
-        <v>4767058142</v>
+        <v>4798778662</v>
       </c>
       <c r="F18" t="n">
-        <v>37987294</v>
+        <v>50688406</v>
       </c>
       <c r="G18" t="n">
-        <v>0.22669</v>
+        <v>0.007990000000000001</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>7.75e-06</v>
+        <v>8.070000000000001e-06</v>
       </c>
       <c r="E19" t="n">
-        <v>4581348393</v>
+        <v>4754482965</v>
       </c>
       <c r="F19" t="n">
-        <v>136193478</v>
+        <v>145855361</v>
       </c>
       <c r="G19" t="n">
-        <v>5.43671</v>
+        <v>-2.64612</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.999682</v>
+        <v>5.79</v>
       </c>
       <c r="E20" t="n">
-        <v>4295568989</v>
+        <v>4365347946</v>
       </c>
       <c r="F20" t="n">
-        <v>56144781</v>
+        <v>74778790</v>
       </c>
       <c r="G20" t="n">
-        <v>0.01237</v>
+        <v>-1.75419</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Binance USD</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.999781</v>
+        <v>1</v>
       </c>
       <c r="E21" t="n">
-        <v>4045267938</v>
+        <v>4287102528</v>
       </c>
       <c r="F21" t="n">
-        <v>2184349579</v>
+        <v>41140048</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0764</v>
+        <v>0.03762</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Binance USD</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>5.26</v>
+        <v>1.001</v>
       </c>
       <c r="E22" t="n">
-        <v>3966710646</v>
+        <v>3972150668</v>
       </c>
       <c r="F22" t="n">
-        <v>68892017</v>
+        <v>1589487997</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.98258</v>
+        <v>0.03933</v>
       </c>
     </row>
     <row r="23">
@@ -1052,16 +1052,16 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>3.83</v>
+        <v>4.01</v>
       </c>
       <c r="E23" t="n">
-        <v>3556172755</v>
+        <v>3723007671</v>
       </c>
       <c r="F23" t="n">
-        <v>1548675</v>
+        <v>811065</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.82997</v>
+        <v>0.84906</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>6.2</v>
+        <v>0.134775</v>
       </c>
       <c r="E24" t="n">
-        <v>3208289369</v>
+        <v>3664590854</v>
       </c>
       <c r="F24" t="n">
-        <v>85341069</v>
+        <v>200501742</v>
       </c>
       <c r="G24" t="n">
-        <v>0.38062</v>
+        <v>2.27628</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>167.43</v>
+        <v>6.84</v>
       </c>
       <c r="E25" t="n">
-        <v>3038666908</v>
+        <v>3543826185</v>
       </c>
       <c r="F25" t="n">
-        <v>62787149</v>
+        <v>141533515</v>
       </c>
       <c r="G25" t="n">
-        <v>0.24568</v>
+        <v>-1.92002</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.9996969999999999</v>
+        <v>164.43</v>
       </c>
       <c r="E26" t="n">
-        <v>2944752923</v>
+        <v>2986834546</v>
       </c>
       <c r="F26" t="n">
-        <v>939878320</v>
+        <v>57203738</v>
       </c>
       <c r="G26" t="n">
-        <v>0.00602</v>
+        <v>0.9755</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>TUSD</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>9.359999999999999</v>
+        <v>1</v>
       </c>
       <c r="E27" t="n">
-        <v>2739496377</v>
+        <v>2845494888</v>
       </c>
       <c r="F27" t="n">
-        <v>64654227</v>
+        <v>894107610</v>
       </c>
       <c r="G27" t="n">
-        <v>1.49827</v>
+        <v>0.07815999999999999</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.098839</v>
+        <v>9.6</v>
       </c>
       <c r="E28" t="n">
-        <v>2673991879</v>
+        <v>2810842987</v>
       </c>
       <c r="F28" t="n">
-        <v>42479530</v>
+        <v>64113749</v>
       </c>
       <c r="G28" t="n">
-        <v>0.39792</v>
+        <v>-2.48926</v>
       </c>
     </row>
     <row r="29">
@@ -1214,16 +1214,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>18.84</v>
+        <v>19.13</v>
       </c>
       <c r="E29" t="n">
-        <v>2672936077</v>
+        <v>2718361584</v>
       </c>
       <c r="F29" t="n">
-        <v>76444042</v>
+        <v>87657147</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.1113</v>
+        <v>-1.53924</v>
       </c>
     </row>
     <row r="30">
@@ -1241,16 +1241,16 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>42.88</v>
+        <v>44.37</v>
       </c>
       <c r="E30" t="n">
-        <v>2572674305</v>
+        <v>2663179561</v>
       </c>
       <c r="F30" t="n">
-        <v>1209900</v>
+        <v>2765240</v>
       </c>
       <c r="G30" t="n">
-        <v>0.62358</v>
+        <v>1.96364</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>1.36</v>
+        <v>2.34</v>
       </c>
       <c r="E31" t="n">
-        <v>2012621476</v>
+        <v>2051128964</v>
       </c>
       <c r="F31" t="n">
-        <v>6785348</v>
+        <v>47872210</v>
       </c>
       <c r="G31" t="n">
-        <v>-1.30378</v>
+        <v>-2.77998</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>4.33</v>
+        <v>1.36</v>
       </c>
       <c r="E32" t="n">
-        <v>1880279223</v>
+        <v>1996434252</v>
       </c>
       <c r="F32" t="n">
-        <v>64236209</v>
+        <v>5958813</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.66376</v>
+        <v>0.73614</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>4.06</v>
+        <v>4.44</v>
       </c>
       <c r="E33" t="n">
-        <v>1776295710</v>
+        <v>1939263133</v>
       </c>
       <c r="F33" t="n">
-        <v>10474983</v>
+        <v>88561125</v>
       </c>
       <c r="G33" t="n">
-        <v>0.28856</v>
+        <v>-0.58205</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>1.95</v>
+        <v>4.16</v>
       </c>
       <c r="E34" t="n">
-        <v>1716789854</v>
+        <v>1826130293</v>
       </c>
       <c r="F34" t="n">
-        <v>14448684</v>
+        <v>16158656</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.61533</v>
+        <v>-1.63878</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.04710601</v>
+        <v>1.3</v>
       </c>
       <c r="E35" t="n">
-        <v>1520906159</v>
+        <v>1662611797</v>
       </c>
       <c r="F35" t="n">
-        <v>11022242</v>
+        <v>287584018</v>
       </c>
       <c r="G35" t="n">
-        <v>0.08827</v>
+        <v>-0.66048</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>102.49</v>
+        <v>0.051243</v>
       </c>
       <c r="E36" t="n">
-        <v>1491014062</v>
+        <v>1654913060</v>
       </c>
       <c r="F36" t="n">
-        <v>10162331</v>
+        <v>20803854</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.81063</v>
+        <v>-2.64609</v>
       </c>
     </row>
     <row r="37">
@@ -1430,16 +1430,16 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>7.1</v>
+        <v>7.58</v>
       </c>
       <c r="E37" t="n">
-        <v>1489407950</v>
+        <v>1627826672</v>
       </c>
       <c r="F37" t="n">
-        <v>53610404</v>
+        <v>72234937</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.92474</v>
+        <v>0.87093</v>
       </c>
     </row>
     <row r="38">
@@ -1457,16 +1457,16 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.056804</v>
+        <v>0.060809</v>
       </c>
       <c r="E38" t="n">
-        <v>1485486803</v>
+        <v>1590196384</v>
       </c>
       <c r="F38" t="n">
-        <v>3786181</v>
+        <v>9419116</v>
       </c>
       <c r="G38" t="n">
-        <v>0.62022</v>
+        <v>0.16994</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1.13</v>
+        <v>102.03</v>
       </c>
       <c r="E39" t="n">
-        <v>1445281418</v>
+        <v>1483216203</v>
       </c>
       <c r="F39" t="n">
-        <v>103634211</v>
+        <v>12586638</v>
       </c>
       <c r="G39" t="n">
-        <v>0.3552</v>
+        <v>-0.47577</v>
       </c>
     </row>
     <row r="40">
@@ -1511,16 +1511,16 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.01868981</v>
+        <v>0.01973754</v>
       </c>
       <c r="E40" t="n">
-        <v>1359078423</v>
+        <v>1436239945</v>
       </c>
       <c r="F40" t="n">
-        <v>31871732</v>
+        <v>37093969</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.34258</v>
+        <v>-1.04918</v>
       </c>
     </row>
     <row r="41">
@@ -1538,16 +1538,16 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1.33</v>
+        <v>1.49</v>
       </c>
       <c r="E41" t="n">
-        <v>1241815875</v>
+        <v>1393918332</v>
       </c>
       <c r="F41" t="n">
-        <v>44290185</v>
+        <v>43521535</v>
       </c>
       <c r="G41" t="n">
-        <v>-3.09645</v>
+        <v>-0.82492</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>AAVE</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Aave</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.114577</v>
+        <v>78.44</v>
       </c>
       <c r="E42" t="n">
-        <v>1043481205</v>
+        <v>1136417724</v>
       </c>
       <c r="F42" t="n">
-        <v>18369847</v>
+        <v>84082017</v>
       </c>
       <c r="G42" t="n">
-        <v>-2.47137</v>
+        <v>-4.38826</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>AAVE</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Aave</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>71.7</v>
+        <v>0.121644</v>
       </c>
       <c r="E43" t="n">
-        <v>1036823892</v>
+        <v>1104398180</v>
       </c>
       <c r="F43" t="n">
-        <v>58130553</v>
+        <v>27493817</v>
       </c>
       <c r="G43" t="n">
-        <v>-5.10367</v>
+        <v>0.399</v>
       </c>
     </row>
     <row r="44">
@@ -1619,16 +1619,16 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.99892</v>
+        <v>1.001</v>
       </c>
       <c r="E44" t="n">
-        <v>1003190654</v>
+        <v>1005435036</v>
       </c>
       <c r="F44" t="n">
-        <v>4275913</v>
+        <v>3507306</v>
       </c>
       <c r="G44" t="n">
-        <v>0.04946</v>
+        <v>0.29938</v>
       </c>
     </row>
     <row r="45">
@@ -1646,16 +1646,16 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>2012.76</v>
+        <v>2085.7</v>
       </c>
       <c r="E45" t="n">
-        <v>940280631</v>
+        <v>998975997</v>
       </c>
       <c r="F45" t="n">
-        <v>698388</v>
+        <v>1230429</v>
       </c>
       <c r="G45" t="n">
-        <v>0.55771</v>
+        <v>-0.18914</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>EGLD</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>MultiversX</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.64361</v>
+        <v>37.49</v>
       </c>
       <c r="E46" t="n">
-        <v>895000675</v>
+        <v>964828911</v>
       </c>
       <c r="F46" t="n">
-        <v>8849550</v>
+        <v>10021752</v>
       </c>
       <c r="G46" t="n">
-        <v>-0.43981</v>
+        <v>1.41532</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>EGLD</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>MultiversX</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>34.49</v>
+        <v>1.48</v>
       </c>
       <c r="E47" t="n">
-        <v>884951931</v>
+        <v>953205503</v>
       </c>
       <c r="F47" t="n">
-        <v>6261926</v>
+        <v>119715687</v>
       </c>
       <c r="G47" t="n">
-        <v>1.2078</v>
+        <v>-2.00554</v>
       </c>
     </row>
     <row r="48">
@@ -1727,16 +1727,16 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.111579</v>
+        <v>0.117502</v>
       </c>
       <c r="E48" t="n">
-        <v>845229390</v>
+        <v>906081022</v>
       </c>
       <c r="F48" t="n">
-        <v>22908520</v>
+        <v>32769066</v>
       </c>
       <c r="G48" t="n">
-        <v>-0.05091</v>
+        <v>2.72119</v>
       </c>
     </row>
     <row r="49">
@@ -1754,16 +1754,16 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>915.73</v>
+        <v>993.4</v>
       </c>
       <c r="E49" t="n">
-        <v>825393175</v>
+        <v>897797164</v>
       </c>
       <c r="F49" t="n">
-        <v>35168653</v>
+        <v>82307323</v>
       </c>
       <c r="G49" t="n">
-        <v>-4.52713</v>
+        <v>12.62316</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>EOS</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>EOS</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.732386</v>
+        <v>0.643779</v>
       </c>
       <c r="E50" t="n">
-        <v>814539108</v>
+        <v>896572036</v>
       </c>
       <c r="F50" t="n">
-        <v>93094383</v>
+        <v>9894914</v>
       </c>
       <c r="G50" t="n">
-        <v>1.83906</v>
+        <v>-0.8104</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>BSV</t>
+          <t>SNX</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Bitcoin SV</t>
+          <t>Synthetix Network</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>40.74</v>
+        <v>2.76</v>
       </c>
       <c r="E51" t="n">
-        <v>784863474</v>
+        <v>885309274</v>
       </c>
       <c r="F51" t="n">
-        <v>17431619</v>
+        <v>109913917</v>
       </c>
       <c r="G51" t="n">
-        <v>-1.87153</v>
+        <v>1.44065</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-07-23
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>30343</v>
+        <v>29898</v>
       </c>
       <c r="E2" t="n">
-        <v>589544684001</v>
+        <v>580986334600</v>
       </c>
       <c r="F2" t="n">
-        <v>6019402119</v>
+        <v>6567055351</v>
       </c>
       <c r="G2" t="n">
-        <v>0.00332</v>
+        <v>0.08076</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1935.52</v>
+        <v>1875.36</v>
       </c>
       <c r="E3" t="n">
-        <v>232618512297</v>
+        <v>225363437431</v>
       </c>
       <c r="F3" t="n">
-        <v>4230895730</v>
+        <v>5168980366</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.24192</v>
+        <v>-0.64466</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1.001</v>
+        <v>0.999833</v>
       </c>
       <c r="E4" t="n">
-        <v>83669568053</v>
+        <v>83780327503</v>
       </c>
       <c r="F4" t="n">
-        <v>12470789930</v>
+        <v>6062061027</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.01269</v>
+        <v>-0.04711</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.751406</v>
+        <v>0.742252</v>
       </c>
       <c r="E5" t="n">
-        <v>39485209298</v>
+        <v>38974495678</v>
       </c>
       <c r="F5" t="n">
-        <v>3054239962</v>
+        <v>1572076246</v>
       </c>
       <c r="G5" t="n">
-        <v>3.62814</v>
+        <v>-3.75616</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>250.45</v>
+        <v>242.3</v>
       </c>
       <c r="E6" t="n">
-        <v>39030804145</v>
+        <v>37734786692</v>
       </c>
       <c r="F6" t="n">
-        <v>418541878</v>
+        <v>220685302</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.24334</v>
+        <v>-0.16139</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1.001</v>
+        <v>0.99993</v>
       </c>
       <c r="E7" t="n">
-        <v>27299501274</v>
+        <v>26852220692</v>
       </c>
       <c r="F7" t="n">
-        <v>1648574761</v>
+        <v>2754304258</v>
       </c>
       <c r="G7" t="n">
-        <v>0.03536</v>
+        <v>-0.01467</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1934.41</v>
+        <v>1874.18</v>
       </c>
       <c r="E8" t="n">
-        <v>14974134987</v>
+        <v>14596700721</v>
       </c>
       <c r="F8" t="n">
-        <v>3991830</v>
+        <v>18994530</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.22958</v>
+        <v>-0.66086</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.323311</v>
+        <v>0.314902</v>
       </c>
       <c r="E9" t="n">
-        <v>11344300187</v>
+        <v>11032322205</v>
       </c>
       <c r="F9" t="n">
-        <v>233325738</v>
+        <v>159912431</v>
       </c>
       <c r="G9" t="n">
-        <v>-2.9888</v>
+        <v>1.02945</v>
       </c>
     </row>
     <row r="10">
@@ -692,25 +692,25 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>SOL</t>
+          <t>DOGE</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Solana</t>
+          <t>Dogecoin</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>28.14</v>
+        <v>0.072154</v>
       </c>
       <c r="E10" t="n">
-        <v>11341103614</v>
+        <v>10107512042</v>
       </c>
       <c r="F10" t="n">
-        <v>841124593</v>
+        <v>322702449</v>
       </c>
       <c r="G10" t="n">
-        <v>-2.53674</v>
+        <v>0.51235</v>
       </c>
     </row>
     <row r="11">
@@ -719,25 +719,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>DOGE</t>
+          <t>SOL</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Dogecoin</t>
+          <t>Solana</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.07169</v>
+        <v>24.69</v>
       </c>
       <c r="E11" t="n">
-        <v>10037623091</v>
+        <v>9968187579</v>
       </c>
       <c r="F11" t="n">
-        <v>683926724</v>
+        <v>368966128</v>
       </c>
       <c r="G11" t="n">
-        <v>-3.05223</v>
+        <v>-3.51955</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +746,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.792743</v>
+        <v>0.083651</v>
       </c>
       <c r="E12" t="n">
-        <v>7391342244</v>
+        <v>7509214563</v>
       </c>
       <c r="F12" t="n">
-        <v>195075352</v>
+        <v>324343535</v>
       </c>
       <c r="G12" t="n">
-        <v>-2.69314</v>
+        <v>-2.7571</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.080164</v>
+        <v>0.752761</v>
       </c>
       <c r="E13" t="n">
-        <v>7195444700</v>
+        <v>7008942776</v>
       </c>
       <c r="F13" t="n">
-        <v>199620290</v>
+        <v>149024466</v>
       </c>
       <c r="G13" t="n">
-        <v>-1.26956</v>
+        <v>-1.2753</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>94.73999999999999</v>
+        <v>5.42</v>
       </c>
       <c r="E14" t="n">
-        <v>6949430314</v>
+        <v>6801666787</v>
       </c>
       <c r="F14" t="n">
-        <v>532406213</v>
+        <v>110138647</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.12233</v>
+        <v>0.97168</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>5.4</v>
+        <v>92.55</v>
       </c>
       <c r="E15" t="n">
-        <v>6782096112</v>
+        <v>6791480445</v>
       </c>
       <c r="F15" t="n">
-        <v>116415831</v>
+        <v>557117996</v>
       </c>
       <c r="G15" t="n">
-        <v>-1.68405</v>
+        <v>-1.02416</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>14.62</v>
+        <v>252.28</v>
       </c>
       <c r="E16" t="n">
-        <v>5049286693</v>
+        <v>4905983265</v>
       </c>
       <c r="F16" t="n">
-        <v>186434379</v>
+        <v>220550362</v>
       </c>
       <c r="G16" t="n">
-        <v>-2.65001</v>
+        <v>3.32662</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>254.1</v>
+        <v>29875</v>
       </c>
       <c r="E17" t="n">
-        <v>4945184316</v>
+        <v>4814361702</v>
       </c>
       <c r="F17" t="n">
-        <v>340341379</v>
+        <v>52848394</v>
       </c>
       <c r="G17" t="n">
-        <v>0.55036</v>
+        <v>-0.05935</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>30332</v>
+        <v>13.57</v>
       </c>
       <c r="E18" t="n">
-        <v>4798778662</v>
+        <v>4694575001</v>
       </c>
       <c r="F18" t="n">
-        <v>50688406</v>
+        <v>98636737</v>
       </c>
       <c r="G18" t="n">
-        <v>0.007990000000000001</v>
+        <v>-1.37094</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>8.070000000000001e-06</v>
+        <v>7.839999999999999e-06</v>
       </c>
       <c r="E19" t="n">
-        <v>4754482965</v>
+        <v>4622799332</v>
       </c>
       <c r="F19" t="n">
-        <v>145855361</v>
+        <v>54224613</v>
       </c>
       <c r="G19" t="n">
-        <v>-2.64612</v>
+        <v>0.45531</v>
       </c>
     </row>
     <row r="20">
@@ -971,16 +971,16 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>5.79</v>
+        <v>6.08</v>
       </c>
       <c r="E20" t="n">
-        <v>4365347946</v>
+        <v>4569999549</v>
       </c>
       <c r="F20" t="n">
-        <v>74778790</v>
+        <v>102999939</v>
       </c>
       <c r="G20" t="n">
-        <v>-1.75419</v>
+        <v>-1.48416</v>
       </c>
     </row>
     <row r="21">
@@ -1001,13 +1001,13 @@
         <v>1</v>
       </c>
       <c r="E21" t="n">
-        <v>4287102528</v>
+        <v>4234992128</v>
       </c>
       <c r="F21" t="n">
-        <v>41140048</v>
+        <v>54746658</v>
       </c>
       <c r="G21" t="n">
-        <v>0.03762</v>
+        <v>0.05196</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Binance USD</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>1.001</v>
+        <v>0.155064</v>
       </c>
       <c r="E22" t="n">
-        <v>3972150668</v>
+        <v>4222602628</v>
       </c>
       <c r="F22" t="n">
-        <v>1589487997</v>
+        <v>176012334</v>
       </c>
       <c r="G22" t="n">
-        <v>0.03933</v>
+        <v>-5.87573</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>4.01</v>
+        <v>8.02</v>
       </c>
       <c r="E23" t="n">
-        <v>3723007671</v>
+        <v>4143991913</v>
       </c>
       <c r="F23" t="n">
-        <v>811065</v>
+        <v>253962078</v>
       </c>
       <c r="G23" t="n">
-        <v>0.84906</v>
+        <v>0.85036</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Binance USD</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.134775</v>
+        <v>0.999604</v>
       </c>
       <c r="E24" t="n">
-        <v>3664590854</v>
+        <v>3850889917</v>
       </c>
       <c r="F24" t="n">
-        <v>200501742</v>
+        <v>1441267226</v>
       </c>
       <c r="G24" t="n">
-        <v>2.27628</v>
+        <v>-0.02774</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>6.84</v>
+        <v>4.02</v>
       </c>
       <c r="E25" t="n">
-        <v>3543826185</v>
+        <v>3730118520</v>
       </c>
       <c r="F25" t="n">
-        <v>141533515</v>
+        <v>1967230</v>
       </c>
       <c r="G25" t="n">
-        <v>-1.92002</v>
+        <v>-2.57592</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>164.43</v>
+        <v>164.96</v>
       </c>
       <c r="E26" t="n">
-        <v>2986834546</v>
+        <v>2992147722</v>
       </c>
       <c r="F26" t="n">
-        <v>57203738</v>
+        <v>102390742</v>
       </c>
       <c r="G26" t="n">
-        <v>0.9755</v>
+        <v>1.56219</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>0.999214</v>
       </c>
       <c r="E27" t="n">
-        <v>2845494888</v>
+        <v>2804903993</v>
       </c>
       <c r="F27" t="n">
-        <v>894107610</v>
+        <v>983081241</v>
       </c>
       <c r="G27" t="n">
-        <v>0.07815999999999999</v>
+        <v>-0.00399</v>
       </c>
     </row>
     <row r="28">
@@ -1187,16 +1187,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>9.6</v>
+        <v>9.26</v>
       </c>
       <c r="E28" t="n">
-        <v>2810842987</v>
+        <v>2706713855</v>
       </c>
       <c r="F28" t="n">
-        <v>64113749</v>
+        <v>55609814</v>
       </c>
       <c r="G28" t="n">
-        <v>-2.48926</v>
+        <v>-1.10054</v>
       </c>
     </row>
     <row r="29">
@@ -1214,16 +1214,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>19.13</v>
+        <v>18.72</v>
       </c>
       <c r="E29" t="n">
-        <v>2718361584</v>
+        <v>2659255878</v>
       </c>
       <c r="F29" t="n">
-        <v>87657147</v>
+        <v>93249591</v>
       </c>
       <c r="G29" t="n">
-        <v>-1.53924</v>
+        <v>-0.05692</v>
       </c>
     </row>
     <row r="30">
@@ -1241,16 +1241,16 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>44.37</v>
+        <v>42.98</v>
       </c>
       <c r="E30" t="n">
-        <v>2663179561</v>
+        <v>2578976709</v>
       </c>
       <c r="F30" t="n">
-        <v>2765240</v>
+        <v>1786469</v>
       </c>
       <c r="G30" t="n">
-        <v>1.96364</v>
+        <v>-0.01688</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>2.34</v>
+        <v>1.51</v>
       </c>
       <c r="E31" t="n">
-        <v>2051128964</v>
+        <v>2224389858</v>
       </c>
       <c r="F31" t="n">
-        <v>47872210</v>
+        <v>36244226</v>
       </c>
       <c r="G31" t="n">
-        <v>-2.77998</v>
+        <v>4.64268</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>1.36</v>
+        <v>4.61</v>
       </c>
       <c r="E32" t="n">
-        <v>1996434252</v>
+        <v>2014581584</v>
       </c>
       <c r="F32" t="n">
-        <v>5958813</v>
+        <v>136856611</v>
       </c>
       <c r="G32" t="n">
-        <v>0.73614</v>
+        <v>2.22632</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>4.44</v>
+        <v>4.31</v>
       </c>
       <c r="E33" t="n">
-        <v>1939263133</v>
+        <v>1886624054</v>
       </c>
       <c r="F33" t="n">
-        <v>88561125</v>
+        <v>30943276</v>
       </c>
       <c r="G33" t="n">
-        <v>-0.58205</v>
+        <v>5.08884</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>4.16</v>
+        <v>2.03</v>
       </c>
       <c r="E34" t="n">
-        <v>1826130293</v>
+        <v>1784162289</v>
       </c>
       <c r="F34" t="n">
-        <v>16158656</v>
+        <v>30249874</v>
       </c>
       <c r="G34" t="n">
-        <v>-1.63878</v>
+        <v>-0.38791</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1.3</v>
+        <v>0.05333</v>
       </c>
       <c r="E35" t="n">
-        <v>1662611797</v>
+        <v>1724584728</v>
       </c>
       <c r="F35" t="n">
-        <v>287584018</v>
+        <v>43330230</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.66048</v>
+        <v>-1.73472</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.051243</v>
+        <v>7.62</v>
       </c>
       <c r="E36" t="n">
-        <v>1654913060</v>
+        <v>1650453199</v>
       </c>
       <c r="F36" t="n">
-        <v>20803854</v>
+        <v>57840880</v>
       </c>
       <c r="G36" t="n">
-        <v>-2.64609</v>
+        <v>-0.16152</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>7.58</v>
+        <v>0.060651</v>
       </c>
       <c r="E37" t="n">
-        <v>1627826672</v>
+        <v>1586543952</v>
       </c>
       <c r="F37" t="n">
-        <v>72234937</v>
+        <v>5511953</v>
       </c>
       <c r="G37" t="n">
-        <v>0.87093</v>
+        <v>-0.193</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.060809</v>
+        <v>1.24</v>
       </c>
       <c r="E38" t="n">
-        <v>1590196384</v>
+        <v>1575608466</v>
       </c>
       <c r="F38" t="n">
-        <v>9419116</v>
+        <v>89718095</v>
       </c>
       <c r="G38" t="n">
-        <v>0.16994</v>
+        <v>-0.03452</v>
       </c>
     </row>
     <row r="39">
@@ -1484,16 +1484,16 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>102.03</v>
+        <v>103.58</v>
       </c>
       <c r="E39" t="n">
-        <v>1483216203</v>
+        <v>1507102098</v>
       </c>
       <c r="F39" t="n">
-        <v>12586638</v>
+        <v>13883033</v>
       </c>
       <c r="G39" t="n">
-        <v>-0.47577</v>
+        <v>1.09311</v>
       </c>
     </row>
     <row r="40">
@@ -1511,16 +1511,16 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.01973754</v>
+        <v>0.01964414</v>
       </c>
       <c r="E40" t="n">
-        <v>1436239945</v>
+        <v>1426896190</v>
       </c>
       <c r="F40" t="n">
-        <v>37093969</v>
+        <v>34625931</v>
       </c>
       <c r="G40" t="n">
-        <v>-1.04918</v>
+        <v>0.21474</v>
       </c>
     </row>
     <row r="41">
@@ -1538,16 +1538,16 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1.49</v>
+        <v>1.46</v>
       </c>
       <c r="E41" t="n">
-        <v>1393918332</v>
+        <v>1367080915</v>
       </c>
       <c r="F41" t="n">
-        <v>43521535</v>
+        <v>39438315</v>
       </c>
       <c r="G41" t="n">
-        <v>-0.82492</v>
+        <v>-0.49028</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>AAVE</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Aave</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>78.44</v>
+        <v>1.57</v>
       </c>
       <c r="E42" t="n">
-        <v>1136417724</v>
+        <v>1067536026</v>
       </c>
       <c r="F42" t="n">
-        <v>84082017</v>
+        <v>89711411</v>
       </c>
       <c r="G42" t="n">
-        <v>-4.38826</v>
+        <v>2.95097</v>
       </c>
     </row>
     <row r="43">
@@ -1592,16 +1592,16 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.121644</v>
+        <v>0.116991</v>
       </c>
       <c r="E43" t="n">
-        <v>1104398180</v>
+        <v>1064787770</v>
       </c>
       <c r="F43" t="n">
-        <v>27493817</v>
+        <v>18310684</v>
       </c>
       <c r="G43" t="n">
-        <v>0.399</v>
+        <v>0.2467</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>FRAX</t>
+          <t>AAVE</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Frax</t>
+          <t>Aave</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1.001</v>
+        <v>72.37</v>
       </c>
       <c r="E44" t="n">
-        <v>1005435036</v>
+        <v>1047921093</v>
       </c>
       <c r="F44" t="n">
-        <v>3507306</v>
+        <v>40156166</v>
       </c>
       <c r="G44" t="n">
-        <v>0.29938</v>
+        <v>-0.64191</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>RETH</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Rocket Pool ETH</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>2085.7</v>
+        <v>1109.98</v>
       </c>
       <c r="E45" t="n">
-        <v>998975997</v>
+        <v>1000889234</v>
       </c>
       <c r="F45" t="n">
-        <v>1230429</v>
+        <v>62102236</v>
       </c>
       <c r="G45" t="n">
-        <v>-0.18914</v>
+        <v>0.07396</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>EGLD</t>
+          <t>RETH</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>MultiversX</t>
+          <t>Rocket Pool ETH</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>37.49</v>
+        <v>2021.97</v>
       </c>
       <c r="E46" t="n">
-        <v>964828911</v>
+        <v>994839764</v>
       </c>
       <c r="F46" t="n">
-        <v>10021752</v>
+        <v>4503824</v>
       </c>
       <c r="G46" t="n">
-        <v>1.41532</v>
+        <v>-0.60471</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>SNX</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Synthetix Network</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>1.48</v>
+        <v>2.91</v>
       </c>
       <c r="E47" t="n">
-        <v>953205503</v>
+        <v>932745423</v>
       </c>
       <c r="F47" t="n">
-        <v>119715687</v>
+        <v>69020758</v>
       </c>
       <c r="G47" t="n">
-        <v>-2.00554</v>
+        <v>-2.1377</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ALGO</t>
+          <t>FRAX</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Algorand</t>
+          <t>Frax</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.117502</v>
+        <v>0.998453</v>
       </c>
       <c r="E48" t="n">
-        <v>906081022</v>
+        <v>921050953</v>
       </c>
       <c r="F48" t="n">
-        <v>32769066</v>
+        <v>4144615</v>
       </c>
       <c r="G48" t="n">
-        <v>2.72119</v>
+        <v>0.01445</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>ALGO</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Algorand</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>993.4</v>
+        <v>0.115529</v>
       </c>
       <c r="E49" t="n">
-        <v>897797164</v>
+        <v>899761348</v>
       </c>
       <c r="F49" t="n">
-        <v>82307323</v>
+        <v>28532752</v>
       </c>
       <c r="G49" t="n">
-        <v>12.62316</v>
+        <v>-0.50173</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>SAND</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>The Sandbox</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.643779</v>
+        <v>0.4543</v>
       </c>
       <c r="E50" t="n">
-        <v>896572036</v>
+        <v>879892274</v>
       </c>
       <c r="F50" t="n">
-        <v>9894914</v>
+        <v>47492284</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.8104</v>
+        <v>1.86553</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>SNX</t>
+          <t>EGLD</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Synthetix Network</t>
+          <t>MultiversX</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>2.76</v>
+        <v>33.88</v>
       </c>
       <c r="E51" t="n">
-        <v>885309274</v>
+        <v>869873872</v>
       </c>
       <c r="F51" t="n">
-        <v>109913917</v>
+        <v>7763618</v>
       </c>
       <c r="G51" t="n">
-        <v>1.44065</v>
+        <v>0.21955</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-07-30
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>29898</v>
+        <v>29325</v>
       </c>
       <c r="E2" t="n">
-        <v>580986334600</v>
+        <v>570032056521</v>
       </c>
       <c r="F2" t="n">
-        <v>6567055351</v>
+        <v>5242729362</v>
       </c>
       <c r="G2" t="n">
-        <v>0.08076</v>
+        <v>0.1717</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1875.36</v>
+        <v>1876.16</v>
       </c>
       <c r="E3" t="n">
-        <v>225363437431</v>
+        <v>225431593307</v>
       </c>
       <c r="F3" t="n">
-        <v>5168980366</v>
+        <v>3230890677</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.64466</v>
+        <v>0.25618</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999833</v>
+        <v>0.999892</v>
       </c>
       <c r="E4" t="n">
-        <v>83780327503</v>
+        <v>83816533176</v>
       </c>
       <c r="F4" t="n">
-        <v>6062061027</v>
+        <v>7584568985</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.04711</v>
+        <v>0.00054</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.742252</v>
+        <v>0.720912</v>
       </c>
       <c r="E5" t="n">
-        <v>38974495678</v>
+        <v>37947659364</v>
       </c>
       <c r="F5" t="n">
-        <v>1572076246</v>
+        <v>787121276</v>
       </c>
       <c r="G5" t="n">
-        <v>-3.75616</v>
+        <v>1.62797</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>242.3</v>
+        <v>242.31</v>
       </c>
       <c r="E6" t="n">
-        <v>37734786692</v>
+        <v>37274007780</v>
       </c>
       <c r="F6" t="n">
-        <v>220685302</v>
+        <v>326225353</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.16139</v>
+        <v>0.29641</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.99993</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>26852220692</v>
+        <v>26552861517</v>
       </c>
       <c r="F7" t="n">
-        <v>2754304258</v>
+        <v>1678874930</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.01467</v>
+        <v>-0.02898</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1874.18</v>
+        <v>1875.71</v>
       </c>
       <c r="E8" t="n">
-        <v>14596700721</v>
+        <v>14861884752</v>
       </c>
       <c r="F8" t="n">
-        <v>18994530</v>
+        <v>15262107</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.66086</v>
+        <v>0.28481</v>
       </c>
     </row>
     <row r="9">
@@ -665,25 +665,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ADA</t>
+          <t>DOGE</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Cardano</t>
+          <t>Dogecoin</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.314902</v>
+        <v>0.080179</v>
       </c>
       <c r="E9" t="n">
-        <v>11032322205</v>
+        <v>11248371166</v>
       </c>
       <c r="F9" t="n">
-        <v>159912431</v>
+        <v>601097859</v>
       </c>
       <c r="G9" t="n">
-        <v>1.02945</v>
+        <v>2.6147</v>
       </c>
     </row>
     <row r="10">
@@ -692,25 +692,25 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>DOGE</t>
+          <t>ADA</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Dogecoin</t>
+          <t>Cardano</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.072154</v>
+        <v>0.31423</v>
       </c>
       <c r="E10" t="n">
-        <v>10107512042</v>
+        <v>11014127034</v>
       </c>
       <c r="F10" t="n">
-        <v>322702449</v>
+        <v>144511044</v>
       </c>
       <c r="G10" t="n">
-        <v>0.51235</v>
+        <v>1.52226</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>24.69</v>
+        <v>24.98</v>
       </c>
       <c r="E11" t="n">
-        <v>9968187579</v>
+        <v>10093471873</v>
       </c>
       <c r="F11" t="n">
-        <v>368966128</v>
+        <v>245013141</v>
       </c>
       <c r="G11" t="n">
-        <v>-3.51955</v>
+        <v>-0.14491</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.083651</v>
+        <v>0.081881</v>
       </c>
       <c r="E12" t="n">
-        <v>7509214563</v>
+        <v>7342197506</v>
       </c>
       <c r="F12" t="n">
-        <v>324343535</v>
+        <v>233944871</v>
       </c>
       <c r="G12" t="n">
-        <v>-2.7571</v>
+        <v>-2.5746</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.752761</v>
+        <v>94.56</v>
       </c>
       <c r="E13" t="n">
-        <v>7008942776</v>
+        <v>6945205662</v>
       </c>
       <c r="F13" t="n">
-        <v>149024466</v>
+        <v>971326813</v>
       </c>
       <c r="G13" t="n">
-        <v>-1.2753</v>
+        <v>3.90549</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>5.42</v>
+        <v>0.712296</v>
       </c>
       <c r="E14" t="n">
-        <v>6801666787</v>
+        <v>6635121757</v>
       </c>
       <c r="F14" t="n">
-        <v>110138647</v>
+        <v>133360835</v>
       </c>
       <c r="G14" t="n">
-        <v>0.97168</v>
+        <v>0.2121</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>92.55</v>
+        <v>5.23</v>
       </c>
       <c r="E15" t="n">
-        <v>6791480445</v>
+        <v>6577578181</v>
       </c>
       <c r="F15" t="n">
-        <v>557117996</v>
+        <v>72966184</v>
       </c>
       <c r="G15" t="n">
-        <v>-1.02416</v>
+        <v>-0.09211</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>252.28</v>
+        <v>8.51e-06</v>
       </c>
       <c r="E16" t="n">
-        <v>4905983265</v>
+        <v>5018654493</v>
       </c>
       <c r="F16" t="n">
-        <v>220550362</v>
+        <v>243230312</v>
       </c>
       <c r="G16" t="n">
-        <v>3.32662</v>
+        <v>3.90805</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>29875</v>
+        <v>6.4</v>
       </c>
       <c r="E17" t="n">
-        <v>4814361702</v>
+        <v>4826523067</v>
       </c>
       <c r="F17" t="n">
-        <v>52848394</v>
+        <v>148256215</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.05935</v>
+        <v>5.48412</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>13.57</v>
+        <v>29357</v>
       </c>
       <c r="E18" t="n">
-        <v>4694575001</v>
+        <v>4738917991</v>
       </c>
       <c r="F18" t="n">
-        <v>98636737</v>
+        <v>24063273</v>
       </c>
       <c r="G18" t="n">
-        <v>-1.37094</v>
+        <v>0.13688</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>7.839999999999999e-06</v>
+        <v>243.48</v>
       </c>
       <c r="E19" t="n">
-        <v>4622799332</v>
+        <v>4730881411</v>
       </c>
       <c r="F19" t="n">
-        <v>54224613</v>
+        <v>117413214</v>
       </c>
       <c r="G19" t="n">
-        <v>0.45531</v>
+        <v>1.507</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>6.08</v>
+        <v>13.29</v>
       </c>
       <c r="E20" t="n">
-        <v>4569999549</v>
+        <v>4595772815</v>
       </c>
       <c r="F20" t="n">
-        <v>102999939</v>
+        <v>64229971</v>
       </c>
       <c r="G20" t="n">
-        <v>-1.48416</v>
+        <v>0.63089</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>0.1596</v>
       </c>
       <c r="E21" t="n">
-        <v>4234992128</v>
+        <v>4351163512</v>
       </c>
       <c r="F21" t="n">
-        <v>54746658</v>
+        <v>121616276</v>
       </c>
       <c r="G21" t="n">
-        <v>0.05196</v>
+        <v>0.10115</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.155064</v>
+        <v>7.75</v>
       </c>
       <c r="E22" t="n">
-        <v>4222602628</v>
+        <v>4169407411</v>
       </c>
       <c r="F22" t="n">
-        <v>176012334</v>
+        <v>131714157</v>
       </c>
       <c r="G22" t="n">
-        <v>-5.87573</v>
+        <v>0.14586</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>8.02</v>
+        <v>1.21</v>
       </c>
       <c r="E23" t="n">
-        <v>4143991913</v>
+        <v>4162500783</v>
       </c>
       <c r="F23" t="n">
-        <v>253962078</v>
+        <v>33747336</v>
       </c>
       <c r="G23" t="n">
-        <v>0.85036</v>
+        <v>-6.56901</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Binance USD</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.999604</v>
+        <v>1</v>
       </c>
       <c r="E24" t="n">
-        <v>3850889917</v>
+        <v>4151401398</v>
       </c>
       <c r="F24" t="n">
-        <v>1441267226</v>
+        <v>46218550</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.02774</v>
+        <v>0.01485</v>
       </c>
     </row>
     <row r="25">
@@ -1106,16 +1106,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>4.02</v>
+        <v>4</v>
       </c>
       <c r="E25" t="n">
-        <v>3730118520</v>
+        <v>3725423698</v>
       </c>
       <c r="F25" t="n">
-        <v>1967230</v>
+        <v>1043572</v>
       </c>
       <c r="G25" t="n">
-        <v>-2.57592</v>
+        <v>1.52728</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Binance USD</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>164.96</v>
+        <v>1</v>
       </c>
       <c r="E26" t="n">
-        <v>2992147722</v>
+        <v>3705611563</v>
       </c>
       <c r="F26" t="n">
-        <v>102390742</v>
+        <v>712448899</v>
       </c>
       <c r="G26" t="n">
-        <v>1.56219</v>
+        <v>0.0121</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.999214</v>
+        <v>0.998335</v>
       </c>
       <c r="E27" t="n">
-        <v>2804903993</v>
+        <v>3053818573</v>
       </c>
       <c r="F27" t="n">
-        <v>983081241</v>
+        <v>74033362</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.00399</v>
+        <v>-0.09396</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>9.26</v>
+        <v>162.46</v>
       </c>
       <c r="E28" t="n">
-        <v>2706713855</v>
+        <v>2944328612</v>
       </c>
       <c r="F28" t="n">
-        <v>55609814</v>
+        <v>54333416</v>
       </c>
       <c r="G28" t="n">
-        <v>-1.10054</v>
+        <v>-0.09002</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>18.72</v>
+        <v>9.029999999999999</v>
       </c>
       <c r="E29" t="n">
-        <v>2659255878</v>
+        <v>2641700611</v>
       </c>
       <c r="F29" t="n">
-        <v>93249591</v>
+        <v>54545411</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.05692</v>
+        <v>0.27636</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>42.98</v>
+        <v>18.48</v>
       </c>
       <c r="E30" t="n">
-        <v>2578976709</v>
+        <v>2629216357</v>
       </c>
       <c r="F30" t="n">
-        <v>1786469</v>
+        <v>57201279</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.01688</v>
+        <v>0.24892</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>1.51</v>
+        <v>42.73</v>
       </c>
       <c r="E31" t="n">
-        <v>2224389858</v>
+        <v>2564141781</v>
       </c>
       <c r="F31" t="n">
-        <v>36244226</v>
+        <v>1395193</v>
       </c>
       <c r="G31" t="n">
-        <v>4.64268</v>
+        <v>0.14302</v>
       </c>
     </row>
     <row r="32">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>4.61</v>
+        <v>4.4</v>
       </c>
       <c r="E32" t="n">
-        <v>2014581584</v>
+        <v>1929573013</v>
       </c>
       <c r="F32" t="n">
-        <v>136856611</v>
+        <v>52314459</v>
       </c>
       <c r="G32" t="n">
-        <v>2.22632</v>
+        <v>0.30659</v>
       </c>
     </row>
     <row r="33">
@@ -1322,16 +1322,16 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>4.31</v>
+        <v>4.29</v>
       </c>
       <c r="E33" t="n">
-        <v>1886624054</v>
+        <v>1887796438</v>
       </c>
       <c r="F33" t="n">
-        <v>30943276</v>
+        <v>12690369</v>
       </c>
       <c r="G33" t="n">
-        <v>5.08884</v>
+        <v>-0.1649</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>2.03</v>
+        <v>0.053558</v>
       </c>
       <c r="E34" t="n">
-        <v>1784162289</v>
+        <v>1735835648</v>
       </c>
       <c r="F34" t="n">
-        <v>30249874</v>
+        <v>19061521</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.38791</v>
+        <v>0.04295</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.05333</v>
+        <v>1.93</v>
       </c>
       <c r="E35" t="n">
-        <v>1724584728</v>
+        <v>1698206638</v>
       </c>
       <c r="F35" t="n">
-        <v>43330230</v>
+        <v>20429035</v>
       </c>
       <c r="G35" t="n">
-        <v>-1.73472</v>
+        <v>-0.47739</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>7.62</v>
+        <v>0.521925</v>
       </c>
       <c r="E36" t="n">
-        <v>1650453199</v>
+        <v>1687718650</v>
       </c>
       <c r="F36" t="n">
-        <v>57840880</v>
+        <v>6546496</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.16152</v>
+        <v>0.4054</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.060651</v>
+        <v>112.88</v>
       </c>
       <c r="E37" t="n">
-        <v>1586543952</v>
+        <v>1640994986</v>
       </c>
       <c r="F37" t="n">
-        <v>5511953</v>
+        <v>19975585</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.193</v>
+        <v>3.84517</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1.24</v>
+        <v>0.059765</v>
       </c>
       <c r="E38" t="n">
-        <v>1575608466</v>
+        <v>1570026240</v>
       </c>
       <c r="F38" t="n">
-        <v>89718095</v>
+        <v>3760921</v>
       </c>
       <c r="G38" t="n">
-        <v>-0.03452</v>
+        <v>-0.24554</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>103.58</v>
+        <v>7.09</v>
       </c>
       <c r="E39" t="n">
-        <v>1507102098</v>
+        <v>1546432165</v>
       </c>
       <c r="F39" t="n">
-        <v>13883033</v>
+        <v>26643714</v>
       </c>
       <c r="G39" t="n">
-        <v>1.09311</v>
+        <v>0.34894</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.01964414</v>
+        <v>1.18</v>
       </c>
       <c r="E40" t="n">
-        <v>1426896190</v>
+        <v>1500095010</v>
       </c>
       <c r="F40" t="n">
-        <v>34625931</v>
+        <v>53154525</v>
       </c>
       <c r="G40" t="n">
-        <v>0.21474</v>
+        <v>0.12822</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1.46</v>
+        <v>0.01874645</v>
       </c>
       <c r="E41" t="n">
-        <v>1367080915</v>
+        <v>1362328054</v>
       </c>
       <c r="F41" t="n">
-        <v>39438315</v>
+        <v>27407729</v>
       </c>
       <c r="G41" t="n">
-        <v>-0.49028</v>
+        <v>0.28904</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1.57</v>
+        <v>1.41</v>
       </c>
       <c r="E42" t="n">
-        <v>1067536026</v>
+        <v>1330956238</v>
       </c>
       <c r="F42" t="n">
-        <v>89711411</v>
+        <v>33739112</v>
       </c>
       <c r="G42" t="n">
-        <v>2.95097</v>
+        <v>0.8604000000000001</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.116991</v>
+        <v>1276.84</v>
       </c>
       <c r="E43" t="n">
-        <v>1064787770</v>
+        <v>1150872039</v>
       </c>
       <c r="F43" t="n">
-        <v>18310684</v>
+        <v>115632210</v>
       </c>
       <c r="G43" t="n">
-        <v>0.2467</v>
+        <v>4.74207</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>AAVE</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Aave</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>72.37</v>
+        <v>1.58</v>
       </c>
       <c r="E44" t="n">
-        <v>1047921093</v>
+        <v>1074440841</v>
       </c>
       <c r="F44" t="n">
-        <v>40156166</v>
+        <v>98374366</v>
       </c>
       <c r="G44" t="n">
-        <v>-0.64191</v>
+        <v>5.86569</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>AAVE</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Aave</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>1109.98</v>
+        <v>74.15000000000001</v>
       </c>
       <c r="E45" t="n">
-        <v>1000889234</v>
+        <v>1073493413</v>
       </c>
       <c r="F45" t="n">
-        <v>62102236</v>
+        <v>49869146</v>
       </c>
       <c r="G45" t="n">
-        <v>0.07396</v>
+        <v>2.62686</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>RETH</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Rocket Pool ETH</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>2021.97</v>
+        <v>0.11188</v>
       </c>
       <c r="E46" t="n">
-        <v>994839764</v>
+        <v>1019200908</v>
       </c>
       <c r="F46" t="n">
-        <v>4503824</v>
+        <v>11864905</v>
       </c>
       <c r="G46" t="n">
-        <v>-0.60471</v>
+        <v>-0.03139</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>SNX</t>
+          <t>RETH</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Synthetix Network</t>
+          <t>Rocket Pool ETH</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>2.91</v>
+        <v>2022.88</v>
       </c>
       <c r="E47" t="n">
-        <v>932745423</v>
+        <v>985444103</v>
       </c>
       <c r="F47" t="n">
-        <v>69020758</v>
+        <v>1796287</v>
       </c>
       <c r="G47" t="n">
-        <v>-2.1377</v>
+        <v>0.28585</v>
       </c>
     </row>
     <row r="48">
@@ -1727,16 +1727,16 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.998453</v>
+        <v>0.9993069999999999</v>
       </c>
       <c r="E48" t="n">
-        <v>921050953</v>
+        <v>911805361</v>
       </c>
       <c r="F48" t="n">
-        <v>4144615</v>
+        <v>3186966</v>
       </c>
       <c r="G48" t="n">
-        <v>0.01445</v>
+        <v>0.11279</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ALGO</t>
+          <t>SNX</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Algorand</t>
+          <t>Synthetix Network</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.115529</v>
+        <v>2.81</v>
       </c>
       <c r="E49" t="n">
-        <v>899761348</v>
+        <v>900803317</v>
       </c>
       <c r="F49" t="n">
-        <v>28532752</v>
+        <v>38084042</v>
       </c>
       <c r="G49" t="n">
-        <v>-0.50173</v>
+        <v>-0.00086</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SAND</t>
+          <t>ALGO</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>The Sandbox</t>
+          <t>Algorand</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.4543</v>
+        <v>0.110922</v>
       </c>
       <c r="E50" t="n">
-        <v>879892274</v>
+        <v>865397798</v>
       </c>
       <c r="F50" t="n">
-        <v>47492284</v>
+        <v>25471750</v>
       </c>
       <c r="G50" t="n">
-        <v>1.86553</v>
+        <v>0.5053299999999999</v>
       </c>
     </row>
     <row r="51">
@@ -1808,16 +1808,16 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>33.88</v>
+        <v>32.66</v>
       </c>
       <c r="E51" t="n">
-        <v>869873872</v>
+        <v>841245870</v>
       </c>
       <c r="F51" t="n">
-        <v>7763618</v>
+        <v>5878902</v>
       </c>
       <c r="G51" t="n">
-        <v>0.21955</v>
+        <v>-0.0592</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-08-06
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>29325</v>
+        <v>29043</v>
       </c>
       <c r="E2" t="n">
-        <v>570032056521</v>
+        <v>564859265747</v>
       </c>
       <c r="F2" t="n">
-        <v>5242729362</v>
+        <v>4686382596</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1717</v>
+        <v>0.1864</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1876.16</v>
+        <v>1830.57</v>
       </c>
       <c r="E3" t="n">
-        <v>225431593307</v>
+        <v>219940033289</v>
       </c>
       <c r="F3" t="n">
-        <v>3230890677</v>
+        <v>2850334802</v>
       </c>
       <c r="G3" t="n">
-        <v>0.25618</v>
+        <v>0.04394</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999892</v>
+        <v>0.998856</v>
       </c>
       <c r="E4" t="n">
-        <v>83816533176</v>
+        <v>83807808883</v>
       </c>
       <c r="F4" t="n">
-        <v>7584568985</v>
+        <v>7890074017</v>
       </c>
       <c r="G4" t="n">
-        <v>0.00054</v>
+        <v>0.06114</v>
       </c>
     </row>
     <row r="5">
@@ -557,25 +557,25 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>BNB</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>BNB</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.720912</v>
+        <v>244.17</v>
       </c>
       <c r="E5" t="n">
-        <v>37947659364</v>
+        <v>37561392502</v>
       </c>
       <c r="F5" t="n">
-        <v>787121276</v>
+        <v>321361698</v>
       </c>
       <c r="G5" t="n">
-        <v>1.62797</v>
+        <v>1.1592</v>
       </c>
     </row>
     <row r="6">
@@ -584,25 +584,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BNB</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>BNB</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>242.31</v>
+        <v>0.631925</v>
       </c>
       <c r="E6" t="n">
-        <v>37274007780</v>
+        <v>33334014662</v>
       </c>
       <c r="F6" t="n">
-        <v>326225353</v>
+        <v>808895231</v>
       </c>
       <c r="G6" t="n">
-        <v>0.29641</v>
+        <v>1.10985</v>
       </c>
     </row>
     <row r="7">
@@ -623,13 +623,13 @@
         <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>26552861517</v>
+        <v>26051364257</v>
       </c>
       <c r="F7" t="n">
-        <v>1678874930</v>
+        <v>1819552024</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.02898</v>
+        <v>0.05179</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1875.71</v>
+        <v>1828.56</v>
       </c>
       <c r="E8" t="n">
-        <v>14861884752</v>
+        <v>14601568803</v>
       </c>
       <c r="F8" t="n">
-        <v>15262107</v>
+        <v>7631986</v>
       </c>
       <c r="G8" t="n">
-        <v>0.28481</v>
+        <v>0.04419</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.080179</v>
+        <v>0.07517699999999999</v>
       </c>
       <c r="E9" t="n">
-        <v>11248371166</v>
+        <v>10558746261</v>
       </c>
       <c r="F9" t="n">
-        <v>601097859</v>
+        <v>443347385</v>
       </c>
       <c r="G9" t="n">
-        <v>2.6147</v>
+        <v>-1.24</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.31423</v>
+        <v>0.294552</v>
       </c>
       <c r="E10" t="n">
-        <v>11014127034</v>
+        <v>10321851414</v>
       </c>
       <c r="F10" t="n">
-        <v>144511044</v>
+        <v>158873178</v>
       </c>
       <c r="G10" t="n">
-        <v>1.52226</v>
+        <v>1.39015</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>24.98</v>
+        <v>23.2</v>
       </c>
       <c r="E11" t="n">
-        <v>10093471873</v>
+        <v>9401949422</v>
       </c>
       <c r="F11" t="n">
-        <v>245013141</v>
+        <v>309850817</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.14491</v>
+        <v>2.26719</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.081881</v>
+        <v>0.077129</v>
       </c>
       <c r="E12" t="n">
-        <v>7342197506</v>
+        <v>6906643033</v>
       </c>
       <c r="F12" t="n">
-        <v>233944871</v>
+        <v>163162283</v>
       </c>
       <c r="G12" t="n">
-        <v>-2.5746</v>
+        <v>-0.35102</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>94.56</v>
+        <v>5</v>
       </c>
       <c r="E13" t="n">
-        <v>6945205662</v>
+        <v>6311831344</v>
       </c>
       <c r="F13" t="n">
-        <v>971326813</v>
+        <v>71916117</v>
       </c>
       <c r="G13" t="n">
-        <v>3.90549</v>
+        <v>1.1746</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.712296</v>
+        <v>0.668238</v>
       </c>
       <c r="E14" t="n">
-        <v>6635121757</v>
+        <v>6228832397</v>
       </c>
       <c r="F14" t="n">
-        <v>133360835</v>
+        <v>174531251</v>
       </c>
       <c r="G14" t="n">
-        <v>0.2121</v>
+        <v>0.92513</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>5.23</v>
+        <v>83.26000000000001</v>
       </c>
       <c r="E15" t="n">
-        <v>6577578181</v>
+        <v>6120130955</v>
       </c>
       <c r="F15" t="n">
-        <v>72966184</v>
+        <v>282178143</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.09211</v>
+        <v>1.19595</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>8.51e-06</v>
+        <v>9.77e-06</v>
       </c>
       <c r="E16" t="n">
-        <v>5018654493</v>
+        <v>5770889760</v>
       </c>
       <c r="F16" t="n">
-        <v>243230312</v>
+        <v>833295208</v>
       </c>
       <c r="G16" t="n">
-        <v>3.90805</v>
+        <v>3.36204</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>6.4</v>
+        <v>29037</v>
       </c>
       <c r="E17" t="n">
-        <v>4826523067</v>
+        <v>4710158683</v>
       </c>
       <c r="F17" t="n">
-        <v>148256215</v>
+        <v>30287320</v>
       </c>
       <c r="G17" t="n">
-        <v>5.48412</v>
+        <v>0.24604</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>29357</v>
+        <v>6.06</v>
       </c>
       <c r="E18" t="n">
-        <v>4738917991</v>
+        <v>4562970588</v>
       </c>
       <c r="F18" t="n">
-        <v>24063273</v>
+        <v>60049745</v>
       </c>
       <c r="G18" t="n">
-        <v>0.13688</v>
+        <v>1.5731</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>243.48</v>
+        <v>225.82</v>
       </c>
       <c r="E19" t="n">
-        <v>4730881411</v>
+        <v>4395929329</v>
       </c>
       <c r="F19" t="n">
-        <v>117413214</v>
+        <v>130978863</v>
       </c>
       <c r="G19" t="n">
-        <v>1.507</v>
+        <v>0.93953</v>
       </c>
     </row>
     <row r="20">
@@ -971,16 +971,16 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>13.29</v>
+        <v>12.6</v>
       </c>
       <c r="E20" t="n">
-        <v>4595772815</v>
+        <v>4363320291</v>
       </c>
       <c r="F20" t="n">
-        <v>64229971</v>
+        <v>92117487</v>
       </c>
       <c r="G20" t="n">
-        <v>0.63089</v>
+        <v>2.46253</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.1596</v>
+        <v>1.2</v>
       </c>
       <c r="E21" t="n">
-        <v>4351163512</v>
+        <v>4141467095</v>
       </c>
       <c r="F21" t="n">
-        <v>121616276</v>
+        <v>21567840</v>
       </c>
       <c r="G21" t="n">
-        <v>0.10115</v>
+        <v>0.49407</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>7.75</v>
+        <v>1</v>
       </c>
       <c r="E22" t="n">
-        <v>4169407411</v>
+        <v>4044572604</v>
       </c>
       <c r="F22" t="n">
-        <v>131714157</v>
+        <v>68618576</v>
       </c>
       <c r="G22" t="n">
-        <v>0.14586</v>
+        <v>0.10263</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>1.21</v>
+        <v>0.141593</v>
       </c>
       <c r="E23" t="n">
-        <v>4162500783</v>
+        <v>3869370199</v>
       </c>
       <c r="F23" t="n">
-        <v>33747336</v>
+        <v>107226817</v>
       </c>
       <c r="G23" t="n">
-        <v>-6.56901</v>
+        <v>4.26286</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>7.14</v>
       </c>
       <c r="E24" t="n">
-        <v>4151401398</v>
+        <v>3843051482</v>
       </c>
       <c r="F24" t="n">
-        <v>46218550</v>
+        <v>131028854</v>
       </c>
       <c r="G24" t="n">
-        <v>0.01485</v>
+        <v>-0.45324</v>
       </c>
     </row>
     <row r="25">
@@ -1106,16 +1106,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>4</v>
+        <v>4.02</v>
       </c>
       <c r="E25" t="n">
-        <v>3725423698</v>
+        <v>3731907083</v>
       </c>
       <c r="F25" t="n">
-        <v>1043572</v>
+        <v>1825781</v>
       </c>
       <c r="G25" t="n">
-        <v>1.52728</v>
+        <v>-0.19076</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>0.9997239999999999</v>
       </c>
       <c r="E26" t="n">
-        <v>3705611563</v>
+        <v>3415836319</v>
       </c>
       <c r="F26" t="n">
-        <v>712448899</v>
+        <v>983733960</v>
       </c>
       <c r="G26" t="n">
-        <v>0.0121</v>
+        <v>0.0266</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.998335</v>
+        <v>0.999098</v>
       </c>
       <c r="E27" t="n">
-        <v>3053818573</v>
+        <v>2962479271</v>
       </c>
       <c r="F27" t="n">
-        <v>74033362</v>
+        <v>852152725</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.09396</v>
+        <v>-0.05358</v>
       </c>
     </row>
     <row r="28">
@@ -1187,16 +1187,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>162.46</v>
+        <v>160.31</v>
       </c>
       <c r="E28" t="n">
-        <v>2944328612</v>
+        <v>2917536909</v>
       </c>
       <c r="F28" t="n">
-        <v>54333416</v>
+        <v>89069659</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.09002</v>
+        <v>0.43787</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>9.029999999999999</v>
+        <v>45.55</v>
       </c>
       <c r="E29" t="n">
-        <v>2641700611</v>
+        <v>2732843518</v>
       </c>
       <c r="F29" t="n">
-        <v>54545411</v>
+        <v>5467927</v>
       </c>
       <c r="G29" t="n">
-        <v>0.27636</v>
+        <v>0.35866</v>
       </c>
     </row>
     <row r="30">
@@ -1241,16 +1241,16 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>18.48</v>
+        <v>17.94</v>
       </c>
       <c r="E30" t="n">
-        <v>2629216357</v>
+        <v>2554069026</v>
       </c>
       <c r="F30" t="n">
-        <v>57201279</v>
+        <v>52734198</v>
       </c>
       <c r="G30" t="n">
-        <v>0.24892</v>
+        <v>0.93449</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>42.73</v>
+        <v>8.52</v>
       </c>
       <c r="E31" t="n">
-        <v>2564141781</v>
+        <v>2491798732</v>
       </c>
       <c r="F31" t="n">
-        <v>1395193</v>
+        <v>103870626</v>
       </c>
       <c r="G31" t="n">
-        <v>0.14302</v>
+        <v>1.43999</v>
       </c>
     </row>
     <row r="32">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>4.4</v>
+        <v>4.13</v>
       </c>
       <c r="E32" t="n">
-        <v>1929573013</v>
+        <v>1814013626</v>
       </c>
       <c r="F32" t="n">
-        <v>52314459</v>
+        <v>59806171</v>
       </c>
       <c r="G32" t="n">
-        <v>0.30659</v>
+        <v>1.99424</v>
       </c>
     </row>
     <row r="33">
@@ -1322,16 +1322,16 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>4.29</v>
+        <v>4.06</v>
       </c>
       <c r="E33" t="n">
-        <v>1887796438</v>
+        <v>1790335119</v>
       </c>
       <c r="F33" t="n">
-        <v>12690369</v>
+        <v>13610391</v>
       </c>
       <c r="G33" t="n">
-        <v>-0.1649</v>
+        <v>1.14665</v>
       </c>
     </row>
     <row r="34">
@@ -1349,16 +1349,16 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.053558</v>
+        <v>0.054888</v>
       </c>
       <c r="E34" t="n">
-        <v>1735835648</v>
+        <v>1787889471</v>
       </c>
       <c r="F34" t="n">
-        <v>19061521</v>
+        <v>29697902</v>
       </c>
       <c r="G34" t="n">
-        <v>0.04295</v>
+        <v>5.70609</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1.93</v>
+        <v>0.508229</v>
       </c>
       <c r="E35" t="n">
-        <v>1698206638</v>
+        <v>1644115400</v>
       </c>
       <c r="F35" t="n">
-        <v>20429035</v>
+        <v>7948757</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.47739</v>
+        <v>-0.54503</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.521925</v>
+        <v>1.86</v>
       </c>
       <c r="E36" t="n">
-        <v>1687718650</v>
+        <v>1634824146</v>
       </c>
       <c r="F36" t="n">
-        <v>6546496</v>
+        <v>54104342</v>
       </c>
       <c r="G36" t="n">
-        <v>0.4054</v>
+        <v>1.10114</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>112.88</v>
+        <v>0.058012</v>
       </c>
       <c r="E37" t="n">
-        <v>1640994986</v>
+        <v>1521078722</v>
       </c>
       <c r="F37" t="n">
-        <v>19975585</v>
+        <v>4525889</v>
       </c>
       <c r="G37" t="n">
-        <v>3.84517</v>
+        <v>1.09347</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.059765</v>
+        <v>6.78</v>
       </c>
       <c r="E38" t="n">
-        <v>1570026240</v>
+        <v>1486794977</v>
       </c>
       <c r="F38" t="n">
-        <v>3760921</v>
+        <v>42734260</v>
       </c>
       <c r="G38" t="n">
-        <v>-0.24554</v>
+        <v>1.46874</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>7.09</v>
+        <v>101.88</v>
       </c>
       <c r="E39" t="n">
-        <v>1546432165</v>
+        <v>1481368981</v>
       </c>
       <c r="F39" t="n">
-        <v>26643714</v>
+        <v>16212791</v>
       </c>
       <c r="G39" t="n">
-        <v>0.34894</v>
+        <v>0.48671</v>
       </c>
     </row>
     <row r="40">
@@ -1511,16 +1511,16 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1.18</v>
+        <v>1.14</v>
       </c>
       <c r="E40" t="n">
-        <v>1500095010</v>
+        <v>1451998905</v>
       </c>
       <c r="F40" t="n">
-        <v>53154525</v>
+        <v>114484250</v>
       </c>
       <c r="G40" t="n">
-        <v>0.12822</v>
+        <v>-0.57778</v>
       </c>
     </row>
     <row r="41">
@@ -1538,16 +1538,16 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.01874645</v>
+        <v>0.01785485</v>
       </c>
       <c r="E41" t="n">
-        <v>1362328054</v>
+        <v>1296451013</v>
       </c>
       <c r="F41" t="n">
-        <v>27407729</v>
+        <v>25984554</v>
       </c>
       <c r="G41" t="n">
-        <v>0.28904</v>
+        <v>0.26489</v>
       </c>
     </row>
     <row r="42">
@@ -1565,16 +1565,16 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1.41</v>
+        <v>1.36</v>
       </c>
       <c r="E42" t="n">
-        <v>1330956238</v>
+        <v>1277768501</v>
       </c>
       <c r="F42" t="n">
-        <v>33739112</v>
+        <v>37264658</v>
       </c>
       <c r="G42" t="n">
-        <v>0.8604000000000001</v>
+        <v>1.26672</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1276.84</v>
+        <v>1.69</v>
       </c>
       <c r="E43" t="n">
-        <v>1150872039</v>
+        <v>1214847082</v>
       </c>
       <c r="F43" t="n">
-        <v>115632210</v>
+        <v>91062255</v>
       </c>
       <c r="G43" t="n">
-        <v>4.74207</v>
+        <v>2.10258</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1.58</v>
+        <v>1246.18</v>
       </c>
       <c r="E44" t="n">
-        <v>1074440841</v>
+        <v>1123296555</v>
       </c>
       <c r="F44" t="n">
-        <v>98374366</v>
+        <v>150814405</v>
       </c>
       <c r="G44" t="n">
-        <v>5.86569</v>
+        <v>-1.48139</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>AAVE</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Aave</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>74.15000000000001</v>
+        <v>0.051558</v>
       </c>
       <c r="E45" t="n">
-        <v>1073493413</v>
+        <v>1035295811</v>
       </c>
       <c r="F45" t="n">
-        <v>49869146</v>
+        <v>26209171</v>
       </c>
       <c r="G45" t="n">
-        <v>2.62686</v>
+        <v>12.4698</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>XDC</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>XDC Network</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.11188</v>
+        <v>0.07346</v>
       </c>
       <c r="E46" t="n">
-        <v>1019200908</v>
+        <v>1020134211</v>
       </c>
       <c r="F46" t="n">
-        <v>11864905</v>
+        <v>23573112</v>
       </c>
       <c r="G46" t="n">
-        <v>-0.03139</v>
+        <v>1.75388</v>
       </c>
     </row>
     <row r="47">
@@ -1700,16 +1700,16 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>2022.88</v>
+        <v>1977.08</v>
       </c>
       <c r="E47" t="n">
-        <v>985444103</v>
+        <v>978869063</v>
       </c>
       <c r="F47" t="n">
-        <v>1796287</v>
+        <v>2153055</v>
       </c>
       <c r="G47" t="n">
-        <v>0.28585</v>
+        <v>0.1216</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>FRAX</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Frax</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.9993069999999999</v>
+        <v>0.106285</v>
       </c>
       <c r="E48" t="n">
-        <v>911805361</v>
+        <v>970398056</v>
       </c>
       <c r="F48" t="n">
-        <v>3186966</v>
+        <v>58437186</v>
       </c>
       <c r="G48" t="n">
-        <v>0.11279</v>
+        <v>1.97488</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>SNX</t>
+          <t>AAVE</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Synthetix Network</t>
+          <t>Aave</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>2.81</v>
+        <v>65.40000000000001</v>
       </c>
       <c r="E49" t="n">
-        <v>900803317</v>
+        <v>949423102</v>
       </c>
       <c r="F49" t="n">
-        <v>38084042</v>
+        <v>61364375</v>
       </c>
       <c r="G49" t="n">
-        <v>-0.00086</v>
+        <v>1.71488</v>
       </c>
     </row>
     <row r="50">
@@ -1781,16 +1781,16 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.110922</v>
+        <v>0.107631</v>
       </c>
       <c r="E50" t="n">
-        <v>865397798</v>
+        <v>840906547</v>
       </c>
       <c r="F50" t="n">
-        <v>25471750</v>
+        <v>20316973</v>
       </c>
       <c r="G50" t="n">
-        <v>0.5053299999999999</v>
+        <v>2.24045</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>EGLD</t>
+          <t>SAND</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>MultiversX</t>
+          <t>The Sandbox</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>32.66</v>
+        <v>0.406102</v>
       </c>
       <c r="E51" t="n">
-        <v>841245870</v>
+        <v>834622081</v>
       </c>
       <c r="F51" t="n">
-        <v>5878902</v>
+        <v>70818243</v>
       </c>
       <c r="G51" t="n">
-        <v>-0.0592</v>
+        <v>2.33244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-08-13
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>29043</v>
+        <v>29363</v>
       </c>
       <c r="E2" t="n">
-        <v>564859265747</v>
+        <v>571333545378</v>
       </c>
       <c r="F2" t="n">
-        <v>4686382596</v>
+        <v>3303796092</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1864</v>
+        <v>-0.13376</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1830.57</v>
+        <v>1848.18</v>
       </c>
       <c r="E3" t="n">
-        <v>219940033289</v>
+        <v>222076564062</v>
       </c>
       <c r="F3" t="n">
-        <v>2850334802</v>
+        <v>2310450298</v>
       </c>
       <c r="G3" t="n">
-        <v>0.04394</v>
+        <v>-0.08673</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.998856</v>
+        <v>0.999184</v>
       </c>
       <c r="E4" t="n">
-        <v>83807808883</v>
+        <v>83342810176</v>
       </c>
       <c r="F4" t="n">
-        <v>7890074017</v>
+        <v>7108679688</v>
       </c>
       <c r="G4" t="n">
-        <v>0.06114</v>
+        <v>-0.008789999999999999</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>244.17</v>
+        <v>240.58</v>
       </c>
       <c r="E5" t="n">
-        <v>37561392502</v>
+        <v>37018923781</v>
       </c>
       <c r="F5" t="n">
-        <v>321361698</v>
+        <v>213453442</v>
       </c>
       <c r="G5" t="n">
-        <v>1.1592</v>
+        <v>-0.07003</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.631925</v>
+        <v>0.62698</v>
       </c>
       <c r="E6" t="n">
-        <v>33334014662</v>
+        <v>33106832695</v>
       </c>
       <c r="F6" t="n">
-        <v>808895231</v>
+        <v>483544806</v>
       </c>
       <c r="G6" t="n">
-        <v>1.10985</v>
+        <v>-0.39903</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0.999383</v>
       </c>
       <c r="E7" t="n">
-        <v>26051364257</v>
+        <v>26149288275</v>
       </c>
       <c r="F7" t="n">
-        <v>1819552024</v>
+        <v>1179107340</v>
       </c>
       <c r="G7" t="n">
-        <v>0.05179</v>
+        <v>-0.06833</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1828.56</v>
+        <v>1846.9</v>
       </c>
       <c r="E8" t="n">
-        <v>14601568803</v>
+        <v>14936655272</v>
       </c>
       <c r="F8" t="n">
-        <v>7631986</v>
+        <v>3754359</v>
       </c>
       <c r="G8" t="n">
-        <v>0.04419</v>
+        <v>-0.17284</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.07517699999999999</v>
+        <v>0.076025</v>
       </c>
       <c r="E9" t="n">
-        <v>10558746261</v>
+        <v>10692730010</v>
       </c>
       <c r="F9" t="n">
-        <v>443347385</v>
+        <v>312734566</v>
       </c>
       <c r="G9" t="n">
-        <v>-1.24</v>
+        <v>-1.02666</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.294552</v>
+        <v>0.290117</v>
       </c>
       <c r="E10" t="n">
-        <v>10321851414</v>
+        <v>10171497411</v>
       </c>
       <c r="F10" t="n">
-        <v>158873178</v>
+        <v>107779936</v>
       </c>
       <c r="G10" t="n">
-        <v>1.39015</v>
+        <v>-1.28148</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>23.2</v>
+        <v>24.65</v>
       </c>
       <c r="E11" t="n">
-        <v>9401949422</v>
+        <v>10008374813</v>
       </c>
       <c r="F11" t="n">
-        <v>309850817</v>
+        <v>287251378</v>
       </c>
       <c r="G11" t="n">
-        <v>2.26719</v>
+        <v>0.50687</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.077129</v>
+        <v>0.077405</v>
       </c>
       <c r="E12" t="n">
-        <v>6906643033</v>
+        <v>6929030335</v>
       </c>
       <c r="F12" t="n">
-        <v>163162283</v>
+        <v>143140064</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.35102</v>
+        <v>-0.02841</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>5</v>
+        <v>5.03</v>
       </c>
       <c r="E13" t="n">
-        <v>6311831344</v>
+        <v>6354890239</v>
       </c>
       <c r="F13" t="n">
-        <v>71916117</v>
+        <v>66099430</v>
       </c>
       <c r="G13" t="n">
-        <v>1.1746</v>
+        <v>0.02147</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.668238</v>
+        <v>0.678663</v>
       </c>
       <c r="E14" t="n">
-        <v>6228832397</v>
+        <v>6325172732</v>
       </c>
       <c r="F14" t="n">
-        <v>174531251</v>
+        <v>93208608</v>
       </c>
       <c r="G14" t="n">
-        <v>0.92513</v>
+        <v>-0.36905</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>83.26000000000001</v>
+        <v>1.063e-05</v>
       </c>
       <c r="E15" t="n">
-        <v>6120130955</v>
+        <v>6277730810</v>
       </c>
       <c r="F15" t="n">
-        <v>282178143</v>
+        <v>431703613</v>
       </c>
       <c r="G15" t="n">
-        <v>1.19595</v>
+        <v>-2.46102</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>9.77e-06</v>
+        <v>82.90000000000001</v>
       </c>
       <c r="E16" t="n">
-        <v>5770889760</v>
+        <v>6096772616</v>
       </c>
       <c r="F16" t="n">
-        <v>833295208</v>
+        <v>356812368</v>
       </c>
       <c r="G16" t="n">
-        <v>3.36204</v>
+        <v>-0.99549</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>29037</v>
+        <v>1.43</v>
       </c>
       <c r="E17" t="n">
-        <v>4710158683</v>
+        <v>4936033777</v>
       </c>
       <c r="F17" t="n">
-        <v>30287320</v>
+        <v>30373319</v>
       </c>
       <c r="G17" t="n">
-        <v>0.24604</v>
+        <v>9.212440000000001</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>6.06</v>
+        <v>29391</v>
       </c>
       <c r="E18" t="n">
-        <v>4562970588</v>
+        <v>4768484517</v>
       </c>
       <c r="F18" t="n">
-        <v>60049745</v>
+        <v>30522230</v>
       </c>
       <c r="G18" t="n">
-        <v>1.5731</v>
+        <v>-0.1164</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>225.82</v>
+        <v>6.12</v>
       </c>
       <c r="E19" t="n">
-        <v>4395929329</v>
+        <v>4617066618</v>
       </c>
       <c r="F19" t="n">
-        <v>130978863</v>
+        <v>53502521</v>
       </c>
       <c r="G19" t="n">
-        <v>0.93953</v>
+        <v>-0.5577</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>12.6</v>
+        <v>227.82</v>
       </c>
       <c r="E20" t="n">
-        <v>4363320291</v>
+        <v>4438553491</v>
       </c>
       <c r="F20" t="n">
-        <v>92117487</v>
+        <v>98148620</v>
       </c>
       <c r="G20" t="n">
-        <v>2.46253</v>
+        <v>-0.61341</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>1.2</v>
+        <v>12.35</v>
       </c>
       <c r="E21" t="n">
-        <v>4141467095</v>
+        <v>4245537266</v>
       </c>
       <c r="F21" t="n">
-        <v>21567840</v>
+        <v>82754761</v>
       </c>
       <c r="G21" t="n">
-        <v>0.49407</v>
+        <v>-1.0073</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>7.5</v>
       </c>
       <c r="E22" t="n">
-        <v>4044572604</v>
+        <v>4038541357</v>
       </c>
       <c r="F22" t="n">
-        <v>68618576</v>
+        <v>122835487</v>
       </c>
       <c r="G22" t="n">
-        <v>0.10263</v>
+        <v>0.71173</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.141593</v>
+        <v>0.999619</v>
       </c>
       <c r="E23" t="n">
-        <v>3869370199</v>
+        <v>3999458311</v>
       </c>
       <c r="F23" t="n">
-        <v>107226817</v>
+        <v>56265311</v>
       </c>
       <c r="G23" t="n">
-        <v>4.26286</v>
+        <v>-0.01704</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>7.14</v>
+        <v>0.138305</v>
       </c>
       <c r="E24" t="n">
-        <v>3843051482</v>
+        <v>3786616248</v>
       </c>
       <c r="F24" t="n">
-        <v>131028854</v>
+        <v>58806981</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.45324</v>
+        <v>-0.08619</v>
       </c>
     </row>
     <row r="25">
@@ -1106,16 +1106,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>4.02</v>
+        <v>4.03</v>
       </c>
       <c r="E25" t="n">
-        <v>3731907083</v>
+        <v>3757947879</v>
       </c>
       <c r="F25" t="n">
-        <v>1825781</v>
+        <v>829456</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.19076</v>
+        <v>1.27446</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.9997239999999999</v>
+        <v>0.999841</v>
       </c>
       <c r="E26" t="n">
-        <v>3415836319</v>
+        <v>3371446673</v>
       </c>
       <c r="F26" t="n">
-        <v>983733960</v>
+        <v>953231543</v>
       </c>
       <c r="G26" t="n">
-        <v>0.0266</v>
+        <v>-0.01211</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.999098</v>
+        <v>0.999184</v>
       </c>
       <c r="E27" t="n">
-        <v>2962479271</v>
+        <v>2970859209</v>
       </c>
       <c r="F27" t="n">
-        <v>852152725</v>
+        <v>61108173</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.05358</v>
+        <v>-0.06144</v>
       </c>
     </row>
     <row r="28">
@@ -1187,16 +1187,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>160.31</v>
+        <v>159.02</v>
       </c>
       <c r="E28" t="n">
-        <v>2917536909</v>
+        <v>2883280463</v>
       </c>
       <c r="F28" t="n">
-        <v>89069659</v>
+        <v>72144578</v>
       </c>
       <c r="G28" t="n">
-        <v>0.43787</v>
+        <v>1.16487</v>
       </c>
     </row>
     <row r="29">
@@ -1214,16 +1214,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>45.55</v>
+        <v>46.71</v>
       </c>
       <c r="E29" t="n">
-        <v>2732843518</v>
+        <v>2802373037</v>
       </c>
       <c r="F29" t="n">
-        <v>5467927</v>
+        <v>5304234</v>
       </c>
       <c r="G29" t="n">
-        <v>0.35866</v>
+        <v>-3.00401</v>
       </c>
     </row>
     <row r="30">
@@ -1241,16 +1241,16 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>17.94</v>
+        <v>17.66</v>
       </c>
       <c r="E30" t="n">
-        <v>2554069026</v>
+        <v>2514932071</v>
       </c>
       <c r="F30" t="n">
-        <v>52734198</v>
+        <v>54094016</v>
       </c>
       <c r="G30" t="n">
-        <v>0.93449</v>
+        <v>-0.07174999999999999</v>
       </c>
     </row>
     <row r="31">
@@ -1268,16 +1268,16 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>8.52</v>
+        <v>8.44</v>
       </c>
       <c r="E31" t="n">
-        <v>2491798732</v>
+        <v>2469359258</v>
       </c>
       <c r="F31" t="n">
-        <v>103870626</v>
+        <v>64621810</v>
       </c>
       <c r="G31" t="n">
-        <v>1.43999</v>
+        <v>0.67488</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>4.13</v>
+        <v>0.056172</v>
       </c>
       <c r="E32" t="n">
-        <v>1814013626</v>
+        <v>1852562666</v>
       </c>
       <c r="F32" t="n">
-        <v>59806171</v>
+        <v>16324683</v>
       </c>
       <c r="G32" t="n">
-        <v>1.99424</v>
+        <v>-1.60931</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>4.06</v>
+        <v>4.1</v>
       </c>
       <c r="E33" t="n">
-        <v>1790335119</v>
+        <v>1810280167</v>
       </c>
       <c r="F33" t="n">
-        <v>13610391</v>
+        <v>52786199</v>
       </c>
       <c r="G33" t="n">
-        <v>1.14665</v>
+        <v>-0.41291</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.054888</v>
+        <v>4.06</v>
       </c>
       <c r="E34" t="n">
-        <v>1787889471</v>
+        <v>1793068862</v>
       </c>
       <c r="F34" t="n">
-        <v>29697902</v>
+        <v>14078567</v>
       </c>
       <c r="G34" t="n">
-        <v>5.70609</v>
+        <v>0.11028</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.508229</v>
+        <v>7.21</v>
       </c>
       <c r="E35" t="n">
-        <v>1644115400</v>
+        <v>1621145976</v>
       </c>
       <c r="F35" t="n">
-        <v>7948757</v>
+        <v>58254185</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.54503</v>
+        <v>0.9799099999999999</v>
       </c>
     </row>
     <row r="36">
@@ -1403,16 +1403,16 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1.86</v>
+        <v>1.83</v>
       </c>
       <c r="E36" t="n">
-        <v>1634824146</v>
+        <v>1608902042</v>
       </c>
       <c r="F36" t="n">
-        <v>54104342</v>
+        <v>64275190</v>
       </c>
       <c r="G36" t="n">
-        <v>1.10114</v>
+        <v>-1.10577</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.058012</v>
+        <v>0.462679</v>
       </c>
       <c r="E37" t="n">
-        <v>1521078722</v>
+        <v>1496606169</v>
       </c>
       <c r="F37" t="n">
-        <v>4525889</v>
+        <v>4522297</v>
       </c>
       <c r="G37" t="n">
-        <v>1.09347</v>
+        <v>0.007889999999999999</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>6.78</v>
+        <v>0.056974</v>
       </c>
       <c r="E38" t="n">
-        <v>1486794977</v>
+        <v>1492000194</v>
       </c>
       <c r="F38" t="n">
-        <v>42734260</v>
+        <v>3365776</v>
       </c>
       <c r="G38" t="n">
-        <v>1.46874</v>
+        <v>-0.38157</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>101.88</v>
+        <v>1.16</v>
       </c>
       <c r="E39" t="n">
-        <v>1481368981</v>
+        <v>1479485675</v>
       </c>
       <c r="F39" t="n">
-        <v>16212791</v>
+        <v>96635627</v>
       </c>
       <c r="G39" t="n">
-        <v>0.48671</v>
+        <v>0.08483</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1.14</v>
+        <v>101.44</v>
       </c>
       <c r="E40" t="n">
-        <v>1451998905</v>
+        <v>1475426292</v>
       </c>
       <c r="F40" t="n">
-        <v>114484250</v>
+        <v>10583241</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.57778</v>
+        <v>-0.05005</v>
       </c>
     </row>
     <row r="41">
@@ -1538,16 +1538,16 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.01785485</v>
+        <v>0.01798175</v>
       </c>
       <c r="E41" t="n">
-        <v>1296451013</v>
+        <v>1307156169</v>
       </c>
       <c r="F41" t="n">
-        <v>25984554</v>
+        <v>23665482</v>
       </c>
       <c r="G41" t="n">
-        <v>0.26489</v>
+        <v>-0.01439</v>
       </c>
     </row>
     <row r="42">
@@ -1565,16 +1565,16 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1.36</v>
+        <v>1.34</v>
       </c>
       <c r="E42" t="n">
-        <v>1277768501</v>
+        <v>1264025411</v>
       </c>
       <c r="F42" t="n">
-        <v>37264658</v>
+        <v>40244806</v>
       </c>
       <c r="G42" t="n">
-        <v>1.26672</v>
+        <v>-0.57759</v>
       </c>
     </row>
     <row r="43">
@@ -1592,16 +1592,16 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1.69</v>
+        <v>1.55</v>
       </c>
       <c r="E43" t="n">
-        <v>1214847082</v>
+        <v>1112859925</v>
       </c>
       <c r="F43" t="n">
-        <v>91062255</v>
+        <v>60081069</v>
       </c>
       <c r="G43" t="n">
-        <v>2.10258</v>
+        <v>-0.85655</v>
       </c>
     </row>
     <row r="44">
@@ -1619,16 +1619,16 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1246.18</v>
+        <v>1232.86</v>
       </c>
       <c r="E44" t="n">
-        <v>1123296555</v>
+        <v>1110384600</v>
       </c>
       <c r="F44" t="n">
-        <v>150814405</v>
+        <v>92594121</v>
       </c>
       <c r="G44" t="n">
-        <v>-1.48139</v>
+        <v>0.73881</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>RETH</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Rocket Pool ETH</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.051558</v>
+        <v>2006.7</v>
       </c>
       <c r="E45" t="n">
-        <v>1035295811</v>
+        <v>1005438874</v>
       </c>
       <c r="F45" t="n">
-        <v>26209171</v>
+        <v>5396065</v>
       </c>
       <c r="G45" t="n">
-        <v>12.4698</v>
+        <v>-0.13538</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>XDC</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>XDC Network</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.07346</v>
+        <v>0.107169</v>
       </c>
       <c r="E46" t="n">
-        <v>1020134211</v>
+        <v>979040189</v>
       </c>
       <c r="F46" t="n">
-        <v>23573112</v>
+        <v>34257496</v>
       </c>
       <c r="G46" t="n">
-        <v>1.75388</v>
+        <v>1.27626</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>RETH</t>
+          <t>AAVE</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Rocket Pool ETH</t>
+          <t>Aave</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>1977.08</v>
+        <v>65.29000000000001</v>
       </c>
       <c r="E47" t="n">
-        <v>978869063</v>
+        <v>948408667</v>
       </c>
       <c r="F47" t="n">
-        <v>2153055</v>
+        <v>56626564</v>
       </c>
       <c r="G47" t="n">
-        <v>0.1216</v>
+        <v>-1.34104</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.106285</v>
+        <v>0.04492355</v>
       </c>
       <c r="E48" t="n">
-        <v>970398056</v>
+        <v>911413390</v>
       </c>
       <c r="F48" t="n">
-        <v>58437186</v>
+        <v>17374165</v>
       </c>
       <c r="G48" t="n">
-        <v>1.97488</v>
+        <v>-2.66644</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>AAVE</t>
+          <t>ALGO</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Aave</t>
+          <t>Algorand</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>65.40000000000001</v>
+        <v>0.114077</v>
       </c>
       <c r="E49" t="n">
-        <v>949423102</v>
+        <v>891551189</v>
       </c>
       <c r="F49" t="n">
-        <v>61364375</v>
+        <v>34316017</v>
       </c>
       <c r="G49" t="n">
-        <v>1.71488</v>
+        <v>1.16763</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ALGO</t>
+          <t>XDC</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Algorand</t>
+          <t>XDC Network</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.107631</v>
+        <v>0.06385200000000001</v>
       </c>
       <c r="E50" t="n">
-        <v>840906547</v>
+        <v>884943140</v>
       </c>
       <c r="F50" t="n">
-        <v>20316973</v>
+        <v>13176740</v>
       </c>
       <c r="G50" t="n">
-        <v>2.24045</v>
+        <v>-2.9785</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>SAND</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>The Sandbox</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.406102</v>
+        <v>0.5944199999999999</v>
       </c>
       <c r="E51" t="n">
-        <v>834622081</v>
+        <v>832994043</v>
       </c>
       <c r="F51" t="n">
-        <v>70818243</v>
+        <v>15906286</v>
       </c>
       <c r="G51" t="n">
-        <v>2.33244</v>
+        <v>2.15945</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-08-20
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>29363</v>
+        <v>26147</v>
       </c>
       <c r="E2" t="n">
-        <v>571333545378</v>
+        <v>508944419962</v>
       </c>
       <c r="F2" t="n">
-        <v>3303796092</v>
+        <v>8354720331</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.13376</v>
+        <v>0.94137</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1848.18</v>
+        <v>1672.63</v>
       </c>
       <c r="E3" t="n">
-        <v>222076564062</v>
+        <v>201082244499</v>
       </c>
       <c r="F3" t="n">
-        <v>2310450298</v>
+        <v>8654979325</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.08673</v>
+        <v>0.79074</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999184</v>
+        <v>0.999888</v>
       </c>
       <c r="E4" t="n">
-        <v>83342810176</v>
+        <v>82782523125</v>
       </c>
       <c r="F4" t="n">
-        <v>7108679688</v>
+        <v>12887084993</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.008789999999999999</v>
+        <v>-0.07586</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>240.58</v>
+        <v>216.55</v>
       </c>
       <c r="E5" t="n">
-        <v>37018923781</v>
+        <v>33314509412</v>
       </c>
       <c r="F5" t="n">
-        <v>213453442</v>
+        <v>352761642</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.07003</v>
+        <v>0.63412</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.62698</v>
+        <v>0.5439580000000001</v>
       </c>
       <c r="E6" t="n">
-        <v>33106832695</v>
+        <v>28719636842</v>
       </c>
       <c r="F6" t="n">
-        <v>483544806</v>
+        <v>1339261159</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.39903</v>
+        <v>8.025550000000001</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.999383</v>
+        <v>0.99897</v>
       </c>
       <c r="E7" t="n">
-        <v>26149288275</v>
+        <v>25963465049</v>
       </c>
       <c r="F7" t="n">
-        <v>1179107340</v>
+        <v>4338512583</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.06833</v>
+        <v>-0.11487</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1846.9</v>
+        <v>1673.48</v>
       </c>
       <c r="E8" t="n">
-        <v>14936655272</v>
+        <v>13737122850</v>
       </c>
       <c r="F8" t="n">
-        <v>3754359</v>
+        <v>4876107</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.17284</v>
+        <v>0.84137</v>
       </c>
     </row>
     <row r="9">
@@ -665,25 +665,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>DOGE</t>
+          <t>ADA</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Dogecoin</t>
+          <t>Cardano</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.076025</v>
+        <v>0.267765</v>
       </c>
       <c r="E9" t="n">
-        <v>10692730010</v>
+        <v>9378891535</v>
       </c>
       <c r="F9" t="n">
-        <v>312734566</v>
+        <v>145815909</v>
       </c>
       <c r="G9" t="n">
-        <v>-1.02666</v>
+        <v>1.47134</v>
       </c>
     </row>
     <row r="10">
@@ -692,25 +692,25 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ADA</t>
+          <t>DOGE</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Cardano</t>
+          <t>Dogecoin</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.290117</v>
+        <v>0.064161</v>
       </c>
       <c r="E10" t="n">
-        <v>10171497411</v>
+        <v>9017665408</v>
       </c>
       <c r="F10" t="n">
-        <v>107779936</v>
+        <v>248625097</v>
       </c>
       <c r="G10" t="n">
-        <v>-1.28148</v>
+        <v>1.2268</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>24.65</v>
+        <v>21.89</v>
       </c>
       <c r="E11" t="n">
-        <v>10008374813</v>
+        <v>8928837932</v>
       </c>
       <c r="F11" t="n">
-        <v>287251378</v>
+        <v>226571899</v>
       </c>
       <c r="G11" t="n">
-        <v>0.50687</v>
+        <v>1.06256</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.077405</v>
+        <v>0.074889</v>
       </c>
       <c r="E12" t="n">
-        <v>6929030335</v>
+        <v>6696107467</v>
       </c>
       <c r="F12" t="n">
-        <v>143140064</v>
+        <v>155580362</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.02841</v>
+        <v>1.51578</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>5.03</v>
+        <v>4.52</v>
       </c>
       <c r="E13" t="n">
-        <v>6354890239</v>
+        <v>5725168908</v>
       </c>
       <c r="F13" t="n">
-        <v>66099430</v>
+        <v>81404260</v>
       </c>
       <c r="G13" t="n">
-        <v>0.02147</v>
+        <v>0.96538</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.678663</v>
+        <v>0.576191</v>
       </c>
       <c r="E14" t="n">
-        <v>6325172732</v>
+        <v>5368123016</v>
       </c>
       <c r="F14" t="n">
-        <v>93208608</v>
+        <v>172996725</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.36905</v>
+        <v>-0.41416</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>1.063e-05</v>
+        <v>8.389999999999999e-06</v>
       </c>
       <c r="E15" t="n">
-        <v>6277730810</v>
+        <v>4945250637</v>
       </c>
       <c r="F15" t="n">
-        <v>431703613</v>
+        <v>150797169</v>
       </c>
       <c r="G15" t="n">
-        <v>-2.46102</v>
+        <v>-1.08194</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>82.90000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="E16" t="n">
-        <v>6096772616</v>
+        <v>4802898610</v>
       </c>
       <c r="F16" t="n">
-        <v>356812368</v>
+        <v>15630116</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.99549</v>
+        <v>4.96089</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1.43</v>
+        <v>64.83</v>
       </c>
       <c r="E17" t="n">
-        <v>4936033777</v>
+        <v>4773195935</v>
       </c>
       <c r="F17" t="n">
-        <v>30373319</v>
+        <v>420143451</v>
       </c>
       <c r="G17" t="n">
-        <v>9.212440000000001</v>
+        <v>1.57336</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>29391</v>
+        <v>26226</v>
       </c>
       <c r="E18" t="n">
-        <v>4768484517</v>
+        <v>4256375499</v>
       </c>
       <c r="F18" t="n">
-        <v>30522230</v>
+        <v>58600219</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.1164</v>
+        <v>1.07334</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>6.12</v>
+        <v>0.999447</v>
       </c>
       <c r="E19" t="n">
-        <v>4617066618</v>
+        <v>3933070634</v>
       </c>
       <c r="F19" t="n">
-        <v>53502521</v>
+        <v>59512314</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.5577</v>
+        <v>-0.01357</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>227.82</v>
+        <v>10.86</v>
       </c>
       <c r="E20" t="n">
-        <v>4438553491</v>
+        <v>3736125562</v>
       </c>
       <c r="F20" t="n">
-        <v>98148620</v>
+        <v>79838820</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.61341</v>
+        <v>1.35132</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>12.35</v>
+        <v>4.9</v>
       </c>
       <c r="E21" t="n">
-        <v>4245537266</v>
+        <v>3695707344</v>
       </c>
       <c r="F21" t="n">
-        <v>82754761</v>
+        <v>81427803</v>
       </c>
       <c r="G21" t="n">
-        <v>-1.0073</v>
+        <v>-0.00773</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>7.5</v>
+        <v>188.22</v>
       </c>
       <c r="E22" t="n">
-        <v>4038541357</v>
+        <v>3665294031</v>
       </c>
       <c r="F22" t="n">
-        <v>122835487</v>
+        <v>165327543</v>
       </c>
       <c r="G22" t="n">
-        <v>0.71173</v>
+        <v>-0.12432</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.999619</v>
+        <v>3.85</v>
       </c>
       <c r="E23" t="n">
-        <v>3999458311</v>
+        <v>3614542293</v>
       </c>
       <c r="F23" t="n">
-        <v>56265311</v>
+        <v>492404</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.01704</v>
+        <v>-1.96984</v>
       </c>
     </row>
     <row r="24">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.138305</v>
+        <v>0.130233</v>
       </c>
       <c r="E24" t="n">
-        <v>3786616248</v>
+        <v>3570084986</v>
       </c>
       <c r="F24" t="n">
-        <v>58806981</v>
+        <v>134743513</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.08619</v>
+        <v>9.23034</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>4.03</v>
+        <v>6.2</v>
       </c>
       <c r="E25" t="n">
-        <v>3757947879</v>
+        <v>3335883953</v>
       </c>
       <c r="F25" t="n">
-        <v>829456</v>
+        <v>140922148</v>
       </c>
       <c r="G25" t="n">
-        <v>1.27446</v>
+        <v>0.80148</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.999841</v>
+        <v>0.998811</v>
       </c>
       <c r="E26" t="n">
-        <v>3371446673</v>
+        <v>3240223616</v>
       </c>
       <c r="F26" t="n">
-        <v>953231543</v>
+        <v>498448592</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.01211</v>
+        <v>-0.17773</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.999184</v>
+        <v>0.999126</v>
       </c>
       <c r="E27" t="n">
-        <v>2970859209</v>
+        <v>2761696957</v>
       </c>
       <c r="F27" t="n">
-        <v>61108173</v>
+        <v>1161988410</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.06144</v>
+        <v>0.07542</v>
       </c>
     </row>
     <row r="28">
@@ -1187,16 +1187,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>159.02</v>
+        <v>148.19</v>
       </c>
       <c r="E28" t="n">
-        <v>2883280463</v>
+        <v>2684835985</v>
       </c>
       <c r="F28" t="n">
-        <v>72144578</v>
+        <v>50372267</v>
       </c>
       <c r="G28" t="n">
-        <v>1.16487</v>
+        <v>3.04446</v>
       </c>
     </row>
     <row r="29">
@@ -1214,16 +1214,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>46.71</v>
+        <v>43.83</v>
       </c>
       <c r="E29" t="n">
-        <v>2802373037</v>
+        <v>2626366118</v>
       </c>
       <c r="F29" t="n">
-        <v>5304234</v>
+        <v>4992821</v>
       </c>
       <c r="G29" t="n">
-        <v>-3.00401</v>
+        <v>3.49681</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>17.66</v>
+        <v>7.84</v>
       </c>
       <c r="E30" t="n">
-        <v>2514932071</v>
+        <v>2292591070</v>
       </c>
       <c r="F30" t="n">
-        <v>54094016</v>
+        <v>93820497</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.07174999999999999</v>
+        <v>3.63317</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>8.44</v>
+        <v>15.54</v>
       </c>
       <c r="E31" t="n">
-        <v>2469359258</v>
+        <v>2215647967</v>
       </c>
       <c r="F31" t="n">
-        <v>64621810</v>
+        <v>55613456</v>
       </c>
       <c r="G31" t="n">
-        <v>0.67488</v>
+        <v>0.87935</v>
       </c>
     </row>
     <row r="32">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.056172</v>
+        <v>0.06232</v>
       </c>
       <c r="E32" t="n">
-        <v>1852562666</v>
+        <v>2056081744</v>
       </c>
       <c r="F32" t="n">
-        <v>16324683</v>
+        <v>90202973</v>
       </c>
       <c r="G32" t="n">
-        <v>-1.60931</v>
+        <v>-4.27712</v>
       </c>
     </row>
     <row r="33">
@@ -1322,16 +1322,16 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>4.1</v>
+        <v>3.56</v>
       </c>
       <c r="E33" t="n">
-        <v>1810280167</v>
+        <v>1574386555</v>
       </c>
       <c r="F33" t="n">
-        <v>52786199</v>
+        <v>63378654</v>
       </c>
       <c r="G33" t="n">
-        <v>-0.41291</v>
+        <v>0.57764</v>
       </c>
     </row>
     <row r="34">
@@ -1349,16 +1349,16 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>4.06</v>
+        <v>3.56</v>
       </c>
       <c r="E34" t="n">
-        <v>1793068862</v>
+        <v>1571248282</v>
       </c>
       <c r="F34" t="n">
-        <v>14078567</v>
+        <v>13634734</v>
       </c>
       <c r="G34" t="n">
-        <v>0.11028</v>
+        <v>1.66302</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>7.21</v>
+        <v>1.66</v>
       </c>
       <c r="E35" t="n">
-        <v>1621145976</v>
+        <v>1458687561</v>
       </c>
       <c r="F35" t="n">
-        <v>58254185</v>
+        <v>30772007</v>
       </c>
       <c r="G35" t="n">
-        <v>0.9799099999999999</v>
+        <v>0.64093</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1.83</v>
+        <v>100.01</v>
       </c>
       <c r="E36" t="n">
-        <v>1608902042</v>
+        <v>1454294861</v>
       </c>
       <c r="F36" t="n">
-        <v>64275190</v>
+        <v>12262212</v>
       </c>
       <c r="G36" t="n">
-        <v>-1.10577</v>
+        <v>-0.6747</v>
       </c>
     </row>
     <row r="37">
@@ -1430,16 +1430,16 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.462679</v>
+        <v>0.426022</v>
       </c>
       <c r="E37" t="n">
-        <v>1496606169</v>
+        <v>1377793336</v>
       </c>
       <c r="F37" t="n">
-        <v>4522297</v>
+        <v>9373096</v>
       </c>
       <c r="G37" t="n">
-        <v>0.007889999999999999</v>
+        <v>-0.15404</v>
       </c>
     </row>
     <row r="38">
@@ -1457,16 +1457,16 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.056974</v>
+        <v>0.052297</v>
       </c>
       <c r="E38" t="n">
-        <v>1492000194</v>
+        <v>1371820858</v>
       </c>
       <c r="F38" t="n">
-        <v>3365776</v>
+        <v>2899323</v>
       </c>
       <c r="G38" t="n">
-        <v>-0.38157</v>
+        <v>0.64296</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1.16</v>
+        <v>6.04</v>
       </c>
       <c r="E39" t="n">
-        <v>1479485675</v>
+        <v>1364650353</v>
       </c>
       <c r="F39" t="n">
-        <v>96635627</v>
+        <v>71113112</v>
       </c>
       <c r="G39" t="n">
-        <v>0.08483</v>
+        <v>1.10033</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>101.44</v>
+        <v>1.036</v>
       </c>
       <c r="E40" t="n">
-        <v>1475426292</v>
+        <v>1318623451</v>
       </c>
       <c r="F40" t="n">
-        <v>10583241</v>
+        <v>129140637</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.05005</v>
+        <v>2.4892</v>
       </c>
     </row>
     <row r="41">
@@ -1538,16 +1538,16 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.01798175</v>
+        <v>0.01625167</v>
       </c>
       <c r="E41" t="n">
-        <v>1307156169</v>
+        <v>1180954868</v>
       </c>
       <c r="F41" t="n">
-        <v>23665482</v>
+        <v>25085614</v>
       </c>
       <c r="G41" t="n">
-        <v>-0.01439</v>
+        <v>2.93322</v>
       </c>
     </row>
     <row r="42">
@@ -1565,16 +1565,16 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1.34</v>
+        <v>1.17</v>
       </c>
       <c r="E42" t="n">
-        <v>1264025411</v>
+        <v>1100934464</v>
       </c>
       <c r="F42" t="n">
-        <v>40244806</v>
+        <v>43223163</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.57759</v>
+        <v>1.64873</v>
       </c>
     </row>
     <row r="43">
@@ -1592,16 +1592,16 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1.55</v>
+        <v>1.47</v>
       </c>
       <c r="E43" t="n">
-        <v>1112859925</v>
+        <v>1053828862</v>
       </c>
       <c r="F43" t="n">
-        <v>60081069</v>
+        <v>66391038</v>
       </c>
       <c r="G43" t="n">
-        <v>-0.85655</v>
+        <v>0.13124</v>
       </c>
     </row>
     <row r="44">
@@ -1619,16 +1619,16 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1232.86</v>
+        <v>1110.31</v>
       </c>
       <c r="E44" t="n">
-        <v>1110384600</v>
+        <v>999837767</v>
       </c>
       <c r="F44" t="n">
-        <v>92594121</v>
+        <v>42632921</v>
       </c>
       <c r="G44" t="n">
-        <v>0.73881</v>
+        <v>1.89615</v>
       </c>
     </row>
     <row r="45">
@@ -1646,16 +1646,16 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>2006.7</v>
+        <v>1823.58</v>
       </c>
       <c r="E45" t="n">
-        <v>1005438874</v>
+        <v>913435101</v>
       </c>
       <c r="F45" t="n">
-        <v>5396065</v>
+        <v>10297184</v>
       </c>
       <c r="G45" t="n">
-        <v>-0.13538</v>
+        <v>0.97265</v>
       </c>
     </row>
     <row r="46">
@@ -1673,16 +1673,16 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.107169</v>
+        <v>0.09526900000000001</v>
       </c>
       <c r="E46" t="n">
-        <v>979040189</v>
+        <v>870904701</v>
       </c>
       <c r="F46" t="n">
-        <v>34257496</v>
+        <v>51708501</v>
       </c>
       <c r="G46" t="n">
-        <v>1.27626</v>
+        <v>3.07448</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>AAVE</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Aave</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>65.29000000000001</v>
+        <v>0.04144989</v>
       </c>
       <c r="E47" t="n">
-        <v>948408667</v>
+        <v>841880643</v>
       </c>
       <c r="F47" t="n">
-        <v>56626564</v>
+        <v>10174393</v>
       </c>
       <c r="G47" t="n">
-        <v>-1.34104</v>
+        <v>2.67073</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>AAVE</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Aave</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.04492355</v>
+        <v>56.94</v>
       </c>
       <c r="E48" t="n">
-        <v>911413390</v>
+        <v>826532196</v>
       </c>
       <c r="F48" t="n">
-        <v>17374165</v>
+        <v>57731717</v>
       </c>
       <c r="G48" t="n">
-        <v>-2.66644</v>
+        <v>1.68619</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ALGO</t>
+          <t>XDC</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Algorand</t>
+          <t>XDC Network</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.114077</v>
+        <v>0.058346</v>
       </c>
       <c r="E49" t="n">
-        <v>891551189</v>
+        <v>808337205</v>
       </c>
       <c r="F49" t="n">
-        <v>34316017</v>
+        <v>9862155</v>
       </c>
       <c r="G49" t="n">
-        <v>1.16763</v>
+        <v>2.50754</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>XDC</t>
+          <t>FRAX</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>XDC Network</t>
+          <t>Frax</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.06385200000000001</v>
+        <v>0.997945</v>
       </c>
       <c r="E50" t="n">
-        <v>884943140</v>
+        <v>805507599</v>
       </c>
       <c r="F50" t="n">
-        <v>13176740</v>
+        <v>7701598</v>
       </c>
       <c r="G50" t="n">
-        <v>-2.9785</v>
+        <v>0.02373</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>WBT</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>WhiteBIT Coin</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.5944199999999999</v>
+        <v>5.42</v>
       </c>
       <c r="E51" t="n">
-        <v>832994043</v>
+        <v>779302478</v>
       </c>
       <c r="F51" t="n">
-        <v>15906286</v>
+        <v>11509550</v>
       </c>
       <c r="G51" t="n">
-        <v>2.15945</v>
+        <v>0.08634</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-08-27
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>26147</v>
+        <v>26044</v>
       </c>
       <c r="E2" t="n">
-        <v>508944419962</v>
+        <v>506958697449</v>
       </c>
       <c r="F2" t="n">
-        <v>8354720331</v>
+        <v>3434370591</v>
       </c>
       <c r="G2" t="n">
-        <v>0.94137</v>
+        <v>0.07351000000000001</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1672.63</v>
+        <v>1648.51</v>
       </c>
       <c r="E3" t="n">
-        <v>201082244499</v>
+        <v>198127113636</v>
       </c>
       <c r="F3" t="n">
-        <v>8654979325</v>
+        <v>2370169187</v>
       </c>
       <c r="G3" t="n">
-        <v>0.79074</v>
+        <v>-0.02006</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999888</v>
+        <v>0.999378</v>
       </c>
       <c r="E4" t="n">
-        <v>82782523125</v>
+        <v>82802491526</v>
       </c>
       <c r="F4" t="n">
-        <v>12887084993</v>
+        <v>5828650468</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.07586</v>
+        <v>0.01024</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>216.55</v>
+        <v>216.72</v>
       </c>
       <c r="E5" t="n">
-        <v>33314509412</v>
+        <v>33329943321</v>
       </c>
       <c r="F5" t="n">
-        <v>352761642</v>
+        <v>190237548</v>
       </c>
       <c r="G5" t="n">
-        <v>0.63412</v>
+        <v>-0.06942</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.5439580000000001</v>
+        <v>0.526204</v>
       </c>
       <c r="E6" t="n">
-        <v>28719636842</v>
+        <v>27847136797</v>
       </c>
       <c r="F6" t="n">
-        <v>1339261159</v>
+        <v>466732452</v>
       </c>
       <c r="G6" t="n">
-        <v>8.025550000000001</v>
+        <v>0.77638</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.99897</v>
+        <v>0.999864</v>
       </c>
       <c r="E7" t="n">
-        <v>25963465049</v>
+        <v>26018604483</v>
       </c>
       <c r="F7" t="n">
-        <v>4338512583</v>
+        <v>1445591984</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.11487</v>
+        <v>-0.04011</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1673.48</v>
+        <v>1647.32</v>
       </c>
       <c r="E8" t="n">
-        <v>13737122850</v>
+        <v>13834721080</v>
       </c>
       <c r="F8" t="n">
-        <v>4876107</v>
+        <v>3947369</v>
       </c>
       <c r="G8" t="n">
-        <v>0.84137</v>
+        <v>-0.10148</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.267765</v>
+        <v>0.263356</v>
       </c>
       <c r="E9" t="n">
-        <v>9378891535</v>
+        <v>9224372100</v>
       </c>
       <c r="F9" t="n">
-        <v>145815909</v>
+        <v>127404453</v>
       </c>
       <c r="G9" t="n">
-        <v>1.47134</v>
+        <v>1.74286</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.064161</v>
+        <v>0.063135</v>
       </c>
       <c r="E10" t="n">
-        <v>9017665408</v>
+        <v>8882092728</v>
       </c>
       <c r="F10" t="n">
-        <v>248625097</v>
+        <v>140667452</v>
       </c>
       <c r="G10" t="n">
-        <v>1.2268</v>
+        <v>0.54836</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>21.89</v>
+        <v>20.6</v>
       </c>
       <c r="E11" t="n">
-        <v>8928837932</v>
+        <v>8389845541</v>
       </c>
       <c r="F11" t="n">
-        <v>226571899</v>
+        <v>163396346</v>
       </c>
       <c r="G11" t="n">
-        <v>1.06256</v>
+        <v>1.79039</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.074889</v>
+        <v>0.077309</v>
       </c>
       <c r="E12" t="n">
-        <v>6696107467</v>
+        <v>6908836430</v>
       </c>
       <c r="F12" t="n">
-        <v>155580362</v>
+        <v>129835797</v>
       </c>
       <c r="G12" t="n">
-        <v>1.51578</v>
+        <v>-0.15625</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>4.52</v>
+        <v>4.51</v>
       </c>
       <c r="E13" t="n">
-        <v>5725168908</v>
+        <v>5718452130</v>
       </c>
       <c r="F13" t="n">
-        <v>81404260</v>
+        <v>60712450</v>
       </c>
       <c r="G13" t="n">
-        <v>0.96538</v>
+        <v>0.1519</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.576191</v>
+        <v>1.48</v>
       </c>
       <c r="E14" t="n">
-        <v>5368123016</v>
+        <v>5102228069</v>
       </c>
       <c r="F14" t="n">
-        <v>172996725</v>
+        <v>22210101</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.41416</v>
+        <v>3.64884</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>8.389999999999999e-06</v>
+        <v>0.547096</v>
       </c>
       <c r="E15" t="n">
-        <v>4945250637</v>
+        <v>5096431700</v>
       </c>
       <c r="F15" t="n">
-        <v>150797169</v>
+        <v>130975474</v>
       </c>
       <c r="G15" t="n">
-        <v>-1.08194</v>
+        <v>0.01687</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1.4</v>
+        <v>65.2</v>
       </c>
       <c r="E16" t="n">
-        <v>4802898610</v>
+        <v>4796859420</v>
       </c>
       <c r="F16" t="n">
-        <v>15630116</v>
+        <v>188968239</v>
       </c>
       <c r="G16" t="n">
-        <v>4.96089</v>
+        <v>-0.28737</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>64.83</v>
+        <v>8.080000000000001e-06</v>
       </c>
       <c r="E17" t="n">
-        <v>4773195935</v>
+        <v>4767444805</v>
       </c>
       <c r="F17" t="n">
-        <v>420143451</v>
+        <v>73137453</v>
       </c>
       <c r="G17" t="n">
-        <v>1.57336</v>
+        <v>-1.15629</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>26226</v>
+        <v>26049</v>
       </c>
       <c r="E18" t="n">
-        <v>4256375499</v>
+        <v>4240351254</v>
       </c>
       <c r="F18" t="n">
-        <v>58600219</v>
+        <v>23139057</v>
       </c>
       <c r="G18" t="n">
-        <v>1.07334</v>
+        <v>0.1081</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.999447</v>
+        <v>0.999682</v>
       </c>
       <c r="E19" t="n">
-        <v>3933070634</v>
+        <v>3895962922</v>
       </c>
       <c r="F19" t="n">
-        <v>59512314</v>
+        <v>47510977</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.01357</v>
+        <v>-0.03604</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>10.86</v>
+        <v>191.16</v>
       </c>
       <c r="E20" t="n">
-        <v>3736125562</v>
+        <v>3723021445</v>
       </c>
       <c r="F20" t="n">
-        <v>79838820</v>
+        <v>68082496</v>
       </c>
       <c r="G20" t="n">
-        <v>1.35132</v>
+        <v>0.93882</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>4.9</v>
+        <v>10.18</v>
       </c>
       <c r="E21" t="n">
-        <v>3695707344</v>
+        <v>3598828249</v>
       </c>
       <c r="F21" t="n">
-        <v>81427803</v>
+        <v>92423171</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.00773</v>
+        <v>1.40042</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>188.22</v>
+        <v>3.81</v>
       </c>
       <c r="E22" t="n">
-        <v>3665294031</v>
+        <v>3540009135</v>
       </c>
       <c r="F22" t="n">
-        <v>165327543</v>
+        <v>142091</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.12432</v>
+        <v>-1.19456</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>3.85</v>
+        <v>4.63</v>
       </c>
       <c r="E23" t="n">
-        <v>3614542293</v>
+        <v>3486187353</v>
       </c>
       <c r="F23" t="n">
-        <v>492404</v>
+        <v>56023469</v>
       </c>
       <c r="G23" t="n">
-        <v>-1.96984</v>
+        <v>1.53667</v>
       </c>
     </row>
     <row r="24">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.130233</v>
+        <v>0.121001</v>
       </c>
       <c r="E24" t="n">
-        <v>3570084986</v>
+        <v>3316709829</v>
       </c>
       <c r="F24" t="n">
-        <v>134743513</v>
+        <v>55830039</v>
       </c>
       <c r="G24" t="n">
-        <v>9.23034</v>
+        <v>-1.53255</v>
       </c>
     </row>
     <row r="25">
@@ -1106,16 +1106,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>6.2</v>
+        <v>5.97</v>
       </c>
       <c r="E25" t="n">
-        <v>3335883953</v>
+        <v>3207520741</v>
       </c>
       <c r="F25" t="n">
-        <v>140922148</v>
+        <v>88308038</v>
       </c>
       <c r="G25" t="n">
-        <v>0.80148</v>
+        <v>-0.648</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.998811</v>
+        <v>0.99984</v>
       </c>
       <c r="E26" t="n">
-        <v>3240223616</v>
+        <v>3144617444</v>
       </c>
       <c r="F26" t="n">
-        <v>498448592</v>
+        <v>601426693</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.17773</v>
+        <v>0.00784</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.999126</v>
+        <v>0.998996</v>
       </c>
       <c r="E27" t="n">
-        <v>2761696957</v>
+        <v>2904170794</v>
       </c>
       <c r="F27" t="n">
-        <v>1161988410</v>
+        <v>470443550</v>
       </c>
       <c r="G27" t="n">
-        <v>0.07542</v>
+        <v>0.03631</v>
       </c>
     </row>
     <row r="28">
@@ -1187,16 +1187,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>148.19</v>
+        <v>144.34</v>
       </c>
       <c r="E28" t="n">
-        <v>2684835985</v>
+        <v>2619510023</v>
       </c>
       <c r="F28" t="n">
-        <v>50372267</v>
+        <v>70241292</v>
       </c>
       <c r="G28" t="n">
-        <v>3.04446</v>
+        <v>1.2331</v>
       </c>
     </row>
     <row r="29">
@@ -1214,16 +1214,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>43.83</v>
+        <v>42.87</v>
       </c>
       <c r="E29" t="n">
-        <v>2626366118</v>
+        <v>2572151879</v>
       </c>
       <c r="F29" t="n">
-        <v>4992821</v>
+        <v>1535814</v>
       </c>
       <c r="G29" t="n">
-        <v>3.49681</v>
+        <v>0.03573</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>7.84</v>
+        <v>15.85</v>
       </c>
       <c r="E30" t="n">
-        <v>2292591070</v>
+        <v>2260260690</v>
       </c>
       <c r="F30" t="n">
-        <v>93820497</v>
+        <v>41445753</v>
       </c>
       <c r="G30" t="n">
-        <v>3.63317</v>
+        <v>0.1097</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>15.54</v>
+        <v>7.12</v>
       </c>
       <c r="E31" t="n">
-        <v>2215647967</v>
+        <v>2081985459</v>
       </c>
       <c r="F31" t="n">
-        <v>55613456</v>
+        <v>77102043</v>
       </c>
       <c r="G31" t="n">
-        <v>0.87935</v>
+        <v>-1.18019</v>
       </c>
     </row>
     <row r="32">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.06232</v>
+        <v>0.057744</v>
       </c>
       <c r="E32" t="n">
-        <v>2056081744</v>
+        <v>1907007600</v>
       </c>
       <c r="F32" t="n">
-        <v>90202973</v>
+        <v>54014405</v>
       </c>
       <c r="G32" t="n">
-        <v>-4.27712</v>
+        <v>0.06707</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>3.56</v>
+        <v>3.54</v>
       </c>
       <c r="E33" t="n">
-        <v>1574386555</v>
+        <v>1562823720</v>
       </c>
       <c r="F33" t="n">
-        <v>63378654</v>
+        <v>16920048</v>
       </c>
       <c r="G33" t="n">
-        <v>0.57764</v>
+        <v>-0.0267</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>3.56</v>
+        <v>103.31</v>
       </c>
       <c r="E34" t="n">
-        <v>1571248282</v>
+        <v>1504118148</v>
       </c>
       <c r="F34" t="n">
-        <v>13634734</v>
+        <v>15589299</v>
       </c>
       <c r="G34" t="n">
-        <v>1.66302</v>
+        <v>-1.24585</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1.66</v>
+        <v>3.24</v>
       </c>
       <c r="E35" t="n">
-        <v>1458687561</v>
+        <v>1436290899</v>
       </c>
       <c r="F35" t="n">
-        <v>30772007</v>
+        <v>53987319</v>
       </c>
       <c r="G35" t="n">
-        <v>0.64093</v>
+        <v>-0.50931</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>100.01</v>
+        <v>0.435081</v>
       </c>
       <c r="E36" t="n">
-        <v>1454294861</v>
+        <v>1407806378</v>
       </c>
       <c r="F36" t="n">
-        <v>12262212</v>
+        <v>3310735</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.6747</v>
+        <v>0.59217</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.426022</v>
+        <v>1.59</v>
       </c>
       <c r="E37" t="n">
-        <v>1377793336</v>
+        <v>1405900344</v>
       </c>
       <c r="F37" t="n">
-        <v>9373096</v>
+        <v>45896445</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.15404</v>
+        <v>-0.05311</v>
       </c>
     </row>
     <row r="38">
@@ -1457,16 +1457,16 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.052297</v>
+        <v>0.05107</v>
       </c>
       <c r="E38" t="n">
-        <v>1371820858</v>
+        <v>1339413478</v>
       </c>
       <c r="F38" t="n">
-        <v>2899323</v>
+        <v>3029891</v>
       </c>
       <c r="G38" t="n">
-        <v>0.64296</v>
+        <v>0.00362</v>
       </c>
     </row>
     <row r="39">
@@ -1484,16 +1484,16 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>6.04</v>
+        <v>5.7</v>
       </c>
       <c r="E39" t="n">
-        <v>1364650353</v>
+        <v>1297184221</v>
       </c>
       <c r="F39" t="n">
-        <v>71113112</v>
+        <v>29566935</v>
       </c>
       <c r="G39" t="n">
-        <v>1.10033</v>
+        <v>-0.79947</v>
       </c>
     </row>
     <row r="40">
@@ -1511,16 +1511,16 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1.036</v>
+        <v>0.956992</v>
       </c>
       <c r="E40" t="n">
-        <v>1318623451</v>
+        <v>1219301114</v>
       </c>
       <c r="F40" t="n">
-        <v>129140637</v>
+        <v>90823071</v>
       </c>
       <c r="G40" t="n">
-        <v>2.4892</v>
+        <v>1.82277</v>
       </c>
     </row>
     <row r="41">
@@ -1538,16 +1538,16 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.01625167</v>
+        <v>0.01584905</v>
       </c>
       <c r="E41" t="n">
-        <v>1180954868</v>
+        <v>1151043225</v>
       </c>
       <c r="F41" t="n">
-        <v>25085614</v>
+        <v>19879938</v>
       </c>
       <c r="G41" t="n">
-        <v>2.93322</v>
+        <v>-0.77488</v>
       </c>
     </row>
     <row r="42">
@@ -1565,16 +1565,16 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1.17</v>
+        <v>1.2</v>
       </c>
       <c r="E42" t="n">
-        <v>1100934464</v>
+        <v>1125050969</v>
       </c>
       <c r="F42" t="n">
-        <v>43223163</v>
+        <v>53752245</v>
       </c>
       <c r="G42" t="n">
-        <v>1.64873</v>
+        <v>-0.50285</v>
       </c>
     </row>
     <row r="43">
@@ -1595,13 +1595,13 @@
         <v>1.47</v>
       </c>
       <c r="E43" t="n">
-        <v>1053828862</v>
+        <v>1051579744</v>
       </c>
       <c r="F43" t="n">
-        <v>66391038</v>
+        <v>58995108</v>
       </c>
       <c r="G43" t="n">
-        <v>0.13124</v>
+        <v>-1.51614</v>
       </c>
     </row>
     <row r="44">
@@ -1619,16 +1619,16 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1110.31</v>
+        <v>1053.26</v>
       </c>
       <c r="E44" t="n">
-        <v>999837767</v>
+        <v>948356738</v>
       </c>
       <c r="F44" t="n">
-        <v>42632921</v>
+        <v>42789829</v>
       </c>
       <c r="G44" t="n">
-        <v>1.89615</v>
+        <v>2.21602</v>
       </c>
     </row>
     <row r="45">
@@ -1646,16 +1646,16 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>1823.58</v>
+        <v>1785.7</v>
       </c>
       <c r="E45" t="n">
-        <v>913435101</v>
+        <v>917437844</v>
       </c>
       <c r="F45" t="n">
-        <v>10297184</v>
+        <v>11294099</v>
       </c>
       <c r="G45" t="n">
-        <v>0.97265</v>
+        <v>-0.24803</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>AAVE</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Aave</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.09526900000000001</v>
+        <v>57.12</v>
       </c>
       <c r="E46" t="n">
-        <v>870904701</v>
+        <v>828438467</v>
       </c>
       <c r="F46" t="n">
-        <v>51708501</v>
+        <v>51323287</v>
       </c>
       <c r="G46" t="n">
-        <v>3.07448</v>
+        <v>0.35197</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.04144989</v>
+        <v>0.08867</v>
       </c>
       <c r="E47" t="n">
-        <v>841880643</v>
+        <v>811983493</v>
       </c>
       <c r="F47" t="n">
-        <v>10174393</v>
+        <v>25680687</v>
       </c>
       <c r="G47" t="n">
-        <v>2.67073</v>
+        <v>-0.79378</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>AAVE</t>
+          <t>FRAX</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Aave</t>
+          <t>Frax</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>56.94</v>
+        <v>0.997003</v>
       </c>
       <c r="E48" t="n">
-        <v>826532196</v>
+        <v>804268385</v>
       </c>
       <c r="F48" t="n">
-        <v>57731717</v>
+        <v>3680667</v>
       </c>
       <c r="G48" t="n">
-        <v>1.68619</v>
+        <v>-0.11491</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>XDC</t>
+          <t>WBT</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>XDC Network</t>
+          <t>WhiteBIT Coin</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.058346</v>
+        <v>5.37</v>
       </c>
       <c r="E49" t="n">
-        <v>808337205</v>
+        <v>774075836</v>
       </c>
       <c r="F49" t="n">
-        <v>9862155</v>
+        <v>6518263</v>
       </c>
       <c r="G49" t="n">
-        <v>2.50754</v>
+        <v>-0.27053</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>FRAX</t>
+          <t>ALGO</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Frax</t>
+          <t>Algorand</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.997945</v>
+        <v>0.094763</v>
       </c>
       <c r="E50" t="n">
-        <v>805507599</v>
+        <v>741014084</v>
       </c>
       <c r="F50" t="n">
-        <v>7701598</v>
+        <v>13647532</v>
       </c>
       <c r="G50" t="n">
-        <v>0.02373</v>
+        <v>-1.01591</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>WBT</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>WhiteBIT Coin</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>5.42</v>
+        <v>0.03670698</v>
       </c>
       <c r="E51" t="n">
-        <v>779302478</v>
+        <v>737570345</v>
       </c>
       <c r="F51" t="n">
-        <v>11509550</v>
+        <v>8085140</v>
       </c>
       <c r="G51" t="n">
-        <v>0.08634</v>
+        <v>2.14587</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-09-03
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>26044</v>
+        <v>25923</v>
       </c>
       <c r="E2" t="n">
-        <v>506958697449</v>
+        <v>505056033865</v>
       </c>
       <c r="F2" t="n">
-        <v>3434370591</v>
+        <v>4418612806</v>
       </c>
       <c r="G2" t="n">
-        <v>0.07351000000000001</v>
+        <v>0.40406</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1648.51</v>
+        <v>1633.2</v>
       </c>
       <c r="E3" t="n">
-        <v>198127113636</v>
+        <v>196426979119</v>
       </c>
       <c r="F3" t="n">
-        <v>2370169187</v>
+        <v>3549291287</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.02006</v>
+        <v>-0.03559</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999378</v>
+        <v>0.9994</v>
       </c>
       <c r="E4" t="n">
-        <v>82802491526</v>
+        <v>82891856881</v>
       </c>
       <c r="F4" t="n">
-        <v>5828650468</v>
+        <v>7954811634</v>
       </c>
       <c r="G4" t="n">
-        <v>0.01024</v>
+        <v>-0.01768</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>216.72</v>
+        <v>214.48</v>
       </c>
       <c r="E5" t="n">
-        <v>33329943321</v>
+        <v>33014771455</v>
       </c>
       <c r="F5" t="n">
-        <v>190237548</v>
+        <v>229554722</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.06942</v>
+        <v>-0.06374</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.526204</v>
+        <v>0.502923</v>
       </c>
       <c r="E6" t="n">
-        <v>27847136797</v>
+        <v>26645139059</v>
       </c>
       <c r="F6" t="n">
-        <v>466732452</v>
+        <v>528038859</v>
       </c>
       <c r="G6" t="n">
-        <v>0.77638</v>
+        <v>1.05653</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.999864</v>
+        <v>0.999471</v>
       </c>
       <c r="E7" t="n">
-        <v>26018604483</v>
+        <v>26183102929</v>
       </c>
       <c r="F7" t="n">
-        <v>1445591984</v>
+        <v>1975122872</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.04011</v>
+        <v>-0.05115</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1647.32</v>
+        <v>1632.61</v>
       </c>
       <c r="E8" t="n">
-        <v>13834721080</v>
+        <v>13951987479</v>
       </c>
       <c r="F8" t="n">
-        <v>3947369</v>
+        <v>6404663</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.10148</v>
+        <v>-0.02969</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.263356</v>
+        <v>0.254568</v>
       </c>
       <c r="E9" t="n">
-        <v>9224372100</v>
+        <v>8925549096</v>
       </c>
       <c r="F9" t="n">
-        <v>127404453</v>
+        <v>108085140</v>
       </c>
       <c r="G9" t="n">
-        <v>1.74286</v>
+        <v>-0.2249</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.063135</v>
+        <v>0.063301</v>
       </c>
       <c r="E10" t="n">
-        <v>8882092728</v>
+        <v>8918233250</v>
       </c>
       <c r="F10" t="n">
-        <v>140667452</v>
+        <v>222858490</v>
       </c>
       <c r="G10" t="n">
-        <v>0.54836</v>
+        <v>-0.09375</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>20.6</v>
+        <v>19.4</v>
       </c>
       <c r="E11" t="n">
-        <v>8389845541</v>
+        <v>7939475440</v>
       </c>
       <c r="F11" t="n">
-        <v>163396346</v>
+        <v>195136171</v>
       </c>
       <c r="G11" t="n">
-        <v>1.79039</v>
+        <v>-0.84099</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.077309</v>
+        <v>0.076975</v>
       </c>
       <c r="E12" t="n">
-        <v>6908836430</v>
+        <v>6877035415</v>
       </c>
       <c r="F12" t="n">
-        <v>129835797</v>
+        <v>137841026</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.15625</v>
+        <v>0.45218</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>4.51</v>
+        <v>1.87</v>
       </c>
       <c r="E13" t="n">
-        <v>5718452130</v>
+        <v>6427508543</v>
       </c>
       <c r="F13" t="n">
-        <v>60712450</v>
+        <v>28787534</v>
       </c>
       <c r="G13" t="n">
-        <v>0.1519</v>
+        <v>-2.41439</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>1.48</v>
+        <v>4.27</v>
       </c>
       <c r="E14" t="n">
-        <v>5102228069</v>
+        <v>5430187963</v>
       </c>
       <c r="F14" t="n">
-        <v>22210101</v>
+        <v>68667287</v>
       </c>
       <c r="G14" t="n">
-        <v>3.64884</v>
+        <v>0.81496</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.547096</v>
+        <v>0.543806</v>
       </c>
       <c r="E15" t="n">
-        <v>5096431700</v>
+        <v>5071450465</v>
       </c>
       <c r="F15" t="n">
-        <v>130975474</v>
+        <v>132458424</v>
       </c>
       <c r="G15" t="n">
-        <v>0.01687</v>
+        <v>0.08871</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>65.2</v>
+        <v>64.06999999999999</v>
       </c>
       <c r="E16" t="n">
-        <v>4796859420</v>
+        <v>4717511503</v>
       </c>
       <c r="F16" t="n">
-        <v>188968239</v>
+        <v>258219481</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.28737</v>
+        <v>0.15161</v>
       </c>
     </row>
     <row r="17">
@@ -890,16 +890,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>8.080000000000001e-06</v>
+        <v>7.8e-06</v>
       </c>
       <c r="E17" t="n">
-        <v>4767444805</v>
+        <v>4603976979</v>
       </c>
       <c r="F17" t="n">
-        <v>73137453</v>
+        <v>66639681</v>
       </c>
       <c r="G17" t="n">
-        <v>-1.15629</v>
+        <v>-0.72229</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>26049</v>
+        <v>25927</v>
       </c>
       <c r="E18" t="n">
-        <v>4240351254</v>
+        <v>4224992976</v>
       </c>
       <c r="F18" t="n">
-        <v>23139057</v>
+        <v>25511543</v>
       </c>
       <c r="G18" t="n">
-        <v>0.1081</v>
+        <v>0.34156</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.999682</v>
+        <v>0.999483</v>
       </c>
       <c r="E19" t="n">
-        <v>3895962922</v>
+        <v>3874000837</v>
       </c>
       <c r="F19" t="n">
-        <v>47510977</v>
+        <v>46237840</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.03604</v>
+        <v>-0.16045</v>
       </c>
     </row>
     <row r="20">
@@ -971,16 +971,16 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>191.16</v>
+        <v>195.13</v>
       </c>
       <c r="E20" t="n">
-        <v>3723021445</v>
+        <v>3806659582</v>
       </c>
       <c r="F20" t="n">
-        <v>68082496</v>
+        <v>119764334</v>
       </c>
       <c r="G20" t="n">
-        <v>0.93882</v>
+        <v>-2.42734</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>10.18</v>
+        <v>3.9</v>
       </c>
       <c r="E21" t="n">
-        <v>3598828249</v>
+        <v>3629732023</v>
       </c>
       <c r="F21" t="n">
-        <v>92423171</v>
+        <v>138620</v>
       </c>
       <c r="G21" t="n">
-        <v>1.40042</v>
+        <v>-0.01904</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>3.81</v>
+        <v>9.92</v>
       </c>
       <c r="E22" t="n">
-        <v>3540009135</v>
+        <v>3512172570</v>
       </c>
       <c r="F22" t="n">
-        <v>142091</v>
+        <v>95226789</v>
       </c>
       <c r="G22" t="n">
-        <v>-1.19456</v>
+        <v>0.7204199999999999</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>TUSD</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>4.63</v>
+        <v>0.998293</v>
       </c>
       <c r="E23" t="n">
-        <v>3486187353</v>
+        <v>3443012753</v>
       </c>
       <c r="F23" t="n">
-        <v>56023469</v>
+        <v>878740664</v>
       </c>
       <c r="G23" t="n">
-        <v>1.53667</v>
+        <v>0.00778</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.121001</v>
+        <v>4.44</v>
       </c>
       <c r="E24" t="n">
-        <v>3316709829</v>
+        <v>3348371247</v>
       </c>
       <c r="F24" t="n">
-        <v>55830039</v>
+        <v>61143801</v>
       </c>
       <c r="G24" t="n">
-        <v>-1.53255</v>
+        <v>1.8923</v>
       </c>
     </row>
     <row r="25">
@@ -1106,16 +1106,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>5.97</v>
+        <v>6.03</v>
       </c>
       <c r="E25" t="n">
-        <v>3207520741</v>
+        <v>3246988179</v>
       </c>
       <c r="F25" t="n">
-        <v>88308038</v>
+        <v>176635621</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.648</v>
+        <v>1.48924</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Binance USD</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.99984</v>
+        <v>0.114821</v>
       </c>
       <c r="E26" t="n">
-        <v>3144617444</v>
+        <v>3155281863</v>
       </c>
       <c r="F26" t="n">
-        <v>601426693</v>
+        <v>59611121</v>
       </c>
       <c r="G26" t="n">
-        <v>0.00784</v>
+        <v>1.98807</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>Binance USD</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.998996</v>
+        <v>1</v>
       </c>
       <c r="E27" t="n">
-        <v>2904170794</v>
+        <v>2857631613</v>
       </c>
       <c r="F27" t="n">
-        <v>470443550</v>
+        <v>1401855790</v>
       </c>
       <c r="G27" t="n">
-        <v>0.03631</v>
+        <v>-0.01037</v>
       </c>
     </row>
     <row r="28">
@@ -1187,16 +1187,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>144.34</v>
+        <v>140.69</v>
       </c>
       <c r="E28" t="n">
-        <v>2619510023</v>
+        <v>2555100174</v>
       </c>
       <c r="F28" t="n">
-        <v>70241292</v>
+        <v>46399656</v>
       </c>
       <c r="G28" t="n">
-        <v>1.2331</v>
+        <v>0.13799</v>
       </c>
     </row>
     <row r="29">
@@ -1214,16 +1214,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>42.87</v>
+        <v>42.04</v>
       </c>
       <c r="E29" t="n">
-        <v>2572151879</v>
+        <v>2524796778</v>
       </c>
       <c r="F29" t="n">
-        <v>1535814</v>
+        <v>5375862</v>
       </c>
       <c r="G29" t="n">
-        <v>0.03573</v>
+        <v>-1.60429</v>
       </c>
     </row>
     <row r="30">
@@ -1241,16 +1241,16 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>15.85</v>
+        <v>15.46</v>
       </c>
       <c r="E30" t="n">
-        <v>2260260690</v>
+        <v>2208522245</v>
       </c>
       <c r="F30" t="n">
-        <v>41445753</v>
+        <v>41431556</v>
       </c>
       <c r="G30" t="n">
-        <v>0.1097</v>
+        <v>0.31018</v>
       </c>
     </row>
     <row r="31">
@@ -1268,16 +1268,16 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>7.12</v>
+        <v>6.85</v>
       </c>
       <c r="E31" t="n">
-        <v>2081985459</v>
+        <v>2004316497</v>
       </c>
       <c r="F31" t="n">
-        <v>77102043</v>
+        <v>78929214</v>
       </c>
       <c r="G31" t="n">
-        <v>-1.18019</v>
+        <v>2.01979</v>
       </c>
     </row>
     <row r="32">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.057744</v>
+        <v>0.04984048</v>
       </c>
       <c r="E32" t="n">
-        <v>1907007600</v>
+        <v>1656547219</v>
       </c>
       <c r="F32" t="n">
-        <v>54014405</v>
+        <v>52399637</v>
       </c>
       <c r="G32" t="n">
-        <v>0.06707</v>
+        <v>1.29392</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>3.54</v>
+        <v>0.452298</v>
       </c>
       <c r="E33" t="n">
-        <v>1562823720</v>
+        <v>1462493425</v>
       </c>
       <c r="F33" t="n">
-        <v>16920048</v>
+        <v>7834196</v>
       </c>
       <c r="G33" t="n">
-        <v>-0.0267</v>
+        <v>-0.02991</v>
       </c>
     </row>
     <row r="34">
@@ -1349,16 +1349,16 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>103.31</v>
+        <v>100.01</v>
       </c>
       <c r="E34" t="n">
-        <v>1504118148</v>
+        <v>1454863824</v>
       </c>
       <c r="F34" t="n">
-        <v>15589299</v>
+        <v>9057600</v>
       </c>
       <c r="G34" t="n">
-        <v>-1.24585</v>
+        <v>0.37744</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D35" t="n">
         <v>3.24</v>
       </c>
       <c r="E35" t="n">
-        <v>1436290899</v>
+        <v>1435096866</v>
       </c>
       <c r="F35" t="n">
-        <v>53987319</v>
+        <v>11741138</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.50931</v>
+        <v>-0.71478</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.435081</v>
+        <v>3.18</v>
       </c>
       <c r="E36" t="n">
-        <v>1407806378</v>
+        <v>1416937040</v>
       </c>
       <c r="F36" t="n">
-        <v>3310735</v>
+        <v>65446688</v>
       </c>
       <c r="G36" t="n">
-        <v>0.59217</v>
+        <v>0.107</v>
       </c>
     </row>
     <row r="37">
@@ -1430,16 +1430,16 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1.59</v>
+        <v>1.54</v>
       </c>
       <c r="E37" t="n">
-        <v>1405900344</v>
+        <v>1366131615</v>
       </c>
       <c r="F37" t="n">
-        <v>45896445</v>
+        <v>33125198</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.05311</v>
+        <v>-0.18547</v>
       </c>
     </row>
     <row r="38">
@@ -1457,16 +1457,16 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.05107</v>
+        <v>0.05039</v>
       </c>
       <c r="E38" t="n">
-        <v>1339413478</v>
+        <v>1324134397</v>
       </c>
       <c r="F38" t="n">
-        <v>3029891</v>
+        <v>4280772</v>
       </c>
       <c r="G38" t="n">
-        <v>0.00362</v>
+        <v>0.28518</v>
       </c>
     </row>
     <row r="39">
@@ -1484,16 +1484,16 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>5.7</v>
+        <v>5.55</v>
       </c>
       <c r="E39" t="n">
-        <v>1297184221</v>
+        <v>1270569880</v>
       </c>
       <c r="F39" t="n">
-        <v>29566935</v>
+        <v>47496346</v>
       </c>
       <c r="G39" t="n">
-        <v>-0.79947</v>
+        <v>-0.44056</v>
       </c>
     </row>
     <row r="40">
@@ -1511,16 +1511,16 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.956992</v>
+        <v>0.893548</v>
       </c>
       <c r="E40" t="n">
-        <v>1219301114</v>
+        <v>1140722630</v>
       </c>
       <c r="F40" t="n">
-        <v>90823071</v>
+        <v>72456501</v>
       </c>
       <c r="G40" t="n">
-        <v>1.82277</v>
+        <v>0.60575</v>
       </c>
     </row>
     <row r="41">
@@ -1538,16 +1538,16 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.01584905</v>
+        <v>0.01546759</v>
       </c>
       <c r="E41" t="n">
-        <v>1151043225</v>
+        <v>1126488234</v>
       </c>
       <c r="F41" t="n">
-        <v>19879938</v>
+        <v>29302542</v>
       </c>
       <c r="G41" t="n">
-        <v>-0.77488</v>
+        <v>-0.38207</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1.2</v>
+        <v>1.34</v>
       </c>
       <c r="E42" t="n">
-        <v>1125050969</v>
+        <v>1067077806</v>
       </c>
       <c r="F42" t="n">
-        <v>53752245</v>
+        <v>64205586</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.50285</v>
+        <v>0.38549</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1.47</v>
+        <v>1.13</v>
       </c>
       <c r="E43" t="n">
-        <v>1051579744</v>
+        <v>1064718009</v>
       </c>
       <c r="F43" t="n">
-        <v>58995108</v>
+        <v>38574968</v>
       </c>
       <c r="G43" t="n">
-        <v>-1.51614</v>
+        <v>0.21191</v>
       </c>
     </row>
     <row r="44">
@@ -1619,16 +1619,16 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1053.26</v>
+        <v>1129.01</v>
       </c>
       <c r="E44" t="n">
-        <v>948356738</v>
+        <v>1017292323</v>
       </c>
       <c r="F44" t="n">
-        <v>42789829</v>
+        <v>66882826</v>
       </c>
       <c r="G44" t="n">
-        <v>2.21602</v>
+        <v>-2.01109</v>
       </c>
     </row>
     <row r="45">
@@ -1646,16 +1646,16 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>1785.7</v>
+        <v>1769.6</v>
       </c>
       <c r="E45" t="n">
-        <v>917437844</v>
+        <v>926134410</v>
       </c>
       <c r="F45" t="n">
-        <v>11294099</v>
+        <v>3521798</v>
       </c>
       <c r="G45" t="n">
-        <v>-0.24803</v>
+        <v>-0.11296</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>AAVE</t>
+          <t>XDC</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Aave</t>
+          <t>XDC Network</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>57.12</v>
+        <v>0.058294</v>
       </c>
       <c r="E46" t="n">
-        <v>828438467</v>
+        <v>808335912</v>
       </c>
       <c r="F46" t="n">
-        <v>51323287</v>
+        <v>11862776</v>
       </c>
       <c r="G46" t="n">
-        <v>0.35197</v>
+        <v>0.25537</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>FRAX</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Frax</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.08867</v>
+        <v>0.997702</v>
       </c>
       <c r="E47" t="n">
-        <v>811983493</v>
+        <v>805006687</v>
       </c>
       <c r="F47" t="n">
-        <v>25680687</v>
+        <v>4835283</v>
       </c>
       <c r="G47" t="n">
-        <v>-0.79378</v>
+        <v>-0.08524</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>FRAX</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Frax</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.997003</v>
+        <v>0.087434</v>
       </c>
       <c r="E48" t="n">
-        <v>804268385</v>
+        <v>803609370</v>
       </c>
       <c r="F48" t="n">
-        <v>3680667</v>
+        <v>26240002</v>
       </c>
       <c r="G48" t="n">
-        <v>-0.11491</v>
+        <v>1.89629</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>WBT</t>
+          <t>AAVE</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>WhiteBIT Coin</t>
+          <t>Aave</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>5.37</v>
+        <v>54.61</v>
       </c>
       <c r="E49" t="n">
-        <v>774075836</v>
+        <v>794272734</v>
       </c>
       <c r="F49" t="n">
-        <v>6518263</v>
+        <v>61599885</v>
       </c>
       <c r="G49" t="n">
-        <v>-0.27053</v>
+        <v>0.14874</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ALGO</t>
+          <t>WBT</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Algorand</t>
+          <t>WhiteBIT Coin</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.094763</v>
+        <v>5.34</v>
       </c>
       <c r="E50" t="n">
-        <v>741014084</v>
+        <v>770440438</v>
       </c>
       <c r="F50" t="n">
-        <v>13647532</v>
+        <v>6008766</v>
       </c>
       <c r="G50" t="n">
-        <v>-1.01591</v>
+        <v>-0.10526</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>ALGO</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Algorand</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.03670698</v>
+        <v>0.094304</v>
       </c>
       <c r="E51" t="n">
-        <v>737570345</v>
+        <v>739219103</v>
       </c>
       <c r="F51" t="n">
-        <v>8085140</v>
+        <v>14335328</v>
       </c>
       <c r="G51" t="n">
-        <v>2.14587</v>
+        <v>1.71761</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-09-10
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>25923</v>
+        <v>25810</v>
       </c>
       <c r="E2" t="n">
-        <v>505056033865</v>
+        <v>502572400738</v>
       </c>
       <c r="F2" t="n">
-        <v>4418612806</v>
+        <v>4541272403</v>
       </c>
       <c r="G2" t="n">
-        <v>0.40406</v>
+        <v>-0.16589</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1633.2</v>
+        <v>1625.83</v>
       </c>
       <c r="E3" t="n">
-        <v>196426979119</v>
+        <v>195386934022</v>
       </c>
       <c r="F3" t="n">
-        <v>3549291287</v>
+        <v>3420405220</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.03559</v>
+        <v>-0.5466800000000001</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.9994</v>
+        <v>0.999846</v>
       </c>
       <c r="E4" t="n">
-        <v>82891856881</v>
+        <v>83002670998</v>
       </c>
       <c r="F4" t="n">
-        <v>7954811634</v>
+        <v>10100280055</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.01768</v>
+        <v>0.00924</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>214.48</v>
+        <v>213.03</v>
       </c>
       <c r="E5" t="n">
-        <v>33014771455</v>
+        <v>32749186633</v>
       </c>
       <c r="F5" t="n">
-        <v>229554722</v>
+        <v>234969881</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.06374</v>
+        <v>-0.96637</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.502923</v>
+        <v>0.499586</v>
       </c>
       <c r="E6" t="n">
-        <v>26645139059</v>
+        <v>26516032516</v>
       </c>
       <c r="F6" t="n">
-        <v>528038859</v>
+        <v>343609476</v>
       </c>
       <c r="G6" t="n">
-        <v>1.05653</v>
+        <v>-0.69555</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.999471</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>26183102929</v>
+        <v>26154764800</v>
       </c>
       <c r="F7" t="n">
-        <v>1975122872</v>
+        <v>1518882011</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.05115</v>
+        <v>0.05348</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1632.61</v>
+        <v>1625.38</v>
       </c>
       <c r="E8" t="n">
-        <v>13951987479</v>
+        <v>13977019653</v>
       </c>
       <c r="F8" t="n">
-        <v>6404663</v>
+        <v>4757010</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.02969</v>
+        <v>-0.54683</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.254568</v>
+        <v>0.250578</v>
       </c>
       <c r="E9" t="n">
-        <v>8925549096</v>
+        <v>8771955317</v>
       </c>
       <c r="F9" t="n">
-        <v>108085140</v>
+        <v>95055376</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.2249</v>
+        <v>-1.63708</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.063301</v>
+        <v>0.061855</v>
       </c>
       <c r="E10" t="n">
-        <v>8918233250</v>
+        <v>8711510172</v>
       </c>
       <c r="F10" t="n">
-        <v>222858490</v>
+        <v>210802392</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.09375</v>
+        <v>-2.79266</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>19.4</v>
+        <v>18.39</v>
       </c>
       <c r="E11" t="n">
-        <v>7939475440</v>
+        <v>7548025975</v>
       </c>
       <c r="F11" t="n">
-        <v>195136171</v>
+        <v>363090373</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.84099</v>
+        <v>-5.91508</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.076975</v>
+        <v>0.078515</v>
       </c>
       <c r="E12" t="n">
-        <v>6877035415</v>
+        <v>7005447037</v>
       </c>
       <c r="F12" t="n">
-        <v>137841026</v>
+        <v>127459856</v>
       </c>
       <c r="G12" t="n">
-        <v>0.45218</v>
+        <v>-0.50712</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1.87</v>
+        <v>1.75</v>
       </c>
       <c r="E13" t="n">
-        <v>6427508543</v>
+        <v>6016950131</v>
       </c>
       <c r="F13" t="n">
-        <v>28787534</v>
+        <v>13201608</v>
       </c>
       <c r="G13" t="n">
-        <v>-2.41439</v>
+        <v>-2.45465</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>4.27</v>
+        <v>4.16</v>
       </c>
       <c r="E14" t="n">
-        <v>5430187963</v>
+        <v>5287464634</v>
       </c>
       <c r="F14" t="n">
-        <v>68667287</v>
+        <v>73693347</v>
       </c>
       <c r="G14" t="n">
-        <v>0.81496</v>
+        <v>-2.59101</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.543806</v>
+        <v>0.5289970000000001</v>
       </c>
       <c r="E15" t="n">
-        <v>5071450465</v>
+        <v>4927451356</v>
       </c>
       <c r="F15" t="n">
-        <v>132458424</v>
+        <v>128831131</v>
       </c>
       <c r="G15" t="n">
-        <v>0.08871</v>
+        <v>-2.4883</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>64.06999999999999</v>
+        <v>61.38</v>
       </c>
       <c r="E16" t="n">
-        <v>4717511503</v>
+        <v>4514830144</v>
       </c>
       <c r="F16" t="n">
-        <v>258219481</v>
+        <v>260349702</v>
       </c>
       <c r="G16" t="n">
-        <v>0.15161</v>
+        <v>-2.18587</v>
       </c>
     </row>
     <row r="17">
@@ -890,16 +890,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>7.8e-06</v>
+        <v>7.41e-06</v>
       </c>
       <c r="E17" t="n">
-        <v>4603976979</v>
+        <v>4363166347</v>
       </c>
       <c r="F17" t="n">
-        <v>66639681</v>
+        <v>65169882</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.72229</v>
+        <v>-2.71464</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>25927</v>
+        <v>25827</v>
       </c>
       <c r="E18" t="n">
-        <v>4224992976</v>
+        <v>4203782118</v>
       </c>
       <c r="F18" t="n">
-        <v>25511543</v>
+        <v>17790539</v>
       </c>
       <c r="G18" t="n">
-        <v>0.34156</v>
+        <v>-0.27365</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.999483</v>
+        <v>1</v>
       </c>
       <c r="E19" t="n">
-        <v>3874000837</v>
+        <v>3834891838</v>
       </c>
       <c r="F19" t="n">
-        <v>46237840</v>
+        <v>40445432</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.16045</v>
+        <v>0.07126</v>
       </c>
     </row>
     <row r="20">
@@ -971,16 +971,16 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>195.13</v>
+        <v>189.27</v>
       </c>
       <c r="E20" t="n">
-        <v>3806659582</v>
+        <v>3684649922</v>
       </c>
       <c r="F20" t="n">
-        <v>119764334</v>
+        <v>114084241</v>
       </c>
       <c r="G20" t="n">
-        <v>-2.42734</v>
+        <v>-1.2484</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>3.9</v>
+        <v>0.13151</v>
       </c>
       <c r="E21" t="n">
-        <v>3629732023</v>
+        <v>3600439224</v>
       </c>
       <c r="F21" t="n">
-        <v>138620</v>
+        <v>116742276</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.01904</v>
+        <v>-0.24153</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>9.92</v>
+        <v>3.85</v>
       </c>
       <c r="E22" t="n">
-        <v>3512172570</v>
+        <v>3582222481</v>
       </c>
       <c r="F22" t="n">
-        <v>95226789</v>
+        <v>133997</v>
       </c>
       <c r="G22" t="n">
-        <v>0.7204199999999999</v>
+        <v>2.00064</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.998293</v>
+        <v>9.56</v>
       </c>
       <c r="E23" t="n">
-        <v>3443012753</v>
+        <v>3367882831</v>
       </c>
       <c r="F23" t="n">
-        <v>878740664</v>
+        <v>100070315</v>
       </c>
       <c r="G23" t="n">
-        <v>0.00778</v>
+        <v>-3.34149</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>4.44</v>
+        <v>6.09</v>
       </c>
       <c r="E24" t="n">
-        <v>3348371247</v>
+        <v>3277434808</v>
       </c>
       <c r="F24" t="n">
-        <v>61143801</v>
+        <v>124532301</v>
       </c>
       <c r="G24" t="n">
-        <v>1.8923</v>
+        <v>-1.9651</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>TUSD</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>6.03</v>
+        <v>0.998596</v>
       </c>
       <c r="E25" t="n">
-        <v>3246988179</v>
+        <v>3182576832</v>
       </c>
       <c r="F25" t="n">
-        <v>176635621</v>
+        <v>129415266</v>
       </c>
       <c r="G25" t="n">
-        <v>1.48924</v>
+        <v>0.03605</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.114821</v>
+        <v>4.22</v>
       </c>
       <c r="E26" t="n">
-        <v>3155281863</v>
+        <v>3178704633</v>
       </c>
       <c r="F26" t="n">
-        <v>59611121</v>
+        <v>71035227</v>
       </c>
       <c r="G26" t="n">
-        <v>1.98807</v>
+        <v>-2.52796</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>1.001</v>
       </c>
       <c r="E27" t="n">
-        <v>2857631613</v>
+        <v>2590861430</v>
       </c>
       <c r="F27" t="n">
-        <v>1401855790</v>
+        <v>1171585271</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.01037</v>
+        <v>0.07191</v>
       </c>
     </row>
     <row r="28">
@@ -1187,16 +1187,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>140.69</v>
+        <v>142.48</v>
       </c>
       <c r="E28" t="n">
-        <v>2555100174</v>
+        <v>2584957418</v>
       </c>
       <c r="F28" t="n">
-        <v>46399656</v>
+        <v>32696345</v>
       </c>
       <c r="G28" t="n">
-        <v>0.13799</v>
+        <v>-0.58231</v>
       </c>
     </row>
     <row r="29">
@@ -1214,16 +1214,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>42.04</v>
+        <v>41.85</v>
       </c>
       <c r="E29" t="n">
-        <v>2524796778</v>
+        <v>2508596267</v>
       </c>
       <c r="F29" t="n">
-        <v>5375862</v>
+        <v>1974297</v>
       </c>
       <c r="G29" t="n">
-        <v>-1.60429</v>
+        <v>-0.82369</v>
       </c>
     </row>
     <row r="30">
@@ -1241,16 +1241,16 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>15.46</v>
+        <v>15.12</v>
       </c>
       <c r="E30" t="n">
-        <v>2208522245</v>
+        <v>2160942273</v>
       </c>
       <c r="F30" t="n">
-        <v>41431556</v>
+        <v>45265153</v>
       </c>
       <c r="G30" t="n">
-        <v>0.31018</v>
+        <v>-1.8132</v>
       </c>
     </row>
     <row r="31">
@@ -1268,16 +1268,16 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>6.85</v>
+        <v>6.76</v>
       </c>
       <c r="E31" t="n">
-        <v>2004316497</v>
+        <v>1974384776</v>
       </c>
       <c r="F31" t="n">
-        <v>78929214</v>
+        <v>85204957</v>
       </c>
       <c r="G31" t="n">
-        <v>2.01979</v>
+        <v>-1.91456</v>
       </c>
     </row>
     <row r="32">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.04984048</v>
+        <v>0.04797207</v>
       </c>
       <c r="E32" t="n">
-        <v>1656547219</v>
+        <v>1592166311</v>
       </c>
       <c r="F32" t="n">
-        <v>52399637</v>
+        <v>20368711</v>
       </c>
       <c r="G32" t="n">
-        <v>1.29392</v>
+        <v>-3.24234</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.452298</v>
+        <v>98.04000000000001</v>
       </c>
       <c r="E33" t="n">
-        <v>1462493425</v>
+        <v>1424904498</v>
       </c>
       <c r="F33" t="n">
-        <v>7834196</v>
+        <v>11371847</v>
       </c>
       <c r="G33" t="n">
-        <v>-0.02991</v>
+        <v>-1.10383</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>100.01</v>
+        <v>3.14</v>
       </c>
       <c r="E34" t="n">
-        <v>1454863824</v>
+        <v>1402654454</v>
       </c>
       <c r="F34" t="n">
-        <v>9057600</v>
+        <v>70471845</v>
       </c>
       <c r="G34" t="n">
-        <v>0.37744</v>
+        <v>-2.92886</v>
       </c>
     </row>
     <row r="35">
@@ -1376,16 +1376,16 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>3.24</v>
+        <v>3.13</v>
       </c>
       <c r="E35" t="n">
-        <v>1435096866</v>
+        <v>1387615616</v>
       </c>
       <c r="F35" t="n">
-        <v>11741138</v>
+        <v>16985546</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.71478</v>
+        <v>-4.33338</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>3.18</v>
+        <v>0.052346</v>
       </c>
       <c r="E36" t="n">
-        <v>1416937040</v>
+        <v>1373858278</v>
       </c>
       <c r="F36" t="n">
-        <v>65446688</v>
+        <v>5901636</v>
       </c>
       <c r="G36" t="n">
-        <v>0.107</v>
+        <v>-0.76576</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1.54</v>
+        <v>0.411831</v>
       </c>
       <c r="E37" t="n">
-        <v>1366131615</v>
+        <v>1332171118</v>
       </c>
       <c r="F37" t="n">
-        <v>33125198</v>
+        <v>8308340</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.18547</v>
+        <v>-0.46895</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.05039</v>
+        <v>1.49</v>
       </c>
       <c r="E38" t="n">
-        <v>1324134397</v>
+        <v>1320996090</v>
       </c>
       <c r="F38" t="n">
-        <v>4280772</v>
+        <v>20344793</v>
       </c>
       <c r="G38" t="n">
-        <v>0.28518</v>
+        <v>-2.49411</v>
       </c>
     </row>
     <row r="39">
@@ -1484,16 +1484,16 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>5.55</v>
+        <v>5.26</v>
       </c>
       <c r="E39" t="n">
-        <v>1270569880</v>
+        <v>1207945936</v>
       </c>
       <c r="F39" t="n">
-        <v>47496346</v>
+        <v>47304259</v>
       </c>
       <c r="G39" t="n">
-        <v>-0.44056</v>
+        <v>-4.05173</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.893548</v>
+        <v>0.01539834</v>
       </c>
       <c r="E40" t="n">
-        <v>1140722630</v>
+        <v>1119107073</v>
       </c>
       <c r="F40" t="n">
-        <v>72456501</v>
+        <v>23096777</v>
       </c>
       <c r="G40" t="n">
-        <v>0.60575</v>
+        <v>-1.19616</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.01546759</v>
+        <v>0.858495</v>
       </c>
       <c r="E41" t="n">
-        <v>1126488234</v>
+        <v>1094266274</v>
       </c>
       <c r="F41" t="n">
-        <v>29302542</v>
+        <v>87288365</v>
       </c>
       <c r="G41" t="n">
-        <v>-0.38207</v>
+        <v>-4.66631</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1.34</v>
+        <v>1.15</v>
       </c>
       <c r="E42" t="n">
-        <v>1067077806</v>
+        <v>1084854956</v>
       </c>
       <c r="F42" t="n">
-        <v>64205586</v>
+        <v>52143362</v>
       </c>
       <c r="G42" t="n">
-        <v>0.38549</v>
+        <v>-0.5269</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1.13</v>
+        <v>1130.13</v>
       </c>
       <c r="E43" t="n">
-        <v>1064718009</v>
+        <v>1017781504</v>
       </c>
       <c r="F43" t="n">
-        <v>38574968</v>
+        <v>39836692</v>
       </c>
       <c r="G43" t="n">
-        <v>0.21191</v>
+        <v>0.42214</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1129.01</v>
+        <v>1.27</v>
       </c>
       <c r="E44" t="n">
-        <v>1017292323</v>
+        <v>1010841617</v>
       </c>
       <c r="F44" t="n">
-        <v>66882826</v>
+        <v>50161313</v>
       </c>
       <c r="G44" t="n">
-        <v>-2.01109</v>
+        <v>-2.05708</v>
       </c>
     </row>
     <row r="45">
@@ -1646,16 +1646,16 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>1769.6</v>
+        <v>1762.65</v>
       </c>
       <c r="E45" t="n">
-        <v>926134410</v>
+        <v>925453190</v>
       </c>
       <c r="F45" t="n">
-        <v>3521798</v>
+        <v>3994106</v>
       </c>
       <c r="G45" t="n">
-        <v>-0.11296</v>
+        <v>-0.47508</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>XDC</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>XDC Network</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.058294</v>
+        <v>0.03944771</v>
       </c>
       <c r="E46" t="n">
-        <v>808335912</v>
+        <v>810610232</v>
       </c>
       <c r="F46" t="n">
-        <v>11862776</v>
+        <v>6394252</v>
       </c>
       <c r="G46" t="n">
-        <v>0.25537</v>
+        <v>2.30071</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>FRAX</t>
+          <t>AAVE</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Frax</t>
+          <t>Aave</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.997702</v>
+        <v>54.89</v>
       </c>
       <c r="E47" t="n">
-        <v>805006687</v>
+        <v>797125957</v>
       </c>
       <c r="F47" t="n">
-        <v>4835283</v>
+        <v>42325523</v>
       </c>
       <c r="G47" t="n">
-        <v>-0.08524</v>
+        <v>-2.50719</v>
       </c>
     </row>
     <row r="48">
@@ -1727,16 +1727,16 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.087434</v>
+        <v>0.084642</v>
       </c>
       <c r="E48" t="n">
-        <v>803609370</v>
+        <v>776118330</v>
       </c>
       <c r="F48" t="n">
-        <v>26240002</v>
+        <v>16744748</v>
       </c>
       <c r="G48" t="n">
-        <v>1.89629</v>
+        <v>-2.7648</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>AAVE</t>
+          <t>WBT</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Aave</t>
+          <t>WhiteBIT Coin</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>54.61</v>
+        <v>5.29</v>
       </c>
       <c r="E49" t="n">
-        <v>794272734</v>
+        <v>761992873</v>
       </c>
       <c r="F49" t="n">
-        <v>61599885</v>
+        <v>7216652</v>
       </c>
       <c r="G49" t="n">
-        <v>0.14874</v>
+        <v>-0.09889000000000001</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>WBT</t>
+          <t>XDC</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>WhiteBIT Coin</t>
+          <t>XDC Network</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>5.34</v>
+        <v>0.054645</v>
       </c>
       <c r="E50" t="n">
-        <v>770440438</v>
+        <v>757674777</v>
       </c>
       <c r="F50" t="n">
-        <v>6008766</v>
+        <v>5277795</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.10526</v>
+        <v>-2.84529</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ALGO</t>
+          <t>USDD</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Algorand</t>
+          <t>USDD</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.094304</v>
+        <v>0.997434</v>
       </c>
       <c r="E51" t="n">
-        <v>739219103</v>
+        <v>723197562</v>
       </c>
       <c r="F51" t="n">
-        <v>14335328</v>
+        <v>17825348</v>
       </c>
       <c r="G51" t="n">
-        <v>1.71761</v>
+        <v>0.0483</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-09-17
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>25810</v>
+        <v>26584</v>
       </c>
       <c r="E2" t="n">
-        <v>502572400738</v>
+        <v>518165158028</v>
       </c>
       <c r="F2" t="n">
-        <v>4541272403</v>
+        <v>5839501584</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.16589</v>
+        <v>0.28158</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1625.83</v>
+        <v>1631.21</v>
       </c>
       <c r="E3" t="n">
-        <v>195386934022</v>
+        <v>196052662000</v>
       </c>
       <c r="F3" t="n">
-        <v>3420405220</v>
+        <v>3906952610</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.5466800000000001</v>
+        <v>-0.21511</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999846</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>83002670998</v>
+        <v>83065234589</v>
       </c>
       <c r="F4" t="n">
-        <v>10100280055</v>
+        <v>10276939792</v>
       </c>
       <c r="G4" t="n">
-        <v>0.00924</v>
+        <v>0.00714</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>213.03</v>
+        <v>214.91</v>
       </c>
       <c r="E5" t="n">
-        <v>32749186633</v>
+        <v>33041536843</v>
       </c>
       <c r="F5" t="n">
-        <v>234969881</v>
+        <v>316341184</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.96637</v>
+        <v>0.3917</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.499586</v>
+        <v>0.49768</v>
       </c>
       <c r="E6" t="n">
-        <v>26516032516</v>
+        <v>26465863331</v>
       </c>
       <c r="F6" t="n">
-        <v>343609476</v>
+        <v>372474800</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.69555</v>
+        <v>-0.6498</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0.9999130000000001</v>
       </c>
       <c r="E7" t="n">
-        <v>26154764800</v>
+        <v>26160397739</v>
       </c>
       <c r="F7" t="n">
-        <v>1518882011</v>
+        <v>2066493106</v>
       </c>
       <c r="G7" t="n">
-        <v>0.05348</v>
+        <v>0.00254</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1625.38</v>
+        <v>1631.47</v>
       </c>
       <c r="E8" t="n">
-        <v>13977019653</v>
+        <v>14106344663</v>
       </c>
       <c r="F8" t="n">
-        <v>4757010</v>
+        <v>5269809</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.54683</v>
+        <v>-0.2427</v>
       </c>
     </row>
     <row r="9">
@@ -665,25 +665,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ADA</t>
+          <t>DOGE</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Cardano</t>
+          <t>Dogecoin</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.250578</v>
+        <v>0.062321</v>
       </c>
       <c r="E9" t="n">
-        <v>8771955317</v>
+        <v>8789177308</v>
       </c>
       <c r="F9" t="n">
-        <v>95055376</v>
+        <v>167179588</v>
       </c>
       <c r="G9" t="n">
-        <v>-1.63708</v>
+        <v>-0.05315</v>
       </c>
     </row>
     <row r="10">
@@ -692,25 +692,25 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>DOGE</t>
+          <t>ADA</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Dogecoin</t>
+          <t>Cardano</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.061855</v>
+        <v>0.250248</v>
       </c>
       <c r="E10" t="n">
-        <v>8711510172</v>
+        <v>8767878478</v>
       </c>
       <c r="F10" t="n">
-        <v>210802392</v>
+        <v>73026140</v>
       </c>
       <c r="G10" t="n">
-        <v>-2.79266</v>
+        <v>-0.30638</v>
       </c>
     </row>
     <row r="11">
@@ -719,25 +719,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SOL</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Solana</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>18.39</v>
+        <v>2.43</v>
       </c>
       <c r="E11" t="n">
-        <v>7548025975</v>
+        <v>8375803632</v>
       </c>
       <c r="F11" t="n">
-        <v>363090373</v>
+        <v>68178591</v>
       </c>
       <c r="G11" t="n">
-        <v>-5.91508</v>
+        <v>7.9063</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +746,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>SOL</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Solana</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.078515</v>
+        <v>19.06</v>
       </c>
       <c r="E12" t="n">
-        <v>7005447037</v>
+        <v>7838277357</v>
       </c>
       <c r="F12" t="n">
-        <v>127459856</v>
+        <v>122627495</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.50712</v>
+        <v>-0.50687</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1.75</v>
+        <v>0.083727</v>
       </c>
       <c r="E13" t="n">
-        <v>6016950131</v>
+        <v>7462129731</v>
       </c>
       <c r="F13" t="n">
-        <v>13201608</v>
+        <v>176537629</v>
       </c>
       <c r="G13" t="n">
-        <v>-2.45465</v>
+        <v>0.1771</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>4.16</v>
+        <v>4.12</v>
       </c>
       <c r="E14" t="n">
-        <v>5287464634</v>
+        <v>5257682319</v>
       </c>
       <c r="F14" t="n">
-        <v>73693347</v>
+        <v>67246162</v>
       </c>
       <c r="G14" t="n">
-        <v>-2.59101</v>
+        <v>-1.02201</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.5289970000000001</v>
+        <v>0.524705</v>
       </c>
       <c r="E15" t="n">
-        <v>4927451356</v>
+        <v>4889796203</v>
       </c>
       <c r="F15" t="n">
-        <v>128831131</v>
+        <v>111531762</v>
       </c>
       <c r="G15" t="n">
-        <v>-2.4883</v>
+        <v>-0.45731</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>61.38</v>
+        <v>64.19</v>
       </c>
       <c r="E16" t="n">
-        <v>4514830144</v>
+        <v>4727271061</v>
       </c>
       <c r="F16" t="n">
-        <v>260349702</v>
+        <v>279974983</v>
       </c>
       <c r="G16" t="n">
-        <v>-2.18587</v>
+        <v>-1.14495</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>7.41e-06</v>
+        <v>26607</v>
       </c>
       <c r="E17" t="n">
-        <v>4363166347</v>
+        <v>4331716641</v>
       </c>
       <c r="F17" t="n">
-        <v>65169882</v>
+        <v>22514198</v>
       </c>
       <c r="G17" t="n">
-        <v>-2.71464</v>
+        <v>0.29601</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>25827</v>
+        <v>7.3e-06</v>
       </c>
       <c r="E18" t="n">
-        <v>4203782118</v>
+        <v>4304061575</v>
       </c>
       <c r="F18" t="n">
-        <v>17790539</v>
+        <v>59269706</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.27365</v>
+        <v>-1.634</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>212.73</v>
       </c>
       <c r="E19" t="n">
-        <v>3834891838</v>
+        <v>4151114857</v>
       </c>
       <c r="F19" t="n">
-        <v>40445432</v>
+        <v>125780347</v>
       </c>
       <c r="G19" t="n">
-        <v>0.07126</v>
+        <v>-1.19077</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>189.27</v>
+        <v>0.999627</v>
       </c>
       <c r="E20" t="n">
-        <v>3684649922</v>
+        <v>3842286310</v>
       </c>
       <c r="F20" t="n">
-        <v>114084241</v>
+        <v>40100406</v>
       </c>
       <c r="G20" t="n">
-        <v>-1.2484</v>
+        <v>0.09317</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.13151</v>
+        <v>3.69</v>
       </c>
       <c r="E21" t="n">
-        <v>3600439224</v>
+        <v>3437538747</v>
       </c>
       <c r="F21" t="n">
-        <v>116742276</v>
+        <v>227597</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.24153</v>
+        <v>1.2463</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>3.85</v>
+        <v>6.21</v>
       </c>
       <c r="E22" t="n">
-        <v>3582222481</v>
+        <v>3342759802</v>
       </c>
       <c r="F22" t="n">
-        <v>133997</v>
+        <v>102251195</v>
       </c>
       <c r="G22" t="n">
-        <v>2.00064</v>
+        <v>-0.40433</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>9.56</v>
+        <v>4.36</v>
       </c>
       <c r="E23" t="n">
-        <v>3367882831</v>
+        <v>3283186735</v>
       </c>
       <c r="F23" t="n">
-        <v>100070315</v>
+        <v>66321209</v>
       </c>
       <c r="G23" t="n">
-        <v>-3.34149</v>
+        <v>0.79449</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>6.09</v>
+        <v>9.27</v>
       </c>
       <c r="E24" t="n">
-        <v>3277434808</v>
+        <v>3280165452</v>
       </c>
       <c r="F24" t="n">
-        <v>124532301</v>
+        <v>78287052</v>
       </c>
       <c r="G24" t="n">
-        <v>-1.9651</v>
+        <v>-2.0715</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.998596</v>
+        <v>0.117484</v>
       </c>
       <c r="E25" t="n">
-        <v>3182576832</v>
+        <v>3237432412</v>
       </c>
       <c r="F25" t="n">
-        <v>129415266</v>
+        <v>43956628</v>
       </c>
       <c r="G25" t="n">
-        <v>0.03605</v>
+        <v>-1.34729</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>TUSD</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>4.22</v>
+        <v>0.999344</v>
       </c>
       <c r="E26" t="n">
-        <v>3178704633</v>
+        <v>3101719109</v>
       </c>
       <c r="F26" t="n">
-        <v>71035227</v>
+        <v>136856015</v>
       </c>
       <c r="G26" t="n">
-        <v>-2.52796</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Binance USD</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>1.001</v>
+        <v>145.22</v>
       </c>
       <c r="E27" t="n">
-        <v>2590861430</v>
+        <v>2636840774</v>
       </c>
       <c r="F27" t="n">
-        <v>1171585271</v>
+        <v>32891264</v>
       </c>
       <c r="G27" t="n">
-        <v>0.07191</v>
+        <v>-0.16323</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>142.48</v>
+        <v>43.45</v>
       </c>
       <c r="E28" t="n">
-        <v>2584957418</v>
+        <v>2606526110</v>
       </c>
       <c r="F28" t="n">
-        <v>32696345</v>
+        <v>6564723</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.58231</v>
+        <v>1.55008</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Binance USD</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>41.85</v>
+        <v>1</v>
       </c>
       <c r="E29" t="n">
-        <v>2508596267</v>
+        <v>2492512278</v>
       </c>
       <c r="F29" t="n">
-        <v>1974297</v>
+        <v>1348891962</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.82369</v>
+        <v>0.0431</v>
       </c>
     </row>
     <row r="30">
@@ -1241,16 +1241,16 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>15.12</v>
+        <v>15.52</v>
       </c>
       <c r="E30" t="n">
-        <v>2160942273</v>
+        <v>2219503426</v>
       </c>
       <c r="F30" t="n">
-        <v>45265153</v>
+        <v>37420130</v>
       </c>
       <c r="G30" t="n">
-        <v>-1.8132</v>
+        <v>-0.62252</v>
       </c>
     </row>
     <row r="31">
@@ -1268,16 +1268,16 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>6.76</v>
+        <v>7.13</v>
       </c>
       <c r="E31" t="n">
-        <v>1974384776</v>
+        <v>2084088817</v>
       </c>
       <c r="F31" t="n">
-        <v>85204957</v>
+        <v>87593162</v>
       </c>
       <c r="G31" t="n">
-        <v>-1.91456</v>
+        <v>0.01459</v>
       </c>
     </row>
     <row r="32">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.04797207</v>
+        <v>0.050395</v>
       </c>
       <c r="E32" t="n">
-        <v>1592166311</v>
+        <v>1673977779</v>
       </c>
       <c r="F32" t="n">
-        <v>20368711</v>
+        <v>17388285</v>
       </c>
       <c r="G32" t="n">
-        <v>-3.24234</v>
+        <v>-2.03297</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>98.04000000000001</v>
+        <v>3.33</v>
       </c>
       <c r="E33" t="n">
-        <v>1424904498</v>
+        <v>1495739765</v>
       </c>
       <c r="F33" t="n">
-        <v>11371847</v>
+        <v>64115371</v>
       </c>
       <c r="G33" t="n">
-        <v>-1.10383</v>
+        <v>-1.16372</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>3.14</v>
+        <v>0.051696</v>
       </c>
       <c r="E34" t="n">
-        <v>1402654454</v>
+        <v>1358552943</v>
       </c>
       <c r="F34" t="n">
-        <v>70471845</v>
+        <v>9605855</v>
       </c>
       <c r="G34" t="n">
-        <v>-2.92886</v>
+        <v>0.9466599999999999</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>3.13</v>
+        <v>1.52</v>
       </c>
       <c r="E35" t="n">
-        <v>1387615616</v>
+        <v>1353083285</v>
       </c>
       <c r="F35" t="n">
-        <v>16985546</v>
+        <v>21451619</v>
       </c>
       <c r="G35" t="n">
-        <v>-4.33338</v>
+        <v>-0.56306</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.052346</v>
+        <v>2.99</v>
       </c>
       <c r="E36" t="n">
-        <v>1373858278</v>
+        <v>1329876596</v>
       </c>
       <c r="F36" t="n">
-        <v>5901636</v>
+        <v>14847374</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.76576</v>
+        <v>-1.45445</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.411831</v>
+        <v>91.36</v>
       </c>
       <c r="E37" t="n">
-        <v>1332171118</v>
+        <v>1328352347</v>
       </c>
       <c r="F37" t="n">
-        <v>8308340</v>
+        <v>16181164</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.46895</v>
+        <v>0.16614</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1.49</v>
+        <v>0.404231</v>
       </c>
       <c r="E38" t="n">
-        <v>1320996090</v>
+        <v>1307214768</v>
       </c>
       <c r="F38" t="n">
-        <v>20344793</v>
+        <v>14721043</v>
       </c>
       <c r="G38" t="n">
-        <v>-2.49411</v>
+        <v>-0.09135</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>5.26</v>
+        <v>0.01765241</v>
       </c>
       <c r="E39" t="n">
-        <v>1207945936</v>
+        <v>1279049631</v>
       </c>
       <c r="F39" t="n">
-        <v>47304259</v>
+        <v>39276705</v>
       </c>
       <c r="G39" t="n">
-        <v>-4.05173</v>
+        <v>-1.29015</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.01539834</v>
+        <v>5.3</v>
       </c>
       <c r="E40" t="n">
-        <v>1119107073</v>
+        <v>1247192374</v>
       </c>
       <c r="F40" t="n">
-        <v>23096777</v>
+        <v>41858751</v>
       </c>
       <c r="G40" t="n">
-        <v>-1.19616</v>
+        <v>-0.6208900000000001</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.858495</v>
+        <v>1275.77</v>
       </c>
       <c r="E41" t="n">
-        <v>1094266274</v>
+        <v>1149935656</v>
       </c>
       <c r="F41" t="n">
-        <v>87288365</v>
+        <v>62288340</v>
       </c>
       <c r="G41" t="n">
-        <v>-4.66631</v>
+        <v>0.77069</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1.15</v>
+        <v>1.38</v>
       </c>
       <c r="E42" t="n">
-        <v>1084854956</v>
+        <v>1097406751</v>
       </c>
       <c r="F42" t="n">
-        <v>52143362</v>
+        <v>41073477</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.5269</v>
+        <v>-1.74013</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1130.13</v>
+        <v>1.12</v>
       </c>
       <c r="E43" t="n">
-        <v>1017781504</v>
+        <v>1050057796</v>
       </c>
       <c r="F43" t="n">
-        <v>39836692</v>
+        <v>28951221</v>
       </c>
       <c r="G43" t="n">
-        <v>0.42214</v>
+        <v>-0.92431</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1.27</v>
+        <v>0.814459</v>
       </c>
       <c r="E44" t="n">
-        <v>1010841617</v>
+        <v>1038670651</v>
       </c>
       <c r="F44" t="n">
-        <v>50161313</v>
+        <v>80208761</v>
       </c>
       <c r="G44" t="n">
-        <v>-2.05708</v>
+        <v>-1.29652</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>RETH</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Rocket Pool ETH</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>1762.65</v>
+        <v>0.04594901</v>
       </c>
       <c r="E45" t="n">
-        <v>925453190</v>
+        <v>950618857</v>
       </c>
       <c r="F45" t="n">
-        <v>3994106</v>
+        <v>12786607</v>
       </c>
       <c r="G45" t="n">
-        <v>-0.47508</v>
+        <v>-7.86616</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>RETH</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Rocket Pool ETH</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.03944771</v>
+        <v>1770.79</v>
       </c>
       <c r="E46" t="n">
-        <v>810610232</v>
+        <v>932330934</v>
       </c>
       <c r="F46" t="n">
-        <v>6394252</v>
+        <v>2911711</v>
       </c>
       <c r="G46" t="n">
-        <v>2.30071</v>
+        <v>-0.24243</v>
       </c>
     </row>
     <row r="47">
@@ -1700,16 +1700,16 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>54.89</v>
+        <v>61.02</v>
       </c>
       <c r="E47" t="n">
-        <v>797125957</v>
+        <v>885940889</v>
       </c>
       <c r="F47" t="n">
-        <v>42325523</v>
+        <v>98662769</v>
       </c>
       <c r="G47" t="n">
-        <v>-2.50719</v>
+        <v>3.12624</v>
       </c>
     </row>
     <row r="48">
@@ -1727,16 +1727,16 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.084642</v>
+        <v>0.086552</v>
       </c>
       <c r="E48" t="n">
-        <v>776118330</v>
+        <v>794266152</v>
       </c>
       <c r="F48" t="n">
-        <v>16744748</v>
+        <v>18397855</v>
       </c>
       <c r="G48" t="n">
-        <v>-2.7648</v>
+        <v>0.20492</v>
       </c>
     </row>
     <row r="49">
@@ -1754,16 +1754,16 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>5.29</v>
+        <v>5.28</v>
       </c>
       <c r="E49" t="n">
-        <v>761992873</v>
+        <v>760123446</v>
       </c>
       <c r="F49" t="n">
-        <v>7216652</v>
+        <v>6746252</v>
       </c>
       <c r="G49" t="n">
-        <v>-0.09889000000000001</v>
+        <v>-0.98405</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>XDC</t>
+          <t>ALGO</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>XDC Network</t>
+          <t>Algorand</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.054645</v>
+        <v>0.096162</v>
       </c>
       <c r="E50" t="n">
-        <v>757674777</v>
+        <v>752848302</v>
       </c>
       <c r="F50" t="n">
-        <v>5277795</v>
+        <v>15907026</v>
       </c>
       <c r="G50" t="n">
-        <v>-2.84529</v>
+        <v>-0.29322</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>USDD</t>
+          <t>XDC</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>USDD</t>
+          <t>XDC Network</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.997434</v>
+        <v>0.053273</v>
       </c>
       <c r="E51" t="n">
-        <v>723197562</v>
+        <v>738987447</v>
       </c>
       <c r="F51" t="n">
-        <v>17825348</v>
+        <v>5486661</v>
       </c>
       <c r="G51" t="n">
-        <v>0.0483</v>
+        <v>-2.0207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-09-24
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>26584</v>
+        <v>26604</v>
       </c>
       <c r="E2" t="n">
-        <v>518165158028</v>
+        <v>518561249912</v>
       </c>
       <c r="F2" t="n">
-        <v>5839501584</v>
+        <v>5286209623</v>
       </c>
       <c r="G2" t="n">
-        <v>0.28158</v>
+        <v>0.12943</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1631.21</v>
+        <v>1593.69</v>
       </c>
       <c r="E3" t="n">
-        <v>196052662000</v>
+        <v>191627710580</v>
       </c>
       <c r="F3" t="n">
-        <v>3906952610</v>
+        <v>2651407000</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.21511</v>
+        <v>0.07874</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0.999966</v>
       </c>
       <c r="E4" t="n">
-        <v>83065234589</v>
+        <v>83203330822</v>
       </c>
       <c r="F4" t="n">
-        <v>10276939792</v>
+        <v>8061869039</v>
       </c>
       <c r="G4" t="n">
-        <v>0.00714</v>
+        <v>0.02274</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>214.91</v>
+        <v>210.8</v>
       </c>
       <c r="E5" t="n">
-        <v>33041536843</v>
+        <v>32437149245</v>
       </c>
       <c r="F5" t="n">
-        <v>316341184</v>
+        <v>173764446</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3917</v>
+        <v>0.03377</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.49768</v>
+        <v>0.510581</v>
       </c>
       <c r="E6" t="n">
-        <v>26465863331</v>
+        <v>27212561438</v>
       </c>
       <c r="F6" t="n">
-        <v>372474800</v>
+        <v>313455140</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.6498</v>
+        <v>-0.16132</v>
       </c>
     </row>
     <row r="7">
@@ -616,20 +616,20 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>USD Coin</t>
+          <t>USDC</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.9999130000000001</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>26160397739</v>
+        <v>25774759109</v>
       </c>
       <c r="F7" t="n">
-        <v>2066493106</v>
+        <v>1600202498</v>
       </c>
       <c r="G7" t="n">
-        <v>0.00254</v>
+        <v>0.02076</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1631.47</v>
+        <v>1594.35</v>
       </c>
       <c r="E8" t="n">
-        <v>14106344663</v>
+        <v>13911269449</v>
       </c>
       <c r="F8" t="n">
-        <v>5269809</v>
+        <v>7147333</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.2427</v>
+        <v>0.17159</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.062321</v>
+        <v>0.061518</v>
       </c>
       <c r="E9" t="n">
-        <v>8789177308</v>
+        <v>8685449215</v>
       </c>
       <c r="F9" t="n">
-        <v>167179588</v>
+        <v>109822523</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.05315</v>
+        <v>-0.13686</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.250248</v>
+        <v>0.245805</v>
       </c>
       <c r="E10" t="n">
-        <v>8767878478</v>
+        <v>8616299607</v>
       </c>
       <c r="F10" t="n">
-        <v>73026140</v>
+        <v>60362852</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.30638</v>
+        <v>-0.22022</v>
       </c>
     </row>
     <row r="11">
@@ -719,25 +719,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>SOL</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Solana</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2.43</v>
+        <v>19.62</v>
       </c>
       <c r="E11" t="n">
-        <v>8375803632</v>
+        <v>8106142524</v>
       </c>
       <c r="F11" t="n">
-        <v>68178591</v>
+        <v>111207653</v>
       </c>
       <c r="G11" t="n">
-        <v>7.9063</v>
+        <v>0.75925</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +746,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SOL</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Solana</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>19.06</v>
+        <v>2.23</v>
       </c>
       <c r="E12" t="n">
-        <v>7838277357</v>
+        <v>7703772619</v>
       </c>
       <c r="F12" t="n">
-        <v>122627495</v>
+        <v>12353611</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.50687</v>
+        <v>-4.14935</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.083727</v>
+        <v>0.08418100000000001</v>
       </c>
       <c r="E13" t="n">
-        <v>7462129731</v>
+        <v>7506255995</v>
       </c>
       <c r="F13" t="n">
-        <v>176537629</v>
+        <v>135022365</v>
       </c>
       <c r="G13" t="n">
-        <v>0.1771</v>
+        <v>0.77325</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>4.12</v>
+        <v>4.04</v>
       </c>
       <c r="E14" t="n">
-        <v>5257682319</v>
+        <v>5168460808</v>
       </c>
       <c r="F14" t="n">
-        <v>67246162</v>
+        <v>54035810</v>
       </c>
       <c r="G14" t="n">
-        <v>-1.02201</v>
+        <v>0.84137</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.524705</v>
+        <v>0.52183</v>
       </c>
       <c r="E15" t="n">
-        <v>4889796203</v>
+        <v>4862313303</v>
       </c>
       <c r="F15" t="n">
-        <v>111531762</v>
+        <v>73001878</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.45731</v>
+        <v>0.00797</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>64.19</v>
+        <v>64.66</v>
       </c>
       <c r="E16" t="n">
-        <v>4727271061</v>
+        <v>4766430982</v>
       </c>
       <c r="F16" t="n">
-        <v>279974983</v>
+        <v>184268355</v>
       </c>
       <c r="G16" t="n">
-        <v>-1.14495</v>
+        <v>-0.23203</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>26607</v>
+        <v>7.37e-06</v>
       </c>
       <c r="E17" t="n">
-        <v>4331716641</v>
+        <v>4339994115</v>
       </c>
       <c r="F17" t="n">
-        <v>22514198</v>
+        <v>151783928</v>
       </c>
       <c r="G17" t="n">
-        <v>0.29601</v>
+        <v>0.18089</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>7.3e-06</v>
+        <v>26567</v>
       </c>
       <c r="E18" t="n">
-        <v>4304061575</v>
+        <v>4326498996</v>
       </c>
       <c r="F18" t="n">
-        <v>59269706</v>
+        <v>18358826</v>
       </c>
       <c r="G18" t="n">
-        <v>-1.634</v>
+        <v>0.12348</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>212.73</v>
+        <v>208.64</v>
       </c>
       <c r="E19" t="n">
-        <v>4151114857</v>
+        <v>4073114887</v>
       </c>
       <c r="F19" t="n">
-        <v>125780347</v>
+        <v>71390949</v>
       </c>
       <c r="G19" t="n">
-        <v>-1.19077</v>
+        <v>0.30936</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.999627</v>
+        <v>7.1</v>
       </c>
       <c r="E20" t="n">
-        <v>3842286310</v>
+        <v>3951101258</v>
       </c>
       <c r="F20" t="n">
-        <v>40100406</v>
+        <v>259440126</v>
       </c>
       <c r="G20" t="n">
-        <v>0.09317</v>
+        <v>1.30578</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>3.69</v>
+        <v>1</v>
       </c>
       <c r="E21" t="n">
-        <v>3437538747</v>
+        <v>3843467995</v>
       </c>
       <c r="F21" t="n">
-        <v>227597</v>
+        <v>57549519</v>
       </c>
       <c r="G21" t="n">
-        <v>1.2463</v>
+        <v>0.09417</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>TUSD</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>6.21</v>
+        <v>0.99898</v>
       </c>
       <c r="E22" t="n">
-        <v>3342759802</v>
+        <v>3507279323</v>
       </c>
       <c r="F22" t="n">
-        <v>102251195</v>
+        <v>46760150</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.40433</v>
+        <v>0.01398</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>4.36</v>
+        <v>3.75</v>
       </c>
       <c r="E23" t="n">
-        <v>3283186735</v>
+        <v>3485171333</v>
       </c>
       <c r="F23" t="n">
-        <v>66321209</v>
+        <v>180450</v>
       </c>
       <c r="G23" t="n">
-        <v>0.79449</v>
+        <v>-2.26696</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>9.27</v>
+        <v>4.28</v>
       </c>
       <c r="E24" t="n">
-        <v>3280165452</v>
+        <v>3224902193</v>
       </c>
       <c r="F24" t="n">
-        <v>78287052</v>
+        <v>39446281</v>
       </c>
       <c r="G24" t="n">
-        <v>-2.0715</v>
+        <v>0.1842</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.117484</v>
+        <v>9.01</v>
       </c>
       <c r="E25" t="n">
-        <v>3237432412</v>
+        <v>3188662677</v>
       </c>
       <c r="F25" t="n">
-        <v>43956628</v>
+        <v>73583184</v>
       </c>
       <c r="G25" t="n">
-        <v>-1.34729</v>
+        <v>0.56853</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.999344</v>
+        <v>0.113434</v>
       </c>
       <c r="E26" t="n">
-        <v>3101719109</v>
+        <v>3142869270</v>
       </c>
       <c r="F26" t="n">
-        <v>136856015</v>
+        <v>29612413</v>
       </c>
       <c r="G26" t="n">
-        <v>0.08</v>
+        <v>-0.36688</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>145.22</v>
+        <v>142.94</v>
       </c>
       <c r="E27" t="n">
-        <v>2636840774</v>
+        <v>2593165477</v>
       </c>
       <c r="F27" t="n">
-        <v>32891264</v>
+        <v>37268065</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.16323</v>
+        <v>-0.70748</v>
       </c>
     </row>
     <row r="28">
@@ -1187,16 +1187,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>43.45</v>
+        <v>42.85</v>
       </c>
       <c r="E28" t="n">
-        <v>2606526110</v>
+        <v>2573393240</v>
       </c>
       <c r="F28" t="n">
-        <v>6564723</v>
+        <v>1437314</v>
       </c>
       <c r="G28" t="n">
-        <v>1.55008</v>
+        <v>0.28249</v>
       </c>
     </row>
     <row r="29">
@@ -1217,13 +1217,13 @@
         <v>1</v>
       </c>
       <c r="E29" t="n">
-        <v>2492512278</v>
+        <v>2381668298</v>
       </c>
       <c r="F29" t="n">
-        <v>1348891962</v>
+        <v>684960026</v>
       </c>
       <c r="G29" t="n">
-        <v>0.0431</v>
+        <v>0.00317</v>
       </c>
     </row>
     <row r="30">
@@ -1241,16 +1241,16 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>15.52</v>
+        <v>15.27</v>
       </c>
       <c r="E30" t="n">
-        <v>2219503426</v>
+        <v>2184472345</v>
       </c>
       <c r="F30" t="n">
-        <v>37420130</v>
+        <v>38858988</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.62252</v>
+        <v>0.47672</v>
       </c>
     </row>
     <row r="31">
@@ -1268,16 +1268,16 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>7.13</v>
+        <v>7.06</v>
       </c>
       <c r="E31" t="n">
-        <v>2084088817</v>
+        <v>2064306033</v>
       </c>
       <c r="F31" t="n">
-        <v>87593162</v>
+        <v>79706843</v>
       </c>
       <c r="G31" t="n">
-        <v>0.01459</v>
+        <v>-0.44987</v>
       </c>
     </row>
     <row r="32">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.050395</v>
+        <v>0.050437</v>
       </c>
       <c r="E32" t="n">
-        <v>1673977779</v>
+        <v>1685403380</v>
       </c>
       <c r="F32" t="n">
-        <v>17388285</v>
+        <v>15665416</v>
       </c>
       <c r="G32" t="n">
-        <v>-2.03297</v>
+        <v>-1.63668</v>
       </c>
     </row>
     <row r="33">
@@ -1322,16 +1322,16 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>3.33</v>
+        <v>3.25</v>
       </c>
       <c r="E33" t="n">
-        <v>1495739765</v>
+        <v>1468511796</v>
       </c>
       <c r="F33" t="n">
-        <v>64115371</v>
+        <v>46443126</v>
       </c>
       <c r="G33" t="n">
-        <v>-1.16372</v>
+        <v>0.78301</v>
       </c>
     </row>
     <row r="34">
@@ -1349,16 +1349,16 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.051696</v>
+        <v>0.051313</v>
       </c>
       <c r="E34" t="n">
-        <v>1358552943</v>
+        <v>1353733630</v>
       </c>
       <c r="F34" t="n">
-        <v>9605855</v>
+        <v>13112024</v>
       </c>
       <c r="G34" t="n">
-        <v>0.9466599999999999</v>
+        <v>1.58151</v>
       </c>
     </row>
     <row r="35">
@@ -1376,16 +1376,16 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1.52</v>
+        <v>1.49</v>
       </c>
       <c r="E35" t="n">
-        <v>1353083285</v>
+        <v>1323768554</v>
       </c>
       <c r="F35" t="n">
-        <v>21451619</v>
+        <v>9894668</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.56306</v>
+        <v>0.26614</v>
       </c>
     </row>
     <row r="36">
@@ -1403,16 +1403,16 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>2.99</v>
+        <v>2.96</v>
       </c>
       <c r="E36" t="n">
-        <v>1329876596</v>
+        <v>1315129194</v>
       </c>
       <c r="F36" t="n">
-        <v>14847374</v>
+        <v>9140714</v>
       </c>
       <c r="G36" t="n">
-        <v>-1.45445</v>
+        <v>0.35466</v>
       </c>
     </row>
     <row r="37">
@@ -1430,16 +1430,16 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>91.36</v>
+        <v>90.11</v>
       </c>
       <c r="E37" t="n">
-        <v>1328352347</v>
+        <v>1311742154</v>
       </c>
       <c r="F37" t="n">
-        <v>16181164</v>
+        <v>9116989</v>
       </c>
       <c r="G37" t="n">
-        <v>0.16614</v>
+        <v>-0.70339</v>
       </c>
     </row>
     <row r="38">
@@ -1457,16 +1457,16 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.404231</v>
+        <v>0.39705</v>
       </c>
       <c r="E38" t="n">
-        <v>1307214768</v>
+        <v>1284065364</v>
       </c>
       <c r="F38" t="n">
-        <v>14721043</v>
+        <v>11973910</v>
       </c>
       <c r="G38" t="n">
-        <v>-0.09135</v>
+        <v>1.43755</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.01765241</v>
+        <v>5.32</v>
       </c>
       <c r="E39" t="n">
-        <v>1279049631</v>
+        <v>1258831819</v>
       </c>
       <c r="F39" t="n">
-        <v>39276705</v>
+        <v>32581917</v>
       </c>
       <c r="G39" t="n">
-        <v>-1.29015</v>
+        <v>3.91372</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>5.3</v>
+        <v>0.01691804</v>
       </c>
       <c r="E40" t="n">
-        <v>1247192374</v>
+        <v>1230279023</v>
       </c>
       <c r="F40" t="n">
-        <v>41858751</v>
+        <v>22117596</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.6208900000000001</v>
+        <v>0.09121</v>
       </c>
     </row>
     <row r="41">
@@ -1538,16 +1538,16 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1275.77</v>
+        <v>1284.43</v>
       </c>
       <c r="E41" t="n">
-        <v>1149935656</v>
+        <v>1157407724</v>
       </c>
       <c r="F41" t="n">
-        <v>62288340</v>
+        <v>34979828</v>
       </c>
       <c r="G41" t="n">
-        <v>0.77069</v>
+        <v>0.49575</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1.38</v>
+        <v>0.829186</v>
       </c>
       <c r="E42" t="n">
-        <v>1097406751</v>
+        <v>1056989634</v>
       </c>
       <c r="F42" t="n">
-        <v>41073477</v>
+        <v>40649559</v>
       </c>
       <c r="G42" t="n">
-        <v>-1.74013</v>
+        <v>-0.04506</v>
       </c>
     </row>
     <row r="43">
@@ -1592,16 +1592,16 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1.12</v>
+        <v>1.11</v>
       </c>
       <c r="E43" t="n">
-        <v>1050057796</v>
+        <v>1046629964</v>
       </c>
       <c r="F43" t="n">
-        <v>28951221</v>
+        <v>24376532</v>
       </c>
       <c r="G43" t="n">
-        <v>-0.92431</v>
+        <v>0.02613</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.814459</v>
+        <v>1.29</v>
       </c>
       <c r="E44" t="n">
-        <v>1038670651</v>
+        <v>1033573587</v>
       </c>
       <c r="F44" t="n">
-        <v>80208761</v>
+        <v>32730120</v>
       </c>
       <c r="G44" t="n">
-        <v>-1.29652</v>
+        <v>0.29553</v>
       </c>
     </row>
     <row r="45">
@@ -1646,16 +1646,16 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.04594901</v>
+        <v>0.04600801</v>
       </c>
       <c r="E45" t="n">
-        <v>950618857</v>
+        <v>958455531</v>
       </c>
       <c r="F45" t="n">
-        <v>12786607</v>
+        <v>7400215</v>
       </c>
       <c r="G45" t="n">
-        <v>-7.86616</v>
+        <v>0.68474</v>
       </c>
     </row>
     <row r="46">
@@ -1673,16 +1673,16 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>1770.79</v>
+        <v>1734.01</v>
       </c>
       <c r="E46" t="n">
-        <v>932330934</v>
+        <v>917043628</v>
       </c>
       <c r="F46" t="n">
-        <v>2911711</v>
+        <v>3699007</v>
       </c>
       <c r="G46" t="n">
-        <v>-0.24243</v>
+        <v>0.21567</v>
       </c>
     </row>
     <row r="47">
@@ -1700,16 +1700,16 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>61.02</v>
+        <v>62.72</v>
       </c>
       <c r="E47" t="n">
-        <v>885940889</v>
+        <v>914090373</v>
       </c>
       <c r="F47" t="n">
-        <v>98662769</v>
+        <v>38349036</v>
       </c>
       <c r="G47" t="n">
-        <v>3.12624</v>
+        <v>-0.8118</v>
       </c>
     </row>
     <row r="48">
@@ -1727,16 +1727,16 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.086552</v>
+        <v>0.08741699999999999</v>
       </c>
       <c r="E48" t="n">
-        <v>794266152</v>
+        <v>807561413</v>
       </c>
       <c r="F48" t="n">
-        <v>18397855</v>
+        <v>14652153</v>
       </c>
       <c r="G48" t="n">
-        <v>0.20492</v>
+        <v>-1.38595</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>WBT</t>
+          <t>ALGO</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>WhiteBIT Coin</t>
+          <t>Algorand</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>5.28</v>
+        <v>0.101447</v>
       </c>
       <c r="E49" t="n">
-        <v>760123446</v>
+        <v>794019115</v>
       </c>
       <c r="F49" t="n">
-        <v>6746252</v>
+        <v>15826954</v>
       </c>
       <c r="G49" t="n">
-        <v>-0.98405</v>
+        <v>0.33846</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ALGO</t>
+          <t>WBT</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Algorand</t>
+          <t>WhiteBIT Coin</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.096162</v>
+        <v>5.31</v>
       </c>
       <c r="E50" t="n">
-        <v>752848302</v>
+        <v>764812777</v>
       </c>
       <c r="F50" t="n">
-        <v>15907026</v>
+        <v>7890381</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.29322</v>
+        <v>-0.14292</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>XDC</t>
+          <t>USDD</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>XDC Network</t>
+          <t>USDD</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.053273</v>
+        <v>1</v>
       </c>
       <c r="E51" t="n">
-        <v>738987447</v>
+        <v>726432006</v>
       </c>
       <c r="F51" t="n">
-        <v>5486661</v>
+        <v>1806466</v>
       </c>
       <c r="G51" t="n">
-        <v>-2.0207</v>
+        <v>0.14603</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-10-01
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>26604</v>
+        <v>27148</v>
       </c>
       <c r="E2" t="n">
-        <v>518561249912</v>
+        <v>529466684050</v>
       </c>
       <c r="F2" t="n">
-        <v>5286209623</v>
+        <v>7335447880</v>
       </c>
       <c r="G2" t="n">
-        <v>0.12943</v>
+        <v>0.7349599999999999</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1593.69</v>
+        <v>1685.26</v>
       </c>
       <c r="E3" t="n">
-        <v>191627710580</v>
+        <v>202673538772</v>
       </c>
       <c r="F3" t="n">
-        <v>2651407000</v>
+        <v>5919445066</v>
       </c>
       <c r="G3" t="n">
-        <v>0.07874</v>
+        <v>0.46486</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999966</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>83203330822</v>
+        <v>83226160343</v>
       </c>
       <c r="F4" t="n">
-        <v>8061869039</v>
+        <v>13219102802</v>
       </c>
       <c r="G4" t="n">
-        <v>0.02274</v>
+        <v>0.01029</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>210.8</v>
+        <v>215.88</v>
       </c>
       <c r="E5" t="n">
-        <v>32437149245</v>
+        <v>33219783537</v>
       </c>
       <c r="F5" t="n">
-        <v>173764446</v>
+        <v>250734242</v>
       </c>
       <c r="G5" t="n">
-        <v>0.03377</v>
+        <v>0.51341</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.510581</v>
+        <v>0.5199009999999999</v>
       </c>
       <c r="E6" t="n">
-        <v>27212561438</v>
+        <v>27728182731</v>
       </c>
       <c r="F6" t="n">
-        <v>313455140</v>
+        <v>482646947</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.16132</v>
+        <v>0.49799</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0.999266</v>
       </c>
       <c r="E7" t="n">
-        <v>25774759109</v>
+        <v>25098663953</v>
       </c>
       <c r="F7" t="n">
-        <v>1600202498</v>
+        <v>3454445392</v>
       </c>
       <c r="G7" t="n">
-        <v>0.02076</v>
+        <v>-0.08739</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1594.35</v>
+        <v>1685.45</v>
       </c>
       <c r="E8" t="n">
-        <v>13911269449</v>
+        <v>14818585841</v>
       </c>
       <c r="F8" t="n">
-        <v>7147333</v>
+        <v>11242663</v>
       </c>
       <c r="G8" t="n">
-        <v>0.17159</v>
+        <v>0.53595</v>
       </c>
     </row>
     <row r="9">
@@ -665,25 +665,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>DOGE</t>
+          <t>SOL</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Dogecoin</t>
+          <t>Solana</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.061518</v>
+        <v>22.99</v>
       </c>
       <c r="E9" t="n">
-        <v>8685449215</v>
+        <v>9497678799</v>
       </c>
       <c r="F9" t="n">
-        <v>109822523</v>
+        <v>626214031</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.13686</v>
+        <v>13.01524</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.245805</v>
+        <v>0.261157</v>
       </c>
       <c r="E10" t="n">
-        <v>8616299607</v>
+        <v>9171376999</v>
       </c>
       <c r="F10" t="n">
-        <v>60362852</v>
+        <v>162181179</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.22022</v>
+        <v>4.1124</v>
       </c>
     </row>
     <row r="11">
@@ -719,25 +719,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SOL</t>
+          <t>DOGE</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Solana</t>
+          <t>Dogecoin</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>19.62</v>
+        <v>0.06266099999999999</v>
       </c>
       <c r="E11" t="n">
-        <v>8106142524</v>
+        <v>8852289807</v>
       </c>
       <c r="F11" t="n">
-        <v>111207653</v>
+        <v>201524618</v>
       </c>
       <c r="G11" t="n">
-        <v>0.75925</v>
+        <v>1.31411</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +746,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>2.23</v>
+        <v>0.088904</v>
       </c>
       <c r="E12" t="n">
-        <v>7703772619</v>
+        <v>7915877087</v>
       </c>
       <c r="F12" t="n">
-        <v>12353611</v>
+        <v>184908066</v>
       </c>
       <c r="G12" t="n">
-        <v>-4.14935</v>
+        <v>0.17106</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.08418100000000001</v>
+        <v>2.1</v>
       </c>
       <c r="E13" t="n">
-        <v>7506255995</v>
+        <v>7227839322</v>
       </c>
       <c r="F13" t="n">
-        <v>135022365</v>
+        <v>17147204</v>
       </c>
       <c r="G13" t="n">
-        <v>0.77325</v>
+        <v>-2.55712</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>4.04</v>
+        <v>4.19</v>
       </c>
       <c r="E14" t="n">
-        <v>5168460808</v>
+        <v>5367637334</v>
       </c>
       <c r="F14" t="n">
-        <v>54035810</v>
+        <v>89058084</v>
       </c>
       <c r="G14" t="n">
-        <v>0.84137</v>
+        <v>2.52768</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.52183</v>
+        <v>0.552614</v>
       </c>
       <c r="E15" t="n">
-        <v>4862313303</v>
+        <v>5144445816</v>
       </c>
       <c r="F15" t="n">
-        <v>73001878</v>
+        <v>238031391</v>
       </c>
       <c r="G15" t="n">
-        <v>0.00797</v>
+        <v>4.6195</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>64.66</v>
+        <v>67.52</v>
       </c>
       <c r="E16" t="n">
-        <v>4766430982</v>
+        <v>4970462410</v>
       </c>
       <c r="F16" t="n">
-        <v>184268355</v>
+        <v>310908092</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.23203</v>
+        <v>2.77152</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>7.37e-06</v>
+        <v>236.71</v>
       </c>
       <c r="E17" t="n">
-        <v>4339994115</v>
+        <v>4614459960</v>
       </c>
       <c r="F17" t="n">
-        <v>151783928</v>
+        <v>178071022</v>
       </c>
       <c r="G17" t="n">
-        <v>0.18089</v>
+        <v>0.37469</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>26567</v>
+        <v>8.109999999999999</v>
       </c>
       <c r="E18" t="n">
-        <v>4326498996</v>
+        <v>4517134590</v>
       </c>
       <c r="F18" t="n">
-        <v>18358826</v>
+        <v>250192533</v>
       </c>
       <c r="G18" t="n">
-        <v>0.12348</v>
+        <v>-0.95086</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>208.64</v>
+        <v>27202</v>
       </c>
       <c r="E19" t="n">
-        <v>4073114887</v>
+        <v>4429924911</v>
       </c>
       <c r="F19" t="n">
-        <v>71390949</v>
+        <v>68158618</v>
       </c>
       <c r="G19" t="n">
-        <v>0.30936</v>
+        <v>0.7868000000000001</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>7.1</v>
+        <v>7.44e-06</v>
       </c>
       <c r="E20" t="n">
-        <v>3951101258</v>
+        <v>4385265787</v>
       </c>
       <c r="F20" t="n">
-        <v>259440126</v>
+        <v>82935896</v>
       </c>
       <c r="G20" t="n">
-        <v>1.30578</v>
+        <v>1.53487</v>
       </c>
     </row>
     <row r="21">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>0.999956</v>
       </c>
       <c r="E21" t="n">
-        <v>3843467995</v>
+        <v>3811411700</v>
       </c>
       <c r="F21" t="n">
-        <v>57549519</v>
+        <v>81941999</v>
       </c>
       <c r="G21" t="n">
-        <v>0.09417</v>
+        <v>0.0391</v>
       </c>
     </row>
     <row r="22">
@@ -1025,16 +1025,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.99898</v>
+        <v>0.998552</v>
       </c>
       <c r="E22" t="n">
-        <v>3507279323</v>
+        <v>3443358645</v>
       </c>
       <c r="F22" t="n">
-        <v>46760150</v>
+        <v>161418993</v>
       </c>
       <c r="G22" t="n">
-        <v>0.01398</v>
+        <v>-0.02249</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>3.75</v>
+        <v>4.55</v>
       </c>
       <c r="E23" t="n">
-        <v>3485171333</v>
+        <v>3436812641</v>
       </c>
       <c r="F23" t="n">
-        <v>180450</v>
+        <v>81775290</v>
       </c>
       <c r="G23" t="n">
-        <v>-2.26696</v>
+        <v>2.49827</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>4.28</v>
+        <v>9.6</v>
       </c>
       <c r="E24" t="n">
-        <v>3224902193</v>
+        <v>3407204364</v>
       </c>
       <c r="F24" t="n">
-        <v>39446281</v>
+        <v>120468649</v>
       </c>
       <c r="G24" t="n">
-        <v>0.1842</v>
+        <v>4.71103</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>9.01</v>
+        <v>3.67</v>
       </c>
       <c r="E25" t="n">
-        <v>3188662677</v>
+        <v>3404107808</v>
       </c>
       <c r="F25" t="n">
-        <v>73583184</v>
+        <v>367579</v>
       </c>
       <c r="G25" t="n">
-        <v>0.56853</v>
+        <v>-0.16756</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.113434</v>
+        <v>0.113649</v>
       </c>
       <c r="E26" t="n">
-        <v>3142869270</v>
+        <v>3153938778</v>
       </c>
       <c r="F26" t="n">
-        <v>29612413</v>
+        <v>41914333</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.36688</v>
+        <v>1.15305</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>142.94</v>
+        <v>147.92</v>
       </c>
       <c r="E27" t="n">
-        <v>2593165477</v>
+        <v>2686242122</v>
       </c>
       <c r="F27" t="n">
-        <v>37268065</v>
+        <v>54791971</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.70748</v>
+        <v>1.07574</v>
       </c>
     </row>
     <row r="28">
@@ -1187,16 +1187,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>42.85</v>
+        <v>43.29</v>
       </c>
       <c r="E28" t="n">
-        <v>2573393240</v>
+        <v>2598185668</v>
       </c>
       <c r="F28" t="n">
-        <v>1437314</v>
+        <v>2182104</v>
       </c>
       <c r="G28" t="n">
-        <v>0.28249</v>
+        <v>0.52967</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Binance USD</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>16.43</v>
       </c>
       <c r="E29" t="n">
-        <v>2381668298</v>
+        <v>2353488191</v>
       </c>
       <c r="F29" t="n">
-        <v>684960026</v>
+        <v>143436672</v>
       </c>
       <c r="G29" t="n">
-        <v>0.00317</v>
+        <v>2.30659</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>15.27</v>
+        <v>0.999973</v>
       </c>
       <c r="E30" t="n">
-        <v>2184472345</v>
+        <v>2259921762</v>
       </c>
       <c r="F30" t="n">
-        <v>38858988</v>
+        <v>2535888906</v>
       </c>
       <c r="G30" t="n">
-        <v>0.47672</v>
+        <v>-0.01782</v>
       </c>
     </row>
     <row r="31">
@@ -1268,16 +1268,16 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>7.06</v>
+        <v>7.28</v>
       </c>
       <c r="E31" t="n">
-        <v>2064306033</v>
+        <v>2131431692</v>
       </c>
       <c r="F31" t="n">
-        <v>79706843</v>
+        <v>73008444</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.44987</v>
+        <v>0.97719</v>
       </c>
     </row>
     <row r="32">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.050437</v>
+        <v>0.050017</v>
       </c>
       <c r="E32" t="n">
-        <v>1685403380</v>
+        <v>1674609003</v>
       </c>
       <c r="F32" t="n">
-        <v>15665416</v>
+        <v>17145550</v>
       </c>
       <c r="G32" t="n">
-        <v>-1.63668</v>
+        <v>0.56653</v>
       </c>
     </row>
     <row r="33">
@@ -1322,16 +1322,16 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>3.25</v>
+        <v>3.39</v>
       </c>
       <c r="E33" t="n">
-        <v>1468511796</v>
+        <v>1537129891</v>
       </c>
       <c r="F33" t="n">
-        <v>46443126</v>
+        <v>64284138</v>
       </c>
       <c r="G33" t="n">
-        <v>0.78301</v>
+        <v>2.44599</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.051313</v>
+        <v>1.68</v>
       </c>
       <c r="E34" t="n">
-        <v>1353733630</v>
+        <v>1498303539</v>
       </c>
       <c r="F34" t="n">
-        <v>13112024</v>
+        <v>28593893</v>
       </c>
       <c r="G34" t="n">
-        <v>1.58151</v>
+        <v>-0.17632</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1.49</v>
+        <v>3.23</v>
       </c>
       <c r="E35" t="n">
-        <v>1323768554</v>
+        <v>1441226669</v>
       </c>
       <c r="F35" t="n">
-        <v>9894668</v>
+        <v>16354090</v>
       </c>
       <c r="G35" t="n">
-        <v>0.26614</v>
+        <v>1.84671</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>2.96</v>
+        <v>1558.04</v>
       </c>
       <c r="E36" t="n">
-        <v>1315129194</v>
+        <v>1405063488</v>
       </c>
       <c r="F36" t="n">
-        <v>9140714</v>
+        <v>76955416</v>
       </c>
       <c r="G36" t="n">
-        <v>0.35466</v>
+        <v>5.18035</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>90.11</v>
+        <v>0.051144</v>
       </c>
       <c r="E37" t="n">
-        <v>1311742154</v>
+        <v>1345138792</v>
       </c>
       <c r="F37" t="n">
-        <v>9116989</v>
+        <v>5904226</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.70339</v>
+        <v>0.81387</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.39705</v>
+        <v>90.98</v>
       </c>
       <c r="E38" t="n">
-        <v>1284065364</v>
+        <v>1324262915</v>
       </c>
       <c r="F38" t="n">
-        <v>11973910</v>
+        <v>11333737</v>
       </c>
       <c r="G38" t="n">
-        <v>1.43755</v>
+        <v>0.62295</v>
       </c>
     </row>
     <row r="39">
@@ -1484,16 +1484,16 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>5.32</v>
+        <v>5.53</v>
       </c>
       <c r="E39" t="n">
-        <v>1258831819</v>
+        <v>1315625053</v>
       </c>
       <c r="F39" t="n">
-        <v>32581917</v>
+        <v>67202150</v>
       </c>
       <c r="G39" t="n">
-        <v>3.91372</v>
+        <v>2.65963</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.01691804</v>
+        <v>0.396476</v>
       </c>
       <c r="E40" t="n">
-        <v>1230279023</v>
+        <v>1282459757</v>
       </c>
       <c r="F40" t="n">
-        <v>22117596</v>
+        <v>25708811</v>
       </c>
       <c r="G40" t="n">
-        <v>0.09121</v>
+        <v>-0.6499200000000001</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1284.43</v>
+        <v>0.01738331</v>
       </c>
       <c r="E41" t="n">
-        <v>1157407724</v>
+        <v>1264706234</v>
       </c>
       <c r="F41" t="n">
-        <v>34979828</v>
+        <v>28513262</v>
       </c>
       <c r="G41" t="n">
-        <v>0.49575</v>
+        <v>-0.91248</v>
       </c>
     </row>
     <row r="42">
@@ -1565,16 +1565,16 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.829186</v>
+        <v>0.9487679999999999</v>
       </c>
       <c r="E42" t="n">
-        <v>1056989634</v>
+        <v>1211002777</v>
       </c>
       <c r="F42" t="n">
-        <v>40649559</v>
+        <v>149551333</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.04506</v>
+        <v>4.88995</v>
       </c>
     </row>
     <row r="43">
@@ -1592,16 +1592,16 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1.11</v>
+        <v>1.15</v>
       </c>
       <c r="E43" t="n">
-        <v>1046629964</v>
+        <v>1126482424</v>
       </c>
       <c r="F43" t="n">
-        <v>24376532</v>
+        <v>38626621</v>
       </c>
       <c r="G43" t="n">
-        <v>0.02613</v>
+        <v>1.62656</v>
       </c>
     </row>
     <row r="44">
@@ -1619,16 +1619,16 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1.29</v>
+        <v>1.38</v>
       </c>
       <c r="E44" t="n">
-        <v>1033573587</v>
+        <v>1105457918</v>
       </c>
       <c r="F44" t="n">
-        <v>32730120</v>
+        <v>61155858</v>
       </c>
       <c r="G44" t="n">
-        <v>0.29553</v>
+        <v>4.6135</v>
       </c>
     </row>
     <row r="45">
@@ -1646,16 +1646,16 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.04600801</v>
+        <v>0.04999857</v>
       </c>
       <c r="E45" t="n">
-        <v>958455531</v>
+        <v>1047100321</v>
       </c>
       <c r="F45" t="n">
-        <v>7400215</v>
+        <v>11646597</v>
       </c>
       <c r="G45" t="n">
-        <v>0.68474</v>
+        <v>3.02333</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>RETH</t>
+          <t>AAVE</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Rocket Pool ETH</t>
+          <t>Aave</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>1734.01</v>
+        <v>69.14</v>
       </c>
       <c r="E46" t="n">
-        <v>917043628</v>
+        <v>1009315532</v>
       </c>
       <c r="F46" t="n">
-        <v>3699007</v>
+        <v>85141078</v>
       </c>
       <c r="G46" t="n">
-        <v>0.21567</v>
+        <v>2.73448</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>AAVE</t>
+          <t>RETH</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Aave</t>
+          <t>Rocket Pool ETH</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>62.72</v>
+        <v>1832.77</v>
       </c>
       <c r="E47" t="n">
-        <v>914090373</v>
+        <v>970210527</v>
       </c>
       <c r="F47" t="n">
-        <v>38349036</v>
+        <v>2026564</v>
       </c>
       <c r="G47" t="n">
-        <v>-0.8118</v>
+        <v>0.611</v>
       </c>
     </row>
     <row r="48">
@@ -1727,16 +1727,16 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.08741699999999999</v>
+        <v>0.091276</v>
       </c>
       <c r="E48" t="n">
-        <v>807561413</v>
+        <v>845367723</v>
       </c>
       <c r="F48" t="n">
-        <v>14652153</v>
+        <v>23879727</v>
       </c>
       <c r="G48" t="n">
-        <v>-1.38595</v>
+        <v>4.03684</v>
       </c>
     </row>
     <row r="49">
@@ -1754,16 +1754,16 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.101447</v>
+        <v>0.1046</v>
       </c>
       <c r="E49" t="n">
-        <v>794019115</v>
+        <v>820814306</v>
       </c>
       <c r="F49" t="n">
-        <v>15826954</v>
+        <v>24458656</v>
       </c>
       <c r="G49" t="n">
-        <v>0.33846</v>
+        <v>2.15688</v>
       </c>
     </row>
     <row r="50">
@@ -1781,16 +1781,16 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>5.31</v>
+        <v>5.16</v>
       </c>
       <c r="E50" t="n">
-        <v>764812777</v>
+        <v>743787475</v>
       </c>
       <c r="F50" t="n">
-        <v>7890381</v>
+        <v>7077158</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.14292</v>
+        <v>-0.51532</v>
       </c>
     </row>
     <row r="51">
@@ -1808,16 +1808,16 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>0.997862</v>
       </c>
       <c r="E51" t="n">
-        <v>726432006</v>
+        <v>726949805</v>
       </c>
       <c r="F51" t="n">
-        <v>1806466</v>
+        <v>19499517</v>
       </c>
       <c r="G51" t="n">
-        <v>0.14603</v>
+        <v>-0.058</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-10-08
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>27148</v>
+        <v>27843</v>
       </c>
       <c r="E2" t="n">
-        <v>529466684050</v>
+        <v>543181485383</v>
       </c>
       <c r="F2" t="n">
-        <v>7335447880</v>
+        <v>4667714232</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7349599999999999</v>
+        <v>-0.51074</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1685.26</v>
+        <v>1620.97</v>
       </c>
       <c r="E3" t="n">
-        <v>202673538772</v>
+        <v>194910373595</v>
       </c>
       <c r="F3" t="n">
-        <v>5919445066</v>
+        <v>4555745239</v>
       </c>
       <c r="G3" t="n">
-        <v>0.46486</v>
+        <v>-1.20362</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>1.001</v>
       </c>
       <c r="E4" t="n">
-        <v>83226160343</v>
+        <v>83497079037</v>
       </c>
       <c r="F4" t="n">
-        <v>13219102802</v>
+        <v>11283577884</v>
       </c>
       <c r="G4" t="n">
-        <v>0.01029</v>
+        <v>0.01407</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>215.88</v>
+        <v>210.27</v>
       </c>
       <c r="E5" t="n">
-        <v>33219783537</v>
+        <v>32363234631</v>
       </c>
       <c r="F5" t="n">
-        <v>250734242</v>
+        <v>208839090</v>
       </c>
       <c r="G5" t="n">
-        <v>0.51341</v>
+        <v>-1.1398</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.5199009999999999</v>
+        <v>0.519411</v>
       </c>
       <c r="E6" t="n">
-        <v>27728182731</v>
+        <v>27714558076</v>
       </c>
       <c r="F6" t="n">
-        <v>482646947</v>
+        <v>283173955</v>
       </c>
       <c r="G6" t="n">
-        <v>0.49799</v>
+        <v>-0.70167</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.999266</v>
+        <v>0.999915</v>
       </c>
       <c r="E7" t="n">
-        <v>25098663953</v>
+        <v>25538586130</v>
       </c>
       <c r="F7" t="n">
-        <v>3454445392</v>
+        <v>2248218712</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.08739</v>
+        <v>0.0305</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1685.45</v>
+        <v>1619.8</v>
       </c>
       <c r="E8" t="n">
-        <v>14818585841</v>
+        <v>14240451895</v>
       </c>
       <c r="F8" t="n">
-        <v>11242663</v>
+        <v>42235171</v>
       </c>
       <c r="G8" t="n">
-        <v>0.53595</v>
+        <v>-1.25206</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>22.99</v>
+        <v>23.22</v>
       </c>
       <c r="E9" t="n">
-        <v>9497678799</v>
+        <v>9621133504</v>
       </c>
       <c r="F9" t="n">
-        <v>626214031</v>
+        <v>240271740</v>
       </c>
       <c r="G9" t="n">
-        <v>13.01524</v>
+        <v>-1.36738</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.261157</v>
+        <v>0.256061</v>
       </c>
       <c r="E10" t="n">
-        <v>9171376999</v>
+        <v>9280973293</v>
       </c>
       <c r="F10" t="n">
-        <v>162181179</v>
+        <v>91551002</v>
       </c>
       <c r="G10" t="n">
-        <v>4.1124</v>
+        <v>-0.82157</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.06266099999999999</v>
+        <v>0.060984</v>
       </c>
       <c r="E11" t="n">
-        <v>8852289807</v>
+        <v>8618302159</v>
       </c>
       <c r="F11" t="n">
-        <v>201524618</v>
+        <v>137713814</v>
       </c>
       <c r="G11" t="n">
-        <v>1.31411</v>
+        <v>-0.81281</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.088904</v>
+        <v>0.087643</v>
       </c>
       <c r="E12" t="n">
-        <v>7915877087</v>
+        <v>7797204560</v>
       </c>
       <c r="F12" t="n">
-        <v>184908066</v>
+        <v>150078518</v>
       </c>
       <c r="G12" t="n">
-        <v>0.17106</v>
+        <v>-0.5502</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2.1</v>
+        <v>2.03</v>
       </c>
       <c r="E13" t="n">
-        <v>7227839322</v>
+        <v>7005225406</v>
       </c>
       <c r="F13" t="n">
-        <v>17147204</v>
+        <v>12154480</v>
       </c>
       <c r="G13" t="n">
-        <v>-2.55712</v>
+        <v>-2.93037</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>4.19</v>
+        <v>0.5585869999999999</v>
       </c>
       <c r="E14" t="n">
-        <v>5367637334</v>
+        <v>5195438559</v>
       </c>
       <c r="F14" t="n">
-        <v>89058084</v>
+        <v>159289213</v>
       </c>
       <c r="G14" t="n">
-        <v>2.52768</v>
+        <v>-2.86546</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.552614</v>
+        <v>4.01</v>
       </c>
       <c r="E15" t="n">
-        <v>5144445816</v>
+        <v>5148118672</v>
       </c>
       <c r="F15" t="n">
-        <v>238031391</v>
+        <v>59178587</v>
       </c>
       <c r="G15" t="n">
-        <v>4.6195</v>
+        <v>-1.9589</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>67.52</v>
+        <v>65.15000000000001</v>
       </c>
       <c r="E16" t="n">
-        <v>4970462410</v>
+        <v>4799278724</v>
       </c>
       <c r="F16" t="n">
-        <v>310908092</v>
+        <v>242324233</v>
       </c>
       <c r="G16" t="n">
-        <v>2.77152</v>
+        <v>-1.06136</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>236.71</v>
+        <v>27856</v>
       </c>
       <c r="E17" t="n">
-        <v>4614459960</v>
+        <v>4534784820</v>
       </c>
       <c r="F17" t="n">
-        <v>178071022</v>
+        <v>50537413</v>
       </c>
       <c r="G17" t="n">
-        <v>0.37469</v>
+        <v>-0.53415</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>8.109999999999999</v>
+        <v>227.86</v>
       </c>
       <c r="E18" t="n">
-        <v>4517134590</v>
+        <v>4451834097</v>
       </c>
       <c r="F18" t="n">
-        <v>250192533</v>
+        <v>88738457</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.95086</v>
+        <v>-2.35166</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>27202</v>
+        <v>7.19e-06</v>
       </c>
       <c r="E19" t="n">
-        <v>4429924911</v>
+        <v>4234829252</v>
       </c>
       <c r="F19" t="n">
-        <v>68158618</v>
+        <v>53035715</v>
       </c>
       <c r="G19" t="n">
-        <v>0.7868000000000001</v>
+        <v>-0.6211</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>7.44e-06</v>
+        <v>7.59</v>
       </c>
       <c r="E20" t="n">
-        <v>4385265787</v>
+        <v>4225501918</v>
       </c>
       <c r="F20" t="n">
-        <v>82935896</v>
+        <v>178343111</v>
       </c>
       <c r="G20" t="n">
-        <v>1.53487</v>
+        <v>-0.30151</v>
       </c>
     </row>
     <row r="21">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.999956</v>
+        <v>0.999371</v>
       </c>
       <c r="E21" t="n">
-        <v>3811411700</v>
+        <v>3830717813</v>
       </c>
       <c r="F21" t="n">
-        <v>81941999</v>
+        <v>66564302</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0391</v>
+        <v>-0.08259</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.998552</v>
+        <v>3.84</v>
       </c>
       <c r="E22" t="n">
-        <v>3443358645</v>
+        <v>3572187099</v>
       </c>
       <c r="F22" t="n">
-        <v>161418993</v>
+        <v>94473</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.02249</v>
+        <v>-0.11313</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>4.55</v>
+        <v>10.05</v>
       </c>
       <c r="E23" t="n">
-        <v>3436812641</v>
+        <v>3560326948</v>
       </c>
       <c r="F23" t="n">
-        <v>81775290</v>
+        <v>175127595</v>
       </c>
       <c r="G23" t="n">
-        <v>2.49827</v>
+        <v>-4.09623</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>TUSD</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>9.6</v>
+        <v>0.999342</v>
       </c>
       <c r="E24" t="n">
-        <v>3407204364</v>
+        <v>3414527602</v>
       </c>
       <c r="F24" t="n">
-        <v>120468649</v>
+        <v>92031925</v>
       </c>
       <c r="G24" t="n">
-        <v>4.71103</v>
+        <v>-0.04549</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>3.67</v>
+        <v>4.3</v>
       </c>
       <c r="E25" t="n">
-        <v>3404107808</v>
+        <v>3243716129</v>
       </c>
       <c r="F25" t="n">
-        <v>367579</v>
+        <v>35493289</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.16756</v>
+        <v>-1.49434</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.113649</v>
+        <v>0.110797</v>
       </c>
       <c r="E26" t="n">
-        <v>3153938778</v>
+        <v>3075498370</v>
       </c>
       <c r="F26" t="n">
-        <v>41914333</v>
+        <v>32658899</v>
       </c>
       <c r="G26" t="n">
-        <v>1.15305</v>
+        <v>-0.19885</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>147.92</v>
+        <v>153.94</v>
       </c>
       <c r="E27" t="n">
-        <v>2686242122</v>
+        <v>2792048247</v>
       </c>
       <c r="F27" t="n">
-        <v>54791971</v>
+        <v>68984675</v>
       </c>
       <c r="G27" t="n">
-        <v>1.07574</v>
+        <v>1.16349</v>
       </c>
     </row>
     <row r="28">
@@ -1187,16 +1187,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>43.29</v>
+        <v>42.85</v>
       </c>
       <c r="E28" t="n">
-        <v>2598185668</v>
+        <v>2570480471</v>
       </c>
       <c r="F28" t="n">
-        <v>2182104</v>
+        <v>1207154</v>
       </c>
       <c r="G28" t="n">
-        <v>0.52967</v>
+        <v>-0.19429</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>16.43</v>
+        <v>1</v>
       </c>
       <c r="E29" t="n">
-        <v>2353488191</v>
+        <v>2214208023</v>
       </c>
       <c r="F29" t="n">
-        <v>143436672</v>
+        <v>1595223858</v>
       </c>
       <c r="G29" t="n">
-        <v>2.30659</v>
+        <v>-0.00874</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.999973</v>
+        <v>15.43</v>
       </c>
       <c r="E30" t="n">
-        <v>2259921762</v>
+        <v>2208836903</v>
       </c>
       <c r="F30" t="n">
-        <v>2535888906</v>
+        <v>50433624</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.01782</v>
+        <v>-1.49947</v>
       </c>
     </row>
     <row r="31">
@@ -1268,16 +1268,16 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>7.28</v>
+        <v>6.88</v>
       </c>
       <c r="E31" t="n">
-        <v>2131431692</v>
+        <v>2008088814</v>
       </c>
       <c r="F31" t="n">
-        <v>73008444</v>
+        <v>122999552</v>
       </c>
       <c r="G31" t="n">
-        <v>0.97719</v>
+        <v>-1.17377</v>
       </c>
     </row>
     <row r="32">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.050017</v>
+        <v>0.04795734</v>
       </c>
       <c r="E32" t="n">
-        <v>1674609003</v>
+        <v>1603977505</v>
       </c>
       <c r="F32" t="n">
-        <v>17145550</v>
+        <v>19266014</v>
       </c>
       <c r="G32" t="n">
-        <v>0.56653</v>
+        <v>-0.80767</v>
       </c>
     </row>
     <row r="33">
@@ -1322,16 +1322,16 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>3.39</v>
+        <v>3.42</v>
       </c>
       <c r="E33" t="n">
-        <v>1537129891</v>
+        <v>1555539778</v>
       </c>
       <c r="F33" t="n">
-        <v>64284138</v>
+        <v>67793600</v>
       </c>
       <c r="G33" t="n">
-        <v>2.44599</v>
+        <v>1.56894</v>
       </c>
     </row>
     <row r="34">
@@ -1349,16 +1349,16 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>1.68</v>
+        <v>1.57</v>
       </c>
       <c r="E34" t="n">
-        <v>1498303539</v>
+        <v>1394637434</v>
       </c>
       <c r="F34" t="n">
-        <v>28593893</v>
+        <v>20067004</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.17632</v>
+        <v>-0.24166</v>
       </c>
     </row>
     <row r="35">
@@ -1376,16 +1376,16 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>3.23</v>
+        <v>3.07</v>
       </c>
       <c r="E35" t="n">
-        <v>1441226669</v>
+        <v>1366329278</v>
       </c>
       <c r="F35" t="n">
-        <v>16354090</v>
+        <v>12142992</v>
       </c>
       <c r="G35" t="n">
-        <v>1.84671</v>
+        <v>-1.70944</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1558.04</v>
+        <v>0.050046</v>
       </c>
       <c r="E36" t="n">
-        <v>1405063488</v>
+        <v>1316610464</v>
       </c>
       <c r="F36" t="n">
-        <v>76955416</v>
+        <v>3075579</v>
       </c>
       <c r="G36" t="n">
-        <v>5.18035</v>
+        <v>-1.01384</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.051144</v>
+        <v>87.52</v>
       </c>
       <c r="E37" t="n">
-        <v>1345138792</v>
+        <v>1273274244</v>
       </c>
       <c r="F37" t="n">
-        <v>5904226</v>
+        <v>7477937</v>
       </c>
       <c r="G37" t="n">
-        <v>0.81387</v>
+        <v>-0.22121</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>90.98</v>
+        <v>1383.35</v>
       </c>
       <c r="E38" t="n">
-        <v>1324262915</v>
+        <v>1246758994</v>
       </c>
       <c r="F38" t="n">
-        <v>11333737</v>
+        <v>43444629</v>
       </c>
       <c r="G38" t="n">
-        <v>0.62295</v>
+        <v>-2.18273</v>
       </c>
     </row>
     <row r="39">
@@ -1484,16 +1484,16 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>5.53</v>
+        <v>5.21</v>
       </c>
       <c r="E39" t="n">
-        <v>1315625053</v>
+        <v>1246109881</v>
       </c>
       <c r="F39" t="n">
-        <v>67202150</v>
+        <v>26570343</v>
       </c>
       <c r="G39" t="n">
-        <v>2.65963</v>
+        <v>-1.4916</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.396476</v>
+        <v>0.01694127</v>
       </c>
       <c r="E40" t="n">
-        <v>1282459757</v>
+        <v>1230520110</v>
       </c>
       <c r="F40" t="n">
-        <v>25708811</v>
+        <v>22302401</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.6499200000000001</v>
+        <v>0.09877</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.01738331</v>
+        <v>0.382248</v>
       </c>
       <c r="E41" t="n">
-        <v>1264706234</v>
+        <v>1221536771</v>
       </c>
       <c r="F41" t="n">
-        <v>28513262</v>
+        <v>21499108</v>
       </c>
       <c r="G41" t="n">
-        <v>-0.91248</v>
+        <v>-2.82987</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.9487679999999999</v>
+        <v>1.27</v>
       </c>
       <c r="E42" t="n">
-        <v>1211002777</v>
+        <v>1109907699</v>
       </c>
       <c r="F42" t="n">
-        <v>149551333</v>
+        <v>60650998</v>
       </c>
       <c r="G42" t="n">
-        <v>4.88995</v>
+        <v>-2.46999</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1.15</v>
+        <v>0.843456</v>
       </c>
       <c r="E43" t="n">
-        <v>1126482424</v>
+        <v>1075061997</v>
       </c>
       <c r="F43" t="n">
-        <v>38626621</v>
+        <v>68572422</v>
       </c>
       <c r="G43" t="n">
-        <v>1.62656</v>
+        <v>-4.45274</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1.38</v>
+        <v>1.08</v>
       </c>
       <c r="E44" t="n">
-        <v>1105457918</v>
+        <v>1054859374</v>
       </c>
       <c r="F44" t="n">
-        <v>61155858</v>
+        <v>26602837</v>
       </c>
       <c r="G44" t="n">
-        <v>4.6135</v>
+        <v>-1.27591</v>
       </c>
     </row>
     <row r="45">
@@ -1646,16 +1646,16 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.04999857</v>
+        <v>0.04888521</v>
       </c>
       <c r="E45" t="n">
-        <v>1047100321</v>
+        <v>1028373473</v>
       </c>
       <c r="F45" t="n">
-        <v>11646597</v>
+        <v>9156830</v>
       </c>
       <c r="G45" t="n">
-        <v>3.02333</v>
+        <v>-3.48943</v>
       </c>
     </row>
     <row r="46">
@@ -1673,16 +1673,16 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>69.14</v>
+        <v>65.5</v>
       </c>
       <c r="E46" t="n">
-        <v>1009315532</v>
+        <v>955582001</v>
       </c>
       <c r="F46" t="n">
-        <v>85141078</v>
+        <v>55199316</v>
       </c>
       <c r="G46" t="n">
-        <v>2.73448</v>
+        <v>-1.9766</v>
       </c>
     </row>
     <row r="47">
@@ -1700,16 +1700,16 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>1832.77</v>
+        <v>1756.3</v>
       </c>
       <c r="E47" t="n">
-        <v>970210527</v>
+        <v>936515414</v>
       </c>
       <c r="F47" t="n">
-        <v>2026564</v>
+        <v>8380306</v>
       </c>
       <c r="G47" t="n">
-        <v>0.611</v>
+        <v>-1.19005</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>ALGO</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Algorand</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.091276</v>
+        <v>0.100913</v>
       </c>
       <c r="E48" t="n">
-        <v>845367723</v>
+        <v>798367111</v>
       </c>
       <c r="F48" t="n">
-        <v>23879727</v>
+        <v>26889711</v>
       </c>
       <c r="G48" t="n">
-        <v>4.03684</v>
+        <v>0.76251</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ALGO</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Algorand</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.1046</v>
+        <v>0.08459999999999999</v>
       </c>
       <c r="E49" t="n">
-        <v>820814306</v>
+        <v>781364370</v>
       </c>
       <c r="F49" t="n">
-        <v>24458656</v>
+        <v>15997145</v>
       </c>
       <c r="G49" t="n">
-        <v>2.15688</v>
+        <v>-1.06353</v>
       </c>
     </row>
     <row r="50">
@@ -1781,16 +1781,16 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>5.16</v>
+        <v>5.17</v>
       </c>
       <c r="E50" t="n">
-        <v>743787475</v>
+        <v>756728465</v>
       </c>
       <c r="F50" t="n">
-        <v>7077158</v>
+        <v>3988397</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.51532</v>
+        <v>-0.2926</v>
       </c>
     </row>
     <row r="51">
@@ -1808,16 +1808,16 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.997862</v>
+        <v>0.999309</v>
       </c>
       <c r="E51" t="n">
-        <v>726949805</v>
+        <v>728779070</v>
       </c>
       <c r="F51" t="n">
-        <v>19499517</v>
+        <v>21387464</v>
       </c>
       <c r="G51" t="n">
-        <v>-0.058</v>
+        <v>-0.07804999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-10-15
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>27843</v>
+        <v>26831</v>
       </c>
       <c r="E2" t="n">
-        <v>543181485383</v>
+        <v>523778156497</v>
       </c>
       <c r="F2" t="n">
-        <v>4667714232</v>
+        <v>5423976183</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.51074</v>
+        <v>-0.09397</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1620.97</v>
+        <v>1554.14</v>
       </c>
       <c r="E3" t="n">
-        <v>194910373595</v>
+        <v>186950386334</v>
       </c>
       <c r="F3" t="n">
-        <v>4555745239</v>
+        <v>2456993720</v>
       </c>
       <c r="G3" t="n">
-        <v>-1.20362</v>
+        <v>0.48933</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1.001</v>
+        <v>0.999956</v>
       </c>
       <c r="E4" t="n">
-        <v>83497079037</v>
+        <v>83523310091</v>
       </c>
       <c r="F4" t="n">
-        <v>11283577884</v>
+        <v>8866877614</v>
       </c>
       <c r="G4" t="n">
-        <v>0.01407</v>
+        <v>0.01701</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>210.27</v>
+        <v>206.87</v>
       </c>
       <c r="E5" t="n">
-        <v>32363234631</v>
+        <v>31846892603</v>
       </c>
       <c r="F5" t="n">
-        <v>208839090</v>
+        <v>202274670</v>
       </c>
       <c r="G5" t="n">
-        <v>-1.1398</v>
+        <v>0.51519</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.519411</v>
+        <v>0.486281</v>
       </c>
       <c r="E6" t="n">
-        <v>27714558076</v>
+        <v>25991088961</v>
       </c>
       <c r="F6" t="n">
-        <v>283173955</v>
+        <v>282398047</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.70167</v>
+        <v>0.12439</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.999915</v>
+        <v>0.999383</v>
       </c>
       <c r="E7" t="n">
-        <v>25538586130</v>
+        <v>25111780254</v>
       </c>
       <c r="F7" t="n">
-        <v>2248218712</v>
+        <v>2408120721</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0305</v>
+        <v>-0.07718</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1619.8</v>
+        <v>1554.33</v>
       </c>
       <c r="E8" t="n">
-        <v>14240451895</v>
+        <v>13711685780</v>
       </c>
       <c r="F8" t="n">
-        <v>42235171</v>
+        <v>15178326</v>
       </c>
       <c r="G8" t="n">
-        <v>-1.25206</v>
+        <v>0.49134</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>23.22</v>
+        <v>21.79</v>
       </c>
       <c r="E9" t="n">
-        <v>9621133504</v>
+        <v>9079614066</v>
       </c>
       <c r="F9" t="n">
-        <v>240271740</v>
+        <v>160621207</v>
       </c>
       <c r="G9" t="n">
-        <v>-1.36738</v>
+        <v>-0.46341</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.256061</v>
+        <v>0.246233</v>
       </c>
       <c r="E10" t="n">
-        <v>9280973293</v>
+        <v>8595337336</v>
       </c>
       <c r="F10" t="n">
-        <v>91551002</v>
+        <v>76973323</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.82157</v>
+        <v>0.00062</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.060984</v>
+        <v>0.059116</v>
       </c>
       <c r="E11" t="n">
-        <v>8618302159</v>
+        <v>8369733123</v>
       </c>
       <c r="F11" t="n">
-        <v>137713814</v>
+        <v>147973120</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.81281</v>
+        <v>0.45077</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.087643</v>
+        <v>0.08538</v>
       </c>
       <c r="E12" t="n">
-        <v>7797204560</v>
+        <v>7596548689</v>
       </c>
       <c r="F12" t="n">
-        <v>150078518</v>
+        <v>200737055</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.5502</v>
+        <v>0.03473</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2.03</v>
+        <v>1.92</v>
       </c>
       <c r="E13" t="n">
-        <v>7005225406</v>
+        <v>6628379109</v>
       </c>
       <c r="F13" t="n">
-        <v>12154480</v>
+        <v>13710188</v>
       </c>
       <c r="G13" t="n">
-        <v>-2.93037</v>
+        <v>-1.0927</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.5585869999999999</v>
+        <v>3.73</v>
       </c>
       <c r="E14" t="n">
-        <v>5195438559</v>
+        <v>4798308944</v>
       </c>
       <c r="F14" t="n">
-        <v>159289213</v>
+        <v>67436843</v>
       </c>
       <c r="G14" t="n">
-        <v>-2.86546</v>
+        <v>-0.05501</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>4.01</v>
+        <v>0.515084</v>
       </c>
       <c r="E15" t="n">
-        <v>5148118672</v>
+        <v>4791926070</v>
       </c>
       <c r="F15" t="n">
-        <v>59178587</v>
+        <v>93527363</v>
       </c>
       <c r="G15" t="n">
-        <v>-1.9589</v>
+        <v>-0.3185</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>65.15000000000001</v>
+        <v>61.46</v>
       </c>
       <c r="E16" t="n">
-        <v>4799278724</v>
+        <v>4534635047</v>
       </c>
       <c r="F16" t="n">
-        <v>242324233</v>
+        <v>145957665</v>
       </c>
       <c r="G16" t="n">
-        <v>-1.06136</v>
+        <v>-0.04898</v>
       </c>
     </row>
     <row r="17">
@@ -890,16 +890,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>27856</v>
+        <v>26817</v>
       </c>
       <c r="E17" t="n">
-        <v>4534784820</v>
+        <v>4371497770</v>
       </c>
       <c r="F17" t="n">
-        <v>50537413</v>
+        <v>27278860</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.53415</v>
+        <v>-0.17271</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>227.86</v>
+        <v>213.45</v>
       </c>
       <c r="E18" t="n">
-        <v>4451834097</v>
+        <v>4170310656</v>
       </c>
       <c r="F18" t="n">
-        <v>88738457</v>
+        <v>67161082</v>
       </c>
       <c r="G18" t="n">
-        <v>-2.35166</v>
+        <v>-1.15309</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>7.19e-06</v>
+        <v>6.99e-06</v>
       </c>
       <c r="E19" t="n">
-        <v>4234829252</v>
+        <v>4120307764</v>
       </c>
       <c r="F19" t="n">
-        <v>53035715</v>
+        <v>73670495</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.6211</v>
+        <v>-1.85399</v>
       </c>
     </row>
     <row r="20">
@@ -971,16 +971,16 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>7.59</v>
+        <v>7.34</v>
       </c>
       <c r="E20" t="n">
-        <v>4225501918</v>
+        <v>4089650602</v>
       </c>
       <c r="F20" t="n">
-        <v>178343111</v>
+        <v>108370812</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.30151</v>
+        <v>1.35632</v>
       </c>
     </row>
     <row r="21">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.999371</v>
+        <v>0.999561</v>
       </c>
       <c r="E21" t="n">
-        <v>3830717813</v>
+        <v>3783747143</v>
       </c>
       <c r="F21" t="n">
-        <v>66564302</v>
+        <v>40242195</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.08259</v>
+        <v>-0.01461</v>
       </c>
     </row>
     <row r="22">
@@ -1025,16 +1025,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>3.84</v>
+        <v>3.81</v>
       </c>
       <c r="E22" t="n">
-        <v>3572187099</v>
+        <v>3536976356</v>
       </c>
       <c r="F22" t="n">
-        <v>94473</v>
+        <v>171107</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.11313</v>
+        <v>2.12704</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>TUSD</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>10.05</v>
+        <v>0.999133</v>
       </c>
       <c r="E23" t="n">
-        <v>3560326948</v>
+        <v>3366138724</v>
       </c>
       <c r="F23" t="n">
-        <v>175127595</v>
+        <v>56196315</v>
       </c>
       <c r="G23" t="n">
-        <v>-4.09623</v>
+        <v>-0.00339</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.999342</v>
+        <v>9.1</v>
       </c>
       <c r="E24" t="n">
-        <v>3414527602</v>
+        <v>3231314749</v>
       </c>
       <c r="F24" t="n">
-        <v>92031925</v>
+        <v>79655091</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.04549</v>
+        <v>-0.82112</v>
       </c>
     </row>
     <row r="25">
@@ -1106,16 +1106,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>4.3</v>
+        <v>4.11</v>
       </c>
       <c r="E25" t="n">
-        <v>3243716129</v>
+        <v>3097965772</v>
       </c>
       <c r="F25" t="n">
-        <v>35493289</v>
+        <v>36833040</v>
       </c>
       <c r="G25" t="n">
-        <v>-1.49434</v>
+        <v>0.81024</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.110797</v>
+        <v>0.104614</v>
       </c>
       <c r="E26" t="n">
-        <v>3075498370</v>
+        <v>2906201000</v>
       </c>
       <c r="F26" t="n">
-        <v>32658899</v>
+        <v>37239204</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.19885</v>
+        <v>0.8154400000000001</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>153.94</v>
+        <v>152.63</v>
       </c>
       <c r="E27" t="n">
-        <v>2792048247</v>
+        <v>2772332911</v>
       </c>
       <c r="F27" t="n">
-        <v>68984675</v>
+        <v>33984604</v>
       </c>
       <c r="G27" t="n">
-        <v>1.16349</v>
+        <v>-0.21978</v>
       </c>
     </row>
     <row r="28">
@@ -1187,16 +1187,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>42.85</v>
+        <v>43.06</v>
       </c>
       <c r="E28" t="n">
-        <v>2570480471</v>
+        <v>2584193964</v>
       </c>
       <c r="F28" t="n">
-        <v>1207154</v>
+        <v>2063446</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.19429</v>
+        <v>-0.40202</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>14.9</v>
       </c>
       <c r="E29" t="n">
-        <v>2214208023</v>
+        <v>2134682284</v>
       </c>
       <c r="F29" t="n">
-        <v>1595223858</v>
+        <v>37499873</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.00874</v>
+        <v>0.14464</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>15.43</v>
+        <v>1</v>
       </c>
       <c r="E30" t="n">
-        <v>2208836903</v>
+        <v>2124771813</v>
       </c>
       <c r="F30" t="n">
-        <v>50433624</v>
+        <v>951097462</v>
       </c>
       <c r="G30" t="n">
-        <v>-1.49947</v>
+        <v>-0.01297</v>
       </c>
     </row>
     <row r="31">
@@ -1268,16 +1268,16 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>6.88</v>
+        <v>6.55</v>
       </c>
       <c r="E31" t="n">
-        <v>2008088814</v>
+        <v>1917984094</v>
       </c>
       <c r="F31" t="n">
-        <v>122999552</v>
+        <v>64769227</v>
       </c>
       <c r="G31" t="n">
-        <v>-1.17377</v>
+        <v>-0.91562</v>
       </c>
     </row>
     <row r="32">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.04795734</v>
+        <v>0.04690354</v>
       </c>
       <c r="E32" t="n">
-        <v>1603977505</v>
+        <v>1570965561</v>
       </c>
       <c r="F32" t="n">
-        <v>19266014</v>
+        <v>19818919</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.80767</v>
+        <v>0.26215</v>
       </c>
     </row>
     <row r="33">
@@ -1322,16 +1322,16 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>3.42</v>
+        <v>3.2</v>
       </c>
       <c r="E33" t="n">
-        <v>1555539778</v>
+        <v>1468035047</v>
       </c>
       <c r="F33" t="n">
-        <v>67793600</v>
+        <v>34954945</v>
       </c>
       <c r="G33" t="n">
-        <v>1.56894</v>
+        <v>-0.08821</v>
       </c>
     </row>
     <row r="34">
@@ -1349,16 +1349,16 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>1.57</v>
+        <v>1.6</v>
       </c>
       <c r="E34" t="n">
-        <v>1394637434</v>
+        <v>1421785067</v>
       </c>
       <c r="F34" t="n">
-        <v>20067004</v>
+        <v>14852466</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.24166</v>
+        <v>0.45377</v>
       </c>
     </row>
     <row r="35">
@@ -1376,16 +1376,16 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>3.07</v>
+        <v>3.16</v>
       </c>
       <c r="E35" t="n">
-        <v>1366329278</v>
+        <v>1415363775</v>
       </c>
       <c r="F35" t="n">
-        <v>12142992</v>
+        <v>24730898</v>
       </c>
       <c r="G35" t="n">
-        <v>-1.70944</v>
+        <v>2.09883</v>
       </c>
     </row>
     <row r="36">
@@ -1403,16 +1403,16 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.050046</v>
+        <v>0.051391</v>
       </c>
       <c r="E36" t="n">
-        <v>1316610464</v>
+        <v>1353443301</v>
       </c>
       <c r="F36" t="n">
-        <v>3075579</v>
+        <v>3633620</v>
       </c>
       <c r="G36" t="n">
-        <v>-1.01384</v>
+        <v>-0.59581</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>87.52</v>
+        <v>1417.72</v>
       </c>
       <c r="E37" t="n">
-        <v>1273274244</v>
+        <v>1276913760</v>
       </c>
       <c r="F37" t="n">
-        <v>7477937</v>
+        <v>37041590</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.22121</v>
+        <v>0.91169</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1383.35</v>
+        <v>86.12</v>
       </c>
       <c r="E38" t="n">
-        <v>1246758994</v>
+        <v>1252838514</v>
       </c>
       <c r="F38" t="n">
-        <v>43444629</v>
+        <v>9424440</v>
       </c>
       <c r="G38" t="n">
-        <v>-2.18273</v>
+        <v>-0.86638</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>5.21</v>
+        <v>0.01656644</v>
       </c>
       <c r="E39" t="n">
-        <v>1246109881</v>
+        <v>1204534632</v>
       </c>
       <c r="F39" t="n">
-        <v>26570343</v>
+        <v>24668204</v>
       </c>
       <c r="G39" t="n">
-        <v>-1.4916</v>
+        <v>0.5394</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.01694127</v>
+        <v>4.89</v>
       </c>
       <c r="E40" t="n">
-        <v>1230520110</v>
+        <v>1195886411</v>
       </c>
       <c r="F40" t="n">
-        <v>22302401</v>
+        <v>29687707</v>
       </c>
       <c r="G40" t="n">
-        <v>0.09877</v>
+        <v>-0.6807299999999999</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.382248</v>
+        <v>1.2</v>
       </c>
       <c r="E41" t="n">
-        <v>1221536771</v>
+        <v>1055268557</v>
       </c>
       <c r="F41" t="n">
-        <v>21499108</v>
+        <v>37201743</v>
       </c>
       <c r="G41" t="n">
-        <v>-2.82987</v>
+        <v>-0.41282</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1.27</v>
+        <v>0.803496</v>
       </c>
       <c r="E42" t="n">
-        <v>1109907699</v>
+        <v>1024802318</v>
       </c>
       <c r="F42" t="n">
-        <v>60650998</v>
+        <v>45444086</v>
       </c>
       <c r="G42" t="n">
-        <v>-2.46999</v>
+        <v>-0.16054</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.843456</v>
+        <v>1.017</v>
       </c>
       <c r="E43" t="n">
-        <v>1075061997</v>
+        <v>1002174436</v>
       </c>
       <c r="F43" t="n">
-        <v>68572422</v>
+        <v>28109989</v>
       </c>
       <c r="G43" t="n">
-        <v>-4.45274</v>
+        <v>0.58691</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1.08</v>
+        <v>0.322835</v>
       </c>
       <c r="E44" t="n">
-        <v>1054859374</v>
+        <v>1001508467</v>
       </c>
       <c r="F44" t="n">
-        <v>26602837</v>
+        <v>26859380</v>
       </c>
       <c r="G44" t="n">
-        <v>-1.27591</v>
+        <v>-0.89456</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>AAVE</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Aave</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.04888521</v>
+        <v>63.94</v>
       </c>
       <c r="E45" t="n">
-        <v>1028373473</v>
+        <v>932703645</v>
       </c>
       <c r="F45" t="n">
-        <v>9156830</v>
+        <v>39716994</v>
       </c>
       <c r="G45" t="n">
-        <v>-3.48943</v>
+        <v>-0.44775</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>AAVE</t>
+          <t>RETH</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Aave</t>
+          <t>Rocket Pool ETH</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>65.5</v>
+        <v>1691.63</v>
       </c>
       <c r="E46" t="n">
-        <v>955582001</v>
+        <v>907461020</v>
       </c>
       <c r="F46" t="n">
-        <v>55199316</v>
+        <v>4276457</v>
       </c>
       <c r="G46" t="n">
-        <v>-1.9766</v>
+        <v>0.55769</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>RETH</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Rocket Pool ETH</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>1756.3</v>
+        <v>0.04282639</v>
       </c>
       <c r="E47" t="n">
-        <v>936515414</v>
+        <v>903409493</v>
       </c>
       <c r="F47" t="n">
-        <v>8380306</v>
+        <v>6053272</v>
       </c>
       <c r="G47" t="n">
-        <v>-1.19005</v>
+        <v>-0.34977</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ALGO</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Algorand</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.100913</v>
+        <v>0.082245</v>
       </c>
       <c r="E48" t="n">
-        <v>798367111</v>
+        <v>760500385</v>
       </c>
       <c r="F48" t="n">
-        <v>26889711</v>
+        <v>15582143</v>
       </c>
       <c r="G48" t="n">
-        <v>0.76251</v>
+        <v>1.16705</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>ALGO</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Algorand</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.08459999999999999</v>
+        <v>0.09535100000000001</v>
       </c>
       <c r="E49" t="n">
-        <v>781364370</v>
+        <v>756286461</v>
       </c>
       <c r="F49" t="n">
-        <v>15997145</v>
+        <v>18430589</v>
       </c>
       <c r="G49" t="n">
-        <v>-1.06353</v>
+        <v>0.09649000000000001</v>
       </c>
     </row>
     <row r="50">
@@ -1781,16 +1781,16 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>5.17</v>
+        <v>5.09</v>
       </c>
       <c r="E50" t="n">
-        <v>756728465</v>
+        <v>733969660</v>
       </c>
       <c r="F50" t="n">
-        <v>3988397</v>
+        <v>9486386</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.2926</v>
+        <v>1.56067</v>
       </c>
     </row>
     <row r="51">
@@ -1808,16 +1808,16 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.999309</v>
+        <v>1.001</v>
       </c>
       <c r="E51" t="n">
-        <v>728779070</v>
+        <v>726907273</v>
       </c>
       <c r="F51" t="n">
-        <v>21387464</v>
+        <v>42838119</v>
       </c>
       <c r="G51" t="n">
-        <v>-0.07804999999999999</v>
+        <v>0.1704</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-10-22
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>26831</v>
+        <v>29957</v>
       </c>
       <c r="E2" t="n">
-        <v>523778156497</v>
+        <v>584808995221</v>
       </c>
       <c r="F2" t="n">
-        <v>5423976183</v>
+        <v>10849693265</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.09397</v>
+        <v>0.65991</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1554.14</v>
+        <v>1632.8</v>
       </c>
       <c r="E3" t="n">
-        <v>186950386334</v>
+        <v>196053085743</v>
       </c>
       <c r="F3" t="n">
-        <v>2456993720</v>
+        <v>8864498457</v>
       </c>
       <c r="G3" t="n">
-        <v>0.48933</v>
+        <v>1.63451</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999956</v>
+        <v>1.001</v>
       </c>
       <c r="E4" t="n">
-        <v>83523310091</v>
+        <v>84206193325</v>
       </c>
       <c r="F4" t="n">
-        <v>8866877614</v>
+        <v>20825028473</v>
       </c>
       <c r="G4" t="n">
-        <v>0.01701</v>
+        <v>0.08513999999999999</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>206.87</v>
+        <v>214.51</v>
       </c>
       <c r="E5" t="n">
-        <v>31846892603</v>
+        <v>33004927207</v>
       </c>
       <c r="F5" t="n">
-        <v>202274670</v>
+        <v>315721272</v>
       </c>
       <c r="G5" t="n">
-        <v>0.51519</v>
+        <v>0.72909</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.486281</v>
+        <v>0.517364</v>
       </c>
       <c r="E6" t="n">
-        <v>25991088961</v>
+        <v>27633664259</v>
       </c>
       <c r="F6" t="n">
-        <v>282398047</v>
+        <v>780442138</v>
       </c>
       <c r="G6" t="n">
-        <v>0.12439</v>
+        <v>0.1232</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.999383</v>
+        <v>1.001</v>
       </c>
       <c r="E7" t="n">
-        <v>25111780254</v>
+        <v>25574900868</v>
       </c>
       <c r="F7" t="n">
-        <v>2408120721</v>
+        <v>3849453521</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.07718</v>
+        <v>0.15668</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1554.33</v>
+        <v>1630.58</v>
       </c>
       <c r="E8" t="n">
-        <v>13711685780</v>
+        <v>14394544085</v>
       </c>
       <c r="F8" t="n">
-        <v>15178326</v>
+        <v>5090755</v>
       </c>
       <c r="G8" t="n">
-        <v>0.49134</v>
+        <v>1.55775</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>21.79</v>
+        <v>28.53</v>
       </c>
       <c r="E9" t="n">
-        <v>9079614066</v>
+        <v>11834165412</v>
       </c>
       <c r="F9" t="n">
-        <v>160621207</v>
+        <v>1100945229</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.46341</v>
+        <v>-2.58965</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.246233</v>
+        <v>0.258067</v>
       </c>
       <c r="E10" t="n">
-        <v>8595337336</v>
+        <v>9008125407</v>
       </c>
       <c r="F10" t="n">
-        <v>76973323</v>
+        <v>154301151</v>
       </c>
       <c r="G10" t="n">
-        <v>0.00062</v>
+        <v>0.4562</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.059116</v>
+        <v>0.060826</v>
       </c>
       <c r="E11" t="n">
-        <v>8369733123</v>
+        <v>8599337024</v>
       </c>
       <c r="F11" t="n">
-        <v>147973120</v>
+        <v>257674055</v>
       </c>
       <c r="G11" t="n">
-        <v>0.45077</v>
+        <v>0.69101</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.08538</v>
+        <v>0.090682</v>
       </c>
       <c r="E12" t="n">
-        <v>7596548689</v>
+        <v>8050993822</v>
       </c>
       <c r="F12" t="n">
-        <v>200737055</v>
+        <v>239012195</v>
       </c>
       <c r="G12" t="n">
-        <v>0.03473</v>
+        <v>0.07381</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1.92</v>
+        <v>2.19</v>
       </c>
       <c r="E13" t="n">
-        <v>6628379109</v>
+        <v>7467835445</v>
       </c>
       <c r="F13" t="n">
-        <v>13710188</v>
+        <v>11540544</v>
       </c>
       <c r="G13" t="n">
-        <v>-1.0927</v>
+        <v>3.96587</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>3.73</v>
+        <v>0.562612</v>
       </c>
       <c r="E14" t="n">
-        <v>4798308944</v>
+        <v>5226864715</v>
       </c>
       <c r="F14" t="n">
-        <v>67436843</v>
+        <v>288390118</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.05501</v>
+        <v>1.07601</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.515084</v>
+        <v>9.16</v>
       </c>
       <c r="E15" t="n">
-        <v>4791926070</v>
+        <v>5103687268</v>
       </c>
       <c r="F15" t="n">
-        <v>93527363</v>
+        <v>1433618634</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.3185</v>
+        <v>12.96827</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>61.46</v>
+        <v>3.85</v>
       </c>
       <c r="E16" t="n">
-        <v>4534635047</v>
+        <v>4943845852</v>
       </c>
       <c r="F16" t="n">
-        <v>145957665</v>
+        <v>163364869</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.04898</v>
+        <v>1.25749</v>
       </c>
     </row>
     <row r="17">
@@ -890,21 +890,21 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>26817</v>
+        <v>29947</v>
       </c>
       <c r="E17" t="n">
-        <v>4371497770</v>
+        <v>4878864838</v>
       </c>
       <c r="F17" t="n">
-        <v>27278860</v>
+        <v>166556288</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.17271</v>
+        <v>0.70744</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -917,43 +917,43 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>213.45</v>
+        <v>241.89</v>
       </c>
       <c r="E18" t="n">
-        <v>4170310656</v>
+        <v>4726605181</v>
       </c>
       <c r="F18" t="n">
-        <v>67161082</v>
+        <v>259004248</v>
       </c>
       <c r="G18" t="n">
-        <v>-1.15309</v>
+        <v>-0.13808</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>6.99e-06</v>
+        <v>64.16</v>
       </c>
       <c r="E19" t="n">
-        <v>4120307764</v>
+        <v>4725106929</v>
       </c>
       <c r="F19" t="n">
-        <v>73670495</v>
+        <v>367994420</v>
       </c>
       <c r="G19" t="n">
-        <v>-1.85399</v>
+        <v>-0.18957</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>7.34</v>
+        <v>7e-06</v>
       </c>
       <c r="E20" t="n">
-        <v>4089650602</v>
+        <v>4124028390</v>
       </c>
       <c r="F20" t="n">
-        <v>108370812</v>
+        <v>105502611</v>
       </c>
       <c r="G20" t="n">
-        <v>1.35632</v>
+        <v>0.04033</v>
       </c>
     </row>
     <row r="21">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.999561</v>
+        <v>0.999839</v>
       </c>
       <c r="E21" t="n">
-        <v>3783747143</v>
+        <v>3807741408</v>
       </c>
       <c r="F21" t="n">
-        <v>40242195</v>
+        <v>117659311</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.01461</v>
+        <v>0.10244</v>
       </c>
     </row>
     <row r="22">
@@ -1025,16 +1025,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>3.81</v>
+        <v>3.83</v>
       </c>
       <c r="E22" t="n">
-        <v>3536976356</v>
+        <v>3593981215</v>
       </c>
       <c r="F22" t="n">
-        <v>171107</v>
+        <v>244056</v>
       </c>
       <c r="G22" t="n">
-        <v>2.12704</v>
+        <v>0.01329</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.999133</v>
+        <v>9.75</v>
       </c>
       <c r="E23" t="n">
-        <v>3366138724</v>
+        <v>3460709312</v>
       </c>
       <c r="F23" t="n">
-        <v>56196315</v>
+        <v>256660296</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.00339</v>
+        <v>2.32995</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>TUSD</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>9.1</v>
+        <v>0.9987740000000001</v>
       </c>
       <c r="E24" t="n">
-        <v>3231314749</v>
+        <v>3363082850</v>
       </c>
       <c r="F24" t="n">
-        <v>79655091</v>
+        <v>216297492</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.82112</v>
+        <v>-0.05971</v>
       </c>
     </row>
     <row r="25">
@@ -1106,16 +1106,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>4.11</v>
+        <v>4.13</v>
       </c>
       <c r="E25" t="n">
-        <v>3097965772</v>
+        <v>3107938437</v>
       </c>
       <c r="F25" t="n">
-        <v>36833040</v>
+        <v>101989244</v>
       </c>
       <c r="G25" t="n">
-        <v>0.81024</v>
+        <v>2.31216</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.104614</v>
+        <v>0.109592</v>
       </c>
       <c r="E26" t="n">
-        <v>2906201000</v>
+        <v>3042204571</v>
       </c>
       <c r="F26" t="n">
-        <v>37239204</v>
+        <v>79748345</v>
       </c>
       <c r="G26" t="n">
-        <v>0.8154400000000001</v>
+        <v>0.38027</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>152.63</v>
+        <v>157.82</v>
       </c>
       <c r="E27" t="n">
-        <v>2772332911</v>
+        <v>2878984486</v>
       </c>
       <c r="F27" t="n">
-        <v>33984604</v>
+        <v>67192067</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.21978</v>
+        <v>0.92359</v>
       </c>
     </row>
     <row r="28">
@@ -1187,16 +1187,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>43.06</v>
+        <v>43.66</v>
       </c>
       <c r="E28" t="n">
-        <v>2584193964</v>
+        <v>2619542072</v>
       </c>
       <c r="F28" t="n">
-        <v>2063446</v>
+        <v>6072831</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.40202</v>
+        <v>-0.32057</v>
       </c>
     </row>
     <row r="29">
@@ -1214,16 +1214,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>14.9</v>
+        <v>15.5</v>
       </c>
       <c r="E29" t="n">
-        <v>2134682284</v>
+        <v>2217780253</v>
       </c>
       <c r="F29" t="n">
-        <v>37499873</v>
+        <v>101375393</v>
       </c>
       <c r="G29" t="n">
-        <v>0.14464</v>
+        <v>-0.22062</v>
       </c>
     </row>
     <row r="30">
@@ -1244,13 +1244,13 @@
         <v>1</v>
       </c>
       <c r="E30" t="n">
-        <v>2124771813</v>
+        <v>2094650385</v>
       </c>
       <c r="F30" t="n">
-        <v>951097462</v>
+        <v>2515079753</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.01297</v>
+        <v>-0.03057</v>
       </c>
     </row>
     <row r="31">
@@ -1268,16 +1268,16 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>6.55</v>
+        <v>6.6</v>
       </c>
       <c r="E31" t="n">
-        <v>1917984094</v>
+        <v>1931582900</v>
       </c>
       <c r="F31" t="n">
-        <v>64769227</v>
+        <v>124031551</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.91562</v>
+        <v>1.95326</v>
       </c>
     </row>
     <row r="32">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.04690354</v>
+        <v>0.04868511</v>
       </c>
       <c r="E32" t="n">
-        <v>1570965561</v>
+        <v>1628148619</v>
       </c>
       <c r="F32" t="n">
-        <v>19818919</v>
+        <v>40929832</v>
       </c>
       <c r="G32" t="n">
-        <v>0.26215</v>
+        <v>1.25622</v>
       </c>
     </row>
     <row r="33">
@@ -1322,16 +1322,16 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>3.2</v>
+        <v>3.37</v>
       </c>
       <c r="E33" t="n">
-        <v>1468035047</v>
+        <v>1545506907</v>
       </c>
       <c r="F33" t="n">
-        <v>34954945</v>
+        <v>135260877</v>
       </c>
       <c r="G33" t="n">
-        <v>-0.08821</v>
+        <v>3.91071</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>1.6</v>
+        <v>6.1</v>
       </c>
       <c r="E34" t="n">
-        <v>1421785067</v>
+        <v>1501761414</v>
       </c>
       <c r="F34" t="n">
-        <v>14852466</v>
+        <v>451877110</v>
       </c>
       <c r="G34" t="n">
-        <v>0.45377</v>
+        <v>17.29901</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>3.16</v>
+        <v>1.65</v>
       </c>
       <c r="E35" t="n">
-        <v>1415363775</v>
+        <v>1464195804</v>
       </c>
       <c r="F35" t="n">
-        <v>24730898</v>
+        <v>42586699</v>
       </c>
       <c r="G35" t="n">
-        <v>2.09883</v>
+        <v>4.74214</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.051391</v>
+        <v>3.17</v>
       </c>
       <c r="E36" t="n">
-        <v>1353443301</v>
+        <v>1416024233</v>
       </c>
       <c r="F36" t="n">
-        <v>3633620</v>
+        <v>17251454</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.59581</v>
+        <v>-0.09295</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1417.72</v>
+        <v>0.052775</v>
       </c>
       <c r="E37" t="n">
-        <v>1276913760</v>
+        <v>1389772735</v>
       </c>
       <c r="F37" t="n">
-        <v>37041590</v>
+        <v>5888898</v>
       </c>
       <c r="G37" t="n">
-        <v>0.91169</v>
+        <v>0.31882</v>
       </c>
     </row>
     <row r="38">
@@ -1457,16 +1457,16 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>86.12</v>
+        <v>90.17</v>
       </c>
       <c r="E38" t="n">
-        <v>1252838514</v>
+        <v>1311303058</v>
       </c>
       <c r="F38" t="n">
-        <v>9424440</v>
+        <v>20762406</v>
       </c>
       <c r="G38" t="n">
-        <v>-0.86638</v>
+        <v>3.75501</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.01656644</v>
+        <v>1426.64</v>
       </c>
       <c r="E39" t="n">
-        <v>1204534632</v>
+        <v>1283850151</v>
       </c>
       <c r="F39" t="n">
-        <v>24668204</v>
+        <v>46788514</v>
       </c>
       <c r="G39" t="n">
-        <v>0.5394</v>
+        <v>-0.02245</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>4.89</v>
+        <v>0.0168811</v>
       </c>
       <c r="E40" t="n">
-        <v>1195886411</v>
+        <v>1226940730</v>
       </c>
       <c r="F40" t="n">
-        <v>29687707</v>
+        <v>34526179</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.6807299999999999</v>
+        <v>-0.28323</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1.2</v>
+        <v>0.382322</v>
       </c>
       <c r="E41" t="n">
-        <v>1055268557</v>
+        <v>1185564412</v>
       </c>
       <c r="F41" t="n">
-        <v>37201743</v>
+        <v>39905135</v>
       </c>
       <c r="G41" t="n">
-        <v>-0.41282</v>
+        <v>1.28823</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.803496</v>
+        <v>1.26</v>
       </c>
       <c r="E42" t="n">
-        <v>1024802318</v>
+        <v>1105751472</v>
       </c>
       <c r="F42" t="n">
-        <v>45444086</v>
+        <v>80085346</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.16054</v>
+        <v>0.86395</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>AAVE</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Aave</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1.017</v>
+        <v>75.64</v>
       </c>
       <c r="E43" t="n">
-        <v>1002174436</v>
+        <v>1101568659</v>
       </c>
       <c r="F43" t="n">
-        <v>28109989</v>
+        <v>268628968</v>
       </c>
       <c r="G43" t="n">
-        <v>0.58691</v>
+        <v>11.96005</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.322835</v>
+        <v>0.826438</v>
       </c>
       <c r="E44" t="n">
-        <v>1001508467</v>
+        <v>1053330801</v>
       </c>
       <c r="F44" t="n">
-        <v>26859380</v>
+        <v>154914980</v>
       </c>
       <c r="G44" t="n">
-        <v>-0.89456</v>
+        <v>0.54126</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>AAVE</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Aave</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>63.94</v>
+        <v>0.04892129</v>
       </c>
       <c r="E45" t="n">
-        <v>932703645</v>
+        <v>1038032171</v>
       </c>
       <c r="F45" t="n">
-        <v>39716994</v>
+        <v>12762572</v>
       </c>
       <c r="G45" t="n">
-        <v>-0.44775</v>
+        <v>-1.44755</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>RETH</t>
+          <t>BSV</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Rocket Pool ETH</t>
+          <t>Bitcoin SV</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>1691.63</v>
+        <v>51.94</v>
       </c>
       <c r="E46" t="n">
-        <v>907461020</v>
+        <v>1014313569</v>
       </c>
       <c r="F46" t="n">
-        <v>4276457</v>
+        <v>147757498</v>
       </c>
       <c r="G46" t="n">
-        <v>0.55769</v>
+        <v>-6.68381</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.04282639</v>
+        <v>1.03</v>
       </c>
       <c r="E47" t="n">
-        <v>903409493</v>
+        <v>1013833104</v>
       </c>
       <c r="F47" t="n">
-        <v>6053272</v>
+        <v>52755402</v>
       </c>
       <c r="G47" t="n">
-        <v>-0.34977</v>
+        <v>0.73341</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>RETH</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Rocket Pool ETH</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.082245</v>
+        <v>1768.61</v>
       </c>
       <c r="E48" t="n">
-        <v>760500385</v>
+        <v>948879933</v>
       </c>
       <c r="F48" t="n">
-        <v>15582143</v>
+        <v>16197010</v>
       </c>
       <c r="G48" t="n">
-        <v>1.16705</v>
+        <v>1.3773</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ALGO</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Algorand</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.09535100000000001</v>
+        <v>0.620717</v>
       </c>
       <c r="E49" t="n">
-        <v>756286461</v>
+        <v>877865760</v>
       </c>
       <c r="F49" t="n">
-        <v>18430589</v>
+        <v>48132465</v>
       </c>
       <c r="G49" t="n">
-        <v>0.09649000000000001</v>
+        <v>-4.11212</v>
       </c>
     </row>
     <row r="50">
@@ -1781,16 +1781,16 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>5.09</v>
+        <v>5.38</v>
       </c>
       <c r="E50" t="n">
-        <v>733969660</v>
+        <v>775002566</v>
       </c>
       <c r="F50" t="n">
-        <v>9486386</v>
+        <v>7474904</v>
       </c>
       <c r="G50" t="n">
-        <v>1.56067</v>
+        <v>0.57728</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>USDD</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>USDD</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>1.001</v>
+        <v>0.08258799999999999</v>
       </c>
       <c r="E51" t="n">
-        <v>726907273</v>
+        <v>764581909</v>
       </c>
       <c r="F51" t="n">
-        <v>42838119</v>
+        <v>32318616</v>
       </c>
       <c r="G51" t="n">
-        <v>0.1704</v>
+        <v>1.02293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-10-29
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>29957</v>
+        <v>34312</v>
       </c>
       <c r="E2" t="n">
-        <v>584808995221</v>
+        <v>670427960957</v>
       </c>
       <c r="F2" t="n">
-        <v>10849693265</v>
+        <v>7289511810</v>
       </c>
       <c r="G2" t="n">
-        <v>0.65991</v>
+        <v>0.52088</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1632.8</v>
+        <v>1790</v>
       </c>
       <c r="E3" t="n">
-        <v>196053085743</v>
+        <v>215363841937</v>
       </c>
       <c r="F3" t="n">
-        <v>8864498457</v>
+        <v>5305371011</v>
       </c>
       <c r="G3" t="n">
-        <v>1.63451</v>
+        <v>0.29337</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1.001</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>84206193325</v>
+        <v>84618317471</v>
       </c>
       <c r="F4" t="n">
-        <v>20825028473</v>
+        <v>13296117472</v>
       </c>
       <c r="G4" t="n">
-        <v>0.08513999999999999</v>
+        <v>-0.02686</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>214.51</v>
+        <v>226.19</v>
       </c>
       <c r="E5" t="n">
-        <v>33004927207</v>
+        <v>34800995032</v>
       </c>
       <c r="F5" t="n">
-        <v>315721272</v>
+        <v>266714652</v>
       </c>
       <c r="G5" t="n">
-        <v>0.72909</v>
+        <v>0.09859999999999999</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.517364</v>
+        <v>0.556534</v>
       </c>
       <c r="E6" t="n">
-        <v>27633664259</v>
+        <v>29786263009</v>
       </c>
       <c r="F6" t="n">
-        <v>780442138</v>
+        <v>567077708</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1232</v>
+        <v>1.88312</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1.001</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>25574900868</v>
+        <v>24989383116</v>
       </c>
       <c r="F7" t="n">
-        <v>3849453521</v>
+        <v>2972893263</v>
       </c>
       <c r="G7" t="n">
-        <v>0.15668</v>
+        <v>0.07561</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1630.58</v>
+        <v>1789.78</v>
       </c>
       <c r="E8" t="n">
-        <v>14394544085</v>
+        <v>15732806790</v>
       </c>
       <c r="F8" t="n">
-        <v>5090755</v>
+        <v>4009453</v>
       </c>
       <c r="G8" t="n">
-        <v>1.55775</v>
+        <v>0.262</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>28.53</v>
+        <v>32.23</v>
       </c>
       <c r="E9" t="n">
-        <v>11834165412</v>
+        <v>13511907624</v>
       </c>
       <c r="F9" t="n">
-        <v>1100945229</v>
+        <v>461434586</v>
       </c>
       <c r="G9" t="n">
-        <v>-2.58965</v>
+        <v>0.94301</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.258067</v>
+        <v>0.295553</v>
       </c>
       <c r="E10" t="n">
-        <v>9008125407</v>
+        <v>10330747553</v>
       </c>
       <c r="F10" t="n">
-        <v>154301151</v>
+        <v>121520297</v>
       </c>
       <c r="G10" t="n">
-        <v>0.4562</v>
+        <v>1.32929</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.060826</v>
+        <v>0.068906</v>
       </c>
       <c r="E11" t="n">
-        <v>8599337024</v>
+        <v>9762582123</v>
       </c>
       <c r="F11" t="n">
-        <v>257674055</v>
+        <v>254676570</v>
       </c>
       <c r="G11" t="n">
-        <v>0.69101</v>
+        <v>-0.03868</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.090682</v>
+        <v>0.09482599999999999</v>
       </c>
       <c r="E12" t="n">
-        <v>8050993822</v>
+        <v>8429182348</v>
       </c>
       <c r="F12" t="n">
-        <v>239012195</v>
+        <v>180000698</v>
       </c>
       <c r="G12" t="n">
-        <v>0.07381</v>
+        <v>0.5876</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2.19</v>
+        <v>2.06</v>
       </c>
       <c r="E13" t="n">
-        <v>7467835445</v>
+        <v>7124038571</v>
       </c>
       <c r="F13" t="n">
-        <v>11540544</v>
+        <v>5748835</v>
       </c>
       <c r="G13" t="n">
-        <v>3.96587</v>
+        <v>0.88487</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.562612</v>
+        <v>10.96</v>
       </c>
       <c r="E14" t="n">
-        <v>5226864715</v>
+        <v>6093250598</v>
       </c>
       <c r="F14" t="n">
-        <v>288390118</v>
+        <v>452217852</v>
       </c>
       <c r="G14" t="n">
-        <v>1.07601</v>
+        <v>-2.31299</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>9.16</v>
+        <v>0.626914</v>
       </c>
       <c r="E15" t="n">
-        <v>5103687268</v>
+        <v>5799087071</v>
       </c>
       <c r="F15" t="n">
-        <v>1433618634</v>
+        <v>127574608</v>
       </c>
       <c r="G15" t="n">
-        <v>12.96827</v>
+        <v>1.23815</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>3.85</v>
+        <v>34304</v>
       </c>
       <c r="E16" t="n">
-        <v>4943845852</v>
+        <v>5622338627</v>
       </c>
       <c r="F16" t="n">
-        <v>163364869</v>
+        <v>70012413</v>
       </c>
       <c r="G16" t="n">
-        <v>1.25749</v>
+        <v>0.50054</v>
       </c>
     </row>
     <row r="17">
@@ -881,79 +881,79 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>29947</v>
+        <v>4.2</v>
       </c>
       <c r="E17" t="n">
-        <v>4878864838</v>
+        <v>5419861274</v>
       </c>
       <c r="F17" t="n">
-        <v>166556288</v>
+        <v>107760588</v>
       </c>
       <c r="G17" t="n">
-        <v>0.70744</v>
+        <v>0.15275</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>241.89</v>
+        <v>68.06</v>
       </c>
       <c r="E18" t="n">
-        <v>4726605181</v>
+        <v>5026013898</v>
       </c>
       <c r="F18" t="n">
-        <v>259004248</v>
+        <v>272887019</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.13808</v>
+        <v>0.19949</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>64.16</v>
+        <v>246.37</v>
       </c>
       <c r="E19" t="n">
-        <v>4725106929</v>
+        <v>4821140562</v>
       </c>
       <c r="F19" t="n">
-        <v>367994420</v>
+        <v>118671321</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.18957</v>
+        <v>0.11192</v>
       </c>
     </row>
     <row r="20">
@@ -971,16 +971,16 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>7e-06</v>
+        <v>8.01e-06</v>
       </c>
       <c r="E20" t="n">
-        <v>4124028390</v>
+        <v>4721249722</v>
       </c>
       <c r="F20" t="n">
-        <v>105502611</v>
+        <v>158580199</v>
       </c>
       <c r="G20" t="n">
-        <v>0.04033</v>
+        <v>2.69355</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.999839</v>
+        <v>10.94</v>
       </c>
       <c r="E21" t="n">
-        <v>3807741408</v>
+        <v>3882843494</v>
       </c>
       <c r="F21" t="n">
-        <v>117659311</v>
+        <v>145213718</v>
       </c>
       <c r="G21" t="n">
-        <v>0.10244</v>
+        <v>1.05547</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>3.83</v>
+        <v>0.998963</v>
       </c>
       <c r="E22" t="n">
-        <v>3593981215</v>
+        <v>3742177861</v>
       </c>
       <c r="F22" t="n">
-        <v>244056</v>
+        <v>73001340</v>
       </c>
       <c r="G22" t="n">
-        <v>0.01329</v>
+        <v>-0.07834000000000001</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>9.75</v>
+        <v>4</v>
       </c>
       <c r="E23" t="n">
-        <v>3460709312</v>
+        <v>3713293536</v>
       </c>
       <c r="F23" t="n">
-        <v>256660296</v>
+        <v>255942</v>
       </c>
       <c r="G23" t="n">
-        <v>2.32995</v>
+        <v>1.02362</v>
       </c>
     </row>
     <row r="24">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.9987740000000001</v>
+        <v>1</v>
       </c>
       <c r="E24" t="n">
-        <v>3363082850</v>
+        <v>3361113405</v>
       </c>
       <c r="F24" t="n">
-        <v>216297492</v>
+        <v>187773264</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.05971</v>
+        <v>-0.00718</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>4.13</v>
+        <v>0.115538</v>
       </c>
       <c r="E25" t="n">
-        <v>3107938437</v>
+        <v>3215715246</v>
       </c>
       <c r="F25" t="n">
-        <v>101989244</v>
+        <v>44207029</v>
       </c>
       <c r="G25" t="n">
-        <v>2.31216</v>
+        <v>1.58621</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.109592</v>
+        <v>4.17</v>
       </c>
       <c r="E26" t="n">
-        <v>3042204571</v>
+        <v>3138489478</v>
       </c>
       <c r="F26" t="n">
-        <v>79748345</v>
+        <v>104711873</v>
       </c>
       <c r="G26" t="n">
-        <v>0.38027</v>
+        <v>1.56608</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>157.82</v>
+        <v>162.21</v>
       </c>
       <c r="E27" t="n">
-        <v>2878984486</v>
+        <v>2944524217</v>
       </c>
       <c r="F27" t="n">
-        <v>67192067</v>
+        <v>57844779</v>
       </c>
       <c r="G27" t="n">
-        <v>0.92359</v>
+        <v>0.66301</v>
       </c>
     </row>
     <row r="28">
@@ -1187,16 +1187,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>43.66</v>
+        <v>44.87</v>
       </c>
       <c r="E28" t="n">
-        <v>2619542072</v>
+        <v>2692308748</v>
       </c>
       <c r="F28" t="n">
-        <v>6072831</v>
+        <v>2594793</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.32057</v>
+        <v>-0.25991</v>
       </c>
     </row>
     <row r="29">
@@ -1214,16 +1214,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>15.5</v>
+        <v>16.35</v>
       </c>
       <c r="E29" t="n">
-        <v>2217780253</v>
+        <v>2342375469</v>
       </c>
       <c r="F29" t="n">
-        <v>101375393</v>
+        <v>86432836</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.22062</v>
+        <v>0.35726</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>1</v>
+        <v>7.17</v>
       </c>
       <c r="E30" t="n">
-        <v>2094650385</v>
+        <v>2098086872</v>
       </c>
       <c r="F30" t="n">
-        <v>2515079753</v>
+        <v>77202991</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.03057</v>
+        <v>0.33921</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>6.6</v>
+        <v>1.001</v>
       </c>
       <c r="E31" t="n">
-        <v>1931582900</v>
+        <v>2057461892</v>
       </c>
       <c r="F31" t="n">
-        <v>124031551</v>
+        <v>1089222194</v>
       </c>
       <c r="G31" t="n">
-        <v>1.95326</v>
+        <v>-0.02034</v>
       </c>
     </row>
     <row r="32">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.04868511</v>
+        <v>0.05198</v>
       </c>
       <c r="E32" t="n">
-        <v>1628148619</v>
+        <v>1743188688</v>
       </c>
       <c r="F32" t="n">
-        <v>40929832</v>
+        <v>28586125</v>
       </c>
       <c r="G32" t="n">
-        <v>1.25622</v>
+        <v>0.18661</v>
       </c>
     </row>
     <row r="33">
@@ -1322,16 +1322,16 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>3.37</v>
+        <v>3.77</v>
       </c>
       <c r="E33" t="n">
-        <v>1545506907</v>
+        <v>1742400804</v>
       </c>
       <c r="F33" t="n">
-        <v>135260877</v>
+        <v>81970210</v>
       </c>
       <c r="G33" t="n">
-        <v>3.91071</v>
+        <v>2.91673</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>6.1</v>
+        <v>3.9</v>
       </c>
       <c r="E34" t="n">
-        <v>1501761414</v>
+        <v>1737586813</v>
       </c>
       <c r="F34" t="n">
-        <v>451877110</v>
+        <v>36349825</v>
       </c>
       <c r="G34" t="n">
-        <v>17.29901</v>
+        <v>7.81084</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1.65</v>
+        <v>6.68</v>
       </c>
       <c r="E35" t="n">
-        <v>1464195804</v>
+        <v>1651969900</v>
       </c>
       <c r="F35" t="n">
-        <v>42586699</v>
+        <v>83649689</v>
       </c>
       <c r="G35" t="n">
-        <v>4.74214</v>
+        <v>0.19053</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>3.17</v>
+        <v>1.81</v>
       </c>
       <c r="E36" t="n">
-        <v>1416024233</v>
+        <v>1608679194</v>
       </c>
       <c r="F36" t="n">
-        <v>17251454</v>
+        <v>17415570</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.09295</v>
+        <v>-0.24381</v>
       </c>
     </row>
     <row r="37">
@@ -1430,16 +1430,16 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.052775</v>
+        <v>0.058995</v>
       </c>
       <c r="E37" t="n">
-        <v>1389772735</v>
+        <v>1553667644</v>
       </c>
       <c r="F37" t="n">
-        <v>5888898</v>
+        <v>7224861</v>
       </c>
       <c r="G37" t="n">
-        <v>0.31882</v>
+        <v>-0.81924</v>
       </c>
     </row>
     <row r="38">
@@ -1457,16 +1457,16 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>90.17</v>
+        <v>105.41</v>
       </c>
       <c r="E38" t="n">
-        <v>1311303058</v>
+        <v>1532154903</v>
       </c>
       <c r="F38" t="n">
-        <v>20762406</v>
+        <v>16603066</v>
       </c>
       <c r="G38" t="n">
-        <v>3.75501</v>
+        <v>-2.05444</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1426.64</v>
+        <v>0.01900394</v>
       </c>
       <c r="E39" t="n">
-        <v>1283850151</v>
+        <v>1381922766</v>
       </c>
       <c r="F39" t="n">
-        <v>46788514</v>
+        <v>31984549</v>
       </c>
       <c r="G39" t="n">
-        <v>-0.02245</v>
+        <v>-1.26509</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.0168811</v>
+        <v>1436.92</v>
       </c>
       <c r="E40" t="n">
-        <v>1226940730</v>
+        <v>1296806385</v>
       </c>
       <c r="F40" t="n">
-        <v>34526179</v>
+        <v>68243485</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.28323</v>
+        <v>-0.76574</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.382322</v>
+        <v>1.38</v>
       </c>
       <c r="E41" t="n">
-        <v>1185564412</v>
+        <v>1212599841</v>
       </c>
       <c r="F41" t="n">
-        <v>39905135</v>
+        <v>47806352</v>
       </c>
       <c r="G41" t="n">
-        <v>1.28823</v>
+        <v>0.06126</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1.26</v>
+        <v>1.22</v>
       </c>
       <c r="E42" t="n">
-        <v>1105751472</v>
+        <v>1209576589</v>
       </c>
       <c r="F42" t="n">
-        <v>80085346</v>
+        <v>52886797</v>
       </c>
       <c r="G42" t="n">
-        <v>0.86395</v>
+        <v>0.23659</v>
       </c>
     </row>
     <row r="43">
@@ -1592,16 +1592,16 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>75.64</v>
+        <v>82.09999999999999</v>
       </c>
       <c r="E43" t="n">
-        <v>1101568659</v>
+        <v>1198453475</v>
       </c>
       <c r="F43" t="n">
-        <v>268628968</v>
+        <v>77616671</v>
       </c>
       <c r="G43" t="n">
-        <v>11.96005</v>
+        <v>2.73772</v>
       </c>
     </row>
     <row r="44">
@@ -1619,16 +1619,16 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.826438</v>
+        <v>0.926768</v>
       </c>
       <c r="E44" t="n">
-        <v>1053330801</v>
+        <v>1181616421</v>
       </c>
       <c r="F44" t="n">
-        <v>154914980</v>
+        <v>107877458</v>
       </c>
       <c r="G44" t="n">
-        <v>0.54126</v>
+        <v>0.82775</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.04892129</v>
+        <v>0.379514</v>
       </c>
       <c r="E45" t="n">
-        <v>1038032171</v>
+        <v>1179222082</v>
       </c>
       <c r="F45" t="n">
-        <v>12762572</v>
+        <v>24218652</v>
       </c>
       <c r="G45" t="n">
-        <v>-1.44755</v>
+        <v>0.13123</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>BSV</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Bitcoin SV</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>51.94</v>
+        <v>14.05</v>
       </c>
       <c r="E46" t="n">
-        <v>1014313569</v>
+        <v>1178185684</v>
       </c>
       <c r="F46" t="n">
-        <v>147757498</v>
+        <v>77864110</v>
       </c>
       <c r="G46" t="n">
-        <v>-6.68381</v>
+        <v>5.11589</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>1.03</v>
+        <v>0.051999</v>
       </c>
       <c r="E47" t="n">
-        <v>1013833104</v>
+        <v>1108233448</v>
       </c>
       <c r="F47" t="n">
-        <v>52755402</v>
+        <v>8548916</v>
       </c>
       <c r="G47" t="n">
-        <v>0.73341</v>
+        <v>1.9511</v>
       </c>
     </row>
     <row r="48">
@@ -1727,16 +1727,16 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>1768.61</v>
+        <v>1946.53</v>
       </c>
       <c r="E48" t="n">
-        <v>948879933</v>
+        <v>1042370166</v>
       </c>
       <c r="F48" t="n">
-        <v>16197010</v>
+        <v>5309743</v>
       </c>
       <c r="G48" t="n">
-        <v>1.3773</v>
+        <v>0.04407</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>BSV</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Bitcoin SV</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.620717</v>
+        <v>50.62</v>
       </c>
       <c r="E49" t="n">
-        <v>877865760</v>
+        <v>991091310</v>
       </c>
       <c r="F49" t="n">
-        <v>48132465</v>
+        <v>68993912</v>
       </c>
       <c r="G49" t="n">
-        <v>-4.11212</v>
+        <v>3.44628</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>WBT</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>WhiteBIT Coin</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>5.38</v>
+        <v>2.61</v>
       </c>
       <c r="E50" t="n">
-        <v>775002566</v>
+        <v>974275092</v>
       </c>
       <c r="F50" t="n">
-        <v>7474904</v>
+        <v>102135896</v>
       </c>
       <c r="G50" t="n">
-        <v>0.57728</v>
+        <v>8.50577</v>
       </c>
     </row>
     <row r="51">
@@ -1808,16 +1808,16 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.08258799999999999</v>
+        <v>0.105171</v>
       </c>
       <c r="E51" t="n">
-        <v>764581909</v>
+        <v>972697824</v>
       </c>
       <c r="F51" t="n">
-        <v>32318616</v>
+        <v>46344605</v>
       </c>
       <c r="G51" t="n">
-        <v>1.02293</v>
+        <v>3.43311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-11-05
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>34312</v>
+        <v>35162</v>
       </c>
       <c r="E2" t="n">
-        <v>670427960957</v>
+        <v>687076224789</v>
       </c>
       <c r="F2" t="n">
-        <v>7289511810</v>
+        <v>9734232794</v>
       </c>
       <c r="G2" t="n">
-        <v>0.52088</v>
+        <v>1.26128</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1790</v>
+        <v>1896.57</v>
       </c>
       <c r="E3" t="n">
-        <v>215363841937</v>
+        <v>228059391070</v>
       </c>
       <c r="F3" t="n">
-        <v>5305371011</v>
+        <v>10608584320</v>
       </c>
       <c r="G3" t="n">
-        <v>0.29337</v>
+        <v>3.14884</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>1.001</v>
       </c>
       <c r="E4" t="n">
-        <v>84618317471</v>
+        <v>85358927601</v>
       </c>
       <c r="F4" t="n">
-        <v>13296117472</v>
+        <v>12373158796</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.02686</v>
+        <v>0.0718</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>226.19</v>
+        <v>244.11</v>
       </c>
       <c r="E5" t="n">
-        <v>34800995032</v>
+        <v>37550287562</v>
       </c>
       <c r="F5" t="n">
-        <v>266714652</v>
+        <v>473599097</v>
       </c>
       <c r="G5" t="n">
-        <v>0.09859999999999999</v>
+        <v>4.02452</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.556534</v>
+        <v>0.64471</v>
       </c>
       <c r="E6" t="n">
-        <v>29786263009</v>
+        <v>34501044249</v>
       </c>
       <c r="F6" t="n">
-        <v>567077708</v>
+        <v>1138004336</v>
       </c>
       <c r="G6" t="n">
-        <v>1.88312</v>
+        <v>5.07296</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0.999987</v>
       </c>
       <c r="E7" t="n">
-        <v>24989383116</v>
+        <v>24562938966</v>
       </c>
       <c r="F7" t="n">
-        <v>2972893263</v>
+        <v>4012060204</v>
       </c>
       <c r="G7" t="n">
-        <v>0.07561</v>
+        <v>0.02933</v>
       </c>
     </row>
     <row r="8">
@@ -638,25 +638,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>STETH</t>
+          <t>SOL</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Lido Staked Ether</t>
+          <t>Solana</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1789.78</v>
+        <v>41.75</v>
       </c>
       <c r="E8" t="n">
-        <v>15732806790</v>
+        <v>17470329514</v>
       </c>
       <c r="F8" t="n">
-        <v>4009453</v>
+        <v>931833435</v>
       </c>
       <c r="G8" t="n">
-        <v>0.262</v>
+        <v>0.81813</v>
       </c>
     </row>
     <row r="9">
@@ -665,25 +665,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>SOL</t>
+          <t>STETH</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Solana</t>
+          <t>Lido Staked Ether</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>32.23</v>
+        <v>1888.27</v>
       </c>
       <c r="E9" t="n">
-        <v>13511907624</v>
+        <v>16756138643</v>
       </c>
       <c r="F9" t="n">
-        <v>461434586</v>
+        <v>7340541</v>
       </c>
       <c r="G9" t="n">
-        <v>0.94301</v>
+        <v>2.56979</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.295553</v>
+        <v>0.344995</v>
       </c>
       <c r="E10" t="n">
-        <v>10330747553</v>
+        <v>12038944621</v>
       </c>
       <c r="F10" t="n">
-        <v>121520297</v>
+        <v>234442875</v>
       </c>
       <c r="G10" t="n">
-        <v>1.32929</v>
+        <v>6.35501</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.068906</v>
+        <v>0.070879</v>
       </c>
       <c r="E11" t="n">
-        <v>9762582123</v>
+        <v>10044238864</v>
       </c>
       <c r="F11" t="n">
-        <v>254676570</v>
+        <v>362071857</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.03868</v>
+        <v>3.24175</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +746,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.09482599999999999</v>
+        <v>2.28</v>
       </c>
       <c r="E12" t="n">
-        <v>8429182348</v>
+        <v>9064058075</v>
       </c>
       <c r="F12" t="n">
-        <v>180000698</v>
+        <v>12010261</v>
       </c>
       <c r="G12" t="n">
-        <v>0.5876</v>
+        <v>1.99037</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2.06</v>
+        <v>0.098971</v>
       </c>
       <c r="E13" t="n">
-        <v>7124038571</v>
+        <v>8769367934</v>
       </c>
       <c r="F13" t="n">
-        <v>5748835</v>
+        <v>209642443</v>
       </c>
       <c r="G13" t="n">
-        <v>0.88487</v>
+        <v>1.23022</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>10.96</v>
+        <v>12.15</v>
       </c>
       <c r="E14" t="n">
-        <v>6093250598</v>
+        <v>6766887160</v>
       </c>
       <c r="F14" t="n">
-        <v>452217852</v>
+        <v>671965452</v>
       </c>
       <c r="G14" t="n">
-        <v>-2.31299</v>
+        <v>7.39234</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.626914</v>
+        <v>0.6961270000000001</v>
       </c>
       <c r="E15" t="n">
-        <v>5799087071</v>
+        <v>6373371461</v>
       </c>
       <c r="F15" t="n">
-        <v>127574608</v>
+        <v>216107257</v>
       </c>
       <c r="G15" t="n">
-        <v>1.23815</v>
+        <v>3.80566</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>34304</v>
+        <v>4.83</v>
       </c>
       <c r="E16" t="n">
-        <v>5622338627</v>
+        <v>6209660529</v>
       </c>
       <c r="F16" t="n">
-        <v>70012413</v>
+        <v>190226600</v>
       </c>
       <c r="G16" t="n">
-        <v>0.50054</v>
+        <v>4.04255</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>4.2</v>
+        <v>35099</v>
       </c>
       <c r="E17" t="n">
-        <v>5419861274</v>
+        <v>5739244211</v>
       </c>
       <c r="F17" t="n">
-        <v>107760588</v>
+        <v>127256614</v>
       </c>
       <c r="G17" t="n">
-        <v>0.15275</v>
+        <v>1.01391</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>68.06</v>
+        <v>71.66</v>
       </c>
       <c r="E18" t="n">
-        <v>5026013898</v>
+        <v>5291206154</v>
       </c>
       <c r="F18" t="n">
-        <v>272887019</v>
+        <v>495598951</v>
       </c>
       <c r="G18" t="n">
-        <v>0.19949</v>
+        <v>2.90199</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>246.37</v>
+        <v>8.17e-06</v>
       </c>
       <c r="E19" t="n">
-        <v>4821140562</v>
+        <v>4800231104</v>
       </c>
       <c r="F19" t="n">
-        <v>118671321</v>
+        <v>167032983</v>
       </c>
       <c r="G19" t="n">
-        <v>0.11192</v>
+        <v>3.75247</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>8.01e-06</v>
+        <v>242.13</v>
       </c>
       <c r="E20" t="n">
-        <v>4721249722</v>
+        <v>4733473724</v>
       </c>
       <c r="F20" t="n">
-        <v>158580199</v>
+        <v>94741860</v>
       </c>
       <c r="G20" t="n">
-        <v>2.69355</v>
+        <v>2.09059</v>
       </c>
     </row>
     <row r="21">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>10.94</v>
+        <v>12.57</v>
       </c>
       <c r="E21" t="n">
-        <v>3882843494</v>
+        <v>4466763899</v>
       </c>
       <c r="F21" t="n">
-        <v>145213718</v>
+        <v>189783815</v>
       </c>
       <c r="G21" t="n">
-        <v>1.05547</v>
+        <v>4.57189</v>
       </c>
     </row>
     <row r="22">
@@ -1025,16 +1025,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.998963</v>
+        <v>0.999287</v>
       </c>
       <c r="E22" t="n">
-        <v>3742177861</v>
+        <v>3722563356</v>
       </c>
       <c r="F22" t="n">
-        <v>73001340</v>
+        <v>117423740</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.07834000000000001</v>
+        <v>0.04194</v>
       </c>
     </row>
     <row r="23">
@@ -1052,16 +1052,16 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>4</v>
+        <v>3.94</v>
       </c>
       <c r="E23" t="n">
-        <v>3713293536</v>
+        <v>3655689501</v>
       </c>
       <c r="F23" t="n">
-        <v>255942</v>
+        <v>534110</v>
       </c>
       <c r="G23" t="n">
-        <v>1.02362</v>
+        <v>-0.64447</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>4.79</v>
       </c>
       <c r="E24" t="n">
-        <v>3361113405</v>
+        <v>3598636704</v>
       </c>
       <c r="F24" t="n">
-        <v>187773264</v>
+        <v>320213940</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.00718</v>
+        <v>1.26873</v>
       </c>
     </row>
     <row r="25">
@@ -1106,16 +1106,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.115538</v>
+        <v>0.126972</v>
       </c>
       <c r="E25" t="n">
-        <v>3215715246</v>
+        <v>3533750066</v>
       </c>
       <c r="F25" t="n">
-        <v>44207029</v>
+        <v>84418258</v>
       </c>
       <c r="G25" t="n">
-        <v>1.58621</v>
+        <v>3.18377</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>TUSD</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>4.17</v>
+        <v>0.999024</v>
       </c>
       <c r="E26" t="n">
-        <v>3138489478</v>
+        <v>3332262803</v>
       </c>
       <c r="F26" t="n">
-        <v>104711873</v>
+        <v>132869399</v>
       </c>
       <c r="G26" t="n">
-        <v>1.56608</v>
+        <v>-0.03853</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>162.21</v>
+        <v>169.47</v>
       </c>
       <c r="E27" t="n">
-        <v>2944524217</v>
+        <v>3073093932</v>
       </c>
       <c r="F27" t="n">
-        <v>57844779</v>
+        <v>53362385</v>
       </c>
       <c r="G27" t="n">
-        <v>0.66301</v>
+        <v>0.24299</v>
       </c>
     </row>
     <row r="28">
@@ -1187,16 +1187,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>44.87</v>
+        <v>48.66</v>
       </c>
       <c r="E28" t="n">
-        <v>2692308748</v>
+        <v>2913254912</v>
       </c>
       <c r="F28" t="n">
-        <v>2594793</v>
+        <v>16979495</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.25991</v>
+        <v>4.78792</v>
       </c>
     </row>
     <row r="29">
@@ -1214,16 +1214,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>16.35</v>
+        <v>18.18</v>
       </c>
       <c r="E29" t="n">
-        <v>2342375469</v>
+        <v>2599938731</v>
       </c>
       <c r="F29" t="n">
-        <v>86432836</v>
+        <v>83208055</v>
       </c>
       <c r="G29" t="n">
-        <v>0.35726</v>
+        <v>4.76539</v>
       </c>
     </row>
     <row r="30">
@@ -1241,16 +1241,16 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>7.17</v>
+        <v>8.390000000000001</v>
       </c>
       <c r="E30" t="n">
-        <v>2098086872</v>
+        <v>2454193351</v>
       </c>
       <c r="F30" t="n">
-        <v>77202991</v>
+        <v>201724445</v>
       </c>
       <c r="G30" t="n">
-        <v>0.33921</v>
+        <v>6.55821</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>1.001</v>
+        <v>4.11</v>
       </c>
       <c r="E31" t="n">
-        <v>2057461892</v>
+        <v>1906661475</v>
       </c>
       <c r="F31" t="n">
-        <v>1089222194</v>
+        <v>115763225</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.02034</v>
+        <v>3.90937</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.05198</v>
+        <v>1</v>
       </c>
       <c r="E32" t="n">
-        <v>1743188688</v>
+        <v>1897531359</v>
       </c>
       <c r="F32" t="n">
-        <v>28586125</v>
+        <v>3235136233</v>
       </c>
       <c r="G32" t="n">
-        <v>0.18661</v>
+        <v>-0.0323</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>3.77</v>
+        <v>0.056376</v>
       </c>
       <c r="E33" t="n">
-        <v>1742400804</v>
+        <v>1890777818</v>
       </c>
       <c r="F33" t="n">
-        <v>81970210</v>
+        <v>25487278</v>
       </c>
       <c r="G33" t="n">
-        <v>2.91673</v>
+        <v>2.65749</v>
       </c>
     </row>
     <row r="34">
@@ -1349,16 +1349,16 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>3.9</v>
+        <v>4.15</v>
       </c>
       <c r="E34" t="n">
-        <v>1737586813</v>
+        <v>1861459510</v>
       </c>
       <c r="F34" t="n">
-        <v>36349825</v>
+        <v>30287938</v>
       </c>
       <c r="G34" t="n">
-        <v>7.81084</v>
+        <v>4.12787</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>6.68</v>
+        <v>0.06884999999999999</v>
       </c>
       <c r="E35" t="n">
-        <v>1651969900</v>
+        <v>1813222675</v>
       </c>
       <c r="F35" t="n">
-        <v>83649689</v>
+        <v>9452427</v>
       </c>
       <c r="G35" t="n">
-        <v>0.19053</v>
+        <v>2.2761</v>
       </c>
     </row>
     <row r="36">
@@ -1403,16 +1403,16 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1.81</v>
+        <v>2.03</v>
       </c>
       <c r="E36" t="n">
-        <v>1608679194</v>
+        <v>1803670925</v>
       </c>
       <c r="F36" t="n">
-        <v>17415570</v>
+        <v>48772634</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.24381</v>
+        <v>1.18192</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.058995</v>
+        <v>7.01</v>
       </c>
       <c r="E37" t="n">
-        <v>1553667644</v>
+        <v>1742531649</v>
       </c>
       <c r="F37" t="n">
-        <v>7224861</v>
+        <v>77872833</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.81924</v>
+        <v>1.4844</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>105.41</v>
+        <v>1.63</v>
       </c>
       <c r="E38" t="n">
-        <v>1532154903</v>
+        <v>1608683341</v>
       </c>
       <c r="F38" t="n">
-        <v>16603066</v>
+        <v>139110282</v>
       </c>
       <c r="G38" t="n">
-        <v>-2.05444</v>
+        <v>9.21252</v>
       </c>
     </row>
     <row r="39">
@@ -1484,16 +1484,16 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.01900394</v>
+        <v>0.02078443</v>
       </c>
       <c r="E39" t="n">
-        <v>1381922766</v>
+        <v>1510140826</v>
       </c>
       <c r="F39" t="n">
-        <v>31984549</v>
+        <v>41336559</v>
       </c>
       <c r="G39" t="n">
-        <v>-1.26509</v>
+        <v>3.69558</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1436.92</v>
+        <v>101.31</v>
       </c>
       <c r="E40" t="n">
-        <v>1296806385</v>
+        <v>1467701750</v>
       </c>
       <c r="F40" t="n">
-        <v>68243485</v>
+        <v>19746836</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.76574</v>
+        <v>1.54054</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1.38</v>
+        <v>1.1</v>
       </c>
       <c r="E41" t="n">
-        <v>1212599841</v>
+        <v>1407878860</v>
       </c>
       <c r="F41" t="n">
-        <v>47806352</v>
+        <v>301587224</v>
       </c>
       <c r="G41" t="n">
-        <v>0.06126</v>
+        <v>3.11647</v>
       </c>
     </row>
     <row r="42">
@@ -1556,30 +1556,30 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1.22</v>
+        <v>1.54</v>
       </c>
       <c r="E42" t="n">
-        <v>1209576589</v>
+        <v>1349299437</v>
       </c>
       <c r="F42" t="n">
-        <v>52886797</v>
+        <v>126616269</v>
       </c>
       <c r="G42" t="n">
-        <v>0.23659</v>
+        <v>6.16335</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -1592,43 +1592,43 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>82.09999999999999</v>
+        <v>91.31</v>
       </c>
       <c r="E43" t="n">
-        <v>1198453475</v>
+        <v>1336074956</v>
       </c>
       <c r="F43" t="n">
-        <v>77616671</v>
+        <v>124207911</v>
       </c>
       <c r="G43" t="n">
-        <v>2.73772</v>
+        <v>0.72412</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.926768</v>
+        <v>0.062127</v>
       </c>
       <c r="E44" t="n">
-        <v>1181616421</v>
+        <v>1329531275</v>
       </c>
       <c r="F44" t="n">
-        <v>107877458</v>
+        <v>44839987</v>
       </c>
       <c r="G44" t="n">
-        <v>0.82775</v>
+        <v>13.29736</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.379514</v>
+        <v>15.65</v>
       </c>
       <c r="E45" t="n">
-        <v>1179222082</v>
+        <v>1311769081</v>
       </c>
       <c r="F45" t="n">
-        <v>24218652</v>
+        <v>68968162</v>
       </c>
       <c r="G45" t="n">
-        <v>0.13123</v>
+        <v>6.78456</v>
       </c>
     </row>
     <row r="46">
@@ -1664,133 +1664,133 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>14.05</v>
+        <v>0.414792</v>
       </c>
       <c r="E46" t="n">
-        <v>1178185684</v>
+        <v>1288338765</v>
       </c>
       <c r="F46" t="n">
-        <v>77864110</v>
+        <v>56708987</v>
       </c>
       <c r="G46" t="n">
-        <v>5.11589</v>
+        <v>1.24488</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>EGLD</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>MultiversX</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.051999</v>
+        <v>46.43</v>
       </c>
       <c r="E47" t="n">
-        <v>1108233448</v>
+        <v>1216981858</v>
       </c>
       <c r="F47" t="n">
-        <v>8548916</v>
+        <v>290287143</v>
       </c>
       <c r="G47" t="n">
-        <v>1.9511</v>
+        <v>37.59187</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>RETH</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Rocket Pool ETH</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>1946.53</v>
+        <v>1339.55</v>
       </c>
       <c r="E48" t="n">
-        <v>1042370166</v>
+        <v>1207352218</v>
       </c>
       <c r="F48" t="n">
-        <v>5309743</v>
+        <v>33851538</v>
       </c>
       <c r="G48" t="n">
-        <v>0.04407</v>
+        <v>0.133</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>BSV</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Bitcoin SV</t>
+          <t>ImmutableX</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>50.62</v>
+        <v>0.951439</v>
       </c>
       <c r="E49" t="n">
-        <v>991091310</v>
+        <v>1190900088</v>
       </c>
       <c r="F49" t="n">
-        <v>68993912</v>
+        <v>770261663</v>
       </c>
       <c r="G49" t="n">
-        <v>3.44628</v>
+        <v>24.78934</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>2.61</v>
+        <v>0.12779</v>
       </c>
       <c r="E50" t="n">
-        <v>974275092</v>
+        <v>1184634620</v>
       </c>
       <c r="F50" t="n">
-        <v>102135896</v>
+        <v>125277039</v>
       </c>
       <c r="G50" t="n">
-        <v>8.50577</v>
+        <v>9.78881</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>RETH</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Rocket Pool ETH</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.105171</v>
+        <v>2072.79</v>
       </c>
       <c r="E51" t="n">
-        <v>972697824</v>
+        <v>1109107345</v>
       </c>
       <c r="F51" t="n">
-        <v>46344605</v>
+        <v>8102440</v>
       </c>
       <c r="G51" t="n">
-        <v>3.43311</v>
+        <v>2.49026</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-11-12
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>35162</v>
+        <v>37040</v>
       </c>
       <c r="E2" t="n">
-        <v>687076224789</v>
+        <v>724605718990</v>
       </c>
       <c r="F2" t="n">
-        <v>9734232794</v>
+        <v>12522762620</v>
       </c>
       <c r="G2" t="n">
-        <v>1.26128</v>
+        <v>-0.16848</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1896.57</v>
+        <v>2041.15</v>
       </c>
       <c r="E3" t="n">
-        <v>228059391070</v>
+        <v>246157223708</v>
       </c>
       <c r="F3" t="n">
-        <v>10608584320</v>
+        <v>11951582315</v>
       </c>
       <c r="G3" t="n">
-        <v>3.14884</v>
+        <v>-1.03607</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1.001</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>85358927601</v>
+        <v>86823534820</v>
       </c>
       <c r="F4" t="n">
-        <v>12373158796</v>
+        <v>34449847337</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0718</v>
+        <v>-0.09526</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>244.11</v>
+        <v>248.65</v>
       </c>
       <c r="E5" t="n">
-        <v>37550287562</v>
+        <v>38317048614</v>
       </c>
       <c r="F5" t="n">
-        <v>473599097</v>
+        <v>879651128</v>
       </c>
       <c r="G5" t="n">
-        <v>4.02452</v>
+        <v>-0.40342</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.64471</v>
+        <v>0.664659</v>
       </c>
       <c r="E6" t="n">
-        <v>34501044249</v>
+        <v>35757221274</v>
       </c>
       <c r="F6" t="n">
-        <v>1138004336</v>
+        <v>1365124642</v>
       </c>
       <c r="G6" t="n">
-        <v>5.07296</v>
+        <v>-1.08723</v>
       </c>
     </row>
     <row r="7">
@@ -611,25 +611,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>USDC</t>
+          <t>SOL</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>USDC</t>
+          <t>Solana</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.999987</v>
+        <v>58.68</v>
       </c>
       <c r="E7" t="n">
-        <v>24562938966</v>
+        <v>25117403863</v>
       </c>
       <c r="F7" t="n">
-        <v>4012060204</v>
+        <v>4628222328</v>
       </c>
       <c r="G7" t="n">
-        <v>0.02933</v>
+        <v>4.41822</v>
       </c>
     </row>
     <row r="8">
@@ -638,25 +638,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SOL</t>
+          <t>USDC</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Solana</t>
+          <t>USDC</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>41.75</v>
+        <v>0.999221</v>
       </c>
       <c r="E8" t="n">
-        <v>17470329514</v>
+        <v>24224936652</v>
       </c>
       <c r="F8" t="n">
-        <v>931833435</v>
+        <v>6413967726</v>
       </c>
       <c r="G8" t="n">
-        <v>0.81813</v>
+        <v>-0.16951</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1888.27</v>
+        <v>2045.19</v>
       </c>
       <c r="E9" t="n">
-        <v>16756138643</v>
+        <v>18343678764</v>
       </c>
       <c r="F9" t="n">
-        <v>7340541</v>
+        <v>12354607</v>
       </c>
       <c r="G9" t="n">
-        <v>2.56979</v>
+        <v>-0.79071</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.344995</v>
+        <v>0.384794</v>
       </c>
       <c r="E10" t="n">
-        <v>12038944621</v>
+        <v>13504796837</v>
       </c>
       <c r="F10" t="n">
-        <v>234442875</v>
+        <v>538761565</v>
       </c>
       <c r="G10" t="n">
-        <v>6.35501</v>
+        <v>1.52594</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.070879</v>
+        <v>0.078669</v>
       </c>
       <c r="E11" t="n">
-        <v>10044238864</v>
+        <v>11209518930</v>
       </c>
       <c r="F11" t="n">
-        <v>362071857</v>
+        <v>1452450603</v>
       </c>
       <c r="G11" t="n">
-        <v>3.24175</v>
+        <v>-1.92124</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +746,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>2.28</v>
+        <v>0.108046</v>
       </c>
       <c r="E12" t="n">
-        <v>9064058075</v>
+        <v>9592159930</v>
       </c>
       <c r="F12" t="n">
-        <v>12010261</v>
+        <v>296989630</v>
       </c>
       <c r="G12" t="n">
-        <v>1.99037</v>
+        <v>1.23702</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.098971</v>
+        <v>15.91</v>
       </c>
       <c r="E13" t="n">
-        <v>8769367934</v>
+        <v>8921358550</v>
       </c>
       <c r="F13" t="n">
-        <v>209642443</v>
+        <v>1392273390</v>
       </c>
       <c r="G13" t="n">
-        <v>1.23022</v>
+        <v>4.70082</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>12.15</v>
+        <v>0.832392</v>
       </c>
       <c r="E14" t="n">
-        <v>6766887160</v>
+        <v>7730131211</v>
       </c>
       <c r="F14" t="n">
-        <v>671965452</v>
+        <v>696743261</v>
       </c>
       <c r="G14" t="n">
-        <v>7.39234</v>
+        <v>2.1093</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.6961270000000001</v>
+        <v>5.77</v>
       </c>
       <c r="E15" t="n">
-        <v>6373371461</v>
+        <v>7507447148</v>
       </c>
       <c r="F15" t="n">
-        <v>216107257</v>
+        <v>536924480</v>
       </c>
       <c r="G15" t="n">
-        <v>3.80566</v>
+        <v>8.306940000000001</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>4.83</v>
+        <v>18.44</v>
       </c>
       <c r="E16" t="n">
-        <v>6209660529</v>
+        <v>6577465473</v>
       </c>
       <c r="F16" t="n">
-        <v>190226600</v>
+        <v>1402997291</v>
       </c>
       <c r="G16" t="n">
-        <v>4.04255</v>
+        <v>29.19223</v>
       </c>
     </row>
     <row r="17">
@@ -890,16 +890,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>35099</v>
+        <v>37045</v>
       </c>
       <c r="E17" t="n">
-        <v>5739244211</v>
+        <v>6068339256</v>
       </c>
       <c r="F17" t="n">
-        <v>127256614</v>
+        <v>229323005</v>
       </c>
       <c r="G17" t="n">
-        <v>1.01391</v>
+        <v>-0.01298</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>71.66</v>
+        <v>75.13</v>
       </c>
       <c r="E18" t="n">
-        <v>5291206154</v>
+        <v>5589109160</v>
       </c>
       <c r="F18" t="n">
-        <v>495598951</v>
+        <v>604310194</v>
       </c>
       <c r="G18" t="n">
-        <v>2.90199</v>
+        <v>0.82397</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>8.17e-06</v>
+        <v>0.998789</v>
       </c>
       <c r="E19" t="n">
-        <v>4800231104</v>
+        <v>5344232878</v>
       </c>
       <c r="F19" t="n">
-        <v>167032983</v>
+        <v>149291487</v>
       </c>
       <c r="G19" t="n">
-        <v>3.75247</v>
+        <v>-0.09699000000000001</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>242.13</v>
+        <v>8.970000000000001e-06</v>
       </c>
       <c r="E20" t="n">
-        <v>4733473724</v>
+        <v>5317565933</v>
       </c>
       <c r="F20" t="n">
-        <v>94741860</v>
+        <v>316725240</v>
       </c>
       <c r="G20" t="n">
-        <v>2.09059</v>
+        <v>-2.31299</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>12.57</v>
+        <v>2.42</v>
       </c>
       <c r="E21" t="n">
-        <v>4466763899</v>
+        <v>5176194300</v>
       </c>
       <c r="F21" t="n">
-        <v>189783815</v>
+        <v>54764374</v>
       </c>
       <c r="G21" t="n">
-        <v>4.57189</v>
+        <v>-0.30984</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.999287</v>
+        <v>236.81</v>
       </c>
       <c r="E22" t="n">
-        <v>3722563356</v>
+        <v>4645632726</v>
       </c>
       <c r="F22" t="n">
-        <v>117423740</v>
+        <v>143715572</v>
       </c>
       <c r="G22" t="n">
-        <v>0.04194</v>
+        <v>-0.36195</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>3.94</v>
+        <v>5.35</v>
       </c>
       <c r="E23" t="n">
-        <v>3655689501</v>
+        <v>4054865364</v>
       </c>
       <c r="F23" t="n">
-        <v>534110</v>
+        <v>168902663</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.64447</v>
+        <v>-0.83385</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>4.79</v>
+        <v>4.09</v>
       </c>
       <c r="E24" t="n">
-        <v>3598636704</v>
+        <v>3797066618</v>
       </c>
       <c r="F24" t="n">
-        <v>320213940</v>
+        <v>1027107</v>
       </c>
       <c r="G24" t="n">
-        <v>1.26873</v>
+        <v>-0.25779</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.126972</v>
+        <v>60.22</v>
       </c>
       <c r="E25" t="n">
-        <v>3533750066</v>
+        <v>3619693066</v>
       </c>
       <c r="F25" t="n">
-        <v>84418258</v>
+        <v>14205455</v>
       </c>
       <c r="G25" t="n">
-        <v>3.18377</v>
+        <v>-1.30488</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.999024</v>
+        <v>0.125533</v>
       </c>
       <c r="E26" t="n">
-        <v>3332262803</v>
+        <v>3520446780</v>
       </c>
       <c r="F26" t="n">
-        <v>132869399</v>
+        <v>117958647</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.03853</v>
+        <v>0.50259</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>TUSD</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>169.47</v>
+        <v>0.997806</v>
       </c>
       <c r="E27" t="n">
-        <v>3073093932</v>
+        <v>3334473511</v>
       </c>
       <c r="F27" t="n">
-        <v>53362385</v>
+        <v>137459642</v>
       </c>
       <c r="G27" t="n">
-        <v>0.24299</v>
+        <v>-0.24576</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>48.66</v>
+        <v>169.29</v>
       </c>
       <c r="E28" t="n">
-        <v>2913254912</v>
+        <v>3078729747</v>
       </c>
       <c r="F28" t="n">
-        <v>16979495</v>
+        <v>100387755</v>
       </c>
       <c r="G28" t="n">
-        <v>4.78792</v>
+        <v>-1.39343</v>
       </c>
     </row>
     <row r="29">
@@ -1214,16 +1214,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>18.18</v>
+        <v>20.08</v>
       </c>
       <c r="E29" t="n">
-        <v>2599938731</v>
+        <v>2884038090</v>
       </c>
       <c r="F29" t="n">
-        <v>83208055</v>
+        <v>256770497</v>
       </c>
       <c r="G29" t="n">
-        <v>4.76539</v>
+        <v>0.01911</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>8.390000000000001</v>
+        <v>0.107997</v>
       </c>
       <c r="E30" t="n">
-        <v>2454193351</v>
+        <v>2870973380</v>
       </c>
       <c r="F30" t="n">
-        <v>201724445</v>
+        <v>98245056</v>
       </c>
       <c r="G30" t="n">
-        <v>6.55821</v>
+        <v>2.31098</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>4.11</v>
+        <v>9.41</v>
       </c>
       <c r="E31" t="n">
-        <v>1906661475</v>
+        <v>2770617037</v>
       </c>
       <c r="F31" t="n">
-        <v>115763225</v>
+        <v>187429296</v>
       </c>
       <c r="G31" t="n">
-        <v>3.90937</v>
+        <v>3.5936</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>1</v>
+        <v>4.79</v>
       </c>
       <c r="E32" t="n">
-        <v>1897531359</v>
+        <v>2249195580</v>
       </c>
       <c r="F32" t="n">
-        <v>3235136233</v>
+        <v>265052488</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.0323</v>
+        <v>4.02152</v>
       </c>
     </row>
     <row r="33">
@@ -1322,16 +1322,16 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.056376</v>
+        <v>0.062824</v>
       </c>
       <c r="E33" t="n">
-        <v>1890777818</v>
+        <v>2116099234</v>
       </c>
       <c r="F33" t="n">
-        <v>25487278</v>
+        <v>91131862</v>
       </c>
       <c r="G33" t="n">
-        <v>2.65749</v>
+        <v>0.03713</v>
       </c>
     </row>
     <row r="34">
@@ -1349,16 +1349,16 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>4.15</v>
+        <v>4.53</v>
       </c>
       <c r="E34" t="n">
-        <v>1861459510</v>
+        <v>2044221073</v>
       </c>
       <c r="F34" t="n">
-        <v>30287938</v>
+        <v>69334403</v>
       </c>
       <c r="G34" t="n">
-        <v>4.12787</v>
+        <v>3.18482</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.06884999999999999</v>
+        <v>8.130000000000001</v>
       </c>
       <c r="E35" t="n">
-        <v>1813222675</v>
+        <v>2040217993</v>
       </c>
       <c r="F35" t="n">
-        <v>9452427</v>
+        <v>320428875</v>
       </c>
       <c r="G35" t="n">
-        <v>2.2761</v>
+        <v>10.08906</v>
       </c>
     </row>
     <row r="36">
@@ -1403,16 +1403,16 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>2.03</v>
+        <v>2.22</v>
       </c>
       <c r="E36" t="n">
-        <v>1803670925</v>
+        <v>1987240220</v>
       </c>
       <c r="F36" t="n">
-        <v>48772634</v>
+        <v>113720477</v>
       </c>
       <c r="G36" t="n">
-        <v>1.18192</v>
+        <v>-2.3128</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>7.01</v>
+        <v>0.08903899999999999</v>
       </c>
       <c r="E37" t="n">
-        <v>1742531649</v>
+        <v>1921720603</v>
       </c>
       <c r="F37" t="n">
-        <v>77872833</v>
+        <v>40047333</v>
       </c>
       <c r="G37" t="n">
-        <v>1.4844</v>
+        <v>2.48551</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1.63</v>
+        <v>0.99847</v>
       </c>
       <c r="E38" t="n">
-        <v>1608683341</v>
+        <v>1876120940</v>
       </c>
       <c r="F38" t="n">
-        <v>139110282</v>
+        <v>1146168399</v>
       </c>
       <c r="G38" t="n">
-        <v>9.21252</v>
+        <v>-0.238</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.02078443</v>
+        <v>1.77</v>
       </c>
       <c r="E39" t="n">
-        <v>1510140826</v>
+        <v>1768201614</v>
       </c>
       <c r="F39" t="n">
-        <v>41336559</v>
+        <v>325462030</v>
       </c>
       <c r="G39" t="n">
-        <v>3.69558</v>
+        <v>13.83276</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>101.31</v>
+        <v>0.02230666</v>
       </c>
       <c r="E40" t="n">
-        <v>1467701750</v>
+        <v>1627184770</v>
       </c>
       <c r="F40" t="n">
-        <v>19746836</v>
+        <v>56816636</v>
       </c>
       <c r="G40" t="n">
-        <v>1.54054</v>
+        <v>-0.80003</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>RUNE</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>THORChain</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1.1</v>
+        <v>5.29</v>
       </c>
       <c r="E41" t="n">
-        <v>1407878860</v>
+        <v>1613622408</v>
       </c>
       <c r="F41" t="n">
-        <v>301587224</v>
+        <v>1329471861</v>
       </c>
       <c r="G41" t="n">
-        <v>3.11647</v>
+        <v>20.84753</v>
       </c>
     </row>
     <row r="42">
@@ -1556,79 +1556,79 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1.54</v>
+        <v>106.25</v>
       </c>
       <c r="E42" t="n">
-        <v>1349299437</v>
+        <v>1551057007</v>
       </c>
       <c r="F42" t="n">
-        <v>126616269</v>
+        <v>31319853</v>
       </c>
       <c r="G42" t="n">
-        <v>6.16335</v>
+        <v>-4.27393</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>AAVE</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Aave</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>91.31</v>
+        <v>1.71</v>
       </c>
       <c r="E43" t="n">
-        <v>1336074956</v>
+        <v>1513960032</v>
       </c>
       <c r="F43" t="n">
-        <v>124207911</v>
+        <v>166336923</v>
       </c>
       <c r="G43" t="n">
-        <v>0.72412</v>
+        <v>1.24694</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.062127</v>
+        <v>17.61</v>
       </c>
       <c r="E44" t="n">
-        <v>1329531275</v>
+        <v>1481359860</v>
       </c>
       <c r="F44" t="n">
-        <v>44839987</v>
+        <v>148087340</v>
       </c>
       <c r="G44" t="n">
-        <v>13.29736</v>
+        <v>-3.02037</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>15.65</v>
+        <v>1.14</v>
       </c>
       <c r="E45" t="n">
-        <v>1311769081</v>
+        <v>1454452587</v>
       </c>
       <c r="F45" t="n">
-        <v>68968162</v>
+        <v>418265046</v>
       </c>
       <c r="G45" t="n">
-        <v>6.78456</v>
+        <v>-1.01507</v>
       </c>
     </row>
     <row r="46">
@@ -1664,133 +1664,133 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.414792</v>
+        <v>1.13</v>
       </c>
       <c r="E46" t="n">
-        <v>1288338765</v>
+        <v>1434707009</v>
       </c>
       <c r="F46" t="n">
-        <v>56708987</v>
+        <v>785432074</v>
       </c>
       <c r="G46" t="n">
-        <v>1.24488</v>
+        <v>6.84381</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>EGLD</t>
+          <t>AAVE</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>MultiversX</t>
+          <t>Aave</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>46.43</v>
+        <v>96.59999999999999</v>
       </c>
       <c r="E47" t="n">
-        <v>1216981858</v>
+        <v>1421197962</v>
       </c>
       <c r="F47" t="n">
-        <v>290287143</v>
+        <v>202826884</v>
       </c>
       <c r="G47" t="n">
-        <v>37.59187</v>
+        <v>-0.37999</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>1339.55</v>
+        <v>0.438165</v>
       </c>
       <c r="E48" t="n">
-        <v>1207352218</v>
+        <v>1362766826</v>
       </c>
       <c r="F48" t="n">
-        <v>33851538</v>
+        <v>7078277</v>
       </c>
       <c r="G48" t="n">
-        <v>0.133</v>
+        <v>-3.38986</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ImmutableX</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.951439</v>
+        <v>0.137074</v>
       </c>
       <c r="E49" t="n">
-        <v>1190900088</v>
+        <v>1279826091</v>
       </c>
       <c r="F49" t="n">
-        <v>770261663</v>
+        <v>123752311</v>
       </c>
       <c r="G49" t="n">
-        <v>24.78934</v>
+        <v>2.20593</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>RETH</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Rocket Pool ETH</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.12779</v>
+        <v>2233.25</v>
       </c>
       <c r="E50" t="n">
-        <v>1184634620</v>
+        <v>1197182243</v>
       </c>
       <c r="F50" t="n">
-        <v>125277039</v>
+        <v>7983732</v>
       </c>
       <c r="G50" t="n">
-        <v>9.78881</v>
+        <v>-0.61734</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>RETH</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Rocket Pool ETH</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>2072.79</v>
+        <v>1293.12</v>
       </c>
       <c r="E51" t="n">
-        <v>1109107345</v>
+        <v>1168378184</v>
       </c>
       <c r="F51" t="n">
-        <v>8102440</v>
+        <v>86633999</v>
       </c>
       <c r="G51" t="n">
-        <v>2.49026</v>
+        <v>-0.483</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-11-19
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>37040</v>
+        <v>36463</v>
       </c>
       <c r="E2" t="n">
-        <v>724605718990</v>
+        <v>713278345221</v>
       </c>
       <c r="F2" t="n">
-        <v>12522762620</v>
+        <v>10638135767</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.16848</v>
+        <v>-0.1178</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2041.15</v>
+        <v>1948.62</v>
       </c>
       <c r="E3" t="n">
-        <v>246157223708</v>
+        <v>234674236247</v>
       </c>
       <c r="F3" t="n">
-        <v>11951582315</v>
+        <v>10594386967</v>
       </c>
       <c r="G3" t="n">
-        <v>-1.03607</v>
+        <v>0.28584</v>
       </c>
     </row>
     <row r="4">
@@ -542,13 +542,13 @@
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>86823534820</v>
+        <v>87727232727</v>
       </c>
       <c r="F4" t="n">
-        <v>34449847337</v>
+        <v>25595322252</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.09526</v>
+        <v>-0.04898</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>248.65</v>
+        <v>243.13</v>
       </c>
       <c r="E5" t="n">
-        <v>38317048614</v>
+        <v>37441079374</v>
       </c>
       <c r="F5" t="n">
-        <v>879651128</v>
+        <v>433375700</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.40342</v>
+        <v>-0.19928</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.664659</v>
+        <v>0.611469</v>
       </c>
       <c r="E6" t="n">
-        <v>35757221274</v>
+        <v>32841490138</v>
       </c>
       <c r="F6" t="n">
-        <v>1365124642</v>
+        <v>643918749</v>
       </c>
       <c r="G6" t="n">
-        <v>-1.08723</v>
+        <v>1.20883</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>58.68</v>
+        <v>59.72</v>
       </c>
       <c r="E7" t="n">
-        <v>25117403863</v>
+        <v>25314152605</v>
       </c>
       <c r="F7" t="n">
-        <v>4628222328</v>
+        <v>2163595384</v>
       </c>
       <c r="G7" t="n">
-        <v>4.41822</v>
+        <v>4.22775</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.999221</v>
+        <v>0.999458</v>
       </c>
       <c r="E8" t="n">
-        <v>24224936652</v>
+        <v>24425990390</v>
       </c>
       <c r="F8" t="n">
-        <v>6413967726</v>
+        <v>5674596136</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.16951</v>
+        <v>-0.20277</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2045.19</v>
+        <v>1951.33</v>
       </c>
       <c r="E9" t="n">
-        <v>18343678764</v>
+        <v>17527907826</v>
       </c>
       <c r="F9" t="n">
-        <v>12354607</v>
+        <v>4600282</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.79071</v>
+        <v>0.76795</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.384794</v>
+        <v>0.375245</v>
       </c>
       <c r="E10" t="n">
-        <v>13504796837</v>
+        <v>13141902803</v>
       </c>
       <c r="F10" t="n">
-        <v>538761565</v>
+        <v>326601194</v>
       </c>
       <c r="G10" t="n">
-        <v>1.52594</v>
+        <v>4.20721</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.078669</v>
+        <v>0.07828</v>
       </c>
       <c r="E11" t="n">
-        <v>11209518930</v>
+        <v>11137299245</v>
       </c>
       <c r="F11" t="n">
-        <v>1452450603</v>
+        <v>1338360892</v>
       </c>
       <c r="G11" t="n">
-        <v>-1.92124</v>
+        <v>-7.97257</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.108046</v>
+        <v>0.102614</v>
       </c>
       <c r="E12" t="n">
-        <v>9592159930</v>
+        <v>9096532280</v>
       </c>
       <c r="F12" t="n">
-        <v>296989630</v>
+        <v>256923700</v>
       </c>
       <c r="G12" t="n">
-        <v>1.23702</v>
+        <v>0.23388</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>15.91</v>
+        <v>14.13</v>
       </c>
       <c r="E13" t="n">
-        <v>8921358550</v>
+        <v>7908120394</v>
       </c>
       <c r="F13" t="n">
-        <v>1392273390</v>
+        <v>624270650</v>
       </c>
       <c r="G13" t="n">
-        <v>4.70082</v>
+        <v>5.6966</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.832392</v>
+        <v>0.820777</v>
       </c>
       <c r="E14" t="n">
-        <v>7730131211</v>
+        <v>7630221460</v>
       </c>
       <c r="F14" t="n">
-        <v>696743261</v>
+        <v>439224307</v>
       </c>
       <c r="G14" t="n">
-        <v>2.1093</v>
+        <v>1.11809</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>5.77</v>
+        <v>21.25</v>
       </c>
       <c r="E15" t="n">
-        <v>7507447148</v>
+        <v>7584458524</v>
       </c>
       <c r="F15" t="n">
-        <v>536924480</v>
+        <v>723623568</v>
       </c>
       <c r="G15" t="n">
-        <v>8.306940000000001</v>
+        <v>-0.25366</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>18.44</v>
+        <v>5.22</v>
       </c>
       <c r="E16" t="n">
-        <v>6577465473</v>
+        <v>6792552843</v>
       </c>
       <c r="F16" t="n">
-        <v>1402997291</v>
+        <v>177863428</v>
       </c>
       <c r="G16" t="n">
-        <v>29.19223</v>
+        <v>1.23394</v>
       </c>
     </row>
     <row r="17">
@@ -890,16 +890,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>37045</v>
+        <v>36423</v>
       </c>
       <c r="E17" t="n">
-        <v>6068339256</v>
+        <v>5952233544</v>
       </c>
       <c r="F17" t="n">
-        <v>229323005</v>
+        <v>63126562</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.01298</v>
+        <v>0.2034</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>75.13</v>
+        <v>1</v>
       </c>
       <c r="E18" t="n">
-        <v>5589109160</v>
+        <v>5290743624</v>
       </c>
       <c r="F18" t="n">
-        <v>604310194</v>
+        <v>292545455</v>
       </c>
       <c r="G18" t="n">
-        <v>0.82397</v>
+        <v>0.0931</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.998789</v>
+        <v>69.04000000000001</v>
       </c>
       <c r="E19" t="n">
-        <v>5344232878</v>
+        <v>5115863614</v>
       </c>
       <c r="F19" t="n">
-        <v>149291487</v>
+        <v>262479821</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.09699000000000001</v>
+        <v>-0.31536</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>8.970000000000001e-06</v>
+        <v>2.34</v>
       </c>
       <c r="E20" t="n">
-        <v>5317565933</v>
+        <v>5034445988</v>
       </c>
       <c r="F20" t="n">
-        <v>316725240</v>
+        <v>35889737</v>
       </c>
       <c r="G20" t="n">
-        <v>-2.31299</v>
+        <v>1.57073</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>2.42</v>
+        <v>8.47e-06</v>
       </c>
       <c r="E21" t="n">
-        <v>5176194300</v>
+        <v>5002062801</v>
       </c>
       <c r="F21" t="n">
-        <v>54764374</v>
+        <v>130075973</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.30984</v>
+        <v>-1.59884</v>
       </c>
     </row>
     <row r="22">
@@ -1025,16 +1025,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>236.81</v>
+        <v>227.02</v>
       </c>
       <c r="E22" t="n">
-        <v>4645632726</v>
+        <v>4445785916</v>
       </c>
       <c r="F22" t="n">
-        <v>143715572</v>
+        <v>77077961</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.36195</v>
+        <v>0.43486</v>
       </c>
     </row>
     <row r="23">
@@ -1052,16 +1052,16 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>5.35</v>
+        <v>5.06</v>
       </c>
       <c r="E23" t="n">
-        <v>4054865364</v>
+        <v>3827734223</v>
       </c>
       <c r="F23" t="n">
-        <v>168902663</v>
+        <v>113650291</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.83385</v>
+        <v>1.65777</v>
       </c>
     </row>
     <row r="24">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>4.09</v>
+        <v>4.08</v>
       </c>
       <c r="E24" t="n">
-        <v>3797066618</v>
+        <v>3786576519</v>
       </c>
       <c r="F24" t="n">
-        <v>1027107</v>
+        <v>1208205</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.25779</v>
+        <v>0.14174</v>
       </c>
     </row>
     <row r="25">
@@ -1106,16 +1106,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>60.22</v>
+        <v>57.12</v>
       </c>
       <c r="E25" t="n">
-        <v>3619693066</v>
+        <v>3423812857</v>
       </c>
       <c r="F25" t="n">
-        <v>14205455</v>
+        <v>14897677</v>
       </c>
       <c r="G25" t="n">
-        <v>-1.30488</v>
+        <v>1.72499</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.125533</v>
+        <v>0.118755</v>
       </c>
       <c r="E26" t="n">
-        <v>3520446780</v>
+        <v>3325107382</v>
       </c>
       <c r="F26" t="n">
-        <v>117958647</v>
+        <v>49276479</v>
       </c>
       <c r="G26" t="n">
-        <v>0.50259</v>
+        <v>0.92264</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.997806</v>
+        <v>0.998617</v>
       </c>
       <c r="E27" t="n">
-        <v>3334473511</v>
+        <v>3304441994</v>
       </c>
       <c r="F27" t="n">
-        <v>137459642</v>
+        <v>130823149</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.24576</v>
+        <v>-0.12079</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>169.29</v>
+        <v>0.143476</v>
       </c>
       <c r="E28" t="n">
-        <v>3078729747</v>
+        <v>3113433913</v>
       </c>
       <c r="F28" t="n">
-        <v>100387755</v>
+        <v>127212618</v>
       </c>
       <c r="G28" t="n">
-        <v>-1.39343</v>
+        <v>9.01388</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>20.08</v>
+        <v>159.89</v>
       </c>
       <c r="E29" t="n">
-        <v>2884038090</v>
+        <v>2906522015</v>
       </c>
       <c r="F29" t="n">
-        <v>256770497</v>
+        <v>64871691</v>
       </c>
       <c r="G29" t="n">
-        <v>0.01911</v>
+        <v>-0.47624</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.107997</v>
+        <v>19.03</v>
       </c>
       <c r="E30" t="n">
-        <v>2870973380</v>
+        <v>2732624860</v>
       </c>
       <c r="F30" t="n">
-        <v>98245056</v>
+        <v>97990304</v>
       </c>
       <c r="G30" t="n">
-        <v>2.31098</v>
+        <v>0.57941</v>
       </c>
     </row>
     <row r="31">
@@ -1268,16 +1268,16 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>9.41</v>
+        <v>9.109999999999999</v>
       </c>
       <c r="E31" t="n">
-        <v>2770617037</v>
+        <v>2668287560</v>
       </c>
       <c r="F31" t="n">
-        <v>187429296</v>
+        <v>184072785</v>
       </c>
       <c r="G31" t="n">
-        <v>3.5936</v>
+        <v>-0.55987</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>4.79</v>
+        <v>0.096206</v>
       </c>
       <c r="E32" t="n">
-        <v>2249195580</v>
+        <v>2538933153</v>
       </c>
       <c r="F32" t="n">
-        <v>265052488</v>
+        <v>17683434</v>
       </c>
       <c r="G32" t="n">
-        <v>4.02152</v>
+        <v>-1.19075</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.062824</v>
+        <v>4.73</v>
       </c>
       <c r="E33" t="n">
-        <v>2116099234</v>
+        <v>2232087839</v>
       </c>
       <c r="F33" t="n">
-        <v>91131862</v>
+        <v>154823470</v>
       </c>
       <c r="G33" t="n">
-        <v>0.03713</v>
+        <v>3.01535</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>4.53</v>
+        <v>0.060779</v>
       </c>
       <c r="E34" t="n">
-        <v>2044221073</v>
+        <v>2045255233</v>
       </c>
       <c r="F34" t="n">
-        <v>69334403</v>
+        <v>44063818</v>
       </c>
       <c r="G34" t="n">
-        <v>3.18482</v>
+        <v>-0.46653</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>8.130000000000001</v>
+        <v>2.27</v>
       </c>
       <c r="E35" t="n">
-        <v>2040217993</v>
+        <v>2025086884</v>
       </c>
       <c r="F35" t="n">
-        <v>320428875</v>
+        <v>94278091</v>
       </c>
       <c r="G35" t="n">
-        <v>10.08906</v>
+        <v>4.31648</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>2.22</v>
+        <v>4.43</v>
       </c>
       <c r="E36" t="n">
-        <v>1987240220</v>
+        <v>1999639978</v>
       </c>
       <c r="F36" t="n">
-        <v>113720477</v>
+        <v>57417254</v>
       </c>
       <c r="G36" t="n">
-        <v>-2.3128</v>
+        <v>6.10653</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.08903899999999999</v>
+        <v>6.97</v>
       </c>
       <c r="E37" t="n">
-        <v>1921720603</v>
+        <v>1927349159</v>
       </c>
       <c r="F37" t="n">
-        <v>40047333</v>
+        <v>90417905</v>
       </c>
       <c r="G37" t="n">
-        <v>2.48551</v>
+        <v>0.76695</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.99847</v>
+        <v>1.81</v>
       </c>
       <c r="E38" t="n">
-        <v>1876120940</v>
+        <v>1819106245</v>
       </c>
       <c r="F38" t="n">
-        <v>1146168399</v>
+        <v>220442547</v>
       </c>
       <c r="G38" t="n">
-        <v>-0.238</v>
+        <v>4.21148</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1.77</v>
+        <v>0.999793</v>
       </c>
       <c r="E39" t="n">
-        <v>1768201614</v>
+        <v>1803129302</v>
       </c>
       <c r="F39" t="n">
-        <v>325462030</v>
+        <v>2178141636</v>
       </c>
       <c r="G39" t="n">
-        <v>13.83276</v>
+        <v>-0.09601999999999999</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>RUNE</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>THORChain</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.02230666</v>
+        <v>5.37</v>
       </c>
       <c r="E40" t="n">
-        <v>1627184770</v>
+        <v>1626569223</v>
       </c>
       <c r="F40" t="n">
-        <v>56816636</v>
+        <v>606647457</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.80003</v>
+        <v>-13.20237</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>RUNE</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>THORChain</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>5.29</v>
+        <v>1.29</v>
       </c>
       <c r="E41" t="n">
-        <v>1613622408</v>
+        <v>1610125084</v>
       </c>
       <c r="F41" t="n">
-        <v>1329471861</v>
+        <v>746641476</v>
       </c>
       <c r="G41" t="n">
-        <v>20.84753</v>
+        <v>19.17595</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>106.25</v>
+        <v>0.496844</v>
       </c>
       <c r="E42" t="n">
-        <v>1551057007</v>
+        <v>1546042804</v>
       </c>
       <c r="F42" t="n">
-        <v>31319853</v>
+        <v>16626316</v>
       </c>
       <c r="G42" t="n">
-        <v>-4.27393</v>
+        <v>-1.81646</v>
       </c>
     </row>
     <row r="43">
@@ -1592,16 +1592,16 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1.71</v>
+        <v>1.72</v>
       </c>
       <c r="E43" t="n">
-        <v>1513960032</v>
+        <v>1512620694</v>
       </c>
       <c r="F43" t="n">
-        <v>166336923</v>
+        <v>110625115</v>
       </c>
       <c r="G43" t="n">
-        <v>1.24694</v>
+        <v>2.44179</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>17.61</v>
+        <v>0.02075484</v>
       </c>
       <c r="E44" t="n">
-        <v>1481359860</v>
+        <v>1511557383</v>
       </c>
       <c r="F44" t="n">
-        <v>148087340</v>
+        <v>29933293</v>
       </c>
       <c r="G44" t="n">
-        <v>-3.02037</v>
+        <v>0.17407</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>1.14</v>
+        <v>256.86</v>
       </c>
       <c r="E45" t="n">
-        <v>1454452587</v>
+        <v>1460659872</v>
       </c>
       <c r="F45" t="n">
-        <v>418265046</v>
+        <v>20209119</v>
       </c>
       <c r="G45" t="n">
-        <v>-1.01507</v>
+        <v>19.43234</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>1.13</v>
+        <v>98.78</v>
       </c>
       <c r="E46" t="n">
-        <v>1434707009</v>
+        <v>1437243683</v>
       </c>
       <c r="F46" t="n">
-        <v>785432074</v>
+        <v>19494840</v>
       </c>
       <c r="G46" t="n">
-        <v>6.84381</v>
+        <v>-0.11649</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>AAVE</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Aave</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>96.59999999999999</v>
+        <v>15.68</v>
       </c>
       <c r="E47" t="n">
-        <v>1421197962</v>
+        <v>1317429856</v>
       </c>
       <c r="F47" t="n">
-        <v>202826884</v>
+        <v>68947999</v>
       </c>
       <c r="G47" t="n">
-        <v>-0.37999</v>
+        <v>-0.54709</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.438165</v>
+        <v>1.02</v>
       </c>
       <c r="E48" t="n">
-        <v>1362766826</v>
+        <v>1303115892</v>
       </c>
       <c r="F48" t="n">
-        <v>7078277</v>
+        <v>227473803</v>
       </c>
       <c r="G48" t="n">
-        <v>-3.38986</v>
+        <v>-0.44736</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>AAVE</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Aave</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.137074</v>
+        <v>88.33</v>
       </c>
       <c r="E49" t="n">
-        <v>1279826091</v>
+        <v>1296056485</v>
       </c>
       <c r="F49" t="n">
-        <v>123752311</v>
+        <v>130091736</v>
       </c>
       <c r="G49" t="n">
-        <v>2.20593</v>
+        <v>2.99954</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>RETH</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Rocket Pool ETH</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>2233.25</v>
+        <v>3.42</v>
       </c>
       <c r="E50" t="n">
-        <v>1197182243</v>
+        <v>1285194729</v>
       </c>
       <c r="F50" t="n">
-        <v>7983732</v>
+        <v>247908508</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.61734</v>
+        <v>9.540710000000001</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>1293.12</v>
+        <v>0.131363</v>
       </c>
       <c r="E51" t="n">
-        <v>1168378184</v>
+        <v>1226772951</v>
       </c>
       <c r="F51" t="n">
-        <v>86633999</v>
+        <v>53392678</v>
       </c>
       <c r="G51" t="n">
-        <v>-0.483</v>
+        <v>5.22045</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-11-26
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>36463</v>
+        <v>37625</v>
       </c>
       <c r="E2" t="n">
-        <v>713278345221</v>
+        <v>736259302345</v>
       </c>
       <c r="F2" t="n">
-        <v>10638135767</v>
+        <v>3517346364</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.1178</v>
+        <v>-0.22492</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1948.62</v>
+        <v>2079.34</v>
       </c>
       <c r="E3" t="n">
-        <v>234674236247</v>
+        <v>250171234092</v>
       </c>
       <c r="F3" t="n">
-        <v>10594386967</v>
+        <v>6903048294</v>
       </c>
       <c r="G3" t="n">
-        <v>0.28584</v>
+        <v>0.12591</v>
       </c>
     </row>
     <row r="4">
@@ -542,13 +542,13 @@
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>87727232727</v>
+        <v>88749057889</v>
       </c>
       <c r="F4" t="n">
-        <v>25595322252</v>
+        <v>16309226426</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.04898</v>
+        <v>-0.06523</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>243.13</v>
+        <v>233.52</v>
       </c>
       <c r="E5" t="n">
-        <v>37441079374</v>
+        <v>35936092441</v>
       </c>
       <c r="F5" t="n">
-        <v>433375700</v>
+        <v>326624169</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.19928</v>
+        <v>-0.11017</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.611469</v>
+        <v>0.635868</v>
       </c>
       <c r="E6" t="n">
-        <v>32841490138</v>
+        <v>34055784577</v>
       </c>
       <c r="F6" t="n">
-        <v>643918749</v>
+        <v>673962406</v>
       </c>
       <c r="G6" t="n">
-        <v>1.20883</v>
+        <v>2.64056</v>
       </c>
     </row>
     <row r="7">
@@ -611,25 +611,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>SOL</t>
+          <t>USDC</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Solana</t>
+          <t>USDC</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>59.72</v>
+        <v>0.999526</v>
       </c>
       <c r="E7" t="n">
-        <v>25314152605</v>
+        <v>24692866617</v>
       </c>
       <c r="F7" t="n">
-        <v>2163595384</v>
+        <v>3454915825</v>
       </c>
       <c r="G7" t="n">
-        <v>4.22775</v>
+        <v>-0.07556</v>
       </c>
     </row>
     <row r="8">
@@ -638,25 +638,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>USDC</t>
+          <t>SOL</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>USDC</t>
+          <t>Solana</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.999458</v>
+        <v>57.73</v>
       </c>
       <c r="E8" t="n">
-        <v>24425990390</v>
+        <v>24447092537</v>
       </c>
       <c r="F8" t="n">
-        <v>5674596136</v>
+        <v>750421402</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.20277</v>
+        <v>-0.54648</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1951.33</v>
+        <v>2080.02</v>
       </c>
       <c r="E9" t="n">
-        <v>17527907826</v>
+        <v>19168159089</v>
       </c>
       <c r="F9" t="n">
-        <v>4600282</v>
+        <v>5566434</v>
       </c>
       <c r="G9" t="n">
-        <v>0.76795</v>
+        <v>0.36862</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.375245</v>
+        <v>0.389958</v>
       </c>
       <c r="E10" t="n">
-        <v>13141902803</v>
+        <v>13641644069</v>
       </c>
       <c r="F10" t="n">
-        <v>326601194</v>
+        <v>204086224</v>
       </c>
       <c r="G10" t="n">
-        <v>4.20721</v>
+        <v>-0.02658</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.07828</v>
+        <v>0.077693</v>
       </c>
       <c r="E11" t="n">
-        <v>11137299245</v>
+        <v>11028564613</v>
       </c>
       <c r="F11" t="n">
-        <v>1338360892</v>
+        <v>320176930</v>
       </c>
       <c r="G11" t="n">
-        <v>-7.97257</v>
+        <v>-0.57238</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.102614</v>
+        <v>0.108234</v>
       </c>
       <c r="E12" t="n">
-        <v>9096532280</v>
+        <v>9585065252</v>
       </c>
       <c r="F12" t="n">
-        <v>256923700</v>
+        <v>345169432</v>
       </c>
       <c r="G12" t="n">
-        <v>0.23388</v>
+        <v>2.81656</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>14.13</v>
+        <v>15.08</v>
       </c>
       <c r="E13" t="n">
-        <v>7908120394</v>
+        <v>8425946669</v>
       </c>
       <c r="F13" t="n">
-        <v>624270650</v>
+        <v>416451209</v>
       </c>
       <c r="G13" t="n">
-        <v>5.6966</v>
+        <v>1.76866</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.820777</v>
+        <v>2.34</v>
       </c>
       <c r="E14" t="n">
-        <v>7630221460</v>
+        <v>8158304662</v>
       </c>
       <c r="F14" t="n">
-        <v>439224307</v>
+        <v>28675464</v>
       </c>
       <c r="G14" t="n">
-        <v>1.11809</v>
+        <v>-1.68925</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>21.25</v>
+        <v>21</v>
       </c>
       <c r="E15" t="n">
-        <v>7584458524</v>
+        <v>7664721349</v>
       </c>
       <c r="F15" t="n">
-        <v>723623568</v>
+        <v>283746740</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.25366</v>
+        <v>0.78611</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>5.22</v>
+        <v>0.772644</v>
       </c>
       <c r="E16" t="n">
-        <v>6792552843</v>
+        <v>7163367529</v>
       </c>
       <c r="F16" t="n">
-        <v>177863428</v>
+        <v>279760699</v>
       </c>
       <c r="G16" t="n">
-        <v>1.23394</v>
+        <v>0.05195</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>36423</v>
+        <v>5.32</v>
       </c>
       <c r="E17" t="n">
-        <v>5952233544</v>
+        <v>6929814098</v>
       </c>
       <c r="F17" t="n">
-        <v>63126562</v>
+        <v>125154645</v>
       </c>
       <c r="G17" t="n">
-        <v>0.2034</v>
+        <v>0.5367499999999999</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>37610</v>
       </c>
       <c r="E18" t="n">
-        <v>5290743624</v>
+        <v>6074201967</v>
       </c>
       <c r="F18" t="n">
-        <v>292545455</v>
+        <v>69735164</v>
       </c>
       <c r="G18" t="n">
-        <v>0.0931</v>
+        <v>-0.16635</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>69.04000000000001</v>
+        <v>0.998215</v>
       </c>
       <c r="E19" t="n">
-        <v>5115863614</v>
+        <v>5343350641</v>
       </c>
       <c r="F19" t="n">
-        <v>262479821</v>
+        <v>259647744</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.31536</v>
+        <v>-0.14416</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>2.34</v>
+        <v>70.76000000000001</v>
       </c>
       <c r="E20" t="n">
-        <v>5034445988</v>
+        <v>5231368559</v>
       </c>
       <c r="F20" t="n">
-        <v>35889737</v>
+        <v>202438192</v>
       </c>
       <c r="G20" t="n">
-        <v>1.57073</v>
+        <v>-0.47644</v>
       </c>
     </row>
     <row r="21">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>8.47e-06</v>
+        <v>8.31e-06</v>
       </c>
       <c r="E21" t="n">
-        <v>5002062801</v>
+        <v>4902843612</v>
       </c>
       <c r="F21" t="n">
-        <v>130075973</v>
+        <v>114301831</v>
       </c>
       <c r="G21" t="n">
-        <v>-1.59884</v>
+        <v>-0.02722</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>227.02</v>
+        <v>6.05</v>
       </c>
       <c r="E22" t="n">
-        <v>4445785916</v>
+        <v>4574283751</v>
       </c>
       <c r="F22" t="n">
-        <v>77077961</v>
+        <v>189062114</v>
       </c>
       <c r="G22" t="n">
-        <v>0.43486</v>
+        <v>-1.89668</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>5.06</v>
+        <v>227.81</v>
       </c>
       <c r="E23" t="n">
-        <v>3827734223</v>
+        <v>4460955545</v>
       </c>
       <c r="F23" t="n">
-        <v>113650291</v>
+        <v>74078147</v>
       </c>
       <c r="G23" t="n">
-        <v>1.65777</v>
+        <v>-0.0746</v>
       </c>
     </row>
     <row r="24">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>4.08</v>
+        <v>3.98</v>
       </c>
       <c r="E24" t="n">
-        <v>3786576519</v>
+        <v>3694153322</v>
       </c>
       <c r="F24" t="n">
-        <v>1208205</v>
+        <v>773897</v>
       </c>
       <c r="G24" t="n">
-        <v>0.14174</v>
+        <v>0.50341</v>
       </c>
     </row>
     <row r="25">
@@ -1106,16 +1106,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>57.12</v>
+        <v>57.93</v>
       </c>
       <c r="E25" t="n">
-        <v>3423812857</v>
+        <v>3480226996</v>
       </c>
       <c r="F25" t="n">
-        <v>14897677</v>
+        <v>5335786</v>
       </c>
       <c r="G25" t="n">
-        <v>1.72499</v>
+        <v>-0.69929</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.118755</v>
+        <v>0.122306</v>
       </c>
       <c r="E26" t="n">
-        <v>3325107382</v>
+        <v>3424261647</v>
       </c>
       <c r="F26" t="n">
-        <v>49276479</v>
+        <v>64942610</v>
       </c>
       <c r="G26" t="n">
-        <v>0.92264</v>
+        <v>0.9911</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.998617</v>
+        <v>0.997935</v>
       </c>
       <c r="E27" t="n">
-        <v>3304441994</v>
+        <v>3166077989</v>
       </c>
       <c r="F27" t="n">
-        <v>130823149</v>
+        <v>89159985</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.12079</v>
+        <v>-0.08445999999999999</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.143476</v>
+        <v>170.93</v>
       </c>
       <c r="E28" t="n">
-        <v>3113433913</v>
+        <v>3097072361</v>
       </c>
       <c r="F28" t="n">
-        <v>127212618</v>
+        <v>53908513</v>
       </c>
       <c r="G28" t="n">
-        <v>9.01388</v>
+        <v>0.05869</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>159.89</v>
+        <v>0.132229</v>
       </c>
       <c r="E29" t="n">
-        <v>2906522015</v>
+        <v>2877422719</v>
       </c>
       <c r="F29" t="n">
-        <v>64871691</v>
+        <v>38454528</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.47624</v>
+        <v>-4.55337</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>19.03</v>
+        <v>9.630000000000001</v>
       </c>
       <c r="E30" t="n">
-        <v>2732624860</v>
+        <v>2816881054</v>
       </c>
       <c r="F30" t="n">
-        <v>97990304</v>
+        <v>180594648</v>
       </c>
       <c r="G30" t="n">
-        <v>0.57941</v>
+        <v>7.14754</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>9.109999999999999</v>
+        <v>19.3</v>
       </c>
       <c r="E31" t="n">
-        <v>2668287560</v>
+        <v>2768898134</v>
       </c>
       <c r="F31" t="n">
-        <v>184072785</v>
+        <v>77080672</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.55987</v>
+        <v>0.05147</v>
       </c>
     </row>
     <row r="32">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.096206</v>
+        <v>0.095499</v>
       </c>
       <c r="E32" t="n">
-        <v>2538933153</v>
+        <v>2518642602</v>
       </c>
       <c r="F32" t="n">
-        <v>17683434</v>
+        <v>9855637</v>
       </c>
       <c r="G32" t="n">
-        <v>-1.19075</v>
+        <v>-0.96205</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>4.73</v>
+        <v>2.48</v>
       </c>
       <c r="E33" t="n">
-        <v>2232087839</v>
+        <v>2210278660</v>
       </c>
       <c r="F33" t="n">
-        <v>154823470</v>
+        <v>54562650</v>
       </c>
       <c r="G33" t="n">
-        <v>3.01535</v>
+        <v>0.74139</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.060779</v>
+        <v>4.64</v>
       </c>
       <c r="E34" t="n">
-        <v>2045255233</v>
+        <v>2197865478</v>
       </c>
       <c r="F34" t="n">
-        <v>44063818</v>
+        <v>99172801</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.46653</v>
+        <v>-0.5920800000000001</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>2.27</v>
+        <v>0.063441</v>
       </c>
       <c r="E35" t="n">
-        <v>2025086884</v>
+        <v>2126752404</v>
       </c>
       <c r="F35" t="n">
-        <v>94278091</v>
+        <v>31632008</v>
       </c>
       <c r="G35" t="n">
-        <v>4.31648</v>
+        <v>0.79944</v>
       </c>
     </row>
     <row r="36">
@@ -1403,16 +1403,16 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>4.43</v>
+        <v>4.62</v>
       </c>
       <c r="E36" t="n">
-        <v>1999639978</v>
+        <v>2077475492</v>
       </c>
       <c r="F36" t="n">
-        <v>57417254</v>
+        <v>45637801</v>
       </c>
       <c r="G36" t="n">
-        <v>6.10653</v>
+        <v>-0.78127</v>
       </c>
     </row>
     <row r="37">
@@ -1430,16 +1430,16 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>6.97</v>
+        <v>7.31</v>
       </c>
       <c r="E37" t="n">
-        <v>1927349159</v>
+        <v>2025376564</v>
       </c>
       <c r="F37" t="n">
-        <v>90417905</v>
+        <v>62320791</v>
       </c>
       <c r="G37" t="n">
-        <v>0.76695</v>
+        <v>-0.5928600000000001</v>
       </c>
     </row>
     <row r="38">
@@ -1457,16 +1457,16 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1.81</v>
+        <v>1.86</v>
       </c>
       <c r="E38" t="n">
-        <v>1819106245</v>
+        <v>1867777797</v>
       </c>
       <c r="F38" t="n">
-        <v>220442547</v>
+        <v>126974564</v>
       </c>
       <c r="G38" t="n">
-        <v>4.21148</v>
+        <v>1.20068</v>
       </c>
     </row>
     <row r="39">
@@ -1484,16 +1484,16 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.999793</v>
+        <v>0.999615</v>
       </c>
       <c r="E39" t="n">
-        <v>1803129302</v>
+        <v>1740659335</v>
       </c>
       <c r="F39" t="n">
-        <v>2178141636</v>
+        <v>1163919679</v>
       </c>
       <c r="G39" t="n">
-        <v>-0.09601999999999999</v>
+        <v>-0.06347999999999999</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>RUNE</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>THORChain</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>5.37</v>
+        <v>1.36</v>
       </c>
       <c r="E40" t="n">
-        <v>1626569223</v>
+        <v>1709477315</v>
       </c>
       <c r="F40" t="n">
-        <v>606647457</v>
+        <v>516895990</v>
       </c>
       <c r="G40" t="n">
-        <v>-13.20237</v>
+        <v>-0.26468</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1.29</v>
+        <v>0.02332331</v>
       </c>
       <c r="E41" t="n">
-        <v>1610125084</v>
+        <v>1694355234</v>
       </c>
       <c r="F41" t="n">
-        <v>746641476</v>
+        <v>119369299</v>
       </c>
       <c r="G41" t="n">
-        <v>19.17595</v>
+        <v>8.832420000000001</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>RUNE</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>THORChain</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.496844</v>
+        <v>5.34</v>
       </c>
       <c r="E42" t="n">
-        <v>1546042804</v>
+        <v>1607650362</v>
       </c>
       <c r="F42" t="n">
-        <v>16626316</v>
+        <v>249071320</v>
       </c>
       <c r="G42" t="n">
-        <v>-1.81646</v>
+        <v>1.23576</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1.72</v>
+        <v>0.514692</v>
       </c>
       <c r="E43" t="n">
-        <v>1512620694</v>
+        <v>1595857577</v>
       </c>
       <c r="F43" t="n">
-        <v>110625115</v>
+        <v>5899884</v>
       </c>
       <c r="G43" t="n">
-        <v>2.44179</v>
+        <v>0.75026</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.02075484</v>
+        <v>1.81</v>
       </c>
       <c r="E44" t="n">
-        <v>1511557383</v>
+        <v>1591982737</v>
       </c>
       <c r="F44" t="n">
-        <v>29933293</v>
+        <v>85305610</v>
       </c>
       <c r="G44" t="n">
-        <v>0.17407</v>
+        <v>1.84431</v>
       </c>
     </row>
     <row r="45">
@@ -1646,16 +1646,16 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>256.86</v>
+        <v>267.08</v>
       </c>
       <c r="E45" t="n">
-        <v>1460659872</v>
+        <v>1507931258</v>
       </c>
       <c r="F45" t="n">
-        <v>20209119</v>
+        <v>6805136</v>
       </c>
       <c r="G45" t="n">
-        <v>19.43234</v>
+        <v>-1.27712</v>
       </c>
     </row>
     <row r="46">
@@ -1673,16 +1673,16 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>98.78</v>
+        <v>103.35</v>
       </c>
       <c r="E46" t="n">
-        <v>1437243683</v>
+        <v>1499940147</v>
       </c>
       <c r="F46" t="n">
-        <v>19494840</v>
+        <v>29965834</v>
       </c>
       <c r="G46" t="n">
-        <v>-0.11649</v>
+        <v>2.68999</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>AAVE</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>Aave</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>15.68</v>
+        <v>100.67</v>
       </c>
       <c r="E47" t="n">
-        <v>1317429856</v>
+        <v>1476802660</v>
       </c>
       <c r="F47" t="n">
-        <v>68947999</v>
+        <v>131182539</v>
       </c>
       <c r="G47" t="n">
-        <v>-0.54709</v>
+        <v>2.71381</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>1.02</v>
+        <v>16.61</v>
       </c>
       <c r="E48" t="n">
-        <v>1303115892</v>
+        <v>1398934277</v>
       </c>
       <c r="F48" t="n">
-        <v>227473803</v>
+        <v>92506417</v>
       </c>
       <c r="G48" t="n">
-        <v>-0.44736</v>
+        <v>1.91013</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>AAVE</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Aave</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>88.33</v>
+        <v>0.147035</v>
       </c>
       <c r="E49" t="n">
-        <v>1296056485</v>
+        <v>1371488248</v>
       </c>
       <c r="F49" t="n">
-        <v>130091736</v>
+        <v>56695825</v>
       </c>
       <c r="G49" t="n">
-        <v>2.99954</v>
+        <v>-3.99781</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>3.42</v>
+        <v>1464.8</v>
       </c>
       <c r="E50" t="n">
-        <v>1285194729</v>
+        <v>1346583457</v>
       </c>
       <c r="F50" t="n">
-        <v>247908508</v>
+        <v>64790759</v>
       </c>
       <c r="G50" t="n">
-        <v>9.540710000000001</v>
+        <v>0.75963</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.131363</v>
+        <v>1.046</v>
       </c>
       <c r="E51" t="n">
-        <v>1226772951</v>
+        <v>1335801236</v>
       </c>
       <c r="F51" t="n">
-        <v>53392678</v>
+        <v>125533010</v>
       </c>
       <c r="G51" t="n">
-        <v>5.22045</v>
+        <v>-1.14785</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-12-03
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>37625</v>
+        <v>39495</v>
       </c>
       <c r="E2" t="n">
-        <v>736259302345</v>
+        <v>772518782873</v>
       </c>
       <c r="F2" t="n">
-        <v>3517346364</v>
+        <v>15307010795</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.22492</v>
+        <v>1.79578</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2079.34</v>
+        <v>2157.91</v>
       </c>
       <c r="E3" t="n">
-        <v>250171234092</v>
+        <v>259558614486</v>
       </c>
       <c r="F3" t="n">
-        <v>6903048294</v>
+        <v>16058033983</v>
       </c>
       <c r="G3" t="n">
-        <v>0.12591</v>
+        <v>2.50008</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>1.001</v>
       </c>
       <c r="E4" t="n">
-        <v>88749057889</v>
+        <v>89655985363</v>
       </c>
       <c r="F4" t="n">
-        <v>16309226426</v>
+        <v>29490113955</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.06523</v>
+        <v>-0.00565</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>233.52</v>
+        <v>228.16</v>
       </c>
       <c r="E5" t="n">
-        <v>35936092441</v>
+        <v>35109942764</v>
       </c>
       <c r="F5" t="n">
-        <v>326624169</v>
+        <v>566591965</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.11017</v>
+        <v>0.15644</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.635868</v>
+        <v>0.626402</v>
       </c>
       <c r="E6" t="n">
-        <v>34055784577</v>
+        <v>33742948711</v>
       </c>
       <c r="F6" t="n">
-        <v>673962406</v>
+        <v>775896413</v>
       </c>
       <c r="G6" t="n">
-        <v>2.64056</v>
+        <v>1.98595</v>
       </c>
     </row>
     <row r="7">
@@ -611,25 +611,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>USDC</t>
+          <t>SOL</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>USDC</t>
+          <t>Solana</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.999526</v>
+        <v>63.31</v>
       </c>
       <c r="E7" t="n">
-        <v>24692866617</v>
+        <v>26884038459</v>
       </c>
       <c r="F7" t="n">
-        <v>3454915825</v>
+        <v>1493532645</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.07556</v>
+        <v>1.70548</v>
       </c>
     </row>
     <row r="8">
@@ -638,25 +638,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SOL</t>
+          <t>USDC</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Solana</t>
+          <t>USDC</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>57.73</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>24447092537</v>
+        <v>24520889685</v>
       </c>
       <c r="F8" t="n">
-        <v>750421402</v>
+        <v>7462921120</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.54648</v>
+        <v>-0.01928</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2080.02</v>
+        <v>2156.92</v>
       </c>
       <c r="E9" t="n">
-        <v>19168159089</v>
+        <v>20025263480</v>
       </c>
       <c r="F9" t="n">
-        <v>5566434</v>
+        <v>12206808</v>
       </c>
       <c r="G9" t="n">
-        <v>0.36862</v>
+        <v>2.70264</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.389958</v>
+        <v>0.39372</v>
       </c>
       <c r="E10" t="n">
-        <v>13641644069</v>
+        <v>13779915710</v>
       </c>
       <c r="F10" t="n">
-        <v>204086224</v>
+        <v>281930639</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.02658</v>
+        <v>1.05876</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.077693</v>
+        <v>0.084936</v>
       </c>
       <c r="E11" t="n">
-        <v>11028564613</v>
+        <v>12071076492</v>
       </c>
       <c r="F11" t="n">
-        <v>320176930</v>
+        <v>711440186</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.57238</v>
+        <v>1.09001</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.108234</v>
+        <v>0.103278</v>
       </c>
       <c r="E12" t="n">
-        <v>9585065252</v>
+        <v>9139206937</v>
       </c>
       <c r="F12" t="n">
-        <v>345169432</v>
+        <v>296902443</v>
       </c>
       <c r="G12" t="n">
-        <v>2.81656</v>
+        <v>0.36781</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>15.08</v>
+        <v>16.04</v>
       </c>
       <c r="E13" t="n">
-        <v>8425946669</v>
+        <v>8915592446</v>
       </c>
       <c r="F13" t="n">
-        <v>416451209</v>
+        <v>628175606</v>
       </c>
       <c r="G13" t="n">
-        <v>1.76866</v>
+        <v>2.45334</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2.34</v>
+        <v>22</v>
       </c>
       <c r="E14" t="n">
-        <v>8158304662</v>
+        <v>8037567030</v>
       </c>
       <c r="F14" t="n">
-        <v>28675464</v>
+        <v>330663452</v>
       </c>
       <c r="G14" t="n">
-        <v>-1.68925</v>
+        <v>-0.26374</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>21</v>
+        <v>2.32</v>
       </c>
       <c r="E15" t="n">
-        <v>7664721349</v>
+        <v>8016239262</v>
       </c>
       <c r="F15" t="n">
-        <v>283746740</v>
+        <v>26926304</v>
       </c>
       <c r="G15" t="n">
-        <v>0.78611</v>
+        <v>-4.71039</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.772644</v>
+        <v>0.81019</v>
       </c>
       <c r="E16" t="n">
-        <v>7163367529</v>
+        <v>7515392716</v>
       </c>
       <c r="F16" t="n">
-        <v>279760699</v>
+        <v>469198570</v>
       </c>
       <c r="G16" t="n">
-        <v>0.05195</v>
+        <v>-0.29367</v>
       </c>
     </row>
     <row r="17">
@@ -890,16 +890,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>5.32</v>
+        <v>5.51</v>
       </c>
       <c r="E17" t="n">
-        <v>6929814098</v>
+        <v>7178365396</v>
       </c>
       <c r="F17" t="n">
-        <v>125154645</v>
+        <v>123917949</v>
       </c>
       <c r="G17" t="n">
-        <v>0.5367499999999999</v>
+        <v>-0.36889</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>37610</v>
+        <v>39439</v>
       </c>
       <c r="E18" t="n">
-        <v>6074201967</v>
+        <v>6320098194</v>
       </c>
       <c r="F18" t="n">
-        <v>69735164</v>
+        <v>126027439</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.16635</v>
+        <v>1.66095</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.998215</v>
+        <v>72.3</v>
       </c>
       <c r="E19" t="n">
-        <v>5343350641</v>
+        <v>5343801826</v>
       </c>
       <c r="F19" t="n">
-        <v>259647744</v>
+        <v>296141519</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.14416</v>
+        <v>0.8087299999999999</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>70.76000000000001</v>
+        <v>0.998915</v>
       </c>
       <c r="E20" t="n">
-        <v>5231368559</v>
+        <v>5327941206</v>
       </c>
       <c r="F20" t="n">
-        <v>202438192</v>
+        <v>314164095</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.47644</v>
+        <v>0.03063</v>
       </c>
     </row>
     <row r="21">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>8.31e-06</v>
+        <v>8.48e-06</v>
       </c>
       <c r="E21" t="n">
-        <v>4902843612</v>
+        <v>4993193171</v>
       </c>
       <c r="F21" t="n">
-        <v>114301831</v>
+        <v>148225909</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.02722</v>
+        <v>0.7681</v>
       </c>
     </row>
     <row r="22">
@@ -1025,16 +1025,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>6.05</v>
+        <v>6.18</v>
       </c>
       <c r="E22" t="n">
-        <v>4574283751</v>
+        <v>4658480190</v>
       </c>
       <c r="F22" t="n">
-        <v>189062114</v>
+        <v>249085885</v>
       </c>
       <c r="G22" t="n">
-        <v>-1.89668</v>
+        <v>0.42131</v>
       </c>
     </row>
     <row r="23">
@@ -1052,16 +1052,16 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>227.81</v>
+        <v>227.9</v>
       </c>
       <c r="E23" t="n">
-        <v>4460955545</v>
+        <v>4461502287</v>
       </c>
       <c r="F23" t="n">
-        <v>74078147</v>
+        <v>114129659</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.0746</v>
+        <v>0.28814</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>3.98</v>
+        <v>58.08</v>
       </c>
       <c r="E24" t="n">
-        <v>3694153322</v>
+        <v>3485569851</v>
       </c>
       <c r="F24" t="n">
-        <v>773897</v>
+        <v>11062413</v>
       </c>
       <c r="G24" t="n">
-        <v>0.50341</v>
+        <v>-0.41796</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>57.93</v>
+        <v>3.74</v>
       </c>
       <c r="E25" t="n">
-        <v>3480226996</v>
+        <v>3471061565</v>
       </c>
       <c r="F25" t="n">
-        <v>5335786</v>
+        <v>1460084</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.69929</v>
+        <v>-6.02915</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.122306</v>
+        <v>0.121997</v>
       </c>
       <c r="E26" t="n">
-        <v>3424261647</v>
+        <v>3419876393</v>
       </c>
       <c r="F26" t="n">
-        <v>64942610</v>
+        <v>51516454</v>
       </c>
       <c r="G26" t="n">
-        <v>0.9911</v>
+        <v>1.66959</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.997935</v>
+        <v>172.57</v>
       </c>
       <c r="E27" t="n">
-        <v>3166077989</v>
+        <v>3131879300</v>
       </c>
       <c r="F27" t="n">
-        <v>89159985</v>
+        <v>61509738</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.08445999999999999</v>
+        <v>-0.06211</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>170.93</v>
+        <v>0.138882</v>
       </c>
       <c r="E28" t="n">
-        <v>3097072361</v>
+        <v>3019095002</v>
       </c>
       <c r="F28" t="n">
-        <v>53908513</v>
+        <v>40140016</v>
       </c>
       <c r="G28" t="n">
-        <v>0.05869</v>
+        <v>1.12971</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>TUSD</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.132229</v>
+        <v>0.9994690000000001</v>
       </c>
       <c r="E29" t="n">
-        <v>2877422719</v>
+        <v>2954322170</v>
       </c>
       <c r="F29" t="n">
-        <v>38454528</v>
+        <v>143196884</v>
       </c>
       <c r="G29" t="n">
-        <v>-4.55337</v>
+        <v>-0.04414</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>9.630000000000001</v>
+        <v>19.62</v>
       </c>
       <c r="E30" t="n">
-        <v>2816881054</v>
+        <v>2810403759</v>
       </c>
       <c r="F30" t="n">
-        <v>180594648</v>
+        <v>125222865</v>
       </c>
       <c r="G30" t="n">
-        <v>7.14754</v>
+        <v>2.14564</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>19.3</v>
+        <v>9.52</v>
       </c>
       <c r="E31" t="n">
-        <v>2768898134</v>
+        <v>2785997675</v>
       </c>
       <c r="F31" t="n">
-        <v>77080672</v>
+        <v>119433190</v>
       </c>
       <c r="G31" t="n">
-        <v>0.05147</v>
+        <v>-0.38629</v>
       </c>
     </row>
     <row r="32">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.095499</v>
+        <v>0.092071</v>
       </c>
       <c r="E32" t="n">
-        <v>2518642602</v>
+        <v>2430527856</v>
       </c>
       <c r="F32" t="n">
-        <v>9855637</v>
+        <v>10056999</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.96205</v>
+        <v>0.69543</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>2.48</v>
+        <v>4.61</v>
       </c>
       <c r="E33" t="n">
-        <v>2210278660</v>
+        <v>2194137524</v>
       </c>
       <c r="F33" t="n">
-        <v>54562650</v>
+        <v>111528327</v>
       </c>
       <c r="G33" t="n">
-        <v>0.74139</v>
+        <v>1.38422</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>4.64</v>
+        <v>2.42</v>
       </c>
       <c r="E34" t="n">
-        <v>2197865478</v>
+        <v>2161051507</v>
       </c>
       <c r="F34" t="n">
-        <v>99172801</v>
+        <v>61064034</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.5920800000000001</v>
+        <v>1.07251</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.063441</v>
+        <v>4.7</v>
       </c>
       <c r="E35" t="n">
-        <v>2126752404</v>
+        <v>2116239363</v>
       </c>
       <c r="F35" t="n">
-        <v>31632008</v>
+        <v>31640207</v>
       </c>
       <c r="G35" t="n">
-        <v>0.79944</v>
+        <v>-1.23783</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>RUNE</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>THORChain</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>4.62</v>
+        <v>6.98</v>
       </c>
       <c r="E36" t="n">
-        <v>2077475492</v>
+        <v>2105945371</v>
       </c>
       <c r="F36" t="n">
-        <v>45637801</v>
+        <v>526307184</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.78127</v>
+        <v>-1.13234</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>7.31</v>
+        <v>0.062065</v>
       </c>
       <c r="E37" t="n">
-        <v>2025376564</v>
+        <v>2083333046</v>
       </c>
       <c r="F37" t="n">
-        <v>62320791</v>
+        <v>23556789</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.5928600000000001</v>
+        <v>0.54426</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1.86</v>
+        <v>7.36</v>
       </c>
       <c r="E38" t="n">
-        <v>1867777797</v>
+        <v>2046657856</v>
       </c>
       <c r="F38" t="n">
-        <v>126974564</v>
+        <v>87332896</v>
       </c>
       <c r="G38" t="n">
-        <v>1.20068</v>
+        <v>1.91829</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.999615</v>
+        <v>1.99</v>
       </c>
       <c r="E39" t="n">
-        <v>1740659335</v>
+        <v>1992663764</v>
       </c>
       <c r="F39" t="n">
-        <v>1163919679</v>
+        <v>136459021</v>
       </c>
       <c r="G39" t="n">
-        <v>-0.06347999999999999</v>
+        <v>-1.2216</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1.36</v>
+        <v>338.01</v>
       </c>
       <c r="E40" t="n">
-        <v>1709477315</v>
+        <v>1946366825</v>
       </c>
       <c r="F40" t="n">
-        <v>516895990</v>
+        <v>13869063</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.26468</v>
+        <v>17.26199</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.02332331</v>
+        <v>1.42</v>
       </c>
       <c r="E41" t="n">
-        <v>1694355234</v>
+        <v>1818049043</v>
       </c>
       <c r="F41" t="n">
-        <v>119369299</v>
+        <v>80758681</v>
       </c>
       <c r="G41" t="n">
-        <v>8.832420000000001</v>
+        <v>1.0308</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>RUNE</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>THORChain</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>5.34</v>
+        <v>0.5425140000000001</v>
       </c>
       <c r="E42" t="n">
-        <v>1607650362</v>
+        <v>1695251817</v>
       </c>
       <c r="F42" t="n">
-        <v>249071320</v>
+        <v>9834396</v>
       </c>
       <c r="G42" t="n">
-        <v>1.23576</v>
+        <v>-0.8942099999999999</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.514692</v>
+        <v>1</v>
       </c>
       <c r="E43" t="n">
-        <v>1595857577</v>
+        <v>1653773559</v>
       </c>
       <c r="F43" t="n">
-        <v>5899884</v>
+        <v>3266705450</v>
       </c>
       <c r="G43" t="n">
-        <v>0.75026</v>
+        <v>0.00735</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1.81</v>
+        <v>0.02255082</v>
       </c>
       <c r="E44" t="n">
-        <v>1591982737</v>
+        <v>1640638062</v>
       </c>
       <c r="F44" t="n">
-        <v>85305610</v>
+        <v>42908257</v>
       </c>
       <c r="G44" t="n">
-        <v>1.84431</v>
+        <v>-0.28369</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>267.08</v>
+        <v>1.73</v>
       </c>
       <c r="E45" t="n">
-        <v>1507931258</v>
+        <v>1570810069</v>
       </c>
       <c r="F45" t="n">
-        <v>6805136</v>
+        <v>113354116</v>
       </c>
       <c r="G45" t="n">
-        <v>-1.27712</v>
+        <v>1.37128</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>AAVE</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>Aave</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>103.35</v>
+        <v>102.35</v>
       </c>
       <c r="E46" t="n">
-        <v>1499940147</v>
+        <v>1502030180</v>
       </c>
       <c r="F46" t="n">
-        <v>29965834</v>
+        <v>101653170</v>
       </c>
       <c r="G46" t="n">
-        <v>2.68999</v>
+        <v>-0.43851</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>AAVE</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Aave</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>100.67</v>
+        <v>17.81</v>
       </c>
       <c r="E47" t="n">
-        <v>1476802660</v>
+        <v>1500172413</v>
       </c>
       <c r="F47" t="n">
-        <v>131182539</v>
+        <v>98274773</v>
       </c>
       <c r="G47" t="n">
-        <v>2.71381</v>
+        <v>-1.83675</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>16.61</v>
+        <v>100.7</v>
       </c>
       <c r="E48" t="n">
-        <v>1398934277</v>
+        <v>1464908269</v>
       </c>
       <c r="F48" t="n">
-        <v>92506417</v>
+        <v>23279856</v>
       </c>
       <c r="G48" t="n">
-        <v>1.91013</v>
+        <v>0.0106</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.147035</v>
+        <v>1.1</v>
       </c>
       <c r="E49" t="n">
-        <v>1371488248</v>
+        <v>1404340942</v>
       </c>
       <c r="F49" t="n">
-        <v>56695825</v>
+        <v>264011806</v>
       </c>
       <c r="G49" t="n">
-        <v>-3.99781</v>
+        <v>2.29868</v>
       </c>
     </row>
     <row r="50">
@@ -1781,16 +1781,16 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>1464.8</v>
+        <v>1524.39</v>
       </c>
       <c r="E50" t="n">
-        <v>1346583457</v>
+        <v>1401150682</v>
       </c>
       <c r="F50" t="n">
-        <v>64790759</v>
+        <v>63798098</v>
       </c>
       <c r="G50" t="n">
-        <v>0.75963</v>
+        <v>-0.35539</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>1.046</v>
+        <v>0.149269</v>
       </c>
       <c r="E51" t="n">
-        <v>1335801236</v>
+        <v>1391613627</v>
       </c>
       <c r="F51" t="n">
-        <v>125533010</v>
+        <v>41776832</v>
       </c>
       <c r="G51" t="n">
-        <v>-1.14785</v>
+        <v>-0.82706</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-12-10
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>39495</v>
+        <v>43786</v>
       </c>
       <c r="E2" t="n">
-        <v>772518782873</v>
+        <v>856663314701</v>
       </c>
       <c r="F2" t="n">
-        <v>15307010795</v>
+        <v>13429325067</v>
       </c>
       <c r="G2" t="n">
-        <v>1.79578</v>
+        <v>-0.05802</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2157.91</v>
+        <v>2342.8</v>
       </c>
       <c r="E3" t="n">
-        <v>259558614486</v>
+        <v>281679393489</v>
       </c>
       <c r="F3" t="n">
-        <v>16058033983</v>
+        <v>11447335822</v>
       </c>
       <c r="G3" t="n">
-        <v>2.50008</v>
+        <v>-0.53816</v>
       </c>
     </row>
     <row r="4">
@@ -542,13 +542,13 @@
         <v>1.001</v>
       </c>
       <c r="E4" t="n">
-        <v>89655985363</v>
+        <v>90634565590</v>
       </c>
       <c r="F4" t="n">
-        <v>29490113955</v>
+        <v>32628239434</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.00565</v>
+        <v>0.0265</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>228.16</v>
+        <v>239.15</v>
       </c>
       <c r="E5" t="n">
-        <v>35109942764</v>
+        <v>36771511247</v>
       </c>
       <c r="F5" t="n">
-        <v>566591965</v>
+        <v>663402131</v>
       </c>
       <c r="G5" t="n">
-        <v>0.15644</v>
+        <v>-1.2681</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.626402</v>
+        <v>0.659102</v>
       </c>
       <c r="E6" t="n">
-        <v>33742948711</v>
+        <v>35544704216</v>
       </c>
       <c r="F6" t="n">
-        <v>775896413</v>
+        <v>1390707472</v>
       </c>
       <c r="G6" t="n">
-        <v>1.98595</v>
+        <v>-3.71253</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>63.31</v>
+        <v>72.17</v>
       </c>
       <c r="E7" t="n">
-        <v>26884038459</v>
+        <v>30721567472</v>
       </c>
       <c r="F7" t="n">
-        <v>1493532645</v>
+        <v>2248614651</v>
       </c>
       <c r="G7" t="n">
-        <v>1.70548</v>
+        <v>-6.31586</v>
       </c>
     </row>
     <row r="8">
@@ -650,13 +650,13 @@
         <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>24520889685</v>
+        <v>24551289562</v>
       </c>
       <c r="F8" t="n">
-        <v>7462921120</v>
+        <v>6588430696</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.01928</v>
+        <v>-0.08277</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2156.92</v>
+        <v>2339.66</v>
       </c>
       <c r="E9" t="n">
-        <v>20025263480</v>
+        <v>21581083249</v>
       </c>
       <c r="F9" t="n">
-        <v>12206808</v>
+        <v>24010751</v>
       </c>
       <c r="G9" t="n">
-        <v>2.70264</v>
+        <v>-0.42705</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.39372</v>
+        <v>0.596977</v>
       </c>
       <c r="E10" t="n">
-        <v>13779915710</v>
+        <v>20821338858</v>
       </c>
       <c r="F10" t="n">
-        <v>281930639</v>
+        <v>1544977249</v>
       </c>
       <c r="G10" t="n">
-        <v>1.05876</v>
+        <v>-5.00953</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.084936</v>
+        <v>0.099148</v>
       </c>
       <c r="E11" t="n">
-        <v>12071076492</v>
+        <v>14084536479</v>
       </c>
       <c r="F11" t="n">
-        <v>711440186</v>
+        <v>1147059410</v>
       </c>
       <c r="G11" t="n">
-        <v>1.09001</v>
+        <v>-2.57604</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +746,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.103278</v>
+        <v>32.56</v>
       </c>
       <c r="E12" t="n">
-        <v>9139206937</v>
+        <v>11867937817</v>
       </c>
       <c r="F12" t="n">
-        <v>296902443</v>
+        <v>1202243194</v>
       </c>
       <c r="G12" t="n">
-        <v>0.36781</v>
+        <v>-3.29568</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>16.04</v>
+        <v>0.107163</v>
       </c>
       <c r="E13" t="n">
-        <v>8915592446</v>
+        <v>9483396758</v>
       </c>
       <c r="F13" t="n">
-        <v>628175606</v>
+        <v>342331969</v>
       </c>
       <c r="G13" t="n">
-        <v>2.45334</v>
+        <v>-0.56198</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>22</v>
+        <v>7.2</v>
       </c>
       <c r="E14" t="n">
-        <v>8037567030</v>
+        <v>9371740976</v>
       </c>
       <c r="F14" t="n">
-        <v>330663452</v>
+        <v>385992652</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.26374</v>
+        <v>-5.29052</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>2.32</v>
+        <v>16.03</v>
       </c>
       <c r="E15" t="n">
-        <v>8016239262</v>
+        <v>8908056779</v>
       </c>
       <c r="F15" t="n">
-        <v>26926304</v>
+        <v>711143092</v>
       </c>
       <c r="G15" t="n">
-        <v>-4.71039</v>
+        <v>-5.41228</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.81019</v>
+        <v>0.898182</v>
       </c>
       <c r="E16" t="n">
-        <v>7515392716</v>
+        <v>8338188820</v>
       </c>
       <c r="F16" t="n">
-        <v>469198570</v>
+        <v>610106446</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.29367</v>
+        <v>-3.12373</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>5.51</v>
+        <v>2.31</v>
       </c>
       <c r="E17" t="n">
-        <v>7178365396</v>
+        <v>8121723900</v>
       </c>
       <c r="F17" t="n">
-        <v>123917949</v>
+        <v>11666911</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.36889</v>
+        <v>-0.64437</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>39439</v>
+        <v>43741</v>
       </c>
       <c r="E18" t="n">
-        <v>6320098194</v>
+        <v>6766780585</v>
       </c>
       <c r="F18" t="n">
-        <v>126027439</v>
+        <v>149131786</v>
       </c>
       <c r="G18" t="n">
-        <v>1.66095</v>
+        <v>0.15431</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>72.3</v>
+        <v>1.007e-05</v>
       </c>
       <c r="E19" t="n">
-        <v>5343801826</v>
+        <v>5932161616</v>
       </c>
       <c r="F19" t="n">
-        <v>296141519</v>
+        <v>446837436</v>
       </c>
       <c r="G19" t="n">
-        <v>0.8087299999999999</v>
+        <v>-1.77626</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.998915</v>
+        <v>77.70999999999999</v>
       </c>
       <c r="E20" t="n">
-        <v>5327941206</v>
+        <v>5750231658</v>
       </c>
       <c r="F20" t="n">
-        <v>314164095</v>
+        <v>782209266</v>
       </c>
       <c r="G20" t="n">
-        <v>0.03063</v>
+        <v>0.08064</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>8.48e-06</v>
+        <v>1</v>
       </c>
       <c r="E21" t="n">
-        <v>4993193171</v>
+        <v>5423264512</v>
       </c>
       <c r="F21" t="n">
-        <v>148225909</v>
+        <v>249835221</v>
       </c>
       <c r="G21" t="n">
-        <v>0.7681</v>
+        <v>0.00762</v>
       </c>
     </row>
     <row r="22">
@@ -1025,16 +1025,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>6.18</v>
+        <v>6.62</v>
       </c>
       <c r="E22" t="n">
-        <v>4658480190</v>
+        <v>4987631838</v>
       </c>
       <c r="F22" t="n">
-        <v>249085885</v>
+        <v>232568980</v>
       </c>
       <c r="G22" t="n">
-        <v>0.42131</v>
+        <v>-0.98506</v>
       </c>
     </row>
     <row r="23">
@@ -1052,16 +1052,16 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>227.9</v>
+        <v>248.9</v>
       </c>
       <c r="E23" t="n">
-        <v>4461502287</v>
+        <v>4869103156</v>
       </c>
       <c r="F23" t="n">
-        <v>114129659</v>
+        <v>149665351</v>
       </c>
       <c r="G23" t="n">
-        <v>0.28814</v>
+        <v>-2.48626</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>58.08</v>
+        <v>0.132588</v>
       </c>
       <c r="E24" t="n">
-        <v>3485569851</v>
+        <v>3735848768</v>
       </c>
       <c r="F24" t="n">
-        <v>11062413</v>
+        <v>97186014</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.41796</v>
+        <v>-1.80773</v>
       </c>
     </row>
     <row r="25">
@@ -1106,16 +1106,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>3.74</v>
+        <v>3.79</v>
       </c>
       <c r="E25" t="n">
-        <v>3471061565</v>
+        <v>3520894905</v>
       </c>
       <c r="F25" t="n">
-        <v>1460084</v>
+        <v>1143483</v>
       </c>
       <c r="G25" t="n">
-        <v>-6.02915</v>
+        <v>-0.16781</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.121997</v>
+        <v>58.12</v>
       </c>
       <c r="E26" t="n">
-        <v>3419876393</v>
+        <v>3484801297</v>
       </c>
       <c r="F26" t="n">
-        <v>51516454</v>
+        <v>46371021</v>
       </c>
       <c r="G26" t="n">
-        <v>1.66959</v>
+        <v>1.2512</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>172.57</v>
+        <v>176.89</v>
       </c>
       <c r="E27" t="n">
-        <v>3131879300</v>
+        <v>3202302250</v>
       </c>
       <c r="F27" t="n">
-        <v>61509738</v>
+        <v>68883053</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.06211</v>
+        <v>0.7456700000000001</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.138882</v>
+        <v>21.88</v>
       </c>
       <c r="E28" t="n">
-        <v>3019095002</v>
+        <v>3130812756</v>
       </c>
       <c r="F28" t="n">
-        <v>40140016</v>
+        <v>197032243</v>
       </c>
       <c r="G28" t="n">
-        <v>1.12971</v>
+        <v>-3.20925</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.9994690000000001</v>
+        <v>10.29</v>
       </c>
       <c r="E29" t="n">
-        <v>2954322170</v>
+        <v>3007229065</v>
       </c>
       <c r="F29" t="n">
-        <v>143196884</v>
+        <v>175846988</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.04414</v>
+        <v>-6.37044</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>19.62</v>
+        <v>0.105902</v>
       </c>
       <c r="E30" t="n">
-        <v>2810403759</v>
+        <v>2801076291</v>
       </c>
       <c r="F30" t="n">
-        <v>125222865</v>
+        <v>51937612</v>
       </c>
       <c r="G30" t="n">
-        <v>2.14564</v>
+        <v>-0.19628</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>9.52</v>
+        <v>0.125818</v>
       </c>
       <c r="E31" t="n">
-        <v>2785997675</v>
+        <v>2740235633</v>
       </c>
       <c r="F31" t="n">
-        <v>119433190</v>
+        <v>30193224</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.38629</v>
+        <v>-2.3427</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>TUSD</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.092071</v>
+        <v>0.998962</v>
       </c>
       <c r="E32" t="n">
-        <v>2430527856</v>
+        <v>2630853649</v>
       </c>
       <c r="F32" t="n">
-        <v>10056999</v>
+        <v>126764272</v>
       </c>
       <c r="G32" t="n">
-        <v>0.69543</v>
+        <v>0.26312</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>4.61</v>
+        <v>0.073156</v>
       </c>
       <c r="E33" t="n">
-        <v>2194137524</v>
+        <v>2454658936</v>
       </c>
       <c r="F33" t="n">
-        <v>111528327</v>
+        <v>63871760</v>
       </c>
       <c r="G33" t="n">
-        <v>1.38422</v>
+        <v>-4.00019</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>2.42</v>
+        <v>5.09</v>
       </c>
       <c r="E34" t="n">
-        <v>2161051507</v>
+        <v>2428199572</v>
       </c>
       <c r="F34" t="n">
-        <v>61064034</v>
+        <v>224424030</v>
       </c>
       <c r="G34" t="n">
-        <v>1.07251</v>
+        <v>-5.33712</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>4.7</v>
+        <v>2.41</v>
       </c>
       <c r="E35" t="n">
-        <v>2116239363</v>
+        <v>2420473466</v>
       </c>
       <c r="F35" t="n">
-        <v>31640207</v>
+        <v>250522557</v>
       </c>
       <c r="G35" t="n">
-        <v>-1.23783</v>
+        <v>-4.86508</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>RUNE</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>THORChain</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>6.98</v>
+        <v>5.34</v>
       </c>
       <c r="E36" t="n">
-        <v>2105945371</v>
+        <v>2402137200</v>
       </c>
       <c r="F36" t="n">
-        <v>526307184</v>
+        <v>67952558</v>
       </c>
       <c r="G36" t="n">
-        <v>-1.13234</v>
+        <v>-1.12428</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.062065</v>
+        <v>1.83</v>
       </c>
       <c r="E37" t="n">
-        <v>2083333046</v>
+        <v>2351447661</v>
       </c>
       <c r="F37" t="n">
-        <v>23556789</v>
+        <v>1308624556</v>
       </c>
       <c r="G37" t="n">
-        <v>0.54426</v>
+        <v>2.90395</v>
       </c>
     </row>
     <row r="38">
@@ -1457,16 +1457,16 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>7.36</v>
+        <v>8.18</v>
       </c>
       <c r="E38" t="n">
-        <v>2046657856</v>
+        <v>2284748587</v>
       </c>
       <c r="F38" t="n">
-        <v>87332896</v>
+        <v>145919568</v>
       </c>
       <c r="G38" t="n">
-        <v>1.91829</v>
+        <v>-4.86736</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1.99</v>
+        <v>2.37</v>
       </c>
       <c r="E39" t="n">
-        <v>1992663764</v>
+        <v>2103184514</v>
       </c>
       <c r="F39" t="n">
-        <v>136459021</v>
+        <v>55662851</v>
       </c>
       <c r="G39" t="n">
-        <v>-1.2216</v>
+        <v>-2.88263</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>338.01</v>
+        <v>2.2</v>
       </c>
       <c r="E40" t="n">
-        <v>1946366825</v>
+        <v>1992984289</v>
       </c>
       <c r="F40" t="n">
-        <v>13869063</v>
+        <v>291256819</v>
       </c>
       <c r="G40" t="n">
-        <v>17.26199</v>
+        <v>4.25876</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1.42</v>
+        <v>0.02687952</v>
       </c>
       <c r="E41" t="n">
-        <v>1818049043</v>
+        <v>1952221059</v>
       </c>
       <c r="F41" t="n">
-        <v>80758681</v>
+        <v>59769243</v>
       </c>
       <c r="G41" t="n">
-        <v>1.0308</v>
+        <v>-2.54601</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.5425140000000001</v>
+        <v>335.69</v>
       </c>
       <c r="E42" t="n">
-        <v>1695251817</v>
+        <v>1950759039</v>
       </c>
       <c r="F42" t="n">
-        <v>9834396</v>
+        <v>4056577</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.8942099999999999</v>
+        <v>-1.0043</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>RUNE</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>THORChain</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1</v>
+        <v>6.39</v>
       </c>
       <c r="E43" t="n">
-        <v>1653773559</v>
+        <v>1918702746</v>
       </c>
       <c r="F43" t="n">
-        <v>3266705450</v>
+        <v>416539843</v>
       </c>
       <c r="G43" t="n">
-        <v>0.00735</v>
+        <v>-1.1742</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.02255082</v>
+        <v>0.606142</v>
       </c>
       <c r="E44" t="n">
-        <v>1640638062</v>
+        <v>1899717987</v>
       </c>
       <c r="F44" t="n">
-        <v>42908257</v>
+        <v>6424115</v>
       </c>
       <c r="G44" t="n">
-        <v>-0.28369</v>
+        <v>-2.71496</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>EGLD</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>MultiversX</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>1.73</v>
+        <v>64.55</v>
       </c>
       <c r="E45" t="n">
-        <v>1570810069</v>
+        <v>1702130997</v>
       </c>
       <c r="F45" t="n">
-        <v>113354116</v>
+        <v>163415276</v>
       </c>
       <c r="G45" t="n">
-        <v>1.37128</v>
+        <v>15.21462</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>AAVE</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Aave</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>102.35</v>
+        <v>115.47</v>
       </c>
       <c r="E46" t="n">
-        <v>1502030180</v>
+        <v>1677477962</v>
       </c>
       <c r="F46" t="n">
-        <v>101653170</v>
+        <v>30136318</v>
       </c>
       <c r="G46" t="n">
-        <v>-0.43851</v>
+        <v>-2.6346</v>
       </c>
     </row>
     <row r="47">
@@ -1700,16 +1700,16 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>17.81</v>
+        <v>18.84</v>
       </c>
       <c r="E47" t="n">
-        <v>1500172413</v>
+        <v>1581668185</v>
       </c>
       <c r="F47" t="n">
-        <v>98274773</v>
+        <v>94653951</v>
       </c>
       <c r="G47" t="n">
-        <v>-1.83675</v>
+        <v>-2.69951</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>100.7</v>
+        <v>0.168841</v>
       </c>
       <c r="E48" t="n">
-        <v>1464908269</v>
+        <v>1572126142</v>
       </c>
       <c r="F48" t="n">
-        <v>23279856</v>
+        <v>74881659</v>
       </c>
       <c r="G48" t="n">
-        <v>0.0106</v>
+        <v>-1.58061</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>ALGO</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Algorand</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>1.1</v>
+        <v>0.193841</v>
       </c>
       <c r="E49" t="n">
-        <v>1404340942</v>
+        <v>1546298373</v>
       </c>
       <c r="F49" t="n">
-        <v>264011806</v>
+        <v>212675441</v>
       </c>
       <c r="G49" t="n">
-        <v>2.29868</v>
+        <v>-4.17292</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>BUSD</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>1524.39</v>
+        <v>1</v>
       </c>
       <c r="E50" t="n">
-        <v>1401150682</v>
+        <v>1506606703</v>
       </c>
       <c r="F50" t="n">
-        <v>63798098</v>
+        <v>2040555489</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.35539</v>
+        <v>0.03979</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.149269</v>
+        <v>1.14</v>
       </c>
       <c r="E51" t="n">
-        <v>1391613627</v>
+        <v>1448577421</v>
       </c>
       <c r="F51" t="n">
-        <v>41776832</v>
+        <v>375115468</v>
       </c>
       <c r="G51" t="n">
-        <v>-0.82706</v>
+        <v>-4.03384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-12-17
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>43786</v>
+        <v>41903</v>
       </c>
       <c r="E2" t="n">
-        <v>856663314701</v>
+        <v>819830538014</v>
       </c>
       <c r="F2" t="n">
-        <v>13429325067</v>
+        <v>11986194231</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.05802</v>
+        <v>-0.93288</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2342.8</v>
+        <v>2215.2</v>
       </c>
       <c r="E3" t="n">
-        <v>281679393489</v>
+        <v>265963134104</v>
       </c>
       <c r="F3" t="n">
-        <v>11447335822</v>
+        <v>7828168667</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.53816</v>
+        <v>-1.48965</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1.001</v>
+        <v>0.999436</v>
       </c>
       <c r="E4" t="n">
-        <v>90634565590</v>
+        <v>90850654807</v>
       </c>
       <c r="F4" t="n">
-        <v>32628239434</v>
+        <v>28581861881</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0265</v>
+        <v>0.0507</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>239.15</v>
+        <v>241.3</v>
       </c>
       <c r="E5" t="n">
-        <v>36771511247</v>
+        <v>37104049349</v>
       </c>
       <c r="F5" t="n">
-        <v>663402131</v>
+        <v>540505107</v>
       </c>
       <c r="G5" t="n">
-        <v>-1.2681</v>
+        <v>-2.17504</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.659102</v>
+        <v>0.618808</v>
       </c>
       <c r="E6" t="n">
-        <v>35544704216</v>
+        <v>33380399594</v>
       </c>
       <c r="F6" t="n">
-        <v>1390707472</v>
+        <v>744026594</v>
       </c>
       <c r="G6" t="n">
-        <v>-3.71253</v>
+        <v>-0.72162</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>72.17</v>
+        <v>72.72</v>
       </c>
       <c r="E7" t="n">
-        <v>30721567472</v>
+        <v>31082596893</v>
       </c>
       <c r="F7" t="n">
-        <v>2248614651</v>
+        <v>1609319506</v>
       </c>
       <c r="G7" t="n">
-        <v>-6.31586</v>
+        <v>-3.14503</v>
       </c>
     </row>
     <row r="8">
@@ -650,13 +650,13 @@
         <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>24551289562</v>
+        <v>24629116934</v>
       </c>
       <c r="F8" t="n">
-        <v>6588430696</v>
+        <v>4662777447</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.08277</v>
+        <v>-0.04887</v>
       </c>
     </row>
     <row r="9">
@@ -665,25 +665,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>STETH</t>
+          <t>ADA</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Lido Staked Ether</t>
+          <t>Cardano</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2339.66</v>
+        <v>0.598587</v>
       </c>
       <c r="E9" t="n">
-        <v>21581083249</v>
+        <v>20918001986</v>
       </c>
       <c r="F9" t="n">
-        <v>24010751</v>
+        <v>521318006</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.42705</v>
+        <v>-2.58032</v>
       </c>
     </row>
     <row r="10">
@@ -692,25 +692,25 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ADA</t>
+          <t>STETH</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Cardano</t>
+          <t>Lido Staked Ether</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.596977</v>
+        <v>2212.43</v>
       </c>
       <c r="E10" t="n">
-        <v>20821338858</v>
+        <v>20363989148</v>
       </c>
       <c r="F10" t="n">
-        <v>1544977249</v>
+        <v>33663356</v>
       </c>
       <c r="G10" t="n">
-        <v>-5.00953</v>
+        <v>-1.58137</v>
       </c>
     </row>
     <row r="11">
@@ -719,25 +719,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>DOGE</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Dogecoin</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.099148</v>
+        <v>41.95</v>
       </c>
       <c r="E11" t="n">
-        <v>14084536479</v>
+        <v>15378544016</v>
       </c>
       <c r="F11" t="n">
-        <v>1147059410</v>
+        <v>1663507734</v>
       </c>
       <c r="G11" t="n">
-        <v>-2.57604</v>
+        <v>-3.43542</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +746,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>DOGE</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Dogecoin</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>32.56</v>
+        <v>0.095038</v>
       </c>
       <c r="E12" t="n">
-        <v>11867937817</v>
+        <v>13491081604</v>
       </c>
       <c r="F12" t="n">
-        <v>1202243194</v>
+        <v>718179527</v>
       </c>
       <c r="G12" t="n">
-        <v>-3.29568</v>
+        <v>0.87824</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.107163</v>
+        <v>6.98</v>
       </c>
       <c r="E13" t="n">
-        <v>9483396758</v>
+        <v>9113772784</v>
       </c>
       <c r="F13" t="n">
-        <v>342331969</v>
+        <v>290157745</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.56198</v>
+        <v>-2.58047</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>7.2</v>
+        <v>0.103019</v>
       </c>
       <c r="E14" t="n">
-        <v>9371740976</v>
+        <v>9096921069</v>
       </c>
       <c r="F14" t="n">
-        <v>385992652</v>
+        <v>316781809</v>
       </c>
       <c r="G14" t="n">
-        <v>-5.29052</v>
+        <v>0.32609</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>16.03</v>
+        <v>14.19</v>
       </c>
       <c r="E15" t="n">
-        <v>8908056779</v>
+        <v>7888449740</v>
       </c>
       <c r="F15" t="n">
-        <v>711143092</v>
+        <v>397109911</v>
       </c>
       <c r="G15" t="n">
-        <v>-5.41228</v>
+        <v>-2.43447</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.898182</v>
+        <v>0.832436</v>
       </c>
       <c r="E16" t="n">
-        <v>8338188820</v>
+        <v>7715664850</v>
       </c>
       <c r="F16" t="n">
-        <v>610106446</v>
+        <v>296001104</v>
       </c>
       <c r="G16" t="n">
-        <v>-3.12373</v>
+        <v>-2.53698</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2.31</v>
+        <v>41832</v>
       </c>
       <c r="E17" t="n">
-        <v>8121723900</v>
+        <v>6469794031</v>
       </c>
       <c r="F17" t="n">
-        <v>11666911</v>
+        <v>76901311</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.64437</v>
+        <v>-1.04351</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>43741</v>
+        <v>1.073e-05</v>
       </c>
       <c r="E18" t="n">
-        <v>6766780585</v>
+        <v>6284307348</v>
       </c>
       <c r="F18" t="n">
-        <v>149131786</v>
+        <v>842700935</v>
       </c>
       <c r="G18" t="n">
-        <v>0.15431</v>
+        <v>7.09315</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1.007e-05</v>
+        <v>72.55</v>
       </c>
       <c r="E19" t="n">
-        <v>5932161616</v>
+        <v>5356673447</v>
       </c>
       <c r="F19" t="n">
-        <v>446837436</v>
+        <v>465843609</v>
       </c>
       <c r="G19" t="n">
-        <v>-1.77626</v>
+        <v>0.43497</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>77.70999999999999</v>
+        <v>0.997801</v>
       </c>
       <c r="E20" t="n">
-        <v>5750231658</v>
+        <v>5271229056</v>
       </c>
       <c r="F20" t="n">
-        <v>782209266</v>
+        <v>199752100</v>
       </c>
       <c r="G20" t="n">
-        <v>0.08064</v>
+        <v>-0.07549</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>11.05</v>
       </c>
       <c r="E21" t="n">
-        <v>5423264512</v>
+        <v>4894968201</v>
       </c>
       <c r="F21" t="n">
-        <v>249835221</v>
+        <v>708763029</v>
       </c>
       <c r="G21" t="n">
-        <v>0.00762</v>
+        <v>20.67143</v>
       </c>
     </row>
     <row r="22">
@@ -1025,16 +1025,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>6.62</v>
+        <v>6.2</v>
       </c>
       <c r="E22" t="n">
-        <v>4987631838</v>
+        <v>4662259783</v>
       </c>
       <c r="F22" t="n">
-        <v>232568980</v>
+        <v>164051700</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.98506</v>
+        <v>0.39648</v>
       </c>
     </row>
     <row r="23">
@@ -1052,16 +1052,16 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>248.9</v>
+        <v>228.55</v>
       </c>
       <c r="E23" t="n">
-        <v>4869103156</v>
+        <v>4473661291</v>
       </c>
       <c r="F23" t="n">
-        <v>149665351</v>
+        <v>116735430</v>
       </c>
       <c r="G23" t="n">
-        <v>-2.48626</v>
+        <v>-0.80994</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.132588</v>
+        <v>3.79</v>
       </c>
       <c r="E24" t="n">
-        <v>3735848768</v>
+        <v>3513093157</v>
       </c>
       <c r="F24" t="n">
-        <v>97186014</v>
+        <v>924406</v>
       </c>
       <c r="G24" t="n">
-        <v>-1.80773</v>
+        <v>0.47316</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>3.79</v>
+        <v>0.12429</v>
       </c>
       <c r="E25" t="n">
-        <v>3520894905</v>
+        <v>3501286906</v>
       </c>
       <c r="F25" t="n">
-        <v>1143483</v>
+        <v>61499931</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.16781</v>
+        <v>-0.5351900000000001</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>58.12</v>
+        <v>57.27</v>
       </c>
       <c r="E26" t="n">
-        <v>3484801297</v>
+        <v>3437124414</v>
       </c>
       <c r="F26" t="n">
-        <v>46371021</v>
+        <v>10572128</v>
       </c>
       <c r="G26" t="n">
-        <v>1.2512</v>
+        <v>-0.8827199999999999</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>176.89</v>
+        <v>11.62</v>
       </c>
       <c r="E27" t="n">
-        <v>3202302250</v>
+        <v>3412192174</v>
       </c>
       <c r="F27" t="n">
-        <v>68883053</v>
+        <v>285810926</v>
       </c>
       <c r="G27" t="n">
-        <v>0.7456700000000001</v>
+        <v>1.79435</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>21.88</v>
+        <v>169.42</v>
       </c>
       <c r="E28" t="n">
-        <v>3130812756</v>
+        <v>3070847929</v>
       </c>
       <c r="F28" t="n">
-        <v>197032243</v>
+        <v>64575945</v>
       </c>
       <c r="G28" t="n">
-        <v>-3.20925</v>
+        <v>-1.35297</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>10.29</v>
+        <v>20.21</v>
       </c>
       <c r="E29" t="n">
-        <v>3007229065</v>
+        <v>2884407004</v>
       </c>
       <c r="F29" t="n">
-        <v>175846988</v>
+        <v>94711177</v>
       </c>
       <c r="G29" t="n">
-        <v>-6.37044</v>
+        <v>-0.78112</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.105902</v>
+        <v>5.68</v>
       </c>
       <c r="E30" t="n">
-        <v>2801076291</v>
+        <v>2761809364</v>
       </c>
       <c r="F30" t="n">
-        <v>51937612</v>
+        <v>851350434</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.19628</v>
+        <v>5.75791</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.125818</v>
+        <v>0.079457</v>
       </c>
       <c r="E31" t="n">
-        <v>2740235633</v>
+        <v>2660696932</v>
       </c>
       <c r="F31" t="n">
-        <v>30193224</v>
+        <v>65957945</v>
       </c>
       <c r="G31" t="n">
-        <v>-2.3427</v>
+        <v>-3.12502</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.998962</v>
+        <v>0.099772</v>
       </c>
       <c r="E32" t="n">
-        <v>2630853649</v>
+        <v>2636325655</v>
       </c>
       <c r="F32" t="n">
-        <v>126764272</v>
+        <v>11076988</v>
       </c>
       <c r="G32" t="n">
-        <v>0.26312</v>
+        <v>-2.29744</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.073156</v>
+        <v>2.03</v>
       </c>
       <c r="E33" t="n">
-        <v>2454658936</v>
+        <v>2613492214</v>
       </c>
       <c r="F33" t="n">
-        <v>63871760</v>
+        <v>158354376</v>
       </c>
       <c r="G33" t="n">
-        <v>-4.00019</v>
+        <v>-6.52462</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>5.09</v>
+        <v>30.14</v>
       </c>
       <c r="E34" t="n">
-        <v>2428199572</v>
+        <v>2530781982</v>
       </c>
       <c r="F34" t="n">
-        <v>224424030</v>
+        <v>251068783</v>
       </c>
       <c r="G34" t="n">
-        <v>-5.33712</v>
+        <v>-2.50865</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>2.41</v>
+        <v>8.17</v>
       </c>
       <c r="E35" t="n">
-        <v>2420473466</v>
+        <v>2483820305</v>
       </c>
       <c r="F35" t="n">
-        <v>250522557</v>
+        <v>139336047</v>
       </c>
       <c r="G35" t="n">
-        <v>-4.86508</v>
+        <v>-1.90593</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>TUSD</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>5.34</v>
+        <v>0.996213</v>
       </c>
       <c r="E36" t="n">
-        <v>2402137200</v>
+        <v>2431725952</v>
       </c>
       <c r="F36" t="n">
-        <v>67952558</v>
+        <v>127083746</v>
       </c>
       <c r="G36" t="n">
-        <v>-1.12428</v>
+        <v>-0.24066</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1.83</v>
+        <v>0.109192</v>
       </c>
       <c r="E37" t="n">
-        <v>2351447661</v>
+        <v>2382753721</v>
       </c>
       <c r="F37" t="n">
-        <v>1308624556</v>
+        <v>47991154</v>
       </c>
       <c r="G37" t="n">
-        <v>2.90395</v>
+        <v>-10.27094</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>8.18</v>
+        <v>2.37</v>
       </c>
       <c r="E38" t="n">
-        <v>2284748587</v>
+        <v>2382299533</v>
       </c>
       <c r="F38" t="n">
-        <v>145919568</v>
+        <v>215167572</v>
       </c>
       <c r="G38" t="n">
-        <v>-4.86736</v>
+        <v>2.44583</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>2.37</v>
+        <v>0.02983601</v>
       </c>
       <c r="E39" t="n">
-        <v>2103184514</v>
+        <v>2166426628</v>
       </c>
       <c r="F39" t="n">
-        <v>55662851</v>
+        <v>55024016</v>
       </c>
       <c r="G39" t="n">
-        <v>-2.88263</v>
+        <v>-3.7473</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>TIA</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Celestia</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>2.2</v>
+        <v>13.65</v>
       </c>
       <c r="E40" t="n">
-        <v>1992984289</v>
+        <v>1986988583</v>
       </c>
       <c r="F40" t="n">
-        <v>291256819</v>
+        <v>319276355</v>
       </c>
       <c r="G40" t="n">
-        <v>4.25876</v>
+        <v>-0.93387</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.02687952</v>
+        <v>2.12</v>
       </c>
       <c r="E41" t="n">
-        <v>1952221059</v>
+        <v>1928913091</v>
       </c>
       <c r="F41" t="n">
-        <v>59769243</v>
+        <v>222874379</v>
       </c>
       <c r="G41" t="n">
-        <v>-2.54601</v>
+        <v>-1.929</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>335.69</v>
+        <v>2.12</v>
       </c>
       <c r="E42" t="n">
-        <v>1950759039</v>
+        <v>1879284878</v>
       </c>
       <c r="F42" t="n">
-        <v>4056577</v>
+        <v>46221938</v>
       </c>
       <c r="G42" t="n">
-        <v>-1.0043</v>
+        <v>-3.26419</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>RUNE</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>THORChain</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>6.39</v>
+        <v>316.42</v>
       </c>
       <c r="E43" t="n">
-        <v>1918702746</v>
+        <v>1856107096</v>
       </c>
       <c r="F43" t="n">
-        <v>416539843</v>
+        <v>6125048</v>
       </c>
       <c r="G43" t="n">
-        <v>-1.1742</v>
+        <v>-7.10268</v>
       </c>
     </row>
     <row r="44">
@@ -1619,16 +1619,16 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.606142</v>
+        <v>0.573271</v>
       </c>
       <c r="E44" t="n">
-        <v>1899717987</v>
+        <v>1793498467</v>
       </c>
       <c r="F44" t="n">
-        <v>6424115</v>
+        <v>27516972</v>
       </c>
       <c r="G44" t="n">
-        <v>-2.71496</v>
+        <v>-2.00601</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>EGLD</t>
+          <t>RUNE</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>MultiversX</t>
+          <t>THORChain</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>64.55</v>
+        <v>5.63</v>
       </c>
       <c r="E45" t="n">
-        <v>1702130997</v>
+        <v>1690565929</v>
       </c>
       <c r="F45" t="n">
-        <v>163415276</v>
+        <v>243385448</v>
       </c>
       <c r="G45" t="n">
-        <v>15.21462</v>
+        <v>-2.94588</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>EGLD</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>MultiversX</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>115.47</v>
+        <v>63.25</v>
       </c>
       <c r="E46" t="n">
-        <v>1677477962</v>
+        <v>1660101565</v>
       </c>
       <c r="F46" t="n">
-        <v>30136318</v>
+        <v>49650886</v>
       </c>
       <c r="G46" t="n">
-        <v>-2.6346</v>
+        <v>2.50615</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>FDUSD</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>First Digital USD</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>18.84</v>
+        <v>0.998126</v>
       </c>
       <c r="E47" t="n">
-        <v>1581668185</v>
+        <v>1650714700</v>
       </c>
       <c r="F47" t="n">
-        <v>94653951</v>
+        <v>2190988124</v>
       </c>
       <c r="G47" t="n">
-        <v>-2.69951</v>
+        <v>-0.11755</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.168841</v>
+        <v>111.9</v>
       </c>
       <c r="E48" t="n">
-        <v>1572126142</v>
+        <v>1625742004</v>
       </c>
       <c r="F48" t="n">
-        <v>74881659</v>
+        <v>18684808</v>
       </c>
       <c r="G48" t="n">
-        <v>-1.58061</v>
+        <v>-1.28326</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ALGO</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Algorand</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.193841</v>
+        <v>4.25</v>
       </c>
       <c r="E49" t="n">
-        <v>1546298373</v>
+        <v>1586314388</v>
       </c>
       <c r="F49" t="n">
-        <v>212675441</v>
+        <v>124761442</v>
       </c>
       <c r="G49" t="n">
-        <v>-4.17292</v>
+        <v>-4.54793</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>ALGO</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>BUSD</t>
+          <t>Algorand</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>1</v>
+        <v>0.19567</v>
       </c>
       <c r="E50" t="n">
-        <v>1506606703</v>
+        <v>1564042085</v>
       </c>
       <c r="F50" t="n">
-        <v>2040555489</v>
+        <v>66958706</v>
       </c>
       <c r="G50" t="n">
-        <v>0.03979</v>
+        <v>-3.32793</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>AAVE</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Aave</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>1.14</v>
+        <v>104.45</v>
       </c>
       <c r="E51" t="n">
-        <v>1448577421</v>
+        <v>1521640124</v>
       </c>
       <c r="F51" t="n">
-        <v>375115468</v>
+        <v>156756034</v>
       </c>
       <c r="G51" t="n">
-        <v>-4.03384</v>
+        <v>-3.21341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-12-24
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>41903</v>
+        <v>43605</v>
       </c>
       <c r="E2" t="n">
-        <v>819830538014</v>
+        <v>853742003833</v>
       </c>
       <c r="F2" t="n">
-        <v>11986194231</v>
+        <v>11057977487</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.93288</v>
+        <v>-0.12968</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2215.2</v>
+        <v>2289</v>
       </c>
       <c r="E3" t="n">
-        <v>265963134104</v>
+        <v>275175557796</v>
       </c>
       <c r="F3" t="n">
-        <v>7828168667</v>
+        <v>12143182508</v>
       </c>
       <c r="G3" t="n">
-        <v>-1.48965</v>
+        <v>-0.23747</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999436</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>90850654807</v>
+        <v>91217301562</v>
       </c>
       <c r="F4" t="n">
-        <v>28581861881</v>
+        <v>33329855612</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0507</v>
+        <v>-0.04523</v>
       </c>
     </row>
     <row r="5">
@@ -557,25 +557,25 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BNB</t>
+          <t>SOL</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>BNB</t>
+          <t>Solana</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>241.3</v>
+        <v>109.99</v>
       </c>
       <c r="E5" t="n">
-        <v>37104049349</v>
+        <v>46879984480</v>
       </c>
       <c r="F5" t="n">
-        <v>540505107</v>
+        <v>6277323524</v>
       </c>
       <c r="G5" t="n">
-        <v>-2.17504</v>
+        <v>14.53062</v>
       </c>
     </row>
     <row r="6">
@@ -584,25 +584,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>BNB</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>BNB</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.618808</v>
+        <v>268.05</v>
       </c>
       <c r="E6" t="n">
-        <v>33380399594</v>
+        <v>41186146760</v>
       </c>
       <c r="F6" t="n">
-        <v>744026594</v>
+        <v>564429863</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.72162</v>
+        <v>-0.466</v>
       </c>
     </row>
     <row r="7">
@@ -611,25 +611,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>SOL</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Solana</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>72.72</v>
+        <v>0.617929</v>
       </c>
       <c r="E7" t="n">
-        <v>31082596893</v>
+        <v>33411209077</v>
       </c>
       <c r="F7" t="n">
-        <v>1609319506</v>
+        <v>855018661</v>
       </c>
       <c r="G7" t="n">
-        <v>-3.14503</v>
+        <v>0.21732</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0.999838</v>
       </c>
       <c r="E8" t="n">
-        <v>24629116934</v>
+        <v>25066662336</v>
       </c>
       <c r="F8" t="n">
-        <v>4662777447</v>
+        <v>5984360710</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.04887</v>
+        <v>-0.04116</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.598587</v>
+        <v>0.612484</v>
       </c>
       <c r="E9" t="n">
-        <v>20918001986</v>
+        <v>21457221904</v>
       </c>
       <c r="F9" t="n">
-        <v>521318006</v>
+        <v>650933583</v>
       </c>
       <c r="G9" t="n">
-        <v>-2.58032</v>
+        <v>0.84197</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>2212.43</v>
+        <v>2283</v>
       </c>
       <c r="E10" t="n">
-        <v>20363989148</v>
+        <v>20891958878</v>
       </c>
       <c r="F10" t="n">
-        <v>33663356</v>
+        <v>36533900</v>
       </c>
       <c r="G10" t="n">
-        <v>-1.58137</v>
+        <v>-0.38421</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>41.95</v>
+        <v>47.3</v>
       </c>
       <c r="E11" t="n">
-        <v>15378544016</v>
+        <v>17258054768</v>
       </c>
       <c r="F11" t="n">
-        <v>1663507734</v>
+        <v>1636236523</v>
       </c>
       <c r="G11" t="n">
-        <v>-3.43542</v>
+        <v>4.33921</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.095038</v>
+        <v>0.094156</v>
       </c>
       <c r="E12" t="n">
-        <v>13491081604</v>
+        <v>13407861660</v>
       </c>
       <c r="F12" t="n">
-        <v>718179527</v>
+        <v>594683216</v>
       </c>
       <c r="G12" t="n">
-        <v>0.87824</v>
+        <v>1.12547</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>6.98</v>
+        <v>8.98</v>
       </c>
       <c r="E13" t="n">
-        <v>9113772784</v>
+        <v>11818629222</v>
       </c>
       <c r="F13" t="n">
-        <v>290157745</v>
+        <v>930229646</v>
       </c>
       <c r="G13" t="n">
-        <v>-2.58047</v>
+        <v>13.69242</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.103019</v>
+        <v>0.105826</v>
       </c>
       <c r="E14" t="n">
-        <v>9096921069</v>
+        <v>9351114274</v>
       </c>
       <c r="F14" t="n">
-        <v>316781809</v>
+        <v>358350602</v>
       </c>
       <c r="G14" t="n">
-        <v>0.32609</v>
+        <v>-0.08069999999999999</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>14.19</v>
+        <v>15.62</v>
       </c>
       <c r="E15" t="n">
-        <v>7888449740</v>
+        <v>8701679339</v>
       </c>
       <c r="F15" t="n">
-        <v>397109911</v>
+        <v>688157223</v>
       </c>
       <c r="G15" t="n">
-        <v>-2.43447</v>
+        <v>1.64231</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.832436</v>
+        <v>0.842726</v>
       </c>
       <c r="E16" t="n">
-        <v>7715664850</v>
+        <v>7821360687</v>
       </c>
       <c r="F16" t="n">
-        <v>296001104</v>
+        <v>484423732</v>
       </c>
       <c r="G16" t="n">
-        <v>-2.53698</v>
+        <v>-0.17359</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>41832</v>
+        <v>2.22</v>
       </c>
       <c r="E17" t="n">
-        <v>6469794031</v>
+        <v>7680868642</v>
       </c>
       <c r="F17" t="n">
-        <v>76901311</v>
+        <v>34534980</v>
       </c>
       <c r="G17" t="n">
-        <v>-1.04351</v>
+        <v>-0.80431</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1.073e-05</v>
+        <v>43522</v>
       </c>
       <c r="E18" t="n">
-        <v>6284307348</v>
+        <v>6778191618</v>
       </c>
       <c r="F18" t="n">
-        <v>842700935</v>
+        <v>114214627</v>
       </c>
       <c r="G18" t="n">
-        <v>7.09315</v>
+        <v>-0.44355</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>72.55</v>
+        <v>1.087e-05</v>
       </c>
       <c r="E19" t="n">
-        <v>5356673447</v>
+        <v>6405276409</v>
       </c>
       <c r="F19" t="n">
-        <v>465843609</v>
+        <v>252379549</v>
       </c>
       <c r="G19" t="n">
-        <v>0.43497</v>
+        <v>-1.36134</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.997801</v>
+        <v>72.16</v>
       </c>
       <c r="E20" t="n">
-        <v>5271229056</v>
+        <v>5340922334</v>
       </c>
       <c r="F20" t="n">
-        <v>199752100</v>
+        <v>421855162</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.07549</v>
+        <v>0.13757</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>11.05</v>
+        <v>0.999008</v>
       </c>
       <c r="E21" t="n">
-        <v>4894968201</v>
+        <v>5330469213</v>
       </c>
       <c r="F21" t="n">
-        <v>708763029</v>
+        <v>160905099</v>
       </c>
       <c r="G21" t="n">
-        <v>20.67143</v>
+        <v>-0.00906</v>
       </c>
     </row>
     <row r="22">
@@ -1025,16 +1025,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>6.2</v>
+        <v>6.73</v>
       </c>
       <c r="E22" t="n">
-        <v>4662259783</v>
+        <v>5077628403</v>
       </c>
       <c r="F22" t="n">
-        <v>164051700</v>
+        <v>208362209</v>
       </c>
       <c r="G22" t="n">
-        <v>0.39648</v>
+        <v>8.45017</v>
       </c>
     </row>
     <row r="23">
@@ -1052,16 +1052,16 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>228.55</v>
+        <v>230.43</v>
       </c>
       <c r="E23" t="n">
-        <v>4473661291</v>
+        <v>4512405536</v>
       </c>
       <c r="F23" t="n">
-        <v>116735430</v>
+        <v>140888564</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.80994</v>
+        <v>-0.52056</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>3.79</v>
+        <v>9.92</v>
       </c>
       <c r="E24" t="n">
-        <v>3513093157</v>
+        <v>4488023595</v>
       </c>
       <c r="F24" t="n">
-        <v>924406</v>
+        <v>189680473</v>
       </c>
       <c r="G24" t="n">
-        <v>0.47316</v>
+        <v>8.778370000000001</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.12429</v>
+        <v>3.8</v>
       </c>
       <c r="E25" t="n">
-        <v>3501286906</v>
+        <v>3828676488</v>
       </c>
       <c r="F25" t="n">
-        <v>61499931</v>
+        <v>621308525</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.5351900000000001</v>
+        <v>13.16078</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>57.27</v>
+        <v>3.92</v>
       </c>
       <c r="E26" t="n">
-        <v>3437124414</v>
+        <v>3633874473</v>
       </c>
       <c r="F26" t="n">
-        <v>10572128</v>
+        <v>1379772</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.8827199999999999</v>
+        <v>0.30423</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>11.62</v>
+        <v>0.126885</v>
       </c>
       <c r="E27" t="n">
-        <v>3412192174</v>
+        <v>3590740842</v>
       </c>
       <c r="F27" t="n">
-        <v>285810926</v>
+        <v>54949241</v>
       </c>
       <c r="G27" t="n">
-        <v>1.79435</v>
+        <v>1.49727</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>169.42</v>
+        <v>41.73</v>
       </c>
       <c r="E28" t="n">
-        <v>3070847929</v>
+        <v>3505217737</v>
       </c>
       <c r="F28" t="n">
-        <v>64575945</v>
+        <v>449240568</v>
       </c>
       <c r="G28" t="n">
-        <v>-1.35297</v>
+        <v>5.27654</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>20.21</v>
+        <v>11.56</v>
       </c>
       <c r="E29" t="n">
-        <v>2884407004</v>
+        <v>3384782350</v>
       </c>
       <c r="F29" t="n">
-        <v>94711177</v>
+        <v>234914884</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.78112</v>
+        <v>2.9608</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>5.68</v>
+        <v>55.32</v>
       </c>
       <c r="E30" t="n">
-        <v>2761809364</v>
+        <v>3316072675</v>
       </c>
       <c r="F30" t="n">
-        <v>851350434</v>
+        <v>7948240</v>
       </c>
       <c r="G30" t="n">
-        <v>5.75791</v>
+        <v>-0.91259</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.079457</v>
+        <v>3.51</v>
       </c>
       <c r="E31" t="n">
-        <v>2660696932</v>
+        <v>3190796334</v>
       </c>
       <c r="F31" t="n">
-        <v>65957945</v>
+        <v>759367695</v>
       </c>
       <c r="G31" t="n">
-        <v>-3.12502</v>
+        <v>8.08742</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.099772</v>
+        <v>175.37</v>
       </c>
       <c r="E32" t="n">
-        <v>2636325655</v>
+        <v>3186743681</v>
       </c>
       <c r="F32" t="n">
-        <v>11076988</v>
+        <v>87392499</v>
       </c>
       <c r="G32" t="n">
-        <v>-2.29744</v>
+        <v>-0.18206</v>
       </c>
     </row>
     <row r="33">
@@ -1322,16 +1322,16 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>2.03</v>
+        <v>2.41</v>
       </c>
       <c r="E33" t="n">
-        <v>2613492214</v>
+        <v>3119258840</v>
       </c>
       <c r="F33" t="n">
-        <v>158354376</v>
+        <v>136221435</v>
       </c>
       <c r="G33" t="n">
-        <v>-6.52462</v>
+        <v>-4.6143</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>30.14</v>
+        <v>0.091975</v>
       </c>
       <c r="E34" t="n">
-        <v>2530781982</v>
+        <v>3088396252</v>
       </c>
       <c r="F34" t="n">
-        <v>251068783</v>
+        <v>88096463</v>
       </c>
       <c r="G34" t="n">
-        <v>-2.50865</v>
+        <v>2.43528</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>8.17</v>
+        <v>21.06</v>
       </c>
       <c r="E35" t="n">
-        <v>2483820305</v>
+        <v>3016100128</v>
       </c>
       <c r="F35" t="n">
-        <v>139336047</v>
+        <v>128156042</v>
       </c>
       <c r="G35" t="n">
-        <v>-1.90593</v>
+        <v>-1.2539</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.996213</v>
+        <v>9.43</v>
       </c>
       <c r="E36" t="n">
-        <v>2431725952</v>
+        <v>2886804660</v>
       </c>
       <c r="F36" t="n">
-        <v>127083746</v>
+        <v>270780693</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.24066</v>
+        <v>0.93492</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.109192</v>
+        <v>5.62</v>
       </c>
       <c r="E37" t="n">
-        <v>2382753721</v>
+        <v>2730409211</v>
       </c>
       <c r="F37" t="n">
-        <v>47991154</v>
+        <v>245464098</v>
       </c>
       <c r="G37" t="n">
-        <v>-10.27094</v>
+        <v>4.14724</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>2.37</v>
+        <v>0.03595505</v>
       </c>
       <c r="E38" t="n">
-        <v>2382299533</v>
+        <v>2615844748</v>
       </c>
       <c r="F38" t="n">
-        <v>215167572</v>
+        <v>69767280</v>
       </c>
       <c r="G38" t="n">
-        <v>2.44583</v>
+        <v>2.77417</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.02983601</v>
+        <v>0.098604</v>
       </c>
       <c r="E39" t="n">
-        <v>2166426628</v>
+        <v>2599844959</v>
       </c>
       <c r="F39" t="n">
-        <v>55024016</v>
+        <v>12881767</v>
       </c>
       <c r="G39" t="n">
-        <v>-3.7473</v>
+        <v>-2.21099</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>TIA</t>
+          <t>TUSD</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Celestia</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>13.65</v>
+        <v>0.998974</v>
       </c>
       <c r="E40" t="n">
-        <v>1986988583</v>
+        <v>2428705500</v>
       </c>
       <c r="F40" t="n">
-        <v>319276355</v>
+        <v>164430757</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.93387</v>
+        <v>-0.07778</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>2.12</v>
+        <v>0.107191</v>
       </c>
       <c r="E41" t="n">
-        <v>1928913091</v>
+        <v>2361004532</v>
       </c>
       <c r="F41" t="n">
-        <v>222874379</v>
+        <v>34917686</v>
       </c>
       <c r="G41" t="n">
-        <v>-1.929</v>
+        <v>-0.24342</v>
       </c>
     </row>
     <row r="42">
@@ -1565,16 +1565,16 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>2.12</v>
+        <v>2.39</v>
       </c>
       <c r="E42" t="n">
-        <v>1879284878</v>
+        <v>2128356383</v>
       </c>
       <c r="F42" t="n">
-        <v>46221938</v>
+        <v>89349215</v>
       </c>
       <c r="G42" t="n">
-        <v>-3.26419</v>
+        <v>1.91646</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>316.42</v>
+        <v>1.41</v>
       </c>
       <c r="E43" t="n">
-        <v>1856107096</v>
+        <v>2026192637</v>
       </c>
       <c r="F43" t="n">
-        <v>6125048</v>
+        <v>108071205</v>
       </c>
       <c r="G43" t="n">
-        <v>-7.10268</v>
+        <v>-3.38912</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>TIA</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Celestia</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.573271</v>
+        <v>13.71</v>
       </c>
       <c r="E44" t="n">
-        <v>1793498467</v>
+        <v>1999770118</v>
       </c>
       <c r="F44" t="n">
-        <v>27516972</v>
+        <v>258674427</v>
       </c>
       <c r="G44" t="n">
-        <v>-2.00601</v>
+        <v>10.92248</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>RUNE</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>THORChain</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>5.63</v>
+        <v>0.621167</v>
       </c>
       <c r="E45" t="n">
-        <v>1690565929</v>
+        <v>1944487057</v>
       </c>
       <c r="F45" t="n">
-        <v>243385448</v>
+        <v>9482064</v>
       </c>
       <c r="G45" t="n">
-        <v>-2.94588</v>
+        <v>4.27293</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>EGLD</t>
+          <t>ALGO</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>MultiversX</t>
+          <t>Algorand</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>63.25</v>
+        <v>0.238034</v>
       </c>
       <c r="E46" t="n">
-        <v>1660101565</v>
+        <v>1906307005</v>
       </c>
       <c r="F46" t="n">
-        <v>49650886</v>
+        <v>108214904</v>
       </c>
       <c r="G46" t="n">
-        <v>2.50615</v>
+        <v>0.66772</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>FDUSD</t>
+          <t>RUNE</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>First Digital USD</t>
+          <t>THORChain</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.998126</v>
+        <v>6.31</v>
       </c>
       <c r="E47" t="n">
-        <v>1650714700</v>
+        <v>1894663804</v>
       </c>
       <c r="F47" t="n">
-        <v>2190988124</v>
+        <v>814828624</v>
       </c>
       <c r="G47" t="n">
-        <v>-0.11755</v>
+        <v>22.04921</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>EGLD</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>MultiversX</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>111.9</v>
+        <v>71.18000000000001</v>
       </c>
       <c r="E48" t="n">
-        <v>1625742004</v>
+        <v>1875088617</v>
       </c>
       <c r="F48" t="n">
-        <v>18684808</v>
+        <v>117866510</v>
       </c>
       <c r="G48" t="n">
-        <v>-1.28326</v>
+        <v>11.82114</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>FDUSD</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>First Digital USD</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>4.25</v>
+        <v>0.998849</v>
       </c>
       <c r="E49" t="n">
-        <v>1586314388</v>
+        <v>1793428025</v>
       </c>
       <c r="F49" t="n">
-        <v>124761442</v>
+        <v>1274063858</v>
       </c>
       <c r="G49" t="n">
-        <v>-4.54793</v>
+        <v>-0.09893</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ALGO</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Algorand</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.19567</v>
+        <v>4.67</v>
       </c>
       <c r="E50" t="n">
-        <v>1564042085</v>
+        <v>1749619269</v>
       </c>
       <c r="F50" t="n">
-        <v>66958706</v>
+        <v>203591907</v>
       </c>
       <c r="G50" t="n">
-        <v>-3.32793</v>
+        <v>6.00432</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>AAVE</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Aave</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>104.45</v>
+        <v>1.37</v>
       </c>
       <c r="E51" t="n">
-        <v>1521640124</v>
+        <v>1740769212</v>
       </c>
       <c r="F51" t="n">
-        <v>156756034</v>
+        <v>806571831</v>
       </c>
       <c r="G51" t="n">
-        <v>-3.21341</v>
+        <v>1.82588</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2023-12-31
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>43605</v>
+        <v>42549</v>
       </c>
       <c r="E2" t="n">
-        <v>853742003833</v>
+        <v>833838111405</v>
       </c>
       <c r="F2" t="n">
-        <v>11057977487</v>
+        <v>15784397386</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.12968</v>
+        <v>1.15327</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2289</v>
+        <v>2312.96</v>
       </c>
       <c r="E3" t="n">
-        <v>275175557796</v>
+        <v>278223852789</v>
       </c>
       <c r="F3" t="n">
-        <v>12143182508</v>
+        <v>13770484760</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.23747</v>
+        <v>0.66005</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0.999816</v>
       </c>
       <c r="E4" t="n">
-        <v>91217301562</v>
+        <v>91703323180</v>
       </c>
       <c r="F4" t="n">
-        <v>33329855612</v>
+        <v>26972034979</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.04523</v>
+        <v>-0.06954</v>
       </c>
     </row>
     <row r="5">
@@ -557,25 +557,25 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SOL</t>
+          <t>BNB</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Solana</t>
+          <t>BNB</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>109.99</v>
+        <v>317.71</v>
       </c>
       <c r="E5" t="n">
-        <v>46879984480</v>
+        <v>48864314566</v>
       </c>
       <c r="F5" t="n">
-        <v>6277323524</v>
+        <v>762319018</v>
       </c>
       <c r="G5" t="n">
-        <v>14.53062</v>
+        <v>-0.13952</v>
       </c>
     </row>
     <row r="6">
@@ -584,25 +584,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BNB</t>
+          <t>SOL</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>BNB</t>
+          <t>Solana</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>268.05</v>
+        <v>104.85</v>
       </c>
       <c r="E6" t="n">
-        <v>41186146760</v>
+        <v>45040650600</v>
       </c>
       <c r="F6" t="n">
-        <v>564429863</v>
+        <v>1801340041</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.466</v>
+        <v>1.67517</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.617929</v>
+        <v>0.623647</v>
       </c>
       <c r="E7" t="n">
-        <v>33411209077</v>
+        <v>33763237785</v>
       </c>
       <c r="F7" t="n">
-        <v>855018661</v>
+        <v>587930520</v>
       </c>
       <c r="G7" t="n">
-        <v>0.21732</v>
+        <v>-0.03098</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.999838</v>
+        <v>0.9994729999999999</v>
       </c>
       <c r="E8" t="n">
-        <v>25066662336</v>
+        <v>24624218935</v>
       </c>
       <c r="F8" t="n">
-        <v>5984360710</v>
+        <v>7727557381</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.04116</v>
+        <v>-0.12624</v>
       </c>
     </row>
     <row r="9">
@@ -665,25 +665,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ADA</t>
+          <t>STETH</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Cardano</t>
+          <t>Lido Staked Ether</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.612484</v>
+        <v>2312.41</v>
       </c>
       <c r="E9" t="n">
-        <v>21457221904</v>
+        <v>21303488758</v>
       </c>
       <c r="F9" t="n">
-        <v>650933583</v>
+        <v>14139218</v>
       </c>
       <c r="G9" t="n">
-        <v>0.84197</v>
+        <v>0.75459</v>
       </c>
     </row>
     <row r="10">
@@ -692,25 +692,25 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>STETH</t>
+          <t>ADA</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Lido Staked Ether</t>
+          <t>Cardano</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>2283</v>
+        <v>0.606781</v>
       </c>
       <c r="E10" t="n">
-        <v>20891958878</v>
+        <v>21251961193</v>
       </c>
       <c r="F10" t="n">
-        <v>36533900</v>
+        <v>366605693</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.38421</v>
+        <v>0.67725</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>47.3</v>
+        <v>40.15</v>
       </c>
       <c r="E11" t="n">
-        <v>17258054768</v>
+        <v>14689094580</v>
       </c>
       <c r="F11" t="n">
-        <v>1636236523</v>
+        <v>592484813</v>
       </c>
       <c r="G11" t="n">
-        <v>4.33921</v>
+        <v>2.0011</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.094156</v>
+        <v>0.09050800000000001</v>
       </c>
       <c r="E12" t="n">
-        <v>13407861660</v>
+        <v>12902780919</v>
       </c>
       <c r="F12" t="n">
-        <v>594683216</v>
+        <v>280079440</v>
       </c>
       <c r="G12" t="n">
-        <v>1.12547</v>
+        <v>0.25808</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>8.98</v>
+        <v>8.51</v>
       </c>
       <c r="E13" t="n">
-        <v>11818629222</v>
+        <v>11191211124</v>
       </c>
       <c r="F13" t="n">
-        <v>930229646</v>
+        <v>281015881</v>
       </c>
       <c r="G13" t="n">
-        <v>13.69242</v>
+        <v>3.16845</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.105826</v>
+        <v>0.106548</v>
       </c>
       <c r="E14" t="n">
-        <v>9351114274</v>
+        <v>9413708410</v>
       </c>
       <c r="F14" t="n">
-        <v>358350602</v>
+        <v>298570097</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.08069999999999999</v>
+        <v>0.49362</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>15.62</v>
+        <v>0.983429</v>
       </c>
       <c r="E15" t="n">
-        <v>8701679339</v>
+        <v>9110381862</v>
       </c>
       <c r="F15" t="n">
-        <v>688157223</v>
+        <v>359830884</v>
       </c>
       <c r="G15" t="n">
-        <v>1.64231</v>
+        <v>2.17208</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.842726</v>
+        <v>15.45</v>
       </c>
       <c r="E16" t="n">
-        <v>7821360687</v>
+        <v>8592085839</v>
       </c>
       <c r="F16" t="n">
-        <v>484423732</v>
+        <v>336739296</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.17359</v>
+        <v>1.47146</v>
       </c>
     </row>
     <row r="17">
@@ -890,16 +890,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2.22</v>
+        <v>2.28</v>
       </c>
       <c r="E17" t="n">
-        <v>7680868642</v>
+        <v>7880132911</v>
       </c>
       <c r="F17" t="n">
-        <v>34534980</v>
+        <v>44025587</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.80431</v>
+        <v>-2.56502</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>43522</v>
+        <v>42530</v>
       </c>
       <c r="E18" t="n">
-        <v>6778191618</v>
+        <v>6725943326</v>
       </c>
       <c r="F18" t="n">
-        <v>114214627</v>
+        <v>117952231</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.44355</v>
+        <v>1.0643</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1.087e-05</v>
+        <v>13.71</v>
       </c>
       <c r="E19" t="n">
-        <v>6405276409</v>
+        <v>6264159141</v>
       </c>
       <c r="F19" t="n">
-        <v>252379549</v>
+        <v>805580925</v>
       </c>
       <c r="G19" t="n">
-        <v>-1.36134</v>
+        <v>36.85761</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>72.16</v>
+        <v>1.056e-05</v>
       </c>
       <c r="E20" t="n">
-        <v>5340922334</v>
+        <v>6223907198</v>
       </c>
       <c r="F20" t="n">
-        <v>421855162</v>
+        <v>83318161</v>
       </c>
       <c r="G20" t="n">
-        <v>0.13757</v>
+        <v>0.55955</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.999008</v>
+        <v>7.66</v>
       </c>
       <c r="E21" t="n">
-        <v>5330469213</v>
+        <v>5771585711</v>
       </c>
       <c r="F21" t="n">
-        <v>160905099</v>
+        <v>214019179</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.00906</v>
+        <v>2.05048</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>6.73</v>
+        <v>73.88</v>
       </c>
       <c r="E22" t="n">
-        <v>5077628403</v>
+        <v>5472217772</v>
       </c>
       <c r="F22" t="n">
-        <v>208362209</v>
+        <v>427636268</v>
       </c>
       <c r="G22" t="n">
-        <v>8.45017</v>
+        <v>0.43561</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>230.43</v>
+        <v>0.9989130000000001</v>
       </c>
       <c r="E23" t="n">
-        <v>4512405536</v>
+        <v>5236682697</v>
       </c>
       <c r="F23" t="n">
-        <v>140888564</v>
+        <v>211424426</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.52056</v>
+        <v>-0.03898</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>9.92</v>
+        <v>266.96</v>
       </c>
       <c r="E24" t="n">
-        <v>4488023595</v>
+        <v>5231494920</v>
       </c>
       <c r="F24" t="n">
-        <v>189680473</v>
+        <v>300857479</v>
       </c>
       <c r="G24" t="n">
-        <v>8.778370000000001</v>
+        <v>-3.40793</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>3.8</v>
+        <v>10.88</v>
       </c>
       <c r="E25" t="n">
-        <v>3828676488</v>
+        <v>4146133046</v>
       </c>
       <c r="F25" t="n">
-        <v>621308525</v>
+        <v>178852410</v>
       </c>
       <c r="G25" t="n">
-        <v>13.16078</v>
+        <v>0.84501</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>3.92</v>
+        <v>3.71</v>
       </c>
       <c r="E26" t="n">
-        <v>3633874473</v>
+        <v>3768776847</v>
       </c>
       <c r="F26" t="n">
-        <v>1379772</v>
+        <v>212761672</v>
       </c>
       <c r="G26" t="n">
-        <v>0.30423</v>
+        <v>0.04485</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.126885</v>
+        <v>0.131129</v>
       </c>
       <c r="E27" t="n">
-        <v>3590740842</v>
+        <v>3704208892</v>
       </c>
       <c r="F27" t="n">
-        <v>54949241</v>
+        <v>95242832</v>
       </c>
       <c r="G27" t="n">
-        <v>1.49727</v>
+        <v>-3.51395</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>41.73</v>
+        <v>3.94</v>
       </c>
       <c r="E28" t="n">
-        <v>3505217737</v>
+        <v>3650161960</v>
       </c>
       <c r="F28" t="n">
-        <v>449240568</v>
+        <v>1312282</v>
       </c>
       <c r="G28" t="n">
-        <v>5.27654</v>
+        <v>-0.71728</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>11.56</v>
+        <v>3.87</v>
       </c>
       <c r="E29" t="n">
-        <v>3384782350</v>
+        <v>3523741775</v>
       </c>
       <c r="F29" t="n">
-        <v>234914884</v>
+        <v>316138700</v>
       </c>
       <c r="G29" t="n">
-        <v>2.9608</v>
+        <v>5.91692</v>
       </c>
     </row>
     <row r="30">
@@ -1241,16 +1241,16 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>55.32</v>
+        <v>54.89</v>
       </c>
       <c r="E30" t="n">
-        <v>3316072675</v>
+        <v>3289278678</v>
       </c>
       <c r="F30" t="n">
-        <v>7948240</v>
+        <v>4780484</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.91259</v>
+        <v>0.53542</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>3.51</v>
+        <v>38.39</v>
       </c>
       <c r="E31" t="n">
-        <v>3190796334</v>
+        <v>3234833395</v>
       </c>
       <c r="F31" t="n">
-        <v>759367695</v>
+        <v>233504804</v>
       </c>
       <c r="G31" t="n">
-        <v>8.08742</v>
+        <v>4.77637</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>175.37</v>
+        <v>22.39</v>
       </c>
       <c r="E32" t="n">
-        <v>3186743681</v>
+        <v>3205672000</v>
       </c>
       <c r="F32" t="n">
-        <v>87392499</v>
+        <v>132182532</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.18206</v>
+        <v>-0.42793</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>2.41</v>
+        <v>6.38</v>
       </c>
       <c r="E33" t="n">
-        <v>3119258840</v>
+        <v>3112565864</v>
       </c>
       <c r="F33" t="n">
-        <v>136221435</v>
+        <v>303018046</v>
       </c>
       <c r="G33" t="n">
-        <v>-4.6143</v>
+        <v>9.403180000000001</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.091975</v>
+        <v>167.39</v>
       </c>
       <c r="E34" t="n">
-        <v>3088396252</v>
+        <v>3037950711</v>
       </c>
       <c r="F34" t="n">
-        <v>88096463</v>
+        <v>63398344</v>
       </c>
       <c r="G34" t="n">
-        <v>2.43528</v>
+        <v>2.27132</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>21.06</v>
+        <v>0.08870500000000001</v>
       </c>
       <c r="E35" t="n">
-        <v>3016100128</v>
+        <v>2984347616</v>
       </c>
       <c r="F35" t="n">
-        <v>128156042</v>
+        <v>51347560</v>
       </c>
       <c r="G35" t="n">
-        <v>-1.2539</v>
+        <v>1.44135</v>
       </c>
     </row>
     <row r="36">
@@ -1403,16 +1403,16 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>9.43</v>
+        <v>9.59</v>
       </c>
       <c r="E36" t="n">
-        <v>2886804660</v>
+        <v>2951402404</v>
       </c>
       <c r="F36" t="n">
-        <v>270780693</v>
+        <v>107270399</v>
       </c>
       <c r="G36" t="n">
-        <v>0.93492</v>
+        <v>-0.14932</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>5.62</v>
+        <v>2.23</v>
       </c>
       <c r="E37" t="n">
-        <v>2730409211</v>
+        <v>2945222558</v>
       </c>
       <c r="F37" t="n">
-        <v>245464098</v>
+        <v>65944518</v>
       </c>
       <c r="G37" t="n">
-        <v>4.14724</v>
+        <v>-1.04265</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.03595505</v>
+        <v>0.099966</v>
       </c>
       <c r="E38" t="n">
-        <v>2615844748</v>
+        <v>2645218835</v>
       </c>
       <c r="F38" t="n">
-        <v>69767280</v>
+        <v>7745997</v>
       </c>
       <c r="G38" t="n">
-        <v>2.77417</v>
+        <v>0.91401</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.098604</v>
+        <v>0.03503288</v>
       </c>
       <c r="E39" t="n">
-        <v>2599844959</v>
+        <v>2545736406</v>
       </c>
       <c r="F39" t="n">
-        <v>12881767</v>
+        <v>79507761</v>
       </c>
       <c r="G39" t="n">
-        <v>-2.21099</v>
+        <v>0.71673</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.998974</v>
+        <v>0.114377</v>
       </c>
       <c r="E40" t="n">
-        <v>2428705500</v>
+        <v>2530611901</v>
       </c>
       <c r="F40" t="n">
-        <v>164430757</v>
+        <v>26881783</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.07778</v>
+        <v>0.5282</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.107191</v>
+        <v>2.79</v>
       </c>
       <c r="E41" t="n">
-        <v>2361004532</v>
+        <v>2469858099</v>
       </c>
       <c r="F41" t="n">
-        <v>34917686</v>
+        <v>64994509</v>
       </c>
       <c r="G41" t="n">
-        <v>-0.24342</v>
+        <v>-5.4025</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>TUSD</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>2.39</v>
+        <v>0.998</v>
       </c>
       <c r="E42" t="n">
-        <v>2128356383</v>
+        <v>2305914612</v>
       </c>
       <c r="F42" t="n">
-        <v>89349215</v>
+        <v>176055088</v>
       </c>
       <c r="G42" t="n">
-        <v>1.91646</v>
+        <v>-0.29236</v>
       </c>
     </row>
     <row r="43">
@@ -1592,16 +1592,16 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1.41</v>
+        <v>1.48</v>
       </c>
       <c r="E43" t="n">
-        <v>2026192637</v>
+        <v>2112756990</v>
       </c>
       <c r="F43" t="n">
-        <v>108071205</v>
+        <v>72477977</v>
       </c>
       <c r="G43" t="n">
-        <v>-3.38912</v>
+        <v>6.7797</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>TIA</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Celestia</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>13.71</v>
+        <v>1.64</v>
       </c>
       <c r="E44" t="n">
-        <v>1999770118</v>
+        <v>2091112191</v>
       </c>
       <c r="F44" t="n">
-        <v>258674427</v>
+        <v>636633854</v>
       </c>
       <c r="G44" t="n">
-        <v>10.92248</v>
+        <v>12.80495</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.621167</v>
+        <v>142.99</v>
       </c>
       <c r="E45" t="n">
-        <v>1944487057</v>
+        <v>2078948113</v>
       </c>
       <c r="F45" t="n">
-        <v>9482064</v>
+        <v>60813813</v>
       </c>
       <c r="G45" t="n">
-        <v>4.27293</v>
+        <v>6.09684</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ALGO</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Algorand</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.238034</v>
+        <v>0.659605</v>
       </c>
       <c r="E46" t="n">
-        <v>1906307005</v>
+        <v>2069351169</v>
       </c>
       <c r="F46" t="n">
-        <v>108214904</v>
+        <v>118036912</v>
       </c>
       <c r="G46" t="n">
-        <v>0.66772</v>
+        <v>1.89642</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>RUNE</t>
+          <t>BSV</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>THORChain</t>
+          <t>Bitcoin SV</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>6.31</v>
+        <v>101.31</v>
       </c>
       <c r="E47" t="n">
-        <v>1894663804</v>
+        <v>1955875065</v>
       </c>
       <c r="F47" t="n">
-        <v>814828624</v>
+        <v>319053720</v>
       </c>
       <c r="G47" t="n">
-        <v>22.04921</v>
+        <v>4.97823</v>
       </c>
     </row>
     <row r="48">
@@ -1727,16 +1727,16 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>71.18000000000001</v>
+        <v>69.78</v>
       </c>
       <c r="E48" t="n">
-        <v>1875088617</v>
+        <v>1840986477</v>
       </c>
       <c r="F48" t="n">
-        <v>117866510</v>
+        <v>27600506</v>
       </c>
       <c r="G48" t="n">
-        <v>11.82114</v>
+        <v>1.52936</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>FDUSD</t>
+          <t>TIA</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>First Digital USD</t>
+          <t>Celestia</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.998849</v>
+        <v>12.37</v>
       </c>
       <c r="E49" t="n">
-        <v>1793428025</v>
+        <v>1807048999</v>
       </c>
       <c r="F49" t="n">
-        <v>1274063858</v>
+        <v>79580098</v>
       </c>
       <c r="G49" t="n">
-        <v>-0.09893</v>
+        <v>3.1194</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>FDUSD</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>First Digital USD</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>4.67</v>
+        <v>1.001</v>
       </c>
       <c r="E50" t="n">
-        <v>1749619269</v>
+        <v>1802969442</v>
       </c>
       <c r="F50" t="n">
-        <v>203591907</v>
+        <v>1835513314</v>
       </c>
       <c r="G50" t="n">
-        <v>6.00432</v>
+        <v>-0.21075</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>ALGO</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Algorand</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>1.37</v>
+        <v>0.224498</v>
       </c>
       <c r="E51" t="n">
-        <v>1740769212</v>
+        <v>1796537361</v>
       </c>
       <c r="F51" t="n">
-        <v>806571831</v>
+        <v>48908859</v>
       </c>
       <c r="G51" t="n">
-        <v>1.82588</v>
+        <v>0.71004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-01-07
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>42549</v>
+        <v>44074</v>
       </c>
       <c r="E2" t="n">
-        <v>833838111405</v>
+        <v>864386053192</v>
       </c>
       <c r="F2" t="n">
-        <v>15784397386</v>
+        <v>11043791530</v>
       </c>
       <c r="G2" t="n">
-        <v>1.15327</v>
+        <v>0.87121</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2312.96</v>
+        <v>2237.69</v>
       </c>
       <c r="E3" t="n">
-        <v>278223852789</v>
+        <v>269212062847</v>
       </c>
       <c r="F3" t="n">
-        <v>13770484760</v>
+        <v>7942485475</v>
       </c>
       <c r="G3" t="n">
-        <v>0.66005</v>
+        <v>-0.04676</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999816</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>91703323180</v>
+        <v>93690138972</v>
       </c>
       <c r="F4" t="n">
-        <v>26972034979</v>
+        <v>25149150612</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.06954</v>
+        <v>-0.02817</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>317.71</v>
+        <v>306.08</v>
       </c>
       <c r="E5" t="n">
-        <v>48864314566</v>
+        <v>47156237475</v>
       </c>
       <c r="F5" t="n">
-        <v>762319018</v>
+        <v>590373742</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.13952</v>
+        <v>0.07722999999999999</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>104.85</v>
+        <v>94.37</v>
       </c>
       <c r="E6" t="n">
-        <v>45040650600</v>
+        <v>40725519860</v>
       </c>
       <c r="F6" t="n">
-        <v>1801340041</v>
+        <v>2034755507</v>
       </c>
       <c r="G6" t="n">
-        <v>1.67517</v>
+        <v>-0.30898</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.623647</v>
+        <v>0.565615</v>
       </c>
       <c r="E7" t="n">
-        <v>33763237785</v>
+        <v>30690989323</v>
       </c>
       <c r="F7" t="n">
-        <v>587930520</v>
+        <v>684380370</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.03098</v>
+        <v>-0.32723</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.9994729999999999</v>
+        <v>0.999676</v>
       </c>
       <c r="E8" t="n">
-        <v>24624218935</v>
+        <v>25400638532</v>
       </c>
       <c r="F8" t="n">
-        <v>7727557381</v>
+        <v>4009967635</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.12624</v>
+        <v>0.009860000000000001</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2312.41</v>
+        <v>2235.63</v>
       </c>
       <c r="E9" t="n">
-        <v>21303488758</v>
+        <v>20696735176</v>
       </c>
       <c r="F9" t="n">
-        <v>14139218</v>
+        <v>10092396</v>
       </c>
       <c r="G9" t="n">
-        <v>0.75459</v>
+        <v>-0.15267</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.606781</v>
+        <v>0.520087</v>
       </c>
       <c r="E10" t="n">
-        <v>21251961193</v>
+        <v>18247800940</v>
       </c>
       <c r="F10" t="n">
-        <v>366605693</v>
+        <v>383833565</v>
       </c>
       <c r="G10" t="n">
-        <v>0.67725</v>
+        <v>-0.32159</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>40.15</v>
+        <v>34.77</v>
       </c>
       <c r="E11" t="n">
-        <v>14689094580</v>
+        <v>12768889978</v>
       </c>
       <c r="F11" t="n">
-        <v>592484813</v>
+        <v>599429667</v>
       </c>
       <c r="G11" t="n">
-        <v>2.0011</v>
+        <v>0.21768</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.09050800000000001</v>
+        <v>0.079929</v>
       </c>
       <c r="E12" t="n">
-        <v>12902780919</v>
+        <v>11405914852</v>
       </c>
       <c r="F12" t="n">
-        <v>280079440</v>
+        <v>406016514</v>
       </c>
       <c r="G12" t="n">
-        <v>0.25808</v>
+        <v>-1.07632</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>8.51</v>
+        <v>7.18</v>
       </c>
       <c r="E13" t="n">
-        <v>11191211124</v>
+        <v>9446806079</v>
       </c>
       <c r="F13" t="n">
-        <v>281015881</v>
+        <v>221049552</v>
       </c>
       <c r="G13" t="n">
-        <v>3.16845</v>
+        <v>-0.14984</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.106548</v>
+        <v>0.10359</v>
       </c>
       <c r="E14" t="n">
-        <v>9413708410</v>
+        <v>9149646600</v>
       </c>
       <c r="F14" t="n">
-        <v>298570097</v>
+        <v>241935838</v>
       </c>
       <c r="G14" t="n">
-        <v>0.49362</v>
+        <v>-0.09933</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.983429</v>
+        <v>0.830101</v>
       </c>
       <c r="E15" t="n">
-        <v>9110381862</v>
+        <v>7712435868</v>
       </c>
       <c r="F15" t="n">
-        <v>359830884</v>
+        <v>309242215</v>
       </c>
       <c r="G15" t="n">
-        <v>2.17208</v>
+        <v>0.98666</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>15.45</v>
+        <v>13.5</v>
       </c>
       <c r="E16" t="n">
-        <v>8592085839</v>
+        <v>7673317699</v>
       </c>
       <c r="F16" t="n">
-        <v>336739296</v>
+        <v>340513217</v>
       </c>
       <c r="G16" t="n">
-        <v>1.47146</v>
+        <v>-0.34877</v>
       </c>
     </row>
     <row r="17">
@@ -890,16 +890,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2.28</v>
+        <v>2.21</v>
       </c>
       <c r="E17" t="n">
-        <v>7880132911</v>
+        <v>7636013413</v>
       </c>
       <c r="F17" t="n">
-        <v>44025587</v>
+        <v>48563694</v>
       </c>
       <c r="G17" t="n">
-        <v>-2.56502</v>
+        <v>3.40942</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>42530</v>
+        <v>44133</v>
       </c>
       <c r="E18" t="n">
-        <v>6725943326</v>
+        <v>6984550433</v>
       </c>
       <c r="F18" t="n">
-        <v>117952231</v>
+        <v>139385498</v>
       </c>
       <c r="G18" t="n">
-        <v>1.0643</v>
+        <v>0.89237</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>13.71</v>
+        <v>9.470000000000001e-06</v>
       </c>
       <c r="E19" t="n">
-        <v>6264159141</v>
+        <v>5571906937</v>
       </c>
       <c r="F19" t="n">
-        <v>805580925</v>
+        <v>100097183</v>
       </c>
       <c r="G19" t="n">
-        <v>36.85761</v>
+        <v>-1.13943</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>1.056e-05</v>
+        <v>11.89</v>
       </c>
       <c r="E20" t="n">
-        <v>6223907198</v>
+        <v>5419149196</v>
       </c>
       <c r="F20" t="n">
-        <v>83318161</v>
+        <v>149874381</v>
       </c>
       <c r="G20" t="n">
-        <v>0.55955</v>
+        <v>-1.44022</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>7.66</v>
+        <v>0.996938</v>
       </c>
       <c r="E21" t="n">
-        <v>5771585711</v>
+        <v>5256626275</v>
       </c>
       <c r="F21" t="n">
-        <v>214019179</v>
+        <v>213913316</v>
       </c>
       <c r="G21" t="n">
-        <v>2.05048</v>
+        <v>-0.22965</v>
       </c>
     </row>
     <row r="22">
@@ -1025,16 +1025,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>73.88</v>
+        <v>65.40000000000001</v>
       </c>
       <c r="E22" t="n">
-        <v>5472217772</v>
+        <v>4838776321</v>
       </c>
       <c r="F22" t="n">
-        <v>427636268</v>
+        <v>386254645</v>
       </c>
       <c r="G22" t="n">
-        <v>0.43561</v>
+        <v>0.56813</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.9989130000000001</v>
+        <v>6.3</v>
       </c>
       <c r="E23" t="n">
-        <v>5236682697</v>
+        <v>4749199001</v>
       </c>
       <c r="F23" t="n">
-        <v>211424426</v>
+        <v>204065391</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.03898</v>
+        <v>0.55937</v>
       </c>
     </row>
     <row r="24">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>266.96</v>
+        <v>235.53</v>
       </c>
       <c r="E24" t="n">
-        <v>5231494920</v>
+        <v>4630937966</v>
       </c>
       <c r="F24" t="n">
-        <v>300857479</v>
+        <v>135763306</v>
       </c>
       <c r="G24" t="n">
-        <v>-3.40793</v>
+        <v>-0.12728</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>10.88</v>
+        <v>4.03</v>
       </c>
       <c r="E25" t="n">
-        <v>4146133046</v>
+        <v>3738069445</v>
       </c>
       <c r="F25" t="n">
-        <v>178852410</v>
+        <v>1013178</v>
       </c>
       <c r="G25" t="n">
-        <v>0.84501</v>
+        <v>-0.82098</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>3.71</v>
+        <v>9.789999999999999</v>
       </c>
       <c r="E26" t="n">
-        <v>3768776847</v>
+        <v>3737316528</v>
       </c>
       <c r="F26" t="n">
-        <v>212761672</v>
+        <v>164513430</v>
       </c>
       <c r="G26" t="n">
-        <v>0.04485</v>
+        <v>-1.13326</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.131129</v>
+        <v>3.36</v>
       </c>
       <c r="E27" t="n">
-        <v>3704208892</v>
+        <v>3411741844</v>
       </c>
       <c r="F27" t="n">
-        <v>95242832</v>
+        <v>245125512</v>
       </c>
       <c r="G27" t="n">
-        <v>-3.51395</v>
+        <v>1.09563</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>3.94</v>
+        <v>0.118299</v>
       </c>
       <c r="E28" t="n">
-        <v>3650161960</v>
+        <v>3347630314</v>
       </c>
       <c r="F28" t="n">
-        <v>1312282</v>
+        <v>73161657</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.71728</v>
+        <v>-0.48379</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>3.87</v>
+        <v>54.66</v>
       </c>
       <c r="E29" t="n">
-        <v>3523741775</v>
+        <v>3285621801</v>
       </c>
       <c r="F29" t="n">
-        <v>316138700</v>
+        <v>3616196</v>
       </c>
       <c r="G29" t="n">
-        <v>5.91692</v>
+        <v>0.0766</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>54.89</v>
+        <v>37.52</v>
       </c>
       <c r="E30" t="n">
-        <v>3289278678</v>
+        <v>3166757556</v>
       </c>
       <c r="F30" t="n">
-        <v>4780484</v>
+        <v>306581159</v>
       </c>
       <c r="G30" t="n">
-        <v>0.53542</v>
+        <v>-0.35053</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>38.39</v>
+        <v>3.37</v>
       </c>
       <c r="E31" t="n">
-        <v>3234833395</v>
+        <v>3064274812</v>
       </c>
       <c r="F31" t="n">
-        <v>233504804</v>
+        <v>212211547</v>
       </c>
       <c r="G31" t="n">
-        <v>4.77637</v>
+        <v>3.77319</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>22.39</v>
+        <v>5.94</v>
       </c>
       <c r="E32" t="n">
-        <v>3205672000</v>
+        <v>2931203187</v>
       </c>
       <c r="F32" t="n">
-        <v>132182532</v>
+        <v>234133852</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.42793</v>
+        <v>-1.03097</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>6.38</v>
+        <v>19.71</v>
       </c>
       <c r="E33" t="n">
-        <v>3112565864</v>
+        <v>2824819646</v>
       </c>
       <c r="F33" t="n">
-        <v>303018046</v>
+        <v>83148308</v>
       </c>
       <c r="G33" t="n">
-        <v>9.403180000000001</v>
+        <v>-0.3235</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>167.39</v>
+        <v>8.970000000000001</v>
       </c>
       <c r="E34" t="n">
-        <v>3037950711</v>
+        <v>2767436232</v>
       </c>
       <c r="F34" t="n">
-        <v>63398344</v>
+        <v>163140287</v>
       </c>
       <c r="G34" t="n">
-        <v>2.27132</v>
+        <v>-2.09505</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.08870500000000001</v>
+        <v>152.48</v>
       </c>
       <c r="E35" t="n">
-        <v>2984347616</v>
+        <v>2766137249</v>
       </c>
       <c r="F35" t="n">
-        <v>51347560</v>
+        <v>70156116</v>
       </c>
       <c r="G35" t="n">
-        <v>1.44135</v>
+        <v>-0.32068</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>9.59</v>
+        <v>3.06</v>
       </c>
       <c r="E36" t="n">
-        <v>2951402404</v>
+        <v>2717197183</v>
       </c>
       <c r="F36" t="n">
-        <v>107270399</v>
+        <v>173217378</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.14932</v>
+        <v>-6.53557</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>2.23</v>
+        <v>0.079376</v>
       </c>
       <c r="E37" t="n">
-        <v>2945222558</v>
+        <v>2669707565</v>
       </c>
       <c r="F37" t="n">
-        <v>65944518</v>
+        <v>69649264</v>
       </c>
       <c r="G37" t="n">
-        <v>-1.04265</v>
+        <v>-0.8775500000000001</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.099966</v>
+        <v>1.96</v>
       </c>
       <c r="E38" t="n">
-        <v>2645218835</v>
+        <v>2592097856</v>
       </c>
       <c r="F38" t="n">
-        <v>7745997</v>
+        <v>58094130</v>
       </c>
       <c r="G38" t="n">
-        <v>0.91401</v>
+        <v>0.52605</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.03503288</v>
+        <v>0.110256</v>
       </c>
       <c r="E39" t="n">
-        <v>2545736406</v>
+        <v>2459912405</v>
       </c>
       <c r="F39" t="n">
-        <v>79507761</v>
+        <v>19045231</v>
       </c>
       <c r="G39" t="n">
-        <v>0.71673</v>
+        <v>1.86428</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.114377</v>
+        <v>1.66</v>
       </c>
       <c r="E40" t="n">
-        <v>2530611901</v>
+        <v>2367965630</v>
       </c>
       <c r="F40" t="n">
-        <v>26881783</v>
+        <v>107741983</v>
       </c>
       <c r="G40" t="n">
-        <v>0.5282</v>
+        <v>12.30051</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>2.79</v>
+        <v>0.088865</v>
       </c>
       <c r="E41" t="n">
-        <v>2469858099</v>
+        <v>2351065126</v>
       </c>
       <c r="F41" t="n">
-        <v>64994509</v>
+        <v>13427901</v>
       </c>
       <c r="G41" t="n">
-        <v>-5.4025</v>
+        <v>-0.71765</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.998</v>
+        <v>1.83</v>
       </c>
       <c r="E42" t="n">
-        <v>2305914612</v>
+        <v>2316251069</v>
       </c>
       <c r="F42" t="n">
-        <v>176055088</v>
+        <v>669478108</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.29236</v>
+        <v>2.70562</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>TUSD</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1.48</v>
+        <v>1.001</v>
       </c>
       <c r="E43" t="n">
-        <v>2112756990</v>
+        <v>2200597722</v>
       </c>
       <c r="F43" t="n">
-        <v>72477977</v>
+        <v>137261838</v>
       </c>
       <c r="G43" t="n">
-        <v>6.7797</v>
+        <v>0.08049000000000001</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>TIA</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Celestia</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1.64</v>
+        <v>15.09</v>
       </c>
       <c r="E44" t="n">
-        <v>2091112191</v>
+        <v>2189609758</v>
       </c>
       <c r="F44" t="n">
-        <v>636633854</v>
+        <v>239569105</v>
       </c>
       <c r="G44" t="n">
-        <v>12.80495</v>
+        <v>0.67301</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>142.99</v>
+        <v>0.02981264</v>
       </c>
       <c r="E45" t="n">
-        <v>2078948113</v>
+        <v>2169111215</v>
       </c>
       <c r="F45" t="n">
-        <v>60813813</v>
+        <v>47585818</v>
       </c>
       <c r="G45" t="n">
-        <v>6.09684</v>
+        <v>0.0332</v>
       </c>
     </row>
     <row r="46">
@@ -1673,16 +1673,16 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.659605</v>
+        <v>0.5990799999999999</v>
       </c>
       <c r="E46" t="n">
-        <v>2069351169</v>
+        <v>1876671709</v>
       </c>
       <c r="F46" t="n">
-        <v>118036912</v>
+        <v>51696366</v>
       </c>
       <c r="G46" t="n">
-        <v>1.89642</v>
+        <v>1.19627</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>BSV</t>
+          <t>FDUSD</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Bitcoin SV</t>
+          <t>First Digital USD</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>101.31</v>
+        <v>1.001</v>
       </c>
       <c r="E47" t="n">
-        <v>1955875065</v>
+        <v>1841494564</v>
       </c>
       <c r="F47" t="n">
-        <v>319053720</v>
+        <v>459625980</v>
       </c>
       <c r="G47" t="n">
-        <v>4.97823</v>
+        <v>-0.01856</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>EGLD</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>MultiversX</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>69.78</v>
+        <v>117.97</v>
       </c>
       <c r="E48" t="n">
-        <v>1840986477</v>
+        <v>1715181715</v>
       </c>
       <c r="F48" t="n">
-        <v>27600506</v>
+        <v>25262778</v>
       </c>
       <c r="G48" t="n">
-        <v>1.52936</v>
+        <v>-0.18771</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>TIA</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Celestia</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>12.37</v>
+        <v>1792.66</v>
       </c>
       <c r="E49" t="n">
-        <v>1807048999</v>
+        <v>1648380282</v>
       </c>
       <c r="F49" t="n">
-        <v>79580098</v>
+        <v>82960908</v>
       </c>
       <c r="G49" t="n">
-        <v>3.1194</v>
+        <v>4.33082</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>FDUSD</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>First Digital USD</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>1.001</v>
+        <v>0.170412</v>
       </c>
       <c r="E50" t="n">
-        <v>1802969442</v>
+        <v>1594815052</v>
       </c>
       <c r="F50" t="n">
-        <v>1835513314</v>
+        <v>54716756</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.21075</v>
+        <v>0.20431</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ALGO</t>
+          <t>SEI</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Algorand</t>
+          <t>Sei</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.224498</v>
+        <v>0.667311</v>
       </c>
       <c r="E51" t="n">
-        <v>1796537361</v>
+        <v>1535573064</v>
       </c>
       <c r="F51" t="n">
-        <v>48908859</v>
+        <v>565905294</v>
       </c>
       <c r="G51" t="n">
-        <v>0.71004</v>
+        <v>1.9943</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-01-14
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>44074</v>
+        <v>42790</v>
       </c>
       <c r="E2" t="n">
-        <v>864386053192</v>
+        <v>838715953858</v>
       </c>
       <c r="F2" t="n">
-        <v>11043791530</v>
+        <v>14307408035</v>
       </c>
       <c r="G2" t="n">
-        <v>0.87121</v>
+        <v>0.37919</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2237.69</v>
+        <v>2542.26</v>
       </c>
       <c r="E3" t="n">
-        <v>269212062847</v>
+        <v>305427899450</v>
       </c>
       <c r="F3" t="n">
-        <v>7942485475</v>
+        <v>19893896916</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.04676</v>
+        <v>-0.10441</v>
       </c>
     </row>
     <row r="4">
@@ -542,13 +542,13 @@
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>93690138972</v>
+        <v>95035237385</v>
       </c>
       <c r="F4" t="n">
-        <v>25149150612</v>
+        <v>27751424656</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.02817</v>
+        <v>-0.03898</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>306.08</v>
+        <v>303.96</v>
       </c>
       <c r="E5" t="n">
-        <v>47156237475</v>
+        <v>46804906731</v>
       </c>
       <c r="F5" t="n">
-        <v>590373742</v>
+        <v>563647300</v>
       </c>
       <c r="G5" t="n">
-        <v>0.07722999999999999</v>
+        <v>1.43925</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>94.37</v>
+        <v>96.92</v>
       </c>
       <c r="E6" t="n">
-        <v>40725519860</v>
+        <v>41894712720</v>
       </c>
       <c r="F6" t="n">
-        <v>2034755507</v>
+        <v>2011983791</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.30898</v>
+        <v>5.24875</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.565615</v>
+        <v>0.5768760000000001</v>
       </c>
       <c r="E7" t="n">
-        <v>30690989323</v>
+        <v>31268733409</v>
       </c>
       <c r="F7" t="n">
-        <v>684380370</v>
+        <v>507653248</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.32723</v>
+        <v>0.2911</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.999676</v>
+        <v>1.001</v>
       </c>
       <c r="E8" t="n">
-        <v>25400638532</v>
+        <v>25477897933</v>
       </c>
       <c r="F8" t="n">
-        <v>4009967635</v>
+        <v>9250266594</v>
       </c>
       <c r="G8" t="n">
-        <v>0.009860000000000001</v>
+        <v>-0.01051</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2235.63</v>
+        <v>2539.31</v>
       </c>
       <c r="E9" t="n">
-        <v>20696735176</v>
+        <v>23612768623</v>
       </c>
       <c r="F9" t="n">
-        <v>10092396</v>
+        <v>18193396</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.15267</v>
+        <v>-0.11701</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.520087</v>
+        <v>0.5448809999999999</v>
       </c>
       <c r="E10" t="n">
-        <v>18247800940</v>
+        <v>19120029255</v>
       </c>
       <c r="F10" t="n">
-        <v>383833565</v>
+        <v>318653867</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.32159</v>
+        <v>-0.53882</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>34.77</v>
+        <v>36.42</v>
       </c>
       <c r="E11" t="n">
-        <v>12768889978</v>
+        <v>13366410616</v>
       </c>
       <c r="F11" t="n">
-        <v>599429667</v>
+        <v>509010540</v>
       </c>
       <c r="G11" t="n">
-        <v>0.21768</v>
+        <v>1.19509</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.079929</v>
+        <v>0.082804</v>
       </c>
       <c r="E12" t="n">
-        <v>11405914852</v>
+        <v>11827898157</v>
       </c>
       <c r="F12" t="n">
-        <v>406016514</v>
+        <v>445893724</v>
       </c>
       <c r="G12" t="n">
-        <v>-1.07632</v>
+        <v>3.23823</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>7.18</v>
+        <v>0.114738</v>
       </c>
       <c r="E13" t="n">
-        <v>9446806079</v>
+        <v>10111048246</v>
       </c>
       <c r="F13" t="n">
-        <v>221049552</v>
+        <v>792259148</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.14984</v>
+        <v>1.50546</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.10359</v>
+        <v>7.57</v>
       </c>
       <c r="E14" t="n">
-        <v>9149646600</v>
+        <v>9989356401</v>
       </c>
       <c r="F14" t="n">
-        <v>241935838</v>
+        <v>169120617</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.09933</v>
+        <v>-0.95464</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.830101</v>
+        <v>15.04</v>
       </c>
       <c r="E15" t="n">
-        <v>7712435868</v>
+        <v>8556595787</v>
       </c>
       <c r="F15" t="n">
-        <v>309242215</v>
+        <v>552633744</v>
       </c>
       <c r="G15" t="n">
-        <v>0.98666</v>
+        <v>5.35931</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>13.5</v>
+        <v>0.867233</v>
       </c>
       <c r="E16" t="n">
-        <v>7673317699</v>
+        <v>8041587333</v>
       </c>
       <c r="F16" t="n">
-        <v>340513217</v>
+        <v>315590438</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.34877</v>
+        <v>-0.62422</v>
       </c>
     </row>
     <row r="17">
@@ -890,16 +890,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2.21</v>
+        <v>2.28</v>
       </c>
       <c r="E17" t="n">
-        <v>7636013413</v>
+        <v>7892987706</v>
       </c>
       <c r="F17" t="n">
-        <v>48563694</v>
+        <v>57363484</v>
       </c>
       <c r="G17" t="n">
-        <v>3.40942</v>
+        <v>7.93493</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>44133</v>
+        <v>42781</v>
       </c>
       <c r="E18" t="n">
-        <v>6984550433</v>
+        <v>6763821831</v>
       </c>
       <c r="F18" t="n">
-        <v>139385498</v>
+        <v>250284532</v>
       </c>
       <c r="G18" t="n">
-        <v>0.89237</v>
+        <v>0.43331</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>9.470000000000001e-06</v>
+        <v>13.3</v>
       </c>
       <c r="E19" t="n">
-        <v>5571906937</v>
+        <v>6059479127</v>
       </c>
       <c r="F19" t="n">
-        <v>100097183</v>
+        <v>233563558</v>
       </c>
       <c r="G19" t="n">
-        <v>-1.13943</v>
+        <v>3.88334</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>11.89</v>
+        <v>9.88e-06</v>
       </c>
       <c r="E20" t="n">
-        <v>5419149196</v>
+        <v>5819445309</v>
       </c>
       <c r="F20" t="n">
-        <v>149874381</v>
+        <v>117945167</v>
       </c>
       <c r="G20" t="n">
-        <v>-1.44022</v>
+        <v>0.6561399999999999</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.996938</v>
+        <v>71.69</v>
       </c>
       <c r="E21" t="n">
-        <v>5256626275</v>
+        <v>5312242497</v>
       </c>
       <c r="F21" t="n">
-        <v>213913316</v>
+        <v>514406407</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.22965</v>
+        <v>0.05971</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>65.40000000000001</v>
+        <v>0.99977</v>
       </c>
       <c r="E22" t="n">
-        <v>4838776321</v>
+        <v>5252841442</v>
       </c>
       <c r="F22" t="n">
-        <v>386254645</v>
+        <v>130073276</v>
       </c>
       <c r="G22" t="n">
-        <v>0.56813</v>
+        <v>-0.02637</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>6.3</v>
+        <v>255.96</v>
       </c>
       <c r="E23" t="n">
-        <v>4749199001</v>
+        <v>5033798569</v>
       </c>
       <c r="F23" t="n">
-        <v>204065391</v>
+        <v>215009984</v>
       </c>
       <c r="G23" t="n">
-        <v>0.55937</v>
+        <v>-0.13258</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>235.53</v>
+        <v>6.58</v>
       </c>
       <c r="E24" t="n">
-        <v>4630937966</v>
+        <v>4952303220</v>
       </c>
       <c r="F24" t="n">
-        <v>135763306</v>
+        <v>159412431</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.12728</v>
+        <v>0.38575</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>4.03</v>
+        <v>28.05</v>
       </c>
       <c r="E25" t="n">
-        <v>3738069445</v>
+        <v>4024338787</v>
       </c>
       <c r="F25" t="n">
-        <v>1013178</v>
+        <v>314351946</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.82098</v>
+        <v>-3.78961</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>9.789999999999999</v>
+        <v>10.16</v>
       </c>
       <c r="E26" t="n">
-        <v>3737316528</v>
+        <v>3888245163</v>
       </c>
       <c r="F26" t="n">
-        <v>164513430</v>
+        <v>179077629</v>
       </c>
       <c r="G26" t="n">
-        <v>-1.13326</v>
+        <v>1.09964</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>3.36</v>
+        <v>4.06</v>
       </c>
       <c r="E27" t="n">
-        <v>3411741844</v>
+        <v>3758023659</v>
       </c>
       <c r="F27" t="n">
-        <v>245125512</v>
+        <v>1165327</v>
       </c>
       <c r="G27" t="n">
-        <v>1.09563</v>
+        <v>0.10898</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.118299</v>
+        <v>3.77</v>
       </c>
       <c r="E28" t="n">
-        <v>3347630314</v>
+        <v>3606139832</v>
       </c>
       <c r="F28" t="n">
-        <v>73161657</v>
+        <v>185597732</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.48379</v>
+        <v>-1.15445</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>54.66</v>
+        <v>3.41</v>
       </c>
       <c r="E29" t="n">
-        <v>3285621801</v>
+        <v>3459651464</v>
       </c>
       <c r="F29" t="n">
-        <v>3616196</v>
+        <v>139759161</v>
       </c>
       <c r="G29" t="n">
-        <v>0.0766</v>
+        <v>0.66249</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>37.52</v>
+        <v>0.11992</v>
       </c>
       <c r="E30" t="n">
-        <v>3166757556</v>
+        <v>3394946653</v>
       </c>
       <c r="F30" t="n">
-        <v>306581159</v>
+        <v>56514269</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.35053</v>
+        <v>0.41485</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>3.37</v>
+        <v>9.73</v>
       </c>
       <c r="E31" t="n">
-        <v>3064274812</v>
+        <v>3244770944</v>
       </c>
       <c r="F31" t="n">
-        <v>212211547</v>
+        <v>317224748</v>
       </c>
       <c r="G31" t="n">
-        <v>3.77319</v>
+        <v>0.44356</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>5.94</v>
+        <v>53.73</v>
       </c>
       <c r="E32" t="n">
-        <v>2931203187</v>
+        <v>3224876054</v>
       </c>
       <c r="F32" t="n">
-        <v>234133852</v>
+        <v>4230407</v>
       </c>
       <c r="G32" t="n">
-        <v>-1.03097</v>
+        <v>0.2525</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>19.71</v>
+        <v>38.01</v>
       </c>
       <c r="E33" t="n">
-        <v>2824819646</v>
+        <v>3221424410</v>
       </c>
       <c r="F33" t="n">
-        <v>83148308</v>
+        <v>195260724</v>
       </c>
       <c r="G33" t="n">
-        <v>-0.3235</v>
+        <v>3.00781</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>TIA</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Celestia</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>8.970000000000001</v>
+        <v>19.72</v>
       </c>
       <c r="E34" t="n">
-        <v>2767436232</v>
+        <v>3118861228</v>
       </c>
       <c r="F34" t="n">
-        <v>163140287</v>
+        <v>437259675</v>
       </c>
       <c r="G34" t="n">
-        <v>-2.09505</v>
+        <v>15.74921</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>152.48</v>
+        <v>6.12</v>
       </c>
       <c r="E35" t="n">
-        <v>2766137249</v>
+        <v>3041336526</v>
       </c>
       <c r="F35" t="n">
-        <v>70156116</v>
+        <v>217254639</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.32068</v>
+        <v>2.90776</v>
       </c>
     </row>
     <row r="36">
@@ -1403,16 +1403,16 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>3.06</v>
+        <v>3.31</v>
       </c>
       <c r="E36" t="n">
-        <v>2717197183</v>
+        <v>2938671711</v>
       </c>
       <c r="F36" t="n">
-        <v>173217378</v>
+        <v>109028978</v>
       </c>
       <c r="G36" t="n">
-        <v>-6.53557</v>
+        <v>-2.2742</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.079376</v>
+        <v>157.55</v>
       </c>
       <c r="E37" t="n">
-        <v>2669707565</v>
+        <v>2857647497</v>
       </c>
       <c r="F37" t="n">
-        <v>69649264</v>
+        <v>84625379</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.8775500000000001</v>
+        <v>3.57223</v>
       </c>
     </row>
     <row r="38">
@@ -1457,16 +1457,16 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1.96</v>
+        <v>2.07</v>
       </c>
       <c r="E38" t="n">
-        <v>2592097856</v>
+        <v>2731666421</v>
       </c>
       <c r="F38" t="n">
-        <v>58094130</v>
+        <v>94796208</v>
       </c>
       <c r="G38" t="n">
-        <v>0.52605</v>
+        <v>-2.24083</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.110256</v>
+        <v>2.14</v>
       </c>
       <c r="E39" t="n">
-        <v>2459912405</v>
+        <v>2723260076</v>
       </c>
       <c r="F39" t="n">
-        <v>19045231</v>
+        <v>524765215</v>
       </c>
       <c r="G39" t="n">
-        <v>1.86428</v>
+        <v>-0.79235</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1.66</v>
+        <v>0.079858</v>
       </c>
       <c r="E40" t="n">
-        <v>2367965630</v>
+        <v>2688359204</v>
       </c>
       <c r="F40" t="n">
-        <v>107741983</v>
+        <v>52655919</v>
       </c>
       <c r="G40" t="n">
-        <v>12.30051</v>
+        <v>0.75824</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.088865</v>
+        <v>0.115743</v>
       </c>
       <c r="E41" t="n">
-        <v>2351065126</v>
+        <v>2581956515</v>
       </c>
       <c r="F41" t="n">
-        <v>13427901</v>
+        <v>15714773</v>
       </c>
       <c r="G41" t="n">
-        <v>-0.71765</v>
+        <v>1.34216</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1.83</v>
+        <v>1.67</v>
       </c>
       <c r="E42" t="n">
-        <v>2316251069</v>
+        <v>2407120272</v>
       </c>
       <c r="F42" t="n">
-        <v>669478108</v>
+        <v>49566163</v>
       </c>
       <c r="G42" t="n">
-        <v>2.70562</v>
+        <v>0.21042</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1.001</v>
+        <v>0.089314</v>
       </c>
       <c r="E43" t="n">
-        <v>2200597722</v>
+        <v>2367381478</v>
       </c>
       <c r="F43" t="n">
-        <v>137261838</v>
+        <v>7092169</v>
       </c>
       <c r="G43" t="n">
-        <v>0.08049000000000001</v>
+        <v>1.39985</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>TIA</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Celestia</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>15.09</v>
+        <v>0.715853</v>
       </c>
       <c r="E44" t="n">
-        <v>2189609758</v>
+        <v>2242606657</v>
       </c>
       <c r="F44" t="n">
-        <v>239569105</v>
+        <v>94923001</v>
       </c>
       <c r="G44" t="n">
-        <v>0.67301</v>
+        <v>-5.40362</v>
       </c>
     </row>
     <row r="45">
@@ -1646,16 +1646,16 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.02981264</v>
+        <v>0.03051279</v>
       </c>
       <c r="E45" t="n">
-        <v>2169111215</v>
+        <v>2216643529</v>
       </c>
       <c r="F45" t="n">
-        <v>47585818</v>
+        <v>38033027</v>
       </c>
       <c r="G45" t="n">
-        <v>0.0332</v>
+        <v>-1.68413</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>TUSD</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.5990799999999999</v>
+        <v>0.994175</v>
       </c>
       <c r="E46" t="n">
-        <v>1876671709</v>
+        <v>2037314613</v>
       </c>
       <c r="F46" t="n">
-        <v>51696366</v>
+        <v>95586720</v>
       </c>
       <c r="G46" t="n">
-        <v>1.19627</v>
+        <v>-0.04741</v>
       </c>
     </row>
     <row r="47">
@@ -1700,16 +1700,16 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>1.001</v>
+        <v>0.997501</v>
       </c>
       <c r="E47" t="n">
-        <v>1841494564</v>
+        <v>2015202893</v>
       </c>
       <c r="F47" t="n">
-        <v>459625980</v>
+        <v>2011147005</v>
       </c>
       <c r="G47" t="n">
-        <v>-0.01856</v>
+        <v>-0.2988</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>117.97</v>
+        <v>2088.48</v>
       </c>
       <c r="E48" t="n">
-        <v>1715181715</v>
+        <v>1925059006</v>
       </c>
       <c r="F48" t="n">
-        <v>25262778</v>
+        <v>82932685</v>
       </c>
       <c r="G48" t="n">
-        <v>-0.18771</v>
+        <v>0.23261</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>1792.66</v>
+        <v>118.84</v>
       </c>
       <c r="E49" t="n">
-        <v>1648380282</v>
+        <v>1724872662</v>
       </c>
       <c r="F49" t="n">
-        <v>82960908</v>
+        <v>21658082</v>
       </c>
       <c r="G49" t="n">
-        <v>4.33082</v>
+        <v>-0.4053</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>BSV</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Bitcoin SV</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.170412</v>
+        <v>87.15000000000001</v>
       </c>
       <c r="E50" t="n">
-        <v>1594815052</v>
+        <v>1719689492</v>
       </c>
       <c r="F50" t="n">
-        <v>54716756</v>
+        <v>89331112</v>
       </c>
       <c r="G50" t="n">
-        <v>0.20431</v>
+        <v>3.15771</v>
       </c>
     </row>
     <row r="51">
@@ -1808,16 +1808,16 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.667311</v>
+        <v>0.72019</v>
       </c>
       <c r="E51" t="n">
-        <v>1535573064</v>
+        <v>1655177338</v>
       </c>
       <c r="F51" t="n">
-        <v>565905294</v>
+        <v>226226717</v>
       </c>
       <c r="G51" t="n">
-        <v>1.9943</v>
+        <v>1.88748</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-01-21
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>42790</v>
+        <v>41732</v>
       </c>
       <c r="E2" t="n">
-        <v>838715953858</v>
+        <v>818651115183</v>
       </c>
       <c r="F2" t="n">
-        <v>14307408035</v>
+        <v>8210590456</v>
       </c>
       <c r="G2" t="n">
-        <v>0.37919</v>
+        <v>0.4406</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2542.26</v>
+        <v>2471.05</v>
       </c>
       <c r="E3" t="n">
-        <v>305427899450</v>
+        <v>297005877842</v>
       </c>
       <c r="F3" t="n">
-        <v>19893896916</v>
+        <v>4353025520</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.10441</v>
+        <v>0.1045</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0.999293</v>
       </c>
       <c r="E4" t="n">
-        <v>95035237385</v>
+        <v>94869792209</v>
       </c>
       <c r="F4" t="n">
-        <v>27751424656</v>
+        <v>12333106519</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.03898</v>
+        <v>-0.01366</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>303.96</v>
+        <v>318.37</v>
       </c>
       <c r="E5" t="n">
-        <v>46804906731</v>
+        <v>49039706987</v>
       </c>
       <c r="F5" t="n">
-        <v>563647300</v>
+        <v>338266055</v>
       </c>
       <c r="G5" t="n">
-        <v>1.43925</v>
+        <v>1.21854</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>96.92</v>
+        <v>93.39</v>
       </c>
       <c r="E6" t="n">
-        <v>41894712720</v>
+        <v>40357715765</v>
       </c>
       <c r="F6" t="n">
-        <v>2011983791</v>
+        <v>1048269805</v>
       </c>
       <c r="G6" t="n">
-        <v>5.24875</v>
+        <v>1.60475</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.5768760000000001</v>
+        <v>0.5523400000000001</v>
       </c>
       <c r="E7" t="n">
-        <v>31268733409</v>
+        <v>30020044405</v>
       </c>
       <c r="F7" t="n">
-        <v>507653248</v>
+        <v>575769808</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2911</v>
+        <v>0.60766</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1.001</v>
+        <v>0.999718</v>
       </c>
       <c r="E8" t="n">
-        <v>25477897933</v>
+        <v>25765376748</v>
       </c>
       <c r="F8" t="n">
-        <v>9250266594</v>
+        <v>2256365761</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.01051</v>
+        <v>0.01271</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2539.31</v>
+        <v>2471.51</v>
       </c>
       <c r="E9" t="n">
-        <v>23612768623</v>
+        <v>23065655266</v>
       </c>
       <c r="F9" t="n">
-        <v>18193396</v>
+        <v>14200643</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.11701</v>
+        <v>0.16882</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.5448809999999999</v>
+        <v>0.516809</v>
       </c>
       <c r="E10" t="n">
-        <v>19120029255</v>
+        <v>18149997115</v>
       </c>
       <c r="F10" t="n">
-        <v>318653867</v>
+        <v>256075987</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.53882</v>
+        <v>0.36765</v>
       </c>
     </row>
     <row r="11">
@@ -719,25 +719,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>DOGE</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Dogecoin</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>36.42</v>
+        <v>0.086608</v>
       </c>
       <c r="E11" t="n">
-        <v>13366410616</v>
+        <v>12339343677</v>
       </c>
       <c r="F11" t="n">
-        <v>509010540</v>
+        <v>1360393172</v>
       </c>
       <c r="G11" t="n">
-        <v>1.19509</v>
+        <v>9.10487</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +746,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>DOGE</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Dogecoin</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.082804</v>
+        <v>33.37</v>
       </c>
       <c r="E12" t="n">
-        <v>11827898157</v>
+        <v>12237345227</v>
       </c>
       <c r="F12" t="n">
-        <v>445893724</v>
+        <v>333436050</v>
       </c>
       <c r="G12" t="n">
-        <v>3.23823</v>
+        <v>2.8987</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.114738</v>
+        <v>0.110777</v>
       </c>
       <c r="E13" t="n">
-        <v>10111048246</v>
+        <v>9769610452</v>
       </c>
       <c r="F13" t="n">
-        <v>792259148</v>
+        <v>181906240</v>
       </c>
       <c r="G13" t="n">
-        <v>1.50546</v>
+        <v>0.63397</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>7.57</v>
+        <v>6.92</v>
       </c>
       <c r="E14" t="n">
-        <v>9989356401</v>
+        <v>9135382414</v>
       </c>
       <c r="F14" t="n">
-        <v>169120617</v>
+        <v>125626222</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.95464</v>
+        <v>0.975</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>15.04</v>
+        <v>15.73</v>
       </c>
       <c r="E15" t="n">
-        <v>8556595787</v>
+        <v>8955172366</v>
       </c>
       <c r="F15" t="n">
-        <v>552633744</v>
+        <v>435907981</v>
       </c>
       <c r="G15" t="n">
-        <v>5.35931</v>
+        <v>-1.86797</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.867233</v>
+        <v>2.25</v>
       </c>
       <c r="E16" t="n">
-        <v>8041587333</v>
+        <v>7786165949</v>
       </c>
       <c r="F16" t="n">
-        <v>315590438</v>
+        <v>33127241</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.62422</v>
+        <v>1.02866</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2.28</v>
+        <v>0.7937920000000001</v>
       </c>
       <c r="E17" t="n">
-        <v>7892987706</v>
+        <v>7375343517</v>
       </c>
       <c r="F17" t="n">
-        <v>57363484</v>
+        <v>275391293</v>
       </c>
       <c r="G17" t="n">
-        <v>7.93493</v>
+        <v>2.23151</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>42781</v>
+        <v>41670</v>
       </c>
       <c r="E18" t="n">
-        <v>6763821831</v>
+        <v>6594693649</v>
       </c>
       <c r="F18" t="n">
-        <v>250284532</v>
+        <v>124647440</v>
       </c>
       <c r="G18" t="n">
-        <v>0.43331</v>
+        <v>0.36957</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>13.3</v>
+        <v>9.480000000000001e-06</v>
       </c>
       <c r="E19" t="n">
-        <v>6059479127</v>
+        <v>5591248068</v>
       </c>
       <c r="F19" t="n">
-        <v>233563558</v>
+        <v>135244855</v>
       </c>
       <c r="G19" t="n">
-        <v>3.88334</v>
+        <v>0.5659999999999999</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>9.88e-06</v>
+        <v>71.16</v>
       </c>
       <c r="E20" t="n">
-        <v>5819445309</v>
+        <v>5276264888</v>
       </c>
       <c r="F20" t="n">
-        <v>117945167</v>
+        <v>237949064</v>
       </c>
       <c r="G20" t="n">
-        <v>0.6561399999999999</v>
+        <v>0.08298</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>71.69</v>
+        <v>0.998804</v>
       </c>
       <c r="E21" t="n">
-        <v>5312242497</v>
+        <v>5169190138</v>
       </c>
       <c r="F21" t="n">
-        <v>514406407</v>
+        <v>73015812</v>
       </c>
       <c r="G21" t="n">
-        <v>0.05971</v>
+        <v>-0.08746</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.99977</v>
+        <v>11.29</v>
       </c>
       <c r="E22" t="n">
-        <v>5252841442</v>
+        <v>5158716104</v>
       </c>
       <c r="F22" t="n">
-        <v>130073276</v>
+        <v>83331325</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.02637</v>
+        <v>1.59238</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>255.96</v>
+        <v>6.47</v>
       </c>
       <c r="E23" t="n">
-        <v>5033798569</v>
+        <v>4872321380</v>
       </c>
       <c r="F23" t="n">
-        <v>215009984</v>
+        <v>60082263</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.13258</v>
+        <v>-0.63605</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>6.58</v>
+        <v>239.49</v>
       </c>
       <c r="E24" t="n">
-        <v>4952303220</v>
+        <v>4700144546</v>
       </c>
       <c r="F24" t="n">
-        <v>159412431</v>
+        <v>112819325</v>
       </c>
       <c r="G24" t="n">
-        <v>0.38575</v>
+        <v>1.21861</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>28.05</v>
+        <v>9.789999999999999</v>
       </c>
       <c r="E25" t="n">
-        <v>4024338787</v>
+        <v>3758991054</v>
       </c>
       <c r="F25" t="n">
-        <v>314351946</v>
+        <v>78750916</v>
       </c>
       <c r="G25" t="n">
-        <v>-3.78961</v>
+        <v>1.25138</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>10.16</v>
+        <v>4.01</v>
       </c>
       <c r="E26" t="n">
-        <v>3888245163</v>
+        <v>3702250938</v>
       </c>
       <c r="F26" t="n">
-        <v>179077629</v>
+        <v>875768</v>
       </c>
       <c r="G26" t="n">
-        <v>1.09964</v>
+        <v>0.91174</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>4.06</v>
+        <v>24.69</v>
       </c>
       <c r="E27" t="n">
-        <v>3758023659</v>
+        <v>3539463034</v>
       </c>
       <c r="F27" t="n">
-        <v>1165327</v>
+        <v>168206452</v>
       </c>
       <c r="G27" t="n">
-        <v>0.10898</v>
+        <v>-0.38848</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>3.77</v>
+        <v>0.116119</v>
       </c>
       <c r="E28" t="n">
-        <v>3606139832</v>
+        <v>3294271351</v>
       </c>
       <c r="F28" t="n">
-        <v>185597732</v>
+        <v>48988246</v>
       </c>
       <c r="G28" t="n">
-        <v>-1.15445</v>
+        <v>1.82774</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>3.41</v>
+        <v>53.79</v>
       </c>
       <c r="E29" t="n">
-        <v>3459651464</v>
+        <v>3226646118</v>
       </c>
       <c r="F29" t="n">
-        <v>139759161</v>
+        <v>3652480</v>
       </c>
       <c r="G29" t="n">
-        <v>0.66249</v>
+        <v>0.89825</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.11992</v>
+        <v>36.05</v>
       </c>
       <c r="E30" t="n">
-        <v>3394946653</v>
+        <v>3192947532</v>
       </c>
       <c r="F30" t="n">
-        <v>56514269</v>
+        <v>93781573</v>
       </c>
       <c r="G30" t="n">
-        <v>0.41485</v>
+        <v>2.10215</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>9.73</v>
+        <v>3.23</v>
       </c>
       <c r="E31" t="n">
-        <v>3244770944</v>
+        <v>3092955273</v>
       </c>
       <c r="F31" t="n">
-        <v>317224748</v>
+        <v>111087243</v>
       </c>
       <c r="G31" t="n">
-        <v>0.44356</v>
+        <v>2.42895</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>53.73</v>
+        <v>3</v>
       </c>
       <c r="E32" t="n">
-        <v>3224876054</v>
+        <v>3085812680</v>
       </c>
       <c r="F32" t="n">
-        <v>4230407</v>
+        <v>107933666</v>
       </c>
       <c r="G32" t="n">
-        <v>0.2525</v>
+        <v>2.53166</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>38.01</v>
+        <v>160.21</v>
       </c>
       <c r="E33" t="n">
-        <v>3221424410</v>
+        <v>2901794703</v>
       </c>
       <c r="F33" t="n">
-        <v>195260724</v>
+        <v>67801209</v>
       </c>
       <c r="G33" t="n">
-        <v>3.00781</v>
+        <v>2.85263</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>TIA</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Celestia</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>19.72</v>
+        <v>8.58</v>
       </c>
       <c r="E34" t="n">
-        <v>3118861228</v>
+        <v>2883779617</v>
       </c>
       <c r="F34" t="n">
-        <v>437259675</v>
+        <v>82526323</v>
       </c>
       <c r="G34" t="n">
-        <v>15.74921</v>
+        <v>1.36963</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>TIA</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Celestia</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>6.12</v>
+        <v>17.49</v>
       </c>
       <c r="E35" t="n">
-        <v>3041336526</v>
+        <v>2778428591</v>
       </c>
       <c r="F35" t="n">
-        <v>217254639</v>
+        <v>76335809</v>
       </c>
       <c r="G35" t="n">
-        <v>2.90776</v>
+        <v>1.51008</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>3.31</v>
+        <v>5.51</v>
       </c>
       <c r="E36" t="n">
-        <v>2938671711</v>
+        <v>2739946357</v>
       </c>
       <c r="F36" t="n">
-        <v>109028978</v>
+        <v>114698454</v>
       </c>
       <c r="G36" t="n">
-        <v>-2.2742</v>
+        <v>1.00168</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>FDUSD</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>First Digital USD</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>157.55</v>
+        <v>1.001</v>
       </c>
       <c r="E37" t="n">
-        <v>2857647497</v>
+        <v>2616525084</v>
       </c>
       <c r="F37" t="n">
-        <v>84625379</v>
+        <v>1393055429</v>
       </c>
       <c r="G37" t="n">
-        <v>3.57223</v>
+        <v>-0.13301</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>2.07</v>
+        <v>2.92</v>
       </c>
       <c r="E38" t="n">
-        <v>2731666421</v>
+        <v>2599157514</v>
       </c>
       <c r="F38" t="n">
-        <v>94796208</v>
+        <v>54804017</v>
       </c>
       <c r="G38" t="n">
-        <v>-2.24083</v>
+        <v>1.359</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>2.14</v>
+        <v>0.07657899999999999</v>
       </c>
       <c r="E39" t="n">
-        <v>2723260076</v>
+        <v>2579730768</v>
       </c>
       <c r="F39" t="n">
-        <v>524765215</v>
+        <v>27486604</v>
       </c>
       <c r="G39" t="n">
-        <v>-0.79235</v>
+        <v>0.84907</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.079858</v>
+        <v>1.95</v>
       </c>
       <c r="E40" t="n">
-        <v>2688359204</v>
+        <v>2574695093</v>
       </c>
       <c r="F40" t="n">
-        <v>52655919</v>
+        <v>37602320</v>
       </c>
       <c r="G40" t="n">
-        <v>0.75824</v>
+        <v>1.8173</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.115743</v>
+        <v>1.87</v>
       </c>
       <c r="E41" t="n">
-        <v>2581956515</v>
+        <v>2382085324</v>
       </c>
       <c r="F41" t="n">
-        <v>15714773</v>
+        <v>375978236</v>
       </c>
       <c r="G41" t="n">
-        <v>1.34216</v>
+        <v>4.74167</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1.67</v>
+        <v>0.103367</v>
       </c>
       <c r="E42" t="n">
-        <v>2407120272</v>
+        <v>2317510587</v>
       </c>
       <c r="F42" t="n">
-        <v>49566163</v>
+        <v>9677223</v>
       </c>
       <c r="G42" t="n">
-        <v>0.21042</v>
+        <v>0.3001</v>
       </c>
     </row>
     <row r="43">
@@ -1592,16 +1592,16 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.089314</v>
+        <v>0.083202</v>
       </c>
       <c r="E43" t="n">
-        <v>2367381478</v>
+        <v>2203510605</v>
       </c>
       <c r="F43" t="n">
-        <v>7092169</v>
+        <v>5581298</v>
       </c>
       <c r="G43" t="n">
-        <v>1.39985</v>
+        <v>0.6094000000000001</v>
       </c>
     </row>
     <row r="44">
@@ -1619,16 +1619,16 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.715853</v>
+        <v>0.677505</v>
       </c>
       <c r="E44" t="n">
-        <v>2242606657</v>
+        <v>2143850275</v>
       </c>
       <c r="F44" t="n">
-        <v>94923001</v>
+        <v>27161907</v>
       </c>
       <c r="G44" t="n">
-        <v>-5.40362</v>
+        <v>0.42289</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.03051279</v>
+        <v>1.48</v>
       </c>
       <c r="E45" t="n">
-        <v>2216643529</v>
+        <v>2121913033</v>
       </c>
       <c r="F45" t="n">
-        <v>38033027</v>
+        <v>33888053</v>
       </c>
       <c r="G45" t="n">
-        <v>-1.68413</v>
+        <v>2.2098</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.994175</v>
+        <v>0.02851196</v>
       </c>
       <c r="E46" t="n">
-        <v>2037314613</v>
+        <v>2073132010</v>
       </c>
       <c r="F46" t="n">
-        <v>95586720</v>
+        <v>29553106</v>
       </c>
       <c r="G46" t="n">
-        <v>-0.04741</v>
+        <v>0.79989</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>FDUSD</t>
+          <t>TUSD</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>First Digital USD</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.997501</v>
+        <v>0.987078</v>
       </c>
       <c r="E47" t="n">
-        <v>2015202893</v>
+        <v>1880352089</v>
       </c>
       <c r="F47" t="n">
-        <v>2011147005</v>
+        <v>53543876</v>
       </c>
       <c r="G47" t="n">
-        <v>-0.2988</v>
+        <v>0.03482</v>
       </c>
     </row>
     <row r="48">
@@ -1727,16 +1727,16 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>2088.48</v>
+        <v>1999.51</v>
       </c>
       <c r="E48" t="n">
-        <v>1925059006</v>
+        <v>1842776132</v>
       </c>
       <c r="F48" t="n">
-        <v>82932685</v>
+        <v>57513014</v>
       </c>
       <c r="G48" t="n">
-        <v>0.23261</v>
+        <v>3.02654</v>
       </c>
     </row>
     <row r="49">
@@ -1754,16 +1754,16 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>118.84</v>
+        <v>114.65</v>
       </c>
       <c r="E49" t="n">
-        <v>1724872662</v>
+        <v>1666554225</v>
       </c>
       <c r="F49" t="n">
-        <v>21658082</v>
+        <v>15555296</v>
       </c>
       <c r="G49" t="n">
-        <v>-0.4053</v>
+        <v>1.23717</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>BSV</t>
+          <t>SEI</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Bitcoin SV</t>
+          <t>Sei</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>87.15000000000001</v>
+        <v>0.678054</v>
       </c>
       <c r="E50" t="n">
-        <v>1719689492</v>
+        <v>1647573793</v>
       </c>
       <c r="F50" t="n">
-        <v>89331112</v>
+        <v>127378418</v>
       </c>
       <c r="G50" t="n">
-        <v>3.15771</v>
+        <v>0.94889</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>SEI</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Sei</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.72019</v>
+        <v>264.48</v>
       </c>
       <c r="E51" t="n">
-        <v>1655177338</v>
+        <v>1602743893</v>
       </c>
       <c r="F51" t="n">
-        <v>226226717</v>
+        <v>2831357</v>
       </c>
       <c r="G51" t="n">
-        <v>1.88748</v>
+        <v>8.05456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-01-28
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>41732</v>
+        <v>42321</v>
       </c>
       <c r="E2" t="n">
-        <v>818651115183</v>
+        <v>830492108062</v>
       </c>
       <c r="F2" t="n">
-        <v>8210590456</v>
+        <v>13695151538</v>
       </c>
       <c r="G2" t="n">
-        <v>0.4406</v>
+        <v>1.30507</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2471.05</v>
+        <v>2271.71</v>
       </c>
       <c r="E3" t="n">
-        <v>297005877842</v>
+        <v>273218759616</v>
       </c>
       <c r="F3" t="n">
-        <v>4353025520</v>
+        <v>6117519730</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1045</v>
+        <v>0.17584</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999293</v>
+        <v>0.999547</v>
       </c>
       <c r="E4" t="n">
-        <v>94869792209</v>
+        <v>95993219168</v>
       </c>
       <c r="F4" t="n">
-        <v>12333106519</v>
+        <v>22257190702</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.01366</v>
+        <v>0.0375</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>318.37</v>
+        <v>305.62</v>
       </c>
       <c r="E5" t="n">
-        <v>49039706987</v>
+        <v>47075580775</v>
       </c>
       <c r="F5" t="n">
-        <v>338266055</v>
+        <v>481764802</v>
       </c>
       <c r="G5" t="n">
-        <v>1.21854</v>
+        <v>0.44138</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>93.39</v>
+        <v>97.17</v>
       </c>
       <c r="E6" t="n">
-        <v>40357715765</v>
+        <v>42173109943</v>
       </c>
       <c r="F6" t="n">
-        <v>1048269805</v>
+        <v>1951515852</v>
       </c>
       <c r="G6" t="n">
-        <v>1.60475</v>
+        <v>5.75738</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.5523400000000001</v>
+        <v>0.5288</v>
       </c>
       <c r="E7" t="n">
-        <v>30020044405</v>
+        <v>28734960259</v>
       </c>
       <c r="F7" t="n">
-        <v>575769808</v>
+        <v>419890891</v>
       </c>
       <c r="G7" t="n">
-        <v>0.60766</v>
+        <v>-0.32527</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.999718</v>
+        <v>0.999524</v>
       </c>
       <c r="E8" t="n">
-        <v>25765376748</v>
+        <v>26108619516</v>
       </c>
       <c r="F8" t="n">
-        <v>2256365761</v>
+        <v>3170243521</v>
       </c>
       <c r="G8" t="n">
-        <v>0.01271</v>
+        <v>-0.08237999999999999</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2471.51</v>
+        <v>2272.23</v>
       </c>
       <c r="E9" t="n">
-        <v>23065655266</v>
+        <v>21323826336</v>
       </c>
       <c r="F9" t="n">
-        <v>14200643</v>
+        <v>15608200</v>
       </c>
       <c r="G9" t="n">
-        <v>0.16882</v>
+        <v>0.34966</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.516809</v>
+        <v>0.493538</v>
       </c>
       <c r="E10" t="n">
-        <v>18149997115</v>
+        <v>17373390598</v>
       </c>
       <c r="F10" t="n">
-        <v>256075987</v>
+        <v>302844795</v>
       </c>
       <c r="G10" t="n">
-        <v>0.36765</v>
+        <v>2.07222</v>
       </c>
     </row>
     <row r="11">
@@ -719,25 +719,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>DOGE</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Dogecoin</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.086608</v>
+        <v>35.78</v>
       </c>
       <c r="E11" t="n">
-        <v>12339343677</v>
+        <v>13178504751</v>
       </c>
       <c r="F11" t="n">
-        <v>1360393172</v>
+        <v>779976454</v>
       </c>
       <c r="G11" t="n">
-        <v>9.10487</v>
+        <v>10.41223</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +746,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>DOGE</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Dogecoin</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>33.37</v>
+        <v>0.079541</v>
       </c>
       <c r="E12" t="n">
-        <v>12237345227</v>
+        <v>11395278106</v>
       </c>
       <c r="F12" t="n">
-        <v>333436050</v>
+        <v>281364102</v>
       </c>
       <c r="G12" t="n">
-        <v>2.8987</v>
+        <v>-0.37941</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.110777</v>
+        <v>0.111727</v>
       </c>
       <c r="E13" t="n">
-        <v>9769610452</v>
+        <v>9846267907</v>
       </c>
       <c r="F13" t="n">
-        <v>181906240</v>
+        <v>245437131</v>
       </c>
       <c r="G13" t="n">
-        <v>0.63397</v>
+        <v>-2.41961</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>6.92</v>
+        <v>6.67</v>
       </c>
       <c r="E14" t="n">
-        <v>9135382414</v>
+        <v>8833009018</v>
       </c>
       <c r="F14" t="n">
-        <v>125626222</v>
+        <v>160313695</v>
       </c>
       <c r="G14" t="n">
-        <v>0.975</v>
+        <v>0.22773</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>15.73</v>
+        <v>14.45</v>
       </c>
       <c r="E15" t="n">
-        <v>8955172366</v>
+        <v>8222508628</v>
       </c>
       <c r="F15" t="n">
-        <v>435907981</v>
+        <v>297341015</v>
       </c>
       <c r="G15" t="n">
-        <v>-1.86797</v>
+        <v>1.49187</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2.25</v>
+        <v>0.792156</v>
       </c>
       <c r="E16" t="n">
-        <v>7786165949</v>
+        <v>7362214771</v>
       </c>
       <c r="F16" t="n">
-        <v>33127241</v>
+        <v>310379960</v>
       </c>
       <c r="G16" t="n">
-        <v>1.02866</v>
+        <v>3.07889</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.7937920000000001</v>
+        <v>2.11</v>
       </c>
       <c r="E17" t="n">
-        <v>7375343517</v>
+        <v>7319162621</v>
       </c>
       <c r="F17" t="n">
-        <v>275391293</v>
+        <v>12450200</v>
       </c>
       <c r="G17" t="n">
-        <v>2.23151</v>
+        <v>2.15062</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>41670</v>
+        <v>42165</v>
       </c>
       <c r="E18" t="n">
-        <v>6594693649</v>
+        <v>6659446151</v>
       </c>
       <c r="F18" t="n">
-        <v>124647440</v>
+        <v>155470938</v>
       </c>
       <c r="G18" t="n">
-        <v>0.36957</v>
+        <v>1.13858</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>9.480000000000001e-06</v>
+        <v>12.49</v>
       </c>
       <c r="E19" t="n">
-        <v>5591248068</v>
+        <v>5722725459</v>
       </c>
       <c r="F19" t="n">
-        <v>135244855</v>
+        <v>139861241</v>
       </c>
       <c r="G19" t="n">
-        <v>0.5659999999999999</v>
+        <v>-0.55908</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>71.16</v>
+        <v>9.099999999999999e-06</v>
       </c>
       <c r="E20" t="n">
-        <v>5276264888</v>
+        <v>5364989640</v>
       </c>
       <c r="F20" t="n">
-        <v>237949064</v>
+        <v>80224391</v>
       </c>
       <c r="G20" t="n">
-        <v>0.08298</v>
+        <v>0.55628</v>
       </c>
     </row>
     <row r="21">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.998804</v>
+        <v>0.998708</v>
       </c>
       <c r="E21" t="n">
-        <v>5169190138</v>
+        <v>5227568119</v>
       </c>
       <c r="F21" t="n">
-        <v>73015812</v>
+        <v>140419088</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.08746</v>
+        <v>-0.15169</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>11.29</v>
+        <v>67.45999999999999</v>
       </c>
       <c r="E22" t="n">
-        <v>5158716104</v>
+        <v>5004501090</v>
       </c>
       <c r="F22" t="n">
-        <v>83331325</v>
+        <v>209212851</v>
       </c>
       <c r="G22" t="n">
-        <v>1.59238</v>
+        <v>0.5116000000000001</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>6.47</v>
+        <v>240.82</v>
       </c>
       <c r="E23" t="n">
-        <v>4872321380</v>
+        <v>4737359352</v>
       </c>
       <c r="F23" t="n">
-        <v>60082263</v>
+        <v>135652266</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.63605</v>
+        <v>0.18007</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>239.49</v>
+        <v>5.97</v>
       </c>
       <c r="E24" t="n">
-        <v>4700144546</v>
+        <v>4509306868</v>
       </c>
       <c r="F24" t="n">
-        <v>112819325</v>
+        <v>61099003</v>
       </c>
       <c r="G24" t="n">
-        <v>1.21861</v>
+        <v>0.66314</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>9.789999999999999</v>
+        <v>4.02</v>
       </c>
       <c r="E25" t="n">
-        <v>3758991054</v>
+        <v>3730353999</v>
       </c>
       <c r="F25" t="n">
-        <v>78750916</v>
+        <v>979564</v>
       </c>
       <c r="G25" t="n">
-        <v>1.25138</v>
+        <v>-1.3253</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>4.01</v>
+        <v>9.52</v>
       </c>
       <c r="E26" t="n">
-        <v>3702250938</v>
+        <v>3660579120</v>
       </c>
       <c r="F26" t="n">
-        <v>875768</v>
+        <v>139692498</v>
       </c>
       <c r="G26" t="n">
-        <v>0.91174</v>
+        <v>-0.06261</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>24.69</v>
+        <v>23.75</v>
       </c>
       <c r="E27" t="n">
-        <v>3539463034</v>
+        <v>3410126213</v>
       </c>
       <c r="F27" t="n">
-        <v>168206452</v>
+        <v>143586131</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.38848</v>
+        <v>-0.86826</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.116119</v>
+        <v>37.58</v>
       </c>
       <c r="E28" t="n">
-        <v>3294271351</v>
+        <v>3329054311</v>
       </c>
       <c r="F28" t="n">
-        <v>48988246</v>
+        <v>188625946</v>
       </c>
       <c r="G28" t="n">
-        <v>1.82774</v>
+        <v>7.6221</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>53.79</v>
+        <v>0.11462</v>
       </c>
       <c r="E29" t="n">
-        <v>3226646118</v>
+        <v>3255054834</v>
       </c>
       <c r="F29" t="n">
-        <v>3652480</v>
+        <v>50189685</v>
       </c>
       <c r="G29" t="n">
-        <v>0.89825</v>
+        <v>-1.6747</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>36.05</v>
+        <v>52.04</v>
       </c>
       <c r="E30" t="n">
-        <v>3192947532</v>
+        <v>3128171189</v>
       </c>
       <c r="F30" t="n">
-        <v>93781573</v>
+        <v>8881733</v>
       </c>
       <c r="G30" t="n">
-        <v>2.10215</v>
+        <v>-2.38593</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>3.23</v>
+        <v>2.97</v>
       </c>
       <c r="E31" t="n">
-        <v>3092955273</v>
+        <v>3051305138</v>
       </c>
       <c r="F31" t="n">
-        <v>111087243</v>
+        <v>197751855</v>
       </c>
       <c r="G31" t="n">
-        <v>2.42895</v>
+        <v>2.8764</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>3</v>
+        <v>8.949999999999999</v>
       </c>
       <c r="E32" t="n">
-        <v>3085812680</v>
+        <v>3025189835</v>
       </c>
       <c r="F32" t="n">
-        <v>107933666</v>
+        <v>109030465</v>
       </c>
       <c r="G32" t="n">
-        <v>2.53166</v>
+        <v>-0.94171</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>160.21</v>
+        <v>3.09</v>
       </c>
       <c r="E33" t="n">
-        <v>2901794703</v>
+        <v>2959472583</v>
       </c>
       <c r="F33" t="n">
-        <v>67801209</v>
+        <v>138423608</v>
       </c>
       <c r="G33" t="n">
-        <v>2.85263</v>
+        <v>1.35537</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>8.58</v>
+        <v>159.89</v>
       </c>
       <c r="E34" t="n">
-        <v>2883779617</v>
+        <v>2904573106</v>
       </c>
       <c r="F34" t="n">
-        <v>82526323</v>
+        <v>50570719</v>
       </c>
       <c r="G34" t="n">
-        <v>1.36963</v>
+        <v>-0.68785</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>TIA</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Celestia</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>17.49</v>
+        <v>3.11</v>
       </c>
       <c r="E35" t="n">
-        <v>2778428591</v>
+        <v>2777486006</v>
       </c>
       <c r="F35" t="n">
-        <v>76335809</v>
+        <v>47030840</v>
       </c>
       <c r="G35" t="n">
-        <v>1.51008</v>
+        <v>3.14679</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>TIA</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Celestia</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>5.51</v>
+        <v>17.04</v>
       </c>
       <c r="E36" t="n">
-        <v>2739946357</v>
+        <v>2741641285</v>
       </c>
       <c r="F36" t="n">
-        <v>114698454</v>
+        <v>118633054</v>
       </c>
       <c r="G36" t="n">
-        <v>1.00168</v>
+        <v>1.26898</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>FDUSD</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>First Digital USD</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1.001</v>
+        <v>1.94</v>
       </c>
       <c r="E37" t="n">
-        <v>2616525084</v>
+        <v>2624209123</v>
       </c>
       <c r="F37" t="n">
-        <v>1393055429</v>
+        <v>49551442</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.13301</v>
+        <v>0.77366</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>2.92</v>
+        <v>5.21</v>
       </c>
       <c r="E38" t="n">
-        <v>2599157514</v>
+        <v>2612613145</v>
       </c>
       <c r="F38" t="n">
-        <v>54804017</v>
+        <v>121372607</v>
       </c>
       <c r="G38" t="n">
-        <v>1.359</v>
+        <v>-1.3966</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>FDUSD</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>First Digital USD</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.07657899999999999</v>
+        <v>0.998757</v>
       </c>
       <c r="E39" t="n">
-        <v>2579730768</v>
+        <v>2588859435</v>
       </c>
       <c r="F39" t="n">
-        <v>27486604</v>
+        <v>2065762098</v>
       </c>
       <c r="G39" t="n">
-        <v>0.84907</v>
+        <v>-0.03568</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1.95</v>
+        <v>0.07421999999999999</v>
       </c>
       <c r="E40" t="n">
-        <v>2574695093</v>
+        <v>2502058238</v>
       </c>
       <c r="F40" t="n">
-        <v>37602320</v>
+        <v>23179653</v>
       </c>
       <c r="G40" t="n">
-        <v>1.8173</v>
+        <v>-0.1024</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1.87</v>
+        <v>0.105592</v>
       </c>
       <c r="E41" t="n">
-        <v>2382085324</v>
+        <v>2393681407</v>
       </c>
       <c r="F41" t="n">
-        <v>375978236</v>
+        <v>14871555</v>
       </c>
       <c r="G41" t="n">
-        <v>4.74167</v>
+        <v>0.89373</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.103367</v>
+        <v>1.84</v>
       </c>
       <c r="E42" t="n">
-        <v>2317510587</v>
+        <v>2350679739</v>
       </c>
       <c r="F42" t="n">
-        <v>9677223</v>
+        <v>356313796</v>
       </c>
       <c r="G42" t="n">
-        <v>0.3001</v>
+        <v>2.5058</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.083202</v>
+        <v>372.09</v>
       </c>
       <c r="E43" t="n">
-        <v>2203510605</v>
+        <v>2271967245</v>
       </c>
       <c r="F43" t="n">
-        <v>5581298</v>
+        <v>11501229</v>
       </c>
       <c r="G43" t="n">
-        <v>0.6094000000000001</v>
+        <v>11.69347</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.677505</v>
+        <v>1.52</v>
       </c>
       <c r="E44" t="n">
-        <v>2143850275</v>
+        <v>2191258743</v>
       </c>
       <c r="F44" t="n">
-        <v>27161907</v>
+        <v>44074928</v>
       </c>
       <c r="G44" t="n">
-        <v>0.42289</v>
+        <v>0.21957</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>1.48</v>
+        <v>0.081175</v>
       </c>
       <c r="E45" t="n">
-        <v>2121913033</v>
+        <v>2154171967</v>
       </c>
       <c r="F45" t="n">
-        <v>33888053</v>
+        <v>5721873</v>
       </c>
       <c r="G45" t="n">
-        <v>2.2098</v>
+        <v>-0.37099</v>
       </c>
     </row>
     <row r="46">
@@ -1673,16 +1673,16 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.02851196</v>
+        <v>0.02842794</v>
       </c>
       <c r="E46" t="n">
-        <v>2073132010</v>
+        <v>2069582345</v>
       </c>
       <c r="F46" t="n">
-        <v>29553106</v>
+        <v>36288019</v>
       </c>
       <c r="G46" t="n">
-        <v>0.79989</v>
+        <v>2.05685</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.987078</v>
+        <v>0.648046</v>
       </c>
       <c r="E47" t="n">
-        <v>1880352089</v>
+        <v>2054400826</v>
       </c>
       <c r="F47" t="n">
-        <v>53543876</v>
+        <v>45880692</v>
       </c>
       <c r="G47" t="n">
-        <v>0.03482</v>
+        <v>-0.9555399999999999</v>
       </c>
     </row>
     <row r="48">
@@ -1727,16 +1727,16 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>1999.51</v>
+        <v>1988.7</v>
       </c>
       <c r="E48" t="n">
-        <v>1842776132</v>
+        <v>1837061478</v>
       </c>
       <c r="F48" t="n">
-        <v>57513014</v>
+        <v>56147238</v>
       </c>
       <c r="G48" t="n">
-        <v>3.02654</v>
+        <v>-1.62676</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>SEI</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>Sei</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>114.65</v>
+        <v>0.655002</v>
       </c>
       <c r="E49" t="n">
-        <v>1666554225</v>
+        <v>1615929947</v>
       </c>
       <c r="F49" t="n">
-        <v>15555296</v>
+        <v>157221549</v>
       </c>
       <c r="G49" t="n">
-        <v>1.23717</v>
+        <v>2.23989</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SEI</t>
+          <t>TUSD</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Sei</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.678054</v>
+        <v>0.985966</v>
       </c>
       <c r="E50" t="n">
-        <v>1647573793</v>
+        <v>1595947812</v>
       </c>
       <c r="F50" t="n">
-        <v>127378418</v>
+        <v>54959830</v>
       </c>
       <c r="G50" t="n">
-        <v>0.94889</v>
+        <v>-0.22305</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>QNT</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>264.48</v>
+        <v>107.82</v>
       </c>
       <c r="E51" t="n">
-        <v>1602743893</v>
+        <v>1569694704</v>
       </c>
       <c r="F51" t="n">
-        <v>2831357</v>
+        <v>17163814</v>
       </c>
       <c r="G51" t="n">
-        <v>8.05456</v>
+        <v>-1.30366</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-02-04
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>42321</v>
+        <v>43078</v>
       </c>
       <c r="E2" t="n">
-        <v>830492108062</v>
+        <v>844574158403</v>
       </c>
       <c r="F2" t="n">
-        <v>13695151538</v>
+        <v>8579251721</v>
       </c>
       <c r="G2" t="n">
-        <v>1.30507</v>
+        <v>0.10174</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2271.71</v>
+        <v>2309.29</v>
       </c>
       <c r="E3" t="n">
-        <v>273218759616</v>
+        <v>277313827745</v>
       </c>
       <c r="F3" t="n">
-        <v>6117519730</v>
+        <v>4495841424</v>
       </c>
       <c r="G3" t="n">
-        <v>0.17584</v>
+        <v>0.17041</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999547</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>95993219168</v>
+        <v>96197324041</v>
       </c>
       <c r="F4" t="n">
-        <v>22257190702</v>
+        <v>15934032561</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0375</v>
+        <v>0.07011000000000001</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>305.62</v>
+        <v>300.14</v>
       </c>
       <c r="E5" t="n">
-        <v>47075580775</v>
+        <v>46154995940</v>
       </c>
       <c r="F5" t="n">
-        <v>481764802</v>
+        <v>298877552</v>
       </c>
       <c r="G5" t="n">
-        <v>0.44138</v>
+        <v>-0.5301900000000001</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>97.17</v>
+        <v>98.25</v>
       </c>
       <c r="E6" t="n">
-        <v>42173109943</v>
+        <v>42807942713</v>
       </c>
       <c r="F6" t="n">
-        <v>1951515852</v>
+        <v>1521841560</v>
       </c>
       <c r="G6" t="n">
-        <v>5.75738</v>
+        <v>-0.5954700000000001</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.5288</v>
+        <v>0.51273</v>
       </c>
       <c r="E7" t="n">
-        <v>28734960259</v>
+        <v>27905941067</v>
       </c>
       <c r="F7" t="n">
-        <v>419890891</v>
+        <v>587870855</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.32527</v>
+        <v>-2.02791</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.999524</v>
+        <v>1.001</v>
       </c>
       <c r="E8" t="n">
-        <v>26108619516</v>
+        <v>27077350476</v>
       </c>
       <c r="F8" t="n">
-        <v>3170243521</v>
+        <v>2059829225</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.08237999999999999</v>
+        <v>0.07106</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2272.23</v>
+        <v>2307.44</v>
       </c>
       <c r="E9" t="n">
-        <v>21323826336</v>
+        <v>21891609938</v>
       </c>
       <c r="F9" t="n">
-        <v>15608200</v>
+        <v>8995410</v>
       </c>
       <c r="G9" t="n">
-        <v>0.34966</v>
+        <v>0.10357</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.493538</v>
+        <v>0.508147</v>
       </c>
       <c r="E10" t="n">
-        <v>17373390598</v>
+        <v>17822147261</v>
       </c>
       <c r="F10" t="n">
-        <v>302844795</v>
+        <v>234331370</v>
       </c>
       <c r="G10" t="n">
-        <v>2.07222</v>
+        <v>-2.82757</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>35.78</v>
+        <v>36.09</v>
       </c>
       <c r="E11" t="n">
-        <v>13178504751</v>
+        <v>13227179549</v>
       </c>
       <c r="F11" t="n">
-        <v>779976454</v>
+        <v>401585307</v>
       </c>
       <c r="G11" t="n">
-        <v>10.41223</v>
+        <v>0.97945</v>
       </c>
     </row>
     <row r="12">
@@ -755,70 +755,70 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.079541</v>
+        <v>0.079114</v>
       </c>
       <c r="E12" t="n">
-        <v>11395278106</v>
+        <v>11310731865</v>
       </c>
       <c r="F12" t="n">
-        <v>281364102</v>
+        <v>182765076</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.37941</v>
+        <v>0.03996</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.111727</v>
+        <v>18.16</v>
       </c>
       <c r="E13" t="n">
-        <v>9846267907</v>
+        <v>10652043548</v>
       </c>
       <c r="F13" t="n">
-        <v>245437131</v>
+        <v>649591385</v>
       </c>
       <c r="G13" t="n">
-        <v>-2.41961</v>
+        <v>1.75003</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>6.67</v>
+        <v>0.118736</v>
       </c>
       <c r="E14" t="n">
-        <v>8833009018</v>
+        <v>10457767911</v>
       </c>
       <c r="F14" t="n">
-        <v>160313695</v>
+        <v>185906350</v>
       </c>
       <c r="G14" t="n">
-        <v>0.22773</v>
+        <v>1.97329</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>14.45</v>
+        <v>6.81</v>
       </c>
       <c r="E15" t="n">
-        <v>8222508628</v>
+        <v>9031877303</v>
       </c>
       <c r="F15" t="n">
-        <v>297341015</v>
+        <v>95513990</v>
       </c>
       <c r="G15" t="n">
-        <v>1.49187</v>
+        <v>-1.46021</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.792156</v>
+        <v>0.782527</v>
       </c>
       <c r="E16" t="n">
-        <v>7362214771</v>
+        <v>7257898397</v>
       </c>
       <c r="F16" t="n">
-        <v>310379960</v>
+        <v>216356049</v>
       </c>
       <c r="G16" t="n">
-        <v>3.07889</v>
+        <v>-0.89416</v>
       </c>
     </row>
     <row r="17">
@@ -890,16 +890,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2.11</v>
+        <v>2.03</v>
       </c>
       <c r="E17" t="n">
-        <v>7319162621</v>
+        <v>7008074556</v>
       </c>
       <c r="F17" t="n">
-        <v>12450200</v>
+        <v>10834302</v>
       </c>
       <c r="G17" t="n">
-        <v>2.15062</v>
+        <v>-0.53139</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>42165</v>
+        <v>43041</v>
       </c>
       <c r="E18" t="n">
-        <v>6659446151</v>
+        <v>6789970297</v>
       </c>
       <c r="F18" t="n">
-        <v>155470938</v>
+        <v>54020330</v>
       </c>
       <c r="G18" t="n">
-        <v>1.13858</v>
+        <v>0.29294</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>12.49</v>
+        <v>12.79</v>
       </c>
       <c r="E19" t="n">
-        <v>5722725459</v>
+        <v>5846010965</v>
       </c>
       <c r="F19" t="n">
-        <v>139861241</v>
+        <v>127112967</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.55908</v>
+        <v>-5.4726</v>
       </c>
     </row>
     <row r="20">
@@ -971,16 +971,16 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>9.099999999999999e-06</v>
+        <v>9.04e-06</v>
       </c>
       <c r="E20" t="n">
-        <v>5364989640</v>
+        <v>5328123409</v>
       </c>
       <c r="F20" t="n">
-        <v>80224391</v>
+        <v>68180466</v>
       </c>
       <c r="G20" t="n">
-        <v>0.55628</v>
+        <v>-0.48268</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.998708</v>
+        <v>68.06</v>
       </c>
       <c r="E21" t="n">
-        <v>5227568119</v>
+        <v>5045735459</v>
       </c>
       <c r="F21" t="n">
-        <v>140419088</v>
+        <v>196533260</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.15169</v>
+        <v>-0.28399</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>67.45999999999999</v>
+        <v>0.999953</v>
       </c>
       <c r="E22" t="n">
-        <v>5004501090</v>
+        <v>4883075320</v>
       </c>
       <c r="F22" t="n">
-        <v>209212851</v>
+        <v>137171597</v>
       </c>
       <c r="G22" t="n">
-        <v>0.5116000000000001</v>
+        <v>0.07278</v>
       </c>
     </row>
     <row r="23">
@@ -1052,16 +1052,16 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>240.82</v>
+        <v>240.64</v>
       </c>
       <c r="E23" t="n">
-        <v>4737359352</v>
+        <v>4718223991</v>
       </c>
       <c r="F23" t="n">
-        <v>135652266</v>
+        <v>148152928</v>
       </c>
       <c r="G23" t="n">
-        <v>0.18007</v>
+        <v>0.54599</v>
       </c>
     </row>
     <row r="24">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>5.97</v>
+        <v>6.05</v>
       </c>
       <c r="E24" t="n">
-        <v>4509306868</v>
+        <v>4560214336</v>
       </c>
       <c r="F24" t="n">
-        <v>61099003</v>
+        <v>50631185</v>
       </c>
       <c r="G24" t="n">
-        <v>0.66314</v>
+        <v>-1.779</v>
       </c>
     </row>
     <row r="25">
@@ -1106,16 +1106,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>4.02</v>
+        <v>4.03</v>
       </c>
       <c r="E25" t="n">
-        <v>3730353999</v>
+        <v>3734005183</v>
       </c>
       <c r="F25" t="n">
-        <v>979564</v>
+        <v>3879715</v>
       </c>
       <c r="G25" t="n">
-        <v>-1.3253</v>
+        <v>0.03114</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>9.52</v>
+        <v>25.45</v>
       </c>
       <c r="E26" t="n">
-        <v>3660579120</v>
+        <v>3642954624</v>
       </c>
       <c r="F26" t="n">
-        <v>139692498</v>
+        <v>192279476</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.06261</v>
+        <v>2.34966</v>
       </c>
     </row>
     <row r="27">
@@ -1151,79 +1151,79 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>23.75</v>
+        <v>9.09</v>
       </c>
       <c r="E27" t="n">
-        <v>3410126213</v>
+        <v>3485137010</v>
       </c>
       <c r="F27" t="n">
-        <v>143586131</v>
+        <v>89213967</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.86826</v>
+        <v>-0.418</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>37.58</v>
+        <v>0.110071</v>
       </c>
       <c r="E28" t="n">
-        <v>3329054311</v>
+        <v>3125936788</v>
       </c>
       <c r="F28" t="n">
-        <v>188625946</v>
+        <v>47617622</v>
       </c>
       <c r="G28" t="n">
-        <v>7.6221</v>
+        <v>-1.61404</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.11462</v>
+        <v>9.039999999999999</v>
       </c>
       <c r="E29" t="n">
-        <v>3255054834</v>
+        <v>3056981325</v>
       </c>
       <c r="F29" t="n">
-        <v>50189685</v>
+        <v>91573729</v>
       </c>
       <c r="G29" t="n">
-        <v>-1.6747</v>
+        <v>-5.98236</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>52.04</v>
+        <v>165.81</v>
       </c>
       <c r="E30" t="n">
-        <v>3128171189</v>
+        <v>3007250631</v>
       </c>
       <c r="F30" t="n">
-        <v>8881733</v>
+        <v>59004838</v>
       </c>
       <c r="G30" t="n">
-        <v>-2.38593</v>
+        <v>-0.85444</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>2.97</v>
+        <v>33.27</v>
       </c>
       <c r="E31" t="n">
-        <v>3051305138</v>
+        <v>2939236856</v>
       </c>
       <c r="F31" t="n">
-        <v>197751855</v>
+        <v>78171856</v>
       </c>
       <c r="G31" t="n">
-        <v>2.8764</v>
+        <v>-0.44431</v>
       </c>
     </row>
     <row r="32">
@@ -1286,79 +1286,79 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>8.949999999999999</v>
+        <v>2.14</v>
       </c>
       <c r="E32" t="n">
-        <v>3025189835</v>
+        <v>2910757206</v>
       </c>
       <c r="F32" t="n">
-        <v>109030465</v>
+        <v>56924594</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.94171</v>
+        <v>-1.08566</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>3.09</v>
+        <v>48.31</v>
       </c>
       <c r="E33" t="n">
-        <v>2959472583</v>
+        <v>2897575013</v>
       </c>
       <c r="F33" t="n">
-        <v>138423608</v>
+        <v>3944643</v>
       </c>
       <c r="G33" t="n">
-        <v>1.35537</v>
+        <v>-1.23228</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>159.89</v>
+        <v>2.81</v>
       </c>
       <c r="E34" t="n">
-        <v>2904573106</v>
+        <v>2895186098</v>
       </c>
       <c r="F34" t="n">
-        <v>50570719</v>
+        <v>75562330</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.68785</v>
+        <v>-0.8339800000000001</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>3.11</v>
+        <v>2.98</v>
       </c>
       <c r="E35" t="n">
-        <v>2777486006</v>
+        <v>2851474422</v>
       </c>
       <c r="F35" t="n">
-        <v>47030840</v>
+        <v>67844632</v>
       </c>
       <c r="G35" t="n">
-        <v>3.14679</v>
+        <v>-1.14699</v>
       </c>
     </row>
     <row r="36">
@@ -1403,16 +1403,16 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>17.04</v>
+        <v>17.08</v>
       </c>
       <c r="E36" t="n">
-        <v>2741641285</v>
+        <v>2762642855</v>
       </c>
       <c r="F36" t="n">
-        <v>118633054</v>
+        <v>97207793</v>
       </c>
       <c r="G36" t="n">
-        <v>1.26898</v>
+        <v>-5.60041</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1.94</v>
+        <v>428.69</v>
       </c>
       <c r="E37" t="n">
-        <v>2624209123</v>
+        <v>2646926542</v>
       </c>
       <c r="F37" t="n">
-        <v>49551442</v>
+        <v>6352589</v>
       </c>
       <c r="G37" t="n">
-        <v>0.77366</v>
+        <v>-3.85166</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>FDUSD</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>First Digital USD</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>5.21</v>
+        <v>0.99978</v>
       </c>
       <c r="E38" t="n">
-        <v>2612613145</v>
+        <v>2583312207</v>
       </c>
       <c r="F38" t="n">
-        <v>121372607</v>
+        <v>2083425899</v>
       </c>
       <c r="G38" t="n">
-        <v>-1.3966</v>
+        <v>0.01433</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>FDUSD</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>First Digital USD</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.998757</v>
+        <v>5.04</v>
       </c>
       <c r="E39" t="n">
-        <v>2588859435</v>
+        <v>2540025034</v>
       </c>
       <c r="F39" t="n">
-        <v>2065762098</v>
+        <v>114450557</v>
       </c>
       <c r="G39" t="n">
-        <v>-0.03568</v>
+        <v>-3.83839</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.07421999999999999</v>
+        <v>2.75</v>
       </c>
       <c r="E40" t="n">
-        <v>2502058238</v>
+        <v>2449495979</v>
       </c>
       <c r="F40" t="n">
-        <v>23179653</v>
+        <v>36056375</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.1024</v>
+        <v>-0.26438</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.105592</v>
+        <v>0.068771</v>
       </c>
       <c r="E41" t="n">
-        <v>2393681407</v>
+        <v>2314048921</v>
       </c>
       <c r="F41" t="n">
-        <v>14871555</v>
+        <v>21909276</v>
       </c>
       <c r="G41" t="n">
-        <v>0.89373</v>
+        <v>-0.51732</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1.84</v>
+        <v>0.10075</v>
       </c>
       <c r="E42" t="n">
-        <v>2350679739</v>
+        <v>2272704443</v>
       </c>
       <c r="F42" t="n">
-        <v>356313796</v>
+        <v>9324132</v>
       </c>
       <c r="G42" t="n">
-        <v>2.5058</v>
+        <v>-0.80327</v>
       </c>
     </row>
     <row r="43">
@@ -1583,79 +1583,79 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>372.09</v>
+        <v>1.77</v>
       </c>
       <c r="E43" t="n">
-        <v>2271967245</v>
+        <v>2253347963</v>
       </c>
       <c r="F43" t="n">
-        <v>11501229</v>
+        <v>169051386</v>
       </c>
       <c r="G43" t="n">
-        <v>11.69347</v>
+        <v>-1.53622</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1.52</v>
+        <v>0.081201</v>
       </c>
       <c r="E44" t="n">
-        <v>2191258743</v>
+        <v>2150843073</v>
       </c>
       <c r="F44" t="n">
-        <v>44074928</v>
+        <v>4892980</v>
       </c>
       <c r="G44" t="n">
-        <v>0.21957</v>
+        <v>-0.50139</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.081175</v>
+        <v>1.5</v>
       </c>
       <c r="E45" t="n">
-        <v>2154171967</v>
+        <v>2146889257</v>
       </c>
       <c r="F45" t="n">
-        <v>5721873</v>
+        <v>22016309</v>
       </c>
       <c r="G45" t="n">
-        <v>-0.37099</v>
+        <v>-2.41355</v>
       </c>
     </row>
     <row r="46">
@@ -1673,16 +1673,16 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.02842794</v>
+        <v>0.02826397</v>
       </c>
       <c r="E46" t="n">
-        <v>2069582345</v>
+        <v>2053224914</v>
       </c>
       <c r="F46" t="n">
-        <v>36288019</v>
+        <v>28278693</v>
       </c>
       <c r="G46" t="n">
-        <v>2.05685</v>
+        <v>-2.07937</v>
       </c>
     </row>
     <row r="47">
@@ -1700,97 +1700,97 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.648046</v>
+        <v>0.593969</v>
       </c>
       <c r="E47" t="n">
-        <v>2054400826</v>
+        <v>1880414962</v>
       </c>
       <c r="F47" t="n">
-        <v>45880692</v>
+        <v>21628765</v>
       </c>
       <c r="G47" t="n">
-        <v>-0.9555399999999999</v>
+        <v>0.36955</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>1988.7</v>
+        <v>4.97</v>
       </c>
       <c r="E48" t="n">
-        <v>1837061478</v>
+        <v>1869635138</v>
       </c>
       <c r="F48" t="n">
-        <v>56147238</v>
+        <v>116083089</v>
       </c>
       <c r="G48" t="n">
-        <v>-1.62676</v>
+        <v>2.42232</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>SEI</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Sei</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.655002</v>
+        <v>2020.5</v>
       </c>
       <c r="E49" t="n">
-        <v>1615929947</v>
+        <v>1864293643</v>
       </c>
       <c r="F49" t="n">
-        <v>157221549</v>
+        <v>43379023</v>
       </c>
       <c r="G49" t="n">
-        <v>2.23989</v>
+        <v>0.75641</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>TUSD</t>
+          <t>SUI</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>Sui</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.985966</v>
+        <v>1.51</v>
       </c>
       <c r="E50" t="n">
-        <v>1595947812</v>
+        <v>1759208928</v>
       </c>
       <c r="F50" t="n">
-        <v>54959830</v>
+        <v>263661177</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.22305</v>
+        <v>7.42558</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>QNT</t>
+          <t>SEI</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>Sei</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>107.82</v>
+        <v>0.619074</v>
       </c>
       <c r="E51" t="n">
-        <v>1569694704</v>
+        <v>1499436273</v>
       </c>
       <c r="F51" t="n">
-        <v>17163814</v>
+        <v>100420024</v>
       </c>
       <c r="G51" t="n">
-        <v>-1.30366</v>
+        <v>1.4926</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-02-11
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>43078</v>
+        <v>48461</v>
       </c>
       <c r="E2" t="n">
-        <v>844574158403</v>
+        <v>951190896285</v>
       </c>
       <c r="F2" t="n">
-        <v>8579251721</v>
+        <v>19786255673</v>
       </c>
       <c r="G2" t="n">
-        <v>0.10174</v>
+        <v>2.52235</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2309.29</v>
+        <v>2531</v>
       </c>
       <c r="E3" t="n">
-        <v>277313827745</v>
+        <v>304242038355</v>
       </c>
       <c r="F3" t="n">
-        <v>4495841424</v>
+        <v>7617326047</v>
       </c>
       <c r="G3" t="n">
-        <v>0.17041</v>
+        <v>1.61553</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>1.001</v>
       </c>
       <c r="E4" t="n">
-        <v>96197324041</v>
+        <v>96454290308</v>
       </c>
       <c r="F4" t="n">
-        <v>15934032561</v>
+        <v>26084958286</v>
       </c>
       <c r="G4" t="n">
-        <v>0.07011000000000001</v>
+        <v>-0.01342</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>300.14</v>
+        <v>322.92</v>
       </c>
       <c r="E5" t="n">
-        <v>46154995940</v>
+        <v>49701832805</v>
       </c>
       <c r="F5" t="n">
-        <v>298877552</v>
+        <v>476923714</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.5301900000000001</v>
+        <v>0.56041</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>98.25</v>
+        <v>110.18</v>
       </c>
       <c r="E6" t="n">
-        <v>42807942713</v>
+        <v>48126993126</v>
       </c>
       <c r="F6" t="n">
-        <v>1521841560</v>
+        <v>1469933219</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.5954700000000001</v>
+        <v>2.01941</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.51273</v>
+        <v>0.533124</v>
       </c>
       <c r="E7" t="n">
-        <v>27905941067</v>
+        <v>29068901850</v>
       </c>
       <c r="F7" t="n">
-        <v>587870855</v>
+        <v>620579571</v>
       </c>
       <c r="G7" t="n">
-        <v>-2.02791</v>
+        <v>2.16463</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1.001</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>27077350476</v>
+        <v>27968836234</v>
       </c>
       <c r="F8" t="n">
-        <v>2059829225</v>
+        <v>4219827484</v>
       </c>
       <c r="G8" t="n">
-        <v>0.07106</v>
+        <v>0.01127</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2307.44</v>
+        <v>2530.06</v>
       </c>
       <c r="E9" t="n">
-        <v>21891609938</v>
+        <v>24350888654</v>
       </c>
       <c r="F9" t="n">
-        <v>8995410</v>
+        <v>10464147</v>
       </c>
       <c r="G9" t="n">
-        <v>0.10357</v>
+        <v>1.72665</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.508147</v>
+        <v>0.552951</v>
       </c>
       <c r="E10" t="n">
-        <v>17822147261</v>
+        <v>19426771679</v>
       </c>
       <c r="F10" t="n">
-        <v>234331370</v>
+        <v>517437611</v>
       </c>
       <c r="G10" t="n">
-        <v>-2.82757</v>
+        <v>3.43052</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>36.09</v>
+        <v>40.62</v>
       </c>
       <c r="E11" t="n">
-        <v>13227179549</v>
+        <v>14911805042</v>
       </c>
       <c r="F11" t="n">
-        <v>401585307</v>
+        <v>643057134</v>
       </c>
       <c r="G11" t="n">
-        <v>0.97945</v>
+        <v>5.10293</v>
       </c>
     </row>
     <row r="12">
@@ -746,57 +746,57 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>DOGE</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Dogecoin</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.079114</v>
+        <v>20.47</v>
       </c>
       <c r="E12" t="n">
-        <v>11310731865</v>
+        <v>12022656082</v>
       </c>
       <c r="F12" t="n">
-        <v>182765076</v>
+        <v>921624967</v>
       </c>
       <c r="G12" t="n">
-        <v>0.03996</v>
+        <v>12.23084</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>DOGE</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Dogecoin</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>18.16</v>
+        <v>0.082359</v>
       </c>
       <c r="E13" t="n">
-        <v>10652043548</v>
+        <v>11780265319</v>
       </c>
       <c r="F13" t="n">
-        <v>649591385</v>
+        <v>330291370</v>
       </c>
       <c r="G13" t="n">
-        <v>1.75003</v>
+        <v>1.79812</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.118736</v>
+        <v>0.1248</v>
       </c>
       <c r="E14" t="n">
-        <v>10457767911</v>
+        <v>10994834803</v>
       </c>
       <c r="F14" t="n">
-        <v>185906350</v>
+        <v>199427326</v>
       </c>
       <c r="G14" t="n">
-        <v>1.97329</v>
+        <v>1.15001</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>6.81</v>
+        <v>7.3</v>
       </c>
       <c r="E15" t="n">
-        <v>9031877303</v>
+        <v>9698771289</v>
       </c>
       <c r="F15" t="n">
-        <v>95513990</v>
+        <v>167873726</v>
       </c>
       <c r="G15" t="n">
-        <v>-1.46021</v>
+        <v>2.46307</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.782527</v>
+        <v>0.856474</v>
       </c>
       <c r="E16" t="n">
-        <v>7257898397</v>
+        <v>7951193099</v>
       </c>
       <c r="F16" t="n">
-        <v>216356049</v>
+        <v>261032112</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.89416</v>
+        <v>1.25351</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2.03</v>
+        <v>48277</v>
       </c>
       <c r="E17" t="n">
-        <v>7008074556</v>
+        <v>7620494088</v>
       </c>
       <c r="F17" t="n">
-        <v>10834302</v>
+        <v>208042778</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.53139</v>
+        <v>2.26768</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>43041</v>
+        <v>2.12</v>
       </c>
       <c r="E18" t="n">
-        <v>6789970297</v>
+        <v>7331859545</v>
       </c>
       <c r="F18" t="n">
-        <v>54020330</v>
+        <v>15461018</v>
       </c>
       <c r="G18" t="n">
-        <v>0.29294</v>
+        <v>2.31448</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>12.79</v>
+        <v>13.48</v>
       </c>
       <c r="E19" t="n">
-        <v>5846010965</v>
+        <v>6181614896</v>
       </c>
       <c r="F19" t="n">
-        <v>127112967</v>
+        <v>112206421</v>
       </c>
       <c r="G19" t="n">
-        <v>-5.4726</v>
+        <v>5.70007</v>
       </c>
     </row>
     <row r="20">
@@ -971,16 +971,16 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>9.04e-06</v>
+        <v>9.500000000000001e-06</v>
       </c>
       <c r="E20" t="n">
-        <v>5328123409</v>
+        <v>5599871555</v>
       </c>
       <c r="F20" t="n">
-        <v>68180466</v>
+        <v>111815428</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.48268</v>
+        <v>1.89579</v>
       </c>
     </row>
     <row r="21">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>68.06</v>
+        <v>71.98999999999999</v>
       </c>
       <c r="E21" t="n">
-        <v>5045735459</v>
+        <v>5343077689</v>
       </c>
       <c r="F21" t="n">
-        <v>196533260</v>
+        <v>286191676</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.28399</v>
+        <v>2.25266</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.999953</v>
+        <v>266.82</v>
       </c>
       <c r="E22" t="n">
-        <v>4883075320</v>
+        <v>5216378852</v>
       </c>
       <c r="F22" t="n">
-        <v>137171597</v>
+        <v>408583575</v>
       </c>
       <c r="G22" t="n">
-        <v>0.07278</v>
+        <v>8.665179999999999</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>240.64</v>
+        <v>6.64</v>
       </c>
       <c r="E23" t="n">
-        <v>4718223991</v>
+        <v>5005779821</v>
       </c>
       <c r="F23" t="n">
-        <v>148152928</v>
+        <v>60627289</v>
       </c>
       <c r="G23" t="n">
-        <v>0.54599</v>
+        <v>0.43463</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>6.05</v>
+        <v>0.998206</v>
       </c>
       <c r="E24" t="n">
-        <v>4560214336</v>
+        <v>4917520805</v>
       </c>
       <c r="F24" t="n">
-        <v>50631185</v>
+        <v>228913794</v>
       </c>
       <c r="G24" t="n">
-        <v>-1.779</v>
+        <v>-0.23665</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>4.03</v>
+        <v>10.16</v>
       </c>
       <c r="E25" t="n">
-        <v>3734005183</v>
+        <v>3900295927</v>
       </c>
       <c r="F25" t="n">
-        <v>3879715</v>
+        <v>170728646</v>
       </c>
       <c r="G25" t="n">
-        <v>0.03114</v>
+        <v>1.45881</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>25.45</v>
+        <v>4.12</v>
       </c>
       <c r="E26" t="n">
-        <v>3642954624</v>
+        <v>3818813705</v>
       </c>
       <c r="F26" t="n">
-        <v>192279476</v>
+        <v>1437211</v>
       </c>
       <c r="G26" t="n">
-        <v>2.34966</v>
+        <v>0.43726</v>
       </c>
     </row>
     <row r="27">
@@ -1151,79 +1151,79 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>9.09</v>
+        <v>26.08</v>
       </c>
       <c r="E27" t="n">
-        <v>3485137010</v>
+        <v>3735683370</v>
       </c>
       <c r="F27" t="n">
-        <v>89213967</v>
+        <v>130285848</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.418</v>
+        <v>1.49157</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.110071</v>
+        <v>2.7</v>
       </c>
       <c r="E28" t="n">
-        <v>3125936788</v>
+        <v>3658965022</v>
       </c>
       <c r="F28" t="n">
-        <v>47617622</v>
+        <v>148822987</v>
       </c>
       <c r="G28" t="n">
-        <v>-1.61404</v>
+        <v>-1.18029</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>9.039999999999999</v>
+        <v>569.52</v>
       </c>
       <c r="E29" t="n">
-        <v>3056981325</v>
+        <v>3554949878</v>
       </c>
       <c r="F29" t="n">
-        <v>91573729</v>
+        <v>41851065</v>
       </c>
       <c r="G29" t="n">
-        <v>-5.98236</v>
+        <v>3.33664</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>165.81</v>
+        <v>3.63</v>
       </c>
       <c r="E30" t="n">
-        <v>3007250631</v>
+        <v>3476114169</v>
       </c>
       <c r="F30" t="n">
-        <v>59004838</v>
+        <v>172037473</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.85444</v>
+        <v>7.54606</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>33.27</v>
+        <v>3.16</v>
       </c>
       <c r="E31" t="n">
-        <v>2939236856</v>
+        <v>3275480918</v>
       </c>
       <c r="F31" t="n">
-        <v>78171856</v>
+        <v>190974110</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.44431</v>
+        <v>5.03088</v>
       </c>
     </row>
     <row r="32">
@@ -1286,79 +1286,79 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>2.14</v>
+        <v>0.144584</v>
       </c>
       <c r="E32" t="n">
-        <v>2910757206</v>
+        <v>3275414704</v>
       </c>
       <c r="F32" t="n">
-        <v>56924594</v>
+        <v>50508351</v>
       </c>
       <c r="G32" t="n">
-        <v>-1.08566</v>
+        <v>6.14877</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>TIA</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Celestia</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>48.31</v>
+        <v>19.75</v>
       </c>
       <c r="E33" t="n">
-        <v>2897575013</v>
+        <v>3236508845</v>
       </c>
       <c r="F33" t="n">
-        <v>3944643</v>
+        <v>152970097</v>
       </c>
       <c r="G33" t="n">
-        <v>-1.23228</v>
+        <v>-2.39467</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>2.81</v>
+        <v>0.112147</v>
       </c>
       <c r="E34" t="n">
-        <v>2895186098</v>
+        <v>3186080446</v>
       </c>
       <c r="F34" t="n">
-        <v>75562330</v>
+        <v>53067855</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.8339800000000001</v>
+        <v>0.7483300000000001</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>2.98</v>
+        <v>35.8</v>
       </c>
       <c r="E35" t="n">
-        <v>2851474422</v>
+        <v>3168916238</v>
       </c>
       <c r="F35" t="n">
-        <v>67844632</v>
+        <v>156211623</v>
       </c>
       <c r="G35" t="n">
-        <v>-1.14699</v>
+        <v>4.13752</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>TIA</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Celestia</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>17.08</v>
+        <v>9.18</v>
       </c>
       <c r="E36" t="n">
-        <v>2762642855</v>
+        <v>3117772396</v>
       </c>
       <c r="F36" t="n">
-        <v>97207793</v>
+        <v>78437410</v>
       </c>
       <c r="G36" t="n">
-        <v>-5.60041</v>
+        <v>0.92775</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>428.69</v>
+        <v>49.75</v>
       </c>
       <c r="E37" t="n">
-        <v>2646926542</v>
+        <v>2985974343</v>
       </c>
       <c r="F37" t="n">
-        <v>6352589</v>
+        <v>5012442</v>
       </c>
       <c r="G37" t="n">
-        <v>-3.85166</v>
+        <v>0.37987</v>
       </c>
     </row>
     <row r="38">
@@ -1457,16 +1457,16 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.99978</v>
+        <v>1.005</v>
       </c>
       <c r="E38" t="n">
-        <v>2583312207</v>
+        <v>2773842649</v>
       </c>
       <c r="F38" t="n">
-        <v>2083425899</v>
+        <v>3970353114</v>
       </c>
       <c r="G38" t="n">
-        <v>0.01433</v>
+        <v>-0.01832</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>5.04</v>
+        <v>1.91</v>
       </c>
       <c r="E39" t="n">
-        <v>2540025034</v>
+        <v>2746462690</v>
       </c>
       <c r="F39" t="n">
-        <v>114450557</v>
+        <v>81281031</v>
       </c>
       <c r="G39" t="n">
-        <v>-3.83839</v>
+        <v>8.250690000000001</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>2.75</v>
+        <v>5.41</v>
       </c>
       <c r="E40" t="n">
-        <v>2449495979</v>
+        <v>2741216455</v>
       </c>
       <c r="F40" t="n">
-        <v>36056375</v>
+        <v>109682438</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.26438</v>
+        <v>1.01905</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.068771</v>
+        <v>3.03</v>
       </c>
       <c r="E41" t="n">
-        <v>2314048921</v>
+        <v>2697684726</v>
       </c>
       <c r="F41" t="n">
-        <v>21909276</v>
+        <v>52531883</v>
       </c>
       <c r="G41" t="n">
-        <v>-0.51732</v>
+        <v>3.14664</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.10075</v>
+        <v>0.07879</v>
       </c>
       <c r="E42" t="n">
-        <v>2272704443</v>
+        <v>2654078198</v>
       </c>
       <c r="F42" t="n">
-        <v>9324132</v>
+        <v>29248572</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.80327</v>
+        <v>0.9248499999999999</v>
       </c>
     </row>
     <row r="43">
@@ -1592,21 +1592,21 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1.77</v>
+        <v>2</v>
       </c>
       <c r="E43" t="n">
-        <v>2253347963</v>
+        <v>2549867035</v>
       </c>
       <c r="F43" t="n">
-        <v>169051386</v>
+        <v>193200366</v>
       </c>
       <c r="G43" t="n">
-        <v>-1.53622</v>
+        <v>1.97692</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -1619,43 +1619,43 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.081201</v>
+        <v>0.088699</v>
       </c>
       <c r="E44" t="n">
-        <v>2150843073</v>
+        <v>2354128890</v>
       </c>
       <c r="F44" t="n">
-        <v>4892980</v>
+        <v>6519621</v>
       </c>
       <c r="G44" t="n">
-        <v>-0.50139</v>
+        <v>1.68057</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>1.5</v>
+        <v>121.47</v>
       </c>
       <c r="E45" t="n">
-        <v>2146889257</v>
+        <v>2202964980</v>
       </c>
       <c r="F45" t="n">
-        <v>22016309</v>
+        <v>79035116</v>
       </c>
       <c r="G45" t="n">
-        <v>-2.41355</v>
+        <v>1.89893</v>
       </c>
     </row>
     <row r="46">
@@ -1673,16 +1673,16 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.02826397</v>
+        <v>0.0301961</v>
       </c>
       <c r="E46" t="n">
-        <v>2053224914</v>
+        <v>2196189686</v>
       </c>
       <c r="F46" t="n">
-        <v>28278693</v>
+        <v>36479329</v>
       </c>
       <c r="G46" t="n">
-        <v>-2.07937</v>
+        <v>2.37214</v>
       </c>
     </row>
     <row r="47">
@@ -1700,48 +1700,48 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.593969</v>
+        <v>0.66534</v>
       </c>
       <c r="E47" t="n">
-        <v>1880414962</v>
+        <v>2108005683</v>
       </c>
       <c r="F47" t="n">
-        <v>21628765</v>
+        <v>37928721</v>
       </c>
       <c r="G47" t="n">
-        <v>0.36955</v>
+        <v>3.48303</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>SUI</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>Sui</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>4.97</v>
+        <v>1.73</v>
       </c>
       <c r="E48" t="n">
-        <v>1869635138</v>
+        <v>2012732904</v>
       </c>
       <c r="F48" t="n">
-        <v>116083089</v>
+        <v>248170215</v>
       </c>
       <c r="G48" t="n">
-        <v>2.42232</v>
+        <v>0.7506699999999999</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -1754,43 +1754,43 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>2020.5</v>
+        <v>2029.85</v>
       </c>
       <c r="E49" t="n">
-        <v>1864293643</v>
+        <v>1872841087</v>
       </c>
       <c r="F49" t="n">
-        <v>43379023</v>
+        <v>47817925</v>
       </c>
       <c r="G49" t="n">
-        <v>0.75641</v>
+        <v>2.23151</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SUI</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Sui</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>1.51</v>
+        <v>4.71</v>
       </c>
       <c r="E50" t="n">
-        <v>1759208928</v>
+        <v>1772528355</v>
       </c>
       <c r="F50" t="n">
-        <v>263661177</v>
+        <v>74260857</v>
       </c>
       <c r="G50" t="n">
-        <v>7.42558</v>
+        <v>1.90401</v>
       </c>
     </row>
     <row r="51">
@@ -1808,16 +1808,16 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.619074</v>
+        <v>0.690954</v>
       </c>
       <c r="E51" t="n">
-        <v>1499436273</v>
+        <v>1675176226</v>
       </c>
       <c r="F51" t="n">
-        <v>100420024</v>
+        <v>110078019</v>
       </c>
       <c r="G51" t="n">
-        <v>1.4926</v>
+        <v>0.88615</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-02-18
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>48461</v>
+        <v>51872</v>
       </c>
       <c r="E2" t="n">
-        <v>951190896285</v>
+        <v>1017998543299</v>
       </c>
       <c r="F2" t="n">
-        <v>19786255673</v>
+        <v>21205363662</v>
       </c>
       <c r="G2" t="n">
-        <v>2.52235</v>
+        <v>0.35419</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2531</v>
+        <v>2809.62</v>
       </c>
       <c r="E3" t="n">
-        <v>304242038355</v>
+        <v>337413977458</v>
       </c>
       <c r="F3" t="n">
-        <v>7617326047</v>
+        <v>19945797889</v>
       </c>
       <c r="G3" t="n">
-        <v>1.61553</v>
+        <v>0.9633699999999999</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1.001</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>96454290308</v>
+        <v>97705040238</v>
       </c>
       <c r="F4" t="n">
-        <v>26084958286</v>
+        <v>43428728969</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.01342</v>
+        <v>0.03638</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>322.92</v>
+        <v>354.9</v>
       </c>
       <c r="E5" t="n">
-        <v>49701832805</v>
+        <v>54576196035</v>
       </c>
       <c r="F5" t="n">
-        <v>476923714</v>
+        <v>1037820454</v>
       </c>
       <c r="G5" t="n">
-        <v>0.56041</v>
+        <v>-1.14481</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>110.18</v>
+        <v>111.98</v>
       </c>
       <c r="E6" t="n">
-        <v>48126993126</v>
+        <v>49348754862</v>
       </c>
       <c r="F6" t="n">
-        <v>1469933219</v>
+        <v>1608657980</v>
       </c>
       <c r="G6" t="n">
-        <v>2.01941</v>
+        <v>2.39227</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.533124</v>
+        <v>0.558534</v>
       </c>
       <c r="E7" t="n">
-        <v>29068901850</v>
+        <v>30475429761</v>
       </c>
       <c r="F7" t="n">
-        <v>620579571</v>
+        <v>1138165010</v>
       </c>
       <c r="G7" t="n">
-        <v>2.16463</v>
+        <v>0.91177</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>1.001</v>
       </c>
       <c r="E8" t="n">
-        <v>27968836234</v>
+        <v>28109207081</v>
       </c>
       <c r="F8" t="n">
-        <v>4219827484</v>
+        <v>4437214552</v>
       </c>
       <c r="G8" t="n">
-        <v>0.01127</v>
+        <v>0.13931</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2530.06</v>
+        <v>2806.63</v>
       </c>
       <c r="E9" t="n">
-        <v>24350888654</v>
+        <v>27450979155</v>
       </c>
       <c r="F9" t="n">
-        <v>10464147</v>
+        <v>7579947</v>
       </c>
       <c r="G9" t="n">
-        <v>1.72665</v>
+        <v>0.97972</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.552951</v>
+        <v>0.6345190000000001</v>
       </c>
       <c r="E10" t="n">
-        <v>19426771679</v>
+        <v>22318054875</v>
       </c>
       <c r="F10" t="n">
-        <v>517437611</v>
+        <v>686428302</v>
       </c>
       <c r="G10" t="n">
-        <v>3.43052</v>
+        <v>8.289239999999999</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>40.62</v>
+        <v>40.42</v>
       </c>
       <c r="E11" t="n">
-        <v>14911805042</v>
+        <v>14832671767</v>
       </c>
       <c r="F11" t="n">
-        <v>643057134</v>
+        <v>497055411</v>
       </c>
       <c r="G11" t="n">
-        <v>5.10293</v>
+        <v>1.75858</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +746,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>DOGE</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Dogecoin</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>20.47</v>
+        <v>0.08404300000000001</v>
       </c>
       <c r="E12" t="n">
-        <v>12022656082</v>
+        <v>12037681282</v>
       </c>
       <c r="F12" t="n">
-        <v>921624967</v>
+        <v>331455934</v>
       </c>
       <c r="G12" t="n">
-        <v>12.23084</v>
+        <v>-0.56474</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>DOGE</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Dogecoin</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.082359</v>
+        <v>0.13545</v>
       </c>
       <c r="E13" t="n">
-        <v>11780265319</v>
+        <v>11925909458</v>
       </c>
       <c r="F13" t="n">
-        <v>330291370</v>
+        <v>436704782</v>
       </c>
       <c r="G13" t="n">
-        <v>1.79812</v>
+        <v>-2.11869</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.1248</v>
+        <v>20.08</v>
       </c>
       <c r="E14" t="n">
-        <v>10994834803</v>
+        <v>11778615412</v>
       </c>
       <c r="F14" t="n">
-        <v>199427326</v>
+        <v>480891566</v>
       </c>
       <c r="G14" t="n">
-        <v>1.15001</v>
+        <v>2.10767</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>7.3</v>
+        <v>7.78</v>
       </c>
       <c r="E15" t="n">
-        <v>9698771289</v>
+        <v>10364588487</v>
       </c>
       <c r="F15" t="n">
-        <v>167873726</v>
+        <v>225924736</v>
       </c>
       <c r="G15" t="n">
-        <v>2.46307</v>
+        <v>2.33205</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.856474</v>
+        <v>0.947923</v>
       </c>
       <c r="E16" t="n">
-        <v>7951193099</v>
+        <v>8797705421</v>
       </c>
       <c r="F16" t="n">
-        <v>261032112</v>
+        <v>408236220</v>
       </c>
       <c r="G16" t="n">
-        <v>1.25351</v>
+        <v>1.87194</v>
       </c>
     </row>
     <row r="17">
@@ -890,16 +890,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>48277</v>
+        <v>51813</v>
       </c>
       <c r="E17" t="n">
-        <v>7620494088</v>
+        <v>8126466520</v>
       </c>
       <c r="F17" t="n">
-        <v>208042778</v>
+        <v>114251529</v>
       </c>
       <c r="G17" t="n">
-        <v>2.26768</v>
+        <v>0.3653</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>2.12</v>
+        <v>2.25</v>
       </c>
       <c r="E18" t="n">
-        <v>7331859545</v>
+        <v>7806563017</v>
       </c>
       <c r="F18" t="n">
-        <v>15461018</v>
+        <v>19313971</v>
       </c>
       <c r="G18" t="n">
-        <v>2.31448</v>
+        <v>2.98088</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>13.48</v>
+        <v>13.72</v>
       </c>
       <c r="E19" t="n">
-        <v>6181614896</v>
+        <v>6296033599</v>
       </c>
       <c r="F19" t="n">
-        <v>112206421</v>
+        <v>107697648</v>
       </c>
       <c r="G19" t="n">
-        <v>5.70007</v>
+        <v>3.74993</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>9.500000000000001e-06</v>
+        <v>7.67</v>
       </c>
       <c r="E20" t="n">
-        <v>5599871555</v>
+        <v>5789890433</v>
       </c>
       <c r="F20" t="n">
-        <v>111815428</v>
+        <v>176176979</v>
       </c>
       <c r="G20" t="n">
-        <v>1.89579</v>
+        <v>0.93396</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>71.98999999999999</v>
+        <v>9.77e-06</v>
       </c>
       <c r="E21" t="n">
-        <v>5343077689</v>
+        <v>5759077663</v>
       </c>
       <c r="F21" t="n">
-        <v>286191676</v>
+        <v>155364832</v>
       </c>
       <c r="G21" t="n">
-        <v>2.25266</v>
+        <v>0.9297299999999999</v>
       </c>
     </row>
     <row r="22">
@@ -1025,16 +1025,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>266.82</v>
+        <v>267.59</v>
       </c>
       <c r="E22" t="n">
-        <v>5216378852</v>
+        <v>5260435818</v>
       </c>
       <c r="F22" t="n">
-        <v>408583575</v>
+        <v>172266661</v>
       </c>
       <c r="G22" t="n">
-        <v>8.665179999999999</v>
+        <v>-0.11901</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>6.64</v>
+        <v>70.39</v>
       </c>
       <c r="E23" t="n">
-        <v>5005779821</v>
+        <v>5225289510</v>
       </c>
       <c r="F23" t="n">
-        <v>60627289</v>
+        <v>261464128</v>
       </c>
       <c r="G23" t="n">
-        <v>0.43463</v>
+        <v>0.33215</v>
       </c>
     </row>
     <row r="24">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.998206</v>
+        <v>0.999741</v>
       </c>
       <c r="E24" t="n">
-        <v>4917520805</v>
+        <v>4922832168</v>
       </c>
       <c r="F24" t="n">
-        <v>228913794</v>
+        <v>98238057</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.23665</v>
+        <v>0.01783</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>10.16</v>
+        <v>3.2</v>
       </c>
       <c r="E25" t="n">
-        <v>3900295927</v>
+        <v>4337330916</v>
       </c>
       <c r="F25" t="n">
-        <v>170728646</v>
+        <v>83119337</v>
       </c>
       <c r="G25" t="n">
-        <v>1.45881</v>
+        <v>3.3533</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>4.12</v>
+        <v>649.87</v>
       </c>
       <c r="E26" t="n">
-        <v>3818813705</v>
+        <v>4059177904</v>
       </c>
       <c r="F26" t="n">
-        <v>1437211</v>
+        <v>21971147</v>
       </c>
       <c r="G26" t="n">
-        <v>0.43726</v>
+        <v>1.85878</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>26.08</v>
+        <v>10.39</v>
       </c>
       <c r="E27" t="n">
-        <v>3735683370</v>
+        <v>3990499729</v>
       </c>
       <c r="F27" t="n">
-        <v>130285848</v>
+        <v>176653450</v>
       </c>
       <c r="G27" t="n">
-        <v>1.49157</v>
+        <v>2.12098</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>2.7</v>
+        <v>4.15</v>
       </c>
       <c r="E28" t="n">
-        <v>3658965022</v>
+        <v>3849487386</v>
       </c>
       <c r="F28" t="n">
-        <v>148822987</v>
+        <v>1119726</v>
       </c>
       <c r="G28" t="n">
-        <v>-1.18029</v>
+        <v>0.46465</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>569.52</v>
+        <v>26.24</v>
       </c>
       <c r="E29" t="n">
-        <v>3554949878</v>
+        <v>3756910136</v>
       </c>
       <c r="F29" t="n">
-        <v>41851065</v>
+        <v>139489865</v>
       </c>
       <c r="G29" t="n">
-        <v>3.33664</v>
+        <v>-0.4089</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>3.63</v>
+        <v>0.162431</v>
       </c>
       <c r="E30" t="n">
-        <v>3476114169</v>
+        <v>3694535422</v>
       </c>
       <c r="F30" t="n">
-        <v>172037473</v>
+        <v>72986537</v>
       </c>
       <c r="G30" t="n">
-        <v>7.54606</v>
+        <v>-3.29102</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>3.16</v>
+        <v>2.51</v>
       </c>
       <c r="E31" t="n">
-        <v>3275480918</v>
+        <v>3611508463</v>
       </c>
       <c r="F31" t="n">
-        <v>190974110</v>
+        <v>95586507</v>
       </c>
       <c r="G31" t="n">
-        <v>5.03088</v>
+        <v>0.13227</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.144584</v>
+        <v>3.72</v>
       </c>
       <c r="E32" t="n">
-        <v>3275414704</v>
+        <v>3564175754</v>
       </c>
       <c r="F32" t="n">
-        <v>50508351</v>
+        <v>139695477</v>
       </c>
       <c r="G32" t="n">
-        <v>6.14877</v>
+        <v>4.19683</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>TIA</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Celestia</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>19.75</v>
+        <v>3.43</v>
       </c>
       <c r="E33" t="n">
-        <v>3236508845</v>
+        <v>3564001921</v>
       </c>
       <c r="F33" t="n">
-        <v>152970097</v>
+        <v>246251948</v>
       </c>
       <c r="G33" t="n">
-        <v>-2.39467</v>
+        <v>5.28741</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.112147</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="E34" t="n">
-        <v>3186080446</v>
+        <v>3541783848</v>
       </c>
       <c r="F34" t="n">
-        <v>53067855</v>
+        <v>114642775</v>
       </c>
       <c r="G34" t="n">
-        <v>0.7483300000000001</v>
+        <v>1.96908</v>
       </c>
     </row>
     <row r="35">
@@ -1376,16 +1376,16 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>35.8</v>
+        <v>38.95</v>
       </c>
       <c r="E35" t="n">
-        <v>3168916238</v>
+        <v>3441400584</v>
       </c>
       <c r="F35" t="n">
-        <v>156211623</v>
+        <v>381088555</v>
       </c>
       <c r="G35" t="n">
-        <v>4.13752</v>
+        <v>10.27923</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>9.18</v>
+        <v>0.115572</v>
       </c>
       <c r="E36" t="n">
-        <v>3117772396</v>
+        <v>3288692189</v>
       </c>
       <c r="F36" t="n">
-        <v>78437410</v>
+        <v>58416506</v>
       </c>
       <c r="G36" t="n">
-        <v>0.92775</v>
+        <v>1.26964</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>49.75</v>
+        <v>0.04450379</v>
       </c>
       <c r="E37" t="n">
-        <v>2985974343</v>
+        <v>3236308669</v>
       </c>
       <c r="F37" t="n">
-        <v>5012442</v>
+        <v>125530597</v>
       </c>
       <c r="G37" t="n">
-        <v>0.37987</v>
+        <v>0.28737</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>FDUSD</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>First Digital USD</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1.005</v>
+        <v>6.17</v>
       </c>
       <c r="E38" t="n">
-        <v>2773842649</v>
+        <v>3151154403</v>
       </c>
       <c r="F38" t="n">
-        <v>3970353114</v>
+        <v>401962791</v>
       </c>
       <c r="G38" t="n">
-        <v>-0.01832</v>
+        <v>-0.60083</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1.91</v>
+        <v>52.42</v>
       </c>
       <c r="E39" t="n">
-        <v>2746462690</v>
+        <v>3144932303</v>
       </c>
       <c r="F39" t="n">
-        <v>81281031</v>
+        <v>7777653</v>
       </c>
       <c r="G39" t="n">
-        <v>8.250690000000001</v>
+        <v>0.99581</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>TIA</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Celestia</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>5.41</v>
+        <v>19.05</v>
       </c>
       <c r="E40" t="n">
-        <v>2741216455</v>
+        <v>3143063039</v>
       </c>
       <c r="F40" t="n">
-        <v>109682438</v>
+        <v>125066530</v>
       </c>
       <c r="G40" t="n">
-        <v>1.01905</v>
+        <v>1.74615</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>3.03</v>
+        <v>0.088579</v>
       </c>
       <c r="E41" t="n">
-        <v>2697684726</v>
+        <v>2978859523</v>
       </c>
       <c r="F41" t="n">
-        <v>52531883</v>
+        <v>60830520</v>
       </c>
       <c r="G41" t="n">
-        <v>3.14664</v>
+        <v>5.73682</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>FDUSD</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>First Digital USD</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.07879</v>
+        <v>0.999685</v>
       </c>
       <c r="E42" t="n">
-        <v>2654078198</v>
+        <v>2843180700</v>
       </c>
       <c r="F42" t="n">
-        <v>29248572</v>
+        <v>4052622152</v>
       </c>
       <c r="G42" t="n">
-        <v>0.9248499999999999</v>
+        <v>-0.03238</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>2</v>
+        <v>3.17</v>
       </c>
       <c r="E43" t="n">
-        <v>2549867035</v>
+        <v>2825234309</v>
       </c>
       <c r="F43" t="n">
-        <v>193200366</v>
+        <v>53234698</v>
       </c>
       <c r="G43" t="n">
-        <v>1.97692</v>
+        <v>1.26788</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.088699</v>
+        <v>2.01</v>
       </c>
       <c r="E44" t="n">
-        <v>2354128890</v>
+        <v>2561284754</v>
       </c>
       <c r="F44" t="n">
-        <v>6519621</v>
+        <v>231356886</v>
       </c>
       <c r="G44" t="n">
-        <v>1.68057</v>
+        <v>3.0207</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>121.47</v>
+        <v>0.777794</v>
       </c>
       <c r="E45" t="n">
-        <v>2202964980</v>
+        <v>2505281240</v>
       </c>
       <c r="F45" t="n">
-        <v>79035116</v>
+        <v>80332201</v>
       </c>
       <c r="G45" t="n">
-        <v>1.89893</v>
+        <v>2.92821</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>SEI</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Sei</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.0301961</v>
+        <v>0.963441</v>
       </c>
       <c r="E46" t="n">
-        <v>2196189686</v>
+        <v>2454237009</v>
       </c>
       <c r="F46" t="n">
-        <v>36479329</v>
+        <v>235534622</v>
       </c>
       <c r="G46" t="n">
-        <v>2.37214</v>
+        <v>2.15667</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.66534</v>
+        <v>0.090457</v>
       </c>
       <c r="E47" t="n">
-        <v>2108005683</v>
+        <v>2400524220</v>
       </c>
       <c r="F47" t="n">
-        <v>37928721</v>
+        <v>8120980</v>
       </c>
       <c r="G47" t="n">
-        <v>3.48303</v>
+        <v>0.8381999999999999</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>SUI</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Sui</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>1.73</v>
+        <v>120.64</v>
       </c>
       <c r="E48" t="n">
-        <v>2012732904</v>
+        <v>2189011678</v>
       </c>
       <c r="F48" t="n">
-        <v>248170215</v>
+        <v>52566955</v>
       </c>
       <c r="G48" t="n">
-        <v>0.7506699999999999</v>
+        <v>0.77472</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>2029.85</v>
+        <v>5.63</v>
       </c>
       <c r="E49" t="n">
-        <v>1872841087</v>
+        <v>2130294996</v>
       </c>
       <c r="F49" t="n">
-        <v>47817925</v>
+        <v>230671351</v>
       </c>
       <c r="G49" t="n">
-        <v>2.23151</v>
+        <v>7.41635</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>SUI</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>Sui</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>4.71</v>
+        <v>1.79</v>
       </c>
       <c r="E50" t="n">
-        <v>1772528355</v>
+        <v>2085640983</v>
       </c>
       <c r="F50" t="n">
-        <v>74260857</v>
+        <v>209089080</v>
       </c>
       <c r="G50" t="n">
-        <v>1.90401</v>
+        <v>1.93564</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>SEI</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Sei</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.690954</v>
+        <v>0.217561</v>
       </c>
       <c r="E51" t="n">
-        <v>1675176226</v>
+        <v>2048881958</v>
       </c>
       <c r="F51" t="n">
-        <v>110078019</v>
+        <v>257755273</v>
       </c>
       <c r="G51" t="n">
-        <v>0.88615</v>
+        <v>15.73712</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-02-25
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>51872</v>
+        <v>51606</v>
       </c>
       <c r="E2" t="n">
-        <v>1017998543299</v>
+        <v>1013862656276</v>
       </c>
       <c r="F2" t="n">
-        <v>21205363662</v>
+        <v>14670160193</v>
       </c>
       <c r="G2" t="n">
-        <v>0.35419</v>
+        <v>1.0705</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2809.62</v>
+        <v>3032.71</v>
       </c>
       <c r="E3" t="n">
-        <v>337413977458</v>
+        <v>364756261463</v>
       </c>
       <c r="F3" t="n">
-        <v>19945797889</v>
+        <v>13335510805</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9633699999999999</v>
+        <v>2.53296</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0.999706</v>
       </c>
       <c r="E4" t="n">
-        <v>97705040238</v>
+        <v>97914782829</v>
       </c>
       <c r="F4" t="n">
-        <v>43428728969</v>
+        <v>28324859926</v>
       </c>
       <c r="G4" t="n">
-        <v>0.03638</v>
+        <v>0.00603</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>354.9</v>
+        <v>384.85</v>
       </c>
       <c r="E5" t="n">
-        <v>54576196035</v>
+        <v>59145736339</v>
       </c>
       <c r="F5" t="n">
-        <v>1037820454</v>
+        <v>884386510</v>
       </c>
       <c r="G5" t="n">
-        <v>-1.14481</v>
+        <v>1.21684</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>111.98</v>
+        <v>102.46</v>
       </c>
       <c r="E6" t="n">
-        <v>49348754862</v>
+        <v>45211377309</v>
       </c>
       <c r="F6" t="n">
-        <v>1608657980</v>
+        <v>1238311669</v>
       </c>
       <c r="G6" t="n">
-        <v>2.39227</v>
+        <v>0.60151</v>
       </c>
     </row>
     <row r="7">
@@ -611,25 +611,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>STETH</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>Lido Staked Ether</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.558534</v>
+        <v>3028.7</v>
       </c>
       <c r="E7" t="n">
-        <v>30475429761</v>
+        <v>29707833002</v>
       </c>
       <c r="F7" t="n">
-        <v>1138165010</v>
+        <v>22570638</v>
       </c>
       <c r="G7" t="n">
-        <v>0.91177</v>
+        <v>2.45679</v>
       </c>
     </row>
     <row r="8">
@@ -638,25 +638,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>USDC</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>USDC</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1.001</v>
+        <v>0.543999</v>
       </c>
       <c r="E8" t="n">
-        <v>28109207081</v>
+        <v>29706154673</v>
       </c>
       <c r="F8" t="n">
-        <v>4437214552</v>
+        <v>589557514</v>
       </c>
       <c r="G8" t="n">
-        <v>0.13931</v>
+        <v>0.00053</v>
       </c>
     </row>
     <row r="9">
@@ -665,25 +665,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>STETH</t>
+          <t>USDC</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Lido Staked Ether</t>
+          <t>USDC</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2806.63</v>
+        <v>0.999576</v>
       </c>
       <c r="E9" t="n">
-        <v>27450979155</v>
+        <v>28171147681</v>
       </c>
       <c r="F9" t="n">
-        <v>7579947</v>
+        <v>3426957762</v>
       </c>
       <c r="G9" t="n">
-        <v>0.97972</v>
+        <v>-0.00023</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.6345190000000001</v>
+        <v>0.588214</v>
       </c>
       <c r="E10" t="n">
-        <v>22318054875</v>
+        <v>20690555656</v>
       </c>
       <c r="F10" t="n">
-        <v>686428302</v>
+        <v>327602582</v>
       </c>
       <c r="G10" t="n">
-        <v>8.289239999999999</v>
+        <v>0.45942</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>40.42</v>
+        <v>36.74</v>
       </c>
       <c r="E11" t="n">
-        <v>14832671767</v>
+        <v>13862644871</v>
       </c>
       <c r="F11" t="n">
-        <v>497055411</v>
+        <v>360139432</v>
       </c>
       <c r="G11" t="n">
-        <v>1.75858</v>
+        <v>0.34379</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.08404300000000001</v>
+        <v>0.08595800000000001</v>
       </c>
       <c r="E12" t="n">
-        <v>12037681282</v>
+        <v>12311390346</v>
       </c>
       <c r="F12" t="n">
-        <v>331455934</v>
+        <v>338438917</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.56474</v>
+        <v>0.56513</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.13545</v>
+        <v>0.13742</v>
       </c>
       <c r="E13" t="n">
-        <v>11925909458</v>
+        <v>12099108728</v>
       </c>
       <c r="F13" t="n">
-        <v>436704782</v>
+        <v>228916962</v>
       </c>
       <c r="G13" t="n">
-        <v>-2.11869</v>
+        <v>0.00655</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>20.08</v>
+        <v>18.6</v>
       </c>
       <c r="E14" t="n">
-        <v>11778615412</v>
+        <v>10907148471</v>
       </c>
       <c r="F14" t="n">
-        <v>480891566</v>
+        <v>273892365</v>
       </c>
       <c r="G14" t="n">
-        <v>2.10767</v>
+        <v>1.57551</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>7.78</v>
+        <v>7.75</v>
       </c>
       <c r="E15" t="n">
-        <v>10364588487</v>
+        <v>10348260060</v>
       </c>
       <c r="F15" t="n">
-        <v>225924736</v>
+        <v>183620894</v>
       </c>
       <c r="G15" t="n">
-        <v>2.33205</v>
+        <v>0.05972</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.947923</v>
+        <v>0.973957</v>
       </c>
       <c r="E16" t="n">
-        <v>8797705421</v>
+        <v>9046271197</v>
       </c>
       <c r="F16" t="n">
-        <v>408236220</v>
+        <v>382779312</v>
       </c>
       <c r="G16" t="n">
-        <v>1.87194</v>
+        <v>-2.91932</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>51813</v>
+        <v>10.77</v>
       </c>
       <c r="E17" t="n">
-        <v>8126466520</v>
+        <v>8122875419</v>
       </c>
       <c r="F17" t="n">
-        <v>114251529</v>
+        <v>983919242</v>
       </c>
       <c r="G17" t="n">
-        <v>0.3653</v>
+        <v>-11.64245</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>2.25</v>
+        <v>51610</v>
       </c>
       <c r="E18" t="n">
-        <v>7806563017</v>
+        <v>8099961537</v>
       </c>
       <c r="F18" t="n">
-        <v>19313971</v>
+        <v>216902327</v>
       </c>
       <c r="G18" t="n">
-        <v>2.98088</v>
+        <v>1.14176</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>13.72</v>
+        <v>2.11</v>
       </c>
       <c r="E19" t="n">
-        <v>6296033599</v>
+        <v>7320952881</v>
       </c>
       <c r="F19" t="n">
-        <v>107697648</v>
+        <v>18403467</v>
       </c>
       <c r="G19" t="n">
-        <v>3.74993</v>
+        <v>-0.96721</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>7.67</v>
+        <v>12.43</v>
       </c>
       <c r="E20" t="n">
-        <v>5789890433</v>
+        <v>5721594427</v>
       </c>
       <c r="F20" t="n">
-        <v>176176979</v>
+        <v>92311249</v>
       </c>
       <c r="G20" t="n">
-        <v>0.93396</v>
+        <v>0.56468</v>
       </c>
     </row>
     <row r="21">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>9.77e-06</v>
+        <v>9.609999999999999e-06</v>
       </c>
       <c r="E21" t="n">
-        <v>5759077663</v>
+        <v>5666839136</v>
       </c>
       <c r="F21" t="n">
-        <v>155364832</v>
+        <v>113235736</v>
       </c>
       <c r="G21" t="n">
-        <v>0.9297299999999999</v>
+        <v>0.10224</v>
       </c>
     </row>
     <row r="22">
@@ -1025,16 +1025,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>267.59</v>
+        <v>266.96</v>
       </c>
       <c r="E22" t="n">
-        <v>5260435818</v>
+        <v>5248773175</v>
       </c>
       <c r="F22" t="n">
-        <v>172266661</v>
+        <v>110840520</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.11901</v>
+        <v>-0.37352</v>
       </c>
     </row>
     <row r="23">
@@ -1052,16 +1052,16 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>70.39</v>
+        <v>70</v>
       </c>
       <c r="E23" t="n">
-        <v>5225289510</v>
+        <v>5198847894</v>
       </c>
       <c r="F23" t="n">
-        <v>261464128</v>
+        <v>226573834</v>
       </c>
       <c r="G23" t="n">
-        <v>0.33215</v>
+        <v>0.3166</v>
       </c>
     </row>
     <row r="24">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.999741</v>
+        <v>0.999018</v>
       </c>
       <c r="E24" t="n">
-        <v>4922832168</v>
+        <v>4950163204</v>
       </c>
       <c r="F24" t="n">
-        <v>98238057</v>
+        <v>111253911</v>
       </c>
       <c r="G24" t="n">
-        <v>0.01783</v>
+        <v>0.07504</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>3.2</v>
+        <v>8.33</v>
       </c>
       <c r="E25" t="n">
-        <v>4337330916</v>
+        <v>4288440075</v>
       </c>
       <c r="F25" t="n">
-        <v>83119337</v>
+        <v>449313043</v>
       </c>
       <c r="G25" t="n">
-        <v>3.3533</v>
+        <v>5.22185</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>649.87</v>
+        <v>3.08</v>
       </c>
       <c r="E26" t="n">
-        <v>4059177904</v>
+        <v>4273190716</v>
       </c>
       <c r="F26" t="n">
-        <v>21971147</v>
+        <v>77724632</v>
       </c>
       <c r="G26" t="n">
-        <v>1.85878</v>
+        <v>-0.33811</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>10.39</v>
+        <v>10.28</v>
       </c>
       <c r="E27" t="n">
-        <v>3990499729</v>
+        <v>3989900673</v>
       </c>
       <c r="F27" t="n">
-        <v>176653450</v>
+        <v>175946664</v>
       </c>
       <c r="G27" t="n">
-        <v>2.12098</v>
+        <v>-1.24392</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>4.15</v>
+        <v>0.172915</v>
       </c>
       <c r="E28" t="n">
-        <v>3849487386</v>
+        <v>3931144496</v>
       </c>
       <c r="F28" t="n">
-        <v>1119726</v>
+        <v>33538391</v>
       </c>
       <c r="G28" t="n">
-        <v>0.46465</v>
+        <v>3.85354</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>26.24</v>
+        <v>4.21</v>
       </c>
       <c r="E29" t="n">
-        <v>3756910136</v>
+        <v>3912524924</v>
       </c>
       <c r="F29" t="n">
-        <v>139489865</v>
+        <v>1309497</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.4089</v>
+        <v>2.07278</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.162431</v>
+        <v>3.69</v>
       </c>
       <c r="E30" t="n">
-        <v>3694535422</v>
+        <v>3840784957</v>
       </c>
       <c r="F30" t="n">
-        <v>72986537</v>
+        <v>414525034</v>
       </c>
       <c r="G30" t="n">
-        <v>-3.29102</v>
+        <v>4.54301</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>2.51</v>
+        <v>26.25</v>
       </c>
       <c r="E31" t="n">
-        <v>3611508463</v>
+        <v>3762486384</v>
       </c>
       <c r="F31" t="n">
-        <v>95586507</v>
+        <v>110216642</v>
       </c>
       <c r="G31" t="n">
-        <v>0.13227</v>
+        <v>1.68368</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>3.72</v>
+        <v>579.75</v>
       </c>
       <c r="E32" t="n">
-        <v>3564175754</v>
+        <v>3659611425</v>
       </c>
       <c r="F32" t="n">
-        <v>139695477</v>
+        <v>14266389</v>
       </c>
       <c r="G32" t="n">
-        <v>4.19683</v>
+        <v>-2.55087</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>3.43</v>
+        <v>2.53</v>
       </c>
       <c r="E33" t="n">
-        <v>3564001921</v>
+        <v>3654601547</v>
       </c>
       <c r="F33" t="n">
-        <v>246251948</v>
+        <v>70388012</v>
       </c>
       <c r="G33" t="n">
-        <v>5.28741</v>
+        <v>2.27114</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>9.699999999999999</v>
+        <v>0.107599</v>
       </c>
       <c r="E34" t="n">
-        <v>3541783848</v>
+        <v>3625964033</v>
       </c>
       <c r="F34" t="n">
-        <v>114642775</v>
+        <v>82402468</v>
       </c>
       <c r="G34" t="n">
-        <v>1.96908</v>
+        <v>-1.07704</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>38.95</v>
+        <v>3.7</v>
       </c>
       <c r="E35" t="n">
-        <v>3441400584</v>
+        <v>3545709931</v>
       </c>
       <c r="F35" t="n">
-        <v>381088555</v>
+        <v>164549621</v>
       </c>
       <c r="G35" t="n">
-        <v>10.27923</v>
+        <v>2.96799</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.115572</v>
+        <v>9.539999999999999</v>
       </c>
       <c r="E36" t="n">
-        <v>3288692189</v>
+        <v>3492554059</v>
       </c>
       <c r="F36" t="n">
-        <v>58416506</v>
+        <v>81133865</v>
       </c>
       <c r="G36" t="n">
-        <v>1.26964</v>
+        <v>1.77096</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.04450379</v>
+        <v>0.116357</v>
       </c>
       <c r="E37" t="n">
-        <v>3236308669</v>
+        <v>3312669107</v>
       </c>
       <c r="F37" t="n">
-        <v>125530597</v>
+        <v>57358930</v>
       </c>
       <c r="G37" t="n">
-        <v>0.28737</v>
+        <v>-0.08545999999999999</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>FDUSD</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>First Digital USD</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>6.17</v>
+        <v>0.99766</v>
       </c>
       <c r="E38" t="n">
-        <v>3151154403</v>
+        <v>3301453412</v>
       </c>
       <c r="F38" t="n">
-        <v>401962791</v>
+        <v>3016475587</v>
       </c>
       <c r="G38" t="n">
-        <v>-0.60083</v>
+        <v>-0.35747</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>52.42</v>
+        <v>0.04457198</v>
       </c>
       <c r="E39" t="n">
-        <v>3144932303</v>
+        <v>3242400882</v>
       </c>
       <c r="F39" t="n">
-        <v>7777653</v>
+        <v>78603193</v>
       </c>
       <c r="G39" t="n">
-        <v>0.99581</v>
+        <v>2.56178</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>TIA</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Celestia</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>19.05</v>
+        <v>50.5</v>
       </c>
       <c r="E40" t="n">
-        <v>3143063039</v>
+        <v>3030010080</v>
       </c>
       <c r="F40" t="n">
-        <v>125066530</v>
+        <v>5659343</v>
       </c>
       <c r="G40" t="n">
-        <v>1.74615</v>
+        <v>-0.94948</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.088579</v>
+        <v>33.95</v>
       </c>
       <c r="E41" t="n">
-        <v>2978859523</v>
+        <v>3006829319</v>
       </c>
       <c r="F41" t="n">
-        <v>60830520</v>
+        <v>84559425</v>
       </c>
       <c r="G41" t="n">
-        <v>5.73682</v>
+        <v>-0.94517</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>FDUSD</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>First Digital USD</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.999685</v>
+        <v>3.33</v>
       </c>
       <c r="E42" t="n">
-        <v>2843180700</v>
+        <v>2967465062</v>
       </c>
       <c r="F42" t="n">
-        <v>4052622152</v>
+        <v>89985202</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.03238</v>
+        <v>1.47877</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>TIA</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Celestia</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>3.17</v>
+        <v>17.01</v>
       </c>
       <c r="E43" t="n">
-        <v>2825234309</v>
+        <v>2836340436</v>
       </c>
       <c r="F43" t="n">
-        <v>53234698</v>
+        <v>75099982</v>
       </c>
       <c r="G43" t="n">
-        <v>1.26788</v>
+        <v>2.59609</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>2.01</v>
+        <v>7.47</v>
       </c>
       <c r="E44" t="n">
-        <v>2561284754</v>
+        <v>2823864116</v>
       </c>
       <c r="F44" t="n">
-        <v>231356886</v>
+        <v>262530083</v>
       </c>
       <c r="G44" t="n">
-        <v>3.0207</v>
+        <v>4.86404</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.777794</v>
+        <v>0.292679</v>
       </c>
       <c r="E45" t="n">
-        <v>2505281240</v>
+        <v>2737733373</v>
       </c>
       <c r="F45" t="n">
-        <v>80332201</v>
+        <v>344194202</v>
       </c>
       <c r="G45" t="n">
-        <v>2.92821</v>
+        <v>9.846679999999999</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>SEI</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Sei</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.963441</v>
+        <v>0.797198</v>
       </c>
       <c r="E46" t="n">
-        <v>2454237009</v>
+        <v>2573420780</v>
       </c>
       <c r="F46" t="n">
-        <v>235534622</v>
+        <v>64695810</v>
       </c>
       <c r="G46" t="n">
-        <v>2.15667</v>
+        <v>2.81095</v>
       </c>
     </row>
     <row r="47">
@@ -1700,16 +1700,16 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.090457</v>
+        <v>0.093056</v>
       </c>
       <c r="E47" t="n">
-        <v>2400524220</v>
+        <v>2474964102</v>
       </c>
       <c r="F47" t="n">
-        <v>8120980</v>
+        <v>9614166</v>
       </c>
       <c r="G47" t="n">
-        <v>0.8381999999999999</v>
+        <v>-1.20863</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>120.64</v>
+        <v>1.87</v>
       </c>
       <c r="E48" t="n">
-        <v>2189011678</v>
+        <v>2380126193</v>
       </c>
       <c r="F48" t="n">
-        <v>52566955</v>
+        <v>239833081</v>
       </c>
       <c r="G48" t="n">
-        <v>0.77472</v>
+        <v>1.65933</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>5.63</v>
+        <v>123.94</v>
       </c>
       <c r="E49" t="n">
-        <v>2130294996</v>
+        <v>2250704723</v>
       </c>
       <c r="F49" t="n">
-        <v>230671351</v>
+        <v>33317637</v>
       </c>
       <c r="G49" t="n">
-        <v>7.41635</v>
+        <v>-0.91814</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SUI</t>
+          <t>SEI</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Sui</t>
+          <t>Sei</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>1.79</v>
+        <v>0.829756</v>
       </c>
       <c r="E50" t="n">
-        <v>2085640983</v>
+        <v>2117336370</v>
       </c>
       <c r="F50" t="n">
-        <v>209089080</v>
+        <v>169098247</v>
       </c>
       <c r="G50" t="n">
-        <v>1.93564</v>
+        <v>1.99686</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>SUI</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Sui</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.217561</v>
+        <v>1.64</v>
       </c>
       <c r="E51" t="n">
-        <v>2048881958</v>
+        <v>1906957337</v>
       </c>
       <c r="F51" t="n">
-        <v>257755273</v>
+        <v>155310833</v>
       </c>
       <c r="G51" t="n">
-        <v>15.73712</v>
+        <v>1.50402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-03-03
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>51606</v>
+        <v>62480</v>
       </c>
       <c r="E2" t="n">
-        <v>1013862656276</v>
+        <v>1224975413389</v>
       </c>
       <c r="F2" t="n">
-        <v>14670160193</v>
+        <v>19244343459</v>
       </c>
       <c r="G2" t="n">
-        <v>1.0705</v>
+        <v>0.60659</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3032.71</v>
+        <v>3449.34</v>
       </c>
       <c r="E3" t="n">
-        <v>364756261463</v>
+        <v>413682749278</v>
       </c>
       <c r="F3" t="n">
-        <v>13335510805</v>
+        <v>12842815698</v>
       </c>
       <c r="G3" t="n">
-        <v>2.53296</v>
+        <v>0.67758</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999706</v>
+        <v>1.001</v>
       </c>
       <c r="E4" t="n">
-        <v>97914782829</v>
+        <v>99397291213</v>
       </c>
       <c r="F4" t="n">
-        <v>28324859926</v>
+        <v>45275587693</v>
       </c>
       <c r="G4" t="n">
-        <v>0.00603</v>
+        <v>-0.09734</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>384.85</v>
+        <v>415.5</v>
       </c>
       <c r="E5" t="n">
-        <v>59145736339</v>
+        <v>63916190674</v>
       </c>
       <c r="F5" t="n">
-        <v>884386510</v>
+        <v>1543994524</v>
       </c>
       <c r="G5" t="n">
-        <v>1.21684</v>
+        <v>1.08307</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>102.46</v>
+        <v>129.32</v>
       </c>
       <c r="E6" t="n">
-        <v>45211377309</v>
+        <v>57051482565</v>
       </c>
       <c r="F6" t="n">
-        <v>1238311669</v>
+        <v>3326689612</v>
       </c>
       <c r="G6" t="n">
-        <v>0.60151</v>
+        <v>-0.61344</v>
       </c>
     </row>
     <row r="7">
@@ -611,25 +611,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>STETH</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Lido Staked Ether</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3028.7</v>
+        <v>0.629507</v>
       </c>
       <c r="E7" t="n">
-        <v>29707833002</v>
+        <v>34324377864</v>
       </c>
       <c r="F7" t="n">
-        <v>22570638</v>
+        <v>2241507633</v>
       </c>
       <c r="G7" t="n">
-        <v>2.45679</v>
+        <v>-2.94615</v>
       </c>
     </row>
     <row r="8">
@@ -638,25 +638,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>STETH</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>Lido Staked Ether</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.543999</v>
+        <v>3440.57</v>
       </c>
       <c r="E8" t="n">
-        <v>29706154673</v>
+        <v>33827781061</v>
       </c>
       <c r="F8" t="n">
-        <v>589557514</v>
+        <v>26304596</v>
       </c>
       <c r="G8" t="n">
-        <v>0.00053</v>
+        <v>0.63791</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.999576</v>
+        <v>1.002</v>
       </c>
       <c r="E9" t="n">
-        <v>28171147681</v>
+        <v>28987955848</v>
       </c>
       <c r="F9" t="n">
-        <v>3426957762</v>
+        <v>5316140260</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.00023</v>
+        <v>0.05311</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.588214</v>
+        <v>0.73249</v>
       </c>
       <c r="E10" t="n">
-        <v>20690555656</v>
+        <v>25714596642</v>
       </c>
       <c r="F10" t="n">
-        <v>327602582</v>
+        <v>919826048</v>
       </c>
       <c r="G10" t="n">
-        <v>0.45942</v>
+        <v>-1.41506</v>
       </c>
     </row>
     <row r="11">
@@ -719,25 +719,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>DOGE</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Dogecoin</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>36.74</v>
+        <v>0.142432</v>
       </c>
       <c r="E11" t="n">
-        <v>13862644871</v>
+        <v>20425961864</v>
       </c>
       <c r="F11" t="n">
-        <v>360139432</v>
+        <v>3214142207</v>
       </c>
       <c r="G11" t="n">
-        <v>0.34379</v>
+        <v>-0.26243</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +746,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>DOGE</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Dogecoin</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.08595800000000001</v>
+        <v>43</v>
       </c>
       <c r="E12" t="n">
-        <v>12311390346</v>
+        <v>16196682514</v>
       </c>
       <c r="F12" t="n">
-        <v>338438917</v>
+        <v>771365366</v>
       </c>
       <c r="G12" t="n">
-        <v>0.56513</v>
+        <v>0.56389</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.13742</v>
+        <v>2.238e-05</v>
       </c>
       <c r="E13" t="n">
-        <v>12099108728</v>
+        <v>13137540052</v>
       </c>
       <c r="F13" t="n">
-        <v>228916962</v>
+        <v>4317467105</v>
       </c>
       <c r="G13" t="n">
-        <v>0.00655</v>
+        <v>1.64152</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>18.6</v>
+        <v>0.1408</v>
       </c>
       <c r="E14" t="n">
-        <v>10907148471</v>
+        <v>12357939760</v>
       </c>
       <c r="F14" t="n">
-        <v>273892365</v>
+        <v>348344607</v>
       </c>
       <c r="G14" t="n">
-        <v>1.57551</v>
+        <v>-0.10014</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>7.75</v>
+        <v>9.23</v>
       </c>
       <c r="E15" t="n">
-        <v>10348260060</v>
+        <v>12306673038</v>
       </c>
       <c r="F15" t="n">
-        <v>183620894</v>
+        <v>562809820</v>
       </c>
       <c r="G15" t="n">
-        <v>0.05972</v>
+        <v>0.92471</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.973957</v>
+        <v>20.67</v>
       </c>
       <c r="E16" t="n">
-        <v>9046271197</v>
+        <v>12133699722</v>
       </c>
       <c r="F16" t="n">
-        <v>382779312</v>
+        <v>928928176</v>
       </c>
       <c r="G16" t="n">
-        <v>-2.91932</v>
+        <v>-1.45096</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>10.77</v>
+        <v>1.084</v>
       </c>
       <c r="E17" t="n">
-        <v>8122875419</v>
+        <v>10027721620</v>
       </c>
       <c r="F17" t="n">
-        <v>983919242</v>
+        <v>1012961964</v>
       </c>
       <c r="G17" t="n">
-        <v>-11.64245</v>
+        <v>0.39357</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>51610</v>
+        <v>62419</v>
       </c>
       <c r="E18" t="n">
-        <v>8099961537</v>
+        <v>9706977671</v>
       </c>
       <c r="F18" t="n">
-        <v>216902327</v>
+        <v>133709900</v>
       </c>
       <c r="G18" t="n">
-        <v>1.14176</v>
+        <v>0.4485</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>2.11</v>
+        <v>12.82</v>
       </c>
       <c r="E19" t="n">
-        <v>7320952881</v>
+        <v>9645689666</v>
       </c>
       <c r="F19" t="n">
-        <v>18403467</v>
+        <v>504931027</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.96721</v>
+        <v>5.51719</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>12.43</v>
+        <v>484.45</v>
       </c>
       <c r="E20" t="n">
-        <v>5721594427</v>
+        <v>9553161067</v>
       </c>
       <c r="F20" t="n">
-        <v>92311249</v>
+        <v>2339333868</v>
       </c>
       <c r="G20" t="n">
-        <v>0.56468</v>
+        <v>9.14143</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>9.609999999999999e-06</v>
+        <v>2.66</v>
       </c>
       <c r="E21" t="n">
-        <v>5666839136</v>
+        <v>9189762472</v>
       </c>
       <c r="F21" t="n">
-        <v>113235736</v>
+        <v>69672311</v>
       </c>
       <c r="G21" t="n">
-        <v>0.10224</v>
+        <v>-2.9109</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>266.96</v>
+        <v>92.28</v>
       </c>
       <c r="E22" t="n">
-        <v>5248773175</v>
+        <v>6829953290</v>
       </c>
       <c r="F22" t="n">
-        <v>110840520</v>
+        <v>966291106</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.37352</v>
+        <v>1.06772</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>70</v>
+        <v>13.19</v>
       </c>
       <c r="E23" t="n">
-        <v>5198847894</v>
+        <v>6049707846</v>
       </c>
       <c r="F23" t="n">
-        <v>226573834</v>
+        <v>213881714</v>
       </c>
       <c r="G23" t="n">
-        <v>0.3166</v>
+        <v>0.38476</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.999018</v>
+        <v>9.83</v>
       </c>
       <c r="E24" t="n">
-        <v>4950163204</v>
+        <v>5090928003</v>
       </c>
       <c r="F24" t="n">
-        <v>111253911</v>
+        <v>979192099</v>
       </c>
       <c r="G24" t="n">
-        <v>0.07504</v>
+        <v>11.16078</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>8.33</v>
+        <v>1.001</v>
       </c>
       <c r="E25" t="n">
-        <v>4288440075</v>
+        <v>5016431198</v>
       </c>
       <c r="F25" t="n">
-        <v>449313043</v>
+        <v>193191310</v>
       </c>
       <c r="G25" t="n">
-        <v>5.22185</v>
+        <v>0.1595</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>3.08</v>
+        <v>33.67</v>
       </c>
       <c r="E26" t="n">
-        <v>4273190716</v>
+        <v>4811676787</v>
       </c>
       <c r="F26" t="n">
-        <v>77724632</v>
+        <v>690570406</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.33811</v>
+        <v>-0.46522</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>10.28</v>
+        <v>11.92</v>
       </c>
       <c r="E27" t="n">
-        <v>3989900673</v>
+        <v>4628753546</v>
       </c>
       <c r="F27" t="n">
-        <v>175946664</v>
+        <v>418688877</v>
       </c>
       <c r="G27" t="n">
-        <v>-1.24392</v>
+        <v>-1.32739</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.172915</v>
+        <v>3.27</v>
       </c>
       <c r="E28" t="n">
-        <v>3931144496</v>
+        <v>4543782473</v>
       </c>
       <c r="F28" t="n">
-        <v>33538391</v>
+        <v>126085880</v>
       </c>
       <c r="G28" t="n">
-        <v>3.85354</v>
+        <v>3.08205</v>
       </c>
     </row>
     <row r="29">
@@ -1214,16 +1214,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>4.21</v>
+        <v>4.78</v>
       </c>
       <c r="E29" t="n">
-        <v>3912524924</v>
+        <v>4417329208</v>
       </c>
       <c r="F29" t="n">
-        <v>1309497</v>
+        <v>2770808</v>
       </c>
       <c r="G29" t="n">
-        <v>2.07278</v>
+        <v>0.26881</v>
       </c>
     </row>
     <row r="30">
@@ -1241,16 +1241,16 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>3.69</v>
+        <v>4.27</v>
       </c>
       <c r="E30" t="n">
-        <v>3840784957</v>
+        <v>4413845986</v>
       </c>
       <c r="F30" t="n">
-        <v>414525034</v>
+        <v>480707549</v>
       </c>
       <c r="G30" t="n">
-        <v>4.54301</v>
+        <v>2.3376</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>26.25</v>
+        <v>3.06</v>
       </c>
       <c r="E31" t="n">
-        <v>3762486384</v>
+        <v>4413581530</v>
       </c>
       <c r="F31" t="n">
-        <v>110216642</v>
+        <v>112878011</v>
       </c>
       <c r="G31" t="n">
-        <v>1.68368</v>
+        <v>4.93542</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>579.75</v>
+        <v>11.6</v>
       </c>
       <c r="E32" t="n">
-        <v>3659611425</v>
+        <v>4261614889</v>
       </c>
       <c r="F32" t="n">
-        <v>14266389</v>
+        <v>243151720</v>
       </c>
       <c r="G32" t="n">
-        <v>-2.55087</v>
+        <v>-4.5269</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>2.53</v>
+        <v>641.46</v>
       </c>
       <c r="E33" t="n">
-        <v>3654601547</v>
+        <v>4058982126</v>
       </c>
       <c r="F33" t="n">
-        <v>70388012</v>
+        <v>22296099</v>
       </c>
       <c r="G33" t="n">
-        <v>2.27114</v>
+        <v>-3.18693</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.107599</v>
+        <v>4.04</v>
       </c>
       <c r="E34" t="n">
-        <v>3625964033</v>
+        <v>4058789344</v>
       </c>
       <c r="F34" t="n">
-        <v>82402468</v>
+        <v>520296929</v>
       </c>
       <c r="G34" t="n">
-        <v>-1.07704</v>
+        <v>3.71341</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>3.7</v>
+        <v>0.135141</v>
       </c>
       <c r="E35" t="n">
-        <v>3545709931</v>
+        <v>3845619266</v>
       </c>
       <c r="F35" t="n">
-        <v>164549621</v>
+        <v>196263899</v>
       </c>
       <c r="G35" t="n">
-        <v>2.96799</v>
+        <v>-1.04355</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>9.539999999999999</v>
+        <v>0.16809</v>
       </c>
       <c r="E36" t="n">
-        <v>3492554059</v>
+        <v>3837431056</v>
       </c>
       <c r="F36" t="n">
-        <v>81133865</v>
+        <v>52794694</v>
       </c>
       <c r="G36" t="n">
-        <v>1.77096</v>
+        <v>-0.93492</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.116357</v>
+        <v>0.112103</v>
       </c>
       <c r="E37" t="n">
-        <v>3312669107</v>
+        <v>3771687089</v>
       </c>
       <c r="F37" t="n">
-        <v>57358930</v>
+        <v>108779392</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.08545999999999999</v>
+        <v>-2.82166</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>FDUSD</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>First Digital USD</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.99766</v>
+        <v>0.140655</v>
       </c>
       <c r="E38" t="n">
-        <v>3301453412</v>
+        <v>3691566481</v>
       </c>
       <c r="F38" t="n">
-        <v>3016475587</v>
+        <v>104284280</v>
       </c>
       <c r="G38" t="n">
-        <v>-0.35747</v>
+        <v>8.641310000000001</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.04457198</v>
+        <v>41.17</v>
       </c>
       <c r="E39" t="n">
-        <v>3242400882</v>
+        <v>3634594409</v>
       </c>
       <c r="F39" t="n">
-        <v>78603193</v>
+        <v>239054444</v>
       </c>
       <c r="G39" t="n">
-        <v>2.56178</v>
+        <v>-3.87042</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>50.5</v>
+        <v>0.04905655</v>
       </c>
       <c r="E40" t="n">
-        <v>3030010080</v>
+        <v>3559329986</v>
       </c>
       <c r="F40" t="n">
-        <v>5659343</v>
+        <v>130828517</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.94948</v>
+        <v>-2.62835</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>33.95</v>
+        <v>58.77</v>
       </c>
       <c r="E41" t="n">
-        <v>3006829319</v>
+        <v>3525830676</v>
       </c>
       <c r="F41" t="n">
-        <v>84559425</v>
+        <v>41445280</v>
       </c>
       <c r="G41" t="n">
-        <v>-0.94517</v>
+        <v>8.568619999999999</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>FDUSD</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>First Digital USD</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>3.33</v>
+        <v>1.006</v>
       </c>
       <c r="E42" t="n">
-        <v>2967465062</v>
+        <v>3265112206</v>
       </c>
       <c r="F42" t="n">
-        <v>89985202</v>
+        <v>1819425293</v>
       </c>
       <c r="G42" t="n">
-        <v>1.47877</v>
+        <v>0.6529</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>TIA</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Celestia</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>17.01</v>
+        <v>0.325914</v>
       </c>
       <c r="E43" t="n">
-        <v>2836340436</v>
+        <v>3064133874</v>
       </c>
       <c r="F43" t="n">
-        <v>75099982</v>
+        <v>259955770</v>
       </c>
       <c r="G43" t="n">
-        <v>2.59609</v>
+        <v>3.04899</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>7.47</v>
+        <v>3.35</v>
       </c>
       <c r="E44" t="n">
-        <v>2823864116</v>
+        <v>2976067219</v>
       </c>
       <c r="F44" t="n">
-        <v>262530083</v>
+        <v>111532582</v>
       </c>
       <c r="G44" t="n">
-        <v>4.86404</v>
+        <v>-1.29595</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.292679</v>
+        <v>0.899986</v>
       </c>
       <c r="E45" t="n">
-        <v>2737733373</v>
+        <v>2903673110</v>
       </c>
       <c r="F45" t="n">
-        <v>344194202</v>
+        <v>242961636</v>
       </c>
       <c r="G45" t="n">
-        <v>9.846679999999999</v>
+        <v>-1.51913</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.797198</v>
+        <v>7.69</v>
       </c>
       <c r="E46" t="n">
-        <v>2573420780</v>
+        <v>2902794606</v>
       </c>
       <c r="F46" t="n">
-        <v>64695810</v>
+        <v>272150017</v>
       </c>
       <c r="G46" t="n">
-        <v>2.81095</v>
+        <v>0.20847</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>TIA</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Celestia</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.093056</v>
+        <v>16.45</v>
       </c>
       <c r="E47" t="n">
-        <v>2474964102</v>
+        <v>2759429225</v>
       </c>
       <c r="F47" t="n">
-        <v>9614166</v>
+        <v>135472008</v>
       </c>
       <c r="G47" t="n">
-        <v>-1.20863</v>
+        <v>-1.48676</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>1.87</v>
+        <v>149.06</v>
       </c>
       <c r="E48" t="n">
-        <v>2380126193</v>
+        <v>2703444281</v>
       </c>
       <c r="F48" t="n">
-        <v>239833081</v>
+        <v>66188445</v>
       </c>
       <c r="G48" t="n">
-        <v>1.65933</v>
+        <v>4.28351</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>123.94</v>
+        <v>2.11</v>
       </c>
       <c r="E49" t="n">
-        <v>2250704723</v>
+        <v>2686981752</v>
       </c>
       <c r="F49" t="n">
-        <v>33317637</v>
+        <v>980719162</v>
       </c>
       <c r="G49" t="n">
-        <v>-0.91814</v>
+        <v>6.31939</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SEI</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Sei</t>
+          <t>Pepe</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.829756</v>
+        <v>5.65e-06</v>
       </c>
       <c r="E50" t="n">
-        <v>2117336370</v>
+        <v>2375911933</v>
       </c>
       <c r="F50" t="n">
-        <v>169098247</v>
+        <v>1726638422</v>
       </c>
       <c r="G50" t="n">
-        <v>1.99686</v>
+        <v>30.38714</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>SUI</t>
+          <t>THETA</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Sui</t>
+          <t>Theta Network</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>1.64</v>
+        <v>2.33</v>
       </c>
       <c r="E51" t="n">
-        <v>1906957337</v>
+        <v>2323517156</v>
       </c>
       <c r="F51" t="n">
-        <v>155310833</v>
+        <v>183552566</v>
       </c>
       <c r="G51" t="n">
-        <v>1.50402</v>
+        <v>17.65106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-03-10
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>62480</v>
+        <v>69792</v>
       </c>
       <c r="E2" t="n">
-        <v>1224975413389</v>
+        <v>1372768066343</v>
       </c>
       <c r="F2" t="n">
-        <v>19244343459</v>
+        <v>29480287500</v>
       </c>
       <c r="G2" t="n">
-        <v>0.60659</v>
+        <v>2.11147</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3449.34</v>
+        <v>3947.06</v>
       </c>
       <c r="E3" t="n">
-        <v>413682749278</v>
+        <v>474150365225</v>
       </c>
       <c r="F3" t="n">
-        <v>12842815698</v>
+        <v>14032475055</v>
       </c>
       <c r="G3" t="n">
-        <v>0.67758</v>
+        <v>0.87414</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1.001</v>
+        <v>1.002</v>
       </c>
       <c r="E4" t="n">
-        <v>99397291213</v>
+        <v>102068929003</v>
       </c>
       <c r="F4" t="n">
-        <v>45275587693</v>
+        <v>57138276325</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.09734</v>
+        <v>0.07492</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>415.5</v>
+        <v>535.26</v>
       </c>
       <c r="E5" t="n">
-        <v>63916190674</v>
+        <v>82447329943</v>
       </c>
       <c r="F5" t="n">
-        <v>1543994524</v>
+        <v>3733362208</v>
       </c>
       <c r="G5" t="n">
-        <v>1.08307</v>
+        <v>9.94711</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>129.32</v>
+        <v>145.95</v>
       </c>
       <c r="E6" t="n">
-        <v>57051482565</v>
+        <v>64706400180</v>
       </c>
       <c r="F6" t="n">
-        <v>3326689612</v>
+        <v>3098432302</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.61344</v>
+        <v>-0.21787</v>
       </c>
     </row>
     <row r="7">
@@ -611,25 +611,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>STETH</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>Lido Staked Ether</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.629507</v>
+        <v>3941.66</v>
       </c>
       <c r="E7" t="n">
-        <v>34324377864</v>
+        <v>38901061402</v>
       </c>
       <c r="F7" t="n">
-        <v>2241507633</v>
+        <v>20746321</v>
       </c>
       <c r="G7" t="n">
-        <v>-2.94615</v>
+        <v>0.78876</v>
       </c>
     </row>
     <row r="8">
@@ -638,25 +638,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>STETH</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Lido Staked Ether</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>3440.57</v>
+        <v>0.621121</v>
       </c>
       <c r="E8" t="n">
-        <v>33827781061</v>
+        <v>34008213135</v>
       </c>
       <c r="F8" t="n">
-        <v>26304596</v>
+        <v>1361061218</v>
       </c>
       <c r="G8" t="n">
-        <v>0.63791</v>
+        <v>-0.20643</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1.002</v>
+        <v>0.999821</v>
       </c>
       <c r="E9" t="n">
-        <v>28987955848</v>
+        <v>30163413511</v>
       </c>
       <c r="F9" t="n">
-        <v>5316140260</v>
+        <v>6228037557</v>
       </c>
       <c r="G9" t="n">
-        <v>0.05311</v>
+        <v>0.07328999999999999</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.73249</v>
+        <v>0.7305970000000001</v>
       </c>
       <c r="E10" t="n">
-        <v>25714596642</v>
+        <v>25703642667</v>
       </c>
       <c r="F10" t="n">
-        <v>919826048</v>
+        <v>564037720</v>
       </c>
       <c r="G10" t="n">
-        <v>-1.41506</v>
+        <v>-0.02436</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.142432</v>
+        <v>0.174068</v>
       </c>
       <c r="E11" t="n">
-        <v>20425961864</v>
+        <v>24952662017</v>
       </c>
       <c r="F11" t="n">
-        <v>3214142207</v>
+        <v>3529979595</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.26243</v>
+        <v>4.90671</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +746,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>43</v>
+        <v>3.389e-05</v>
       </c>
       <c r="E12" t="n">
-        <v>16196682514</v>
+        <v>19980795015</v>
       </c>
       <c r="F12" t="n">
-        <v>771365366</v>
+        <v>2159557539</v>
       </c>
       <c r="G12" t="n">
-        <v>0.56389</v>
+        <v>-0.98049</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2.238e-05</v>
+        <v>42.84</v>
       </c>
       <c r="E13" t="n">
-        <v>13137540052</v>
+        <v>16170083382</v>
       </c>
       <c r="F13" t="n">
-        <v>4317467105</v>
+        <v>551695626</v>
       </c>
       <c r="G13" t="n">
-        <v>1.64152</v>
+        <v>-1.01987</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.1408</v>
+        <v>10.44</v>
       </c>
       <c r="E14" t="n">
-        <v>12357939760</v>
+        <v>13999088483</v>
       </c>
       <c r="F14" t="n">
-        <v>348344607</v>
+        <v>392533419</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.10014</v>
+        <v>-3.95771</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>9.23</v>
+        <v>0.13586</v>
       </c>
       <c r="E15" t="n">
-        <v>12306673038</v>
+        <v>11947735137</v>
       </c>
       <c r="F15" t="n">
-        <v>562809820</v>
+        <v>349480182</v>
       </c>
       <c r="G15" t="n">
-        <v>0.92471</v>
+        <v>-0.1146</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>20.67</v>
+        <v>19.89</v>
       </c>
       <c r="E16" t="n">
-        <v>12133699722</v>
+        <v>11689227698</v>
       </c>
       <c r="F16" t="n">
-        <v>928928176</v>
+        <v>464409434</v>
       </c>
       <c r="G16" t="n">
-        <v>-1.45096</v>
+        <v>-0.67979</v>
       </c>
     </row>
     <row r="17">
@@ -890,16 +890,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1.084</v>
+        <v>1.22</v>
       </c>
       <c r="E17" t="n">
-        <v>10027721620</v>
+        <v>11349289853</v>
       </c>
       <c r="F17" t="n">
-        <v>1012961964</v>
+        <v>896885173</v>
       </c>
       <c r="G17" t="n">
-        <v>0.39357</v>
+        <v>7.41905</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>62419</v>
+        <v>69662</v>
       </c>
       <c r="E18" t="n">
-        <v>9706977671</v>
+        <v>10881681787</v>
       </c>
       <c r="F18" t="n">
-        <v>133709900</v>
+        <v>201038582</v>
       </c>
       <c r="G18" t="n">
-        <v>0.4485</v>
+        <v>1.78569</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>12.82</v>
+        <v>14.14</v>
       </c>
       <c r="E19" t="n">
-        <v>9645689666</v>
+        <v>10635468364</v>
       </c>
       <c r="F19" t="n">
-        <v>504931027</v>
+        <v>302493958</v>
       </c>
       <c r="G19" t="n">
-        <v>5.51719</v>
+        <v>-0.73521</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>484.45</v>
+        <v>2.84</v>
       </c>
       <c r="E20" t="n">
-        <v>9553161067</v>
+        <v>9868879057</v>
       </c>
       <c r="F20" t="n">
-        <v>2339333868</v>
+        <v>64675832</v>
       </c>
       <c r="G20" t="n">
-        <v>9.14143</v>
+        <v>-1.26682</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>2.66</v>
+        <v>434.32</v>
       </c>
       <c r="E21" t="n">
-        <v>9189762472</v>
+        <v>8546928858</v>
       </c>
       <c r="F21" t="n">
-        <v>69672311</v>
+        <v>394775514</v>
       </c>
       <c r="G21" t="n">
-        <v>-2.9109</v>
+        <v>0.44527</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>92.28</v>
+        <v>14.6</v>
       </c>
       <c r="E22" t="n">
-        <v>6829953290</v>
+        <v>6717111393</v>
       </c>
       <c r="F22" t="n">
-        <v>966291106</v>
+        <v>181197216</v>
       </c>
       <c r="G22" t="n">
-        <v>1.06772</v>
+        <v>-2.31756</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>13.19</v>
+        <v>88.75</v>
       </c>
       <c r="E23" t="n">
-        <v>6049707846</v>
+        <v>6600340584</v>
       </c>
       <c r="F23" t="n">
-        <v>213881714</v>
+        <v>535070214</v>
       </c>
       <c r="G23" t="n">
-        <v>0.38476</v>
+        <v>0.81255</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>9.83</v>
+        <v>6.09</v>
       </c>
       <c r="E24" t="n">
-        <v>5090928003</v>
+        <v>6353400075</v>
       </c>
       <c r="F24" t="n">
-        <v>979192099</v>
+        <v>510322927</v>
       </c>
       <c r="G24" t="n">
-        <v>11.16078</v>
+        <v>-3.21122</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>1.001</v>
+        <v>10.88</v>
       </c>
       <c r="E25" t="n">
-        <v>5016431198</v>
+        <v>5690830573</v>
       </c>
       <c r="F25" t="n">
-        <v>193191310</v>
+        <v>487998958</v>
       </c>
       <c r="G25" t="n">
-        <v>0.1595</v>
+        <v>-3.57936</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>33.67</v>
+        <v>36.79</v>
       </c>
       <c r="E26" t="n">
-        <v>4811676787</v>
+        <v>5370960040</v>
       </c>
       <c r="F26" t="n">
-        <v>690570406</v>
+        <v>261645856</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.46522</v>
+        <v>-3.17887</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>11.92</v>
+        <v>5.7</v>
       </c>
       <c r="E27" t="n">
-        <v>4628753546</v>
+        <v>5291579047</v>
       </c>
       <c r="F27" t="n">
-        <v>418688877</v>
+        <v>2616817</v>
       </c>
       <c r="G27" t="n">
-        <v>-1.32739</v>
+        <v>-0.10607</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>3.27</v>
+        <v>13.34</v>
       </c>
       <c r="E28" t="n">
-        <v>4543782473</v>
+        <v>5202848287</v>
       </c>
       <c r="F28" t="n">
-        <v>126085880</v>
+        <v>286292175</v>
       </c>
       <c r="G28" t="n">
-        <v>3.08205</v>
+        <v>-2.99241</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>4.78</v>
+        <v>13.07</v>
       </c>
       <c r="E29" t="n">
-        <v>4417329208</v>
+        <v>4825470332</v>
       </c>
       <c r="F29" t="n">
-        <v>2770808</v>
+        <v>167653450</v>
       </c>
       <c r="G29" t="n">
-        <v>0.26881</v>
+        <v>-3.01964</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>4.27</v>
+        <v>3.39</v>
       </c>
       <c r="E30" t="n">
-        <v>4413845986</v>
+        <v>4709282684</v>
       </c>
       <c r="F30" t="n">
-        <v>480707549</v>
+        <v>127754714</v>
       </c>
       <c r="G30" t="n">
-        <v>2.3376</v>
+        <v>-3.29582</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>3.06</v>
+        <v>4.65</v>
       </c>
       <c r="E31" t="n">
-        <v>4413581530</v>
+        <v>4684388479</v>
       </c>
       <c r="F31" t="n">
-        <v>112878011</v>
+        <v>335141421</v>
       </c>
       <c r="G31" t="n">
-        <v>4.93542</v>
+        <v>2.80675</v>
       </c>
     </row>
     <row r="32">
@@ -1286,30 +1286,30 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>11.6</v>
+        <v>3.24</v>
       </c>
       <c r="E32" t="n">
-        <v>4261614889</v>
+        <v>4653182074</v>
       </c>
       <c r="F32" t="n">
-        <v>243151720</v>
+        <v>191954180</v>
       </c>
       <c r="G32" t="n">
-        <v>-4.5269</v>
+        <v>14.64591</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1322,43 +1322,43 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>641.46</v>
+        <v>705.29</v>
       </c>
       <c r="E33" t="n">
-        <v>4058982126</v>
+        <v>4503492201</v>
       </c>
       <c r="F33" t="n">
-        <v>22296099</v>
+        <v>21293526</v>
       </c>
       <c r="G33" t="n">
-        <v>-3.18693</v>
+        <v>-1.49537</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>4.04</v>
+        <v>11.8</v>
       </c>
       <c r="E34" t="n">
-        <v>4058789344</v>
+        <v>4497026052</v>
       </c>
       <c r="F34" t="n">
-        <v>520296929</v>
+        <v>651198464</v>
       </c>
       <c r="G34" t="n">
-        <v>3.71341</v>
+        <v>5.29091</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.135141</v>
+        <v>1.002</v>
       </c>
       <c r="E35" t="n">
-        <v>3845619266</v>
+        <v>4459558988</v>
       </c>
       <c r="F35" t="n">
-        <v>196263899</v>
+        <v>241188651</v>
       </c>
       <c r="G35" t="n">
-        <v>-1.04355</v>
+        <v>0.11011</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.16809</v>
+        <v>0.167438</v>
       </c>
       <c r="E36" t="n">
-        <v>3837431056</v>
+        <v>4445744063</v>
       </c>
       <c r="F36" t="n">
-        <v>52794694</v>
+        <v>57181585</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.93492</v>
+        <v>3.5072</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.112103</v>
+        <v>0.471982</v>
       </c>
       <c r="E37" t="n">
-        <v>3771687089</v>
+        <v>4410355072</v>
       </c>
       <c r="F37" t="n">
-        <v>108779392</v>
+        <v>1157517684</v>
       </c>
       <c r="G37" t="n">
-        <v>-2.82166</v>
+        <v>20.43049</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.140655</v>
+        <v>0.128049</v>
       </c>
       <c r="E38" t="n">
-        <v>3691566481</v>
+        <v>4310912076</v>
       </c>
       <c r="F38" t="n">
-        <v>104284280</v>
+        <v>73505372</v>
       </c>
       <c r="G38" t="n">
-        <v>8.641310000000001</v>
+        <v>-1.23158</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>41.17</v>
+        <v>71.33</v>
       </c>
       <c r="E39" t="n">
-        <v>3634594409</v>
+        <v>4299541978</v>
       </c>
       <c r="F39" t="n">
-        <v>239054444</v>
+        <v>53305462</v>
       </c>
       <c r="G39" t="n">
-        <v>-3.87042</v>
+        <v>17.98066</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.04905655</v>
+        <v>0.14272</v>
       </c>
       <c r="E40" t="n">
-        <v>3559329986</v>
+        <v>4087486935</v>
       </c>
       <c r="F40" t="n">
-        <v>130828517</v>
+        <v>124480744</v>
       </c>
       <c r="G40" t="n">
-        <v>-2.62835</v>
+        <v>1.0794</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Pepe</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>58.77</v>
+        <v>8.54e-06</v>
       </c>
       <c r="E41" t="n">
-        <v>3525830676</v>
+        <v>3605453006</v>
       </c>
       <c r="F41" t="n">
-        <v>41445280</v>
+        <v>1262647504</v>
       </c>
       <c r="G41" t="n">
-        <v>8.568619999999999</v>
+        <v>-2.15797</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>FDUSD</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>First Digital USD</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1.006</v>
+        <v>40.59</v>
       </c>
       <c r="E42" t="n">
-        <v>3265112206</v>
+        <v>3593120848</v>
       </c>
       <c r="F42" t="n">
-        <v>1819425293</v>
+        <v>156925788</v>
       </c>
       <c r="G42" t="n">
-        <v>0.6529</v>
+        <v>-1.94281</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.325914</v>
+        <v>0.04839979</v>
       </c>
       <c r="E43" t="n">
-        <v>3064133874</v>
+        <v>3520741472</v>
       </c>
       <c r="F43" t="n">
-        <v>259955770</v>
+        <v>136526334</v>
       </c>
       <c r="G43" t="n">
-        <v>3.04899</v>
+        <v>-0.35568</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>3.35</v>
+        <v>1.062</v>
       </c>
       <c r="E44" t="n">
-        <v>2976067219</v>
+        <v>3433028163</v>
       </c>
       <c r="F44" t="n">
-        <v>111532582</v>
+        <v>218531795</v>
       </c>
       <c r="G44" t="n">
-        <v>-1.29595</v>
+        <v>2.19989</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.899986</v>
+        <v>0.149773</v>
       </c>
       <c r="E45" t="n">
-        <v>2903673110</v>
+        <v>3428401596</v>
       </c>
       <c r="F45" t="n">
-        <v>242961636</v>
+        <v>83972213</v>
       </c>
       <c r="G45" t="n">
-        <v>-1.51913</v>
+        <v>2.575</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>FDUSD</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>First Digital USD</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>7.69</v>
+        <v>1.003</v>
       </c>
       <c r="E46" t="n">
-        <v>2902794606</v>
+        <v>3303587057</v>
       </c>
       <c r="F46" t="n">
-        <v>272150017</v>
+        <v>9401755959</v>
       </c>
       <c r="G46" t="n">
-        <v>0.20847</v>
+        <v>-0.06571</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>TIA</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Celestia</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>16.45</v>
+        <v>2.1</v>
       </c>
       <c r="E47" t="n">
-        <v>2759429225</v>
+        <v>3042844804</v>
       </c>
       <c r="F47" t="n">
-        <v>135472008</v>
+        <v>520026168</v>
       </c>
       <c r="G47" t="n">
-        <v>-1.48676</v>
+        <v>-1.68752</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>THETA</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Theta Network</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>149.06</v>
+        <v>3.01</v>
       </c>
       <c r="E48" t="n">
-        <v>2703444281</v>
+        <v>3012862586</v>
       </c>
       <c r="F48" t="n">
-        <v>66188445</v>
+        <v>72720603</v>
       </c>
       <c r="G48" t="n">
-        <v>4.28351</v>
+        <v>-3.78113</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>2.11</v>
+        <v>3.34</v>
       </c>
       <c r="E49" t="n">
-        <v>2686981752</v>
+        <v>2977986124</v>
       </c>
       <c r="F49" t="n">
-        <v>980719162</v>
+        <v>82529926</v>
       </c>
       <c r="G49" t="n">
-        <v>6.31939</v>
+        <v>-1.67793</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>FET</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Pepe</t>
+          <t>Fetch.ai</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>5.65e-06</v>
+        <v>2.81</v>
       </c>
       <c r="E50" t="n">
-        <v>2375911933</v>
+        <v>2937498258</v>
       </c>
       <c r="F50" t="n">
-        <v>1726638422</v>
+        <v>627542252</v>
       </c>
       <c r="G50" t="n">
-        <v>30.38714</v>
+        <v>-2.79714</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>THETA</t>
+          <t>TIA</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Theta Network</t>
+          <t>Celestia</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>2.33</v>
+        <v>16.46</v>
       </c>
       <c r="E51" t="n">
-        <v>2323517156</v>
+        <v>2789998305</v>
       </c>
       <c r="F51" t="n">
-        <v>183552566</v>
+        <v>135259188</v>
       </c>
       <c r="G51" t="n">
-        <v>17.65106</v>
+        <v>-4.48562</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-03-17
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>69792</v>
+        <v>66767</v>
       </c>
       <c r="E2" t="n">
-        <v>1372768066343</v>
+        <v>1317540462031</v>
       </c>
       <c r="F2" t="n">
-        <v>29480287500</v>
+        <v>58370774815</v>
       </c>
       <c r="G2" t="n">
-        <v>2.11147</v>
+        <v>-2.30488</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3947.06</v>
+        <v>3570.76</v>
       </c>
       <c r="E3" t="n">
-        <v>474150365225</v>
+        <v>429377428195</v>
       </c>
       <c r="F3" t="n">
-        <v>14032475055</v>
+        <v>26843432307</v>
       </c>
       <c r="G3" t="n">
-        <v>0.87414</v>
+        <v>-3.69067</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1.002</v>
+        <v>0.996949</v>
       </c>
       <c r="E4" t="n">
-        <v>102068929003</v>
+        <v>103211906265</v>
       </c>
       <c r="F4" t="n">
-        <v>57138276325</v>
+        <v>73693896831</v>
       </c>
       <c r="G4" t="n">
-        <v>0.07492</v>
+        <v>-0.56706</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>535.26</v>
+        <v>570.55</v>
       </c>
       <c r="E5" t="n">
-        <v>82447329943</v>
+        <v>88100504532</v>
       </c>
       <c r="F5" t="n">
-        <v>3733362208</v>
+        <v>4885730188</v>
       </c>
       <c r="G5" t="n">
-        <v>9.94711</v>
+        <v>-5.72398</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>145.95</v>
+        <v>191.34</v>
       </c>
       <c r="E6" t="n">
-        <v>64706400180</v>
+        <v>85203844660</v>
       </c>
       <c r="F6" t="n">
-        <v>3098432302</v>
+        <v>12598405929</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.21787</v>
+        <v>0.129</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3941.66</v>
+        <v>3567.87</v>
       </c>
       <c r="E7" t="n">
-        <v>38901061402</v>
+        <v>34946620795</v>
       </c>
       <c r="F7" t="n">
-        <v>20746321</v>
+        <v>76002939</v>
       </c>
       <c r="G7" t="n">
-        <v>0.78876</v>
+        <v>-3.50899</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.621121</v>
+        <v>0.613313</v>
       </c>
       <c r="E8" t="n">
-        <v>34008213135</v>
+        <v>33627532063</v>
       </c>
       <c r="F8" t="n">
-        <v>1361061218</v>
+        <v>2418528876</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.20643</v>
+        <v>-2.48676</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.999821</v>
+        <v>0.998122</v>
       </c>
       <c r="E9" t="n">
-        <v>30163413511</v>
+        <v>30780165989</v>
       </c>
       <c r="F9" t="n">
-        <v>6228037557</v>
+        <v>11918839584</v>
       </c>
       <c r="G9" t="n">
-        <v>0.07328999999999999</v>
+        <v>-0.15399</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.7305970000000001</v>
+        <v>0.676299</v>
       </c>
       <c r="E10" t="n">
-        <v>25703642667</v>
+        <v>23921770520</v>
       </c>
       <c r="F10" t="n">
-        <v>564037720</v>
+        <v>1068617556</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.02436</v>
+        <v>-5.60821</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.174068</v>
+        <v>0.148312</v>
       </c>
       <c r="E11" t="n">
-        <v>24952662017</v>
+        <v>21340672957</v>
       </c>
       <c r="F11" t="n">
-        <v>3529979595</v>
+        <v>3020361808</v>
       </c>
       <c r="G11" t="n">
-        <v>4.90671</v>
+        <v>-5.39815</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +746,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>3.389e-05</v>
+        <v>55.83</v>
       </c>
       <c r="E12" t="n">
-        <v>19980795015</v>
+        <v>21173856921</v>
       </c>
       <c r="F12" t="n">
-        <v>2159557539</v>
+        <v>1990840741</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.98049</v>
+        <v>-4.93622</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>42.84</v>
+        <v>2.68e-05</v>
       </c>
       <c r="E13" t="n">
-        <v>16170083382</v>
+        <v>15854269859</v>
       </c>
       <c r="F13" t="n">
-        <v>551695626</v>
+        <v>2344238830</v>
       </c>
       <c r="G13" t="n">
-        <v>-1.01987</v>
+        <v>-4.63066</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>10.44</v>
+        <v>9.83</v>
       </c>
       <c r="E14" t="n">
-        <v>13999088483</v>
+        <v>13214172041</v>
       </c>
       <c r="F14" t="n">
-        <v>392533419</v>
+        <v>583278730</v>
       </c>
       <c r="G14" t="n">
-        <v>-3.95771</v>
+        <v>-4.83464</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.13586</v>
+        <v>3.62</v>
       </c>
       <c r="E15" t="n">
-        <v>11947735137</v>
+        <v>12591205708</v>
       </c>
       <c r="F15" t="n">
-        <v>349480182</v>
+        <v>105687801</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.1146</v>
+        <v>-2.64036</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>19.89</v>
+        <v>0.124773</v>
       </c>
       <c r="E16" t="n">
-        <v>11689227698</v>
+        <v>10968818908</v>
       </c>
       <c r="F16" t="n">
-        <v>464409434</v>
+        <v>515129095</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.67979</v>
+        <v>-1.81144</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1.22</v>
+        <v>18.24</v>
       </c>
       <c r="E17" t="n">
-        <v>11349289853</v>
+        <v>10771861912</v>
       </c>
       <c r="F17" t="n">
-        <v>896885173</v>
+        <v>794227424</v>
       </c>
       <c r="G17" t="n">
-        <v>7.41905</v>
+        <v>-5.41016</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>69662</v>
+        <v>66936</v>
       </c>
       <c r="E18" t="n">
-        <v>10881681787</v>
+        <v>10399368080</v>
       </c>
       <c r="F18" t="n">
-        <v>201038582</v>
+        <v>418936379</v>
       </c>
       <c r="G18" t="n">
-        <v>1.78569</v>
+        <v>-1.8624</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>14.14</v>
+        <v>1.059</v>
       </c>
       <c r="E19" t="n">
-        <v>10635468364</v>
+        <v>9863606995</v>
       </c>
       <c r="F19" t="n">
-        <v>302493958</v>
+        <v>892614640</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.73521</v>
+        <v>-7.02731</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>2.84</v>
+        <v>12.12</v>
       </c>
       <c r="E20" t="n">
-        <v>9868879057</v>
+        <v>9147147043</v>
       </c>
       <c r="F20" t="n">
-        <v>64675832</v>
+        <v>267528590</v>
       </c>
       <c r="G20" t="n">
-        <v>-1.26682</v>
+        <v>-4.67625</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>434.32</v>
+        <v>7.76</v>
       </c>
       <c r="E21" t="n">
-        <v>8546928858</v>
+        <v>8051637249</v>
       </c>
       <c r="F21" t="n">
-        <v>394775514</v>
+        <v>1068358670</v>
       </c>
       <c r="G21" t="n">
-        <v>0.44527</v>
+        <v>1.00923</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>14.6</v>
+        <v>399.14</v>
       </c>
       <c r="E22" t="n">
-        <v>6717111393</v>
+        <v>7877840183</v>
       </c>
       <c r="F22" t="n">
-        <v>181197216</v>
+        <v>593591227</v>
       </c>
       <c r="G22" t="n">
-        <v>-2.31756</v>
+        <v>-1.49163</v>
       </c>
     </row>
     <row r="23">
@@ -1052,16 +1052,16 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>88.75</v>
+        <v>85.81999999999999</v>
       </c>
       <c r="E23" t="n">
-        <v>6600340584</v>
+        <v>6388271232</v>
       </c>
       <c r="F23" t="n">
-        <v>535070214</v>
+        <v>720251547</v>
       </c>
       <c r="G23" t="n">
-        <v>0.81255</v>
+        <v>-4.07834</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>6.09</v>
+        <v>12.42</v>
       </c>
       <c r="E24" t="n">
-        <v>6353400075</v>
+        <v>5737850176</v>
       </c>
       <c r="F24" t="n">
-        <v>510322927</v>
+        <v>211363273</v>
       </c>
       <c r="G24" t="n">
-        <v>-3.21122</v>
+        <v>-3.12471</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>10.88</v>
+        <v>6.03</v>
       </c>
       <c r="E25" t="n">
-        <v>5690830573</v>
+        <v>5600043458</v>
       </c>
       <c r="F25" t="n">
-        <v>487998958</v>
+        <v>3610533</v>
       </c>
       <c r="G25" t="n">
-        <v>-3.57936</v>
+        <v>0.06342</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>36.79</v>
+        <v>14.08</v>
       </c>
       <c r="E26" t="n">
-        <v>5370960040</v>
+        <v>5594377088</v>
       </c>
       <c r="F26" t="n">
-        <v>261645856</v>
+        <v>534345126</v>
       </c>
       <c r="G26" t="n">
-        <v>-3.17887</v>
+        <v>-5.66227</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>5.7</v>
+        <v>12.1</v>
       </c>
       <c r="E27" t="n">
-        <v>5291579047</v>
+        <v>4740189264</v>
       </c>
       <c r="F27" t="n">
-        <v>2616817</v>
+        <v>368432907</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.10607</v>
+        <v>-3.69979</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>13.34</v>
+        <v>0.998034</v>
       </c>
       <c r="E28" t="n">
-        <v>5202848287</v>
+        <v>4683938253</v>
       </c>
       <c r="F28" t="n">
-        <v>286292175</v>
+        <v>768256322</v>
       </c>
       <c r="G28" t="n">
-        <v>-2.99241</v>
+        <v>-0.11995</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>13.07</v>
+        <v>8.890000000000001</v>
       </c>
       <c r="E29" t="n">
-        <v>4825470332</v>
+        <v>4679781583</v>
       </c>
       <c r="F29" t="n">
-        <v>167653450</v>
+        <v>527310065</v>
       </c>
       <c r="G29" t="n">
-        <v>-3.01964</v>
+        <v>-6.51051</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>3.39</v>
+        <v>31.07</v>
       </c>
       <c r="E30" t="n">
-        <v>4709282684</v>
+        <v>4544696452</v>
       </c>
       <c r="F30" t="n">
-        <v>127754714</v>
+        <v>312339699</v>
       </c>
       <c r="G30" t="n">
-        <v>-3.29582</v>
+        <v>-3.89611</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>4.65</v>
+        <v>11.57</v>
       </c>
       <c r="E31" t="n">
-        <v>4684388479</v>
+        <v>4414049385</v>
       </c>
       <c r="F31" t="n">
-        <v>335141421</v>
+        <v>665371836</v>
       </c>
       <c r="G31" t="n">
-        <v>2.80675</v>
+        <v>-1.45818</v>
       </c>
     </row>
     <row r="32">
@@ -1286,79 +1286,79 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>3.24</v>
+        <v>638.78</v>
       </c>
       <c r="E32" t="n">
-        <v>4653182074</v>
+        <v>4118602027</v>
       </c>
       <c r="F32" t="n">
-        <v>191954180</v>
+        <v>31884705</v>
       </c>
       <c r="G32" t="n">
-        <v>14.64591</v>
+        <v>2.74366</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>705.29</v>
+        <v>2.91</v>
       </c>
       <c r="E33" t="n">
-        <v>4503492201</v>
+        <v>4052562347</v>
       </c>
       <c r="F33" t="n">
-        <v>21293526</v>
+        <v>106967040</v>
       </c>
       <c r="G33" t="n">
-        <v>-1.49537</v>
+        <v>-3.60499</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>11.8</v>
+        <v>2.72</v>
       </c>
       <c r="E34" t="n">
-        <v>4497026052</v>
+        <v>3938353274</v>
       </c>
       <c r="F34" t="n">
-        <v>651198464</v>
+        <v>128412337</v>
       </c>
       <c r="G34" t="n">
-        <v>5.29091</v>
+        <v>-0.45104</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1.002</v>
+        <v>0.113801</v>
       </c>
       <c r="E35" t="n">
-        <v>4459558988</v>
+        <v>3838591906</v>
       </c>
       <c r="F35" t="n">
-        <v>241188651</v>
+        <v>99590958</v>
       </c>
       <c r="G35" t="n">
-        <v>0.11011</v>
+        <v>-5.03746</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.167438</v>
+        <v>63.85</v>
       </c>
       <c r="E36" t="n">
-        <v>4445744063</v>
+        <v>3832538080</v>
       </c>
       <c r="F36" t="n">
-        <v>57181585</v>
+        <v>27764541</v>
       </c>
       <c r="G36" t="n">
-        <v>3.5072</v>
+        <v>-5.51109</v>
       </c>
     </row>
     <row r="37">
@@ -1430,16 +1430,16 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.471982</v>
+        <v>0.399825</v>
       </c>
       <c r="E37" t="n">
-        <v>4410355072</v>
+        <v>3770222674</v>
       </c>
       <c r="F37" t="n">
-        <v>1157517684</v>
+        <v>269482757</v>
       </c>
       <c r="G37" t="n">
-        <v>20.43049</v>
+        <v>-1.59098</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.128049</v>
+        <v>42.03</v>
       </c>
       <c r="E38" t="n">
-        <v>4310912076</v>
+        <v>3720439441</v>
       </c>
       <c r="F38" t="n">
-        <v>73505372</v>
+        <v>366997991</v>
       </c>
       <c r="G38" t="n">
-        <v>-1.23158</v>
+        <v>-9.737579999999999</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>71.33</v>
+        <v>0.129542</v>
       </c>
       <c r="E39" t="n">
-        <v>4299541978</v>
+        <v>3716780240</v>
       </c>
       <c r="F39" t="n">
-        <v>53305462</v>
+        <v>172822366</v>
       </c>
       <c r="G39" t="n">
-        <v>17.98066</v>
+        <v>-6.21046</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.14272</v>
+        <v>0.138837</v>
       </c>
       <c r="E40" t="n">
-        <v>4087486935</v>
+        <v>3698253250</v>
       </c>
       <c r="F40" t="n">
-        <v>124480744</v>
+        <v>41159725</v>
       </c>
       <c r="G40" t="n">
-        <v>1.0794</v>
+        <v>-4.25631</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Pepe</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>8.54e-06</v>
+        <v>3.57</v>
       </c>
       <c r="E41" t="n">
-        <v>3605453006</v>
+        <v>3601601450</v>
       </c>
       <c r="F41" t="n">
-        <v>1262647504</v>
+        <v>370424275</v>
       </c>
       <c r="G41" t="n">
-        <v>-2.15797</v>
+        <v>-4.43856</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>Pepe</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>40.59</v>
+        <v>7.61e-06</v>
       </c>
       <c r="E42" t="n">
-        <v>3593120848</v>
+        <v>3214387150</v>
       </c>
       <c r="F42" t="n">
-        <v>156925788</v>
+        <v>1696661353</v>
       </c>
       <c r="G42" t="n">
-        <v>-1.94281</v>
+        <v>-5.37792</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.04839979</v>
+        <v>0.133093</v>
       </c>
       <c r="E43" t="n">
-        <v>3520741472</v>
+        <v>3071534914</v>
       </c>
       <c r="F43" t="n">
-        <v>136526334</v>
+        <v>68019190</v>
       </c>
       <c r="G43" t="n">
-        <v>-0.35568</v>
+        <v>-2.40645</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1.062</v>
+        <v>0.04129212</v>
       </c>
       <c r="E44" t="n">
-        <v>3433028163</v>
+        <v>3010039080</v>
       </c>
       <c r="F44" t="n">
-        <v>218531795</v>
+        <v>131567142</v>
       </c>
       <c r="G44" t="n">
-        <v>2.19989</v>
+        <v>-5.54854</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>FDUSD</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>First Digital USD</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.149773</v>
+        <v>0.992972</v>
       </c>
       <c r="E45" t="n">
-        <v>3428401596</v>
+        <v>2998597438</v>
       </c>
       <c r="F45" t="n">
-        <v>83972213</v>
+        <v>14657445902</v>
       </c>
       <c r="G45" t="n">
-        <v>2.575</v>
+        <v>-0.77877</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>FDUSD</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>First Digital USD</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>1.003</v>
+        <v>3221.46</v>
       </c>
       <c r="E46" t="n">
-        <v>3303587057</v>
+        <v>2974708156</v>
       </c>
       <c r="F46" t="n">
-        <v>9401755959</v>
+        <v>353552149</v>
       </c>
       <c r="G46" t="n">
-        <v>-0.06571</v>
+        <v>12.16911</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>THETA</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Theta Network</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>2.1</v>
+        <v>2.95</v>
       </c>
       <c r="E47" t="n">
-        <v>3042844804</v>
+        <v>2953977853</v>
       </c>
       <c r="F47" t="n">
-        <v>520026168</v>
+        <v>98078283</v>
       </c>
       <c r="G47" t="n">
-        <v>-1.68752</v>
+        <v>-0.4347</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>THETA</t>
+          <t>FET</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Theta Network</t>
+          <t>Fetch.ai</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>3.01</v>
+        <v>2.7</v>
       </c>
       <c r="E48" t="n">
-        <v>3012862586</v>
+        <v>2824030564</v>
       </c>
       <c r="F48" t="n">
-        <v>72720603</v>
+        <v>688189129</v>
       </c>
       <c r="G48" t="n">
-        <v>-3.78113</v>
+        <v>3.89427</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>3.34</v>
+        <v>0.84972</v>
       </c>
       <c r="E49" t="n">
-        <v>2977986124</v>
+        <v>2750073339</v>
       </c>
       <c r="F49" t="n">
-        <v>82529926</v>
+        <v>381630426</v>
       </c>
       <c r="G49" t="n">
-        <v>-1.67793</v>
+        <v>-1.72282</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>FET</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Fetch.ai</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>2.81</v>
+        <v>142.51</v>
       </c>
       <c r="E50" t="n">
-        <v>2937498258</v>
+        <v>2592686166</v>
       </c>
       <c r="F50" t="n">
-        <v>627542252</v>
+        <v>41985615</v>
       </c>
       <c r="G50" t="n">
-        <v>-2.79714</v>
+        <v>-1.85836</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>TIA</t>
+          <t>RUNE</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Celestia</t>
+          <t>THORChain</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>16.46</v>
+        <v>8.58</v>
       </c>
       <c r="E51" t="n">
-        <v>2789998305</v>
+        <v>2579222805</v>
       </c>
       <c r="F51" t="n">
-        <v>135259188</v>
+        <v>705667367</v>
       </c>
       <c r="G51" t="n">
-        <v>-4.48562</v>
+        <v>-5.75554</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-03-24
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>66767</v>
+        <v>65481</v>
       </c>
       <c r="E2" t="n">
-        <v>1317540462031</v>
+        <v>1283567562392</v>
       </c>
       <c r="F2" t="n">
-        <v>58370774815</v>
+        <v>24328168575</v>
       </c>
       <c r="G2" t="n">
-        <v>-2.30488</v>
+        <v>1.19805</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3570.76</v>
+        <v>3395.01</v>
       </c>
       <c r="E3" t="n">
-        <v>429377428195</v>
+        <v>406561616932</v>
       </c>
       <c r="F3" t="n">
-        <v>26843432307</v>
+        <v>13058337011</v>
       </c>
       <c r="G3" t="n">
-        <v>-3.69067</v>
+        <v>0.7223000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.996949</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>103211906265</v>
+        <v>103968330210</v>
       </c>
       <c r="F4" t="n">
-        <v>73693896831</v>
+        <v>43973686919</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.56706</v>
+        <v>-0.10875</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>570.55</v>
+        <v>558.98</v>
       </c>
       <c r="E5" t="n">
-        <v>88100504532</v>
+        <v>85768973301</v>
       </c>
       <c r="F5" t="n">
-        <v>4885730188</v>
+        <v>1320270956</v>
       </c>
       <c r="G5" t="n">
-        <v>-5.72398</v>
+        <v>0.65806</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>191.34</v>
+        <v>175.55</v>
       </c>
       <c r="E6" t="n">
-        <v>85203844660</v>
+        <v>77732934639</v>
       </c>
       <c r="F6" t="n">
-        <v>12598405929</v>
+        <v>2723617530</v>
       </c>
       <c r="G6" t="n">
-        <v>0.129</v>
+        <v>-0.43472</v>
       </c>
     </row>
     <row r="7">
@@ -611,25 +611,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>STETH</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Lido Staked Ether</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3567.87</v>
+        <v>0.630345</v>
       </c>
       <c r="E7" t="n">
-        <v>34946620795</v>
+        <v>34543249122</v>
       </c>
       <c r="F7" t="n">
-        <v>76002939</v>
+        <v>1206989490</v>
       </c>
       <c r="G7" t="n">
-        <v>-3.50899</v>
+        <v>1.70655</v>
       </c>
     </row>
     <row r="8">
@@ -638,25 +638,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>STETH</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>Lido Staked Ether</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.613313</v>
+        <v>3385.43</v>
       </c>
       <c r="E8" t="n">
-        <v>33627532063</v>
+        <v>33009276406</v>
       </c>
       <c r="F8" t="n">
-        <v>2418528876</v>
+        <v>81706432</v>
       </c>
       <c r="G8" t="n">
-        <v>-2.48676</v>
+        <v>0.59617</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.998122</v>
+        <v>1.002</v>
       </c>
       <c r="E9" t="n">
-        <v>30780165989</v>
+        <v>32020837400</v>
       </c>
       <c r="F9" t="n">
-        <v>11918839584</v>
+        <v>4767864913</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.15399</v>
+        <v>0.0804</v>
       </c>
     </row>
     <row r="10">
@@ -692,25 +692,25 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ADA</t>
+          <t>DOGE</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Cardano</t>
+          <t>Dogecoin</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.676299</v>
+        <v>0.173545</v>
       </c>
       <c r="E10" t="n">
-        <v>23921770520</v>
+        <v>24826396055</v>
       </c>
       <c r="F10" t="n">
-        <v>1068617556</v>
+        <v>3077442030</v>
       </c>
       <c r="G10" t="n">
-        <v>-5.60821</v>
+        <v>5.36736</v>
       </c>
     </row>
     <row r="11">
@@ -719,25 +719,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>DOGE</t>
+          <t>ADA</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Dogecoin</t>
+          <t>Cardano</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.148312</v>
+        <v>0.637866</v>
       </c>
       <c r="E11" t="n">
-        <v>21340672957</v>
+        <v>22431295701</v>
       </c>
       <c r="F11" t="n">
-        <v>3020361808</v>
+        <v>377102053</v>
       </c>
       <c r="G11" t="n">
-        <v>-5.39815</v>
+        <v>1.1198</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>55.83</v>
+        <v>53.8</v>
       </c>
       <c r="E12" t="n">
-        <v>21173856921</v>
+        <v>20236798790</v>
       </c>
       <c r="F12" t="n">
-        <v>1990840741</v>
+        <v>560032838</v>
       </c>
       <c r="G12" t="n">
-        <v>-4.93622</v>
+        <v>-2.11694</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2.68e-05</v>
+        <v>4.88</v>
       </c>
       <c r="E13" t="n">
-        <v>15854269859</v>
+        <v>16895169186</v>
       </c>
       <c r="F13" t="n">
-        <v>2344238830</v>
+        <v>387009199</v>
       </c>
       <c r="G13" t="n">
-        <v>-4.63066</v>
+        <v>1.43286</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>9.83</v>
+        <v>2.804e-05</v>
       </c>
       <c r="E14" t="n">
-        <v>13214172041</v>
+        <v>16481980673</v>
       </c>
       <c r="F14" t="n">
-        <v>583278730</v>
+        <v>1005766188</v>
       </c>
       <c r="G14" t="n">
-        <v>-4.83464</v>
+        <v>1.61418</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>3.62</v>
+        <v>9.210000000000001</v>
       </c>
       <c r="E15" t="n">
-        <v>12591205708</v>
+        <v>12362496107</v>
       </c>
       <c r="F15" t="n">
-        <v>105687801</v>
+        <v>175461629</v>
       </c>
       <c r="G15" t="n">
-        <v>-2.64036</v>
+        <v>1.18725</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.124773</v>
+        <v>18.35</v>
       </c>
       <c r="E16" t="n">
-        <v>10968818908</v>
+        <v>10753840142</v>
       </c>
       <c r="F16" t="n">
-        <v>515129095</v>
+        <v>280987063</v>
       </c>
       <c r="G16" t="n">
-        <v>-1.81144</v>
+        <v>-0.00202</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>18.24</v>
+        <v>0.119023</v>
       </c>
       <c r="E17" t="n">
-        <v>10771861912</v>
+        <v>10422556868</v>
       </c>
       <c r="F17" t="n">
-        <v>794227424</v>
+        <v>389083919</v>
       </c>
       <c r="G17" t="n">
-        <v>-5.41016</v>
+        <v>0.73532</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>66936</v>
+        <v>65408</v>
       </c>
       <c r="E18" t="n">
-        <v>10399368080</v>
+        <v>10144753249</v>
       </c>
       <c r="F18" t="n">
-        <v>418936379</v>
+        <v>193352995</v>
       </c>
       <c r="G18" t="n">
-        <v>-1.8624</v>
+        <v>1.42038</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1.059</v>
+        <v>1.002</v>
       </c>
       <c r="E19" t="n">
-        <v>9863606995</v>
+        <v>9284027628</v>
       </c>
       <c r="F19" t="n">
-        <v>892614640</v>
+        <v>290446146</v>
       </c>
       <c r="G19" t="n">
-        <v>-7.02731</v>
+        <v>1.6188</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>12.12</v>
+        <v>463.21</v>
       </c>
       <c r="E20" t="n">
-        <v>9147147043</v>
+        <v>9109806871</v>
       </c>
       <c r="F20" t="n">
-        <v>267528590</v>
+        <v>668722181</v>
       </c>
       <c r="G20" t="n">
-        <v>-4.67625</v>
+        <v>0.0153</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>7.76</v>
+        <v>11.87</v>
       </c>
       <c r="E21" t="n">
-        <v>8051637249</v>
+        <v>8936120460</v>
       </c>
       <c r="F21" t="n">
-        <v>1068358670</v>
+        <v>120044407</v>
       </c>
       <c r="G21" t="n">
-        <v>1.00923</v>
+        <v>0.00101</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>399.14</v>
+        <v>6.56</v>
       </c>
       <c r="E22" t="n">
-        <v>7877840183</v>
+        <v>6796340442</v>
       </c>
       <c r="F22" t="n">
-        <v>593591227</v>
+        <v>283000619</v>
       </c>
       <c r="G22" t="n">
-        <v>-1.49163</v>
+        <v>-1.87724</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>85.81999999999999</v>
+        <v>16.66</v>
       </c>
       <c r="E23" t="n">
-        <v>6388271232</v>
+        <v>6600529255</v>
       </c>
       <c r="F23" t="n">
-        <v>720251547</v>
+        <v>260320284</v>
       </c>
       <c r="G23" t="n">
-        <v>-4.07834</v>
+        <v>5.03464</v>
       </c>
     </row>
     <row r="24">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>12.42</v>
+        <v>14.13</v>
       </c>
       <c r="E24" t="n">
-        <v>5737850176</v>
+        <v>6532590555</v>
       </c>
       <c r="F24" t="n">
-        <v>211363273</v>
+        <v>246137727</v>
       </c>
       <c r="G24" t="n">
-        <v>-3.12471</v>
+        <v>5.68605</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>6.03</v>
+        <v>87.91</v>
       </c>
       <c r="E25" t="n">
-        <v>5600043458</v>
+        <v>6525933928</v>
       </c>
       <c r="F25" t="n">
-        <v>3610533</v>
+        <v>539907098</v>
       </c>
       <c r="G25" t="n">
-        <v>0.06342</v>
+        <v>1.82594</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>14.08</v>
+        <v>5.96</v>
       </c>
       <c r="E26" t="n">
-        <v>5594377088</v>
+        <v>5584840656</v>
       </c>
       <c r="F26" t="n">
-        <v>534345126</v>
+        <v>1905622</v>
       </c>
       <c r="G26" t="n">
-        <v>-5.66227</v>
+        <v>-1.84799</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>12.1</v>
+        <v>3.64</v>
       </c>
       <c r="E27" t="n">
-        <v>4740189264</v>
+        <v>5269367761</v>
       </c>
       <c r="F27" t="n">
-        <v>368432907</v>
+        <v>150831143</v>
       </c>
       <c r="G27" t="n">
-        <v>-3.69979</v>
+        <v>4.59577</v>
       </c>
     </row>
     <row r="28">
@@ -1187,16 +1187,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.998034</v>
+        <v>1</v>
       </c>
       <c r="E28" t="n">
-        <v>4683938253</v>
+        <v>4898246257</v>
       </c>
       <c r="F28" t="n">
-        <v>768256322</v>
+        <v>632392419</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.11995</v>
+        <v>0.18825</v>
       </c>
     </row>
     <row r="29">
@@ -1214,16 +1214,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>8.890000000000001</v>
+        <v>8.75</v>
       </c>
       <c r="E29" t="n">
-        <v>4679781583</v>
+        <v>4601269851</v>
       </c>
       <c r="F29" t="n">
-        <v>527310065</v>
+        <v>206302815</v>
       </c>
       <c r="G29" t="n">
-        <v>-6.51051</v>
+        <v>-0.25763</v>
       </c>
     </row>
     <row r="30">
@@ -1241,16 +1241,16 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>31.07</v>
+        <v>31.19</v>
       </c>
       <c r="E30" t="n">
-        <v>4544696452</v>
+        <v>4544586158</v>
       </c>
       <c r="F30" t="n">
-        <v>312339699</v>
+        <v>206777211</v>
       </c>
       <c r="G30" t="n">
-        <v>-3.89611</v>
+        <v>3.34493</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>11.57</v>
+        <v>11.5</v>
       </c>
       <c r="E31" t="n">
-        <v>4414049385</v>
+        <v>4482624843</v>
       </c>
       <c r="F31" t="n">
-        <v>665371836</v>
+        <v>125783806</v>
       </c>
       <c r="G31" t="n">
-        <v>-1.45818</v>
+        <v>-0.06662999999999999</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>638.78</v>
+        <v>1.66</v>
       </c>
       <c r="E32" t="n">
-        <v>4118602027</v>
+        <v>4391227721</v>
       </c>
       <c r="F32" t="n">
-        <v>31884705</v>
+        <v>332932527</v>
       </c>
       <c r="G32" t="n">
-        <v>2.74366</v>
+        <v>2.76237</v>
       </c>
     </row>
     <row r="33">
@@ -1322,16 +1322,16 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>2.91</v>
+        <v>2.9</v>
       </c>
       <c r="E33" t="n">
-        <v>4052562347</v>
+        <v>4119167987</v>
       </c>
       <c r="F33" t="n">
-        <v>106967040</v>
+        <v>60584400</v>
       </c>
       <c r="G33" t="n">
-        <v>-3.60499</v>
+        <v>2.18426</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>2.72</v>
+        <v>10.72</v>
       </c>
       <c r="E34" t="n">
-        <v>3938353274</v>
+        <v>4085042563</v>
       </c>
       <c r="F34" t="n">
-        <v>128412337</v>
+        <v>144292582</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.45104</v>
+        <v>-1.78188</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.113801</v>
+        <v>0.133973</v>
       </c>
       <c r="E35" t="n">
-        <v>3838591906</v>
+        <v>3839965345</v>
       </c>
       <c r="F35" t="n">
-        <v>99590958</v>
+        <v>78114191</v>
       </c>
       <c r="G35" t="n">
-        <v>-5.03746</v>
+        <v>2.32075</v>
       </c>
     </row>
     <row r="36">
@@ -1403,16 +1403,16 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>63.85</v>
+        <v>63.53</v>
       </c>
       <c r="E36" t="n">
-        <v>3832538080</v>
+        <v>3802093724</v>
       </c>
       <c r="F36" t="n">
-        <v>27764541</v>
+        <v>16424845</v>
       </c>
       <c r="G36" t="n">
-        <v>-5.51109</v>
+        <v>7.32737</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.399825</v>
+        <v>581.2</v>
       </c>
       <c r="E37" t="n">
-        <v>3770222674</v>
+        <v>3753773682</v>
       </c>
       <c r="F37" t="n">
-        <v>269482757</v>
+        <v>18636199</v>
       </c>
       <c r="G37" t="n">
-        <v>-1.59098</v>
+        <v>-0.0633</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>42.03</v>
+        <v>3.69</v>
       </c>
       <c r="E38" t="n">
-        <v>3720439441</v>
+        <v>3707640826</v>
       </c>
       <c r="F38" t="n">
-        <v>366997991</v>
+        <v>268843205</v>
       </c>
       <c r="G38" t="n">
-        <v>-9.737579999999999</v>
+        <v>7.67278</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.129542</v>
+        <v>0.139415</v>
       </c>
       <c r="E39" t="n">
-        <v>3716780240</v>
+        <v>3697585402</v>
       </c>
       <c r="F39" t="n">
-        <v>172822366</v>
+        <v>21707973</v>
       </c>
       <c r="G39" t="n">
-        <v>-6.21046</v>
+        <v>0.5129</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.138837</v>
+        <v>0.108016</v>
       </c>
       <c r="E40" t="n">
-        <v>3698253250</v>
+        <v>3631863698</v>
       </c>
       <c r="F40" t="n">
-        <v>41159725</v>
+        <v>39545337</v>
       </c>
       <c r="G40" t="n">
-        <v>-4.25631</v>
+        <v>-0.3276</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>3.57</v>
+        <v>0.373521</v>
       </c>
       <c r="E41" t="n">
-        <v>3601601450</v>
+        <v>3521474857</v>
       </c>
       <c r="F41" t="n">
-        <v>370424275</v>
+        <v>114109920</v>
       </c>
       <c r="G41" t="n">
-        <v>-4.43856</v>
+        <v>0.16339</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Pepe</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>7.61e-06</v>
+        <v>0.142686</v>
       </c>
       <c r="E42" t="n">
-        <v>3214387150</v>
+        <v>3285669211</v>
       </c>
       <c r="F42" t="n">
-        <v>1696661353</v>
+        <v>39935998</v>
       </c>
       <c r="G42" t="n">
-        <v>-5.37792</v>
+        <v>1.56118</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.133093</v>
+        <v>35.85</v>
       </c>
       <c r="E43" t="n">
-        <v>3071534914</v>
+        <v>3160342284</v>
       </c>
       <c r="F43" t="n">
-        <v>68019190</v>
+        <v>81952955</v>
       </c>
       <c r="G43" t="n">
-        <v>-2.40645</v>
+        <v>-0.07027</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Pepe</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.04129212</v>
+        <v>7.45e-06</v>
       </c>
       <c r="E44" t="n">
-        <v>3010039080</v>
+        <v>3125220704</v>
       </c>
       <c r="F44" t="n">
-        <v>131567142</v>
+        <v>519655834</v>
       </c>
       <c r="G44" t="n">
-        <v>-5.54854</v>
+        <v>-1.89398</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>FDUSD</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>First Digital USD</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.992972</v>
+        <v>0.04194042</v>
       </c>
       <c r="E45" t="n">
-        <v>2998597438</v>
+        <v>3038933294</v>
       </c>
       <c r="F45" t="n">
-        <v>14657445902</v>
+        <v>56060210</v>
       </c>
       <c r="G45" t="n">
-        <v>-0.77877</v>
+        <v>1.66337</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>FTM</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Fantom</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>3221.46</v>
+        <v>1.064</v>
       </c>
       <c r="E46" t="n">
-        <v>2974708156</v>
+        <v>2948186270</v>
       </c>
       <c r="F46" t="n">
-        <v>353552149</v>
+        <v>315967790</v>
       </c>
       <c r="G46" t="n">
-        <v>12.16911</v>
+        <v>-3.46246</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>THETA</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Theta Network</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>2.95</v>
+        <v>3099.58</v>
       </c>
       <c r="E47" t="n">
-        <v>2953977853</v>
+        <v>2858305401</v>
       </c>
       <c r="F47" t="n">
-        <v>98078283</v>
+        <v>90077218</v>
       </c>
       <c r="G47" t="n">
-        <v>-0.4347</v>
+        <v>-0.38831</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>FET</t>
+          <t>RUNE</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Fetch.ai</t>
+          <t>THORChain</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>2.7</v>
+        <v>8.369999999999999</v>
       </c>
       <c r="E48" t="n">
-        <v>2824030564</v>
+        <v>2803228850</v>
       </c>
       <c r="F48" t="n">
-        <v>688189129</v>
+        <v>359728074</v>
       </c>
       <c r="G48" t="n">
-        <v>3.89427</v>
+        <v>-0.0606</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>THETA</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Theta Network</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.84972</v>
+        <v>2.78</v>
       </c>
       <c r="E49" t="n">
-        <v>2750073339</v>
+        <v>2775639607</v>
       </c>
       <c r="F49" t="n">
-        <v>381630426</v>
+        <v>43253969</v>
       </c>
       <c r="G49" t="n">
-        <v>-1.72282</v>
+        <v>-0.76181</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>142.51</v>
+        <v>3.05</v>
       </c>
       <c r="E50" t="n">
-        <v>2592686166</v>
+        <v>2680421105</v>
       </c>
       <c r="F50" t="n">
-        <v>41985615</v>
+        <v>112328792</v>
       </c>
       <c r="G50" t="n">
-        <v>-1.85836</v>
+        <v>7.22221</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>RUNE</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>THORChain</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>8.58</v>
+        <v>0.825675</v>
       </c>
       <c r="E51" t="n">
-        <v>2579222805</v>
+        <v>2668958705</v>
       </c>
       <c r="F51" t="n">
-        <v>705667367</v>
+        <v>133150251</v>
       </c>
       <c r="G51" t="n">
-        <v>-5.75554</v>
+        <v>0.38305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-03-31
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>65481</v>
+        <v>70538</v>
       </c>
       <c r="E2" t="n">
-        <v>1283567562392</v>
+        <v>1386381840795</v>
       </c>
       <c r="F2" t="n">
-        <v>24328168575</v>
+        <v>17271056717</v>
       </c>
       <c r="G2" t="n">
-        <v>1.19805</v>
+        <v>0.45358</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3395.01</v>
+        <v>3618.96</v>
       </c>
       <c r="E3" t="n">
-        <v>406561616932</v>
+        <v>434252004740</v>
       </c>
       <c r="F3" t="n">
-        <v>13058337011</v>
+        <v>10797253507</v>
       </c>
       <c r="G3" t="n">
-        <v>0.7223000000000001</v>
+        <v>1.67228</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>1.001</v>
       </c>
       <c r="E4" t="n">
-        <v>103968330210</v>
+        <v>104525426959</v>
       </c>
       <c r="F4" t="n">
-        <v>43973686919</v>
+        <v>35083851689</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.10875</v>
+        <v>0.06415999999999999</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>558.98</v>
+        <v>606.34</v>
       </c>
       <c r="E5" t="n">
-        <v>85768973301</v>
+        <v>93283807208</v>
       </c>
       <c r="F5" t="n">
-        <v>1320270956</v>
+        <v>1111850257</v>
       </c>
       <c r="G5" t="n">
-        <v>0.65806</v>
+        <v>0.18988</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>175.55</v>
+        <v>196.5</v>
       </c>
       <c r="E6" t="n">
-        <v>77732934639</v>
+        <v>87275375056</v>
       </c>
       <c r="F6" t="n">
-        <v>2723617530</v>
+        <v>2264556372</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.43472</v>
+        <v>-0.70403</v>
       </c>
     </row>
     <row r="7">
@@ -611,25 +611,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>STETH</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>Lido Staked Ether</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.630345</v>
+        <v>3604.15</v>
       </c>
       <c r="E7" t="n">
-        <v>34543249122</v>
+        <v>34934850880</v>
       </c>
       <c r="F7" t="n">
-        <v>1206989490</v>
+        <v>57655138</v>
       </c>
       <c r="G7" t="n">
-        <v>1.70655</v>
+        <v>1.56875</v>
       </c>
     </row>
     <row r="8">
@@ -638,25 +638,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>STETH</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Lido Staked Ether</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>3385.43</v>
+        <v>0.627454</v>
       </c>
       <c r="E8" t="n">
-        <v>33009276406</v>
+        <v>34469586410</v>
       </c>
       <c r="F8" t="n">
-        <v>81706432</v>
+        <v>930402392</v>
       </c>
       <c r="G8" t="n">
-        <v>0.59617</v>
+        <v>-0.05828</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1.002</v>
+        <v>1.001</v>
       </c>
       <c r="E9" t="n">
-        <v>32020837400</v>
+        <v>32462239140</v>
       </c>
       <c r="F9" t="n">
-        <v>4767864913</v>
+        <v>4824260731</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0804</v>
+        <v>0.10131</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.173545</v>
+        <v>0.207424</v>
       </c>
       <c r="E10" t="n">
-        <v>24826396055</v>
+        <v>29797893772</v>
       </c>
       <c r="F10" t="n">
-        <v>3077442030</v>
+        <v>2295994232</v>
       </c>
       <c r="G10" t="n">
-        <v>5.36736</v>
+        <v>-1.51399</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.637866</v>
+        <v>0.647124</v>
       </c>
       <c r="E11" t="n">
-        <v>22431295701</v>
+        <v>22825795620</v>
       </c>
       <c r="F11" t="n">
-        <v>377102053</v>
+        <v>325283919</v>
       </c>
       <c r="G11" t="n">
-        <v>1.1198</v>
+        <v>-1.52699</v>
       </c>
     </row>
     <row r="12">
@@ -758,13 +758,13 @@
         <v>53.8</v>
       </c>
       <c r="E12" t="n">
-        <v>20236798790</v>
+        <v>20299942121</v>
       </c>
       <c r="F12" t="n">
-        <v>560032838</v>
+        <v>307394853</v>
       </c>
       <c r="G12" t="n">
-        <v>-2.11694</v>
+        <v>-0.91729</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>4.88</v>
+        <v>5.17</v>
       </c>
       <c r="E13" t="n">
-        <v>16895169186</v>
+        <v>17951052549</v>
       </c>
       <c r="F13" t="n">
-        <v>387009199</v>
+        <v>139606248</v>
       </c>
       <c r="G13" t="n">
-        <v>1.43286</v>
+        <v>-1.82854</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2.804e-05</v>
+        <v>3.042e-05</v>
       </c>
       <c r="E14" t="n">
-        <v>16481980673</v>
+        <v>17925156777</v>
       </c>
       <c r="F14" t="n">
-        <v>1005766188</v>
+        <v>513582872</v>
       </c>
       <c r="G14" t="n">
-        <v>1.61418</v>
+        <v>-0.1436</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>9.210000000000001</v>
+        <v>9.58</v>
       </c>
       <c r="E15" t="n">
-        <v>12362496107</v>
+        <v>12894315849</v>
       </c>
       <c r="F15" t="n">
-        <v>175461629</v>
+        <v>155410442</v>
       </c>
       <c r="G15" t="n">
-        <v>1.18725</v>
+        <v>-0.13951</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>18.35</v>
+        <v>595.89</v>
       </c>
       <c r="E16" t="n">
-        <v>10753840142</v>
+        <v>11738234482</v>
       </c>
       <c r="F16" t="n">
-        <v>280987063</v>
+        <v>399114506</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.00202</v>
+        <v>-1.297</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.119023</v>
+        <v>19.05</v>
       </c>
       <c r="E17" t="n">
-        <v>10422556868</v>
+        <v>11183126975</v>
       </c>
       <c r="F17" t="n">
-        <v>389083919</v>
+        <v>362435030</v>
       </c>
       <c r="G17" t="n">
-        <v>0.73532</v>
+        <v>-0.70952</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>65408</v>
+        <v>70564</v>
       </c>
       <c r="E18" t="n">
-        <v>10144753249</v>
+        <v>10956756486</v>
       </c>
       <c r="F18" t="n">
-        <v>193352995</v>
+        <v>183297402</v>
       </c>
       <c r="G18" t="n">
-        <v>1.42038</v>
+        <v>0.44085</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1.002</v>
+        <v>0.122627</v>
       </c>
       <c r="E19" t="n">
-        <v>9284027628</v>
+        <v>10756666177</v>
       </c>
       <c r="F19" t="n">
-        <v>290446146</v>
+        <v>270646828</v>
       </c>
       <c r="G19" t="n">
-        <v>1.6188</v>
+        <v>1.43874</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>463.21</v>
+        <v>13.05</v>
       </c>
       <c r="E20" t="n">
-        <v>9109806871</v>
+        <v>9835281890</v>
       </c>
       <c r="F20" t="n">
-        <v>668722181</v>
+        <v>183951923</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0153</v>
+        <v>2.52941</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>11.87</v>
+        <v>0.998556</v>
       </c>
       <c r="E21" t="n">
-        <v>8936120460</v>
+        <v>9268098271</v>
       </c>
       <c r="F21" t="n">
-        <v>120044407</v>
+        <v>209388759</v>
       </c>
       <c r="G21" t="n">
-        <v>0.00101</v>
+        <v>-0.20482</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>6.56</v>
+        <v>17.83</v>
       </c>
       <c r="E22" t="n">
-        <v>6796340442</v>
+        <v>8242140330</v>
       </c>
       <c r="F22" t="n">
-        <v>283000619</v>
+        <v>227796927</v>
       </c>
       <c r="G22" t="n">
-        <v>-1.87724</v>
+        <v>-1.24331</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>16.66</v>
+        <v>102.27</v>
       </c>
       <c r="E23" t="n">
-        <v>6600529255</v>
+        <v>7612536539</v>
       </c>
       <c r="F23" t="n">
-        <v>260320284</v>
+        <v>588154818</v>
       </c>
       <c r="G23" t="n">
-        <v>5.03464</v>
+        <v>-1.25229</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>14.13</v>
+        <v>7.24</v>
       </c>
       <c r="E24" t="n">
-        <v>6532590555</v>
+        <v>7508174086</v>
       </c>
       <c r="F24" t="n">
-        <v>246137727</v>
+        <v>237992068</v>
       </c>
       <c r="G24" t="n">
-        <v>5.68605</v>
+        <v>1.01461</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>87.91</v>
+        <v>16.48</v>
       </c>
       <c r="E25" t="n">
-        <v>6525933928</v>
+        <v>6543760031</v>
       </c>
       <c r="F25" t="n">
-        <v>539907098</v>
+        <v>143729890</v>
       </c>
       <c r="G25" t="n">
-        <v>1.82594</v>
+        <v>-3.09986</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>5.96</v>
+        <v>5.97</v>
       </c>
       <c r="E26" t="n">
-        <v>5584840656</v>
+        <v>5529214162</v>
       </c>
       <c r="F26" t="n">
-        <v>1905622</v>
+        <v>1824745</v>
       </c>
       <c r="G26" t="n">
-        <v>-1.84799</v>
+        <v>-1.8902</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>3.64</v>
+        <v>3.53</v>
       </c>
       <c r="E27" t="n">
-        <v>5269367761</v>
+        <v>5121062940</v>
       </c>
       <c r="F27" t="n">
-        <v>150831143</v>
+        <v>78707648</v>
       </c>
       <c r="G27" t="n">
-        <v>4.59577</v>
+        <v>-3.59425</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>1</v>
+        <v>9.640000000000001</v>
       </c>
       <c r="E28" t="n">
-        <v>4898246257</v>
+        <v>5115347533</v>
       </c>
       <c r="F28" t="n">
-        <v>632392419</v>
+        <v>206539209</v>
       </c>
       <c r="G28" t="n">
-        <v>0.18825</v>
+        <v>-0.71816</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>8.75</v>
+        <v>33.95</v>
       </c>
       <c r="E29" t="n">
-        <v>4601269851</v>
+        <v>4963592324</v>
       </c>
       <c r="F29" t="n">
-        <v>206302815</v>
+        <v>166387035</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.25763</v>
+        <v>0.35056</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>31.19</v>
+        <v>0.999179</v>
       </c>
       <c r="E30" t="n">
-        <v>4544586158</v>
+        <v>4911796100</v>
       </c>
       <c r="F30" t="n">
-        <v>206777211</v>
+        <v>238880024</v>
       </c>
       <c r="G30" t="n">
-        <v>3.34493</v>
+        <v>-0.02738</v>
       </c>
     </row>
     <row r="31">
@@ -1268,16 +1268,16 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>11.5</v>
+        <v>12.32</v>
       </c>
       <c r="E31" t="n">
-        <v>4482624843</v>
+        <v>4805672661</v>
       </c>
       <c r="F31" t="n">
-        <v>125783806</v>
+        <v>121828600</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.06662999999999999</v>
+        <v>-3.33235</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>WIF</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>dogwifhat</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>1.66</v>
+        <v>4.77</v>
       </c>
       <c r="E32" t="n">
-        <v>4391227721</v>
+        <v>4765035952</v>
       </c>
       <c r="F32" t="n">
-        <v>332932527</v>
+        <v>624374578</v>
       </c>
       <c r="G32" t="n">
-        <v>2.76237</v>
+        <v>5.37514</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>2.9</v>
+        <v>1.66</v>
       </c>
       <c r="E33" t="n">
-        <v>4119167987</v>
+        <v>4388618312</v>
       </c>
       <c r="F33" t="n">
-        <v>60584400</v>
+        <v>236675295</v>
       </c>
       <c r="G33" t="n">
-        <v>2.18426</v>
+        <v>-1.068</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>10.72</v>
+        <v>3.03</v>
       </c>
       <c r="E34" t="n">
-        <v>4085042563</v>
+        <v>4313282802</v>
       </c>
       <c r="F34" t="n">
-        <v>144292582</v>
+        <v>59049519</v>
       </c>
       <c r="G34" t="n">
-        <v>-1.78188</v>
+        <v>-3.17973</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.133973</v>
+        <v>1.31</v>
       </c>
       <c r="E35" t="n">
-        <v>3839965345</v>
+        <v>4246870182</v>
       </c>
       <c r="F35" t="n">
-        <v>78114191</v>
+        <v>143962000</v>
       </c>
       <c r="G35" t="n">
-        <v>2.32075</v>
+        <v>-0.27654</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>63.53</v>
+        <v>10.78</v>
       </c>
       <c r="E36" t="n">
-        <v>3802093724</v>
+        <v>4116422908</v>
       </c>
       <c r="F36" t="n">
-        <v>16424845</v>
+        <v>141029275</v>
       </c>
       <c r="G36" t="n">
-        <v>7.32737</v>
+        <v>-1.83882</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>581.2</v>
+        <v>0.152624</v>
       </c>
       <c r="E37" t="n">
-        <v>3753773682</v>
+        <v>4061305323</v>
       </c>
       <c r="F37" t="n">
-        <v>18636199</v>
+        <v>14683531</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.0633</v>
+        <v>-0.47143</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>3.69</v>
+        <v>0.140521</v>
       </c>
       <c r="E38" t="n">
-        <v>3707640826</v>
+        <v>4047702496</v>
       </c>
       <c r="F38" t="n">
-        <v>268843205</v>
+        <v>66304741</v>
       </c>
       <c r="G38" t="n">
-        <v>7.67278</v>
+        <v>0.03147</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.139415</v>
+        <v>0.117449</v>
       </c>
       <c r="E39" t="n">
-        <v>3697585402</v>
+        <v>3962373628</v>
       </c>
       <c r="F39" t="n">
-        <v>21707973</v>
+        <v>46647765</v>
       </c>
       <c r="G39" t="n">
-        <v>0.5129</v>
+        <v>1.05005</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Pepe</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.108016</v>
+        <v>9.02e-06</v>
       </c>
       <c r="E40" t="n">
-        <v>3631863698</v>
+        <v>3799832344</v>
       </c>
       <c r="F40" t="n">
-        <v>39545337</v>
+        <v>1146524984</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.3276</v>
+        <v>3.94063</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.373521</v>
+        <v>63.24</v>
       </c>
       <c r="E41" t="n">
-        <v>3521474857</v>
+        <v>3794180368</v>
       </c>
       <c r="F41" t="n">
-        <v>114109920</v>
+        <v>7304948</v>
       </c>
       <c r="G41" t="n">
-        <v>0.16339</v>
+        <v>-0.41365</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.142686</v>
+        <v>3.7</v>
       </c>
       <c r="E42" t="n">
-        <v>3285669211</v>
+        <v>3714672850</v>
       </c>
       <c r="F42" t="n">
-        <v>39935998</v>
+        <v>155775414</v>
       </c>
       <c r="G42" t="n">
-        <v>1.56118</v>
+        <v>-0.70314</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>35.85</v>
+        <v>0.39206</v>
       </c>
       <c r="E43" t="n">
-        <v>3160342284</v>
+        <v>3705636054</v>
       </c>
       <c r="F43" t="n">
-        <v>81952955</v>
+        <v>74328806</v>
       </c>
       <c r="G43" t="n">
-        <v>-0.07027</v>
+        <v>-1.19136</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Pepe</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>7.45e-06</v>
+        <v>3894.32</v>
       </c>
       <c r="E44" t="n">
-        <v>3125220704</v>
+        <v>3601277038</v>
       </c>
       <c r="F44" t="n">
-        <v>519655834</v>
+        <v>164010407</v>
       </c>
       <c r="G44" t="n">
-        <v>-1.89398</v>
+        <v>3.54241</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.04194042</v>
+        <v>538.8</v>
       </c>
       <c r="E45" t="n">
-        <v>3038933294</v>
+        <v>3496246783</v>
       </c>
       <c r="F45" t="n">
-        <v>56060210</v>
+        <v>58362788</v>
       </c>
       <c r="G45" t="n">
-        <v>1.66337</v>
+        <v>9.747629999999999</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>FTM</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Fantom</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>1.064</v>
+        <v>0.04554033</v>
       </c>
       <c r="E46" t="n">
-        <v>2948186270</v>
+        <v>3304719594</v>
       </c>
       <c r="F46" t="n">
-        <v>315967790</v>
+        <v>66237651</v>
       </c>
       <c r="G46" t="n">
-        <v>-3.46246</v>
+        <v>-0.51629</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>3099.58</v>
+        <v>37.01</v>
       </c>
       <c r="E47" t="n">
-        <v>2858305401</v>
+        <v>3272486357</v>
       </c>
       <c r="F47" t="n">
-        <v>90077218</v>
+        <v>95670313</v>
       </c>
       <c r="G47" t="n">
-        <v>-0.38831</v>
+        <v>0.00211</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>RUNE</t>
+          <t>FET</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>THORChain</t>
+          <t>Fetch.ai</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>8.369999999999999</v>
+        <v>3.12</v>
       </c>
       <c r="E48" t="n">
-        <v>2803228850</v>
+        <v>3252841533</v>
       </c>
       <c r="F48" t="n">
-        <v>359728074</v>
+        <v>404909325</v>
       </c>
       <c r="G48" t="n">
-        <v>-0.0606</v>
+        <v>0.69363</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>THETA</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Theta Network</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>2.78</v>
+        <v>0.133446</v>
       </c>
       <c r="E49" t="n">
-        <v>2775639607</v>
+        <v>3079428605</v>
       </c>
       <c r="F49" t="n">
-        <v>43253969</v>
+        <v>30092141</v>
       </c>
       <c r="G49" t="n">
-        <v>-0.76181</v>
+        <v>-1.64291</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>RUNE</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>THORChain</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>3.05</v>
+        <v>8.630000000000001</v>
       </c>
       <c r="E50" t="n">
-        <v>2680421105</v>
+        <v>2896186476</v>
       </c>
       <c r="F50" t="n">
-        <v>112328792</v>
+        <v>183133122</v>
       </c>
       <c r="G50" t="n">
-        <v>7.22221</v>
+        <v>-0.83719</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>THETA</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Theta Network</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.825675</v>
+        <v>2.88</v>
       </c>
       <c r="E51" t="n">
-        <v>2668958705</v>
+        <v>2873366488</v>
       </c>
       <c r="F51" t="n">
-        <v>133150251</v>
+        <v>29338379</v>
       </c>
       <c r="G51" t="n">
-        <v>0.38305</v>
+        <v>0.66028</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-04-07
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>70538</v>
+        <v>69306</v>
       </c>
       <c r="E2" t="n">
-        <v>1386381840795</v>
+        <v>1363932763074</v>
       </c>
       <c r="F2" t="n">
-        <v>17271056717</v>
+        <v>19008976614</v>
       </c>
       <c r="G2" t="n">
-        <v>0.45358</v>
+        <v>2.3426</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3618.96</v>
+        <v>3387.36</v>
       </c>
       <c r="E3" t="n">
-        <v>434252004740</v>
+        <v>406710446312</v>
       </c>
       <c r="F3" t="n">
-        <v>10797253507</v>
+        <v>8724892660</v>
       </c>
       <c r="G3" t="n">
-        <v>1.67228</v>
+        <v>1.62731</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1.001</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>104525426959</v>
+        <v>106875023058</v>
       </c>
       <c r="F4" t="n">
-        <v>35083851689</v>
+        <v>28937788824</v>
       </c>
       <c r="G4" t="n">
-        <v>0.06415999999999999</v>
+        <v>-0.05547</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>606.34</v>
+        <v>586.52</v>
       </c>
       <c r="E5" t="n">
-        <v>93283807208</v>
+        <v>90225732038</v>
       </c>
       <c r="F5" t="n">
-        <v>1111850257</v>
+        <v>696239279</v>
       </c>
       <c r="G5" t="n">
-        <v>0.18988</v>
+        <v>0.93176</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>196.5</v>
+        <v>180.46</v>
       </c>
       <c r="E6" t="n">
-        <v>87275375056</v>
+        <v>80447359878</v>
       </c>
       <c r="F6" t="n">
-        <v>2264556372</v>
+        <v>2243774447</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.70403</v>
+        <v>2.49275</v>
       </c>
     </row>
     <row r="7">
@@ -611,25 +611,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>STETH</t>
+          <t>USDC</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Lido Staked Ether</t>
+          <t>USDC</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3604.15</v>
+        <v>0.999366</v>
       </c>
       <c r="E7" t="n">
-        <v>34934850880</v>
+        <v>32910098254</v>
       </c>
       <c r="F7" t="n">
-        <v>57655138</v>
+        <v>3919859957</v>
       </c>
       <c r="G7" t="n">
-        <v>1.56875</v>
+        <v>-0.05639</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.627454</v>
+        <v>0.5969370000000001</v>
       </c>
       <c r="E8" t="n">
-        <v>34469586410</v>
+        <v>32859797063</v>
       </c>
       <c r="F8" t="n">
-        <v>930402392</v>
+        <v>806482083</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.05828</v>
+        <v>1.48356</v>
       </c>
     </row>
     <row r="9">
@@ -665,25 +665,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>USDC</t>
+          <t>STETH</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>USDC</t>
+          <t>Lido Staked Ether</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1.001</v>
+        <v>3381.62</v>
       </c>
       <c r="E9" t="n">
-        <v>32462239140</v>
+        <v>32239574756</v>
       </c>
       <c r="F9" t="n">
-        <v>4824260731</v>
+        <v>101616432</v>
       </c>
       <c r="G9" t="n">
-        <v>0.10131</v>
+        <v>1.64889</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.207424</v>
+        <v>0.197361</v>
       </c>
       <c r="E10" t="n">
-        <v>29797893772</v>
+        <v>28422027126</v>
       </c>
       <c r="F10" t="n">
-        <v>2295994232</v>
+        <v>2356790810</v>
       </c>
       <c r="G10" t="n">
-        <v>-1.51399</v>
+        <v>8.09686</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.647124</v>
+        <v>0.593552</v>
       </c>
       <c r="E11" t="n">
-        <v>22825795620</v>
+        <v>20938694026</v>
       </c>
       <c r="F11" t="n">
-        <v>325283919</v>
+        <v>257759748</v>
       </c>
       <c r="G11" t="n">
-        <v>-1.52699</v>
+        <v>2.28471</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +746,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>53.8</v>
+        <v>5.41</v>
       </c>
       <c r="E12" t="n">
-        <v>20299942121</v>
+        <v>18755291051</v>
       </c>
       <c r="F12" t="n">
-        <v>307394853</v>
+        <v>142795156</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.91729</v>
+        <v>-2.08733</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>5.17</v>
+        <v>48.5</v>
       </c>
       <c r="E13" t="n">
-        <v>17951052549</v>
+        <v>18332218378</v>
       </c>
       <c r="F13" t="n">
-        <v>139606248</v>
+        <v>492988753</v>
       </c>
       <c r="G13" t="n">
-        <v>-1.82854</v>
+        <v>3.38384</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>3.042e-05</v>
+        <v>2.834e-05</v>
       </c>
       <c r="E14" t="n">
-        <v>17925156777</v>
+        <v>16702587269</v>
       </c>
       <c r="F14" t="n">
-        <v>513582872</v>
+        <v>603249154</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.1436</v>
+        <v>4.26076</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>9.58</v>
+        <v>679.48</v>
       </c>
       <c r="E15" t="n">
-        <v>12894315849</v>
+        <v>13382133896</v>
       </c>
       <c r="F15" t="n">
-        <v>155410442</v>
+        <v>773957282</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.13951</v>
+        <v>-1.89252</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>595.89</v>
+        <v>8.66</v>
       </c>
       <c r="E16" t="n">
-        <v>11738234482</v>
+        <v>11684042795</v>
       </c>
       <c r="F16" t="n">
-        <v>399114506</v>
+        <v>169388464</v>
       </c>
       <c r="G16" t="n">
-        <v>-1.297</v>
+        <v>3.06631</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>19.05</v>
+        <v>69333</v>
       </c>
       <c r="E17" t="n">
-        <v>11183126975</v>
+        <v>10779832953</v>
       </c>
       <c r="F17" t="n">
-        <v>362435030</v>
+        <v>141651025</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.70952</v>
+        <v>2.34724</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>70564</v>
+        <v>0.120311</v>
       </c>
       <c r="E18" t="n">
-        <v>10956756486</v>
+        <v>10550006145</v>
       </c>
       <c r="F18" t="n">
-        <v>183297402</v>
+        <v>225653074</v>
       </c>
       <c r="G18" t="n">
-        <v>0.44085</v>
+        <v>1.46164</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.122627</v>
+        <v>17.73</v>
       </c>
       <c r="E19" t="n">
-        <v>10756666177</v>
+        <v>10411138585</v>
       </c>
       <c r="F19" t="n">
-        <v>270646828</v>
+        <v>230512399</v>
       </c>
       <c r="G19" t="n">
-        <v>1.43874</v>
+        <v>0.74143</v>
       </c>
     </row>
     <row r="20">
@@ -971,16 +971,16 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>13.05</v>
+        <v>11.32</v>
       </c>
       <c r="E20" t="n">
-        <v>9835281890</v>
+        <v>8520482254</v>
       </c>
       <c r="F20" t="n">
-        <v>183951923</v>
+        <v>157968113</v>
       </c>
       <c r="G20" t="n">
-        <v>2.52941</v>
+        <v>2.34232</v>
       </c>
     </row>
     <row r="21">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.998556</v>
+        <v>0.906156</v>
       </c>
       <c r="E21" t="n">
-        <v>9268098271</v>
+        <v>8413234951</v>
       </c>
       <c r="F21" t="n">
-        <v>209388759</v>
+        <v>221104999</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.20482</v>
+        <v>1.51905</v>
       </c>
     </row>
     <row r="22">
@@ -1025,16 +1025,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>17.83</v>
+        <v>17.2</v>
       </c>
       <c r="E22" t="n">
-        <v>8242140330</v>
+        <v>7955984665</v>
       </c>
       <c r="F22" t="n">
-        <v>227796927</v>
+        <v>121881233</v>
       </c>
       <c r="G22" t="n">
-        <v>-1.24331</v>
+        <v>1.8232</v>
       </c>
     </row>
     <row r="23">
@@ -1052,16 +1052,16 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>102.27</v>
+        <v>103.18</v>
       </c>
       <c r="E23" t="n">
-        <v>7612536539</v>
+        <v>7677385209</v>
       </c>
       <c r="F23" t="n">
-        <v>588154818</v>
+        <v>601614109</v>
       </c>
       <c r="G23" t="n">
-        <v>-1.25229</v>
+        <v>1.83649</v>
       </c>
     </row>
     <row r="24">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>7.24</v>
+        <v>6.95</v>
       </c>
       <c r="E24" t="n">
-        <v>7508174086</v>
+        <v>7360388208</v>
       </c>
       <c r="F24" t="n">
-        <v>237992068</v>
+        <v>367999243</v>
       </c>
       <c r="G24" t="n">
-        <v>1.01461</v>
+        <v>-1.5515</v>
       </c>
     </row>
     <row r="25">
@@ -1106,16 +1106,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>16.48</v>
+        <v>13.76</v>
       </c>
       <c r="E25" t="n">
-        <v>6543760031</v>
+        <v>5481145643</v>
       </c>
       <c r="F25" t="n">
-        <v>143729890</v>
+        <v>180712599</v>
       </c>
       <c r="G25" t="n">
-        <v>-3.09986</v>
+        <v>5.86007</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>5.97</v>
+        <v>5.78</v>
       </c>
       <c r="E26" t="n">
-        <v>5529214162</v>
+        <v>5350892072</v>
       </c>
       <c r="F26" t="n">
-        <v>1824745</v>
+        <v>1273179</v>
       </c>
       <c r="G26" t="n">
-        <v>-1.8902</v>
+        <v>0.23891</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>3.53</v>
+        <v>0.999645</v>
       </c>
       <c r="E27" t="n">
-        <v>5121062940</v>
+        <v>5106876172</v>
       </c>
       <c r="F27" t="n">
-        <v>78707648</v>
+        <v>646973416</v>
       </c>
       <c r="G27" t="n">
-        <v>-3.59425</v>
+        <v>-0.13723</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>9.640000000000001</v>
+        <v>33.86</v>
       </c>
       <c r="E28" t="n">
-        <v>5115347533</v>
+        <v>4960004530</v>
       </c>
       <c r="F28" t="n">
-        <v>206539209</v>
+        <v>206460816</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.71816</v>
+        <v>2.04751</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>33.95</v>
+        <v>3.27</v>
       </c>
       <c r="E29" t="n">
-        <v>4963592324</v>
+        <v>4752287769</v>
       </c>
       <c r="F29" t="n">
-        <v>166387035</v>
+        <v>57154795</v>
       </c>
       <c r="G29" t="n">
-        <v>0.35056</v>
+        <v>3.63692</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.999179</v>
+        <v>8.789999999999999</v>
       </c>
       <c r="E30" t="n">
-        <v>4911796100</v>
+        <v>4687935910</v>
       </c>
       <c r="F30" t="n">
-        <v>238880024</v>
+        <v>176177202</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.02738</v>
+        <v>2.88181</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>12.32</v>
+        <v>1.4</v>
       </c>
       <c r="E31" t="n">
-        <v>4805672661</v>
+        <v>4457565465</v>
       </c>
       <c r="F31" t="n">
-        <v>121828600</v>
+        <v>42694505</v>
       </c>
       <c r="G31" t="n">
-        <v>-3.33235</v>
+        <v>5.31252</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>WIF</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>dogwifhat</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>4.77</v>
+        <v>11.18</v>
       </c>
       <c r="E32" t="n">
-        <v>4765035952</v>
+        <v>4367259087</v>
       </c>
       <c r="F32" t="n">
-        <v>624374578</v>
+        <v>170447907</v>
       </c>
       <c r="G32" t="n">
-        <v>5.37514</v>
+        <v>1.56546</v>
       </c>
     </row>
     <row r="33">
@@ -1322,16 +1322,16 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>1.66</v>
+        <v>1.5</v>
       </c>
       <c r="E33" t="n">
-        <v>4388618312</v>
+        <v>3969519339</v>
       </c>
       <c r="F33" t="n">
-        <v>236675295</v>
+        <v>168585528</v>
       </c>
       <c r="G33" t="n">
-        <v>-1.068</v>
+        <v>0.7558</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>3.03</v>
+        <v>0.146419</v>
       </c>
       <c r="E34" t="n">
-        <v>4313282802</v>
+        <v>3899929131</v>
       </c>
       <c r="F34" t="n">
-        <v>59049519</v>
+        <v>10582675</v>
       </c>
       <c r="G34" t="n">
-        <v>-3.17973</v>
+        <v>2.32239</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1.31</v>
+        <v>2.73</v>
       </c>
       <c r="E35" t="n">
-        <v>4246870182</v>
+        <v>3881452208</v>
       </c>
       <c r="F35" t="n">
-        <v>143962000</v>
+        <v>24725941</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.27654</v>
+        <v>1.82722</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>10.78</v>
+        <v>0.130072</v>
       </c>
       <c r="E36" t="n">
-        <v>4116422908</v>
+        <v>3752192200</v>
       </c>
       <c r="F36" t="n">
-        <v>141029275</v>
+        <v>48970072</v>
       </c>
       <c r="G36" t="n">
-        <v>-1.83882</v>
+        <v>1.29402</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.152624</v>
+        <v>9.710000000000001</v>
       </c>
       <c r="E37" t="n">
-        <v>4061305323</v>
+        <v>3707584587</v>
       </c>
       <c r="F37" t="n">
-        <v>14683531</v>
+        <v>87759660</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.47143</v>
+        <v>3.11429</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.140521</v>
+        <v>556.42</v>
       </c>
       <c r="E38" t="n">
-        <v>4047702496</v>
+        <v>3648411660</v>
       </c>
       <c r="F38" t="n">
-        <v>66304741</v>
+        <v>13830418</v>
       </c>
       <c r="G38" t="n">
-        <v>0.03147</v>
+        <v>-2.52961</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>WIF</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>dogwifhat</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.117449</v>
+        <v>3.62</v>
       </c>
       <c r="E39" t="n">
-        <v>3962373628</v>
+        <v>3618850501</v>
       </c>
       <c r="F39" t="n">
-        <v>46647765</v>
+        <v>392057021</v>
       </c>
       <c r="G39" t="n">
-        <v>1.05005</v>
+        <v>10.73044</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Pepe</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>9.02e-06</v>
+        <v>0.106466</v>
       </c>
       <c r="E40" t="n">
-        <v>3799832344</v>
+        <v>3592627774</v>
       </c>
       <c r="F40" t="n">
-        <v>1146524984</v>
+        <v>25870450</v>
       </c>
       <c r="G40" t="n">
-        <v>3.94063</v>
+        <v>1.27874</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>FDUSD</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>First Digital USD</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>63.24</v>
+        <v>1.002</v>
       </c>
       <c r="E41" t="n">
-        <v>3794180368</v>
+        <v>3530854261</v>
       </c>
       <c r="F41" t="n">
-        <v>7304948</v>
+        <v>4366880686</v>
       </c>
       <c r="G41" t="n">
-        <v>-0.41365</v>
+        <v>0.02028</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>3.7</v>
+        <v>58.55</v>
       </c>
       <c r="E42" t="n">
-        <v>3714672850</v>
+        <v>3512831253</v>
       </c>
       <c r="F42" t="n">
-        <v>155775414</v>
+        <v>8389308</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.70314</v>
+        <v>2.09003</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.39206</v>
+        <v>3667.29</v>
       </c>
       <c r="E43" t="n">
-        <v>3705636054</v>
+        <v>3390829114</v>
       </c>
       <c r="F43" t="n">
-        <v>74328806</v>
+        <v>91315242</v>
       </c>
       <c r="G43" t="n">
-        <v>-1.19136</v>
+        <v>-1.07582</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>3894.32</v>
+        <v>0.139934</v>
       </c>
       <c r="E44" t="n">
-        <v>3601277038</v>
+        <v>3230871716</v>
       </c>
       <c r="F44" t="n">
-        <v>164010407</v>
+        <v>51320302</v>
       </c>
       <c r="G44" t="n">
-        <v>3.54241</v>
+        <v>5.4082</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>538.8</v>
+        <v>0.33975</v>
       </c>
       <c r="E45" t="n">
-        <v>3496246783</v>
+        <v>3215485222</v>
       </c>
       <c r="F45" t="n">
-        <v>58362788</v>
+        <v>74158652</v>
       </c>
       <c r="G45" t="n">
-        <v>9.747629999999999</v>
+        <v>1.61073</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.04554033</v>
+        <v>35.56</v>
       </c>
       <c r="E46" t="n">
-        <v>3304719594</v>
+        <v>3202455945</v>
       </c>
       <c r="F46" t="n">
-        <v>66237651</v>
+        <v>120757229</v>
       </c>
       <c r="G46" t="n">
-        <v>-0.51629</v>
+        <v>0.7668</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>37.01</v>
+        <v>0.04243749</v>
       </c>
       <c r="E47" t="n">
-        <v>3272486357</v>
+        <v>3085243824</v>
       </c>
       <c r="F47" t="n">
-        <v>95670313</v>
+        <v>53112420</v>
       </c>
       <c r="G47" t="n">
-        <v>0.00211</v>
+        <v>4.27306</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>FET</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Fetch.ai</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>3.12</v>
+        <v>3.06</v>
       </c>
       <c r="E48" t="n">
-        <v>3252841533</v>
+        <v>3078515086</v>
       </c>
       <c r="F48" t="n">
-        <v>404909325</v>
+        <v>156220264</v>
       </c>
       <c r="G48" t="n">
-        <v>0.69363</v>
+        <v>2.9313</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Pepe</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.133446</v>
+        <v>7.19e-06</v>
       </c>
       <c r="E49" t="n">
-        <v>3079428605</v>
+        <v>3022980250</v>
       </c>
       <c r="F49" t="n">
-        <v>30092141</v>
+        <v>364608070</v>
       </c>
       <c r="G49" t="n">
-        <v>-1.64291</v>
+        <v>7.50048</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>RUNE</t>
+          <t>FET</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>THORChain</t>
+          <t>Fetch.ai</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>8.630000000000001</v>
+        <v>2.69</v>
       </c>
       <c r="E50" t="n">
-        <v>2896186476</v>
+        <v>2809851322</v>
       </c>
       <c r="F50" t="n">
-        <v>183133122</v>
+        <v>175702584</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.83719</v>
+        <v>3.24809</v>
       </c>
     </row>
     <row r="51">
@@ -1808,16 +1808,16 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>2.88</v>
+        <v>2.69</v>
       </c>
       <c r="E51" t="n">
-        <v>2873366488</v>
+        <v>2691882686</v>
       </c>
       <c r="F51" t="n">
-        <v>29338379</v>
+        <v>28470429</v>
       </c>
       <c r="G51" t="n">
-        <v>0.66028</v>
+        <v>1.54964</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-04-14
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>69306</v>
+        <v>63788</v>
       </c>
       <c r="E2" t="n">
-        <v>1363932763074</v>
+        <v>1251276371121</v>
       </c>
       <c r="F2" t="n">
-        <v>19008976614</v>
+        <v>64058889462</v>
       </c>
       <c r="G2" t="n">
-        <v>2.3426</v>
+        <v>-5.5655</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3387.36</v>
+        <v>3042.66</v>
       </c>
       <c r="E3" t="n">
-        <v>406710446312</v>
+        <v>363088105363</v>
       </c>
       <c r="F3" t="n">
-        <v>8724892660</v>
+        <v>34549843049</v>
       </c>
       <c r="G3" t="n">
-        <v>1.62731</v>
+        <v>-6.75679</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0.999846</v>
       </c>
       <c r="E4" t="n">
-        <v>106875023058</v>
+        <v>107281972564</v>
       </c>
       <c r="F4" t="n">
-        <v>28937788824</v>
+        <v>125889492954</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.05547</v>
+        <v>-0.01726</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>586.52</v>
+        <v>548.6</v>
       </c>
       <c r="E5" t="n">
-        <v>90225732038</v>
+        <v>83824126043</v>
       </c>
       <c r="F5" t="n">
-        <v>696239279</v>
+        <v>4037942392</v>
       </c>
       <c r="G5" t="n">
-        <v>0.93176</v>
+        <v>-7.08988</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>180.46</v>
+        <v>138.28</v>
       </c>
       <c r="E6" t="n">
-        <v>80447359878</v>
+        <v>61847455906</v>
       </c>
       <c r="F6" t="n">
-        <v>2243774447</v>
+        <v>12080316552</v>
       </c>
       <c r="G6" t="n">
-        <v>2.49275</v>
+        <v>-8.052099999999999</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.999366</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>32910098254</v>
+        <v>32358687395</v>
       </c>
       <c r="F7" t="n">
-        <v>3919859957</v>
+        <v>11684867390</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.05639</v>
+        <v>-0.0554</v>
       </c>
     </row>
     <row r="8">
@@ -638,25 +638,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>STETH</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>Lido Staked Ether</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.5969370000000001</v>
+        <v>3041.54</v>
       </c>
       <c r="E8" t="n">
-        <v>32859797063</v>
+        <v>28570464641</v>
       </c>
       <c r="F8" t="n">
-        <v>806482083</v>
+        <v>408038060</v>
       </c>
       <c r="G8" t="n">
-        <v>1.48356</v>
+        <v>-6.50143</v>
       </c>
     </row>
     <row r="9">
@@ -665,25 +665,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>STETH</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Lido Staked Ether</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>3381.62</v>
+        <v>0.485721</v>
       </c>
       <c r="E9" t="n">
-        <v>32239574756</v>
+        <v>26752711942</v>
       </c>
       <c r="F9" t="n">
-        <v>101616432</v>
+        <v>4697776472</v>
       </c>
       <c r="G9" t="n">
-        <v>1.64889</v>
+        <v>-10.65718</v>
       </c>
     </row>
     <row r="10">
@@ -692,25 +692,25 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>DOGE</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Dogecoin</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.197361</v>
+        <v>6.44</v>
       </c>
       <c r="E10" t="n">
-        <v>28422027126</v>
+        <v>22321043075</v>
       </c>
       <c r="F10" t="n">
-        <v>2356790810</v>
+        <v>1026831209</v>
       </c>
       <c r="G10" t="n">
-        <v>8.09686</v>
+        <v>-3.85049</v>
       </c>
     </row>
     <row r="11">
@@ -719,25 +719,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ADA</t>
+          <t>DOGE</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Cardano</t>
+          <t>Dogecoin</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.593552</v>
+        <v>0.152334</v>
       </c>
       <c r="E11" t="n">
-        <v>20938694026</v>
+        <v>21675964275</v>
       </c>
       <c r="F11" t="n">
-        <v>257759748</v>
+        <v>6110129035</v>
       </c>
       <c r="G11" t="n">
-        <v>2.28471</v>
+        <v>-10.97325</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +746,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>ADA</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Cardano</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>5.41</v>
+        <v>0.456654</v>
       </c>
       <c r="E12" t="n">
-        <v>18755291051</v>
+        <v>15964033014</v>
       </c>
       <c r="F12" t="n">
-        <v>142795156</v>
+        <v>1474309600</v>
       </c>
       <c r="G12" t="n">
-        <v>-2.08733</v>
+        <v>-9.4658</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>48.5</v>
+        <v>35.7</v>
       </c>
       <c r="E13" t="n">
-        <v>18332218378</v>
+        <v>13330755922</v>
       </c>
       <c r="F13" t="n">
-        <v>492988753</v>
+        <v>1971060110</v>
       </c>
       <c r="G13" t="n">
-        <v>3.38384</v>
+        <v>-6.73903</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2.834e-05</v>
+        <v>2.173e-05</v>
       </c>
       <c r="E14" t="n">
-        <v>16702587269</v>
+        <v>12816697217</v>
       </c>
       <c r="F14" t="n">
-        <v>603249154</v>
+        <v>1911392711</v>
       </c>
       <c r="G14" t="n">
-        <v>4.26076</v>
+        <v>-12.03616</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>679.48</v>
+        <v>63924</v>
       </c>
       <c r="E15" t="n">
-        <v>13382133896</v>
+        <v>9930759518</v>
       </c>
       <c r="F15" t="n">
-        <v>773957282</v>
+        <v>764761889</v>
       </c>
       <c r="G15" t="n">
-        <v>-1.89252</v>
+        <v>-5.47332</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>8.66</v>
+        <v>0.110584</v>
       </c>
       <c r="E16" t="n">
-        <v>11684042795</v>
+        <v>9707030759</v>
       </c>
       <c r="F16" t="n">
-        <v>169388464</v>
+        <v>794482894</v>
       </c>
       <c r="G16" t="n">
-        <v>3.06631</v>
+        <v>-3.09989</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>69333</v>
+        <v>482.88</v>
       </c>
       <c r="E17" t="n">
-        <v>10779832953</v>
+        <v>9353845550</v>
       </c>
       <c r="F17" t="n">
-        <v>141651025</v>
+        <v>1325774502</v>
       </c>
       <c r="G17" t="n">
-        <v>2.34724</v>
+        <v>-8.88552</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.120311</v>
+        <v>6.55</v>
       </c>
       <c r="E18" t="n">
-        <v>10550006145</v>
+        <v>8876488618</v>
       </c>
       <c r="F18" t="n">
-        <v>225653074</v>
+        <v>859864388</v>
       </c>
       <c r="G18" t="n">
-        <v>1.46164</v>
+        <v>-8.03687</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>17.73</v>
+        <v>13.61</v>
       </c>
       <c r="E19" t="n">
-        <v>10411138585</v>
+        <v>7917179658</v>
       </c>
       <c r="F19" t="n">
-        <v>230512399</v>
+        <v>1402412091</v>
       </c>
       <c r="G19" t="n">
-        <v>0.74143</v>
+        <v>-9.0284</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>11.32</v>
+        <v>0.681348</v>
       </c>
       <c r="E20" t="n">
-        <v>8520482254</v>
+        <v>6298508280</v>
       </c>
       <c r="F20" t="n">
-        <v>157968113</v>
+        <v>1188473538</v>
       </c>
       <c r="G20" t="n">
-        <v>2.34232</v>
+        <v>-9.85017</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.906156</v>
+        <v>78.09999999999999</v>
       </c>
       <c r="E21" t="n">
-        <v>8413234951</v>
+        <v>5820436033</v>
       </c>
       <c r="F21" t="n">
-        <v>221104999</v>
+        <v>1499889837</v>
       </c>
       <c r="G21" t="n">
-        <v>1.51905</v>
+        <v>-8.69842</v>
       </c>
     </row>
     <row r="22">
@@ -1025,16 +1025,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>17.2</v>
+        <v>12.44</v>
       </c>
       <c r="E22" t="n">
-        <v>7955984665</v>
+        <v>5730989972</v>
       </c>
       <c r="F22" t="n">
-        <v>121881233</v>
+        <v>418637263</v>
       </c>
       <c r="G22" t="n">
-        <v>1.8232</v>
+        <v>-7.74713</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>103.18</v>
+        <v>5.37</v>
       </c>
       <c r="E23" t="n">
-        <v>7677385209</v>
+        <v>5687923057</v>
       </c>
       <c r="F23" t="n">
-        <v>601614109</v>
+        <v>1763259297</v>
       </c>
       <c r="G23" t="n">
-        <v>1.83649</v>
+        <v>-6.06506</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>6.95</v>
+        <v>5.92</v>
       </c>
       <c r="E24" t="n">
-        <v>7360388208</v>
+        <v>5474324308</v>
       </c>
       <c r="F24" t="n">
-        <v>367999243</v>
+        <v>2165961</v>
       </c>
       <c r="G24" t="n">
-        <v>-1.5515</v>
+        <v>2.61709</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>13.76</v>
+        <v>7.11</v>
       </c>
       <c r="E25" t="n">
-        <v>5481145643</v>
+        <v>5342030404</v>
       </c>
       <c r="F25" t="n">
-        <v>180712599</v>
+        <v>631267616</v>
       </c>
       <c r="G25" t="n">
-        <v>5.86007</v>
+        <v>-9.83084</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>5.78</v>
+        <v>1</v>
       </c>
       <c r="E26" t="n">
-        <v>5350892072</v>
+        <v>5119768598</v>
       </c>
       <c r="F26" t="n">
-        <v>1273179</v>
+        <v>798888851</v>
       </c>
       <c r="G26" t="n">
-        <v>0.23891</v>
+        <v>0.07745</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>FDUSD</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>First Digital USD</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.999645</v>
+        <v>1.001</v>
       </c>
       <c r="E27" t="n">
-        <v>5106876172</v>
+        <v>3941873828</v>
       </c>
       <c r="F27" t="n">
-        <v>646973416</v>
+        <v>11949300894</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.13723</v>
+        <v>0.00663</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>33.86</v>
+        <v>9.25</v>
       </c>
       <c r="E28" t="n">
-        <v>4960004530</v>
+        <v>3873352095</v>
       </c>
       <c r="F28" t="n">
-        <v>206460816</v>
+        <v>513013769</v>
       </c>
       <c r="G28" t="n">
-        <v>2.04751</v>
+        <v>-8.01047</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>3.27</v>
+        <v>572.95</v>
       </c>
       <c r="E29" t="n">
-        <v>4752287769</v>
+        <v>3805666688</v>
       </c>
       <c r="F29" t="n">
-        <v>57154795</v>
+        <v>129472649</v>
       </c>
       <c r="G29" t="n">
-        <v>3.63692</v>
+        <v>11.94782</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>8.789999999999999</v>
+        <v>2.63</v>
       </c>
       <c r="E30" t="n">
-        <v>4687935910</v>
+        <v>3775178693</v>
       </c>
       <c r="F30" t="n">
-        <v>176177202</v>
+        <v>283197803</v>
       </c>
       <c r="G30" t="n">
-        <v>2.88181</v>
+        <v>-1.67814</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>1.4</v>
+        <v>25.65</v>
       </c>
       <c r="E31" t="n">
-        <v>4457565465</v>
+        <v>3736131644</v>
       </c>
       <c r="F31" t="n">
-        <v>42694505</v>
+        <v>651256629</v>
       </c>
       <c r="G31" t="n">
-        <v>5.31252</v>
+        <v>-11.88141</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>11.18</v>
+        <v>1.1</v>
       </c>
       <c r="E32" t="n">
-        <v>4367259087</v>
+        <v>3610229282</v>
       </c>
       <c r="F32" t="n">
-        <v>170447907</v>
+        <v>148717178</v>
       </c>
       <c r="G32" t="n">
-        <v>1.56546</v>
+        <v>-7.60669</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>1.5</v>
+        <v>0.128259</v>
       </c>
       <c r="E33" t="n">
-        <v>3969519339</v>
+        <v>3396305543</v>
       </c>
       <c r="F33" t="n">
-        <v>168585528</v>
+        <v>49025328</v>
       </c>
       <c r="G33" t="n">
-        <v>0.7558</v>
+        <v>-6.68048</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.146419</v>
+        <v>8.19</v>
       </c>
       <c r="E34" t="n">
-        <v>3899929131</v>
+        <v>3179428255</v>
       </c>
       <c r="F34" t="n">
-        <v>10582675</v>
+        <v>889703588</v>
       </c>
       <c r="G34" t="n">
-        <v>2.32239</v>
+        <v>-8.401870000000001</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>2.73</v>
+        <v>0.108128</v>
       </c>
       <c r="E35" t="n">
-        <v>3881452208</v>
+        <v>3116808681</v>
       </c>
       <c r="F35" t="n">
-        <v>24725941</v>
+        <v>408562307</v>
       </c>
       <c r="G35" t="n">
-        <v>1.82722</v>
+        <v>-4.55396</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.130072</v>
+        <v>5.84</v>
       </c>
       <c r="E36" t="n">
-        <v>3752192200</v>
+        <v>3115527267</v>
       </c>
       <c r="F36" t="n">
-        <v>48970072</v>
+        <v>789450224</v>
       </c>
       <c r="G36" t="n">
-        <v>1.29402</v>
+        <v>-11.70413</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>9.710000000000001</v>
+        <v>51.73</v>
       </c>
       <c r="E37" t="n">
-        <v>3707584587</v>
+        <v>3102861366</v>
       </c>
       <c r="F37" t="n">
-        <v>87759660</v>
+        <v>27662462</v>
       </c>
       <c r="G37" t="n">
-        <v>3.11429</v>
+        <v>-2.70965</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>556.42</v>
+        <v>0.04098192</v>
       </c>
       <c r="E38" t="n">
-        <v>3648411660</v>
+        <v>2985566543</v>
       </c>
       <c r="F38" t="n">
-        <v>13830418</v>
+        <v>196757479</v>
       </c>
       <c r="G38" t="n">
-        <v>-2.52961</v>
+        <v>-6.81483</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>WIF</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>dogwifhat</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>3.62</v>
+        <v>7.69</v>
       </c>
       <c r="E39" t="n">
-        <v>3618850501</v>
+        <v>2936613852</v>
       </c>
       <c r="F39" t="n">
-        <v>392057021</v>
+        <v>550481339</v>
       </c>
       <c r="G39" t="n">
-        <v>10.73044</v>
+        <v>-4.16378</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.106466</v>
+        <v>1.12</v>
       </c>
       <c r="E40" t="n">
-        <v>3592627774</v>
+        <v>2932869705</v>
       </c>
       <c r="F40" t="n">
-        <v>25870450</v>
+        <v>1187221157</v>
       </c>
       <c r="G40" t="n">
-        <v>1.27874</v>
+        <v>-3.01122</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>FDUSD</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>First Digital USD</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1.002</v>
+        <v>2.07</v>
       </c>
       <c r="E41" t="n">
-        <v>3530854261</v>
+        <v>2923933613</v>
       </c>
       <c r="F41" t="n">
-        <v>4366880686</v>
+        <v>139059990</v>
       </c>
       <c r="G41" t="n">
-        <v>0.02028</v>
+        <v>-3.79748</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>58.55</v>
+        <v>0.07914400000000001</v>
       </c>
       <c r="E42" t="n">
-        <v>3512831253</v>
+        <v>2816382211</v>
       </c>
       <c r="F42" t="n">
-        <v>8389308</v>
+        <v>186250922</v>
       </c>
       <c r="G42" t="n">
-        <v>2.09003</v>
+        <v>-7.37259</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>3667.29</v>
+        <v>0.118083</v>
       </c>
       <c r="E43" t="n">
-        <v>3390829114</v>
+        <v>2752302549</v>
       </c>
       <c r="F43" t="n">
-        <v>91315242</v>
+        <v>121349364</v>
       </c>
       <c r="G43" t="n">
-        <v>-1.07582</v>
+        <v>-6.30125</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>WIF</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>dogwifhat</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.139934</v>
+        <v>2.76</v>
       </c>
       <c r="E44" t="n">
-        <v>3230871716</v>
+        <v>2724264296</v>
       </c>
       <c r="F44" t="n">
-        <v>51320302</v>
+        <v>1113863209</v>
       </c>
       <c r="G44" t="n">
-        <v>5.4082</v>
+        <v>-0.18101</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.33975</v>
+        <v>2919.28</v>
       </c>
       <c r="E45" t="n">
-        <v>3215485222</v>
+        <v>2692446286</v>
       </c>
       <c r="F45" t="n">
-        <v>74158652</v>
+        <v>266140862</v>
       </c>
       <c r="G45" t="n">
-        <v>1.61073</v>
+        <v>-0.533</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>USDE</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>Ethena USDe</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>35.56</v>
+        <v>1</v>
       </c>
       <c r="E46" t="n">
-        <v>3202455945</v>
+        <v>2355595200</v>
       </c>
       <c r="F46" t="n">
-        <v>120757229</v>
+        <v>179615642</v>
       </c>
       <c r="G46" t="n">
-        <v>0.7668</v>
+        <v>-0.04662</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.04243749</v>
+        <v>0.241349</v>
       </c>
       <c r="E47" t="n">
-        <v>3085243824</v>
+        <v>2284072133</v>
       </c>
       <c r="F47" t="n">
-        <v>53112420</v>
+        <v>251962864</v>
       </c>
       <c r="G47" t="n">
-        <v>4.27306</v>
+        <v>-9.14095</v>
       </c>
     </row>
     <row r="48">
@@ -1727,16 +1727,16 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>3.06</v>
+        <v>2.24</v>
       </c>
       <c r="E48" t="n">
-        <v>3078515086</v>
+        <v>2237718405</v>
       </c>
       <c r="F48" t="n">
-        <v>156220264</v>
+        <v>740545088</v>
       </c>
       <c r="G48" t="n">
-        <v>2.9313</v>
+        <v>-7.01342</v>
       </c>
     </row>
     <row r="49">
@@ -1754,16 +1754,16 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>7.19e-06</v>
+        <v>5.31e-06</v>
       </c>
       <c r="E49" t="n">
-        <v>3022980250</v>
+        <v>2223933058</v>
       </c>
       <c r="F49" t="n">
-        <v>364608070</v>
+        <v>1523553234</v>
       </c>
       <c r="G49" t="n">
-        <v>7.50048</v>
+        <v>-9.520659999999999</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>FET</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Fetch.ai</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>2.69</v>
+        <v>24.74</v>
       </c>
       <c r="E50" t="n">
-        <v>2809851322</v>
+        <v>2213363943</v>
       </c>
       <c r="F50" t="n">
-        <v>175702584</v>
+        <v>478163126</v>
       </c>
       <c r="G50" t="n">
-        <v>3.24809</v>
+        <v>-7.11058</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>THETA</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Theta Network</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>2.69</v>
+        <v>117.84</v>
       </c>
       <c r="E51" t="n">
-        <v>2691882686</v>
+        <v>2141065101</v>
       </c>
       <c r="F51" t="n">
-        <v>28470429</v>
+        <v>56399940</v>
       </c>
       <c r="G51" t="n">
-        <v>1.54964</v>
+        <v>-5.68921</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-04-21
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>63788</v>
+        <v>65167</v>
       </c>
       <c r="E2" t="n">
-        <v>1251276371121</v>
+        <v>1285856360537</v>
       </c>
       <c r="F2" t="n">
-        <v>64058889462</v>
+        <v>21650378234</v>
       </c>
       <c r="G2" t="n">
-        <v>-5.5655</v>
+        <v>2.38921</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3042.66</v>
+        <v>3162.43</v>
       </c>
       <c r="E3" t="n">
-        <v>363088105363</v>
+        <v>380656097535</v>
       </c>
       <c r="F3" t="n">
-        <v>34549843049</v>
+        <v>10460133831</v>
       </c>
       <c r="G3" t="n">
-        <v>-6.75679</v>
+        <v>3.81157</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999846</v>
+        <v>0.999634</v>
       </c>
       <c r="E4" t="n">
-        <v>107281972564</v>
+        <v>109837986989</v>
       </c>
       <c r="F4" t="n">
-        <v>125889492954</v>
+        <v>35814660588</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.01726</v>
+        <v>-0.14104</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>548.6</v>
+        <v>577.04</v>
       </c>
       <c r="E5" t="n">
-        <v>83824126043</v>
+        <v>88997377881</v>
       </c>
       <c r="F5" t="n">
-        <v>4037942392</v>
+        <v>1023560824</v>
       </c>
       <c r="G5" t="n">
-        <v>-7.08988</v>
+        <v>3.73376</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>138.28</v>
+        <v>150.38</v>
       </c>
       <c r="E6" t="n">
-        <v>61847455906</v>
+        <v>67323891460</v>
       </c>
       <c r="F6" t="n">
-        <v>12080316552</v>
+        <v>3154837312</v>
       </c>
       <c r="G6" t="n">
-        <v>-8.052099999999999</v>
+        <v>6.31147</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0.999115</v>
       </c>
       <c r="E7" t="n">
-        <v>32358687395</v>
+        <v>33921182729</v>
       </c>
       <c r="F7" t="n">
-        <v>11684867390</v>
+        <v>4967071302</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.0554</v>
+        <v>-0.05891</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>3041.54</v>
+        <v>3161.21</v>
       </c>
       <c r="E8" t="n">
-        <v>28570464641</v>
+        <v>29573964223</v>
       </c>
       <c r="F8" t="n">
-        <v>408038060</v>
+        <v>83475183</v>
       </c>
       <c r="G8" t="n">
-        <v>-6.50143</v>
+        <v>3.84677</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.485721</v>
+        <v>0.528042</v>
       </c>
       <c r="E9" t="n">
-        <v>26752711942</v>
+        <v>29179386461</v>
       </c>
       <c r="F9" t="n">
-        <v>4697776472</v>
+        <v>919870439</v>
       </c>
       <c r="G9" t="n">
-        <v>-10.65718</v>
+        <v>2.02663</v>
       </c>
     </row>
     <row r="10">
@@ -692,25 +692,25 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>DOGE</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Dogecoin</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>6.44</v>
+        <v>0.161294</v>
       </c>
       <c r="E10" t="n">
-        <v>22321043075</v>
+        <v>23338959876</v>
       </c>
       <c r="F10" t="n">
-        <v>1026831209</v>
+        <v>1656714530</v>
       </c>
       <c r="G10" t="n">
-        <v>-3.85049</v>
+        <v>6.07605</v>
       </c>
     </row>
     <row r="11">
@@ -719,25 +719,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>DOGE</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Dogecoin</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.152334</v>
+        <v>6.16</v>
       </c>
       <c r="E11" t="n">
-        <v>21675964275</v>
+        <v>21433855756</v>
       </c>
       <c r="F11" t="n">
-        <v>6110129035</v>
+        <v>263750603</v>
       </c>
       <c r="G11" t="n">
-        <v>-10.97325</v>
+        <v>0.25616</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.456654</v>
+        <v>0.5004150000000001</v>
       </c>
       <c r="E12" t="n">
-        <v>15964033014</v>
+        <v>17732845591</v>
       </c>
       <c r="F12" t="n">
-        <v>1474309600</v>
+        <v>404218775</v>
       </c>
       <c r="G12" t="n">
-        <v>-9.4658</v>
+        <v>4.75736</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>35.7</v>
+        <v>2.68e-05</v>
       </c>
       <c r="E13" t="n">
-        <v>13330755922</v>
+        <v>15808645011</v>
       </c>
       <c r="F13" t="n">
-        <v>1971060110</v>
+        <v>1152002688</v>
       </c>
       <c r="G13" t="n">
-        <v>-6.73903</v>
+        <v>16.35217</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2.173e-05</v>
+        <v>37.31</v>
       </c>
       <c r="E14" t="n">
-        <v>12816697217</v>
+        <v>14152141005</v>
       </c>
       <c r="F14" t="n">
-        <v>1911392711</v>
+        <v>487064009</v>
       </c>
       <c r="G14" t="n">
-        <v>-12.03616</v>
+        <v>6.46406</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>63924</v>
+        <v>65236</v>
       </c>
       <c r="E15" t="n">
-        <v>9930759518</v>
+        <v>10131867455</v>
       </c>
       <c r="F15" t="n">
-        <v>764761889</v>
+        <v>163390002</v>
       </c>
       <c r="G15" t="n">
-        <v>-5.47332</v>
+        <v>2.32286</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.110584</v>
+        <v>510.83</v>
       </c>
       <c r="E16" t="n">
-        <v>9707030759</v>
+        <v>10097849184</v>
       </c>
       <c r="F16" t="n">
-        <v>794482894</v>
+        <v>368311916</v>
       </c>
       <c r="G16" t="n">
-        <v>-3.09989</v>
+        <v>5.21581</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>482.88</v>
+        <v>0.110969</v>
       </c>
       <c r="E17" t="n">
-        <v>9353845550</v>
+        <v>9722501396</v>
       </c>
       <c r="F17" t="n">
-        <v>1325774502</v>
+        <v>278348564</v>
       </c>
       <c r="G17" t="n">
-        <v>-8.88552</v>
+        <v>1.28244</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>6.55</v>
+        <v>7.15</v>
       </c>
       <c r="E18" t="n">
-        <v>8876488618</v>
+        <v>9704039943</v>
       </c>
       <c r="F18" t="n">
-        <v>859864388</v>
+        <v>185315831</v>
       </c>
       <c r="G18" t="n">
-        <v>-8.03687</v>
+        <v>6.10454</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>13.61</v>
+        <v>14.84</v>
       </c>
       <c r="E19" t="n">
-        <v>7917179658</v>
+        <v>8742538777</v>
       </c>
       <c r="F19" t="n">
-        <v>1402412091</v>
+        <v>311903752</v>
       </c>
       <c r="G19" t="n">
-        <v>-9.0284</v>
+        <v>4.81562</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.681348</v>
+        <v>15.25</v>
       </c>
       <c r="E20" t="n">
-        <v>6298508280</v>
+        <v>7088337554</v>
       </c>
       <c r="F20" t="n">
-        <v>1188473538</v>
+        <v>230990072</v>
       </c>
       <c r="G20" t="n">
-        <v>-9.85017</v>
+        <v>5.6414</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>78.09999999999999</v>
+        <v>6.31</v>
       </c>
       <c r="E21" t="n">
-        <v>5820436033</v>
+        <v>6737443843</v>
       </c>
       <c r="F21" t="n">
-        <v>1499889837</v>
+        <v>392598059</v>
       </c>
       <c r="G21" t="n">
-        <v>-8.69842</v>
+        <v>11.21983</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>12.44</v>
+        <v>0.722213</v>
       </c>
       <c r="E22" t="n">
-        <v>5730989972</v>
+        <v>6726904459</v>
       </c>
       <c r="F22" t="n">
-        <v>418637263</v>
+        <v>294092710</v>
       </c>
       <c r="G22" t="n">
-        <v>-7.74713</v>
+        <v>5.81374</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>5.37</v>
+        <v>84.92</v>
       </c>
       <c r="E23" t="n">
-        <v>5687923057</v>
+        <v>6338948133</v>
       </c>
       <c r="F23" t="n">
-        <v>1763259297</v>
+        <v>347638758</v>
       </c>
       <c r="G23" t="n">
-        <v>-6.06506</v>
+        <v>3.0582</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>5.92</v>
+        <v>7.79</v>
       </c>
       <c r="E24" t="n">
-        <v>5474324308</v>
+        <v>5878470129</v>
       </c>
       <c r="F24" t="n">
-        <v>2165961</v>
+        <v>125141781</v>
       </c>
       <c r="G24" t="n">
-        <v>2.61709</v>
+        <v>3.8001</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>7.11</v>
+        <v>5.75</v>
       </c>
       <c r="E25" t="n">
-        <v>5342030404</v>
+        <v>5325304943</v>
       </c>
       <c r="F25" t="n">
-        <v>631267616</v>
+        <v>1123640</v>
       </c>
       <c r="G25" t="n">
-        <v>-9.83084</v>
+        <v>0.20603</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>1.002</v>
       </c>
       <c r="E26" t="n">
-        <v>5119768598</v>
+        <v>5148951014</v>
       </c>
       <c r="F26" t="n">
-        <v>798888851</v>
+        <v>496740453</v>
       </c>
       <c r="G26" t="n">
-        <v>0.07745</v>
+        <v>0.14206</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>FDUSD</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>First Digital USD</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>1.001</v>
+        <v>9.98</v>
       </c>
       <c r="E27" t="n">
-        <v>3941873828</v>
+        <v>4269268905</v>
       </c>
       <c r="F27" t="n">
-        <v>11949300894</v>
+        <v>123275240</v>
       </c>
       <c r="G27" t="n">
-        <v>0.00663</v>
+        <v>4.167</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>9.25</v>
+        <v>2.83</v>
       </c>
       <c r="E28" t="n">
-        <v>3873352095</v>
+        <v>4121088813</v>
       </c>
       <c r="F28" t="n">
-        <v>513013769</v>
+        <v>103656643</v>
       </c>
       <c r="G28" t="n">
-        <v>-8.01047</v>
+        <v>15.16295</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>572.95</v>
+        <v>27.75</v>
       </c>
       <c r="E29" t="n">
-        <v>3805666688</v>
+        <v>4089016384</v>
       </c>
       <c r="F29" t="n">
-        <v>129472649</v>
+        <v>174120125</v>
       </c>
       <c r="G29" t="n">
-        <v>11.94782</v>
+        <v>5.21342</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>2.63</v>
+        <v>1.2</v>
       </c>
       <c r="E30" t="n">
-        <v>3775178693</v>
+        <v>3919913297</v>
       </c>
       <c r="F30" t="n">
-        <v>283197803</v>
+        <v>49545631</v>
       </c>
       <c r="G30" t="n">
-        <v>-1.67814</v>
+        <v>4.27778</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>FDUSD</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>First Digital USD</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>25.65</v>
+        <v>0.996842</v>
       </c>
       <c r="E31" t="n">
-        <v>3736131644</v>
+        <v>3590329941</v>
       </c>
       <c r="F31" t="n">
-        <v>651256629</v>
+        <v>5563716800</v>
       </c>
       <c r="G31" t="n">
-        <v>-11.88141</v>
+        <v>-0.27551</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>1.1</v>
+        <v>6.55</v>
       </c>
       <c r="E32" t="n">
-        <v>3610229282</v>
+        <v>3566125827</v>
       </c>
       <c r="F32" t="n">
-        <v>148717178</v>
+        <v>199944914</v>
       </c>
       <c r="G32" t="n">
-        <v>-7.60669</v>
+        <v>6.07506</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.128259</v>
+        <v>9.039999999999999</v>
       </c>
       <c r="E33" t="n">
-        <v>3396305543</v>
+        <v>3486848953</v>
       </c>
       <c r="F33" t="n">
-        <v>49025328</v>
+        <v>169894511</v>
       </c>
       <c r="G33" t="n">
-        <v>-6.68048</v>
+        <v>11.697</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>8.19</v>
+        <v>0.130083</v>
       </c>
       <c r="E34" t="n">
-        <v>3179428255</v>
+        <v>3482562232</v>
       </c>
       <c r="F34" t="n">
-        <v>889703588</v>
+        <v>16021315</v>
       </c>
       <c r="G34" t="n">
-        <v>-8.401870000000001</v>
+        <v>5.22879</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.108128</v>
+        <v>8.66</v>
       </c>
       <c r="E35" t="n">
-        <v>3116808681</v>
+        <v>3393373696</v>
       </c>
       <c r="F35" t="n">
-        <v>408562307</v>
+        <v>112957758</v>
       </c>
       <c r="G35" t="n">
-        <v>-4.55396</v>
+        <v>4.11151</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>5.84</v>
+        <v>0.114555</v>
       </c>
       <c r="E36" t="n">
-        <v>3115527267</v>
+        <v>3317003152</v>
       </c>
       <c r="F36" t="n">
-        <v>789450224</v>
+        <v>56946743</v>
       </c>
       <c r="G36" t="n">
-        <v>-11.70413</v>
+        <v>0.95014</v>
       </c>
     </row>
     <row r="37">
@@ -1430,16 +1430,16 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>51.73</v>
+        <v>55.19</v>
       </c>
       <c r="E37" t="n">
-        <v>3102861366</v>
+        <v>3315645562</v>
       </c>
       <c r="F37" t="n">
-        <v>27662462</v>
+        <v>10160155</v>
       </c>
       <c r="G37" t="n">
-        <v>-2.70965</v>
+        <v>-0.332</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.04098192</v>
+        <v>0.090183</v>
       </c>
       <c r="E38" t="n">
-        <v>2985566543</v>
+        <v>3245321661</v>
       </c>
       <c r="F38" t="n">
-        <v>196757479</v>
+        <v>47450271</v>
       </c>
       <c r="G38" t="n">
-        <v>-6.81483</v>
+        <v>11.16918</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>7.69</v>
+        <v>1.2</v>
       </c>
       <c r="E39" t="n">
-        <v>2936613852</v>
+        <v>3199726355</v>
       </c>
       <c r="F39" t="n">
-        <v>550481339</v>
+        <v>212985096</v>
       </c>
       <c r="G39" t="n">
-        <v>-4.16378</v>
+        <v>6.11965</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1.12</v>
+        <v>2.18</v>
       </c>
       <c r="E40" t="n">
-        <v>2932869705</v>
+        <v>3185371557</v>
       </c>
       <c r="F40" t="n">
-        <v>1187221157</v>
+        <v>53228825</v>
       </c>
       <c r="G40" t="n">
-        <v>-3.01122</v>
+        <v>7.53123</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>EZETH</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>Renzo Restaked ETH</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>2.07</v>
+        <v>3189.96</v>
       </c>
       <c r="E41" t="n">
-        <v>2923933613</v>
+        <v>3183532399</v>
       </c>
       <c r="F41" t="n">
-        <v>139059990</v>
+        <v>79980860</v>
       </c>
       <c r="G41" t="n">
-        <v>-3.79748</v>
+        <v>3.62206</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.07914400000000001</v>
+        <v>473.03</v>
       </c>
       <c r="E42" t="n">
-        <v>2816382211</v>
+        <v>3151141869</v>
       </c>
       <c r="F42" t="n">
-        <v>186250922</v>
+        <v>32710880</v>
       </c>
       <c r="G42" t="n">
-        <v>-7.37259</v>
+        <v>7.7267</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.118083</v>
+        <v>0.04224241</v>
       </c>
       <c r="E43" t="n">
-        <v>2752302549</v>
+        <v>3080340150</v>
       </c>
       <c r="F43" t="n">
-        <v>121349364</v>
+        <v>69364566</v>
       </c>
       <c r="G43" t="n">
-        <v>-6.30125</v>
+        <v>3.454</v>
       </c>
     </row>
     <row r="44">
@@ -1619,16 +1619,16 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>2.76</v>
+        <v>3.04</v>
       </c>
       <c r="E44" t="n">
-        <v>2724264296</v>
+        <v>3050200015</v>
       </c>
       <c r="F44" t="n">
-        <v>1113863209</v>
+        <v>601623097</v>
       </c>
       <c r="G44" t="n">
-        <v>-0.18101</v>
+        <v>10.44023</v>
       </c>
     </row>
     <row r="45">
@@ -1646,16 +1646,16 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>2919.28</v>
+        <v>3058.8</v>
       </c>
       <c r="E45" t="n">
-        <v>2692446286</v>
+        <v>2837429305</v>
       </c>
       <c r="F45" t="n">
-        <v>266140862</v>
+        <v>104402686</v>
       </c>
       <c r="G45" t="n">
-        <v>-0.533</v>
+        <v>0.49827</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>USDE</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Ethena USDe</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>1</v>
+        <v>0.117434</v>
       </c>
       <c r="E46" t="n">
-        <v>2355595200</v>
+        <v>2716928958</v>
       </c>
       <c r="F46" t="n">
-        <v>179615642</v>
+        <v>33345159</v>
       </c>
       <c r="G46" t="n">
-        <v>-0.04662</v>
+        <v>1.74528</v>
       </c>
     </row>
     <row r="47">
@@ -1700,16 +1700,16 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.241349</v>
+        <v>0.28424</v>
       </c>
       <c r="E47" t="n">
-        <v>2284072133</v>
+        <v>2700089429</v>
       </c>
       <c r="F47" t="n">
-        <v>251962864</v>
+        <v>95829464</v>
       </c>
       <c r="G47" t="n">
-        <v>-9.14095</v>
+        <v>4.70704</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>2.24</v>
+        <v>28.99</v>
       </c>
       <c r="E48" t="n">
-        <v>2237718405</v>
+        <v>2619707541</v>
       </c>
       <c r="F48" t="n">
-        <v>740545088</v>
+        <v>121917233</v>
       </c>
       <c r="G48" t="n">
-        <v>-7.01342</v>
+        <v>5.06998</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Pepe</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>5.31e-06</v>
+        <v>2.47</v>
       </c>
       <c r="E49" t="n">
-        <v>2223933058</v>
+        <v>2589251372</v>
       </c>
       <c r="F49" t="n">
-        <v>1523553234</v>
+        <v>206107489</v>
       </c>
       <c r="G49" t="n">
-        <v>-9.520659999999999</v>
+        <v>8.021940000000001</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>FET</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>Fetch.ai</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>24.74</v>
+        <v>2.45</v>
       </c>
       <c r="E50" t="n">
-        <v>2213363943</v>
+        <v>2573943317</v>
       </c>
       <c r="F50" t="n">
-        <v>478163126</v>
+        <v>369802036</v>
       </c>
       <c r="G50" t="n">
-        <v>-7.11058</v>
+        <v>10.52097</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Pepe</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>117.84</v>
+        <v>6.01e-06</v>
       </c>
       <c r="E51" t="n">
-        <v>2141065101</v>
+        <v>2532730982</v>
       </c>
       <c r="F51" t="n">
-        <v>56399940</v>
+        <v>723356028</v>
       </c>
       <c r="G51" t="n">
-        <v>-5.68921</v>
+        <v>17.65564</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-04-28
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>65167</v>
+        <v>63488</v>
       </c>
       <c r="E2" t="n">
-        <v>1285856360537</v>
+        <v>1251266030203</v>
       </c>
       <c r="F2" t="n">
-        <v>21650378234</v>
+        <v>16951389959</v>
       </c>
       <c r="G2" t="n">
-        <v>2.38921</v>
+        <v>0.65895</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3162.43</v>
+        <v>3286.75</v>
       </c>
       <c r="E3" t="n">
-        <v>380656097535</v>
+        <v>401721209804</v>
       </c>
       <c r="F3" t="n">
-        <v>10460133831</v>
+        <v>13502862795</v>
       </c>
       <c r="G3" t="n">
-        <v>3.81157</v>
+        <v>4.76128</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999634</v>
+        <v>0.999579</v>
       </c>
       <c r="E4" t="n">
-        <v>109837986989</v>
+        <v>110542916254</v>
       </c>
       <c r="F4" t="n">
-        <v>35814660588</v>
+        <v>18832345482</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.14104</v>
+        <v>0.02277</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>577.04</v>
+        <v>601.6900000000001</v>
       </c>
       <c r="E5" t="n">
-        <v>88997377881</v>
+        <v>92675069960</v>
       </c>
       <c r="F5" t="n">
-        <v>1023560824</v>
+        <v>721687671</v>
       </c>
       <c r="G5" t="n">
-        <v>3.73376</v>
+        <v>2.27929</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>150.38</v>
+        <v>141.38</v>
       </c>
       <c r="E6" t="n">
-        <v>67323891460</v>
+        <v>63295584877</v>
       </c>
       <c r="F6" t="n">
-        <v>3154837312</v>
+        <v>2380296592</v>
       </c>
       <c r="G6" t="n">
-        <v>6.31147</v>
+        <v>3.20119</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.999115</v>
+        <v>0.999716</v>
       </c>
       <c r="E7" t="n">
-        <v>33921182729</v>
+        <v>33507244349</v>
       </c>
       <c r="F7" t="n">
-        <v>4967071302</v>
+        <v>4449551523</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.05891</v>
+        <v>-0.03693</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>3161.21</v>
+        <v>3286.35</v>
       </c>
       <c r="E8" t="n">
-        <v>29573964223</v>
+        <v>30765593133</v>
       </c>
       <c r="F8" t="n">
-        <v>83475183</v>
+        <v>92147431</v>
       </c>
       <c r="G8" t="n">
-        <v>3.84677</v>
+        <v>4.89726</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.528042</v>
+        <v>0.517728</v>
       </c>
       <c r="E9" t="n">
-        <v>29179386461</v>
+        <v>28616045471</v>
       </c>
       <c r="F9" t="n">
-        <v>919870439</v>
+        <v>516211197</v>
       </c>
       <c r="G9" t="n">
-        <v>2.02663</v>
+        <v>0.40678</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.161294</v>
+        <v>0.148723</v>
       </c>
       <c r="E10" t="n">
-        <v>23338959876</v>
+        <v>21443343857</v>
       </c>
       <c r="F10" t="n">
-        <v>1656714530</v>
+        <v>702088757</v>
       </c>
       <c r="G10" t="n">
-        <v>6.07605</v>
+        <v>2.51809</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>6.16</v>
+        <v>5.45</v>
       </c>
       <c r="E11" t="n">
-        <v>21433855756</v>
+        <v>18937900907</v>
       </c>
       <c r="F11" t="n">
-        <v>263750603</v>
+        <v>163757771</v>
       </c>
       <c r="G11" t="n">
-        <v>0.25616</v>
+        <v>3.73112</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.5004150000000001</v>
+        <v>0.467783</v>
       </c>
       <c r="E12" t="n">
-        <v>17732845591</v>
+        <v>16535064095</v>
       </c>
       <c r="F12" t="n">
-        <v>404218775</v>
+        <v>261054090</v>
       </c>
       <c r="G12" t="n">
-        <v>4.75736</v>
+        <v>2.67533</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2.68e-05</v>
+        <v>2.456e-05</v>
       </c>
       <c r="E13" t="n">
-        <v>15808645011</v>
+        <v>14486163800</v>
       </c>
       <c r="F13" t="n">
-        <v>1152002688</v>
+        <v>344333433</v>
       </c>
       <c r="G13" t="n">
-        <v>16.35217</v>
+        <v>0.715</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>37.31</v>
+        <v>34.4</v>
       </c>
       <c r="E14" t="n">
-        <v>14152141005</v>
+        <v>13034887033</v>
       </c>
       <c r="F14" t="n">
-        <v>487064009</v>
+        <v>310883405</v>
       </c>
       <c r="G14" t="n">
-        <v>6.46406</v>
+        <v>0.95145</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>65236</v>
+        <v>0.121092</v>
       </c>
       <c r="E15" t="n">
-        <v>10131867455</v>
+        <v>10614772091</v>
       </c>
       <c r="F15" t="n">
-        <v>163390002</v>
+        <v>251070783</v>
       </c>
       <c r="G15" t="n">
-        <v>2.32286</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>510.83</v>
+        <v>63545</v>
       </c>
       <c r="E16" t="n">
-        <v>10097849184</v>
+        <v>9878528213</v>
       </c>
       <c r="F16" t="n">
-        <v>368311916</v>
+        <v>284359962</v>
       </c>
       <c r="G16" t="n">
-        <v>5.21581</v>
+        <v>0.83538</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.110969</v>
+        <v>477.98</v>
       </c>
       <c r="E17" t="n">
-        <v>9722501396</v>
+        <v>9424278716</v>
       </c>
       <c r="F17" t="n">
-        <v>278348564</v>
+        <v>231262089</v>
       </c>
       <c r="G17" t="n">
-        <v>1.28244</v>
+        <v>1.34032</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>7.15</v>
+        <v>6.82</v>
       </c>
       <c r="E18" t="n">
-        <v>9704039943</v>
+        <v>9258124401</v>
       </c>
       <c r="F18" t="n">
-        <v>185315831</v>
+        <v>140412822</v>
       </c>
       <c r="G18" t="n">
-        <v>6.10454</v>
+        <v>2.40286</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>14.84</v>
+        <v>14.04</v>
       </c>
       <c r="E19" t="n">
-        <v>8742538777</v>
+        <v>8254974336</v>
       </c>
       <c r="F19" t="n">
-        <v>311903752</v>
+        <v>281480770</v>
       </c>
       <c r="G19" t="n">
-        <v>4.81562</v>
+        <v>-0.4885</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>15.25</v>
+        <v>7.23</v>
       </c>
       <c r="E20" t="n">
-        <v>7088337554</v>
+        <v>7747521248</v>
       </c>
       <c r="F20" t="n">
-        <v>230990072</v>
+        <v>670497251</v>
       </c>
       <c r="G20" t="n">
-        <v>5.6414</v>
+        <v>5.45859</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>6.31</v>
+        <v>0.725945</v>
       </c>
       <c r="E21" t="n">
-        <v>6737443843</v>
+        <v>6748832234</v>
       </c>
       <c r="F21" t="n">
-        <v>392598059</v>
+        <v>283000054</v>
       </c>
       <c r="G21" t="n">
-        <v>11.21983</v>
+        <v>4.23283</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.722213</v>
+        <v>84.01000000000001</v>
       </c>
       <c r="E22" t="n">
-        <v>6726904459</v>
+        <v>6260460660</v>
       </c>
       <c r="F22" t="n">
-        <v>294092710</v>
+        <v>352925134</v>
       </c>
       <c r="G22" t="n">
-        <v>5.81374</v>
+        <v>-1.59217</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>84.92</v>
+        <v>13.53</v>
       </c>
       <c r="E23" t="n">
-        <v>6338948133</v>
+        <v>6259219232</v>
       </c>
       <c r="F23" t="n">
-        <v>347638758</v>
+        <v>108246132</v>
       </c>
       <c r="G23" t="n">
-        <v>3.0582</v>
+        <v>4.32893</v>
       </c>
     </row>
     <row r="24">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>7.79</v>
+        <v>8</v>
       </c>
       <c r="E24" t="n">
-        <v>5878470129</v>
+        <v>6037159757</v>
       </c>
       <c r="F24" t="n">
-        <v>125141781</v>
+        <v>105914827</v>
       </c>
       <c r="G24" t="n">
-        <v>3.8001</v>
+        <v>4.45935</v>
       </c>
     </row>
     <row r="25">
@@ -1106,16 +1106,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>5.75</v>
+        <v>5.77</v>
       </c>
       <c r="E25" t="n">
-        <v>5325304943</v>
+        <v>5353560880</v>
       </c>
       <c r="F25" t="n">
-        <v>1123640</v>
+        <v>1115193</v>
       </c>
       <c r="G25" t="n">
-        <v>0.20603</v>
+        <v>-0.18576</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>1.002</v>
+        <v>0.9990869999999999</v>
       </c>
       <c r="E26" t="n">
-        <v>5148951014</v>
+        <v>5300051791</v>
       </c>
       <c r="F26" t="n">
-        <v>496740453</v>
+        <v>341533742</v>
       </c>
       <c r="G26" t="n">
-        <v>0.14206</v>
+        <v>-0.04717</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>FDUSD</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>First Digital USD</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>9.98</v>
+        <v>0.999356</v>
       </c>
       <c r="E27" t="n">
-        <v>4269268905</v>
+        <v>4421963328</v>
       </c>
       <c r="F27" t="n">
-        <v>123275240</v>
+        <v>4223605304</v>
       </c>
       <c r="G27" t="n">
-        <v>4.167</v>
+        <v>-0.41116</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>2.83</v>
+        <v>28.64</v>
       </c>
       <c r="E28" t="n">
-        <v>4121088813</v>
+        <v>4208131568</v>
       </c>
       <c r="F28" t="n">
-        <v>103656643</v>
+        <v>292584727</v>
       </c>
       <c r="G28" t="n">
-        <v>15.16295</v>
+        <v>7.47523</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>27.75</v>
+        <v>8.99</v>
       </c>
       <c r="E29" t="n">
-        <v>4089016384</v>
+        <v>3845874138</v>
       </c>
       <c r="F29" t="n">
-        <v>174120125</v>
+        <v>94904639</v>
       </c>
       <c r="G29" t="n">
-        <v>5.21342</v>
+        <v>2.51416</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>1.2</v>
+        <v>0.104187</v>
       </c>
       <c r="E30" t="n">
-        <v>3919913297</v>
+        <v>3730540254</v>
       </c>
       <c r="F30" t="n">
-        <v>49545631</v>
+        <v>127272948</v>
       </c>
       <c r="G30" t="n">
-        <v>4.27778</v>
+        <v>-2.67316</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>FDUSD</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>First Digital USD</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.996842</v>
+        <v>2.52</v>
       </c>
       <c r="E31" t="n">
-        <v>3590329941</v>
+        <v>3670743372</v>
       </c>
       <c r="F31" t="n">
-        <v>5563716800</v>
+        <v>50466822</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.27551</v>
+        <v>-0.30715</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>6.55</v>
+        <v>1.1</v>
       </c>
       <c r="E32" t="n">
-        <v>3566125827</v>
+        <v>3593450469</v>
       </c>
       <c r="F32" t="n">
-        <v>199944914</v>
+        <v>38972817</v>
       </c>
       <c r="G32" t="n">
-        <v>6.07506</v>
+        <v>3.00505</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>9.039999999999999</v>
+        <v>0.128041</v>
       </c>
       <c r="E33" t="n">
-        <v>3486848953</v>
+        <v>3418998297</v>
       </c>
       <c r="F33" t="n">
-        <v>169894511</v>
+        <v>12572539</v>
       </c>
       <c r="G33" t="n">
-        <v>11.697</v>
+        <v>3.33036</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.130083</v>
+        <v>0.114372</v>
       </c>
       <c r="E34" t="n">
-        <v>3482562232</v>
+        <v>3313398133</v>
       </c>
       <c r="F34" t="n">
-        <v>16021315</v>
+        <v>49343280</v>
       </c>
       <c r="G34" t="n">
-        <v>5.22879</v>
+        <v>1.43716</v>
       </c>
     </row>
     <row r="35">
@@ -1376,16 +1376,16 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>8.66</v>
+        <v>8.31</v>
       </c>
       <c r="E35" t="n">
-        <v>3393373696</v>
+        <v>3249455817</v>
       </c>
       <c r="F35" t="n">
-        <v>112957758</v>
+        <v>86327410</v>
       </c>
       <c r="G35" t="n">
-        <v>4.11151</v>
+        <v>1.30525</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.114555</v>
+        <v>5.95</v>
       </c>
       <c r="E36" t="n">
-        <v>3317003152</v>
+        <v>3243569658</v>
       </c>
       <c r="F36" t="n">
-        <v>56946743</v>
+        <v>139021506</v>
       </c>
       <c r="G36" t="n">
-        <v>0.95014</v>
+        <v>3.2917</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>EZETH</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Renzo Restaked ETH</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>55.19</v>
+        <v>3237.11</v>
       </c>
       <c r="E37" t="n">
-        <v>3315645562</v>
+        <v>3227342167</v>
       </c>
       <c r="F37" t="n">
-        <v>10160155</v>
+        <v>76829365</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.332</v>
+        <v>5.24272</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.090183</v>
+        <v>53.13</v>
       </c>
       <c r="E38" t="n">
-        <v>3245321661</v>
+        <v>3194753925</v>
       </c>
       <c r="F38" t="n">
-        <v>47450271</v>
+        <v>4785082</v>
       </c>
       <c r="G38" t="n">
-        <v>11.16918</v>
+        <v>1.50823</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1.2</v>
+        <v>2.16</v>
       </c>
       <c r="E39" t="n">
-        <v>3199726355</v>
+        <v>3147743787</v>
       </c>
       <c r="F39" t="n">
-        <v>212985096</v>
+        <v>45642754</v>
       </c>
       <c r="G39" t="n">
-        <v>6.11965</v>
+        <v>3.17299</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>XT</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>XT.com</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>2.18</v>
+        <v>3.13</v>
       </c>
       <c r="E40" t="n">
-        <v>3185371557</v>
+        <v>3138034436</v>
       </c>
       <c r="F40" t="n">
-        <v>53228825</v>
+        <v>742336</v>
       </c>
       <c r="G40" t="n">
-        <v>7.53123</v>
+        <v>4.62931</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>EZETH</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Renzo Restaked ETH</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>3189.96</v>
+        <v>8.09</v>
       </c>
       <c r="E41" t="n">
-        <v>3183532399</v>
+        <v>3133954511</v>
       </c>
       <c r="F41" t="n">
-        <v>79980860</v>
+        <v>97679653</v>
       </c>
       <c r="G41" t="n">
-        <v>3.62206</v>
+        <v>2.16761</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>Pepe</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>473.03</v>
+        <v>7.37e-06</v>
       </c>
       <c r="E42" t="n">
-        <v>3151141869</v>
+        <v>3098542896</v>
       </c>
       <c r="F42" t="n">
-        <v>32710880</v>
+        <v>669852942</v>
       </c>
       <c r="G42" t="n">
-        <v>7.7267</v>
+        <v>6.81877</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.04224241</v>
+        <v>1.12</v>
       </c>
       <c r="E43" t="n">
-        <v>3080340150</v>
+        <v>2970633387</v>
       </c>
       <c r="F43" t="n">
-        <v>69364566</v>
+        <v>348154838</v>
       </c>
       <c r="G43" t="n">
-        <v>3.454</v>
+        <v>6.60358</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>WIF</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>dogwifhat</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>3.04</v>
+        <v>0.03964638</v>
       </c>
       <c r="E44" t="n">
-        <v>3050200015</v>
+        <v>2888436480</v>
       </c>
       <c r="F44" t="n">
-        <v>601623097</v>
+        <v>48118811</v>
       </c>
       <c r="G44" t="n">
-        <v>10.44023</v>
+        <v>2.84993</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>3058.8</v>
+        <v>427.75</v>
       </c>
       <c r="E45" t="n">
-        <v>2837429305</v>
+        <v>2852288918</v>
       </c>
       <c r="F45" t="n">
-        <v>104402686</v>
+        <v>19784582</v>
       </c>
       <c r="G45" t="n">
-        <v>0.49827</v>
+        <v>2.94756</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.117434</v>
+        <v>3061.68</v>
       </c>
       <c r="E46" t="n">
-        <v>2716928958</v>
+        <v>2832605504</v>
       </c>
       <c r="F46" t="n">
-        <v>33345159</v>
+        <v>95132555</v>
       </c>
       <c r="G46" t="n">
-        <v>1.74528</v>
+        <v>5.36623</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.28424</v>
+        <v>2.64</v>
       </c>
       <c r="E47" t="n">
-        <v>2700089429</v>
+        <v>2776157258</v>
       </c>
       <c r="F47" t="n">
-        <v>95829464</v>
+        <v>431748611</v>
       </c>
       <c r="G47" t="n">
-        <v>4.70704</v>
+        <v>14.87225</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>WIF</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>dogwifhat</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>28.99</v>
+        <v>2.73</v>
       </c>
       <c r="E48" t="n">
-        <v>2619707541</v>
+        <v>2723643176</v>
       </c>
       <c r="F48" t="n">
-        <v>121917233</v>
+        <v>317126823</v>
       </c>
       <c r="G48" t="n">
-        <v>5.06998</v>
+        <v>1.04446</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>WEETH</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Wrapped eETH</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>2.47</v>
+        <v>3405.45</v>
       </c>
       <c r="E49" t="n">
-        <v>2589251372</v>
+        <v>2716518222</v>
       </c>
       <c r="F49" t="n">
-        <v>206107489</v>
+        <v>33378922</v>
       </c>
       <c r="G49" t="n">
-        <v>8.021940000000001</v>
+        <v>4.93554</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>FET</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Fetch.ai</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>2.45</v>
+        <v>0.111848</v>
       </c>
       <c r="E50" t="n">
-        <v>2573943317</v>
+        <v>2584743947</v>
       </c>
       <c r="F50" t="n">
-        <v>369802036</v>
+        <v>44428073</v>
       </c>
       <c r="G50" t="n">
-        <v>10.52097</v>
+        <v>0.15864</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Pepe</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>6.01e-06</v>
+        <v>0.262865</v>
       </c>
       <c r="E51" t="n">
-        <v>2532730982</v>
+        <v>2496616408</v>
       </c>
       <c r="F51" t="n">
-        <v>723356028</v>
+        <v>67095824</v>
       </c>
       <c r="G51" t="n">
-        <v>17.65564</v>
+        <v>0.88644</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-05-05
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>63488</v>
+        <v>63715</v>
       </c>
       <c r="E2" t="n">
-        <v>1251266030203</v>
+        <v>1255762952937</v>
       </c>
       <c r="F2" t="n">
-        <v>16951389959</v>
+        <v>17370474932</v>
       </c>
       <c r="G2" t="n">
-        <v>0.65895</v>
+        <v>-0.29686</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3286.75</v>
+        <v>3130.78</v>
       </c>
       <c r="E3" t="n">
-        <v>401721209804</v>
+        <v>376603418229</v>
       </c>
       <c r="F3" t="n">
-        <v>13502862795</v>
+        <v>8763130860</v>
       </c>
       <c r="G3" t="n">
-        <v>4.76128</v>
+        <v>-0.28135</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999579</v>
+        <v>0.999902</v>
       </c>
       <c r="E4" t="n">
-        <v>110542916254</v>
+        <v>110873401630</v>
       </c>
       <c r="F4" t="n">
-        <v>18832345482</v>
+        <v>25225379420</v>
       </c>
       <c r="G4" t="n">
-        <v>0.02277</v>
+        <v>-0.02078</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>601.6900000000001</v>
+        <v>585.74</v>
       </c>
       <c r="E5" t="n">
-        <v>92675069960</v>
+        <v>90173064375</v>
       </c>
       <c r="F5" t="n">
-        <v>721687671</v>
+        <v>635538159</v>
       </c>
       <c r="G5" t="n">
-        <v>2.27929</v>
+        <v>-0.77922</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>141.38</v>
+        <v>146.05</v>
       </c>
       <c r="E6" t="n">
-        <v>63295584877</v>
+        <v>65529412496</v>
       </c>
       <c r="F6" t="n">
-        <v>2380296592</v>
+        <v>3131231336</v>
       </c>
       <c r="G6" t="n">
-        <v>3.20119</v>
+        <v>-0.789</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.999716</v>
+        <v>0.99929</v>
       </c>
       <c r="E7" t="n">
-        <v>33507244349</v>
+        <v>33571337848</v>
       </c>
       <c r="F7" t="n">
-        <v>4449551523</v>
+        <v>5520914577</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.03693</v>
+        <v>-0.08293</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>3286.35</v>
+        <v>3131.44</v>
       </c>
       <c r="E8" t="n">
-        <v>30765593133</v>
+        <v>29347777369</v>
       </c>
       <c r="F8" t="n">
-        <v>92147431</v>
+        <v>48847870</v>
       </c>
       <c r="G8" t="n">
-        <v>4.89726</v>
+        <v>-0.19961</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.517728</v>
+        <v>0.528321</v>
       </c>
       <c r="E9" t="n">
-        <v>28616045471</v>
+        <v>29221706776</v>
       </c>
       <c r="F9" t="n">
-        <v>516211197</v>
+        <v>553316388</v>
       </c>
       <c r="G9" t="n">
-        <v>0.40678</v>
+        <v>-1.29514</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.148723</v>
+        <v>0.160376</v>
       </c>
       <c r="E10" t="n">
-        <v>21443343857</v>
+        <v>23139460998</v>
       </c>
       <c r="F10" t="n">
-        <v>702088757</v>
+        <v>2522810945</v>
       </c>
       <c r="G10" t="n">
-        <v>2.51809</v>
+        <v>0.3014</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>5.45</v>
+        <v>5.75</v>
       </c>
       <c r="E11" t="n">
-        <v>18937900907</v>
+        <v>20046557385</v>
       </c>
       <c r="F11" t="n">
-        <v>163757771</v>
+        <v>177504637</v>
       </c>
       <c r="G11" t="n">
-        <v>3.73112</v>
+        <v>0.17876</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.467783</v>
+        <v>0.456519</v>
       </c>
       <c r="E12" t="n">
-        <v>16535064095</v>
+        <v>16163549142</v>
       </c>
       <c r="F12" t="n">
-        <v>261054090</v>
+        <v>250731059</v>
       </c>
       <c r="G12" t="n">
-        <v>2.67533</v>
+        <v>-2.83631</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2.456e-05</v>
+        <v>2.466e-05</v>
       </c>
       <c r="E13" t="n">
-        <v>14486163800</v>
+        <v>14570427080</v>
       </c>
       <c r="F13" t="n">
-        <v>344333433</v>
+        <v>562756528</v>
       </c>
       <c r="G13" t="n">
-        <v>0.715</v>
+        <v>-3.40666</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>34.4</v>
+        <v>36.89</v>
       </c>
       <c r="E14" t="n">
-        <v>13034887033</v>
+        <v>14031422692</v>
       </c>
       <c r="F14" t="n">
-        <v>310883405</v>
+        <v>495062915</v>
       </c>
       <c r="G14" t="n">
-        <v>0.95145</v>
+        <v>2.57879</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.121092</v>
+        <v>0.121154</v>
       </c>
       <c r="E15" t="n">
-        <v>10614772091</v>
+        <v>10616002690</v>
       </c>
       <c r="F15" t="n">
-        <v>251070783</v>
+        <v>250269645</v>
       </c>
       <c r="G15" t="n">
-        <v>0.79</v>
+        <v>-1.62527</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>63545</v>
+        <v>63614</v>
       </c>
       <c r="E16" t="n">
-        <v>9878528213</v>
+        <v>9885751780</v>
       </c>
       <c r="F16" t="n">
-        <v>284359962</v>
+        <v>153718717</v>
       </c>
       <c r="G16" t="n">
-        <v>0.83538</v>
+        <v>-0.41951</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>477.98</v>
+        <v>7.05</v>
       </c>
       <c r="E17" t="n">
-        <v>9424278716</v>
+        <v>9614535142</v>
       </c>
       <c r="F17" t="n">
-        <v>231262089</v>
+        <v>148223024</v>
       </c>
       <c r="G17" t="n">
-        <v>1.34032</v>
+        <v>-1.57791</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>6.82</v>
+        <v>462.83</v>
       </c>
       <c r="E18" t="n">
-        <v>9258124401</v>
+        <v>9136636752</v>
       </c>
       <c r="F18" t="n">
-        <v>140412822</v>
+        <v>230303298</v>
       </c>
       <c r="G18" t="n">
-        <v>2.40286</v>
+        <v>-2.23545</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>14.04</v>
+        <v>14.26</v>
       </c>
       <c r="E19" t="n">
-        <v>8254974336</v>
+        <v>8383312870</v>
       </c>
       <c r="F19" t="n">
-        <v>281480770</v>
+        <v>235240482</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.4885</v>
+        <v>0.2694</v>
       </c>
     </row>
     <row r="20">
@@ -971,16 +971,16 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>7.23</v>
+        <v>7.1</v>
       </c>
       <c r="E20" t="n">
-        <v>7747521248</v>
+        <v>7615438426</v>
       </c>
       <c r="F20" t="n">
-        <v>670497251</v>
+        <v>286576740</v>
       </c>
       <c r="G20" t="n">
-        <v>5.45859</v>
+        <v>3.86795</v>
       </c>
     </row>
     <row r="21">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.725945</v>
+        <v>0.732311</v>
       </c>
       <c r="E21" t="n">
-        <v>6748832234</v>
+        <v>6810152586</v>
       </c>
       <c r="F21" t="n">
-        <v>283000054</v>
+        <v>187790863</v>
       </c>
       <c r="G21" t="n">
-        <v>4.23283</v>
+        <v>0.03065</v>
       </c>
     </row>
     <row r="22">
@@ -1025,16 +1025,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>84.01000000000001</v>
+        <v>80.89</v>
       </c>
       <c r="E22" t="n">
-        <v>6260460660</v>
+        <v>6038089372</v>
       </c>
       <c r="F22" t="n">
-        <v>352925134</v>
+        <v>244743312</v>
       </c>
       <c r="G22" t="n">
-        <v>-1.59217</v>
+        <v>-1.7276</v>
       </c>
     </row>
     <row r="23">
@@ -1052,16 +1052,16 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>13.53</v>
+        <v>12.89</v>
       </c>
       <c r="E23" t="n">
-        <v>6259219232</v>
+        <v>5985213594</v>
       </c>
       <c r="F23" t="n">
-        <v>108246132</v>
+        <v>108591653</v>
       </c>
       <c r="G23" t="n">
-        <v>4.32893</v>
+        <v>-3.53464</v>
       </c>
     </row>
     <row r="24">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>8</v>
+        <v>7.41</v>
       </c>
       <c r="E24" t="n">
-        <v>6037159757</v>
+        <v>5604865212</v>
       </c>
       <c r="F24" t="n">
-        <v>105914827</v>
+        <v>109649934</v>
       </c>
       <c r="G24" t="n">
-        <v>4.45935</v>
+        <v>-1.82244</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>FET</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Fetch.ai</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>5.77</v>
+        <v>2.2</v>
       </c>
       <c r="E25" t="n">
-        <v>5353560880</v>
+        <v>5570010786</v>
       </c>
       <c r="F25" t="n">
-        <v>1115193</v>
+        <v>233439366</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.18576</v>
+        <v>0.34556</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.9990869999999999</v>
+        <v>0.999424</v>
       </c>
       <c r="E26" t="n">
-        <v>5300051791</v>
+        <v>5439942790</v>
       </c>
       <c r="F26" t="n">
-        <v>341533742</v>
+        <v>500299494</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.04717</v>
+        <v>-0.06643</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>FDUSD</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>First Digital USD</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.999356</v>
+        <v>5.76</v>
       </c>
       <c r="E27" t="n">
-        <v>4421963328</v>
+        <v>5321884361</v>
       </c>
       <c r="F27" t="n">
-        <v>4223605304</v>
+        <v>1036789</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.41116</v>
+        <v>-2.04791</v>
       </c>
     </row>
     <row r="28">
@@ -1187,16 +1187,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>28.64</v>
+        <v>26.83</v>
       </c>
       <c r="E28" t="n">
-        <v>4208131568</v>
+        <v>3954726449</v>
       </c>
       <c r="F28" t="n">
-        <v>292584727</v>
+        <v>138473074</v>
       </c>
       <c r="G28" t="n">
-        <v>7.47523</v>
+        <v>-0.95644</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>8.99</v>
+        <v>0.108682</v>
       </c>
       <c r="E29" t="n">
-        <v>3845874138</v>
+        <v>3895222731</v>
       </c>
       <c r="F29" t="n">
-        <v>94904639</v>
+        <v>99877542</v>
       </c>
       <c r="G29" t="n">
-        <v>2.51416</v>
+        <v>-0.23268</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.104187</v>
+        <v>9.039999999999999</v>
       </c>
       <c r="E30" t="n">
-        <v>3730540254</v>
+        <v>3870674109</v>
       </c>
       <c r="F30" t="n">
-        <v>127272948</v>
+        <v>100797837</v>
       </c>
       <c r="G30" t="n">
-        <v>-2.67316</v>
+        <v>-1.52464</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>FDUSD</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>First Digital USD</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>2.52</v>
+        <v>0.999702</v>
       </c>
       <c r="E31" t="n">
-        <v>3670743372</v>
+        <v>3851112521</v>
       </c>
       <c r="F31" t="n">
-        <v>50466822</v>
+        <v>3420858087</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.30715</v>
+        <v>0.00936</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>1.1</v>
+        <v>9.31</v>
       </c>
       <c r="E32" t="n">
-        <v>3593450469</v>
+        <v>3612223328</v>
       </c>
       <c r="F32" t="n">
-        <v>38972817</v>
+        <v>222383049</v>
       </c>
       <c r="G32" t="n">
-        <v>3.00505</v>
+        <v>7.28763</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Pepe</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.128041</v>
+        <v>8.49e-06</v>
       </c>
       <c r="E33" t="n">
-        <v>3418998297</v>
+        <v>3568422236</v>
       </c>
       <c r="F33" t="n">
-        <v>12572539</v>
+        <v>794437951</v>
       </c>
       <c r="G33" t="n">
-        <v>3.33036</v>
+        <v>-3.24556</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.114372</v>
+        <v>0.131978</v>
       </c>
       <c r="E34" t="n">
-        <v>3313398133</v>
+        <v>3531686555</v>
       </c>
       <c r="F34" t="n">
-        <v>49343280</v>
+        <v>8920661</v>
       </c>
       <c r="G34" t="n">
-        <v>1.43716</v>
+        <v>-2.00962</v>
       </c>
     </row>
     <row r="35">
@@ -1376,16 +1376,16 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>8.31</v>
+        <v>8.85</v>
       </c>
       <c r="E35" t="n">
-        <v>3249455817</v>
+        <v>3463237811</v>
       </c>
       <c r="F35" t="n">
-        <v>86327410</v>
+        <v>164304035</v>
       </c>
       <c r="G35" t="n">
-        <v>1.30525</v>
+        <v>0.81311</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>5.95</v>
+        <v>1.042</v>
       </c>
       <c r="E36" t="n">
-        <v>3243569658</v>
+        <v>3404435412</v>
       </c>
       <c r="F36" t="n">
-        <v>139021506</v>
+        <v>45617338</v>
       </c>
       <c r="G36" t="n">
-        <v>3.2917</v>
+        <v>-1.05121</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>EZETH</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Renzo Restaked ETH</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>3237.11</v>
+        <v>2.31</v>
       </c>
       <c r="E37" t="n">
-        <v>3227342167</v>
+        <v>3381979948</v>
       </c>
       <c r="F37" t="n">
-        <v>76829365</v>
+        <v>65097875</v>
       </c>
       <c r="G37" t="n">
-        <v>5.24272</v>
+        <v>-4.59003</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>WIF</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>dogwifhat</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>53.13</v>
+        <v>3.34</v>
       </c>
       <c r="E38" t="n">
-        <v>3194753925</v>
+        <v>3327025990</v>
       </c>
       <c r="F38" t="n">
-        <v>4785082</v>
+        <v>577580828</v>
       </c>
       <c r="G38" t="n">
-        <v>1.50823</v>
+        <v>-1.91548</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>2.16</v>
+        <v>6</v>
       </c>
       <c r="E39" t="n">
-        <v>3147743787</v>
+        <v>3293020844</v>
       </c>
       <c r="F39" t="n">
-        <v>45642754</v>
+        <v>121636321</v>
       </c>
       <c r="G39" t="n">
-        <v>3.17299</v>
+        <v>-2.27053</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>XT</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>XT.com</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>3.13</v>
+        <v>2.21</v>
       </c>
       <c r="E40" t="n">
-        <v>3138034436</v>
+        <v>3225875891</v>
       </c>
       <c r="F40" t="n">
-        <v>742336</v>
+        <v>40849830</v>
       </c>
       <c r="G40" t="n">
-        <v>4.62931</v>
+        <v>-0.39315</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>8.09</v>
+        <v>0.110094</v>
       </c>
       <c r="E41" t="n">
-        <v>3133954511</v>
+        <v>3190169472</v>
       </c>
       <c r="F41" t="n">
-        <v>97679653</v>
+        <v>42863956</v>
       </c>
       <c r="G41" t="n">
-        <v>2.16761</v>
+        <v>-1.41801</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>WEETH</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Pepe</t>
+          <t>Wrapped eETH</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>7.37e-06</v>
+        <v>3245.74</v>
       </c>
       <c r="E42" t="n">
-        <v>3098542896</v>
+        <v>3121062474</v>
       </c>
       <c r="F42" t="n">
-        <v>669852942</v>
+        <v>37272846</v>
       </c>
       <c r="G42" t="n">
-        <v>6.81877</v>
+        <v>-0.15604</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>EZETH</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Renzo Restaked ETH</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1.12</v>
+        <v>3083.09</v>
       </c>
       <c r="E43" t="n">
-        <v>2970633387</v>
+        <v>3078346946</v>
       </c>
       <c r="F43" t="n">
-        <v>348154838</v>
+        <v>26804255</v>
       </c>
       <c r="G43" t="n">
-        <v>6.60358</v>
+        <v>-0.02081</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.03964638</v>
+        <v>51.18</v>
       </c>
       <c r="E44" t="n">
-        <v>2888436480</v>
+        <v>3071344610</v>
       </c>
       <c r="F44" t="n">
-        <v>48118811</v>
+        <v>5749835</v>
       </c>
       <c r="G44" t="n">
-        <v>2.84993</v>
+        <v>0.57407</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>427.75</v>
+        <v>2.89</v>
       </c>
       <c r="E45" t="n">
-        <v>2852288918</v>
+        <v>3023067081</v>
       </c>
       <c r="F45" t="n">
-        <v>19784582</v>
+        <v>262692274</v>
       </c>
       <c r="G45" t="n">
-        <v>2.94756</v>
+        <v>-1.79478</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>XT</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>XT.com</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>3061.68</v>
+        <v>2.98</v>
       </c>
       <c r="E46" t="n">
-        <v>2832605504</v>
+        <v>2980539272</v>
       </c>
       <c r="F46" t="n">
-        <v>95132555</v>
+        <v>659540</v>
       </c>
       <c r="G46" t="n">
-        <v>5.36623</v>
+        <v>-5.48551</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>2.64</v>
+        <v>435.37</v>
       </c>
       <c r="E47" t="n">
-        <v>2776157258</v>
+        <v>2932471137</v>
       </c>
       <c r="F47" t="n">
-        <v>431748611</v>
+        <v>28005813</v>
       </c>
       <c r="G47" t="n">
-        <v>14.87225</v>
+        <v>-2.2754</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>WIF</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>dogwifhat</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>2.73</v>
+        <v>1.05</v>
       </c>
       <c r="E48" t="n">
-        <v>2723643176</v>
+        <v>2787204227</v>
       </c>
       <c r="F48" t="n">
-        <v>317126823</v>
+        <v>216046746</v>
       </c>
       <c r="G48" t="n">
-        <v>1.04446</v>
+        <v>-2.09126</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>WEETH</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Wrapped eETH</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>3405.45</v>
+        <v>2909.65</v>
       </c>
       <c r="E49" t="n">
-        <v>2716518222</v>
+        <v>2698000940</v>
       </c>
       <c r="F49" t="n">
-        <v>33378922</v>
+        <v>71951152</v>
       </c>
       <c r="G49" t="n">
-        <v>4.93554</v>
+        <v>-0.54273</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.111848</v>
+        <v>0.03693267</v>
       </c>
       <c r="E50" t="n">
-        <v>2584743947</v>
+        <v>2692056731</v>
       </c>
       <c r="F50" t="n">
-        <v>44428073</v>
+        <v>46001947</v>
       </c>
       <c r="G50" t="n">
-        <v>0.15864</v>
+        <v>-0.77693</v>
       </c>
     </row>
     <row r="51">
@@ -1808,16 +1808,16 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.262865</v>
+        <v>0.278586</v>
       </c>
       <c r="E51" t="n">
-        <v>2496616408</v>
+        <v>2651767808</v>
       </c>
       <c r="F51" t="n">
-        <v>67095824</v>
+        <v>85567902</v>
       </c>
       <c r="G51" t="n">
-        <v>0.88644</v>
+        <v>-1.9587</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-05-12
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>63715</v>
+        <v>61104</v>
       </c>
       <c r="E2" t="n">
-        <v>1255762952937</v>
+        <v>1203494574653</v>
       </c>
       <c r="F2" t="n">
-        <v>17370474932</v>
+        <v>12363680338</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.29686</v>
+        <v>0.56187</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3130.78</v>
+        <v>2926.93</v>
       </c>
       <c r="E3" t="n">
-        <v>376603418229</v>
+        <v>351603917193</v>
       </c>
       <c r="F3" t="n">
-        <v>8763130860</v>
+        <v>5634080405</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.28135</v>
+        <v>0.7301800000000001</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999902</v>
+        <v>0.99978</v>
       </c>
       <c r="E4" t="n">
-        <v>110873401630</v>
+        <v>110823059182</v>
       </c>
       <c r="F4" t="n">
-        <v>25225379420</v>
+        <v>20087751557</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.02078</v>
+        <v>0.03389</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>585.74</v>
+        <v>593.3200000000001</v>
       </c>
       <c r="E5" t="n">
-        <v>90173064375</v>
+        <v>91270299632</v>
       </c>
       <c r="F5" t="n">
-        <v>635538159</v>
+        <v>515291294</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.77922</v>
+        <v>0.60704</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>146.05</v>
+        <v>145.21</v>
       </c>
       <c r="E6" t="n">
-        <v>65529412496</v>
+        <v>65128845258</v>
       </c>
       <c r="F6" t="n">
-        <v>3131231336</v>
+        <v>1118899080</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.789</v>
+        <v>0.40865</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.99929</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>33571337848</v>
+        <v>33130304606</v>
       </c>
       <c r="F7" t="n">
-        <v>5520914577</v>
+        <v>2732154575</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.08293</v>
+        <v>0.00546</v>
       </c>
     </row>
     <row r="8">
@@ -638,25 +638,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>STETH</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Lido Staked Ether</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>3131.44</v>
+        <v>0.504237</v>
       </c>
       <c r="E8" t="n">
-        <v>29347777369</v>
+        <v>27910099562</v>
       </c>
       <c r="F8" t="n">
-        <v>48847870</v>
+        <v>346462825</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.19961</v>
+        <v>0.20126</v>
       </c>
     </row>
     <row r="9">
@@ -665,25 +665,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>STETH</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>Lido Staked Ether</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.528321</v>
+        <v>2925.7</v>
       </c>
       <c r="E9" t="n">
-        <v>29221706776</v>
+        <v>27401981511</v>
       </c>
       <c r="F9" t="n">
-        <v>553316388</v>
+        <v>27041451</v>
       </c>
       <c r="G9" t="n">
-        <v>-1.29514</v>
+        <v>0.7047099999999999</v>
       </c>
     </row>
     <row r="10">
@@ -692,25 +692,25 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>DOGE</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Dogecoin</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.160376</v>
+        <v>7.03</v>
       </c>
       <c r="E10" t="n">
-        <v>23139460998</v>
+        <v>24371890771</v>
       </c>
       <c r="F10" t="n">
-        <v>2522810945</v>
+        <v>280741207</v>
       </c>
       <c r="G10" t="n">
-        <v>0.3014</v>
+        <v>4.90691</v>
       </c>
     </row>
     <row r="11">
@@ -719,25 +719,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>DOGE</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Dogecoin</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>5.75</v>
+        <v>0.142743</v>
       </c>
       <c r="E11" t="n">
-        <v>20046557385</v>
+        <v>20626235301</v>
       </c>
       <c r="F11" t="n">
-        <v>177504637</v>
+        <v>607572981</v>
       </c>
       <c r="G11" t="n">
-        <v>0.17876</v>
+        <v>-0.64562</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.456519</v>
+        <v>0.439853</v>
       </c>
       <c r="E12" t="n">
-        <v>16163549142</v>
+        <v>15559954945</v>
       </c>
       <c r="F12" t="n">
-        <v>250731059</v>
+        <v>161066423</v>
       </c>
       <c r="G12" t="n">
-        <v>-2.83631</v>
+        <v>-0.86084</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2.466e-05</v>
+        <v>2.251e-05</v>
       </c>
       <c r="E13" t="n">
-        <v>14570427080</v>
+        <v>13282895467</v>
       </c>
       <c r="F13" t="n">
-        <v>562756528</v>
+        <v>187059494</v>
       </c>
       <c r="G13" t="n">
-        <v>-3.40666</v>
+        <v>-0.29554</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>36.89</v>
+        <v>33.7</v>
       </c>
       <c r="E14" t="n">
-        <v>14031422692</v>
+        <v>12881563701</v>
       </c>
       <c r="F14" t="n">
-        <v>495062915</v>
+        <v>205379624</v>
       </c>
       <c r="G14" t="n">
-        <v>2.57879</v>
+        <v>0.83646</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.121154</v>
+        <v>0.126671</v>
       </c>
       <c r="E15" t="n">
-        <v>10616002690</v>
+        <v>11080231569</v>
       </c>
       <c r="F15" t="n">
-        <v>250269645</v>
+        <v>222040447</v>
       </c>
       <c r="G15" t="n">
-        <v>-1.62527</v>
+        <v>0.04657</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>63614</v>
+        <v>61145</v>
       </c>
       <c r="E16" t="n">
-        <v>9885751780</v>
+        <v>9491996464</v>
       </c>
       <c r="F16" t="n">
-        <v>153718717</v>
+        <v>81669094</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.41951</v>
+        <v>0.65043</v>
       </c>
     </row>
     <row r="17">
@@ -890,16 +890,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>7.05</v>
+        <v>6.73</v>
       </c>
       <c r="E17" t="n">
-        <v>9614535142</v>
+        <v>9185077286</v>
       </c>
       <c r="F17" t="n">
-        <v>148223024</v>
+        <v>99309899</v>
       </c>
       <c r="G17" t="n">
-        <v>-1.57791</v>
+        <v>0.37324</v>
       </c>
     </row>
     <row r="18">
@@ -917,16 +917,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>462.83</v>
+        <v>435.06</v>
       </c>
       <c r="E18" t="n">
-        <v>9136636752</v>
+        <v>8576584447</v>
       </c>
       <c r="F18" t="n">
-        <v>230303298</v>
+        <v>126456076</v>
       </c>
       <c r="G18" t="n">
-        <v>-2.23545</v>
+        <v>1.31722</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>14.26</v>
+        <v>13.44</v>
       </c>
       <c r="E19" t="n">
-        <v>8383312870</v>
+        <v>7900225468</v>
       </c>
       <c r="F19" t="n">
-        <v>235240482</v>
+        <v>188113916</v>
       </c>
       <c r="G19" t="n">
-        <v>0.2694</v>
+        <v>-0.57428</v>
       </c>
     </row>
     <row r="20">
@@ -971,16 +971,16 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>7.1</v>
+        <v>6.95</v>
       </c>
       <c r="E20" t="n">
-        <v>7615438426</v>
+        <v>7453224300</v>
       </c>
       <c r="F20" t="n">
-        <v>286576740</v>
+        <v>252845305</v>
       </c>
       <c r="G20" t="n">
-        <v>3.86795</v>
+        <v>-1.70197</v>
       </c>
     </row>
     <row r="21">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.732311</v>
+        <v>0.678713</v>
       </c>
       <c r="E21" t="n">
-        <v>6810152586</v>
+        <v>6306894989</v>
       </c>
       <c r="F21" t="n">
-        <v>187790863</v>
+        <v>137243398</v>
       </c>
       <c r="G21" t="n">
-        <v>0.03065</v>
+        <v>-0.48911</v>
       </c>
     </row>
     <row r="22">
@@ -1025,16 +1025,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>80.89</v>
+        <v>81.48</v>
       </c>
       <c r="E22" t="n">
-        <v>6038089372</v>
+        <v>6072821910</v>
       </c>
       <c r="F22" t="n">
-        <v>244743312</v>
+        <v>202169810</v>
       </c>
       <c r="G22" t="n">
-        <v>-1.7276</v>
+        <v>-0.57816</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>FET</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Fetch.ai</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>12.89</v>
+        <v>2.2</v>
       </c>
       <c r="E23" t="n">
-        <v>5985213594</v>
+        <v>5558569059</v>
       </c>
       <c r="F23" t="n">
-        <v>108591653</v>
+        <v>125335431</v>
       </c>
       <c r="G23" t="n">
-        <v>-3.53464</v>
+        <v>-0.78065</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>7.41</v>
+        <v>11.83</v>
       </c>
       <c r="E24" t="n">
-        <v>5604865212</v>
+        <v>5494792187</v>
       </c>
       <c r="F24" t="n">
-        <v>109649934</v>
+        <v>59699771</v>
       </c>
       <c r="G24" t="n">
-        <v>-1.82244</v>
+        <v>-0.92692</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>FET</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Fetch.ai</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>2.2</v>
+        <v>0.999709</v>
       </c>
       <c r="E25" t="n">
-        <v>5570010786</v>
+        <v>5473476264</v>
       </c>
       <c r="F25" t="n">
-        <v>233439366</v>
+        <v>634862514</v>
       </c>
       <c r="G25" t="n">
-        <v>0.34556</v>
+        <v>-0.01465</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.999424</v>
+        <v>5.9</v>
       </c>
       <c r="E26" t="n">
-        <v>5439942790</v>
+        <v>5459889666</v>
       </c>
       <c r="F26" t="n">
-        <v>500299494</v>
+        <v>1568276</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.06643</v>
+        <v>0.31157</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>5.76</v>
+        <v>7.11</v>
       </c>
       <c r="E27" t="n">
-        <v>5321884361</v>
+        <v>5363060020</v>
       </c>
       <c r="F27" t="n">
-        <v>1036789</v>
+        <v>86439897</v>
       </c>
       <c r="G27" t="n">
-        <v>-2.04791</v>
+        <v>0.52007</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>26.83</v>
+        <v>11.03</v>
       </c>
       <c r="E28" t="n">
-        <v>3954726449</v>
+        <v>4296394894</v>
       </c>
       <c r="F28" t="n">
-        <v>138473074</v>
+        <v>198928600</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.95644</v>
+        <v>1.92776</v>
       </c>
     </row>
     <row r="29">
@@ -1214,16 +1214,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.108682</v>
+        <v>0.110663</v>
       </c>
       <c r="E29" t="n">
-        <v>3895222731</v>
+        <v>3949696675</v>
       </c>
       <c r="F29" t="n">
-        <v>99877542</v>
+        <v>53147580</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.23268</v>
+        <v>3.23655</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>9.039999999999999</v>
+        <v>26.69</v>
       </c>
       <c r="E30" t="n">
-        <v>3870674109</v>
+        <v>3925985861</v>
       </c>
       <c r="F30" t="n">
-        <v>100797837</v>
+        <v>90448714</v>
       </c>
       <c r="G30" t="n">
-        <v>-1.52464</v>
+        <v>0.83439</v>
       </c>
     </row>
     <row r="31">
@@ -1268,16 +1268,16 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.999702</v>
+        <v>1</v>
       </c>
       <c r="E31" t="n">
-        <v>3851112521</v>
+        <v>3815889177</v>
       </c>
       <c r="F31" t="n">
-        <v>3420858087</v>
+        <v>3224194212</v>
       </c>
       <c r="G31" t="n">
-        <v>0.00936</v>
+        <v>-0.02008</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>Pepe</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>9.31</v>
+        <v>8.67e-06</v>
       </c>
       <c r="E32" t="n">
-        <v>3612223328</v>
+        <v>3649848628</v>
       </c>
       <c r="F32" t="n">
-        <v>222383049</v>
+        <v>429447213</v>
       </c>
       <c r="G32" t="n">
-        <v>7.28763</v>
+        <v>2.22099</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Pepe</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>8.49e-06</v>
+        <v>8.41</v>
       </c>
       <c r="E33" t="n">
-        <v>3568422236</v>
+        <v>3611222310</v>
       </c>
       <c r="F33" t="n">
-        <v>794437951</v>
+        <v>48373512</v>
       </c>
       <c r="G33" t="n">
-        <v>-3.24556</v>
+        <v>0.15684</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.131978</v>
+        <v>8.58</v>
       </c>
       <c r="E34" t="n">
-        <v>3531686555</v>
+        <v>3355493362</v>
       </c>
       <c r="F34" t="n">
-        <v>8920661</v>
+        <v>99896835</v>
       </c>
       <c r="G34" t="n">
-        <v>-2.00962</v>
+        <v>-0.05023</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>8.85</v>
+        <v>0.124056</v>
       </c>
       <c r="E35" t="n">
-        <v>3463237811</v>
+        <v>3315125367</v>
       </c>
       <c r="F35" t="n">
-        <v>164304035</v>
+        <v>8115194</v>
       </c>
       <c r="G35" t="n">
-        <v>0.81311</v>
+        <v>-0.24031</v>
       </c>
     </row>
     <row r="36">
@@ -1403,16 +1403,16 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1.042</v>
+        <v>1.01</v>
       </c>
       <c r="E36" t="n">
-        <v>3404435412</v>
+        <v>3298484571</v>
       </c>
       <c r="F36" t="n">
-        <v>45617338</v>
+        <v>45519080</v>
       </c>
       <c r="G36" t="n">
-        <v>-1.05121</v>
+        <v>0.15957</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>2.31</v>
+        <v>2.25</v>
       </c>
       <c r="E37" t="n">
-        <v>3381979948</v>
+        <v>3274684827</v>
       </c>
       <c r="F37" t="n">
-        <v>65097875</v>
+        <v>58091866</v>
       </c>
       <c r="G37" t="n">
-        <v>-4.59003</v>
+        <v>0.26236</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>WIF</t>
+          <t>WEETH</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>dogwifhat</t>
+          <t>Wrapped eETH</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>3.34</v>
+        <v>3038.88</v>
       </c>
       <c r="E38" t="n">
-        <v>3327025990</v>
+        <v>3127787678</v>
       </c>
       <c r="F38" t="n">
-        <v>577580828</v>
+        <v>20156069</v>
       </c>
       <c r="G38" t="n">
-        <v>-1.91548</v>
+        <v>0.787</v>
       </c>
     </row>
     <row r="39">
@@ -1484,16 +1484,16 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>6</v>
+        <v>5.64</v>
       </c>
       <c r="E39" t="n">
-        <v>3293020844</v>
+        <v>3112314550</v>
       </c>
       <c r="F39" t="n">
-        <v>121636321</v>
+        <v>76316825</v>
       </c>
       <c r="G39" t="n">
-        <v>-2.27053</v>
+        <v>0.9496</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>2.21</v>
+        <v>0.105414</v>
       </c>
       <c r="E40" t="n">
-        <v>3225875891</v>
+        <v>3051115291</v>
       </c>
       <c r="F40" t="n">
-        <v>40849830</v>
+        <v>30043559</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.39315</v>
+        <v>-0.80449</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.110094</v>
+        <v>49.94</v>
       </c>
       <c r="E41" t="n">
-        <v>3190169472</v>
+        <v>2995043075</v>
       </c>
       <c r="F41" t="n">
-        <v>42863956</v>
+        <v>2712624</v>
       </c>
       <c r="G41" t="n">
-        <v>-1.41801</v>
+        <v>1.08076</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>WEETH</t>
+          <t>WIF</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Wrapped eETH</t>
+          <t>dogwifhat</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>3245.74</v>
+        <v>2.98</v>
       </c>
       <c r="E42" t="n">
-        <v>3121062474</v>
+        <v>2988678110</v>
       </c>
       <c r="F42" t="n">
-        <v>37272846</v>
+        <v>291328777</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.15604</v>
+        <v>-0.85681</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>EZETH</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Renzo Restaked ETH</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>3083.09</v>
+        <v>0.124618</v>
       </c>
       <c r="E43" t="n">
-        <v>3078346946</v>
+        <v>2934998933</v>
       </c>
       <c r="F43" t="n">
-        <v>26804255</v>
+        <v>21796106</v>
       </c>
       <c r="G43" t="n">
-        <v>-0.02081</v>
+        <v>0.08401</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>51.18</v>
+        <v>1.99</v>
       </c>
       <c r="E44" t="n">
-        <v>3071344610</v>
+        <v>2908293840</v>
       </c>
       <c r="F44" t="n">
-        <v>5749835</v>
+        <v>26951589</v>
       </c>
       <c r="G44" t="n">
-        <v>0.57407</v>
+        <v>-0.67747</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>EZETH</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Renzo Restaked ETH</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>2.89</v>
+        <v>2880.77</v>
       </c>
       <c r="E45" t="n">
-        <v>3023067081</v>
+        <v>2870481798</v>
       </c>
       <c r="F45" t="n">
-        <v>262692274</v>
+        <v>26251946</v>
       </c>
       <c r="G45" t="n">
-        <v>-1.79478</v>
+        <v>0.76324</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>XT</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>XT.com</t>
+          <t>Arweave</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>2.98</v>
+        <v>42.08</v>
       </c>
       <c r="E46" t="n">
-        <v>2980539272</v>
+        <v>2749163283</v>
       </c>
       <c r="F46" t="n">
-        <v>659540</v>
+        <v>98722764</v>
       </c>
       <c r="G46" t="n">
-        <v>-5.48551</v>
+        <v>3.42502</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>435.37</v>
+        <v>0.284524</v>
       </c>
       <c r="E47" t="n">
-        <v>2932471137</v>
+        <v>2702710102</v>
       </c>
       <c r="F47" t="n">
-        <v>28005813</v>
+        <v>77186920</v>
       </c>
       <c r="G47" t="n">
-        <v>-2.2754</v>
+        <v>-3.46272</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>1.05</v>
+        <v>2.56</v>
       </c>
       <c r="E48" t="n">
-        <v>2787204227</v>
+        <v>2676668928</v>
       </c>
       <c r="F48" t="n">
-        <v>216046746</v>
+        <v>91814297</v>
       </c>
       <c r="G48" t="n">
-        <v>-2.09126</v>
+        <v>0.22292</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>2909.65</v>
+        <v>1.002</v>
       </c>
       <c r="E49" t="n">
-        <v>2698000940</v>
+        <v>2661095585</v>
       </c>
       <c r="F49" t="n">
-        <v>71951152</v>
+        <v>130334444</v>
       </c>
       <c r="G49" t="n">
-        <v>-0.54273</v>
+        <v>0.50502</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.03693267</v>
+        <v>374.54</v>
       </c>
       <c r="E50" t="n">
-        <v>2692056731</v>
+        <v>2534911721</v>
       </c>
       <c r="F50" t="n">
-        <v>46001947</v>
+        <v>16741618</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.77693</v>
+        <v>0.2283</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>VET</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.278586</v>
+        <v>0.03462744</v>
       </c>
       <c r="E51" t="n">
-        <v>2651767808</v>
+        <v>2518990830</v>
       </c>
       <c r="F51" t="n">
-        <v>85567902</v>
+        <v>39645428</v>
       </c>
       <c r="G51" t="n">
-        <v>-1.9587</v>
+        <v>-0.97274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-05-19
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>61104</v>
+        <v>66967</v>
       </c>
       <c r="E2" t="n">
-        <v>1203494574653</v>
+        <v>1320519938913</v>
       </c>
       <c r="F2" t="n">
-        <v>12363680338</v>
+        <v>14474144487</v>
       </c>
       <c r="G2" t="n">
-        <v>0.56187</v>
+        <v>-0.17983</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2926.93</v>
+        <v>3086.61</v>
       </c>
       <c r="E3" t="n">
-        <v>351603917193</v>
+        <v>372369245273</v>
       </c>
       <c r="F3" t="n">
-        <v>5634080405</v>
+        <v>7025145548</v>
       </c>
       <c r="G3" t="n">
-        <v>0.7301800000000001</v>
+        <v>-1.28505</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.99978</v>
+        <v>0.999985</v>
       </c>
       <c r="E4" t="n">
-        <v>110823059182</v>
+        <v>111432469260</v>
       </c>
       <c r="F4" t="n">
-        <v>20087751557</v>
+        <v>23784105139</v>
       </c>
       <c r="G4" t="n">
-        <v>0.03389</v>
+        <v>-0.08263</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>593.3200000000001</v>
+        <v>578.89</v>
       </c>
       <c r="E5" t="n">
-        <v>91270299632</v>
+        <v>89096283294</v>
       </c>
       <c r="F5" t="n">
-        <v>515291294</v>
+        <v>493976681</v>
       </c>
       <c r="G5" t="n">
-        <v>0.60704</v>
+        <v>0.02361</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>145.21</v>
+        <v>169.98</v>
       </c>
       <c r="E6" t="n">
-        <v>65128845258</v>
+        <v>76840909683</v>
       </c>
       <c r="F6" t="n">
-        <v>1118899080</v>
+        <v>1924984517</v>
       </c>
       <c r="G6" t="n">
-        <v>0.40865</v>
+        <v>-2.20257</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0.99758</v>
       </c>
       <c r="E7" t="n">
-        <v>33130304606</v>
+        <v>33479633976</v>
       </c>
       <c r="F7" t="n">
-        <v>2732154575</v>
+        <v>2282575344</v>
       </c>
       <c r="G7" t="n">
-        <v>0.00546</v>
+        <v>-0.19551</v>
       </c>
     </row>
     <row r="8">
@@ -638,25 +638,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>STETH</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>Lido Staked Ether</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.504237</v>
+        <v>3085.81</v>
       </c>
       <c r="E8" t="n">
-        <v>27910099562</v>
+        <v>28979936067</v>
       </c>
       <c r="F8" t="n">
-        <v>346462825</v>
+        <v>55941511</v>
       </c>
       <c r="G8" t="n">
-        <v>0.20126</v>
+        <v>-1.26909</v>
       </c>
     </row>
     <row r="9">
@@ -665,25 +665,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>STETH</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Lido Staked Ether</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2925.7</v>
+        <v>0.514706</v>
       </c>
       <c r="E9" t="n">
-        <v>27401981511</v>
+        <v>28586230718</v>
       </c>
       <c r="F9" t="n">
-        <v>27041451</v>
+        <v>380731752</v>
       </c>
       <c r="G9" t="n">
-        <v>0.7047099999999999</v>
+        <v>-1.62378</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>7.03</v>
+        <v>6.42</v>
       </c>
       <c r="E10" t="n">
-        <v>24371890771</v>
+        <v>22397447049</v>
       </c>
       <c r="F10" t="n">
-        <v>280741207</v>
+        <v>200945328</v>
       </c>
       <c r="G10" t="n">
-        <v>4.90691</v>
+        <v>-0.8024</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.142743</v>
+        <v>0.15113</v>
       </c>
       <c r="E11" t="n">
-        <v>20626235301</v>
+        <v>21815222440</v>
       </c>
       <c r="F11" t="n">
-        <v>607572981</v>
+        <v>691667227</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.64562</v>
+        <v>-2.45723</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.439853</v>
+        <v>0.473242</v>
       </c>
       <c r="E12" t="n">
-        <v>15559954945</v>
+        <v>16752004740</v>
       </c>
       <c r="F12" t="n">
-        <v>161066423</v>
+        <v>202247949</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.86084</v>
+        <v>-1.45558</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2.251e-05</v>
+        <v>2.438e-05</v>
       </c>
       <c r="E13" t="n">
-        <v>13282895467</v>
+        <v>14408829482</v>
       </c>
       <c r="F13" t="n">
-        <v>187059494</v>
+        <v>310501157</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.29554</v>
+        <v>-2.14294</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>33.7</v>
+        <v>36.35</v>
       </c>
       <c r="E14" t="n">
-        <v>12881563701</v>
+        <v>13927846462</v>
       </c>
       <c r="F14" t="n">
-        <v>205379624</v>
+        <v>273448625</v>
       </c>
       <c r="G14" t="n">
-        <v>0.83646</v>
+        <v>-2.15134</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.126671</v>
+        <v>0.121066</v>
       </c>
       <c r="E15" t="n">
-        <v>11080231569</v>
+        <v>10610782583</v>
       </c>
       <c r="F15" t="n">
-        <v>222040447</v>
+        <v>227741888</v>
       </c>
       <c r="G15" t="n">
-        <v>0.04657</v>
+        <v>-2.19123</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>61145</v>
+        <v>67056</v>
       </c>
       <c r="E16" t="n">
-        <v>9491996464</v>
+        <v>10445875850</v>
       </c>
       <c r="F16" t="n">
-        <v>81669094</v>
+        <v>128505544</v>
       </c>
       <c r="G16" t="n">
-        <v>0.65043</v>
+        <v>-0.12081</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>6.73</v>
+        <v>16.51</v>
       </c>
       <c r="E17" t="n">
-        <v>9185077286</v>
+        <v>9700619238</v>
       </c>
       <c r="F17" t="n">
-        <v>99309899</v>
+        <v>490963145</v>
       </c>
       <c r="G17" t="n">
-        <v>0.37324</v>
+        <v>1.95408</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>435.06</v>
+        <v>7.04</v>
       </c>
       <c r="E18" t="n">
-        <v>8576584447</v>
+        <v>9674917047</v>
       </c>
       <c r="F18" t="n">
-        <v>126456076</v>
+        <v>114487709</v>
       </c>
       <c r="G18" t="n">
-        <v>1.31722</v>
+        <v>-1.70956</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>13.44</v>
+        <v>485.47</v>
       </c>
       <c r="E19" t="n">
-        <v>7900225468</v>
+        <v>9566413219</v>
       </c>
       <c r="F19" t="n">
-        <v>188113916</v>
+        <v>320120396</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.57428</v>
+        <v>0.14765</v>
       </c>
     </row>
     <row r="20">
@@ -971,16 +971,16 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>6.95</v>
+        <v>7.7</v>
       </c>
       <c r="E20" t="n">
-        <v>7453224300</v>
+        <v>8338012375</v>
       </c>
       <c r="F20" t="n">
-        <v>252845305</v>
+        <v>269472104</v>
       </c>
       <c r="G20" t="n">
-        <v>-1.70197</v>
+        <v>-3.45486</v>
       </c>
     </row>
     <row r="21">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.678713</v>
+        <v>0.691872</v>
       </c>
       <c r="E21" t="n">
-        <v>6306894989</v>
+        <v>6455330932</v>
       </c>
       <c r="F21" t="n">
-        <v>137243398</v>
+        <v>177425773</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.48911</v>
+        <v>-3.1812</v>
       </c>
     </row>
     <row r="22">
@@ -1025,16 +1025,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>81.48</v>
+        <v>83.15000000000001</v>
       </c>
       <c r="E22" t="n">
-        <v>6072821910</v>
+        <v>6223255909</v>
       </c>
       <c r="F22" t="n">
-        <v>202169810</v>
+        <v>186616702</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.57816</v>
+        <v>-1.09732</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>FET</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Fetch.ai</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>2.2</v>
+        <v>12.92</v>
       </c>
       <c r="E23" t="n">
-        <v>5558569059</v>
+        <v>6035127219</v>
       </c>
       <c r="F23" t="n">
-        <v>125335431</v>
+        <v>105609739</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.78065</v>
+        <v>-2.83597</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>11.83</v>
+        <v>7.74</v>
       </c>
       <c r="E24" t="n">
-        <v>5494792187</v>
+        <v>5876106544</v>
       </c>
       <c r="F24" t="n">
-        <v>59699771</v>
+        <v>214910775</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.92692</v>
+        <v>0.59509</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>FET</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Fetch.ai</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.999709</v>
+        <v>2.26</v>
       </c>
       <c r="E25" t="n">
-        <v>5473476264</v>
+        <v>5732446964</v>
       </c>
       <c r="F25" t="n">
-        <v>634862514</v>
+        <v>138116160</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.01465</v>
+        <v>-2.74996</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>5.9</v>
+        <v>0.99943</v>
       </c>
       <c r="E26" t="n">
-        <v>5459889666</v>
+        <v>5505872339</v>
       </c>
       <c r="F26" t="n">
-        <v>1568276</v>
+        <v>526143637</v>
       </c>
       <c r="G26" t="n">
-        <v>0.31157</v>
+        <v>-0.04078</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>7.11</v>
+        <v>5.88</v>
       </c>
       <c r="E27" t="n">
-        <v>5363060020</v>
+        <v>5460168590</v>
       </c>
       <c r="F27" t="n">
-        <v>86439897</v>
+        <v>766187</v>
       </c>
       <c r="G27" t="n">
-        <v>0.52007</v>
+        <v>0.36249</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>11.03</v>
+        <v>28.03</v>
       </c>
       <c r="E28" t="n">
-        <v>4296394894</v>
+        <v>4146930109</v>
       </c>
       <c r="F28" t="n">
-        <v>198928600</v>
+        <v>122661438</v>
       </c>
       <c r="G28" t="n">
-        <v>1.92776</v>
+        <v>-2.65344</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.110663</v>
+        <v>10.41</v>
       </c>
       <c r="E29" t="n">
-        <v>3949696675</v>
+        <v>4072390334</v>
       </c>
       <c r="F29" t="n">
-        <v>53147580</v>
+        <v>194213599</v>
       </c>
       <c r="G29" t="n">
-        <v>3.23655</v>
+        <v>3.89625</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>26.69</v>
+        <v>0.111571</v>
       </c>
       <c r="E30" t="n">
-        <v>3925985861</v>
+        <v>4008554045</v>
       </c>
       <c r="F30" t="n">
-        <v>90448714</v>
+        <v>67671445</v>
       </c>
       <c r="G30" t="n">
-        <v>0.83439</v>
+        <v>-1.83067</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>FDUSD</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>First Digital USD</t>
+          <t>Pepe</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>1</v>
+        <v>9.290000000000001e-06</v>
       </c>
       <c r="E31" t="n">
-        <v>3815889177</v>
+        <v>3943199730</v>
       </c>
       <c r="F31" t="n">
-        <v>3224194212</v>
+        <v>611873523</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.02008</v>
+        <v>-6.24193</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Pepe</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>8.67e-06</v>
+        <v>8.380000000000001</v>
       </c>
       <c r="E32" t="n">
-        <v>3649848628</v>
+        <v>3645497965</v>
       </c>
       <c r="F32" t="n">
-        <v>429447213</v>
+        <v>96072083</v>
       </c>
       <c r="G32" t="n">
-        <v>2.22099</v>
+        <v>-2.69209</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>WEETH</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Wrapped eETH</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>8.41</v>
+        <v>3207.45</v>
       </c>
       <c r="E33" t="n">
-        <v>3611222310</v>
+        <v>3635545406</v>
       </c>
       <c r="F33" t="n">
-        <v>48373512</v>
+        <v>19235699</v>
       </c>
       <c r="G33" t="n">
-        <v>0.15684</v>
+        <v>-1.24172</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>FDUSD</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>First Digital USD</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>8.58</v>
+        <v>0.995981</v>
       </c>
       <c r="E34" t="n">
-        <v>3355493362</v>
+        <v>3549612286</v>
       </c>
       <c r="F34" t="n">
-        <v>99896835</v>
+        <v>2811084669</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.05023</v>
+        <v>-0.28767</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.124056</v>
+        <v>2.32</v>
       </c>
       <c r="E35" t="n">
-        <v>3315125367</v>
+        <v>3454320908</v>
       </c>
       <c r="F35" t="n">
-        <v>8115194</v>
+        <v>41496758</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.24031</v>
+        <v>-3.84599</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1.01</v>
+        <v>0.12332</v>
       </c>
       <c r="E36" t="n">
-        <v>3298484571</v>
+        <v>3300456806</v>
       </c>
       <c r="F36" t="n">
-        <v>45519080</v>
+        <v>6037923</v>
       </c>
       <c r="G36" t="n">
-        <v>0.15957</v>
+        <v>-1.9638</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>2.25</v>
+        <v>8.35</v>
       </c>
       <c r="E37" t="n">
-        <v>3274684827</v>
+        <v>3267454256</v>
       </c>
       <c r="F37" t="n">
-        <v>58091866</v>
+        <v>87249589</v>
       </c>
       <c r="G37" t="n">
-        <v>0.26236</v>
+        <v>-3.34919</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>WEETH</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Wrapped eETH</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>3038.88</v>
+        <v>5.72</v>
       </c>
       <c r="E38" t="n">
-        <v>3127787678</v>
+        <v>3189685476</v>
       </c>
       <c r="F38" t="n">
-        <v>20156069</v>
+        <v>108343804</v>
       </c>
       <c r="G38" t="n">
-        <v>0.787</v>
+        <v>-2.8128</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>5.64</v>
+        <v>0.959202</v>
       </c>
       <c r="E39" t="n">
-        <v>3112314550</v>
+        <v>3149728739</v>
       </c>
       <c r="F39" t="n">
-        <v>76316825</v>
+        <v>67835413</v>
       </c>
       <c r="G39" t="n">
-        <v>0.9496</v>
+        <v>-2.68282</v>
       </c>
     </row>
     <row r="40">
@@ -1511,16 +1511,16 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.105414</v>
+        <v>0.106303</v>
       </c>
       <c r="E40" t="n">
-        <v>3051115291</v>
+        <v>3092143447</v>
       </c>
       <c r="F40" t="n">
-        <v>30043559</v>
+        <v>33854070</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.80449</v>
+        <v>-2.14642</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>EZETH</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Renzo Restaked ETH</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>49.94</v>
+        <v>3035.8</v>
       </c>
       <c r="E41" t="n">
-        <v>2995043075</v>
+        <v>3032838819</v>
       </c>
       <c r="F41" t="n">
-        <v>2712624</v>
+        <v>17002935</v>
       </c>
       <c r="G41" t="n">
-        <v>1.08076</v>
+        <v>-1.30834</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>WIF</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>dogwifhat</t>
+          <t>Arweave</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>2.98</v>
+        <v>46.29</v>
       </c>
       <c r="E42" t="n">
-        <v>2988678110</v>
+        <v>3027989864</v>
       </c>
       <c r="F42" t="n">
-        <v>291328777</v>
+        <v>55219072</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.85681</v>
+        <v>-3.20859</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.124618</v>
+        <v>49.44</v>
       </c>
       <c r="E43" t="n">
-        <v>2934998933</v>
+        <v>2976723808</v>
       </c>
       <c r="F43" t="n">
-        <v>21796106</v>
+        <v>2699438</v>
       </c>
       <c r="G43" t="n">
-        <v>0.08401</v>
+        <v>-1.4104</v>
       </c>
     </row>
     <row r="44">
@@ -1619,16 +1619,16 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1.99</v>
+        <v>2.01</v>
       </c>
       <c r="E44" t="n">
-        <v>2908293840</v>
+        <v>2938141802</v>
       </c>
       <c r="F44" t="n">
-        <v>26951589</v>
+        <v>55753791</v>
       </c>
       <c r="G44" t="n">
-        <v>-0.67747</v>
+        <v>-3.78026</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>EZETH</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Renzo Restaked ETH</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>2880.77</v>
+        <v>0.123</v>
       </c>
       <c r="E45" t="n">
-        <v>2870481798</v>
+        <v>2920328228</v>
       </c>
       <c r="F45" t="n">
-        <v>26251946</v>
+        <v>13372071</v>
       </c>
       <c r="G45" t="n">
-        <v>0.76324</v>
+        <v>-0.1086</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Arweave</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>42.08</v>
+        <v>0.302826</v>
       </c>
       <c r="E46" t="n">
-        <v>2749163283</v>
+        <v>2896370076</v>
       </c>
       <c r="F46" t="n">
-        <v>98722764</v>
+        <v>58896835</v>
       </c>
       <c r="G46" t="n">
-        <v>3.42502</v>
+        <v>-2.64366</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.284524</v>
+        <v>2.5</v>
       </c>
       <c r="E47" t="n">
-        <v>2702710102</v>
+        <v>2736925015</v>
       </c>
       <c r="F47" t="n">
-        <v>77186920</v>
+        <v>137954960</v>
       </c>
       <c r="G47" t="n">
-        <v>-3.46272</v>
+        <v>-3.12231</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>2.56</v>
+        <v>0.997154</v>
       </c>
       <c r="E48" t="n">
-        <v>2676668928</v>
+        <v>2655320527</v>
       </c>
       <c r="F48" t="n">
-        <v>91814297</v>
+        <v>171042895</v>
       </c>
       <c r="G48" t="n">
-        <v>0.22292</v>
+        <v>-2.34469</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>1.002</v>
+        <v>2776.56</v>
       </c>
       <c r="E49" t="n">
-        <v>2661095585</v>
+        <v>2590263757</v>
       </c>
       <c r="F49" t="n">
-        <v>130334444</v>
+        <v>63695992</v>
       </c>
       <c r="G49" t="n">
-        <v>0.50502</v>
+        <v>-2.45035</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>WIF</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>dogwifhat</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>374.54</v>
+        <v>2.57</v>
       </c>
       <c r="E50" t="n">
-        <v>2534911721</v>
+        <v>2571125644</v>
       </c>
       <c r="F50" t="n">
-        <v>16741618</v>
+        <v>739488697</v>
       </c>
       <c r="G50" t="n">
-        <v>0.2283</v>
+        <v>-4.39164</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>VET</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.03462744</v>
+        <v>377.72</v>
       </c>
       <c r="E51" t="n">
-        <v>2518990830</v>
+        <v>2565791500</v>
       </c>
       <c r="F51" t="n">
-        <v>39645428</v>
+        <v>15533253</v>
       </c>
       <c r="G51" t="n">
-        <v>-0.97274</v>
+        <v>-1.00432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-05-26
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>66967</v>
+        <v>68983</v>
       </c>
       <c r="E2" t="n">
-        <v>1320519938913</v>
+        <v>1361579868007</v>
       </c>
       <c r="F2" t="n">
-        <v>14474144487</v>
+        <v>17610962012</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.17983</v>
+        <v>-0.37545</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3086.61</v>
+        <v>3800.82</v>
       </c>
       <c r="E3" t="n">
-        <v>372369245273</v>
+        <v>457408957998</v>
       </c>
       <c r="F3" t="n">
-        <v>7025145548</v>
+        <v>9290941563</v>
       </c>
       <c r="G3" t="n">
-        <v>-1.28505</v>
+        <v>1.63758</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999985</v>
+        <v>0.9988669999999999</v>
       </c>
       <c r="E4" t="n">
-        <v>111432469260</v>
+        <v>111888382394</v>
       </c>
       <c r="F4" t="n">
-        <v>23784105139</v>
+        <v>26703735996</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.08263</v>
+        <v>-0.17004</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>578.89</v>
+        <v>600.49</v>
       </c>
       <c r="E5" t="n">
-        <v>89096283294</v>
+        <v>92527029871</v>
       </c>
       <c r="F5" t="n">
-        <v>493976681</v>
+        <v>408008931</v>
       </c>
       <c r="G5" t="n">
-        <v>0.02361</v>
+        <v>-0.53846</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>169.98</v>
+        <v>163.15</v>
       </c>
       <c r="E6" t="n">
-        <v>76840909683</v>
+        <v>73466971974</v>
       </c>
       <c r="F6" t="n">
-        <v>1924984517</v>
+        <v>2054274930</v>
       </c>
       <c r="G6" t="n">
-        <v>-2.20257</v>
+        <v>-3.17117</v>
       </c>
     </row>
     <row r="7">
@@ -611,25 +611,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>USDC</t>
+          <t>STETH</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>USDC</t>
+          <t>Lido Staked Ether</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.99758</v>
+        <v>3799.86</v>
       </c>
       <c r="E7" t="n">
-        <v>33479633976</v>
+        <v>35354597227</v>
       </c>
       <c r="F7" t="n">
-        <v>2282575344</v>
+        <v>62162050</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.19551</v>
+        <v>1.72976</v>
       </c>
     </row>
     <row r="8">
@@ -638,25 +638,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>STETH</t>
+          <t>USDC</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Lido Staked Ether</t>
+          <t>USDC</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>3085.81</v>
+        <v>0.998881</v>
       </c>
       <c r="E8" t="n">
-        <v>28979936067</v>
+        <v>32702003742</v>
       </c>
       <c r="F8" t="n">
-        <v>55941511</v>
+        <v>2933690722</v>
       </c>
       <c r="G8" t="n">
-        <v>-1.26909</v>
+        <v>-0.25052</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.514706</v>
+        <v>0.534792</v>
       </c>
       <c r="E9" t="n">
-        <v>28586230718</v>
+        <v>29698592087</v>
       </c>
       <c r="F9" t="n">
-        <v>380731752</v>
+        <v>442062348</v>
       </c>
       <c r="G9" t="n">
-        <v>-1.62378</v>
+        <v>-0.51252</v>
       </c>
     </row>
     <row r="10">
@@ -692,25 +692,25 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>DOGE</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Dogecoin</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>6.42</v>
+        <v>0.169542</v>
       </c>
       <c r="E10" t="n">
-        <v>22397447049</v>
+        <v>24596121062</v>
       </c>
       <c r="F10" t="n">
-        <v>200945328</v>
+        <v>1318436125</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.8024</v>
+        <v>1.31917</v>
       </c>
     </row>
     <row r="11">
@@ -719,25 +719,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>DOGE</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Dogecoin</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.15113</v>
+        <v>6.3</v>
       </c>
       <c r="E11" t="n">
-        <v>21815222440</v>
+        <v>21917181150</v>
       </c>
       <c r="F11" t="n">
-        <v>691667227</v>
+        <v>136791697</v>
       </c>
       <c r="G11" t="n">
-        <v>-2.45723</v>
+        <v>-1.72868</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.473242</v>
+        <v>0.460149</v>
       </c>
       <c r="E12" t="n">
-        <v>16752004740</v>
+        <v>16316761736</v>
       </c>
       <c r="F12" t="n">
-        <v>202247949</v>
+        <v>203245408</v>
       </c>
       <c r="G12" t="n">
-        <v>-1.45558</v>
+        <v>-0.28653</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2.438e-05</v>
+        <v>37.1</v>
       </c>
       <c r="E13" t="n">
-        <v>14408829482</v>
+        <v>14631138744</v>
       </c>
       <c r="F13" t="n">
-        <v>310501157</v>
+        <v>223073681</v>
       </c>
       <c r="G13" t="n">
-        <v>-2.14294</v>
+        <v>-3.11585</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>36.35</v>
+        <v>2.452e-05</v>
       </c>
       <c r="E14" t="n">
-        <v>13927846462</v>
+        <v>14512897960</v>
       </c>
       <c r="F14" t="n">
-        <v>273448625</v>
+        <v>312350066</v>
       </c>
       <c r="G14" t="n">
-        <v>-2.15134</v>
+        <v>-1.43333</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.121066</v>
+        <v>69094</v>
       </c>
       <c r="E15" t="n">
-        <v>10610782583</v>
+        <v>10742943518</v>
       </c>
       <c r="F15" t="n">
-        <v>227741888</v>
+        <v>141945337</v>
       </c>
       <c r="G15" t="n">
-        <v>-2.19123</v>
+        <v>-0.15439</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>67056</v>
+        <v>7.42</v>
       </c>
       <c r="E16" t="n">
-        <v>10445875850</v>
+        <v>10177998960</v>
       </c>
       <c r="F16" t="n">
-        <v>128505544</v>
+        <v>141874089</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.12081</v>
+        <v>1.58825</v>
       </c>
     </row>
     <row r="17">
@@ -890,16 +890,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>16.51</v>
+        <v>17.23</v>
       </c>
       <c r="E17" t="n">
-        <v>9700619238</v>
+        <v>10166094733</v>
       </c>
       <c r="F17" t="n">
-        <v>490963145</v>
+        <v>467212608</v>
       </c>
       <c r="G17" t="n">
-        <v>1.95408</v>
+        <v>0.83655</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>7.04</v>
+        <v>0.113734</v>
       </c>
       <c r="E18" t="n">
-        <v>9674917047</v>
+        <v>9957112125</v>
       </c>
       <c r="F18" t="n">
-        <v>114487709</v>
+        <v>233286062</v>
       </c>
       <c r="G18" t="n">
-        <v>-1.70956</v>
+        <v>-0.1324</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>485.47</v>
+        <v>486.48</v>
       </c>
       <c r="E19" t="n">
-        <v>9566413219</v>
+        <v>9621422042</v>
       </c>
       <c r="F19" t="n">
-        <v>320120396</v>
+        <v>160681790</v>
       </c>
       <c r="G19" t="n">
-        <v>0.14765</v>
+        <v>-1.54505</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>7.7</v>
+        <v>11.49</v>
       </c>
       <c r="E20" t="n">
-        <v>8338012375</v>
+        <v>8680989209</v>
       </c>
       <c r="F20" t="n">
-        <v>269472104</v>
+        <v>516609249</v>
       </c>
       <c r="G20" t="n">
-        <v>-3.45486</v>
+        <v>5.70289</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.691872</v>
+        <v>7.99</v>
       </c>
       <c r="E21" t="n">
-        <v>6455330932</v>
+        <v>8634095261</v>
       </c>
       <c r="F21" t="n">
-        <v>177425773</v>
+        <v>474344548</v>
       </c>
       <c r="G21" t="n">
-        <v>-3.1812</v>
+        <v>-0.31056</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Pepe</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>83.15000000000001</v>
+        <v>1.603e-05</v>
       </c>
       <c r="E22" t="n">
-        <v>6223255909</v>
+        <v>6812573418</v>
       </c>
       <c r="F22" t="n">
-        <v>186616702</v>
+        <v>1216539355</v>
       </c>
       <c r="G22" t="n">
-        <v>-1.09732</v>
+        <v>4.36425</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>12.92</v>
+        <v>0.718925</v>
       </c>
       <c r="E23" t="n">
-        <v>6035127219</v>
+        <v>6688859440</v>
       </c>
       <c r="F23" t="n">
-        <v>105609739</v>
+        <v>176692953</v>
       </c>
       <c r="G23" t="n">
-        <v>-2.83597</v>
+        <v>-1.17463</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>7.74</v>
+        <v>84.59999999999999</v>
       </c>
       <c r="E24" t="n">
-        <v>5876106544</v>
+        <v>6318083207</v>
       </c>
       <c r="F24" t="n">
-        <v>214910775</v>
+        <v>200457470</v>
       </c>
       <c r="G24" t="n">
-        <v>0.59509</v>
+        <v>-0.37638</v>
       </c>
     </row>
     <row r="25">
@@ -1106,16 +1106,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>2.26</v>
+        <v>2.25</v>
       </c>
       <c r="E25" t="n">
-        <v>5732446964</v>
+        <v>5696376149</v>
       </c>
       <c r="F25" t="n">
-        <v>138116160</v>
+        <v>132653721</v>
       </c>
       <c r="G25" t="n">
-        <v>-2.74996</v>
+        <v>-3.41661</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.99943</v>
+        <v>12.2</v>
       </c>
       <c r="E26" t="n">
-        <v>5505872339</v>
+        <v>5682965485</v>
       </c>
       <c r="F26" t="n">
-        <v>526143637</v>
+        <v>57970608</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.04078</v>
+        <v>-1.30919</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>5.88</v>
+        <v>5.92</v>
       </c>
       <c r="E27" t="n">
-        <v>5460168590</v>
+        <v>5495652741</v>
       </c>
       <c r="F27" t="n">
-        <v>766187</v>
+        <v>1189955</v>
       </c>
       <c r="G27" t="n">
-        <v>0.36249</v>
+        <v>-0.92383</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>28.03</v>
+        <v>0.99834</v>
       </c>
       <c r="E28" t="n">
-        <v>4146930109</v>
+        <v>5287429821</v>
       </c>
       <c r="F28" t="n">
-        <v>122661438</v>
+        <v>165153793</v>
       </c>
       <c r="G28" t="n">
-        <v>-2.65344</v>
+        <v>-0.17315</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>WEETH</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>Wrapped eETH</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>10.41</v>
+        <v>3949.18</v>
       </c>
       <c r="E29" t="n">
-        <v>4072390334</v>
+        <v>4727446826</v>
       </c>
       <c r="F29" t="n">
-        <v>194213599</v>
+        <v>37022681</v>
       </c>
       <c r="G29" t="n">
-        <v>3.89625</v>
+        <v>1.64397</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.111571</v>
+        <v>31.67</v>
       </c>
       <c r="E30" t="n">
-        <v>4008554045</v>
+        <v>4682969733</v>
       </c>
       <c r="F30" t="n">
-        <v>67671445</v>
+        <v>167394549</v>
       </c>
       <c r="G30" t="n">
-        <v>-1.83067</v>
+        <v>-0.46069</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Pepe</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>9.290000000000001e-06</v>
+        <v>8.98</v>
       </c>
       <c r="E31" t="n">
-        <v>3943199730</v>
+        <v>3922489425</v>
       </c>
       <c r="F31" t="n">
-        <v>611873523</v>
+        <v>110137057</v>
       </c>
       <c r="G31" t="n">
-        <v>-6.24193</v>
+        <v>-0.95219</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>8.380000000000001</v>
+        <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>3645497965</v>
+        <v>3894457800</v>
       </c>
       <c r="F32" t="n">
-        <v>96072083</v>
+        <v>98452880</v>
       </c>
       <c r="G32" t="n">
-        <v>-2.69209</v>
+        <v>-2.20133</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>WEETH</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Wrapped eETH</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>3207.45</v>
+        <v>0.10659</v>
       </c>
       <c r="E33" t="n">
-        <v>3635545406</v>
+        <v>3822283349</v>
       </c>
       <c r="F33" t="n">
-        <v>19235699</v>
+        <v>33264651</v>
       </c>
       <c r="G33" t="n">
-        <v>-1.24172</v>
+        <v>-1.95571</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>FDUSD</t>
+          <t>EZETH</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>First Digital USD</t>
+          <t>Renzo Restaked ETH</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.995981</v>
+        <v>3748.42</v>
       </c>
       <c r="E34" t="n">
-        <v>3549612286</v>
+        <v>3741592973</v>
       </c>
       <c r="F34" t="n">
-        <v>2811084669</v>
+        <v>64824196</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.28767</v>
+        <v>2.17674</v>
       </c>
     </row>
     <row r="35">
@@ -1376,16 +1376,16 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>2.32</v>
+        <v>2.38</v>
       </c>
       <c r="E35" t="n">
-        <v>3454320908</v>
+        <v>3542629757</v>
       </c>
       <c r="F35" t="n">
-        <v>41496758</v>
+        <v>40979232</v>
       </c>
       <c r="G35" t="n">
-        <v>-3.84599</v>
+        <v>-5.1917</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.12332</v>
+        <v>0.140425</v>
       </c>
       <c r="E36" t="n">
-        <v>3300456806</v>
+        <v>3350870056</v>
       </c>
       <c r="F36" t="n">
-        <v>6037923</v>
+        <v>29662531</v>
       </c>
       <c r="G36" t="n">
-        <v>-1.9638</v>
+        <v>4.92099</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>8.35</v>
+        <v>1.021</v>
       </c>
       <c r="E37" t="n">
-        <v>3267454256</v>
+        <v>3326088718</v>
       </c>
       <c r="F37" t="n">
-        <v>87249589</v>
+        <v>43819573</v>
       </c>
       <c r="G37" t="n">
-        <v>-3.34919</v>
+        <v>0.54165</v>
       </c>
     </row>
     <row r="38">
@@ -1457,16 +1457,16 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>5.72</v>
+        <v>5.87</v>
       </c>
       <c r="E38" t="n">
-        <v>3189685476</v>
+        <v>3283213723</v>
       </c>
       <c r="F38" t="n">
-        <v>108343804</v>
+        <v>120290762</v>
       </c>
       <c r="G38" t="n">
-        <v>-2.8128</v>
+        <v>-0.20129</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.959202</v>
+        <v>8.359999999999999</v>
       </c>
       <c r="E39" t="n">
-        <v>3149728739</v>
+        <v>3272815131</v>
       </c>
       <c r="F39" t="n">
-        <v>67835413</v>
+        <v>146080703</v>
       </c>
       <c r="G39" t="n">
-        <v>-2.68282</v>
+        <v>-1.45652</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.106303</v>
+        <v>0.119629</v>
       </c>
       <c r="E40" t="n">
-        <v>3092143447</v>
+        <v>3208782836</v>
       </c>
       <c r="F40" t="n">
-        <v>33854070</v>
+        <v>7181770</v>
       </c>
       <c r="G40" t="n">
-        <v>-2.14642</v>
+        <v>-1.63523</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>EZETH</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Renzo Restaked ETH</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>3035.8</v>
+        <v>1.2</v>
       </c>
       <c r="E41" t="n">
-        <v>3032838819</v>
+        <v>3205113286</v>
       </c>
       <c r="F41" t="n">
-        <v>17002935</v>
+        <v>340733390</v>
       </c>
       <c r="G41" t="n">
-        <v>-1.30834</v>
+        <v>0.7222499999999999</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Arweave</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>46.29</v>
+        <v>0.109276</v>
       </c>
       <c r="E42" t="n">
-        <v>3027989864</v>
+        <v>3173165623</v>
       </c>
       <c r="F42" t="n">
-        <v>55219072</v>
+        <v>33229650</v>
       </c>
       <c r="G42" t="n">
-        <v>-3.20859</v>
+        <v>-1.73276</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>FDUSD</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>First Digital USD</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>49.44</v>
+        <v>0.997129</v>
       </c>
       <c r="E43" t="n">
-        <v>2976723808</v>
+        <v>3135416280</v>
       </c>
       <c r="F43" t="n">
-        <v>2699438</v>
+        <v>3135682430</v>
       </c>
       <c r="G43" t="n">
-        <v>-1.4104</v>
+        <v>-0.19632</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>WIF</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>dogwifhat</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>2.01</v>
+        <v>3.04</v>
       </c>
       <c r="E44" t="n">
-        <v>2938141802</v>
+        <v>3045225847</v>
       </c>
       <c r="F44" t="n">
-        <v>55753791</v>
+        <v>520778744</v>
       </c>
       <c r="G44" t="n">
-        <v>-3.78026</v>
+        <v>0.60827</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.123</v>
+        <v>0.318213</v>
       </c>
       <c r="E45" t="n">
-        <v>2920328228</v>
+        <v>3033338471</v>
       </c>
       <c r="F45" t="n">
-        <v>13372071</v>
+        <v>64902188</v>
       </c>
       <c r="G45" t="n">
-        <v>-0.1086</v>
+        <v>-1.91148</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.302826</v>
+        <v>427.2</v>
       </c>
       <c r="E46" t="n">
-        <v>2896370076</v>
+        <v>2925955991</v>
       </c>
       <c r="F46" t="n">
-        <v>58896835</v>
+        <v>17042479</v>
       </c>
       <c r="G46" t="n">
-        <v>-2.64366</v>
+        <v>-1.54337</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>2.5</v>
+        <v>48.48</v>
       </c>
       <c r="E47" t="n">
-        <v>2736925015</v>
+        <v>2912000088</v>
       </c>
       <c r="F47" t="n">
-        <v>137954960</v>
+        <v>4055804</v>
       </c>
       <c r="G47" t="n">
-        <v>-3.12231</v>
+        <v>-0.2425</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.997154</v>
+        <v>1.98</v>
       </c>
       <c r="E48" t="n">
-        <v>2655320527</v>
+        <v>2908053573</v>
       </c>
       <c r="F48" t="n">
-        <v>171042895</v>
+        <v>37016535</v>
       </c>
       <c r="G48" t="n">
-        <v>-2.34469</v>
+        <v>-0.15902</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>2776.56</v>
+        <v>2.56</v>
       </c>
       <c r="E49" t="n">
-        <v>2590263757</v>
+        <v>2793058470</v>
       </c>
       <c r="F49" t="n">
-        <v>63695992</v>
+        <v>198632404</v>
       </c>
       <c r="G49" t="n">
-        <v>-2.45035</v>
+        <v>0.79262</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>WIF</t>
+          <t>USDE</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>dogwifhat</t>
+          <t>Ethena USDe</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>2.57</v>
+        <v>0.999457</v>
       </c>
       <c r="E50" t="n">
-        <v>2571125644</v>
+        <v>2780849112</v>
       </c>
       <c r="F50" t="n">
-        <v>739488697</v>
+        <v>71380328</v>
       </c>
       <c r="G50" t="n">
-        <v>-4.39164</v>
+        <v>-0.17412</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>MKR</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>377.72</v>
+        <v>2822.16</v>
       </c>
       <c r="E51" t="n">
-        <v>2565791500</v>
+        <v>2626688601</v>
       </c>
       <c r="F51" t="n">
-        <v>15533253</v>
+        <v>55645838</v>
       </c>
       <c r="G51" t="n">
-        <v>-1.00432</v>
+        <v>1.27263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-06-02
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>68983</v>
+        <v>67952</v>
       </c>
       <c r="E2" t="n">
-        <v>1361579868007</v>
+        <v>1339820854507</v>
       </c>
       <c r="F2" t="n">
-        <v>17610962012</v>
+        <v>12027414010</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.37545</v>
+        <v>0.44596</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3800.82</v>
+        <v>3791.33</v>
       </c>
       <c r="E3" t="n">
-        <v>457408957998</v>
+        <v>455431131112</v>
       </c>
       <c r="F3" t="n">
-        <v>9290941563</v>
+        <v>8790199617</v>
       </c>
       <c r="G3" t="n">
-        <v>1.63758</v>
+        <v>-0.03487</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.9988669999999999</v>
+        <v>0.99915</v>
       </c>
       <c r="E4" t="n">
-        <v>111888382394</v>
+        <v>112074706805</v>
       </c>
       <c r="F4" t="n">
-        <v>26703735996</v>
+        <v>18644294445</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.17004</v>
+        <v>0.00257</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>600.49</v>
+        <v>599.73</v>
       </c>
       <c r="E5" t="n">
-        <v>92527029871</v>
+        <v>92288356635</v>
       </c>
       <c r="F5" t="n">
-        <v>408008931</v>
+        <v>835855298</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.53846</v>
+        <v>0.6885</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>163.15</v>
+        <v>165.34</v>
       </c>
       <c r="E6" t="n">
-        <v>73466971974</v>
+        <v>75966803423</v>
       </c>
       <c r="F6" t="n">
-        <v>2054274930</v>
+        <v>1109749884</v>
       </c>
       <c r="G6" t="n">
-        <v>-3.17117</v>
+        <v>-0.86615</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3799.86</v>
+        <v>3789.67</v>
       </c>
       <c r="E7" t="n">
-        <v>35354597227</v>
+        <v>35993923577</v>
       </c>
       <c r="F7" t="n">
-        <v>62162050</v>
+        <v>38275320</v>
       </c>
       <c r="G7" t="n">
-        <v>1.72976</v>
+        <v>-0.0379</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.998881</v>
+        <v>0.9998860000000001</v>
       </c>
       <c r="E8" t="n">
-        <v>32702003742</v>
+        <v>32350141391</v>
       </c>
       <c r="F8" t="n">
-        <v>2933690722</v>
+        <v>2433705617</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.25052</v>
+        <v>-0.01199</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.534792</v>
+        <v>0.516373</v>
       </c>
       <c r="E9" t="n">
-        <v>29698592087</v>
+        <v>28613555361</v>
       </c>
       <c r="F9" t="n">
-        <v>442062348</v>
+        <v>455041709</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.51252</v>
+        <v>-0.67903</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.169542</v>
+        <v>0.158682</v>
       </c>
       <c r="E10" t="n">
-        <v>24596121062</v>
+        <v>22899880120</v>
       </c>
       <c r="F10" t="n">
-        <v>1318436125</v>
+        <v>499788700</v>
       </c>
       <c r="G10" t="n">
-        <v>1.31917</v>
+        <v>-0.43382</v>
       </c>
     </row>
     <row r="11">
@@ -719,25 +719,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>ADA</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Cardano</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>6.3</v>
+        <v>0.450885</v>
       </c>
       <c r="E11" t="n">
-        <v>21917181150</v>
+        <v>15962072933</v>
       </c>
       <c r="F11" t="n">
-        <v>136791697</v>
+        <v>183123806</v>
       </c>
       <c r="G11" t="n">
-        <v>-1.72868</v>
+        <v>0.5378500000000001</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +746,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ADA</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Cardano</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.460149</v>
+        <v>6.43</v>
       </c>
       <c r="E12" t="n">
-        <v>16316761736</v>
+        <v>15489964987</v>
       </c>
       <c r="F12" t="n">
-        <v>203245408</v>
+        <v>221780480</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.28653</v>
+        <v>0.89371</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +773,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Shiba Inu</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>37.1</v>
+        <v>2.49e-05</v>
       </c>
       <c r="E13" t="n">
-        <v>14631138744</v>
+        <v>14659811169</v>
       </c>
       <c r="F13" t="n">
-        <v>223073681</v>
+        <v>314260975</v>
       </c>
       <c r="G13" t="n">
-        <v>-3.11585</v>
+        <v>-1.43707</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +800,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Shiba Inu</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2.452e-05</v>
+        <v>35.87</v>
       </c>
       <c r="E14" t="n">
-        <v>14512897960</v>
+        <v>14117469234</v>
       </c>
       <c r="F14" t="n">
-        <v>312350066</v>
+        <v>181205307</v>
       </c>
       <c r="G14" t="n">
-        <v>-1.43333</v>
+        <v>-0.36571</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>69094</v>
+        <v>18.27</v>
       </c>
       <c r="E15" t="n">
-        <v>10742943518</v>
+        <v>10730453044</v>
       </c>
       <c r="F15" t="n">
-        <v>141945337</v>
+        <v>282502776</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.15439</v>
+        <v>-1.71004</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>7.42</v>
+        <v>67964</v>
       </c>
       <c r="E16" t="n">
-        <v>10177998960</v>
+        <v>10597510029</v>
       </c>
       <c r="F16" t="n">
-        <v>141874089</v>
+        <v>105325218</v>
       </c>
       <c r="G16" t="n">
-        <v>1.58825</v>
+        <v>0.35564</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>17.23</v>
+        <v>0.113931</v>
       </c>
       <c r="E17" t="n">
-        <v>10166094733</v>
+        <v>9946431798</v>
       </c>
       <c r="F17" t="n">
-        <v>467212608</v>
+        <v>215966288</v>
       </c>
       <c r="G17" t="n">
-        <v>0.83655</v>
+        <v>1.81523</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.113734</v>
+        <v>7.07</v>
       </c>
       <c r="E18" t="n">
-        <v>9957112125</v>
+        <v>9681551497</v>
       </c>
       <c r="F18" t="n">
-        <v>233286062</v>
+        <v>114845581</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.1324</v>
+        <v>-0.1377</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>486.48</v>
+        <v>461.4</v>
       </c>
       <c r="E19" t="n">
-        <v>9621422042</v>
+        <v>9103498570</v>
       </c>
       <c r="F19" t="n">
-        <v>160681790</v>
+        <v>142833360</v>
       </c>
       <c r="G19" t="n">
-        <v>-1.54505</v>
+        <v>0.37673</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>11.49</v>
+        <v>7.44</v>
       </c>
       <c r="E20" t="n">
-        <v>8680989209</v>
+        <v>8035867171</v>
       </c>
       <c r="F20" t="n">
-        <v>516609249</v>
+        <v>187581016</v>
       </c>
       <c r="G20" t="n">
-        <v>5.70289</v>
+        <v>3.02189</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>7.99</v>
+        <v>9.73</v>
       </c>
       <c r="E21" t="n">
-        <v>8634095261</v>
+        <v>7329448130</v>
       </c>
       <c r="F21" t="n">
-        <v>474344548</v>
+        <v>144247452</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.31056</v>
+        <v>-2.11288</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Pepe</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>1.603e-05</v>
+        <v>0.695935</v>
       </c>
       <c r="E22" t="n">
-        <v>6812573418</v>
+        <v>6454468953</v>
       </c>
       <c r="F22" t="n">
-        <v>1216539355</v>
+        <v>186914552</v>
       </c>
       <c r="G22" t="n">
-        <v>4.36425</v>
+        <v>-0.55875</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Pepe</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.718925</v>
+        <v>1.478e-05</v>
       </c>
       <c r="E23" t="n">
-        <v>6688859440</v>
+        <v>6208897685</v>
       </c>
       <c r="F23" t="n">
-        <v>176692953</v>
+        <v>835937480</v>
       </c>
       <c r="G23" t="n">
-        <v>-1.17463</v>
+        <v>-3.50396</v>
       </c>
     </row>
     <row r="24">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>84.59999999999999</v>
+        <v>82.76000000000001</v>
       </c>
       <c r="E24" t="n">
-        <v>6318083207</v>
+        <v>6167812739</v>
       </c>
       <c r="F24" t="n">
-        <v>200457470</v>
+        <v>185194200</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.37638</v>
+        <v>-0.57738</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>FET</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Fetch.ai</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>2.25</v>
+        <v>12.04</v>
       </c>
       <c r="E25" t="n">
-        <v>5696376149</v>
+        <v>5584233709</v>
       </c>
       <c r="F25" t="n">
-        <v>132653721</v>
+        <v>42712983</v>
       </c>
       <c r="G25" t="n">
-        <v>-3.41661</v>
+        <v>-0.03594</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>12.2</v>
+        <v>5.92</v>
       </c>
       <c r="E26" t="n">
-        <v>5682965485</v>
+        <v>5473902884</v>
       </c>
       <c r="F26" t="n">
-        <v>57970608</v>
+        <v>642839</v>
       </c>
       <c r="G26" t="n">
-        <v>-1.30919</v>
+        <v>-0.00467</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>5.92</v>
+        <v>0.999184</v>
       </c>
       <c r="E27" t="n">
-        <v>5495652741</v>
+        <v>5312543984</v>
       </c>
       <c r="F27" t="n">
-        <v>1189955</v>
+        <v>204981462</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.92383</v>
+        <v>-0.03749</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>FET</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Fetch.ai</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.99834</v>
+        <v>2.11</v>
       </c>
       <c r="E28" t="n">
-        <v>5287429821</v>
+        <v>5312347307</v>
       </c>
       <c r="F28" t="n">
-        <v>165153793</v>
+        <v>97633423</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.17315</v>
+        <v>0.37264</v>
       </c>
     </row>
     <row r="29">
@@ -1214,16 +1214,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>3949.18</v>
+        <v>3938.98</v>
       </c>
       <c r="E29" t="n">
-        <v>4727446826</v>
+        <v>5107325033</v>
       </c>
       <c r="F29" t="n">
-        <v>37022681</v>
+        <v>41455330</v>
       </c>
       <c r="G29" t="n">
-        <v>1.64397</v>
+        <v>-0.13055</v>
       </c>
     </row>
     <row r="30">
@@ -1241,16 +1241,16 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>31.67</v>
+        <v>29.24</v>
       </c>
       <c r="E30" t="n">
-        <v>4682969733</v>
+        <v>4299362771</v>
       </c>
       <c r="F30" t="n">
-        <v>167394549</v>
+        <v>117782146</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.46069</v>
+        <v>-1.19622</v>
       </c>
     </row>
     <row r="31">
@@ -1268,16 +1268,16 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>8.98</v>
+        <v>9</v>
       </c>
       <c r="E31" t="n">
-        <v>3922489425</v>
+        <v>3935174330</v>
       </c>
       <c r="F31" t="n">
-        <v>110137057</v>
+        <v>98322229</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.95219</v>
+        <v>-0.53955</v>
       </c>
     </row>
     <row r="32">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>10</v>
+        <v>9.949999999999999</v>
       </c>
       <c r="E32" t="n">
-        <v>3894457800</v>
+        <v>3861180088</v>
       </c>
       <c r="F32" t="n">
-        <v>98452880</v>
+        <v>78958546</v>
       </c>
       <c r="G32" t="n">
-        <v>-2.20133</v>
+        <v>-0.35211</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>EZETH</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Renzo Restaked ETH</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.10659</v>
+        <v>3737.97</v>
       </c>
       <c r="E33" t="n">
-        <v>3822283349</v>
+        <v>3724119372</v>
       </c>
       <c r="F33" t="n">
-        <v>33264651</v>
+        <v>21078804</v>
       </c>
       <c r="G33" t="n">
-        <v>-1.95571</v>
+        <v>0.06818</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>EZETH</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Renzo Restaked ETH</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>3748.42</v>
+        <v>0.09962</v>
       </c>
       <c r="E34" t="n">
-        <v>3741592973</v>
+        <v>3561302018</v>
       </c>
       <c r="F34" t="n">
-        <v>64824196</v>
+        <v>39588529</v>
       </c>
       <c r="G34" t="n">
-        <v>2.17674</v>
+        <v>-0.28233</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>2.38</v>
+        <v>0.139011</v>
       </c>
       <c r="E35" t="n">
-        <v>3542629757</v>
+        <v>3300630217</v>
       </c>
       <c r="F35" t="n">
-        <v>40979232</v>
+        <v>13861324</v>
       </c>
       <c r="G35" t="n">
-        <v>-5.1917</v>
+        <v>1.04621</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>WIF</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>dogwifhat</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.140425</v>
+        <v>3.27</v>
       </c>
       <c r="E36" t="n">
-        <v>3350870056</v>
+        <v>3273736595</v>
       </c>
       <c r="F36" t="n">
-        <v>29662531</v>
+        <v>344604691</v>
       </c>
       <c r="G36" t="n">
-        <v>4.92099</v>
+        <v>-2.30103</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1.021</v>
+        <v>2.21</v>
       </c>
       <c r="E37" t="n">
-        <v>3326088718</v>
+        <v>3261896696</v>
       </c>
       <c r="F37" t="n">
-        <v>43819573</v>
+        <v>37020514</v>
       </c>
       <c r="G37" t="n">
-        <v>0.54165</v>
+        <v>-1.58343</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>5.87</v>
+        <v>8.359999999999999</v>
       </c>
       <c r="E38" t="n">
-        <v>3283213723</v>
+        <v>3256192618</v>
       </c>
       <c r="F38" t="n">
-        <v>120290762</v>
+        <v>124912323</v>
       </c>
       <c r="G38" t="n">
-        <v>-0.20129</v>
+        <v>0.742</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>8.359999999999999</v>
+        <v>1.12</v>
       </c>
       <c r="E39" t="n">
-        <v>3272815131</v>
+        <v>3243118839</v>
       </c>
       <c r="F39" t="n">
-        <v>146080703</v>
+        <v>148252828</v>
       </c>
       <c r="G39" t="n">
-        <v>-1.45652</v>
+        <v>-0.29229</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.119629</v>
+        <v>5.78</v>
       </c>
       <c r="E40" t="n">
-        <v>3208782836</v>
+        <v>3224187823</v>
       </c>
       <c r="F40" t="n">
-        <v>7181770</v>
+        <v>94334421</v>
       </c>
       <c r="G40" t="n">
-        <v>-1.63523</v>
+        <v>0.32729</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1.2</v>
+        <v>0.986084</v>
       </c>
       <c r="E41" t="n">
-        <v>3205113286</v>
+        <v>3216433285</v>
       </c>
       <c r="F41" t="n">
-        <v>340733390</v>
+        <v>47240688</v>
       </c>
       <c r="G41" t="n">
-        <v>0.7222499999999999</v>
+        <v>-0.831</v>
       </c>
     </row>
     <row r="42">
@@ -1565,16 +1565,16 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.109276</v>
+        <v>0.105776</v>
       </c>
       <c r="E42" t="n">
-        <v>3173165623</v>
+        <v>3069275231</v>
       </c>
       <c r="F42" t="n">
-        <v>33229650</v>
+        <v>31852429</v>
       </c>
       <c r="G42" t="n">
-        <v>-1.73276</v>
+        <v>-0.73455</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>FDUSD</t>
+          <t>USDE</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>First Digital USD</t>
+          <t>Ethena USDe</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.997129</v>
+        <v>1.001</v>
       </c>
       <c r="E43" t="n">
-        <v>3135416280</v>
+        <v>3017705975</v>
       </c>
       <c r="F43" t="n">
-        <v>3135682430</v>
+        <v>34794630</v>
       </c>
       <c r="G43" t="n">
-        <v>-0.19632</v>
+        <v>-0.00293</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>WIF</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>dogwifhat</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>3.04</v>
+        <v>0.112735</v>
       </c>
       <c r="E44" t="n">
-        <v>3045225847</v>
+        <v>3016490752</v>
       </c>
       <c r="F44" t="n">
-        <v>520778744</v>
+        <v>6737163</v>
       </c>
       <c r="G44" t="n">
-        <v>0.60827</v>
+        <v>-0.34543</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>FDUSD</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>First Digital USD</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.318213</v>
+        <v>0.9978320000000001</v>
       </c>
       <c r="E45" t="n">
-        <v>3033338471</v>
+        <v>2899835928</v>
       </c>
       <c r="F45" t="n">
-        <v>64902188</v>
+        <v>2578352222</v>
       </c>
       <c r="G45" t="n">
-        <v>-1.91148</v>
+        <v>-0.07239</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>427.2</v>
+        <v>0.298861</v>
       </c>
       <c r="E46" t="n">
-        <v>2925955991</v>
+        <v>2841885664</v>
       </c>
       <c r="F46" t="n">
-        <v>17042479</v>
+        <v>45098839</v>
       </c>
       <c r="G46" t="n">
-        <v>-1.54337</v>
+        <v>0.78516</v>
       </c>
     </row>
     <row r="47">
@@ -1700,16 +1700,16 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>48.48</v>
+        <v>47.41</v>
       </c>
       <c r="E47" t="n">
-        <v>2912000088</v>
+        <v>2840618927</v>
       </c>
       <c r="F47" t="n">
-        <v>4055804</v>
+        <v>3516527</v>
       </c>
       <c r="G47" t="n">
-        <v>-0.2425</v>
+        <v>-1.45975</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Arweave</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>1.98</v>
+        <v>43.17</v>
       </c>
       <c r="E48" t="n">
-        <v>2908053573</v>
+        <v>2833733478</v>
       </c>
       <c r="F48" t="n">
-        <v>37016535</v>
+        <v>92988423</v>
       </c>
       <c r="G48" t="n">
-        <v>-0.15902</v>
+        <v>-0.892</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Optimism</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>2.56</v>
+        <v>151.03</v>
       </c>
       <c r="E49" t="n">
-        <v>2793058470</v>
+        <v>2741159306</v>
       </c>
       <c r="F49" t="n">
-        <v>198632404</v>
+        <v>47465868</v>
       </c>
       <c r="G49" t="n">
-        <v>0.79262</v>
+        <v>0.21232</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>USDE</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Ethena USDe</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.999457</v>
+        <v>394.84</v>
       </c>
       <c r="E50" t="n">
-        <v>2780849112</v>
+        <v>2727113731</v>
       </c>
       <c r="F50" t="n">
-        <v>71380328</v>
+        <v>28517117</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.17412</v>
+        <v>1.34382</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>MKR</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>2822.16</v>
+        <v>1.86</v>
       </c>
       <c r="E51" t="n">
-        <v>2626688601</v>
+        <v>2722040538</v>
       </c>
       <c r="F51" t="n">
-        <v>55645838</v>
+        <v>21398338</v>
       </c>
       <c r="G51" t="n">
-        <v>1.27263</v>
+        <v>2.65289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-06-09
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>67952</v>
+        <v>69360</v>
       </c>
       <c r="E2" t="n">
-        <v>1339820854507</v>
+        <v>1367250752088</v>
       </c>
       <c r="F2" t="n">
-        <v>12027414010</v>
+        <v>5391088032</v>
       </c>
       <c r="G2" t="n">
-        <v>0.44596</v>
+        <v>0.04864</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3791.33</v>
+        <v>3691.22</v>
       </c>
       <c r="E3" t="n">
-        <v>455431131112</v>
+        <v>443837405773</v>
       </c>
       <c r="F3" t="n">
-        <v>8790199617</v>
+        <v>6365866605</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.03487</v>
+        <v>0.22743</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.99915</v>
+        <v>0.999941</v>
       </c>
       <c r="E4" t="n">
-        <v>112074706805</v>
+        <v>112446454286</v>
       </c>
       <c r="F4" t="n">
-        <v>18644294445</v>
+        <v>20888854477</v>
       </c>
       <c r="G4" t="n">
-        <v>0.00257</v>
+        <v>0.03079</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>599.73</v>
+        <v>680.4</v>
       </c>
       <c r="E5" t="n">
-        <v>92288356635</v>
+        <v>104586807016</v>
       </c>
       <c r="F5" t="n">
-        <v>835855298</v>
+        <v>859051521</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6885</v>
+        <v>-0.47033</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>165.34</v>
+        <v>159.44</v>
       </c>
       <c r="E6" t="n">
-        <v>75966803423</v>
+        <v>73485795630</v>
       </c>
       <c r="F6" t="n">
-        <v>1109749884</v>
+        <v>1462274716</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.86615</v>
+        <v>-0.47263</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3789.67</v>
+        <v>3690.87</v>
       </c>
       <c r="E7" t="n">
-        <v>35993923577</v>
+        <v>35151542265</v>
       </c>
       <c r="F7" t="n">
-        <v>38275320</v>
+        <v>38833881</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.0379</v>
+        <v>0.22836</v>
       </c>
     </row>
     <row r="8">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.9998860000000001</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>32350141391</v>
+        <v>32221765797</v>
       </c>
       <c r="F8" t="n">
-        <v>2433705617</v>
+        <v>1699440036</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.01199</v>
+        <v>-0.00027</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.516373</v>
+        <v>0.49439</v>
       </c>
       <c r="E9" t="n">
-        <v>28613555361</v>
+        <v>27441349530</v>
       </c>
       <c r="F9" t="n">
-        <v>455041709</v>
+        <v>525066688</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.67903</v>
+        <v>0.09417</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.158682</v>
+        <v>0.146092</v>
       </c>
       <c r="E10" t="n">
-        <v>22899880120</v>
+        <v>21150589907</v>
       </c>
       <c r="F10" t="n">
-        <v>499788700</v>
+        <v>708537293</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.43382</v>
+        <v>0.28999</v>
       </c>
     </row>
     <row r="11">
@@ -719,25 +719,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ADA</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Cardano</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.450885</v>
+        <v>7.13</v>
       </c>
       <c r="E11" t="n">
-        <v>15962072933</v>
+        <v>17346977268</v>
       </c>
       <c r="F11" t="n">
-        <v>183123806</v>
+        <v>289865772</v>
       </c>
       <c r="G11" t="n">
-        <v>0.5378500000000001</v>
+        <v>-1.8493</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +746,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>ADA</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Cardano</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>6.43</v>
+        <v>0.440274</v>
       </c>
       <c r="E12" t="n">
-        <v>15489964987</v>
+        <v>15593014921</v>
       </c>
       <c r="F12" t="n">
-        <v>221780480</v>
+        <v>336163380</v>
       </c>
       <c r="G12" t="n">
-        <v>0.89371</v>
+        <v>1.28801</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2.49e-05</v>
+        <v>2.313e-05</v>
       </c>
       <c r="E13" t="n">
-        <v>14659811169</v>
+        <v>13639842151</v>
       </c>
       <c r="F13" t="n">
-        <v>314260975</v>
+        <v>423489431</v>
       </c>
       <c r="G13" t="n">
-        <v>-1.43707</v>
+        <v>-1.26681</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>35.87</v>
+        <v>32.29</v>
       </c>
       <c r="E14" t="n">
-        <v>14117469234</v>
+        <v>12696144106</v>
       </c>
       <c r="F14" t="n">
-        <v>181205307</v>
+        <v>257207003</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.36571</v>
+        <v>-1.06275</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +827,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>18.27</v>
+        <v>69402</v>
       </c>
       <c r="E15" t="n">
-        <v>10730453044</v>
+        <v>10622473308</v>
       </c>
       <c r="F15" t="n">
-        <v>282502776</v>
+        <v>59821082</v>
       </c>
       <c r="G15" t="n">
-        <v>-1.71004</v>
+        <v>0.13685</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +854,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>TRX</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>67964</v>
+        <v>0.116338</v>
       </c>
       <c r="E16" t="n">
-        <v>10597510029</v>
+        <v>10161971502</v>
       </c>
       <c r="F16" t="n">
-        <v>105325218</v>
+        <v>372333833</v>
       </c>
       <c r="G16" t="n">
-        <v>0.35564</v>
+        <v>3.03667</v>
       </c>
     </row>
     <row r="17">
@@ -881,25 +881,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.113931</v>
+        <v>15.97</v>
       </c>
       <c r="E17" t="n">
-        <v>9946431798</v>
+        <v>9378516167</v>
       </c>
       <c r="F17" t="n">
-        <v>215966288</v>
+        <v>270212396</v>
       </c>
       <c r="G17" t="n">
-        <v>1.81523</v>
+        <v>0.72202</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>7.07</v>
+        <v>467.83</v>
       </c>
       <c r="E18" t="n">
-        <v>9681551497</v>
+        <v>9229095789</v>
       </c>
       <c r="F18" t="n">
-        <v>114845581</v>
+        <v>195713396</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.1377</v>
+        <v>-0.6256699999999999</v>
       </c>
     </row>
     <row r="19">
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>461.4</v>
+        <v>6.46</v>
       </c>
       <c r="E19" t="n">
-        <v>9103498570</v>
+        <v>8876322274</v>
       </c>
       <c r="F19" t="n">
-        <v>142833360</v>
+        <v>193568163</v>
       </c>
       <c r="G19" t="n">
-        <v>0.37673</v>
+        <v>0.1943</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>7.44</v>
+        <v>9.91</v>
       </c>
       <c r="E20" t="n">
-        <v>8035867171</v>
+        <v>7470370046</v>
       </c>
       <c r="F20" t="n">
-        <v>187581016</v>
+        <v>210102584</v>
       </c>
       <c r="G20" t="n">
-        <v>3.02189</v>
+        <v>-0.05113</v>
       </c>
     </row>
     <row r="21">
@@ -989,25 +989,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>9.73</v>
+        <v>6.54</v>
       </c>
       <c r="E21" t="n">
-        <v>7329448130</v>
+        <v>7091323441</v>
       </c>
       <c r="F21" t="n">
-        <v>144247452</v>
+        <v>239600691</v>
       </c>
       <c r="G21" t="n">
-        <v>-2.11288</v>
+        <v>-2.7461</v>
       </c>
     </row>
     <row r="22">
@@ -1025,16 +1025,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.695935</v>
+        <v>0.651784</v>
       </c>
       <c r="E22" t="n">
-        <v>6454468953</v>
+        <v>6055759392</v>
       </c>
       <c r="F22" t="n">
-        <v>186914552</v>
+        <v>284662232</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.55875</v>
+        <v>-0.03113</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Pepe</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>1.478e-05</v>
+        <v>80.13</v>
       </c>
       <c r="E23" t="n">
-        <v>6208897685</v>
+        <v>5983680003</v>
       </c>
       <c r="F23" t="n">
-        <v>835937480</v>
+        <v>258747745</v>
       </c>
       <c r="G23" t="n">
-        <v>-3.50396</v>
+        <v>0.68152</v>
       </c>
     </row>
     <row r="24">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>WEETH</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Wrapped eETH</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>82.76000000000001</v>
+        <v>3835.58</v>
       </c>
       <c r="E24" t="n">
-        <v>6167812739</v>
+        <v>5538965554</v>
       </c>
       <c r="F24" t="n">
-        <v>185194200</v>
+        <v>29109773</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.57738</v>
+        <v>0.19887</v>
       </c>
     </row>
     <row r="25">
@@ -1097,25 +1097,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ICP</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>12.04</v>
+        <v>5.82</v>
       </c>
       <c r="E25" t="n">
-        <v>5584233709</v>
+        <v>5394414915</v>
       </c>
       <c r="F25" t="n">
-        <v>42712983</v>
+        <v>1132797</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.03594</v>
+        <v>-2.43816</v>
       </c>
     </row>
     <row r="26">
@@ -1124,25 +1124,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>5.92</v>
+        <v>0.999629</v>
       </c>
       <c r="E26" t="n">
-        <v>5473902884</v>
+        <v>5264485365</v>
       </c>
       <c r="F26" t="n">
-        <v>642839</v>
+        <v>356103332</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.00467</v>
+        <v>0.07213</v>
       </c>
     </row>
     <row r="27">
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Pepe</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.999184</v>
+        <v>1.229e-05</v>
       </c>
       <c r="E27" t="n">
-        <v>5312543984</v>
+        <v>5183671460</v>
       </c>
       <c r="F27" t="n">
-        <v>204981462</v>
+        <v>915086505</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.03749</v>
+        <v>-3.32052</v>
       </c>
     </row>
     <row r="28">
@@ -1178,25 +1178,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>FET</t>
+          <t>ICP</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Fetch.ai</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>2.11</v>
+        <v>10.91</v>
       </c>
       <c r="E28" t="n">
-        <v>5312347307</v>
+        <v>5073896453</v>
       </c>
       <c r="F28" t="n">
-        <v>97633423</v>
+        <v>112212226</v>
       </c>
       <c r="G28" t="n">
-        <v>0.37264</v>
+        <v>-1.46039</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>WEETH</t>
+          <t>FET</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Wrapped eETH</t>
+          <t>Fetch.ai</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>3938.98</v>
+        <v>1.73</v>
       </c>
       <c r="E29" t="n">
-        <v>5107325033</v>
+        <v>4360497542</v>
       </c>
       <c r="F29" t="n">
-        <v>41455330</v>
+        <v>169817660</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.13055</v>
+        <v>-1.61457</v>
       </c>
     </row>
     <row r="30">
@@ -1241,16 +1241,16 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>29.24</v>
+        <v>26.96</v>
       </c>
       <c r="E30" t="n">
-        <v>4299362771</v>
+        <v>3975235754</v>
       </c>
       <c r="F30" t="n">
-        <v>117782146</v>
+        <v>119778644</v>
       </c>
       <c r="G30" t="n">
-        <v>-1.19622</v>
+        <v>0.86816</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>9</v>
+        <v>0.15797</v>
       </c>
       <c r="E31" t="n">
-        <v>3935174330</v>
+        <v>3771816953</v>
       </c>
       <c r="F31" t="n">
-        <v>98322229</v>
+        <v>53432591</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.53955</v>
+        <v>-2.47027</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>EZETH</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>Renzo Restaked ETH</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>9.949999999999999</v>
+        <v>3680.42</v>
       </c>
       <c r="E32" t="n">
-        <v>3861180088</v>
+        <v>3671852348</v>
       </c>
       <c r="F32" t="n">
-        <v>78958546</v>
+        <v>46702882</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.35211</v>
+        <v>0.91612</v>
       </c>
     </row>
     <row r="33">
@@ -1313,25 +1313,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>EZETH</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Renzo Restaked ETH</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>3737.97</v>
+        <v>8.31</v>
       </c>
       <c r="E33" t="n">
-        <v>3724119372</v>
+        <v>3639911893</v>
       </c>
       <c r="F33" t="n">
-        <v>21078804</v>
+        <v>474979193</v>
       </c>
       <c r="G33" t="n">
-        <v>0.06818</v>
+        <v>2.341</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.09962</v>
+        <v>9.130000000000001</v>
       </c>
       <c r="E34" t="n">
-        <v>3561302018</v>
+        <v>3552702522</v>
       </c>
       <c r="F34" t="n">
-        <v>39588529</v>
+        <v>117519541</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.28233</v>
+        <v>-0.00223</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.139011</v>
+        <v>6.25</v>
       </c>
       <c r="E35" t="n">
-        <v>3300630217</v>
+        <v>3528024040</v>
       </c>
       <c r="F35" t="n">
-        <v>13861324</v>
+        <v>279697274</v>
       </c>
       <c r="G35" t="n">
-        <v>1.04621</v>
+        <v>2.25528</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>WIF</t>
+          <t>USDE</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>dogwifhat</t>
+          <t>Ethena USDe</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>3.27</v>
+        <v>1.001</v>
       </c>
       <c r="E36" t="n">
-        <v>3273736595</v>
+        <v>3358999868</v>
       </c>
       <c r="F36" t="n">
-        <v>344604691</v>
+        <v>86596221</v>
       </c>
       <c r="G36" t="n">
-        <v>-2.30103</v>
+        <v>0.08747000000000001</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>FDUSD</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>First Digital USD</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>2.21</v>
+        <v>0.999739</v>
       </c>
       <c r="E37" t="n">
-        <v>3261896696</v>
+        <v>3277803320</v>
       </c>
       <c r="F37" t="n">
-        <v>37020514</v>
+        <v>2685370293</v>
       </c>
       <c r="G37" t="n">
-        <v>-1.58343</v>
+        <v>-0.04643</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Cosmos Hub</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>8.359999999999999</v>
+        <v>2.23</v>
       </c>
       <c r="E38" t="n">
-        <v>3256192618</v>
+        <v>3269110388</v>
       </c>
       <c r="F38" t="n">
-        <v>124912323</v>
+        <v>62105118</v>
       </c>
       <c r="G38" t="n">
-        <v>0.742</v>
+        <v>-1.37302</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1.12</v>
+        <v>0.09024799999999999</v>
       </c>
       <c r="E39" t="n">
-        <v>3243118839</v>
+        <v>3228630561</v>
       </c>
       <c r="F39" t="n">
-        <v>148252828</v>
+        <v>54848058</v>
       </c>
       <c r="G39" t="n">
-        <v>-0.29229</v>
+        <v>-0.59845</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>5.78</v>
+        <v>169.48</v>
       </c>
       <c r="E40" t="n">
-        <v>3224187823</v>
+        <v>3126968415</v>
       </c>
       <c r="F40" t="n">
-        <v>94334421</v>
+        <v>92580678</v>
       </c>
       <c r="G40" t="n">
-        <v>0.32729</v>
+        <v>2.55853</v>
       </c>
     </row>
     <row r="41">
@@ -1538,16 +1538,16 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.986084</v>
+        <v>0.941105</v>
       </c>
       <c r="E41" t="n">
-        <v>3216433285</v>
+        <v>3075451282</v>
       </c>
       <c r="F41" t="n">
-        <v>47240688</v>
+        <v>103410213</v>
       </c>
       <c r="G41" t="n">
-        <v>-0.831</v>
+        <v>-0.49347</v>
       </c>
     </row>
     <row r="42">
@@ -1556,25 +1556,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Cosmos Hub</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.105776</v>
+        <v>7.83</v>
       </c>
       <c r="E42" t="n">
-        <v>3069275231</v>
+        <v>3058099471</v>
       </c>
       <c r="F42" t="n">
-        <v>31852429</v>
+        <v>151033583</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.73455</v>
+        <v>-0.8179999999999999</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>USDE</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Ethena USDe</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1.001</v>
+        <v>0.111544</v>
       </c>
       <c r="E43" t="n">
-        <v>3017705975</v>
+        <v>2992440260</v>
       </c>
       <c r="F43" t="n">
-        <v>34794630</v>
+        <v>8261352</v>
       </c>
       <c r="G43" t="n">
-        <v>-0.00293</v>
+        <v>-0.90934</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.112735</v>
+        <v>1.98</v>
       </c>
       <c r="E44" t="n">
-        <v>3016490752</v>
+        <v>2945446764</v>
       </c>
       <c r="F44" t="n">
-        <v>6737163</v>
+        <v>85315517</v>
       </c>
       <c r="G44" t="n">
-        <v>-0.34543</v>
+        <v>-2.15733</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>FDUSD</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>First Digital USD</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.9978320000000001</v>
+        <v>0.099231</v>
       </c>
       <c r="E45" t="n">
-        <v>2899835928</v>
+        <v>2886348960</v>
       </c>
       <c r="F45" t="n">
-        <v>2578352222</v>
+        <v>38091569</v>
       </c>
       <c r="G45" t="n">
-        <v>-0.07239</v>
+        <v>1.64986</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.298861</v>
+        <v>47.11</v>
       </c>
       <c r="E46" t="n">
-        <v>2841885664</v>
+        <v>2828276549</v>
       </c>
       <c r="F46" t="n">
-        <v>45098839</v>
+        <v>4516645</v>
       </c>
       <c r="G46" t="n">
-        <v>0.78516</v>
+        <v>-1.51584</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>47.41</v>
+        <v>0.974952</v>
       </c>
       <c r="E47" t="n">
-        <v>2840618927</v>
+        <v>2825777370</v>
       </c>
       <c r="F47" t="n">
-        <v>3516527</v>
+        <v>239652288</v>
       </c>
       <c r="G47" t="n">
-        <v>-1.45975</v>
+        <v>0.64466</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>FLOKI</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Arweave</t>
+          <t>FLOKI</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>43.17</v>
+        <v>0.0002792</v>
       </c>
       <c r="E48" t="n">
-        <v>2833733478</v>
+        <v>2708506639</v>
       </c>
       <c r="F48" t="n">
-        <v>92988423</v>
+        <v>384552280</v>
       </c>
       <c r="G48" t="n">
-        <v>-0.892</v>
+        <v>1.65058</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>WIF</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>dogwifhat</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>151.03</v>
+        <v>2.7</v>
       </c>
       <c r="E49" t="n">
-        <v>2741159306</v>
+        <v>2697267573</v>
       </c>
       <c r="F49" t="n">
-        <v>47465868</v>
+        <v>360627832</v>
       </c>
       <c r="G49" t="n">
-        <v>0.21232</v>
+        <v>-0.99758</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>394.84</v>
+        <v>27.92</v>
       </c>
       <c r="E50" t="n">
-        <v>2727113731</v>
+        <v>2684293840</v>
       </c>
       <c r="F50" t="n">
-        <v>28517117</v>
+        <v>199037533</v>
       </c>
       <c r="G50" t="n">
-        <v>1.34382</v>
+        <v>-4.71502</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>SUI</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Sui</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>1.86</v>
+        <v>1.099</v>
       </c>
       <c r="E51" t="n">
-        <v>2722040538</v>
+        <v>2669283318</v>
       </c>
       <c r="F51" t="n">
-        <v>21398338</v>
+        <v>307442437</v>
       </c>
       <c r="G51" t="n">
-        <v>2.65289</v>
+        <v>0.40326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daten aktualisiert am 2024-06-16
</commit_message>
<xml_diff>
--- a/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
+++ b/data/cryptocurrencies/~index_cryptocurrencies_list.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>69360</v>
+        <v>66573</v>
       </c>
       <c r="E2" t="n">
-        <v>1367250752088</v>
+        <v>1311514368074</v>
       </c>
       <c r="F2" t="n">
-        <v>5391088032</v>
+        <v>12152647814</v>
       </c>
       <c r="G2" t="n">
-        <v>0.04864</v>
+        <v>0.48677</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3691.22</v>
+        <v>3557.3</v>
       </c>
       <c r="E3" t="n">
-        <v>443837405773</v>
+        <v>427234503583</v>
       </c>
       <c r="F3" t="n">
-        <v>6365866605</v>
+        <v>9103359556</v>
       </c>
       <c r="G3" t="n">
-        <v>0.22743</v>
+        <v>0.42272</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.999941</v>
+        <v>0.999292</v>
       </c>
       <c r="E4" t="n">
-        <v>112446454286</v>
+        <v>112530262253</v>
       </c>
       <c r="F4" t="n">
-        <v>20888854477</v>
+        <v>13895908664</v>
       </c>
       <c r="G4" t="n">
-        <v>0.03079</v>
+        <v>0.00396</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>680.4</v>
+        <v>606.33</v>
       </c>
       <c r="E5" t="n">
-        <v>104586807016</v>
+        <v>93238905955</v>
       </c>
       <c r="F5" t="n">
-        <v>859051521</v>
+        <v>577747781</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.47033</v>
+        <v>-0.376</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>159.44</v>
+        <v>145.31</v>
       </c>
       <c r="E6" t="n">
-        <v>73485795630</v>
+        <v>67032872604</v>
       </c>
       <c r="F6" t="n">
-        <v>1462274716</v>
+        <v>1101451423</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.47263</v>
+        <v>0.72075</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3690.87</v>
+        <v>3555.75</v>
       </c>
       <c r="E7" t="n">
-        <v>35151542265</v>
+        <v>33891275015</v>
       </c>
       <c r="F7" t="n">
-        <v>38833881</v>
+        <v>39252266</v>
       </c>
       <c r="G7" t="n">
-        <v>0.22836</v>
+        <v>0.42802</v>
       </c>
     </row>
     <row r="8">
@@ -650,13 +650,13 @@
         <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>32221765797</v>
+        <v>32481212897</v>
       </c>
       <c r="F8" t="n">
-        <v>1699440036</v>
+        <v>2347446916</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.00027</v>
+        <v>0.07713</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.49439</v>
+        <v>0.495165</v>
       </c>
       <c r="E9" t="n">
-        <v>27441349530</v>
+        <v>27528514562</v>
       </c>
       <c r="F9" t="n">
-        <v>525066688</v>
+        <v>757893422</v>
       </c>
       <c r="G9" t="n">
-        <v>0.09417</v>
+        <v>3.28048</v>
       </c>
     </row>
     <row r="10">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.146092</v>
+        <v>0.135826</v>
       </c>
       <c r="E10" t="n">
-        <v>21150589907</v>
+        <v>19644021810</v>
       </c>
       <c r="F10" t="n">
-        <v>708537293</v>
+        <v>385990823</v>
       </c>
       <c r="G10" t="n">
-        <v>0.28999</v>
+        <v>-0.56852</v>
       </c>
     </row>
     <row r="11">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>7.13</v>
+        <v>7.99</v>
       </c>
       <c r="E11" t="n">
-        <v>17346977268</v>
+        <v>19412338275</v>
       </c>
       <c r="F11" t="n">
-        <v>289865772</v>
+        <v>388797505</v>
       </c>
       <c r="G11" t="n">
-        <v>-1.8493</v>
+        <v>-1.64512</v>
       </c>
     </row>
     <row r="12">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.440274</v>
+        <v>0.415052</v>
       </c>
       <c r="E12" t="n">
-        <v>15593014921</v>
+        <v>14684055757</v>
       </c>
       <c r="F12" t="n">
-        <v>336163380</v>
+        <v>182088429</v>
       </c>
       <c r="G12" t="n">
-        <v>1.28801</v>
+        <v>1.11794</v>
       </c>
     </row>
     <row r="13">
@@ -782,16 +782,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2.313e-05</v>
+        <v>2.074e-05</v>
       </c>
       <c r="E13" t="n">
-        <v>13639842151</v>
+        <v>12207860611</v>
       </c>
       <c r="F13" t="n">
-        <v>423489431</v>
+        <v>172099522</v>
       </c>
       <c r="G13" t="n">
-        <v>-1.26681</v>
+        <v>-0.06411</v>
       </c>
     </row>
     <row r="14">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>32.29</v>
+        <v>30.03</v>
       </c>
       <c r="E14" t="n">
-        <v>12696144106</v>
+        <v>11797111581</v>
       </c>
       <c r="F14" t="n">
-        <v>257207003</v>
+        <v>189082038</v>
       </c>
       <c r="G14" t="n">
-        <v>-1.06275</v>
+        <v>-0.27576</v>
       </c>
     </row>
     <row r="15">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>69402</v>
+        <v>66597</v>
       </c>
       <c r="E15" t="n">
-        <v>10622473308</v>
+        <v>10186043878</v>
       </c>
       <c r="F15" t="n">
-        <v>59821082</v>
+        <v>137996145</v>
       </c>
       <c r="G15" t="n">
-        <v>0.13685</v>
+        <v>0.45414</v>
       </c>
     </row>
     <row r="16">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.116338</v>
+        <v>0.115298</v>
       </c>
       <c r="E16" t="n">
-        <v>10161971502</v>
+        <v>10058362159</v>
       </c>
       <c r="F16" t="n">
-        <v>372333833</v>
+        <v>196577834</v>
       </c>
       <c r="G16" t="n">
-        <v>3.03667</v>
+        <v>0.10935</v>
       </c>
     </row>
     <row r="17">
@@ -890,16 +890,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>15.97</v>
+        <v>15</v>
       </c>
       <c r="E17" t="n">
-        <v>9378516167</v>
+        <v>8789990886</v>
       </c>
       <c r="F17" t="n">
-        <v>270212396</v>
+        <v>237541729</v>
       </c>
       <c r="G17" t="n">
-        <v>0.72202</v>
+        <v>0.56547</v>
       </c>
     </row>
     <row r="18">
@@ -908,25 +908,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>467.83</v>
+        <v>11.47</v>
       </c>
       <c r="E18" t="n">
-        <v>9229095789</v>
+        <v>8642925175</v>
       </c>
       <c r="F18" t="n">
-        <v>195713396</v>
+        <v>381494663</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.6256699999999999</v>
+        <v>4.79651</v>
       </c>
     </row>
     <row r="19">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>6.46</v>
+        <v>6.22</v>
       </c>
       <c r="E19" t="n">
-        <v>8876322274</v>
+        <v>8554733323</v>
       </c>
       <c r="F19" t="n">
-        <v>193568163</v>
+        <v>98684591</v>
       </c>
       <c r="G19" t="n">
-        <v>0.1943</v>
+        <v>0.26773</v>
       </c>
     </row>
     <row r="20">
@@ -962,25 +962,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>9.91</v>
+        <v>431.6</v>
       </c>
       <c r="E20" t="n">
-        <v>7470370046</v>
+        <v>8506097314</v>
       </c>
       <c r="F20" t="n">
-        <v>210102584</v>
+        <v>127980838</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.05113</v>
+        <v>1.30081</v>
       </c>
     </row>
     <row r="21">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>6.54</v>
+        <v>5.62</v>
       </c>
       <c r="E21" t="n">
-        <v>7091323441</v>
+        <v>6116610822</v>
       </c>
       <c r="F21" t="n">
-        <v>239600691</v>
+        <v>153276288</v>
       </c>
       <c r="G21" t="n">
-        <v>-2.7461</v>
+        <v>-0.19331</v>
       </c>
     </row>
     <row r="22">
@@ -1016,25 +1016,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>LTC</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.651784</v>
+        <v>79.3</v>
       </c>
       <c r="E22" t="n">
-        <v>6055759392</v>
+        <v>5916031717</v>
       </c>
       <c r="F22" t="n">
-        <v>284662232</v>
+        <v>217059682</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.03113</v>
+        <v>0.40544</v>
       </c>
     </row>
     <row r="23">
@@ -1043,25 +1043,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>LTC</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>80.13</v>
+        <v>0.614164</v>
       </c>
       <c r="E23" t="n">
-        <v>5983680003</v>
+        <v>5693888274</v>
       </c>
       <c r="F23" t="n">
-        <v>258747745</v>
+        <v>220684837</v>
       </c>
       <c r="G23" t="n">
-        <v>0.68152</v>
+        <v>2.13205</v>
       </c>
     </row>
     <row r="24">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>3835.58</v>
+        <v>3697.16</v>
       </c>
       <c r="E24" t="n">
-        <v>5538965554</v>
+        <v>5442384333</v>
       </c>
       <c r="F24" t="n">
-        <v>29109773</v>
+        <v>19518612</v>
       </c>
       <c r="G24" t="n">
-        <v>0.19887</v>
+        <v>0.53203</v>
       </c>
     </row>
     <row r="25">
@@ -1106,16 +1106,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>5.82</v>
+        <v>5.84</v>
       </c>
       <c r="E25" t="n">
-        <v>5394414915</v>
+        <v>5408547350</v>
       </c>
       <c r="F25" t="n">
-        <v>1132797</v>
+        <v>976975</v>
       </c>
       <c r="G25" t="n">
-        <v>-2.43816</v>
+        <v>2.16434</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.999629</v>
+        <v>0.998336</v>
       </c>
       <c r="E26" t="n">
-        <v>5264485365</v>
+        <v>5234477104</v>
       </c>
       <c r="F26" t="n">
-        <v>356103332</v>
+        <v>309660990</v>
       </c>
       <c r="G26" t="n">
-        <v>0.07213</v>
+        <v>-0.06297999999999999</v>
       </c>
     </row>
     <row r="27">
@@ -1160,16 +1160,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>1.229e-05</v>
+        <v>1.192e-05</v>
       </c>
       <c r="E27" t="n">
-        <v>5183671460</v>
+        <v>5002219868</v>
       </c>
       <c r="F27" t="n">
-        <v>915086505</v>
+        <v>498642594</v>
       </c>
       <c r="G27" t="n">
-        <v>-3.32052</v>
+        <v>-0.92702</v>
       </c>
     </row>
     <row r="28">
@@ -1187,16 +1187,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>10.91</v>
+        <v>9.16</v>
       </c>
       <c r="E28" t="n">
-        <v>5073896453</v>
+        <v>4255774632</v>
       </c>
       <c r="F28" t="n">
-        <v>112212226</v>
+        <v>64719908</v>
       </c>
       <c r="G28" t="n">
-        <v>-1.46039</v>
+        <v>-0.33152</v>
       </c>
     </row>
     <row r="29">
@@ -1205,25 +1205,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>FET</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Fetch.ai</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>1.73</v>
+        <v>25.32</v>
       </c>
       <c r="E29" t="n">
-        <v>4360497542</v>
+        <v>3732692357</v>
       </c>
       <c r="F29" t="n">
-        <v>169817660</v>
+        <v>77744818</v>
       </c>
       <c r="G29" t="n">
-        <v>-1.61457</v>
+        <v>-0.04392</v>
       </c>
     </row>
     <row r="30">
@@ -1232,25 +1232,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>KAS</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>26.96</v>
+        <v>0.15431</v>
       </c>
       <c r="E30" t="n">
-        <v>3975235754</v>
+        <v>3687473918</v>
       </c>
       <c r="F30" t="n">
-        <v>119778644</v>
+        <v>56796979</v>
       </c>
       <c r="G30" t="n">
-        <v>0.86816</v>
+        <v>-3.07067</v>
       </c>
     </row>
     <row r="31">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>KAS</t>
+          <t>FET</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Fetch.ai</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.15797</v>
+        <v>1.45</v>
       </c>
       <c r="E31" t="n">
-        <v>3771816953</v>
+        <v>3665177792</v>
       </c>
       <c r="F31" t="n">
-        <v>53432591</v>
+        <v>87241720</v>
       </c>
       <c r="G31" t="n">
-        <v>-2.47027</v>
+        <v>-1.90103</v>
       </c>
     </row>
     <row r="32">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>3680.42</v>
+        <v>3545.05</v>
       </c>
       <c r="E32" t="n">
-        <v>3671852348</v>
+        <v>3532389876</v>
       </c>
       <c r="F32" t="n">
-        <v>46702882</v>
+        <v>38546355</v>
       </c>
       <c r="G32" t="n">
-        <v>0.91612</v>
+        <v>0.63964</v>
       </c>
     </row>
     <row r="33">
@@ -1322,16 +1322,16 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>8.31</v>
+        <v>7.83</v>
       </c>
       <c r="E33" t="n">
-        <v>3639911893</v>
+        <v>3527424973</v>
       </c>
       <c r="F33" t="n">
-        <v>474979193</v>
+        <v>125128556</v>
       </c>
       <c r="G33" t="n">
-        <v>2.341</v>
+        <v>0.23057</v>
       </c>
     </row>
     <row r="34">
@@ -1340,25 +1340,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>USDE</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>Ethena USDe</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>9.130000000000001</v>
+        <v>1.001</v>
       </c>
       <c r="E34" t="n">
-        <v>3552702522</v>
+        <v>3524327678</v>
       </c>
       <c r="F34" t="n">
-        <v>117519541</v>
+        <v>28172087</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.00223</v>
+        <v>0.08056000000000001</v>
       </c>
     </row>
     <row r="35">
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>XMR</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>6.25</v>
+        <v>173.32</v>
       </c>
       <c r="E35" t="n">
-        <v>3528024040</v>
+        <v>3195489421</v>
       </c>
       <c r="F35" t="n">
-        <v>279697274</v>
+        <v>54519453</v>
       </c>
       <c r="G35" t="n">
-        <v>2.25528</v>
+        <v>0.20355</v>
       </c>
     </row>
     <row r="36">
@@ -1394,25 +1394,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>USDE</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Ethena USDe</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1.001</v>
+        <v>8.06</v>
       </c>
       <c r="E36" t="n">
-        <v>3358999868</v>
+        <v>3128501298</v>
       </c>
       <c r="F36" t="n">
-        <v>86596221</v>
+        <v>73081803</v>
       </c>
       <c r="G36" t="n">
-        <v>0.08747000000000001</v>
+        <v>-0.51832</v>
       </c>
     </row>
     <row r="37">
@@ -1421,25 +1421,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>FDUSD</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>First Digital USD</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.999739</v>
+        <v>0.084943</v>
       </c>
       <c r="E37" t="n">
-        <v>3277803320</v>
+        <v>3032834269</v>
       </c>
       <c r="F37" t="n">
-        <v>2685370293</v>
+        <v>30866378</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.04643</v>
+        <v>-0.93716</v>
       </c>
     </row>
     <row r="38">
@@ -1448,25 +1448,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>2.23</v>
+        <v>5.19</v>
       </c>
       <c r="E38" t="n">
-        <v>3269110388</v>
+        <v>2924493138</v>
       </c>
       <c r="F38" t="n">
-        <v>62105118</v>
+        <v>116811067</v>
       </c>
       <c r="G38" t="n">
-        <v>-1.37302</v>
+        <v>-1.02652</v>
       </c>
     </row>
     <row r="39">
@@ -1475,25 +1475,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.09024799999999999</v>
+        <v>0.887687</v>
       </c>
       <c r="E39" t="n">
-        <v>3228630561</v>
+        <v>2894677892</v>
       </c>
       <c r="F39" t="n">
-        <v>54848058</v>
+        <v>149708327</v>
       </c>
       <c r="G39" t="n">
-        <v>-0.59845</v>
+        <v>-0.54756</v>
       </c>
     </row>
     <row r="40">
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>XMR</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>169.48</v>
+        <v>0.09858500000000001</v>
       </c>
       <c r="E40" t="n">
-        <v>3126968415</v>
+        <v>2868242366</v>
       </c>
       <c r="F40" t="n">
-        <v>92580678</v>
+        <v>33744802</v>
       </c>
       <c r="G40" t="n">
-        <v>2.55853</v>
+        <v>1.53861</v>
       </c>
     </row>
     <row r="41">
@@ -1529,25 +1529,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.941105</v>
+        <v>1.94</v>
       </c>
       <c r="E41" t="n">
-        <v>3075451282</v>
+        <v>2841483465</v>
       </c>
       <c r="F41" t="n">
-        <v>103410213</v>
+        <v>46703981</v>
       </c>
       <c r="G41" t="n">
-        <v>-0.49347</v>
+        <v>1.80814</v>
       </c>
     </row>
     <row r="42">
@@ -1565,16 +1565,16 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>7.83</v>
+        <v>7.17</v>
       </c>
       <c r="E42" t="n">
-        <v>3058099471</v>
+        <v>2800475214</v>
       </c>
       <c r="F42" t="n">
-        <v>151033583</v>
+        <v>97099455</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.8179999999999999</v>
+        <v>0.76178</v>
       </c>
     </row>
     <row r="43">
@@ -1583,25 +1583,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.111544</v>
+        <v>46.15</v>
       </c>
       <c r="E43" t="n">
-        <v>2992440260</v>
+        <v>2764061492</v>
       </c>
       <c r="F43" t="n">
-        <v>8261352</v>
+        <v>2767354</v>
       </c>
       <c r="G43" t="n">
-        <v>-0.90934</v>
+        <v>1.54254</v>
       </c>
     </row>
     <row r="44">
@@ -1610,25 +1610,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>IMX</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1.98</v>
+        <v>0.099255</v>
       </c>
       <c r="E44" t="n">
-        <v>2945446764</v>
+        <v>2657910274</v>
       </c>
       <c r="F44" t="n">
-        <v>85315517</v>
+        <v>7773194</v>
       </c>
       <c r="G44" t="n">
-        <v>-2.15733</v>
+        <v>-2.63816</v>
       </c>
     </row>
     <row r="45">
@@ -1637,25 +1637,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>ARB</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.099231</v>
+        <v>0.917296</v>
       </c>
       <c r="E45" t="n">
-        <v>2886348960</v>
+        <v>2656067608</v>
       </c>
       <c r="F45" t="n">
-        <v>38091569</v>
+        <v>120568164</v>
       </c>
       <c r="G45" t="n">
-        <v>1.64986</v>
+        <v>-0.57645</v>
       </c>
     </row>
     <row r="46">
@@ -1664,25 +1664,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>IMX</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>47.11</v>
+        <v>1.72</v>
       </c>
       <c r="E46" t="n">
-        <v>2828276549</v>
+        <v>2597179330</v>
       </c>
       <c r="F46" t="n">
-        <v>4516645</v>
+        <v>38097710</v>
       </c>
       <c r="G46" t="n">
-        <v>-1.51584</v>
+        <v>-1.46766</v>
       </c>
     </row>
     <row r="47">
@@ -1691,25 +1691,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ARB</t>
+          <t>FDUSD</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>First Digital USD</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.974952</v>
+        <v>0.999582</v>
       </c>
       <c r="E47" t="n">
-        <v>2825777370</v>
+        <v>2546129009</v>
       </c>
       <c r="F47" t="n">
-        <v>239652288</v>
+        <v>2663389695</v>
       </c>
       <c r="G47" t="n">
-        <v>0.64466</v>
+        <v>0.03561</v>
       </c>
     </row>
     <row r="48">
@@ -1718,25 +1718,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>FLOKI</t>
+          <t>WIF</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>FLOKI</t>
+          <t>dogwifhat</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.0002792</v>
+        <v>2.52</v>
       </c>
       <c r="E48" t="n">
-        <v>2708506639</v>
+        <v>2520038169</v>
       </c>
       <c r="F48" t="n">
-        <v>384552280</v>
+        <v>295054558</v>
       </c>
       <c r="G48" t="n">
-        <v>1.65058</v>
+        <v>4.65933</v>
       </c>
     </row>
     <row r="49">
@@ -1745,25 +1745,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>WIF</t>
+          <t>INJ</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>dogwifhat</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>2.7</v>
+        <v>25.09</v>
       </c>
       <c r="E49" t="n">
-        <v>2697267573</v>
+        <v>2438375783</v>
       </c>
       <c r="F49" t="n">
-        <v>360627832</v>
+        <v>120958787</v>
       </c>
       <c r="G49" t="n">
-        <v>-0.99758</v>
+        <v>-3.51505</v>
       </c>
     </row>
     <row r="50">
@@ -1772,25 +1772,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>INJ</t>
+          <t>SUI</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>Sui</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>27.92</v>
+        <v>0.944039</v>
       </c>
       <c r="E50" t="n">
-        <v>2684293840</v>
+        <v>2288813310</v>
       </c>
       <c r="F50" t="n">
-        <v>199037533</v>
+        <v>99105152</v>
       </c>
       <c r="G50" t="n">
-        <v>-4.71502</v>
+        <v>0.15364</v>
       </c>
     </row>
     <row r="51">
@@ -1799,25 +1799,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>SUI</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Sui</t>
+          <t>Optimism</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>1.099</v>
+        <v>2.06</v>
       </c>
       <c r="E51" t="n">
-        <v>2669283318</v>
+        <v>2238142443</v>
       </c>
       <c r="F51" t="n">
-        <v>307442437</v>
+        <v>154831016</v>
       </c>
       <c r="G51" t="n">
-        <v>0.40326</v>
+        <v>-0.11394</v>
       </c>
     </row>
   </sheetData>

</xml_diff>